<commit_message>
latest updates to editorial manually curated dataset
</commit_message>
<xml_diff>
--- a/qnacrawler/merged.xlsx
+++ b/qnacrawler/merged.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H204"/>
+  <dimension ref="A1:H203"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -645,7 +645,7 @@
         <v>What’s closed statewide?</v>
       </c>
       <c r="B11" t="str">
-        <v>Statewide, the following are still closed:\n\n*   Personal services, like nail salons, body waxing and tattoo parlors\n*   Public events and gatherings, like live audience sports \n*   Convention centers\n*   Theme parks and festivals\n*   Higher education (in person), except where supporting [essential workforce activities](https://covid19.ca.gov/essential-workforce/), including but not limited to providing housing solutions, COVID-19 response, and training and instruction for the essential workforce.\n*   Indoor playgrounds, like bounce centers, ball pits and laser tag\n*   Saunas and steam rooms\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Statewide, the following are still closed:\n\n*   Personal services, like nail salons, body waxing and tattoo parlors\n*   Public events and gatherings, like live audience sports \n*   Convention centers\n*   Theme parks and festivals\n*   Higher education (in person), except where supporting [essential workforce activities](https://covid19.ca.gov/essential-workforce/), including but not limited to providing housing solutions, COVID-19 response, and training and instruction for the essential workforce.\n*   Indoor playgrounds, like bounce centers, ball pits and laser tag\n*   Saunas and steam rooms\n*   Recreational team sports\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- skill, clinic, youth, sports, league, recreational, team --&gt;</v>
       </c>
       <c r="C11" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -694,10 +694,10 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Can I visit my family and friends?</v>
+        <v>Is it safe to shop at open businesses?</v>
       </c>
       <c r="B13" t="str">
-        <v>It is best to stay connected with your loved ones through phone and video calls, as visiting family and friends outside your household still presents a risk of spreading coronavirus. Keeping distance from others is especially important for people that are at higher risk of getting very sick, including older people, and people of any age who have underlying medical conditions. \n\nIf you do visit family or friends that don’t live in your home in person, take steps to keep everyone safe, like:\n\n*   Keep at least 6 feet between yourself and others, even when you wear a face covering\n*   Visit outdoors instead of indoors when possible\n*   Wear a face covering or cloth mask\n*   Wash your hands often\n*   Clean and disinfect commonly-touched surfaces\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- weddings, wedding, travel, small social gathering, tourism, funeral, funerals --&gt;</v>
+        <v>The risk of COVID-19 infection is still real for all Californians and continues to be fatal. That is why every business permitted to open should take every step humanly possible to reduce the risk of infection by following these [state guidelines](https://covid19.ca.gov/roadmap/).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C13" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -720,10 +720,10 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Is it safe to shop at open businesses?</v>
+        <v>Can the Order be changed?</v>
       </c>
       <c r="B14" t="str">
-        <v>The risk of COVID-19 infection is still real for all Californians and continues to be fatal. That is why every business permitted to open should take every step humanly possible to reduce the risk of infection by following these [state guidelines](https://covid19.ca.gov/roadmap/).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes. The State Public Health Officer may issue new orders as the public health situation changes.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C14" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -746,10 +746,10 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Can the Order be changed?</v>
+        <v>How does this order interact with local orders to shelter in place? Does it supersede them?</v>
       </c>
       <c r="B15" t="str">
-        <v>Yes. The State Public Health Officer may issue new orders as the public health situation changes.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>This is a statewide order. Counties may move further into the Resilience Roadmap if they meet certain criteria.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C15" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -772,10 +772,10 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>How does this order interact with local orders to shelter in place? Does it supersede them?</v>
+        <v>If I am not an Essential Critical Infrastructure Worker, can I still leave the house?</v>
       </c>
       <c r="B16" t="str">
-        <v>This is a statewide order. Counties may move further into the Resilience Roadmap if they meet certain criteria.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes. As described in more detail elsewhere in applicable state public health directives (including on this page), there are a wide range of circumstances in which you may leave your home or other place of residence, even if you are not an Essential Critical Infrastructure Worker. For example, you may leave your home to work at any business or other entity that is allowed to open, to engage in in-person worship and protest activities consistent with public health directives, to patronize local businesses, or to care for friends or family members who require assistance (as set forth below). And errands like these are not the only reasons you may leave your home: you may also leave your home with or without a specific destination in mind (for example, to walk your dog, to engage in physical recreation, or simply to get some fresh air) as long as you maintain physical distancing and comply with any other applicable public health directives.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C16" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -798,10 +798,10 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>If I am not an Essential Critical Infrastructure Worker, can I still leave the house?</v>
+        <v>Are mass gatherings permitted?</v>
       </c>
       <c r="B17" t="str">
-        <v>Yes. As described in more detail elsewhere in applicable state public health directives (including on this page), there are a wide range of circumstances in which you may leave your home or other place of residence, even if you are not an Essential Critical Infrastructure Worker. For example, you may leave your home to work at any business or other entity that is allowed to open, to engage in in-person worship and protest activities consistent with public health directives, to patronize local businesses, or to care for friends or family members who require assistance (as set forth below). And errands like these are not the only reasons you may leave your home: you may also leave your home with or without a specific destination in mind (for example, to walk your dog, to engage in physical recreation, or simply to get some fresh air) as long as you maintain physical distancing and comply with any other applicable public health directives.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>State public health directives prohibit professional, social and community mass gatherings. Gatherings are defined as—meetings or other events that bring together persons from multiple households at the same time for a shared or group experience in a single room, space, or place such as an auditorium, stadium, arena, large conference room, meeting hall, or other indoor or outdoor space. They pose an especially high danger of transmission and spread of COVID-19.\n\nOn May 25, 2020, in an effort to balance First Amendment interests with public health, the State Public Health Officer created an exception to the prohibition against mass gatherings for faith-based services and cultural ceremonies as well as protests. Those types of gatherings are now permitted indoors so long as they do not exceed 100 attendees or 25% of the capacity of the space in which the gathering is held, whichever is lower. State public health directives now do not prohibit in-person outdoor faith-based services or protests as long as physical distancing of six feet between persons or groups of persons from different households is maintained at all times. All other mass gatherings are prohibited until further notice, except as otherwise specifically permitted in state public health directives (including in applicable industry guidance).\n\nCrowds and limited physical distancing increase the risk for COVID-19. If you attended a protest, remember that confidential, free testing is available. [Find a testing location near you](https://urldefense.proofpoint.com/v2/url?u=https-3A__covid19.ca.gov_testing-2Dand-2Dtreatment_-23top&amp;d=DwMGaQ&amp;c=Lr0a7ed3egkbwePCNW4ROg&amp;r=yRsi0eKVK6Khc58oFC32XROAJ-JqVGBGabDv9P6148k&amp;m=Iul4bdNDGFuRu3rXHrxPHNWT2PT2bXFITW3YP1tzG94&amp;s=4qpOZ7lX1S5M_STTblq_XAQNu05ccIFwIyu4bvl9U3c&amp;e=). If you test negative it does not mean that you may not develop COVID-19 later on. Therefore, it is advisable that you self-isolate for 14 days if possible.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- wedding, protest, funeral, banquet, event, outdoor, conference, symposium, rally, rallies, assembly, assemblies, convention, congregation, congregate, congregation, crowd, group, forum, worship --&gt;</v>
       </c>
       <c r="C17" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -824,10 +824,10 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Are mass gatherings permitted?</v>
+        <v>Can I get a haircut?</v>
       </c>
       <c r="B18" t="str">
-        <v>State public health directives prohibit professional, social and community mass gatherings. Gatherings are defined as—meetings or other events that bring together persons from multiple households at the same time for a shared or group experience in a single room, space, or place such as an auditorium, stadium, arena, large conference room, meeting hall, or other indoor or outdoor space. They pose an especially high danger of transmission and spread of COVID-19.\n\nOn May 25, 2020, in an effort to balance First Amendment interests with public health, the State Public Health Officer created an exception to the prohibition against mass gatherings for faith-based services and cultural ceremonies as well as protests. Those types of gatherings are now permitted indoors so long as they do not exceed 100 attendees or 25% of the capacity of the space in which the gathering is held, whichever is lower. State public health directives now do not prohibit in-person outdoor faith-based services or protests as long as physical distancing of six feet between persons or groups of persons from different households is maintained at all times. All other mass gatherings are prohibited until further notice, except as otherwise specifically permitted in state public health directives (including in applicable industry guidance).\n\nCrowds and limited physical distancing increase the risk for COVID-19. If you attended a protest, remember that confidential, free testing is available. [Find a testing location near you](https://urldefense.proofpoint.com/v2/url?u=https-3A__covid19.ca.gov_testing-2Dand-2Dtreatment_-23top&amp;d=DwMGaQ&amp;c=Lr0a7ed3egkbwePCNW4ROg&amp;r=yRsi0eKVK6Khc58oFC32XROAJ-JqVGBGabDv9P6148k&amp;m=Iul4bdNDGFuRu3rXHrxPHNWT2PT2bXFITW3YP1tzG94&amp;s=4qpOZ7lX1S5M_STTblq_XAQNu05ccIFwIyu4bvl9U3c&amp;e=). If you test negative it does not mean that you may not develop COVID-19 later on. Therefore, it is advisable that you self-isolate for 14 days if possible.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- wedding, protest, funeral, banquet, event, event planning, outdoor, conference, symposium, rally, rallies, assembly, assemblies, convention, congregation, congregate, congregation, crowd, group, forum --&gt;</v>
+        <v>It depends. If your county has been approved to move further in the Resilience Roadmap, then hair salons and barber shops may reopen in your area. See the list of [counties with a variance](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/County_Variance_Attestation_Form.aspx).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- barbering --&gt;</v>
       </c>
       <c r="C18" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -850,10 +850,10 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Can I get a haircut?</v>
+        <v>I want to express my political views.  How can I make my voice heard without raising public health concerns?</v>
       </c>
       <c r="B19" t="str">
-        <v>It depends. If your county has been approved to move further in the Resilience Roadmap, then hair salons and barber shops may reopen in your area. See the list of [counties with a variance](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/County_Variance_Attestation_Form.aspx).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>There are many ways for you to express your political views without holding a physical, in-person gathering.  For example, you may continue to call or write elected officials, write letters to the editor of news publications, display lawn or window signs, or use online and other electronic media (including Zoom rooms, Twitter feeds, Facebook pages, and other digital forums) to express your views.  \n\nAdditionally, as noted above, you may leave your home for any reason as long as you comply with any other applicable public health directives. When you are otherwise out in public, public health directives do not prevent you from engaging in political expression—such as by wearing or carrying a sign.\n\nIf collective action in physical space is important to you, consider whether you and other participants can safely protest from within your cars.  The State Public Health Officer does not consider in-car activities to be gatherings, if participants stay in their cars and otherwise remain apart from individuals who are not part of their households.  Many activists have organized car-based protests (honking horns, flying flags, displaying signs, and so on) to express their political views while complying with State public health directives.  \n\nWhenever you are considering a protest (including an in-car protest), make sure you comply with all other applicable laws, including any local public-health measures that may be more restrictive than statewide directives and any other applicable local laws.\n\nIf you do wish to engage in in-person protest outside of your car with a group of any size, you must follow the guidelines for political protest gatherings below.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C19" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -876,10 +876,10 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>I want to express my political views.  How can I make my voice heard without raising public health concerns?</v>
+        <v>Can I engage in political protest gatherings?</v>
       </c>
       <c r="B20" t="str">
-        <v>There are many ways for you to express your political views without holding a physical, in-person gathering.  For example, you may continue to call or write elected officials, write letters to the editor of news publications, display lawn or window signs, or use online and other electronic media (including Zoom rooms, Twitter feeds, Facebook pages, and other digital forums) to express your views.  \n\nAdditionally, as noted above, you may leave your home for any reason as long as you comply with any other applicable public health directives. When you are otherwise out in public, public health directives do not prevent you from engaging in political expression—such as by wearing or carrying a sign.\n\nIf collective action in physical space is important to you, consider whether you and other participants can safely protest from within your cars.  The State Public Health Officer does not consider in-car activities to be gatherings, if participants stay in their cars and otherwise remain apart from individuals who are not part of their households.  Many activists have organized car-based protests (honking horns, flying flags, displaying signs, and so on) to express their political views while complying with State public health directives.  \n\nWhenever you are considering a protest (including an in-car protest), make sure you comply with all other applicable laws, including any local public-health measures that may be more restrictive than statewide directives and any other applicable local laws.\n\nIf you do wish to engage in in-person protest outside of your car with a group of any size, you must follow the guidelines for political protest gatherings below.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes, although in-person protests present special public health concerns. \n\nEven with adherence to physical distancing, bringing members of different households together to engage in in-person protest carries a higher risk of widespread transmission of COVID-19.  Such gatherings may result in increased rates of infection, hospitalization, and death, especially among more vulnerable populations. In particular, activities like chanting, shouting, singing, and group recitation negate the risk-reduction achieved through six feet of physical distancing. For this reason, people engaging in these activities should wear face coverings at all times.\n\nTherefore, it is strongly recommended that those exercising their right to engage in political expression (including, for example, their right to petition the government) should utilize alternative channels, such as the many online and broadcasting platforms available in the digital age, in place of in-person gatherings. \n\nHowever, state public health directives do not prohibit in-person _outdoor_ protests as long as physical distancing of six feet between persons or groups of persons from different households is maintained at all times. Local Health Officers are advised to consider appropriate limitations on outdoor attendance capacities, factoring their jurisdiction’s key COVID-19 health indicators. Failure to maintain adequate physical distancing may result in an order to disperse or other enforcement action. Masks and cloth face coverings are strongly recommended.\n\nState public health directives do not prohibit in-person _indoor_ protests as long as (1) attendance is limited to 25% of the relevant area’s maximum occupancy, as defined by the relevant local permitting authority or other relevant authority, or a maximum of 100 attendees, whichever is lower, and (2) physical distancing of six feet between persons or groups of persons from different households is maintained at all times. Failure to maintain adequate physical distancing may result in an order to disperse or other enforcement action. Masks and cloth face coverings are strongly recommended.\n\nParticipants must maintain a physical distance of six feet from any uniformed peace officers and other public safety personnel present, unless otherwise directed, and follow all other requirements and directives imposed by local health officers and law enforcement, or other applicable authorities.\n\nThis limitation on attendance will be reviewed regularly. This review will assess the impacts of these imposed limits on public health and provide further direction as part of a phased-in restoration of gatherings that implicate the First Amendment.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C20" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -902,10 +902,10 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>Can I engage in political protest gatherings?</v>
+        <v>How do I vote?</v>
       </c>
       <c r="B21" t="str">
-        <v>Yes, although in-person protests present special public health concerns. \n\nEven with adherence to physical distancing, bringing members of different households together to engage in in-person protest carries a higher risk of widespread transmission of COVID-19.  Such gatherings may result in increased rates of infection, hospitalization, and death, especially among more vulnerable populations. In particular, activities like chanting, shouting, singing, and group recitation negate the risk-reduction achieved through six feet of physical distancing. For this reason, people engaging in these activities should wear face coverings at all times.\n\nTherefore, it is strongly recommended that those exercising their right to engage in political expression (including, for example, their right to petition the government) should utilize alternative channels, such as the many online and broadcasting platforms available in the digital age, in place of in-person gatherings. \n\nHowever, state public health directives do not prohibit in-person _outdoor_ protests as long as physical distancing of six feet between persons or groups of persons from different households is maintained at all times. Local Health Officers are advised to consider appropriate limitations on outdoor attendance capacities, factoring their jurisdiction’s key COVID-19 health indicators. Failure to maintain adequate physical distancing may result in an order to disperse or other enforcement action. Masks and cloth face coverings are strongly recommended.\n\nState public health directives do not prohibit in-person _indoor_ protests as long as (1) attendance is limited to 25% of the relevant area’s maximum occupancy, as defined by the relevant local permitting authority or other relevant authority, or a maximum of 100 attendees, whichever is lower, and (2) physical distancing of six feet between persons or groups of persons from different households is maintained at all times. Failure to maintain adequate physical distancing may result in an order to disperse or other enforcement action. Masks and cloth face coverings are strongly recommended.\n\nParticipants must maintain a physical distance of six feet from any uniformed peace officers and other public safety personnel present, unless otherwise directed, and follow all other requirements and directives imposed by local health officers and law enforcement, or other applicable authorities.\n\nThis limitation on attendance will be reviewed regularly. This review will assess the impacts of these imposed limits on public health and provide further direction as part of a phased-in restoration of gatherings that implicate the First Amendment.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Elections are an essential activity, and the [Governor has issued executive orders to ensure elections are safe and accessible](https://www.gov.ca.gov/2020/05/08/governor-newsom-issues-executive-order-to-protect-public-health-by-mailing-every-registered-voter-a-ballot-ahead-of-the-november-general-election/). Vote-by-mail ballots will be sent to all registered voters for the November 3, 2020 General Election. Additionally, many in-person voting opportunities will be available: counties are required to provide [three days of early voting](https://www.gov.ca.gov/2020/06/03/governor-newsom-signs-executive-order-on-safe-secure-and-accessible-general-election-in-november/) starting the Saturday before the election, and open ballot drop-box locations between October 6 and November 3, 2020. The Secretary of State and the California Department of Public Health are working on additional guidance to ensure that all Californians are able to participate in elections safely. Except where suspended by Executive Order, existing laws addressing the use of vote-by-mail ballots in California elections remain in effect.\n\nOf course, whenever you engage in any permissible activity—including the collection and drop-off of ballots, or other election-related activities (such as the collection of signatures to qualify candidates or measures for the ballot)—adhere to physical distancing and other applicable public health directives.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C21" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -928,10 +928,10 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>How do I vote?</v>
+        <v>Can I go to church?</v>
       </c>
       <c r="B22" t="str">
-        <v>Elections are an essential activity, and the [Governor has issued executive orders to ensure elections are safe and accessible](https://www.gov.ca.gov/2020/05/08/governor-newsom-issues-executive-order-to-protect-public-health-by-mailing-every-registered-voter-a-ballot-ahead-of-the-november-general-election/). Vote-by-mail ballots will be sent to all registered voters for the November 3, 2020 General Election. Additionally, many in-person voting opportunities will be available: counties are required to provide [three days of early voting](https://www.gov.ca.gov/2020/06/03/governor-newsom-signs-executive-order-on-safe-secure-and-accessible-general-election-in-november/) starting the Saturday before the election, and open ballot drop-box locations between October 6 and November 3, 2020. The Secretary of State and the California Department of Public Health are working on additional guidance to ensure that all Californians are able to participate in elections safely. Except where suspended by Executive Order, existing laws addressing the use of vote-by-mail ballots in California elections remain in effect.\n\nOf course, whenever you engage in any permissible activity—including the collection and drop-off of ballots, or other election-related activities (such as the collection of signatures to qualify candidates or measures for the ballot)—adhere to physical distancing and other applicable public health directives.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes. As of May 25, places of worship such as churches, mosques, temples, and synagogues can open throughout the state, with [modifications for safety (PDF)](https://covid19.ca.gov/pdf/guidance-places-of-worship.pdf).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- church, mosque, synagogue, worship, temple, wedding, funeral, baptism --&gt;</v>
       </c>
       <c r="C22" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -954,10 +954,10 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Can I go to church?</v>
+        <v>Can I practice my religious faith?</v>
       </c>
       <c r="B23" t="str">
-        <v>Yes. As of May 25, places of worship such as churches, mosques, temples, and synagogues can open throughout the state, with [modifications for safety (PDF)](https://covid19.ca.gov/pdf/guidance-places-of-worship.pdf).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes. Practicing your faith is a constitutionally-protected activity and may manifest in many different forms.\n\nAlthough in-person religious gatherings—like other in-person gatherings—have been restricted to prevent the transmission of COVID-19, on May 25, 2020, the State Public Health Officer began to ease restrictions on in-person religious gatherings. In particular, the State Public Health Officer now authorizes County Departments of Public Health to allow collective activities at places of worship, subject to conditions to support a safe, clean environment for employees, interns and trainees, volunteers, scholars, and all other types of workers as well as congregants, worshippers, and visitors.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- church, mosque, synagogue, temple, wedding, funeral, baptism --&gt;</v>
       </c>
       <c r="C23" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -980,10 +980,10 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>Can I practice my religious faith?</v>
+        <v>What conditions must be met to resume religious services at places of worship?</v>
       </c>
       <c r="B24" t="str">
-        <v>Yes. Practicing your faith is a constitutionally-protected activity and may manifest in many different forms.\n\nAlthough in-person religious gatherings—like other in-person gatherings—have been restricted to prevent the transmission of COVID-19, on May 25, 2020, the State Public Health Officer began to ease restrictions on in-person religious gatherings. In particular, the State Public Health Officer now authorizes County Departments of Public Health to allow collective activities at places of worship, subject to conditions to support a safe, clean environment for employees, interns and trainees, volunteers, scholars, and all other types of workers as well as congregants, worshippers, and visitors.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Information on conditions imposed by the state can be found at [guidance for places of worship (PDF)](https://covid19.ca.gov/pdf/guidance-places-of-worship.pdf). Additional conditions may be imposed by local public health officials. This guidance does not obligate places of worship to resume in-person activity. It is strongly recommended that places of worship continue to facilitate remote services and other alternatives to in-person religious practice for those who are vulnerable to COVID19.\n\nEven with adherence to physical distancing, convening in a congregational setting of multiple households to practice a personal faith carries a higher risk of widespread transmission of COVID-19, and may result in increased rates of infection, hospitalization, and death, especially among more vulnerable populations. In particular, activities like singing and group recitation dramatically increase the risk of COVID-19 transmission. For this reason, congregants engaging in singing, particularly in the choir, and group recitation should wear face coverings at all times.\n\nPlaces of worship must therefore limit _indoor_ attendance to 25% of building capacity or a maximum of 100 attendees, whichever is lower. Local Health Officers are advised to consider appropriate limitations on _outdoor_ attendance capacities, factoring their jurisdiction’s key COVID-19 health indicators. At a minimum, outdoor attendance should be limited naturally through implementation of strict physical distancing measures of a minimum of six feet between attendees from different households, in addition to other relevant protocols within this document.\n\nThis limitation will be in effect for the first 21 days of a county public health department’s approval of religious services and cultural ceremonies activities at places of worship within their jurisdictions.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C24" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1006,10 +1006,10 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>What conditions must be met to resume religious services at places of worship?</v>
+        <v>Can children attend group activities (like Sunday school or Hebrew school) at places of worship?</v>
       </c>
       <c r="B25" t="str">
-        <v>Information on conditions imposed by the state can be found at [guidance for places of worship (PDF)](https://covid19.ca.gov/pdf/guidance-places-of-worship.pdf). Additional conditions may be imposed by local public health officials. This guidance does not obligate places of worship to resume in-person activity. It is strongly recommended that places of worship continue to facilitate remote services and other alternatives to in-person religious practice for those who are vulnerable to COVID19.\n\nEven with adherence to physical distancing, convening in a congregational setting of multiple households to practice a personal faith carries a higher risk of widespread transmission of COVID-19, and may result in increased rates of infection, hospitalization, and death, especially among more vulnerable populations. In particular, activities like singing and group recitation dramatically increase the risk of COVID-19 transmission. For this reason, congregants engaging in singing, particularly in the choir, and group recitation should wear face coverings at all times.\n\nPlaces of worship must therefore limit _indoor_ attendance to 25% of building capacity or a maximum of 100 attendees, whichever is lower. Local Health Officers are advised to consider appropriate limitations on _outdoor_ attendance capacities, factoring their jurisdiction’s key COVID-19 health indicators. At a minimum, outdoor attendance should be limited naturally through implementation of strict physical distancing measures of a minimum of six feet between attendees from different households, in addition to other relevant protocols within this document.\n\nThis limitation will be in effect for the first 21 days of a county public health department’s approval of religious services and cultural ceremonies activities at places of worship within their jurisdictions.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>At this time, no. Children should remain in the care of those in their household unit and not interact with children of other parties at all times while visiting facilities. Places of worship must discontinue activities and services for children (for example, shared play areas) where physical distancing of at least six feet cannot be maintained.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C25" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1032,10 +1032,10 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Can children attend group activities (like Sunday school or Hebrew school) at places of worship?</v>
+        <v>When will these conditions change for places of worship?</v>
       </c>
       <c r="B26" t="str">
-        <v>At this time, no. Children should remain in the care of those in their household unit and not interact with children of other parties at all times while visiting facilities. Places of worship must discontinue activities and services for children (for example, shared play areas) where physical distancing of at least six feet cannot be maintained.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Every 21 days, the California Department of Public Health, in consultation with county Departments of Public Health, will review and assess the impacts of these imposed limits on public health and provide further direction as part of a phased-in restoration of activities in places of worship. This is because COVID-19 has an incubation period of 14 days; the 21-day interval accounts for this incubation period and provides for an additional seven days for thorough review, analysis, and preparation of modifications.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C26" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1058,10 +1058,10 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>When will these conditions change for places of worship?</v>
+        <v>Can I still exercise? Take my kids to the park for fresh air? Take a walk around the block?</v>
       </c>
       <c r="B27" t="str">
-        <v>Every 21 days, the California Department of Public Health, in consultation with county Departments of Public Health, will review and assess the impacts of these imposed limits on public health and provide further direction as part of a phased-in restoration of activities in places of worship. This is because COVID-19 has an incubation period of 14 days; the 21-day interval accounts for this incubation period and provides for an additional seven days for thorough review, analysis, and preparation of modifications.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>It’s okay to go outside to go for a walk, to exercise, and participate in healthy activities as long as you **maintain a safe physical distance of six feet and gather only with members of your household.** You can also participate in activities at [outdoor recreational facilities](https://covid19.ca.gov/pdf/guidance-campgrounds.pdf) that are allowed to open. [Parks may be closed](https://covid19.ca.gov/public-recreation/) to help slow the spread of the virus. Check with local officials about park closures in your area. Californians should not travel significant distances for recreation and should stay close to home.\n\nBelow is a list of some outdoor recreational activities.\n\n*   Badminton (singles)\n*   Throwing a baseball/softball\n*   BMX biking\n*   Canoeing (singles)\n*   Crabbing\n*   Cycling\n*   Exploring rock pools\n*   Gardening (not in groups)\n*   Golfing (doubles, only if cart has protective partition)\n*   Hiking (trails/ paths allowing distancing)\n*   Horse riding (singles)\n*   Jogging and running\n*   Kite boarding and kitesurfing\n*   Meditation\n*   Outdoor photography\n*   Picnics (with your household members only)\n*   Quad biking\n*   Rock climbing\n*   Roller skating and rollerblading\n*   Rowing (singles)\n*   Scootering (not in groups)\n*   Skateboarding (not in groups)\n*   Soft martial arts – tai chi, chi kung (not in groups)\n*   Surfing\n*   Tennis and table tennis (singles)\n*   Throwing a football, kicking a soccer ball (not in groups)\n*   Trail running\n*   Trampolining\n*   Tree climbing\n*   Volleyball (singles)\n*   Walk the dog\n*   Wash the car\n*   Watch the sunrise or sunset\n*   Yoga\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C27" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>Can I still exercise? Take my kids to the park for fresh air? Take a walk around the block?</v>
+        <v>Can I walk my dog? Take my pet to the vet?</v>
       </c>
       <c r="B28" t="str">
-        <v>It’s okay to go outside to go for a walk, to exercise, and participate in healthy activities as long as you **maintain a safe physical distance of six feet and gather only with members of your household.** You can also participate in activities at [outdoor recreational facilities](https://covid19.ca.gov/pdf/guidance-campgrounds.pdf) that are allowed to open. [Parks may be closed](https://covid19.ca.gov/public-recreation/) to help slow the spread of the virus. Check with local officials about park closures in your area. Californians should not travel significant distances for recreation and should stay close to home.\n\nBelow is a list of some outdoor recreational activities.\n\n*   Badminton (singles)\n*   Throwing a baseball/softball\n*   BMX biking\n*   Canoeing (singles)\n*   Crabbing\n*   Cycling\n*   Exploring rock pools\n*   Gardening (not in groups)\n*   Golfing (doubles, only if cart has protective partition)\n*   Hiking (trails/ paths allowing distancing)\n*   Horse riding (singles)\n*   Jogging and running\n*   Kite boarding and kitesurfing\n*   Meditation\n*   Outdoor photography\n*   Picnics (with your household members only)\n*   Quad biking\n*   Rock climbing\n*   Roller skating and rollerblading\n*   Rowing (singles)\n*   Scootering (not in groups)\n*   Skateboarding (not in groups)\n*   Soft martial arts – tai chi, chi kung (not in groups)\n*   Surfing\n*   Tennis and table tennis (singles)\n*   Throwing a football, kicking a soccer ball (not in groups)\n*   Trail running\n*   Trampolining\n*   Tree climbing\n*   Volleyball (singles)\n*   Walk the dog\n*   Wash the car\n*   Watch the sunrise or sunset\n*   Yoga\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>You can walk your dog. You can go to the vet or pet hospital if your pet is sick. Remember to distance yourself at least six feet from other pets and owners.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C28" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1110,10 +1110,10 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>Can I walk my dog? Take my pet to the vet?</v>
+        <v>Can I visit State Parks? What outdoor spaces are open?</v>
       </c>
       <c r="B29" t="str">
-        <v>You can walk your dog. You can go to the vet or pet hospital if your pet is sick. Remember to distance yourself at least six feet from other pets and owners.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>State Parks, campgrounds, museums, and visitor centers [may continue to be closed](https://www.parks.ca.gov/?page_id=30350) to help slow the spread of the virus. Starting June 12, some counties may open campgrounds and RV parks. Be sure to check [parks in your area before you travel](https://covid19.ca.gov/public-recreation/). Californians should not travel significant distances for pleasure or recreation and should stay close to home. If you do travel, take steps to keep everyone safe like wearing a face cloth covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently.\n\nYou can walk, run, hike and bike in your local neighborhoods as long as they continue to practice physical distancing of 6 feet. This means avoiding crowded trails and parking lots.\n\nFor information on National Parks, please the [National Park Service website](https://www.nps.gov/aboutus/news/public-health-update.htm).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- park, visitor center, travel, museum, RV parks, recreation, outdoor recreation, sports, RV, tent camping, tent camp, fish, beach, lake, river, event, outdoor event, event planning, wedding, hike, walk, bike, exercise, nature, bird watching, public →&lt;/p&gt;--&gt;</v>
       </c>
       <c r="C29" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1136,10 +1136,10 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>Can I visit State Parks? What outdoor spaces are open?</v>
+        <v>Can I travel?</v>
       </c>
       <c r="B30" t="str">
-        <v>State Parks, campgrounds, museums, and visitor centers [may continue to be closed](https://www.parks.ca.gov/?page_id=30350) to help slow the spread of the virus. Starting June 12, some counties may open campgrounds and RV parks. Be sure to check [parks in your area before you travel](https://covid19.ca.gov/public-recreation/). Californians should not travel significant distances for pleasure or recreation and should stay close to home. If you do travel, take steps to keep everyone safe like wearing a face cloth covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently.\n\nYou can walk, run, hike and bike in your local neighborhoods as long as they continue to practice physical distancing of 6 feet. This means avoiding crowded trails and parking lots.\n\nFor information on National Parks, please the [National Park Service website](https://www.nps.gov/aboutus/news/public-health-update.htm).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- park, visitor center, travel, museum, RV parks, recreation, outdoor recreation, sports, RV, tent camping, tent camp, fish, beach, lake, river, event, outdoor event, event planning, wedding, hike, walk, bike, exercise, nature, bird watching, public →&lt;/p&gt;--&gt;</v>
+        <v>You can travel for urgent matters or if such travel is essential to your permitted work. Even though businesses around the state are opening up, avoid travelling long distances for vacations or pleasure as much as possible. This is to slow the spread of the coronavirus. Do not travel if you are sick, or if someone in your household has had coronavirus in the last two weeks. Do not travel with someone who is sick.\n\nBefore travelling away from your community, consider these questions from the [Center for Disease Control (CDC) travel guidance](https://www.cdc.gov/coronavirus/2019-ncov/travelers/travel-in-the-us.html):\n\n*   Is coronavirus spreading where you are traveling?\n*   Are you or those you are traveling with more likely to get very sick from coronavirus?\n*   Will you be able to keep 6 feet of physical distance from others during or after your trip?\n\nIf you do travel, take steps to keep everyone safe like wearing a face cloth covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently.  \n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- wedding, travel, gathering, tourism, funeral, motel, vacation, airbnb, vrbo, rental home --&gt;</v>
       </c>
       <c r="C30" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1162,10 +1162,10 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>Can I travel?</v>
+        <v>Can I go to the Department of Motor Vehicles (DMV)?</v>
       </c>
       <c r="B31" t="str">
-        <v>You can travel for urgent matters or if such travel is essential to your permitted work. Even though businesses around the state are opening up, avoid travelling long distances for vacations or pleasure as much as possible. This is to slow the spread of the coronavirus. Do not travel if you are sick, or if someone in your household has had coronavirus in the last two weeks. Do not travel with someone who is sick.\n\nBefore travelling away from your community, consider these questions from the [Center for Disease Control (CDC) travel guidance](https://www.cdc.gov/coronavirus/2019-ncov/travelers/travel-in-the-us.html):\n\n*   Is coronavirus spreading where you are traveling?\n*   Are you or those you are traveling with more likely to get very sick from coronavirus?\n*   Will you be able to keep 6 feet of physical distance from others during or after your trip?\n\nIf you do travel, take steps to keep everyone safe like wearing a face cloth covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently.  \n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Beginning June 11, [all DMV offices](https://www.dmv.ca.gov/portal/news-and-media/dmv-reopens-remaining-field-offices-to-public/) are open to the public to help with appointments that require an in-person visit. You will be required to wear a cloth mask and must remain 6 feet apart in line. In-person appointments are limited to:\n\n*   Paying registration for a vehicle impounded because of registration-related issues\n*   Reinstating a suspended or revoked driver license\n*   Applying for a reduced-fee or no-fee identification card\n*   Processing commercial driver license transactions\n*   Applying for a disabled person parking placards\n*   Adding an ambulance certificate or firefighter endorsement to a driver license\n*   Verifying a transit training document to drive a transit bus\n*   Processing DMV Express customers for REAL ID transactions, if time and space allows\n\n*   On June 26, the DMV will begin behind-the-wheel driving tests. The DMV will reschedule all cancelled driving test appointments. New behind-the-wheel driving tests will not be available until all cancelled appointments are completed. \n    *   [For the health and safety of drivers and DMV staff](https://www.dmv.ca.gov/portal/news-and-media/dmv-resumes-behind-the-wheel-drive-tests-with-new-protocols-on-friday/), you must wear a face covering and will have your temperature checked before the test.\n\nDMV services that do not require an in-person office visit can be accessed through the [DMV Virtual Field Office](https://virtual.dmv.ca.gov/), including driver’s license renewals, vehicle registrations, title changes, and more.\n\nDMV has extended deadlines for:\n\n*   All drivers licenses expiring between March 1 through July 31, 2020\n    *   Drivers 70 years of age and older will receive a 120-day paper extension.\n    *   Drivers 69 years of age and younger can request a free temporary [extension online](https://www.dmv.ca.gov/portal/dmv-virtual-office/temporary-driver-license-extension/), though one is not needed to drive.\n*   Expiring commercial licenses, endorsements, and certificates are valid through June 30, 2020.\n*   In-person renewals for vehicle registrations that expire between the dates of March 16, 2020, and May 31, 2020.\n*   In-person renewals for those with safe driving records whose last DMV visit was 15 years ago.\n*   Driver license permits expiring between June through August 2020 are extended six months or to a date 24 months from the date of application, whichever is earlier.\n*   Commercial learner’s permits expiring between March and June 2020 are now valid through June 30, 2020.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C31" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1188,10 +1188,10 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>Can I go to the Department of Motor Vehicles (DMV)?</v>
+        <v>Can I get my car smog checked?</v>
       </c>
       <c r="B32" t="str">
-        <v>Beginning June 11, [all DMV offices](https://www.dmv.ca.gov/portal/news-and-media/dmv-reopens-remaining-field-offices-to-public/) are open to the public to help with appointments that require an in-person visit. You will be required to wear a cloth mask and must remain 6 feet apart in line. In-person appointments are limited to:\n\n*   Paying registration for a vehicle impounded because of registration-related issues\n*   Reinstating a suspended or revoked driver license\n*   Applying for a reduced-fee or no-fee identification card\n*   Processing commercial driver license transactions\n*   Applying for a disabled person parking placards\n*   Adding an ambulance certificate or firefighter endorsement to a driver license\n*   Verifying a transit training document to drive a transit bus\n*   Processing DMV Express customers for REAL ID transactions, if time and space allows\n\nDMV services that do not require an in-person office visit can be accessed through the [DMV Virtual Field Office](https://virtual.dmv.ca.gov/), including driver’s license renewals, vehicle registrations, title changes, and more.\n\nDMV has extended deadlines for:\n\n*   All drivers licenses expiring between March 1 through July 31, 2020\n    *   Drivers 70 years of age and older will receive a 120-day paper extension\n    *   Drivers 69 years of age and younger can request a free temporary [extension online](https://www.dmv.ca.gov/portal/dmv-virtual-office/temporary-driver-license-extension/), though one is not needed to drive\n*   Expiring commercial licenses, endorsements, and certificates are valid through June 30, 2020\n*   In-person renewals for vehicle registrations that expire between the dates of March 16, 2020, and May 31, 2020.\n*   In-person renewals for those with safe driving records whose last DMV visit was 15 years ago \n*   Driver license permits expiring between June through August 2020 are extended six months or to a date 24 months from the date of application, whichever is earlier.\n    *   Behind-the-wheel driving tests are not available due to physical distancing concerns. The DMV will reschedule cancelled appointments for behind-the-wheel tests when it is safe to do so.  \n*   Commercial learner’s permits expiring between March and June 2020 are now valid through June 30, 2020\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>It depends. Some smog check locations may be closed. The [Bureau of Automotive Repair](https://www.bar.ca.gov/COVID-19_Impacts_on_BAR_Programs_and_Services.aspx) advises drivers to still pay DMV vehicle registration fees to avoid any late fees. However, you will not receive your new registration or year sticker until the smog information has been received by DMV. Once state and local orders or directives are no longer in effect, you can then obtain the required smog check certificate to complete the DMV vehicle registration process.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C32" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1214,13 +1214,13 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>Can I get my smog checked?</v>
+        <v>Should I wear a face covering or mask to protect against COVID-19?</v>
       </c>
       <c r="B33" t="str">
-        <v>The [Bureau of Automotive Repair](https://www.bar.ca.gov/COVID-19_Impacts_on_BAR_Programs_and_Services.aspx) advises drivers to still pay DMV vehicle registration fees to avoid any late fees. However, you will not receive your new registration or year sticker until the smog information has been received by DMV. Once state and local orders or directives are no longer in effect, consumers can then obtain the required smog check certificate to complete the DMV vehicle registration process.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes. Californians must wear face coverings when in public spaces, especially indoors and other areas where physical distancing is not possible. Face coverings help reduce the spread of COVID-19. \n\nThe California Department of Public Health (CDPH) has released a [Guidance](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Guidance-for-Face-Coverings_06-18-2020.pdf) for the use of face covering.\n\nThe guidance reminds Californians that the best defense against COVID-19 continues to be: \n\n*   Maintain six feet of physical distance from others \n*   Wash hands frequently\n*   Avoid touching eyes, nose and mouth with unwashed hands\n*   Avoid being around people with COVID-19 symptoms\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C33" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/healthcare/</v>
       </c>
       <c r="D33" t="str">
         <v xml:space="preserve"> </v>
@@ -1240,10 +1240,10 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>Should I wear a face covering or mask to protect against COVID-19?</v>
+        <v>How well do cloth face coverings to prevent spread of COVID-19?</v>
       </c>
       <c r="B34" t="str">
-        <v>Yes. Californians must wear face coverings when in public spaces, especially indoors and other areas where physical distancing is not possible. Face coverings help reduce the spread of COVID-19. \n\nThe California Department of Public Health (CDPH) has released a [Guidance](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Guidance-for-Face-Coverings_06-18-2020.pdf) for the use of face covering.\n\nThe guidance reminds Californians that the best defense against COVID-19 continues to be: \n\n*   Maintain six feet of physical distance from others \n*   Wash hands frequently\n*   Avoid touching eyes, nose and mouth with unwashed hands\n*   Avoid being around people with COVID-19 symptoms\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>There is scientific evidence to suggest that use of cloth face coverings by the public during a pandemic could help reduce disease transmission. Their primary role is to reduce the release of infectious particles into the air when someone speaks, coughs, or sneezes, including someone who has COVID-19 but feels well. Cloth face coverings are not a substitute for physical distancing, washing hands, and staying home when ill, but they may be helpful when combined with these primary interventions.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C34" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1266,10 +1266,10 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>How well do cloth face coverings to prevent spread of COVID-19?</v>
+        <v>What is a cloth face covering?</v>
       </c>
       <c r="B35" t="str">
-        <v>There is scientific evidence to suggest that use of cloth face coverings by the public during a pandemic could help reduce disease transmission. Their primary role is to reduce the release of infectious particles into the air when someone speaks, coughs, or sneezes, including someone who has COVID-19 but feels well. Cloth face coverings are not a substitute for physical distancing, washing hands, and staying home when ill, but they may be helpful when combined with these primary interventions.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>A cloth face covering is [material that covers the nose and mouth](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/diy-cloth-face-coverings.html). It can be secured to the head with ties or straps or simply wrapped around the lower face. It can be made of a variety of materials, such as cotton, silk, or linen. A cloth face covering may be factory-made or sewn by hand, or can be improvised from household items such as scarfs, T-shirts, sweatshirts, or towels.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C35" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1292,10 +1292,10 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>What is a cloth face covering?</v>
+        <v>How should I care for a cloth face covering?</v>
       </c>
       <c r="B36" t="str">
-        <v>A cloth face covering is [material that covers the nose and mouth](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/diy-cloth-face-coverings.html). It can be secured to the head with ties or straps or simply wrapped around the lower face. It can be made of a variety of materials, such as cotton, silk, or linen. A cloth face covering may be factory-made or sewn by hand, or can be improvised from household items such as scarfs, T-shirts, sweatshirts, or towels.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>It’s a good idea to [wash your cloth face covering](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/diy-cloth-face-coverings.html) frequently, ideally after each use. Have a bag or bin to keep cloth face coverings in until they can be laundered with detergent and hot water and dried on a hot cycle. If you must re-wear your cloth face covering before washing, wash your hands immediately after putting it back on and avoid touching your face. Discard cloth face coverings that:\n\n*   No longer cover the nose and mouth\n*   Have stretched out or damaged ties or straps\n*   Cannot stay on the face\n*   Have holes or tears in the fabric\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C36" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1318,10 +1318,10 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>How should I care for a cloth face covering?</v>
+        <v>What if I don’t have health insurance and I need screening,  testing, or treatment for COVID-19?</v>
       </c>
       <c r="B37" t="str">
-        <v>It’s a good idea to [wash your cloth face covering](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/diy-cloth-face-coverings.html) frequently, ideally after each use. Have a bag or bin to keep cloth face coverings in until they can be laundered with detergent and hot water and dried on a hot cycle. If you must re-wear your cloth face covering before washing, wash your hands immediately after putting it back on and avoid touching your face. Discard cloth face coverings that:\n\n*   No longer cover the nose and mouth\n*   Have stretched out or damaged ties or straps\n*   Cannot stay on the face\n*   Have holes or tears in the fabric\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>The cost of coronavirus screening, testing, and treatment for the uninsured is paid for by the [government](https://www.hrsa.gov/CovidUninsuredClaim). You can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor through [telehealth](https://covid19.ca.gov/telehealth/). You can also get free [testing](https://covid19.ca.gov/testing-and-treatment/) through [Verily’s Project Baseline](https://www.projectbaseline.com/study/covid-19/eligibility/) or [OptumServe](https://lhi.care/covidtesting).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C37" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1344,10 +1344,10 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>What if I don’t have health insurance and I need screening,  testing, or treatment for COVID-19?</v>
+        <v>I want to get screened or tested for COVID-19. I have insurance, but what will this cost me out-of-pocket?</v>
       </c>
       <c r="B38" t="str">
-        <v>The cost of coronavirus screening, testing, and treatment for the uninsured is paid for by the [government](https://www.hrsa.gov/CovidUninsuredClaim). You can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor through [telehealth](https://covid19.ca.gov/telehealth/). You can also get free [testing](https://covid19.ca.gov/testing-and-treatment/) through [Verily’s Project Baseline](https://www.projectbaseline.com/study/covid-19/eligibility/) or [OptumServe](https://lhi.care/covidtesting).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Nothing. The state agencies that regulate health care in California have mandated that all full-service insurance plans (including Medi-Cal) waive copayments, coinsurance, and deductibles for medically necessary screening and testing for COVID-19. This includes emergency room, urgent care, or provider office visits when the purpose of the visit is to be screened and tested for COVID-19.\n\n[Testing](https://covid19.ca.gov/testing-and-treatment/) for COVID-19 is covered by insurance, Medicare, and Medi-Cal. If you have no insurance, it’s paid for by the [government](https://www.hrsa.gov/CovidUninsuredClaim). As a first step, you can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor through [telehealth](https://covid19.ca.gov/telehealth/).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C38" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1370,10 +1370,10 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>I want to get screened or tested for COVID-19. I have insurance, but what will this cost me out-of-pocket?</v>
+        <v>I have a concern or complaint about getting care for COVID-19 under my health insurance. What can I do?</v>
       </c>
       <c r="B39" t="str">
-        <v>Nothing. The state agencies that regulate health care in California have mandated that all full-service insurance plans (including Medi-Cal) waive copayments, coinsurance, and deductibles for medically necessary screening and testing for COVID-19. This includes emergency room, urgent care, or provider office visits when the purpose of the visit is to be screened and tested for COVID-19.\n\n[Testing](https://covid19.ca.gov/testing-and-treatment/) for COVID-19 is covered by insurance, Medicare, and Medi-Cal. If you have no insurance, it’s paid for by the [government](https://www.hrsa.gov/CovidUninsuredClaim). As a first step, you can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor through [telehealth](https://covid19.ca.gov/telehealth/).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>If you are having trouble accessing care, or were inappropriately charged for medically necessary screening, testing, or treatment for COVID-19, follow up directly with your health plan by calling the member phone number listed on your health plan card. If your health plan doesn’t resolve the issue, contact the [](https://www.healthhelp.ca.gov/)[California Department of Managed Health Care (DMHC)](http://www.dmhc.ca.gov/?referral=healthhelp.ca.gov) Help Center for assistance at 1-888-466-2219.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C39" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1396,10 +1396,10 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>I have a concern or complaint about getting care for COVID-19 under my health insurance. What can I do?</v>
+        <v>Do Medicare or Medicare Advantage Plans cover coronavirus tests or coronavirus antibody tests?</v>
       </c>
       <c r="B40" t="str">
-        <v>If you are having trouble accessing care, or were inappropriately charged for medically necessary screening, testing, or treatment for COVID-19, follow up directly with your health plan by calling the member phone number listed on your health plan card. If your health plan doesn’t resolve the issue, contact the [](https://www.healthhelp.ca.gov/)[California Department of Managed Health Care (DMHC)](http://www.dmhc.ca.gov/?referral=healthhelp.ca.gov) Help Center for assistance at 1-888-466-2219.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. Both [Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) cover [coronavirus tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test) tests, with no out-of-pocket costs. \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C40" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1422,10 +1422,10 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>Do Medicare or Medicare Advantage Plans cover coronavirus tests or coronavirus antibody tests?</v>
+        <v>Can I use telehealth if I am on Medicare?</v>
       </c>
       <c r="B41" t="str">
-        <v>Yes. Both [Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) cover [coronavirus tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test) tests, with no out-of-pocket costs. \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. Medicare has temporarily expanded its coverage of [telehealth services (medical care via phone, video chat, or online portal)](https://www.medicare.gov/coverage/telehealth) to respond to the current Public Health Emergency. You can now use a wide range of communication tools (including smartphone) from home to interact with a range of providers, like doctors, nurse practitioners, clinical psychologists, licensed clinical social workers, physical therapists, occupational therapists, and speech language pathologists. If you have original Medicare, you can get many services without a copayment through [telehealth,](https://covid19.ca.gov/telehealth/) including evaluation and management visits (common office visits), mental health counseling, and preventive health screenings.\n\nIf you have a [Medicare Advantage Plan](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans), you have access to these same benefits. Many plans offer additional [telehealth](https://covid19.ca.gov/telehealth/) benefits and expanded benefits, like meal delivery or medical transport services. Check with your plan about your coverage and costs.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C41" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>Can I use telehealth if I am on Medicare?</v>
+        <v>I am nervous or scared. What can I do?</v>
       </c>
       <c r="B42" t="str">
-        <v>Yes. Medicare has temporarily expanded its coverage of [telehealth services (medical care via phone, video chat, or online portal)](https://www.medicare.gov/coverage/telehealth) to respond to the current Public Health Emergency. You can now use a wide range of communication tools (including smartphone) from home to interact with a range of providers, like doctors, nurse practitioners, clinical psychologists, licensed clinical social workers, physical therapists, occupational therapists, and speech language pathologists. If you have original Medicare, you can get many services without a copayment through [telehealth,](https://covid19.ca.gov/telehealth/) including evaluation and management visits (common office visits), mental health counseling, and preventive health screenings.\n\nIf you have a [Medicare Advantage Plan](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans), you have access to these same benefits. Many plans offer additional [telehealth](https://covid19.ca.gov/telehealth/) benefits and expanded benefits, like meal delivery or medical transport services. Check with your plan about your coverage and costs.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>You are not alone. The California Surgeon General released [two playbooks for managing stress](https://covid19.ca.gov/manage-stress-for-health/#top) and tips for care-givers and kids. If you feel like you need to talk to someone and want emotional support see this [list of resources](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/#top).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C42" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1474,10 +1474,10 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>I am nervous or scared. What can I do?</v>
+        <v>My safety net eligibility (like CalFresh, Medi-Cal) is expiring and I am under the statewide stay home order for COVID-19. Do I need to renew my eligibility now?</v>
       </c>
       <c r="B43" t="str">
-        <v>You are not alone. The California Surgeon General released [two playbooks for managing stress](https://covid19.ca.gov/manage-stress-for-health/#top) and tips for care-givers and kids. If you feel like you need to talk to someone and want emotional support see this [list of resources](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/#top).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>****No, you will not need to renew until August 17, 2020.**** Governor Gavin Newsom issued an [executive order](https://www.gov.ca.gov/wp-content/uploads/2020/06/6.15.20-EO-N-69-20-text.pdf) to ensure that health care, food assistance, and in-home supportive services continue during the COVID-19 outbreak.\n\nThe order waives eligibility re-determinations for 150 days for participants in:\n\n*   Medi-Cal health coverage\n*   CalFresh food assistance\n*   CalWORKs\n*   Cash Assistance for Immigrants\n*   In-Home Supportive Services\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C43" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1500,10 +1500,10 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>My safety net eligibility (like CalFresh, Medi-Cal) is expiring and I am under the statewide stay home order for COVID-19. Do I need to renew my eligibility now?</v>
+        <v>What if I need to visit a health care provider?</v>
       </c>
       <c r="B44" t="str">
-        <v>****No, you will not need to renew until August 17, 2020.**** Governor Gavin Newsom issued an [executive order](https://www.gov.ca.gov/wp-content/uploads/2020/06/6.15.20-EO-N-69-20-text.pdf) to ensure that health care, food assistance, and in-home supportive services continue during the COVID-19 outbreak.\n\nThe order waives eligibility re-determinations for 150 days for participants in:\n\n*   Medi-Cal health coverage\n*   CalFresh food assistance\n*   CalWORKs\n*   Cash Assistance for Immigrants\n*   In-Home Supportive Services\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>If you have [coronavirus symptoms](https://covid19.ca.gov/symptoms-and-risks/#top), please contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) or use the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) self-checker.\n\nIf you have other illnesses or chronic conditions, use [telehealth](https://covid19.ca.gov/telehealth/) to get care from home.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call 911, tell the 911 operator your exact symptoms so the ambulance provider can be ready to treat you safely.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C44" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1526,10 +1526,10 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>What if I need to visit a health care provider?</v>
+        <v>What about routine, elective, or non-urgent medical or dental appointments?</v>
       </c>
       <c r="B45" t="str">
-        <v>If you have [coronavirus symptoms](https://covid19.ca.gov/symptoms-and-risks/#top), please contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) or use the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) self-checker.\n\nIf you have other illnesses or chronic conditions, use [telehealth](https://covid19.ca.gov/telehealth/) to get care from home.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call 911, tell the 911 operator your exact symptoms so the ambulance provider can be ready to treat you safely.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Preventive care services and non-emergency surgeries, like organ replacements and tumor removals, can take place if hospitals have enough capacity and protective equipment to do so safely. Eye exams, and elective procedures should be cancelled or rescheduled. If possible, health care visits should be done remotely. [Dental services and preventive dental care](https://www.cdc.gov/coronavirus/2019-ncov/hcp/dental-settings.html) may be resumed. Contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) to see what services they are providing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C45" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1552,10 +1552,10 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>What about routine, elective, or non-urgent medical or dental appointments?</v>
+        <v>Can I get my prescriptions filled?</v>
       </c>
       <c r="B46" t="str">
-        <v>Preventive care services and non-emergency surgeries, like organ replacements and tumor removals, can take place if hospitals have enough capacity and protective equipment to do so safely. Eye exams, and elective procedures should be cancelled or rescheduled. If possible, health care visits should be done remotely. [Dental services and preventive dental care](https://www.cdc.gov/coronavirus/2019-ncov/hcp/dental-settings.html) may be resumed. Contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) to see what services they are providing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. You may leave your home to get prescriptions or cannabis from dispensaries with medical permits.\n\nYou can contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) to get a new prescription or adjust your existing prescriptions. \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C46" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1578,10 +1578,10 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>Can I get my prescriptions filled?</v>
+        <v>I am an older Californian who is isolating at home and I need non-urgent assistance. What can I do?</v>
       </c>
       <c r="B47" t="str">
-        <v>Yes. You may leave your home to get prescriptions or cannabis from dispensaries with medical permits.\n\nYou can contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) to get a new prescription or adjust your existing prescriptions. \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>You can call the statewide hotline for older Californians at [1-833-544-2374](tel:1-833-544-2374) for your non-urgent medical needs, to get meals delivered, to track down prescriptions, and more. The most important thing you can do is stay home for your health and wellbeing. If you are experiencing an emergency please call 911.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C47" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1604,10 +1604,10 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>I am an older Californian who is isolating at home and I need non-urgent assistance. What can I do?</v>
+        <v>How can I make sure the older Californians in my life are safe and healthy during the stay home order?</v>
       </c>
       <c r="B48" t="str">
-        <v>You can call the statewide hotline for older Californians at [1-833-544-2374](tel:1-833-544-2374) for your non-urgent medical needs, to get meals delivered, to track down prescriptions, and more. The most important thing you can do is stay home for your health and wellbeing. If you are experiencing an emergency please call 911.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>You should check in on your older neighbors and loved ones with a call, text, or physically-distanced door knock to make sure they are okay. You can also teach them how to use FaceTime, Zoom, Google Duo or Facebook video to communicate. The most important thing you can do is to keep in touch with older loved ones for their mental health and safety.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C48" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1630,10 +1630,10 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>How can I make sure the older Californians in my life are safe and healthy during the stay home order?</v>
+        <v>Can I leave home to care for my elderly parents or friends who require assistance? Or a friend or family member who has disabilities?</v>
       </c>
       <c r="B49" t="str">
-        <v>You should check in on your older neighbors and loved ones with a call, text, or physically-distanced door knock to make sure they are okay. You can also teach them how to use FaceTime, Zoom, Google Duo or Facebook video to communicate. The most important thing you can do is to keep in touch with older loved ones for their mental health and safety.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. Be sure that you protect them and yourself by following physical distancing guidelines such as wearing a mask, washing hands before and after, using hand sanitizer, maintaining at least six feet of distance when possible, and covering your cough or sneeze. If you have early signs of a cold, please stay away from your older loved ones.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)&lt;!-- disability, senior --&gt;</v>
       </c>
       <c r="C49" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1656,10 +1656,10 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>Can I leave home to care for my elderly parents or friends who require assistance? Or a friend or family member who has disabilities?</v>
+        <v>Can I visit loved ones in the hospital, nursing home, skilled nursing facility, or other residential care facility?</v>
       </c>
       <c r="B50" t="str">
-        <v>Yes. Be sure that you protect them and yourself by following physical distancing guidelines such as wearing a mask, washing hands before and after, using hand sanitizer, maintaining at least six feet of distance when possible, and covering your cough or sneeze. If you have early signs of a cold, please stay away from your older loved ones.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)&lt;!-- disability, senior --&gt;</v>
+        <v>Generally, no. There are limited exceptions, such as if you are going to the hospital with a minor who is under 18 or someone who is developmentally disabled and needs assistance. For most other situations, the order prohibits visitation to these kinds of facilities. This is difficult, but necessary to protect hospital staff and other patients. Check the [frequently asked questions for friends and family with a loved one in a skilled nursing or residential care facility](https://www.aging.ca.gov/download.ashx?lE0rcNUV0zaaXLD5JZ%2f6Uw%3d%3d) for more detailed information.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)&lt;!-- elderly, disability, senior --&gt;</v>
       </c>
       <c r="C50" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1682,10 +1682,10 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>Can I visit loved ones in the hospital, nursing home, skilled nursing facility, or other residential care facility?</v>
+        <v>Can a senior, disabled, uninsured or undocumented immigrant get free COVID-19 / Coronavirus test or treatment?</v>
       </c>
       <c r="B51" t="str">
-        <v>Generally, no. There are limited exceptions, such as if you are going to the hospital with a minor who is under 18 or someone who is developmentally disabled and needs assistance. For most other situations, the order prohibits visitation to these kinds of facilities. This is difficult, but necessary to protect hospital staff and other patients. Check the [frequently asked questions for friends and family with a loved one in a skilled nursing or residential care facility](https://www.aging.ca.gov/download.ashx?lE0rcNUV0zaaXLD5JZ%2f6Uw%3d%3d) for more detailed information.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)&lt;!-- elderly, disability, senior --&gt;</v>
+        <v>All patients with full-service Medi-Cal or commercial insurance in California will have copays, coinsurance and deductibles waived for COVID-19 [testing](https://covid19.ca.gov/testing-and-treatment/) and screening.  [Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) cover [coronavirus tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test) tests, with no out-of-pocket costs. The cost of coronavirus screening, testing, and treatment for the uninsured is paid for by the [government](https://www.hrsa.gov/CovidUninsuredClaim). \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C51" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1708,13 +1708,13 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>Can a senior, disabled, uninsured or undocumented immigrant get free COVID-19 / Coronavirus test or treatment?</v>
+        <v>What do taxpayers need to do if they want to take advantage of relief from the California Department of Tax and Fee Administration?</v>
       </c>
       <c r="B52" t="str">
-        <v>All patients with full-service Medi-Cal or commercial insurance in California will have copays, coinsurance and deductibles waived for COVID-19 [testing](https://covid19.ca.gov/testing-and-treatment/) and screening.  [Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) cover [coronavirus tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test) tests, with no out-of-pocket costs. The cost of coronavirus screening, testing, and treatment for the uninsured is paid for by the [government](https://www.hrsa.gov/CovidUninsuredClaim). \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Interested taxpayers should contact CDTFA by visiting the [CDTFA website](http://cdtfa.ca.gov/) or calling [800-400-7115](tel:800-400-7115).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C52" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D52" t="str">
         <v xml:space="preserve"> </v>
@@ -1734,10 +1734,10 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>What do taxpayers need to do if they want to take advantage of relief from the California Department of Tax and Fee Administration?</v>
+        <v>When will taxpayers start on these payment plans?</v>
       </c>
       <c r="B53" t="str">
-        <v>Interested taxpayers should contact CDTFA by visiting the [CDTFA website](http://cdtfa.ca.gov/) or calling [800-400-7115](tel:800-400-7115).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Given that the April deadline to file and pay sales and use tax returns has been extended to late July for all but the largest taxpayers, CDTFA expects that most participating taxpayers will begin their payment arrangements in late July of this year.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C53" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1760,10 +1760,10 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>When will taxpayers start on these payment plans?</v>
+        <v>How will the payment plans work?</v>
       </c>
       <c r="B54" t="str">
-        <v>Given that the April deadline to file and pay sales and use tax returns has been extended to late July for all but the largest taxpayers, CDTFA expects that most participating taxpayers will begin their payment arrangements in late July of this year.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Qualifying sales and use taxpayers with deferred liabilities up to $50,000 will pay their tax due in 12 equal monthly installments. No interest or penalties will be assessed against the liability.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C54" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1786,10 +1786,10 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>How will the payment plans work?</v>
+        <v>Is this only for tax payments due for the 1st quarter of 2020?</v>
       </c>
       <c r="B55" t="str">
-        <v>Qualifying sales and use taxpayers with deferred liabilities up to $50,000 will pay their tax due in 12 equal monthly installments. No interest or penalties will be assessed against the liability.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>If taxpayers choose to use this program to distribute the burden of their May or June prepayments or their July return, CDTFA will work to accommodate those taxpayers.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C55" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1812,10 +1812,10 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>Is this only for tax payments due for the 1st quarter of 2020?</v>
+        <v>What if taxpayers owe more than the $50,000 limit on the relief?</v>
       </c>
       <c r="B56" t="str">
-        <v>If taxpayers choose to use this program to distribute the burden of their May or June prepayments or their July return, CDTFA will work to accommodate those taxpayers.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The maximum amount that any taxpayer can defer interest-free under this relief effort is $50,000.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C56" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1838,10 +1838,10 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>What if taxpayers owe more than the $50,000 limit on the relief?</v>
+        <v>What if taxpayers with more than $5 million in annual taxable sales need this relief?</v>
       </c>
       <c r="B57" t="str">
-        <v>The maximum amount that any taxpayer can defer interest-free under this relief effort is $50,000.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>We recognize that some taxpayers, particularly in low margin businesses, with annual taxable sales over $5 million may also need this relief. Those taxpayers are encouraged to reach out to CDTFA, which will work with them to provide relief where appropriate.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C57" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1864,10 +1864,10 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>What if taxpayers with more than $5 million in annual taxable sales need this relief?</v>
+        <v>Is the deadline for filing California tax returns extended?</v>
       </c>
       <c r="B58" t="str">
-        <v>We recognize that some taxpayers, particularly in low margin businesses, with annual taxable sales over $5 million may also need this relief. Those taxpayers are encouraged to reach out to CDTFA, which will work with them to provide relief where appropriate.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Yes. All California taxpayers (individuals and businesses) can file and pay by July 15, 2020. See [information from the CA Franchise Tax Board](https://www.ftb.ca.gov/about-ftb/newsroom/news-releases/2020-3-state-postpones-tax-deadlines-until-july-15-due-to-the-covid-19-pandemic.html) for more information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C58" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1890,10 +1890,10 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>Is the deadline for filing California tax returns extended?</v>
+        <v>What is a loan guarantee?</v>
       </c>
       <c r="B59" t="str">
-        <v>Yes. All California taxpayers (individuals and businesses) can file and pay by July 15, 2020. See [information from the CA Franchise Tax Board](https://www.ftb.ca.gov/about-ftb/newsroom/news-releases/2020-3-state-postpones-tax-deadlines-until-july-15-due-to-the-covid-19-pandemic.html) for more information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>A loan guarantee is a credit enhancement that helps mitigate the risk assumed by a lending institution when making a loan. With the Small Business Finance Center’s Disaster Relief Loan Guarantee Program, IBank agrees to guarantee up to 95% of the loan, removing the barriers to capital that often exist for small business borrowers that may not otherwise be eligible for traditional lending. This program also can assist those who may not be eligible for a U.S. Small Business Administration (SBA) loan.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C59" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1916,10 +1916,10 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>What is a loan guarantee?</v>
+        <v>Who is eligible to apply?</v>
       </c>
       <c r="B60" t="str">
-        <v>A loan guarantee is a credit enhancement that helps mitigate the risk assumed by a lending institution when making a loan. With the Small Business Finance Center’s Disaster Relief Loan Guarantee Program, IBank agrees to guarantee up to 95% of the loan, removing the barriers to capital that often exist for small business borrowers that may not otherwise be eligible for traditional lending. This program also can assist those who may not be eligible for a U.S. Small Business Administration (SBA) loan.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Small business entities that have been affected by loss, damage or other economic injury due to the COVID-19 pandemic and meet the program’s eligibility requirements. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C60" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1942,10 +1942,10 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>Who is eligible to apply?</v>
+        <v>What do you consider a small business?</v>
       </c>
       <c r="B61" t="str">
-        <v>Small business entities that have been affected by loss, damage or other economic injury due to the COVID-19 pandemic and meet the program’s eligibility requirements. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The business must have between 1-750 employees and be established as an entity, including:\n\n*   Sole Proprietor – Individual using legal name as business name that files a Schedule C, Schedule F, or has a fictitious business name or DBA statement\n    *   If the loan appears to be in the name of an individual, evidence of Sole Proprietorship will be required and may include a Schedule C, Schedule F, Seller’s Permit, and/or fictitious business name or DBA statement\n*   Limited Liability Company \n*   Cooperative\n*   Corporation\n*   Partnership\n*   S-Corporation\n*   Not-for-profit\n\nThe program will not accept an _individual_ as the borrower. It is permissible for an individual to be a guarantor or co-borrower on the loan, but the primary borrower must be a small business. It does not consider citizenship or immigration status for eligibility requirements**,** as long as the entity/individual meets the above criteria. Trucking owners/operators are eligible as long as they are registered as a legal business entity.\n\n**AND**\n\n*   The business activity must be eligible under the program and in one of the industries listed in the [North American Industry Classification System (NAICS) codes list](http://www.census.gov/eos/www/naics), and\n*   It must be located in a declared disaster area. A major disaster area declaration was made for the state of California on March 22, 2020 in regards to the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C61" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1968,10 +1968,10 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>What do you consider a small business?</v>
+        <v>What are excluded businesses?</v>
       </c>
       <c r="B62" t="str">
-        <v>The business must have between 1-750 employees and be established as an entity, including:\n\n*   Sole Proprietor – Individual using legal name as business name that files a Schedule C, Schedule F, or has a fictitious business name or DBA statement\n    *   If the loan appears to be in the name of an individual, evidence of Sole Proprietorship will be required and may include a Schedule C, Schedule F, Seller’s Permit, and/or fictitious business name or DBA statement\n*   Limited Liability Company \n*   Cooperative\n*   Corporation\n*   Partnership\n*   S-Corporation\n*   Not-for-profit\n\nThe program will not accept an _individual_ as the borrower. It is permissible for an individual to be a guarantor or co-borrower on the loan, but the primary borrower must be a small business. It does not consider citizenship or immigration status for eligibility requirements**,** as long as the entity/individual meets the above criteria. Trucking owners/operators are eligible as long as they are registered as a legal business entity.\n\n**AND**\n\n*   The business activity must be eligible under the program and in one of the industries listed in the [North American Industry Classification System (NAICS) codes list](http://www.census.gov/eos/www/naics), and\n*   It must be located in a declared disaster area. A major disaster area declaration was made for the state of California on March 22, 2020 in regards to the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Businesses that are not eligible include passive real estate businesses (rental income, etc.).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C62" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1994,10 +1994,10 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>What are excluded businesses?</v>
+        <v>Can I apply for a loan guarantee only if I am ineligible for federal disaster fund financing, such as a SBA loan?</v>
       </c>
       <c r="B63" t="str">
-        <v>Businesses that are not eligible include passive real estate businesses (rental income, etc.).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Yes, this program is designed for those who do not qualify for federal programs. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C63" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2020,10 +2020,10 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>Can I apply for a loan guarantee only if I am ineligible for federal disaster fund financing, such as a SBA loan?</v>
+        <v>How much can I borrow?</v>
       </c>
       <c r="B64" t="str">
-        <v>Yes, this program is designed for those who do not qualify for federal programs. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The Small Business Finance Center’s Disaster Relief Loan Guarantee Program allows a maximum loan of $1.25 million and a maximum guarantee of $1 million. To serve as many California small businesses as possible, the COVID-19 disaster program is focused on serving small businesses, especially those in low-wealth and immigrant communities with needs from $500 to $50,000. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C64" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2046,10 +2046,10 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>How much can I borrow?</v>
+        <v>What are the loan terms?</v>
       </c>
       <c r="B65" t="str">
-        <v>The Small Business Finance Center’s Disaster Relief Loan Guarantee Program allows a maximum loan of $1.25 million and a maximum guarantee of $1 million. To serve as many California small businesses as possible, the COVID-19 disaster program is focused on serving small businesses, especially those in low-wealth and immigrant communities with needs from $500 to $50,000. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The length of the loan can be negotiated with your lender, but the guarantee is good for up to seven years. The interest rate and loan criteria will be determined by the lender and could depend on the credit strength of the business. The guarantee is designed to lower the interest rate in exchange for a higher guarantee to your lender. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C65" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2072,10 +2072,10 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>What are the loan terms?</v>
+        <v>How can I apply?</v>
       </c>
       <c r="B66" t="str">
-        <v>The length of the loan can be negotiated with your lender, but the guarantee is good for up to seven years. The interest rate and loan criteria will be determined by the lender and could depend on the credit strength of the business. The guarantee is designed to lower the interest rate in exchange for a higher guarantee to your lender. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The Small Business Finance Center partners with Community Development Financial Institutions (CDFIs), Community Lending Institutions, and Financial Development Corporations (FDCs) to provide loan guarantees for small businesses.  To apply,\n\n*   View the [list of FDCs and participating lenders](http://www.ibank.ca.gov/small-business-finance-center/) interested in this Small Business Disaster Relief Loan Guarantee Program. \n*   Contact the lender on the list nearest to your business to apply.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C66" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2098,10 +2098,10 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>How can I apply?</v>
+        <v>What is the timing for the funding of loans?</v>
       </c>
       <c r="B67" t="str">
-        <v>The Small Business Finance Center partners with Community Development Financial Institutions (CDFIs), Community Lending Institutions, and Financial Development Corporations (FDCs) to provide loan guarantees for small businesses.  To apply,\n\n*   View the [list of FDCs and participating lenders](http://www.ibank.ca.gov/small-business-finance-center/) interested in this Small Business Disaster Relief Loan Guarantee Program. \n*   Contact the lender on the list nearest to your business to apply.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The program is in place and businesses can apply immediately. Once you provide your lender with complete information, you could be funded in a matter of days.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C67" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2124,10 +2124,10 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>What is the timing for the funding of loans?</v>
+        <v>What can the money be used for?</v>
       </c>
       <c r="B68" t="str">
-        <v>The program is in place and businesses can apply immediately. Once you provide your lender with complete information, you could be funded in a matter of days.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The funds are meant to help small businesses through this challenging time. Loan proceeds can be used for business continuance or to cure “economic injury” as a result of COVID-19.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C68" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2150,10 +2150,10 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>What can the money be used for?</v>
+        <v>How will this program assist low-wealth and minority communities?</v>
       </c>
       <c r="B69" t="str">
-        <v>The funds are meant to help small businesses through this challenging time. Loan proceeds can be used for business continuance or to cure “economic injury” as a result of COVID-19.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>By working with the Community Development Financial Institutions (CDFIs) throughout the state of California, this disaster relief program can play an important role in generating economic growth and opportunity in some of our most distressed communities. CDFIs and mission-based lenders play a vital role across the state and have experience steering lending and investment to where it is needed and will matter the most, in particular in low-wealth and immigrant communities. CDFIs and our partner Financial Development Corporations (FDCs) that process the loan guarantees are embedded in communities across the state, speak several languages, and are invested in the community successfully managing its way through this pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C69" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2176,10 +2176,10 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>How will this program assist low-wealth and minority communities?</v>
+        <v>Are faith-based businesses eligible for this loan guarantee program?</v>
       </c>
       <c r="B70" t="str">
-        <v>By working with the Community Development Financial Institutions (CDFIs) throughout the state of California, this disaster relief program can play an important role in generating economic growth and opportunity in some of our most distressed communities. CDFIs and mission-based lenders play a vital role across the state and have experience steering lending and investment to where it is needed and will matter the most, in particular in low-wealth and immigrant communities. CDFIs and our partner Financial Development Corporations (FDCs) that process the loan guarantees are embedded in communities across the state, speak several languages, and are invested in the community successfully managing its way through this pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Faith-based businesses (non-profit or otherwise) that have business activity outside of worship are eligible as long as they are a legal business that has been affected by the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C70" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2202,10 +2202,10 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>Are faith-based businesses eligible for this loan guarantee program?</v>
+        <v>What SBA programs are available to small businesses right now?</v>
       </c>
       <c r="B71" t="str">
-        <v>Faith-based businesses (non-profit or otherwise) that have business activity outside of worship are eligible as long as they are a legal business that has been affected by the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The U.S. SBA offers the **Paycheck Protection Program (PPP)** and **Economic Injury Disaster Loan and Advance (EIDL and EIDL Advance)**.\n\nMore about **Paycheck Protection Program (PPP)**:\n\nThe SBA has resumed accepting PPP loan applications from approved lenders. The PPP is a loan program for small businesses, self-employed, independent contractors, nonprofits with a maximum of 500 employees, and it is intended to keep workers paid and employed. The loan amount is calculated based on payroll expenses with a maximum amount of $10 million at a rate of 1% for up to 2 years. The loan is forgivable if 75% of the loan amount is used for payroll, and no employees are laid off, or if laid-off employees are rehired before June 30, 2020. In addition to payroll costs, allowable expenses include mortgage interest, rent, and utilities. Submit your application as soon as possible, even if you need to rehire employees that have been laid off. Check the [Fact Sheet](https://home.treasury.gov/system/files/136/PPP--Fact-Sheet.pdf?mod=article_inline) and [Frequently Asked Questions](https://home.treasury.gov/system/files/136/Paycheck-Protection-Program-Frequently-Asked-Questions.pdf), and see [SBA.gov](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program#section-header-0) for more details. You must apply directly through a lender. [Find a PPP lender in your area](https://www.sba.gov/paycheckprotection/find) to contact right away.\n\nMore about **Economic Injury Disaster Loan and Advance (EIDL and EIDL Advance):**\n\nAs of June 15, the U.S. SBA is accepting new applications from all eligible businesses, and will continue to process **EIDL Loan and Advance applications** already submitted on a first come, first-served basis. Check the U.S. SBA’s [Disaster Loan Applications website](https://www.sba.gov/page/disaster-loan-applications#section-header-0) for more information.\n\nThe EIDL is a direct loan for up to $2 million at a rate of 3.75% for small businesses and 2.75% for nonprofits. Applicants can get an **Advance** of up to $10,000 upon request within days of a successful application. This advance doesn’t have to be repaid. [Apply directly with the SBA](https://covid19relief.sba.gov/#/). For questions, you can contact SBA’s Customer Service Line at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or send an email to [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C71" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2228,10 +2228,10 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>What SBA programs are available to small businesses right now?</v>
+        <v>Which banks are offering the Paycheck Protection Program forgivable loans?</v>
       </c>
       <c r="B72" t="str">
-        <v>The U.S. SBA offers the **Paycheck Protection Program (PPP)** and **Economic Injury Disaster Loan and Advance (EIDL and EIDL Advance)**.\n\nMore about **Paycheck Protection Program (PPP)**:\n\nThe SBA has resumed accepting PPP loan applications from approved lenders. The PPP is a loan program for small businesses, self-employed, independent contractors, nonprofits with a maximum of 500 employees, and it is intended to keep workers paid and employed. The loan amount is calculated based on payroll expenses with a maximum amount of $10 million at a rate of 1% for up to 2 years. The loan is forgivable if 75% of the loan amount is used for payroll, and no employees are laid off, or if laid-off employees are rehired before June 30, 2020. In addition to payroll costs, allowable expenses include mortgage interest, rent, and utilities. Submit your application as soon as possible, even if you need to rehire employees that have been laid off. Check the [Fact Sheet](https://home.treasury.gov/system/files/136/PPP--Fact-Sheet.pdf?mod=article_inline) and [Frequently Asked Questions](https://home.treasury.gov/system/files/136/Paycheck-Protection-Program-Frequently-Asked-Questions.pdf), and see [SBA.gov](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program#section-header-0) for more details. You must apply directly through a lender. [Find a PPP lender in your area](https://www.sba.gov/paycheckprotection/find) to contact right away.\n\nMore about **Economic Injury Disaster Loan and Advance (EIDL and EIDL Advance):**\n\nAs of June 15, the U.S. SBA is accepting new applications from all eligible businesses, and will continue to process **EIDL Loan and Advance applications** already submitted on a first come, first-served basis. Check the U.S. SBA’s [Disaster Loan Applications website](https://www.sba.gov/page/disaster-loan-applications#section-header-0) for more information.\n\nThe EIDL is a direct loan for up to $2 million at a rate of 3.75% for small businesses and 2.75% for nonprofits. Applicants can get an **Advance** of up to $10,000 upon request within days of a successful application. This advance doesn’t have to be repaid. [Apply directly with the SBA](https://covid19relief.sba.gov/#/). For questions, you can contact SBA’s Customer Service Line at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or send an email to [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Interested borrowers can contact any SBA participating bank, credit union, or nonprofit lenders to apply for the [PPP](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program). For more information, contact your local bank or reach out to [SBA’s local district offices](https://www.sba.gov/local-assistance/find/?type=SBA%20District%20Office&amp;pageNumber=1) for assistance.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C72" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2254,10 +2254,10 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>Which banks are offering the Paycheck Protection Program forgivable loans?</v>
+        <v>Where do I find more information on allowable expenses for a forgivable loan under the Paycheck Protection Program?</v>
       </c>
       <c r="B73" t="str">
-        <v>Interested borrowers can contact any SBA participating bank, credit union, or nonprofit lenders to apply for the [PPP](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program). For more information, contact your local bank or reach out to [SBA’s local district offices](https://www.sba.gov/local-assistance/find/?type=SBA%20District%20Office&amp;pageNumber=1) for assistance.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>You can find this on the Paycheck Protection Program’s Loan Forgiveness Application. The application provides detailed instructions on how to apply for forgiveness of PPP loans. Once your business has expended the PPP funds and is ready to pursue loan forgiveness, please review the [Loan Forgiveness Application](https://content.sba.gov/sites/default/files/2020-05/3245-0407%20SBA%20Form%203508%20PPP%20Forgiveness%20Application.pdf) and consult with your accountant, lender, or one of California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) for assistance.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C73" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2280,10 +2280,10 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>Where do I find more information on allowable expenses for a forgivable loan under the Paycheck Protection Program?</v>
+        <v>How does a business know if it is eligible for an SBA loan or loan guarantee program?</v>
       </c>
       <c r="B74" t="str">
-        <v>You can find this on the Paycheck Protection Program’s Loan Forgiveness Application. The application provides detailed instructions on how to apply for forgiveness of PPP loans. Once your business has expended the PPP funds and is ready to pursue loan forgiveness, please review the [Loan Forgiveness Application](https://content.sba.gov/sites/default/files/2020-05/3245-0407%20SBA%20Form%203508%20PPP%20Forgiveness%20Application.pdf) and consult with your accountant, lender, or one of California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) for assistance.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Small businesses with 500 employees or less are eligible to apply for the Paycheck Protection Program (PPP) and/or the Small Business Debt Relief Program. Small businesses are also eligible to apply for the Economic Injury Disaster Loan (EIDL) program and the EIDL Advance. Visit SBA’s comprehensive [COVID-19 support website](https://www.sba.gov/page/coronavirus-covid-19-small-business-guidance-loan-resources#section-header-4%20.) to find out more about SBA’s eligibility requirements for each program.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C74" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2306,10 +2306,10 @@
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>How does a business know if it is eligible for an SBA loan or loan guarantee program?</v>
+        <v>How do I reach SBA for any questions or assistance?</v>
       </c>
       <c r="B75" t="str">
-        <v>Small businesses with 500 employees or less are eligible to apply for the Paycheck Protection Program (PPP) and/or the Small Business Debt Relief Program. Small businesses are also eligible to apply for the Economic Injury Disaster Loan (EIDL) program and the EIDL Advance. Visit SBA’s comprehensive [COVID-19 support website](https://www.sba.gov/page/coronavirus-covid-19-small-business-guidance-loan-resources#section-header-4%20.) to find out more about SBA’s eligibility requirements for each program.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>SBA has district offices in California that are open to answer questions. You can use the [SBA’s Local Assistance Directory](https://www.sba.gov/local-assistance) to locate the office nearest you. You can also contact the SBA by phone at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or by email at [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).  \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C75" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2332,10 +2332,10 @@
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>How do I reach SBA for any questions or assistance?</v>
+        <v>How does a small business know which SBA loan or loan guarantee program is the right one? Can a small business apply to more than one?</v>
       </c>
       <c r="B76" t="str">
-        <v>SBA has district offices in California that are open to answer questions. You can use the [SBA’s Local Assistance Directory](https://www.sba.gov/local-assistance) to locate the office nearest you. You can also contact the SBA by phone at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or by email at [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).  \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Call or email the SBA to find out which program is right for you. While businesses can apply for and receive more than one form of capital assistance through the SBA, they cannot be used for the same purpose. The SBA can advise you on your options. Call [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or email [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C76" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2358,10 +2358,10 @@
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>How does a small business know which SBA loan or loan guarantee program is the right one? Can a small business apply to more than one?</v>
+        <v>How do I get SBA to cover my loan payments on my existing 7(a), 504, or microloan if I cannot pay due to COVID-19?</v>
       </c>
       <c r="B77" t="str">
-        <v>Call or email the SBA to find out which program is right for you. While businesses can apply for and receive more than one form of capital assistance through the SBA, they cannot be used for the same purpose. The SBA can advise you on your options. Call [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or email [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>SBA has a [Debt Relief program](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/sba-debt-relief) and will pay the principal and interest of existing SBA loans. Please contact your lender for information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C77" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2384,10 +2384,10 @@
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>How do I get SBA to cover my loan payments on my existing 7(a), 504, or microloan if I cannot pay due to COVID-19?</v>
+        <v>If I need help to figure out which program is best for me or to submit an application, where can I find support?</v>
       </c>
       <c r="B78" t="str">
-        <v>SBA has a [Debt Relief program](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/sba-debt-relief) and will pay the principal and interest of existing SBA loans. Please contact your lender for information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>California’s network of small business support centers can help you figure out which loans and programs are best for your business, develop resiliency strategies, and find other resources. Go to California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) to find the closest center.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C78" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2410,10 +2410,10 @@
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>If I need help to figure out which program is best for me or to submit an application, where can I find support?</v>
+        <v>How do I maintain a safe workplace?</v>
       </c>
       <c r="B79" t="str">
-        <v>California’s network of small business support centers can help you figure out which loans and programs are best for your business, develop resiliency strategies, and find other resources. Go to California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) to find the closest center.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>As California [reopens](https://covid19.ca.gov/roadmap/), every business will need to create a safer, low-risk environment. If you own or manage a business, follow the [industry-specific guidance](https://covid19.ca.gov/industry-guidance/) that applies to protect your workers and customers. If your county has received state approval to move further into the reopening [roadmap](https://covid19.ca.gov/roadmap/), you may find your industry guidance on the [County Variance](https://covid19.ca.gov/roadmap-counties/) page.\n\nIf your business is approved to reopen, you should take steps to ensure the safety and health of your workers. It’s important that employees with COVID-19 know they should stay home. Your sick leave policies need to support that. \n\n*   Encourage sick employees to stay home if they are sick. See government programs supporting [COVID-19 sick leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) and [workers’ compensation](https://www.labor.ca.gov/coronavirus2019/#chart).\n*   Establish routine cleaning throughout the workplace.\n*   Reduce travel. If possible, encourage video conferencing and limit larger gatherings.\n*   See [Cal/OSHA interim guidelines for general industry](https://www.dir.ca.gov/dosh/coronavirus/General-Industry.html).\n*   Follow [CDC guidance on keeping the workplace safe (PDF)](https://www.cdc.gov/coronavirus/2019-ncov/downloads/workplace-school-and-home-guidance.pdf).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C79" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2436,10 +2436,10 @@
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>How do I maintain a safe workplace?</v>
+        <v>What precautions should healthcare workers and organizations take?</v>
       </c>
       <c r="B80" t="str">
-        <v>As California [reopens](https://covid19.ca.gov/roadmap/), every business will need to create a safer, low-risk environment. If you own or manage a business, follow the [industry-specific guidance](https://covid19.ca.gov/industry-guidance/) that applies to protect your workers and customers. If your county has received state approval to move further into the reopening [roadmap](https://covid19.ca.gov/roadmap/), you may find your industry guidance on the [County Variance](https://covid19.ca.gov/roadmap-counties/) page.\n\nIf your business is approved to reopen, you should take steps to ensure the safety and health of your workers. It’s important that employees with COVID-19 know they should stay home. Your sick leave policies need to support that. \n\n*   Encourage sick employees to stay home if they are sick. See government programs supporting [COVID-19 sick leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) and [workers’ compensation](https://www.labor.ca.gov/coronavirus2019/#chart).\n*   Establish routine cleaning throughout the workplace.\n*   Reduce travel. If possible, encourage video conferencing and limit larger gatherings.\n*   See [Cal/OSHA interim guidelines for general industry](https://www.dir.ca.gov/dosh/coronavirus/General-Industry.html).\n*   Follow [CDC guidance on keeping the workplace safe (PDF)](https://www.cdc.gov/coronavirus/2019-ncov/downloads/workplace-school-and-home-guidance.pdf).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>See [Cal/OSHA’s guidance on protecting workers from coronavirus](https://www.dir.ca.gov/dosh/coronavirus/Health-Care-General-Industry.html).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C80" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2462,10 +2462,10 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>What precautions should healthcare workers and organizations take?</v>
+        <v>How can I avoid laying off employees if my business is impacted by COVID-19?</v>
       </c>
       <c r="B81" t="str">
-        <v>See [Cal/OSHA’s guidance on protecting workers from coronavirus](https://www.dir.ca.gov/dosh/coronavirus/Health-Care-General-Industry.html).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Apply for the [Unemployment Insurance (UI) Work Sharing Program](https://www.edd.ca.gov/Unemployment/Work_Sharing_Program.htm).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C81" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2488,13 +2488,13 @@
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>How can I avoid laying off employees if my business is impacted by COVID-19?</v>
+        <v>Is there financial help for student loans?</v>
       </c>
       <c r="B82" t="str">
-        <v>Apply for the [Unemployment Insurance (UI) Work Sharing Program](https://www.edd.ca.gov/Unemployment/Work_Sharing_Program.htm).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The [governor has ordered](https://www.gov.ca.gov/2020/04/23/governor-newsom-announces-additional-relief-for-californians-impacted-by-covid-19/) relief for students with federal loans. Check with your lender to see what options are available for you.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C82" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D82" t="str">
         <v xml:space="preserve"> </v>
@@ -2514,10 +2514,10 @@
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>Is there financial help for student loans?</v>
+        <v>My school provides free grab-and-go meals. Are those still available?</v>
       </c>
       <c r="B83" t="str">
-        <v>The [governor has ordered](https://www.gov.ca.gov/2020/04/23/governor-newsom-announces-additional-relief-for-californians-impacted-by-covid-19/) relief for students with federal loans. Check with your lender to see what options are available for you.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>Yes. It is essential to keep children fed. Check with your local school district for days and times meals are offered.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C83" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2540,10 +2540,10 @@
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>My school provides free grab-and-go meals. Are those still available?</v>
+        <v>What if I don’t have internet access at home?</v>
       </c>
       <c r="B84" t="str">
-        <v>Yes. It is essential to keep children fed. Check with your local school district for days and times meals are offered.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>Check with your local school district or college to see what resources are available for you.  List of providers offering free internet access currently:\n\n[Spectrum mobile](https://mobile.spectrum.com/support/article/360040980371/coronavirus-covid19-update)  has opened wifi hotspots and are working on assisting school districts with facilitating home internet access. \n\n[Comcast](https://corporate.comcast.com/covid-19) has opened free Xfinity WiFi hotspot access across the country. Xfinity has also paused data plans, late fees, and disconnects for the next 60 days. Families with limited income can receive internet services for free for the next 60 days (usually $9.95 per month). \n\n[AT&amp;T](https://about.att.com/pages/COVID-19.html)  has opened all public WiFi hotspots and will not charge customers for any late fees or overages. AT&amp;T also offers internet access for [$10/month for households on limited income](https://www.att.com/shop/internet/access/index.html?source=ECmj0000000000mbU&amp;wtExtndSource=access#!/#%2F).\n\n[Low-cost Internet access plans](https://www.cde.ca.gov/ls/he/hn/availableinternetplans.asp) are also available.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C84" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2566,10 +2566,10 @@
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>What if I don’t have internet access at home?</v>
+        <v>How will students with disabilities receive services during school closures?</v>
       </c>
       <c r="B85" t="str">
-        <v>Check with your local school district or college to see what resources are available for you.  List of providers offering free internet access currently:\n\n[Spectrum mobile](https://mobile.spectrum.com/support/article/360040980371/coronavirus-covid19-update)  has opened wifi hotspots and are working on assisting school districts with facilitating home internet access. \n\n[Comcast](https://corporate.comcast.com/covid-19) has opened free Xfinity WiFi hotspot access across the country. Xfinity has also paused data plans, late fees, and disconnects for the next 60 days. Families with limited income can receive internet services for free for the next 60 days (usually $9.95 per month). \n\n[AT&amp;T](https://about.att.com/pages/COVID-19.html)  has opened all public WiFi hotspots and will not charge customers for any late fees or overages. AT&amp;T also offers internet access for [$10/month for households on limited income](https://www.att.com/shop/internet/access/index.html?source=ECmj0000000000mbU&amp;wtExtndSource=access#!/#%2F).\n\n[Low-cost Internet access plans](https://www.cde.ca.gov/ls/he/hn/availableinternetplans.asp) are also available.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>The Department of Education has released [guidance on distance learning](https://www.cde.ca.gov/ls/he/hn/distancelearning.asp) to support schools. This guidance includes recommendations to ensure equity and access for all students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C85" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2592,10 +2592,10 @@
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>How will students with disabilities receive services during school closures?</v>
+        <v>Will there be standardized testing? When?</v>
       </c>
       <c r="B86" t="str">
-        <v>The Department of Education has released [guidance on distance learning](https://www.cde.ca.gov/ls/he/hn/distancelearning.asp) to support schools. This guidance includes recommendations to ensure equity and access for all students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>Probably not: on March 18, 2020, Governor Newsom issued an [executive order](https://www.gov.ca.gov/2020/03/18/governor-newsom-issues-executive-order-to-suspend-standardized-testing-for-students-in-response-to-covid-19-outbreak/)  to waive this year’s statewide testing for K-12 schools.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C86" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2618,13 +2618,13 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>Will there be standardized testing? When?</v>
+        <v>Am I allowed to work during the outbreak?</v>
       </c>
       <c r="B87" t="str">
-        <v>Probably not: on March 18, 2020, Governor Newsom issued an [executive order](https://www.gov.ca.gov/2020/03/18/governor-newsom-issues-executive-order-to-suspend-standardized-testing-for-students-in-response-to-covid-19-outbreak/)  to waive this year’s statewide testing for K-12 schools.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>It depends what your job is. Workers in [essential sectors (pdf)](https://covid19.ca.gov/img/EssentialCriticalInfrastructureWorkers.pdf) are allowed to work during the [stay home order](https://covid19.ca.gov/stay-home-except-for-essential-needs/#top). And anyone is allowed to work from their home that has arranged to do so with their employer.\n\nFor information on businesses and industry sectors that are allowed to move further into the reopening roadmap, visit [statewide industry guidance](https://covid19.ca.gov/industry-guidance/).\n\nSome businesses and industry sectors may be open in counties that have received state approval to move further into the reopening roadmap, but are not yet permitted to reopen statewide. Visit [county variance](https://covid19.ca.gov/roadmap-counties/) to learn more.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C87" t="str">
-        <v>https://covid19.ca.gov/education/</v>
+        <v>https://covid19.ca.gov/workers/</v>
       </c>
       <c r="D87" t="str">
         <v xml:space="preserve"> </v>
@@ -2644,10 +2644,10 @@
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>Am I allowed to work during the outbreak?</v>
+        <v>What can I do if my work hours are reduced because of COVID-19?</v>
       </c>
       <c r="B88" t="str">
-        <v>It depends what your job is. Workers in [essential sectors (pdf)](https://covid19.ca.gov/img/EssentialCriticalInfrastructureWorkers.pdf) are allowed to work during the [stay home order](https://covid19.ca.gov/stay-home-except-for-essential-needs/#top). And anyone is allowed to work from their home that has arranged to do so with their employer.\n\nFor information on businesses and industry sectors that are allowed to move further into the reopening roadmap, visit [statewide industry guidance](https://covid19.ca.gov/industry-guidance/).\n\nSome businesses and industry sectors may be open in counties that have received state approval to move further into the reopening roadmap, but are not yet permitted to reopen statewide. Visit [county variance](https://covid19.ca.gov/roadmap-counties/) to learn more.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C88" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2670,10 +2670,10 @@
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>What can I do if my work hours are reduced because of COVID-19?</v>
+        <v>Do I need a note or certificate from a medical provider to file for unemployment?</v>
       </c>
       <c r="B89" t="str">
-        <v>You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>No, a medical certificate is not required.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C89" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2696,10 +2696,10 @@
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>Do I need a note or certificate from a medical provider to file for unemployment?</v>
+        <v>How long will it take to process a claim for unemployment or insurance benefits and to receive a payment?</v>
       </c>
       <c r="B90" t="str">
-        <v>No, a medical certificate is not required.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>After your claim is submitted, it will take at least three weeks to be processed. It may take longer if your information doesn’t match wage records or your identity can’t be verified. \n\nThe Governor has [waived the one-week waiting period](https://www.gov.ca.gov/2020/03/12/governor-newsom-issues-new-executive-order-further-enhancing-state-and-local-governments-ability-to-respond-to-covid-19-pandemic/). This means you can collect benefits for the first week that you were out of work or had reduced hours.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C90" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2722,10 +2722,10 @@
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>How long will it take to process a claim for unemployment or insurance benefits and to receive a payment?</v>
+        <v>What can I do if I miss work because of school closures?</v>
       </c>
       <c r="B91" t="str">
-        <v>After your claim is submitted, it will take at least three weeks to be processed. It may take longer if your information doesn’t match wage records or your identity can’t be verified. \n\nThe Governor has [waived the one-week waiting period](https://www.gov.ca.gov/2020/03/12/governor-newsom-issues-new-executive-order-further-enhancing-state-and-local-governments-ability-to-respond-to-covid-19-pandemic/). This means you can collect benefits for the first week that you were out of work or had reduced hours.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>*   You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n*   Other options may be available. See [Benefits for Workers Impacted by COVID-19](https://www.labor.ca.gov/coronavirus2019/#chart).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C91" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2748,10 +2748,10 @@
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>What can I do if I miss work because of school closures?</v>
+        <v>What if I can’t work because I’m taking care of someone who’s sick or quarantined?</v>
       </c>
       <c r="B92" t="str">
-        <v>*   You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n*   Other options may be available. See [Benefits for Workers Impacted by COVID-19](https://www.labor.ca.gov/coronavirus2019/#chart).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>*   You may use [paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). The Labor and Workforce Development Agency has created a [chart detailing the available paid sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law. \n*   You can [file a Paid Family Leave (PFL) claim](https://www.edd.ca.gov/Disability/How_to_File_a_PFL_Claim_in_SDI_Online.htm).\n*   Unpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C92" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2774,10 +2774,10 @@
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>What if I can’t work because I’m taking care of someone who’s sick or quarantined?</v>
+        <v>What can I do if I can’t work because I’m sick or quarantined because of COVID-19?</v>
       </c>
       <c r="B93" t="str">
-        <v>*   You may use [paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). The Labor and Workforce Development Agency has created a [chart detailing the available paid sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law. \n*   You can [file a Paid Family Leave (PFL) claim](https://www.edd.ca.gov/Disability/How_to_File_a_PFL_Claim_in_SDI_Online.htm).\n*   Unpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>*   You may be able to use [paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). The Labor and Workforce Development Agency has created a [chart detailing the available paid sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law.\n*   If you’re unable to work due to having or being exposed to COVID-19, you can [file a Disability Insurance (DI) claim](https://www.edd.ca.gov/Disability/How_to_File_a_DI_Claim_in_SDI_Online.htm).\n*   You may also file a [Workers’ Compensation Claim](https://www.dir.ca.gov/dwc/FileAClaim.htm) if you suffered a COVID-19 illness that arose from an exposure during the course of your work. Check the California Department of Industrial Relations’ [COVID-19 Resources and Workers’ Compensation](https://www.dir.ca.gov/dwc/Covid-19/Index.html) for more information.\n*   Unpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C93" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2800,10 +2800,10 @@
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>What can I do if I can’t work because I’m sick or quarantined because of COVID-19?</v>
+        <v>What if I don’t have any available sick leave to use?</v>
       </c>
       <c r="B94" t="str">
-        <v>*   You may be able to use [paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). The Labor and Workforce Development Agency has created a [chart detailing the available paid sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law.\n*   If you’re unable to work due to having or being exposed to COVID-19, you can [file a Disability Insurance (DI) claim](https://www.edd.ca.gov/Disability/How_to_File_a_DI_Claim_in_SDI_Online.htm).\n*   You may also file a [Workers’ Compensation Claim](https://www.dir.ca.gov/dwc/FileAClaim.htm) if you suffered a COVID-19 illness that arose from an exposure during the course of your work. Check the California Department of Industrial Relations’ [COVID-19 Resources and Workers’ Compensation](https://www.dir.ca.gov/dwc/Covid-19/Index.html) for more information.\n*   Unpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>Check the Labor and Workforce Development Agency’s [chart detailing the available sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law.\n\nUnpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C94" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2826,13 +2826,13 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>What if I don’t have any available sick leave to use?</v>
+        <v>What effect will this have on my credit report?</v>
       </c>
       <c r="B95" t="str">
-        <v>Check the Labor and Workforce Development Agency’s [chart detailing the available sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law.\n\nUnpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>Financial institutions will not report derogatory information (like late payments) to credit reporting agencies but may report a forbearance. Typically this does not negatively affect a credit score on its own.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C95" t="str">
-        <v>https://covid19.ca.gov/workers/</v>
+        <v>https://covid19.ca.gov/get-financial-help/</v>
       </c>
       <c r="D95" t="str">
         <v xml:space="preserve"> </v>
@@ -2852,10 +2852,10 @@
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>What effect will this have on my credit report?</v>
+        <v>How long will these programs last?</v>
       </c>
       <c r="B96" t="str">
-        <v>Financial institutions will not report derogatory information (like late payments) to credit reporting agencies but may report a forbearance. Typically this does not negatively affect a credit score on its own.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>It is still unclear how severe or how long the COVID-19 impact will be. Financial institutions have committed to necessary relief and will be assessing the ongoing conditions and need for continuing relief.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C96" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -2878,10 +2878,10 @@
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>How long will these programs last?</v>
+        <v>What if my financial institution isn’t offering this relief?</v>
       </c>
       <c r="B97" t="str">
-        <v>It is still unclear how severe or how long the COVID-19 impact will be. Financial institutions have committed to necessary relief and will be assessing the ongoing conditions and need for continuing relief.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>Call or check their website to be sure. At this time, JP Morgan Chase, US Bank, Wells Fargo and Citigroup, [and nearly 200 state-chartered banks](https://dbo.ca.gov/covid19-updates-fi/), credit unions are supporting these commitments. \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C97" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -2904,10 +2904,10 @@
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>What if my financial institution isn’t offering this relief?</v>
+        <v>What if I already made a payment or was hit with a fee because of COVID-19?</v>
       </c>
       <c r="B98" t="str">
-        <v>Call or check their website to be sure. At this time, JP Morgan Chase, US Bank, Wells Fargo and Citigroup, [and nearly 200 state-chartered banks](https://dbo.ca.gov/covid19-updates-fi/), credit unions are supporting these commitments. \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>Talk to your financial institution. These measures go into effect as of March 25, 2020.  \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C98" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -2930,10 +2930,10 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>What if I already made a payment or was hit with a fee because of COVID-19?</v>
+        <v>Is mortgage relief available to businesses?</v>
       </c>
       <c r="B99" t="str">
-        <v>Talk to your financial institution. These measures go into effect as of March 25, 2020.  \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>The relief is currently only available for residential mortgages.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C99" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -2956,10 +2956,10 @@
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>Is mortgage relief available to businesses?</v>
+        <v>What if my mortgage servicer is not communicative or cooperative?</v>
       </c>
       <c r="B100" t="str">
-        <v>The relief is currently only available for residential mortgages.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>You can file a complaint with the Department of Business Oversight:\n\n*   File on their [website](https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fdbo.ca.gov%2Ffile-a-complaint%2F&amp;data=02%7C01%7CManuel.Alvarez%40dbo.ca.gov%7Ce2673837ec6f42fce84508d7d114ed59%7Cd6910b1745b44b7bbb66cb7936fabafe%7C1%7C0%7C637207760136603083&amp;sdata=VR6CdqCvrBGkfC%2Bm%2B6Yj9emco9ldVY5BLWSiLpe3f4c%3D&amp;reserved=0)\n*    Call their Consumer Services Office at [(866) 275-2677](tel:(866) 275-2677) or [(916) 327-7585](tel:(916) 327-7585) \n*   Or email Ask.DBO@dbo.ca.gov\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C100" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -2982,10 +2982,10 @@
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>What if my mortgage servicer is not communicative or cooperative?</v>
+        <v>Can I get child care during the stay home order?</v>
       </c>
       <c r="B101" t="str">
-        <v>You can file a complaint with the Department of Business Oversight:\n\n*   File on their [website](https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fdbo.ca.gov%2Ffile-a-complaint%2F&amp;data=02%7C01%7CManuel.Alvarez%40dbo.ca.gov%7Ce2673837ec6f42fce84508d7d114ed59%7Cd6910b1745b44b7bbb66cb7936fabafe%7C1%7C0%7C637207760136603083&amp;sdata=VR6CdqCvrBGkfC%2Bm%2B6Yj9emco9ldVY5BLWSiLpe3f4c%3D&amp;reserved=0)\n*    Call their Consumer Services Office at [(866) 275-2677](tel:(866) 275-2677) or [(916) 327-7585](tel:(916) 327-7585) \n*   Or email Ask.DBO@dbo.ca.gov\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>[Child care options](https://covid19.ca.gov/childcare/) are available if you work at an [essential job](https://covid19.ca.gov/essential-workforce/) or a permitted job in the [current roadmap stage](https://covid19.ca.gov/roadmap/). If you are not working at a job like this, it is important to keep children at home. \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C101" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -3008,13 +3008,13 @@
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>Can I get child care during the stay home order?</v>
+        <v>I am homeless and I may have come in contact with coronavirus. How can I self-isolate with nowhere to go and services closing down?</v>
       </c>
       <c r="B102" t="str">
-        <v>[Child care options](https://covid19.ca.gov/childcare/) are available if you work at an [essential job](https://covid19.ca.gov/essential-workforce/) or a permitted job in the [current roadmap stage](https://covid19.ca.gov/roadmap/). If you are not working at a job like this, it is important to keep children at home. \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>A motel or hotel room may be available for you and your family. Contact your local homeless [continuum of care](https://www.bcsh.ca.gov/hcfc/documents/coc_poc.pdf) to connect you to this service.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C102" t="str">
-        <v>https://covid19.ca.gov/get-financial-help/</v>
+        <v>https://covid19.ca.gov/housing-and-homelessness/</v>
       </c>
       <c r="D102" t="str">
         <v xml:space="preserve"> </v>
@@ -3034,10 +3034,10 @@
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>I am homeless and I may have come in contact with coronavirus. How can I self-isolate with nowhere to go and services closing down?</v>
+        <v>Will there be a rent freeze or waiver for renters? Are evictions allowed during the stay at home order?</v>
       </c>
       <c r="B103" t="str">
-        <v>A motel or hotel room may be available for you and your family. Contact your local homeless [continuum of care](https://www.bcsh.ca.gov/hcfc/documents/coc_poc.pdf) to connect you to this service.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>There is an [order](https://www.gov.ca.gov/2020/03/16/governor-newsom-issues-executive-order-to-protect-renters-and-homeowners-during-covid-19-pandemic/) in place to halt evictions and protect renters. If you are financially affected by COVID-19 and [can’t pay your full rent](https://bcsh.ca.gov/coronavirus19/graphic_rent.pdf), let your landlord know in writing within seven days of the rent due date. Save documentation as proof. The order does not relieve you from the obligation to pay rent. It also does not restrict the landlord from recovering rent that is due.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C103" t="str">
         <v>https://covid19.ca.gov/housing-and-homelessness/</v>
@@ -3060,10 +3060,10 @@
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>Will there be a rent freeze or waiver for renters? Are evictions allowed during the stay at home order?</v>
+        <v>Can landlords delay their payments while their tenants cannot pay rent?</v>
       </c>
       <c r="B104" t="str">
-        <v>There is an [order](https://www.gov.ca.gov/2020/03/16/governor-newsom-issues-executive-order-to-protect-renters-and-homeowners-during-covid-19-pandemic/) in place to halt evictions and protect renters. If you are financially affected by COVID-19 and [can’t pay your full rent](https://bcsh.ca.gov/coronavirus19/graphic_rent.pdf), let your landlord know in writing within seven days of the rent due date. Save documentation as proof. The order does not relieve you from the obligation to pay rent. It also does not restrict the landlord from recovering rent that is due.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>Yes, there are protections in effect through July 28, 2020 for landlords. The [order](https://www.gov.ca.gov/2020/03/16/governor-newsom-issues-executive-order-to-protect-renters-and-homeowners-during-covid-19-pandemic/) requests lenders to halt foreclosures and related evictions during this time. Property owners should contact their financial institutions.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C104" t="str">
         <v>https://covid19.ca.gov/housing-and-homelessness/</v>
@@ -3086,10 +3086,10 @@
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>Can landlords delay their payments while their tenants cannot pay rent?</v>
+        <v>How do I get mortgage relief and/or forbearance?</v>
       </c>
       <c r="B105" t="str">
-        <v>Yes, there are protections in effect through July 28, 2020 for landlords. The [order](https://www.gov.ca.gov/2020/03/16/governor-newsom-issues-executive-order-to-protect-renters-and-homeowners-during-covid-19-pandemic/) requests lenders to halt foreclosures and related evictions during this time. Property owners should contact their financial institutions.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>You should contact and work directly with your mortgage servicer to learn about and apply for available relief. Please note that financial institutions and their servicers are experiencing high volumes of inquiries.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C105" t="str">
         <v>https://covid19.ca.gov/housing-and-homelessness/</v>
@@ -3112,10 +3112,10 @@
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>How do I get mortgage relief and/or forbearance?</v>
+        <v>How long will the forbearance last?</v>
       </c>
       <c r="B106" t="str">
-        <v>You should contact and work directly with your mortgage servicer to learn about and apply for available relief. Please note that financial institutions and their servicers are experiencing high volumes of inquiries.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>The terms of a forbearance will be agreed to between you and your mortgage service. Financial institutions will confirm approval of and terms of the forbearance program.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C106" t="str">
         <v>https://covid19.ca.gov/housing-and-homelessness/</v>
@@ -3138,13 +3138,13 @@
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>How long will the forbearance last?</v>
+        <v>What if a provider says they have availability on MyChildCare.ca.gov but when I connect with them they have no space?</v>
       </c>
       <c r="B107" t="str">
-        <v>The terms of a forbearance will be agreed to between you and your mortgage service. Financial institutions will confirm approval of and terms of the forbearance program.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>The information on [MyChildCare.ca.gov](http://mychildcare.ca.gov/) will be updated twice each week but it is possible that vacancies are filled between updates. Contact your [local childcare resource and referral agency](http://rrnetwork.org/family-services/find-child-care) to find more vacancies. \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
       </c>
       <c r="C107" t="str">
-        <v>https://covid19.ca.gov/housing-and-homelessness/</v>
+        <v>https://covid19.ca.gov/childcare/</v>
       </c>
       <c r="D107" t="str">
         <v xml:space="preserve"> </v>
@@ -3164,10 +3164,10 @@
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>What if a provider says they have availability on MyChildCare.ca.gov but when I connect with them they have no space?</v>
+        <v>How can I find out more about the provider listed in MyChildCare.ca.gov?</v>
       </c>
       <c r="B108" t="str">
-        <v>The information on [MyChildCare.ca.gov](http://mychildcare.ca.gov/) will be updated twice each week but it is possible that vacancies are filled between updates. Contact your [local childcare resource and referral agency](http://rrnetwork.org/family-services/find-child-care) to find more vacancies. \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
+        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) includes each provider’s facility/license number. This number can be searched at [CDSS Community Care Licensing Database](https://www.ccld.dss.ca.gov/carefacilitysearch/) to find more information about the provider, like information on inspections and complaints.  \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
       </c>
       <c r="C108" t="str">
         <v>https://covid19.ca.gov/childcare/</v>
@@ -3190,10 +3190,10 @@
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>How can I find out more about the provider listed in MyChildCare.ca.gov?</v>
+        <v>How can I find help paying for childcare?</v>
       </c>
       <c r="B109" t="str">
-        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) includes each provider’s facility/license number. This number can be searched at [CDSS Community Care Licensing Database](https://www.ccld.dss.ca.gov/carefacilitysearch/) to find more information about the provider, like information on inspections and complaints.  \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
+        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) provides information on all licensed center-based and family childcare homes. This includes both private-pay and subsidized childcare. Children of essential workers are now eligible to enroll in subsidized emergency childcare through June 30, 2020. This is subject to capacity and eligibility requirements. Your [local childcare resource and referral agency](https://rrnetwork.org/index.php?p=family-services/find-child-care) can answer more questions about childcare subsidies.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
       </c>
       <c r="C109" t="str">
         <v>https://covid19.ca.gov/childcare/</v>
@@ -3216,10 +3216,10 @@
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>How can I find help paying for childcare?</v>
+        <v>Can I get childcare during the stay home order?</v>
       </c>
       <c r="B110" t="str">
-        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) provides information on all licensed center-based and family childcare homes. This includes both private-pay and subsidized childcare. Children of essential workers are now eligible to enroll in subsidized emergency childcare through June 30, 2020. This is subject to capacity and eligibility requirements. Your [local childcare resource and referral agency](https://rrnetwork.org/index.php?p=family-services/find-child-care) can answer more questions about childcare subsidies.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
+        <v>Yes, all childcare facilities can open with necessary modifications.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
       </c>
       <c r="C110" t="str">
         <v>https://covid19.ca.gov/childcare/</v>
@@ -3242,10 +3242,10 @@
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>Can I get childcare during the stay home order?</v>
+        <v>Can my babysitter still come to the house?</v>
       </c>
       <c r="B111" t="str">
-        <v>Yes, all childcare facilities can open with necessary modifications.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
+        <v>Yes, a childcare worker can come to your home if necessary and should practice basic prevention guidelines (like handwashing for at least 20 seconds, physical distancing, and staying home if feeling ill).\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
       </c>
       <c r="C111" t="str">
         <v>https://covid19.ca.gov/childcare/</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>Can my babysitter still come to the house?</v>
+        <v>Counties:</v>
       </c>
       <c r="B112" t="str">
-        <v>Yes, a childcare worker can come to your home if necessary and should practice basic prevention guidelines (like handwashing for at least 20 seconds, physical distancing, and staying home if feeling ill).\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
+        <v>*   [Alameda County](http://www.acphd.org/2019-ncov.aspx)\n*   [Alpine County](http://alpinecountyca.gov/Index.aspx?NID=516)\n*   [Amador County](https://www.amadorgov.org/services/covid-19)\n*   [Butte County](https://www.buttecounty.net/publichealth)\n*   [Calaveras County](https://covid19.calaverasgov.us/)\n*   [Colusa County](https://www.countyofcolusa.org/99/Public-Health)\n*   [Contra Costa County](https://www.coronavirus.cchealth.org/)\n*   [Del Norte County](http://www.co.del-norte.ca.us/departments/health-human-services/public-health)\n*   [El Dorado County](https://www.edcgov.us/Government/hhsa/Pages/EDCCOVID-19.aspx)\n*   [Fresno County](https://www.co.fresno.ca.us/departments/public-health/covid-19)\n*   [Glenn County](https://www.countyofglenn.net/dept/health-human-services/public-health/covid-19)\n*   [Humboldt County](https://humboldtgov.org/2018/Humboldt-Health-Alert)\n*   [Imperial County](http://www.icphd.org/health-information-and-resources/healthy-facts/covid-19/)\n*   [Inyo County](https://www.inyocounty.us/coronavirus-covid-19-response)\n*   [Kern County](https://kernpublichealth.com/2019-novel-coronavirus/)\n*   [Kings County](https://www.countyofkings.com/departments/health-welfare/public-health/coronavirus-disease-2019-covid-19/-fsiteid-1)\n*   [Lake County](http://health.co.lake.ca.us/Coronavirus.htm)\n*   [Lassen County](http://www.co.lassen.ca.us/)\n*   [Los Angeles County](http://publichealth.lacounty.gov/media/Coronavirus/)\n*   [Madera County](https://www.maderacounty.com/government/public-health/health-updates/corona-virus)\n*   [Marin County](https://coronavirus.marinhhs.org/)\n*   [Mariposa County](http://www.mariposacounty.org/1592/COVID-19-Information)\n*   [Mendocino County](https://www.mendocinocounty.org/community/novel-coronavirus)\n*   [Merced County](https://www.co.merced.ca.us/3350/Coronavirus-Disease-2019)\n*   [Modoc County](http://www.co.modoc.ca.us/)\n*   [Mono County](https://coronavirus.monocounty.ca.gov/)\n*   [Monterey County](https://www.co.monterey.ca.us/government/departments-a-h/health/diseases/2019-novel-coronavirus-covid-19)\n*   [Napa County](https://www.countyofnapa.org/2739/Coronavirus)\n*   [Nevada County](https://www.mynevadacounty.com/2924/Coronavirus)\n*   [Orange County](https://www.ochealthinfo.com/phs/about/epidasmt/epi/dip/prevention/novel_coronavirus)\n*   [Placer County](https://www.placer.ca.gov/coronavirus)\n*   [Plumas County](https://www.plumascounty.us/2669/Novel-Coronavirus-2019-COVID-19)\n*   [Riverside County](https://www.rivcoph.org/coronavirus)\n*   [Sacramento County](https://dhs.saccounty.net/PUB/Pages/PUB-Home.aspx)\n*   [San Benito County](https://hhsa.cosb.us/publichealth/communicable-disease/coronavirus/)\n*   [San Bernardino County](http://wp.sbcounty.gov/dph/coronavirus/)\n*   [San Diego County](https://www.sandiegocounty.gov/coronavirus.html)\n*   [San Francisco City and County](https://sf.gov/topics/coronavirus-covid-19)\n*   [San Joaquin County](https://www.sjgov.org/covid19/)\n*   [San Luis Obispo County](https://www.emergencyslo.org/en/covid19.aspx)\n*   [San Mateo County](https://www.smchealth.org/coronavirus)\n*   [Santa Barbara County](https://publichealthsbc.org/)\n*   [Santa Clara County](https://www.sccgov.org/sites/phd/DiseaseInformation/novel-coronavirus/Pages/home.aspx)\n*   [Santa Cruz County](https://www.santacruzhealth.org/HSAHome/HSADivisions/PublicHealth/CommunicableDiseaseControl/Coronavirus.aspx)\n*   [Shasta County](https://www.co.shasta.ca.us/index/hhsa/health-safety/current-heath-concerns/coronavirus)\n*   [Sierra County](http://sierracounty.ca.gov/582/Coronavirus-COVID-19)\n*   [Siskiyou County](https://www.co.siskiyou.ca.us/publichealth/page/coronavirus-covid-19-what-siskiyou-county-residents-need-know)\n*   [Solano County](http://www.solanocounty.com/depts/ph/ncov.asp)\n*   [Sonoma County](https://socoemergency.org/emergency/novel-coronavirus/)\n*   [Stanislaus County](http://schsa.org/publichealth/pages/corona-virus/)\n*   [Sutter County](https://www.suttercounty.org/doc/government/depts/cao/em/coronavirus)\n*   [Tehama County](https://www.tehamacohealthservices.net/services/communicable-diseases/#current-events)\n*   [Trinity County](https://www.trinitycounty.org/)\n*   [Tulare County](https://tchhsa.org/eng/index.cfm/public-health/covid-19-updates-novel-coronavirus/)\n*   [Tuolumne County](https://www.tuolumnecounty.ca.gov/250/Public-Health)\n*   [Ventura County](https://www.vcemergency.com/)\n*   [Yolo County](https://www.yolocounty.org/health-human-services/adults/communicable-disease-investigation-and-control/novel-coronavirus-2019)\n*   [Yuba County](https://www.yuba.org/coronavirus/)\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C112" t="str">
-        <v>https://covid19.ca.gov/childcare/</v>
+        <v>https://covid19.ca.gov/state-local-resources/</v>
       </c>
       <c r="D112" t="str">
         <v xml:space="preserve"> </v>
@@ -3294,10 +3294,10 @@
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>Counties:</v>
+        <v>What are the restrictions in my area?</v>
       </c>
       <c r="B113" t="str">
-        <v>*   [Alameda County](http://www.acphd.org/2019-ncov.aspx)\n*   [Alpine County](http://alpinecountyca.gov/Index.aspx?NID=516)\n*   [Amador County](https://www.amadorgov.org/services/covid-19)\n*   [Butte County](https://www.buttecounty.net/publichealth)\n*   [Calaveras County](https://covid19.calaverasgov.us/)\n*   [Colusa County](https://www.countyofcolusa.org/99/Public-Health)\n*   [Contra Costa County](https://www.coronavirus.cchealth.org/)\n*   [Del Norte County](http://www.co.del-norte.ca.us/departments/health-human-services/public-health)\n*   [El Dorado County](https://www.edcgov.us/Government/hhsa/Pages/EDCCOVID-19.aspx)\n*   [Fresno County](https://www.co.fresno.ca.us/departments/public-health/covid-19)\n*   [Glenn County](https://www.countyofglenn.net/dept/health-human-services/public-health/covid-19)\n*   [Humboldt County](https://humboldtgov.org/2018/Humboldt-Health-Alert)\n*   [Imperial County](http://www.icphd.org/health-information-and-resources/healthy-facts/covid-19/)\n*   [Inyo County](https://www.inyocounty.us/coronavirus-covid-19-response)\n*   [Kern County](https://kernpublichealth.com/2019-novel-coronavirus/)\n*   [Kings County](https://www.countyofkings.com/departments/health-welfare/public-health/coronavirus-disease-2019-covid-19/-fsiteid-1)\n*   [Lake County](http://health.co.lake.ca.us/Coronavirus.htm)\n*   [Lassen County](http://www.co.lassen.ca.us/)\n*   [Los Angeles County](http://publichealth.lacounty.gov/media/Coronavirus/)\n*   [Madera County](https://www.maderacounty.com/government/public-health/health-updates/corona-virus)\n*   [Marin County](https://coronavirus.marinhhs.org/)\n*   [Mariposa County](http://www.mariposacounty.org/1592/COVID-19-Information)\n*   [Mendocino County](https://www.mendocinocounty.org/community/novel-coronavirus)\n*   [Merced County](https://www.co.merced.ca.us/3350/Coronavirus-Disease-2019)\n*   [Modoc County](http://www.co.modoc.ca.us/)\n*   [Mono County](https://coronavirus.monocounty.ca.gov/)\n*   [Monterey County](https://www.co.monterey.ca.us/government/departments-a-h/health/diseases/2019-novel-coronavirus-covid-19)\n*   [Napa County](https://www.countyofnapa.org/2739/Coronavirus)\n*   [Nevada County](https://www.mynevadacounty.com/2924/Coronavirus)\n*   [Orange County](https://www.ochealthinfo.com/phs/about/epidasmt/epi/dip/prevention/novel_coronavirus)\n*   [Placer County](https://www.placer.ca.gov/coronavirus)\n*   [Plumas County](https://www.plumascounty.us/2669/Novel-Coronavirus-2019-COVID-19)\n*   [Riverside County](https://www.rivcoph.org/coronavirus)\n*   [Sacramento County](https://dhs.saccounty.net/PUB/Pages/PUB-Home.aspx)\n*   [San Benito County](https://hhsa.cosb.us/publichealth/communicable-disease/coronavirus/)\n*   [San Bernardino County](http://wp.sbcounty.gov/dph/coronavirus/)\n*   [San Diego County](https://www.sandiegocounty.gov/coronavirus.html)\n*   [San Francisco City and County](https://sf.gov/topics/coronavirus-covid-19)\n*   [San Joaquin County](https://www.sjgov.org/covid19/)\n*   [San Luis Obispo County](https://www.emergencyslo.org/en/covid19.aspx)\n*   [San Mateo County](https://www.smchealth.org/coronavirus)\n*   [Santa Barbara County](https://publichealthsbc.org/)\n*   [Santa Clara County](https://www.sccgov.org/sites/phd/DiseaseInformation/novel-coronavirus/Pages/home.aspx)\n*   [Santa Cruz County](https://www.santacruzhealth.org/HSAHome/HSADivisions/PublicHealth/CommunicableDiseaseControl/Coronavirus.aspx)\n*   [Shasta County](https://www.co.shasta.ca.us/index/hhsa/health-safety/current-heath-concerns/coronavirus)\n*   [Sierra County](http://sierracounty.ca.gov/582/Coronavirus-COVID-19)\n*   [Siskiyou County](https://www.co.siskiyou.ca.us/publichealth/page/coronavirus-covid-19-what-siskiyou-county-residents-need-know)\n*   [Solano County](http://www.solanocounty.com/depts/ph/ncov.asp)\n*   [Sonoma County](https://socoemergency.org/emergency/novel-coronavirus/)\n*   [Stanislaus County](http://schsa.org/publichealth/pages/corona-virus/)\n*   [Sutter County](https://www.suttercounty.org/doc/government/depts/cao/em/coronavirus)\n*   [Tehama County](https://www.tehamacohealthservices.net/services/communicable-diseases/#current-events)\n*   [Trinity County](https://www.trinitycounty.org/)\n*   [Tulare County](https://tchhsa.org/eng/index.cfm/public-health/covid-19-updates-novel-coronavirus/)\n*   [Tuolumne County](https://www.tuolumnecounty.ca.gov/250/Public-Health)\n*   [Ventura County](https://www.vcemergency.com/)\n*   [Yolo County](https://www.yolocounty.org/health-human-services/adults/communicable-disease-investigation-and-control/novel-coronavirus-2019)\n*   [Yuba County](https://www.yuba.org/coronavirus/)\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>While each county may have different restrictions, it is important to stay home as much as possible. If you do go out, stay 6 feet away from others who are not in your household and wear a cloth mask. Your actions save lives.\n\nLearn more about the state’s [roadmap to recovery](https://covid19.ca.gov/roadmap/) and the list of [counties who have met the criteria](https://covid19.ca.gov/roadmap-counties/) to move further ahead in the Resilience Roadmap.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C113" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3320,10 +3320,10 @@
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>What are the restrictions in my area?</v>
+        <v>How are we helping the homeless?</v>
       </c>
       <c r="B114" t="str">
-        <v>While each county may have different restrictions, it is important to stay home as much as possible. If you do go out, stay 6 feet away from others who are not in your household and wear a cloth mask. Your actions save lives.\n\nLearn more about the state’s [roadmap to recovery](https://covid19.ca.gov/roadmap/) and the list of [counties who have met the criteria](https://covid19.ca.gov/roadmap-counties/) to move further ahead in the Resilience Roadmap.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>Each county and local government in California has [increased resources](https://covid19.ca.gov/housing-and-homelessness/#top) to protect people experiencing homelessness during COVID-19. [Financial protections](https://covid19.ca.gov/housing-and-homelessness/#top) were added to prevent others from losing their homes during the outbreak.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C114" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3346,10 +3346,10 @@
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>How are we helping the homeless?</v>
+        <v>How is the state protecting incarcerated people in California?</v>
       </c>
       <c r="B115" t="str">
-        <v>Each county and local government in California has [increased resources](https://covid19.ca.gov/housing-and-homelessness/#top) to protect people experiencing homelessness during COVID-19. [Financial protections](https://covid19.ca.gov/housing-and-homelessness/#top) were added to prevent others from losing their homes during the outbreak.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>[California Department of Corrections and Rehabilitation (CDCR)](https://www.cdcr.ca.gov/covid19/) are dedicated to the safety of everyone who lives in, works in, and visits state prisons. CDCR has given all staff and inmates 2 reusable cloth masks to wear while moving between cells, dorms, meetings with others, or health care appointments. CDCR has also developed density and health care guidance to protect all inmates and staff, and has suspended volunteer services and in-person visiting.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C115" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3372,10 +3372,10 @@
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>How is the state protecting incarcerated people in California?</v>
+        <v>Who can I contact about my child custody order and child visitation rights?</v>
       </c>
       <c r="B116" t="str">
-        <v>[California Department of Corrections and Rehabilitation (CDCR)](https://www.cdcr.ca.gov/covid19/) are dedicated to the safety of everyone who lives in, works in, and visits state prisons. CDCR has given all staff and inmates 2 reusable cloth masks to wear while moving between cells, dorms, meetings with others, or health care appointments. CDCR has also developed density and health care guidance to protect all inmates and staff, and has suspended volunteer services and in-person visiting.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>Court operations vary from county to county. Please reach out to your [local government office](https://www.courts.ca.gov/find-my-court.htm?query=browse_courts) for more information. \n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C116" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3398,13 +3398,13 @@
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>Who can I contact about my child custody order and child visitation rights?</v>
+        <v>When is the disaster relief assistance available?</v>
       </c>
       <c r="B117" t="str">
-        <v>Court operations vary from county to county. Please reach out to your [local government office](https://www.courts.ca.gov/find-my-court.htm?query=browse_courts) for more information. \n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>Individuals may begin applying on May 18, 2020. Assistance will be available until the funding is spent or until June 30, 2020, at the latest. Applicants will be considered on a first-come, first-served basis. Applicants may only apply with the nonprofit organization(s) in their county of residency.\n\n**Please note:**\n\n*   Funding is limited, and disaster relief application services and assistance are not guaranteed.\n*   Nonprofit organizations will not be assisting individuals before May 18. Individuals _should not_ contact them ahead of time regarding disaster relief assistance.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C117" t="str">
-        <v>https://covid19.ca.gov/state-local-resources/</v>
+        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
       </c>
       <c r="D117" t="str">
         <v xml:space="preserve"> </v>
@@ -3424,10 +3424,10 @@
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>When is the disaster relief assistance available?</v>
+        <v>Who is eligible for this disaster relief assistance?</v>
       </c>
       <c r="B118" t="str">
-        <v>Individuals may begin applying on May 18, 2020. Assistance will be available until the funding is spent or until June 30, 2020, at the latest. Applicants will be considered on a first-come, first-served basis. Applicants may only apply with the nonprofit organization(s) in their county of residency.\n\n**Please note:**\n\n*   Funding is limited, and disaster relief application services and assistance are not guaranteed.\n*   Nonprofit organizations will not be assisting individuals before May 18. Individuals _should not_ contact them ahead of time regarding disaster relief assistance.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>Eligible individuals must be able to provide information that they:\n\n*   Are an undocumented adult (person over the age of 18)\n*   Are not eligible for federal COVID-19 assistance, like the CARES Act stimulus payments or pandemic unemployment benefits, and\n*   Have experienced hardship as a result of COVID-19.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C118" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3450,10 +3450,10 @@
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>Who is eligible for this disaster relief assistance?</v>
+        <v>Can getting this assistance affect my ability to get a green card or to become a U.S. Citizen? Will receiving it make me a public charge?</v>
       </c>
       <c r="B119" t="str">
-        <v>Eligible individuals must be able to provide information that they:\n\n*   Are an undocumented adult (person over the age of 18)\n*   Are not eligible for federal COVID-19 assistance, like the CARES Act stimulus payments or pandemic unemployment benefits, and\n*   Have experienced hardship as a result of COVID-19.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>This disaster relief assistance is not means-tested and is one-time assistance. The federal government does not list this assistance as a public benefit for a public charge consideration. However, USCIS has not issued specific guidance related to this assistance.\n\nIf you have questions about your immigration status and this program, please consult an attorney. A list of free and low-cost immigration services providers is available in the [Guide for Immigrant Californians (PDF)](/img/wp/listos_covid_19_immigrant_guidance_en_daf.pdf).\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C119" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3476,10 +3476,10 @@
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>Can getting this assistance affect my ability to get a green card or to become a U.S. Citizen? Will receiving it make me a public charge?</v>
+        <v>Is the personal information I provide to the nonprofits protected?</v>
       </c>
       <c r="B120" t="str">
-        <v>This disaster relief assistance is not means-tested and is one-time assistance. The federal government does not list this assistance as a public benefit for a public charge consideration. However, USCIS has not issued specific guidance related to this assistance.\n\nIf you have questions about your immigration status and this program, please consult an attorney. A list of free and low-cost immigration services providers is available in the [Guide for Immigrant Californians (PDF)](/img/wp/listos_covid_19_immigrant_guidance_en_daf.pdf).\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>Your information is only used to confirm eligibility and provide the assistance. No personal information (like name or address) will be given to any government agency. Only general information like age, gender, and preferred language will be shared with the State of California.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C120" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3502,10 +3502,10 @@
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>Is the personal information I provide to the nonprofits protected?</v>
+        <v>How do I apply?</v>
       </c>
       <c r="B121" t="str">
-        <v>Your information is only used to confirm eligibility and provide the assistance. No personal information (like name or address) will be given to any government agency. Only general information like age, gender, and preferred language will be shared with the State of California.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>The California Department of Social Services (CDSS) has identified non-profit where you can apply for disaster assistance. Find the [nonprofit where you can apply in your area](https://cdss.ca.gov/inforesources/immigration/covid-19-drai).\n\nApply _no sooner than May 18, and only to the organization in your area._ They will assist you with applying, confirm your eligibility, and deliver a payment card if you are approved. Applications will be considered on a first-come, first-served basis.\n\nFunding is limited, and disaster relief application services and assistance are not guaranteed.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C121" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3528,10 +3528,10 @@
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>How do I apply?</v>
+        <v>How many people in a household can receive this assistance?</v>
       </c>
       <c r="B122" t="str">
-        <v>The California Department of Social Services (CDSS) has identified non-profit where you can apply for disaster assistance. Find the [nonprofit where you can apply in your area](https://cdss.ca.gov/inforesources/immigration/covid-19-drai).\n\nApply _no sooner than May 18, and only to the organization in your area._ They will assist you with applying, confirm your eligibility, and deliver a payment card if you are approved. Applications will be considered on a first-come, first-served basis.\n\nFunding is limited, and disaster relief application services and assistance are not guaranteed.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>A maximum of two adults per household can qualify for this assistance, for a total of $1,000 per household. A household is defined as individuals who live, shop, and prepare meals together.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C122" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3554,10 +3554,10 @@
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>How many people in a household can receive this assistance?</v>
+        <v>How do eligible individuals receive this assistance?</v>
       </c>
       <c r="B123" t="str">
-        <v>A maximum of two adults per household can qualify for this assistance, for a total of $1,000 per household. A household is defined as individuals who live, shop, and prepare meals together.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>You will get a payment card either in person or through the mail. The organization in your area can give you more information.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C123" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3580,10 +3580,10 @@
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>How do eligible individuals receive this assistance?</v>
+        <v>How long do I have to apply?</v>
       </c>
       <c r="B124" t="str">
-        <v>You will get a payment card either in person or through the mail. The organization in your area can give you more information.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>Payments will be distributed beginning on May 18, 2020. They will continue until the $75 million in funding is spent, or until June 30, 2020 at the latest. We expect that this disaster relief assistance will run out very quickly. Apply as soon as you can, but not before May 18.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C124" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3606,10 +3606,10 @@
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v>How long do I have to apply?</v>
+        <v>If I am unable to apply for this program, are there other organizations that can help me?</v>
       </c>
       <c r="B125" t="str">
-        <v>Payments will be distributed beginning on May 18, 2020. They will continue until the $75 million in funding is spent, or until June 30, 2020 at the latest. We expect that this disaster relief assistance will run out very quickly. Apply as soon as you can, but not before May 18.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>Yes. The California Immigrant Resilience Fund is raising $50 million to provide cash assistance to undocumented Californians who are ineligible for other COVID-19 programs. Visit the [California Immigrant Resilience Fund](http://www.immigrantfundca.org) website to see if you can benefit from this program.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C125" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3632,10 +3632,10 @@
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v>If I am unable to apply for this program, are there other organizations that can help me?</v>
+        <v>What other government programs may I be eligible for during the COVID-19 pandemic?</v>
       </c>
       <c r="B126" t="str">
-        <v>Yes. The California Immigrant Resilience Fund is raising $50 million to provide cash assistance to undocumented Californians who are ineligible for other COVID-19 programs. Visit the [California Immigrant Resilience Fund](http://www.immigrantfundca.org) website to see if you can benefit from this program.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>Check the [Guide for Immigrant Californians (PDF)](/img/wp/listos_covid_19_immigrant_guidance_en_daf.pdf). It has information about jobs, wages, benefits, and small business and housing support.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C126" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3658,13 +3658,13 @@
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v>What other government programs may I be eligible for during the COVID-19 pandemic?</v>
+        <v>Youth and Teens</v>
       </c>
       <c r="B127" t="str">
-        <v>Check the [Guide for Immigrant Californians (PDF)](/img/wp/listos_covid_19_immigrant_guidance_en_daf.pdf). It has information about jobs, wages, benefits, and small business and housing support.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>*   [California Youth Crisis Line](https://calyouth.org/cycl/)**:** Youth ages 12-24 can call or text [800-843-5200](tel:800-843-5200) or [chat online](https://m2.icarol.com/ConsumerRegistration.aspx?org=53141&amp;pid=326&amp;cc=en-US) for 24/7 crisis support.\n*   [TEEN LINE](https://teenlineonline.org/talk-now/): Teens can talk to another teen by texting “TEEN” to [839863](sms:839863) from 6pm – 9pm, or call [800-852-8336](tel:800-852-8336) from 6pm – 10pm.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C127" t="str">
-        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
+        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
       </c>
       <c r="D127" t="str">
         <v xml:space="preserve"> </v>
@@ -3684,10 +3684,10 @@
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v>Youth and Teens</v>
+        <v>Veterans</v>
       </c>
       <c r="B128" t="str">
-        <v>*   [California Youth Crisis Line](https://calyouth.org/cycl/)**:** Youth ages 12-24 can call or text [800-843-5200](tel:800-843-5200) or [chat online](https://m2.icarol.com/ConsumerRegistration.aspx?org=53141&amp;pid=326&amp;cc=en-US) for 24/7 crisis support.\n*   [TEEN LINE](https://teenlineonline.org/talk-now/): Teens can talk to another teen by texting “TEEN” to [839863](sms:839863) from 6pm – 9pm, or call [800-852-8336](tel:800-852-8336) from 6pm – 10pm.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>[Veterans Crisis Line](https://www.veteranscrisisline.net): Call [800-273-8255](tel:800-273-8255) and Press 1 or text [838255](sms:838255) for 24/7 support.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C128" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -3710,10 +3710,10 @@
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v>Veterans</v>
+        <v>First Responders and Law Enforcement</v>
       </c>
       <c r="B129" t="str">
-        <v>[Veterans Crisis Line](https://www.veteranscrisisline.net): Call [800-273-8255](tel:800-273-8255) and Press 1 or text [838255](sms:838255) for 24/7 support.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>*   [Fire/EMS helpline](https://www.nvfc.org/fireems-helpline/): Call [888-731-FIRE](tel:888-731-FIRE) to get 24/7 help for a variety of behavioral health issues.\n*   [COPLINE](https://www.copline.org/): Call [800-267-5463](tel:800-267-5463) to find support 24/7 for law enforcement officers.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C129" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -3736,10 +3736,10 @@
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v>First Responders and Law Enforcement</v>
+        <v>Older Californians</v>
       </c>
       <c r="B130" t="str">
-        <v>*   [Fire/EMS helpline](https://www.nvfc.org/fireems-helpline/): Call [888-731-FIRE](tel:888-731-FIRE) to get 24/7 help for a variety of behavioral health issues.\n*   [COPLINE](https://www.copline.org/): Call [800-267-5463](tel:800-267-5463) to find support 24/7 for law enforcement officers.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>*   [Friendship Line](https://www.ioaging.org/services/all-inclusive-health-care/friendship-line): Call [888-670-1360](tel:888-670-1360) for 24/7 support if you are 60 years or older, or an adult living with disabilities.  \n*   California Aging and Adult Information Line: Call [800-510-2020](tel:800-510-2020) for help finding local assistance. \n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C130" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -3762,10 +3762,10 @@
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v>Older Californians</v>
+        <v>Deaf and Hard of Hearing Individuals</v>
       </c>
       <c r="B131" t="str">
-        <v>*   [Friendship Line](https://www.ioaging.org/services/all-inclusive-health-care/friendship-line): Call [888-670-1360](tel:888-670-1360) for 24/7 support if you are 60 years or older, or an adult living with disabilities.  \n*   California Aging and Adult Information Line: Call [800-510-2020](tel:800-510-2020) for help finding local assistance. \n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>[National Suicide Prevention Deaf and Hard of Hearing Hotline](https://suicidepreventionlifeline.org/help-yourself/for-deaf-hard-of-hearing/): Access 24/7 video relay service by dialing [800-273-8255](tel:800-273-8255) (TTY [800-799-4889](tel:800-799-4889)).\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C131" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -3788,10 +3788,10 @@
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v>Deaf and Hard of Hearing Individuals</v>
+        <v>Services for Substance Use Disorders</v>
       </c>
       <c r="B132" t="str">
-        <v>[National Suicide Prevention Deaf and Hard of Hearing Hotline](https://suicidepreventionlifeline.org/help-yourself/for-deaf-hard-of-hearing/): Access 24/7 video relay service by dialing [800-273-8255](tel:800-273-8255) (TTY [800-799-4889](tel:800-799-4889)).\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>*   [SAMHSA National Helpline](https://www.samhsa.gov/find-help/national-helpline): Call [800-662-HELP](tel:1-800-662-4357) for 24/7 information and referrals in English and Spanish. \n*   [SAMHSA Treatment Locator](https://findtreatment.samhsa.gov)**:**  Find drug or alcohol treatment programs. \n*   [Local county access lines](https://gcc01.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.dhcs.ca.gov%2Findividuals%2FPages%2FSUD_County_Access_Lines.aspx&amp;data=02%7C01%7CJanne.Olson-Morgan%40osg.ca.gov%7C122307be91754d12e5dc08d7d984f958%7C265c2dcd2a6e43aab2e826421a8c8526%7C0%7C0%7C637217037446186621&amp;sdata=5sx4UdIlVkRL%2BEJR7FrpK0gYAn20yE71TyBDFIw1kJM%3D&amp;reserved=0): Find your local number for help seeking substance use disorder services.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C132" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -3814,10 +3814,10 @@
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v>Services for Substance Use Disorders</v>
+        <v>LGBTQ Individuals</v>
       </c>
       <c r="B133" t="str">
-        <v>*   [SAMHSA National Helpline](https://www.samhsa.gov/find-help/national-helpline): Call [800-662-HELP](tel:1-800-662-4357) for 24/7 information and referrals in English and Spanish. \n*   [SAMHSA Treatment Locator](https://findtreatment.samhsa.gov)**:**  Find drug or alcohol treatment programs. \n*   [Local county access lines](https://gcc01.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.dhcs.ca.gov%2Findividuals%2FPages%2FSUD_County_Access_Lines.aspx&amp;data=02%7C01%7CJanne.Olson-Morgan%40osg.ca.gov%7C122307be91754d12e5dc08d7d984f958%7C265c2dcd2a6e43aab2e826421a8c8526%7C0%7C0%7C637217037446186621&amp;sdata=5sx4UdIlVkRL%2BEJR7FrpK0gYAn20yE71TyBDFIw1kJM%3D&amp;reserved=0): Find your local number for help seeking substance use disorder services.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>*   [Trevor Project](https://www.thetrevorproject.org): Call [866-488-7386](tel:866-488-7386) or text START to [678678](sms:678678) for 24/7 information and suicide prevention resources for LGBTQ youth.\n*   [Lesbian, Gay, Bisexual and Transgender National Hotline](https://www.glbthotline.org/hotline.html): Call [800-273-8255](tel:800-273-8255) from 1pm – 9pm for support, information or help finding resources.\n*   [Victims of Crime Resource Center](https://1800victims.org/): Call or text [800-842-8467](tel:800-842-8467) or [chat online](https://1800victims.org/) for information about LGTBQ rights, legal protections, and local resources.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C133" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -3840,13 +3840,13 @@
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v>LGBTQ Individuals</v>
+        <v>What is a close contact?</v>
       </c>
       <c r="B134" t="str">
-        <v>*   [Trevor Project](https://www.thetrevorproject.org): Call [866-488-7386](tel:866-488-7386) or text START to [678678](sms:678678) for 24/7 information and suicide prevention resources for LGBTQ youth.\n*   [Lesbian, Gay, Bisexual and Transgender National Hotline](https://www.glbthotline.org/hotline.html): Call [800-273-8255](tel:800-273-8255) from 1pm – 9pm for support, information or help finding resources.\n*   [Victims of Crime Resource Center](https://1800victims.org/): Call or text [800-842-8467](tel:800-842-8467) or [chat online](https://1800victims.org/) for information about LGTBQ rights, legal protections, and local resources.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>A close contact is someone who was within 6 feet of a person with COVID-19 for at least 15 minutes. This usually includes household members, intimate contacts, and caregivers, but can include others.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C134" t="str">
-        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D134" t="str">
         <v xml:space="preserve"> </v>
@@ -3866,10 +3866,10 @@
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v>What is a close contact?</v>
+        <v>Will contact tracers track my location?</v>
       </c>
       <c r="B135" t="str">
-        <v>A close contact is someone who was within 6 feet of a person with COVID-19 for at least 15 minutes. This usually includes household members, intimate contacts, and caregivers, but can include others.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>California’s contact tracing program does not use any cell phone tracking technology. Someone from your local public health department will simply speak privately with you. All information is confidential and protected by California’s strict privacy laws. They may stay in touch to make sure your symptoms aren’t worsening.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C135" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -3892,10 +3892,10 @@
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v>Will contact tracers track my location?</v>
+        <v>Is contact tracing help available in my language?</v>
       </c>
       <c r="B136" t="str">
-        <v>California’s contact tracing program does not use any cell phone tracking technology. Someone from your local public health department will simply speak privately with you. All information is confidential and protected by California’s strict privacy laws. They may stay in touch to make sure your symptoms aren’t worsening.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>Your [local health department](https://covid19.ca.gov/state-local-resources/#top) can communicate with you in many different languages.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C136" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -3918,10 +3918,10 @@
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v>Is contact tracing help available in my language?</v>
+        <v>Who should get tested?</v>
       </c>
       <c r="B137" t="str">
-        <v>Your [local health department](https://covid19.ca.gov/state-local-resources/#top) can communicate with you in many different languages.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>You should get tested if you:\n\n*   Are a close contact of anyone who has or may have COVID-19, or\n*   Think you may have been exposed, or\n*   Are having [COVID-19 symptoms](https://covid19.ca.gov/symptoms-and-risks/). \n\nFind a [testing site in your area](https://covid19.ca.gov/testing-and-treatment/).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C137" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -3944,10 +3944,10 @@
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v>Who should get tested?</v>
+        <v>How do I find a testing location?</v>
       </c>
       <c r="B138" t="str">
-        <v>You should get tested if you:\n\n*   Are a close contact of anyone who has or may have COVID-19, or\n*   Think you may have been exposed, or\n*   Are having [COVID-19 symptoms](https://covid19.ca.gov/symptoms-and-risks/). \n\nFind a [testing site in your area](https://covid19.ca.gov/testing-and-treatment/).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>To learn more about testing and care, visit the [Testing and treatment page](https://covid19.ca.gov/testing-and-treatment/). You can search for testing locations there using your zip code. \n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C138" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -3970,10 +3970,10 @@
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>How do I find a testing location?</v>
+        <v>What if I have COVID-19 symptoms and have not been contacted by the health department?</v>
       </c>
       <c r="B139" t="str">
-        <v>To learn more about testing and care, visit the [Testing and treatment page](https://covid19.ca.gov/testing-and-treatment/). You can search for testing locations there using your zip code. \n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>[Get tested](https://covid19.ca.gov/testing-and-treatment/) immediately, contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing, and isolate yourself while waiting for your test results.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C139" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -3996,10 +3996,10 @@
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>What if I have COVID-19 symptoms and have not been contacted by the health department?</v>
+        <v>What if I came in contact with someone who has COVID-19 symptoms, but my local health department is not aware of it?</v>
       </c>
       <c r="B140" t="str">
-        <v>[Get tested](https://covid19.ca.gov/testing-and-treatment/) immediately, contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing, and isolate yourself while waiting for your test results.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>You should [get tested](https://covid19.ca.gov/testing-and-treatment/). Contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing, and isolate yourself while waiting for your test results.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C140" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4022,10 +4022,10 @@
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>What if I came in contact with someone who has COVID-19 symptoms, but my local health department is not aware of it?</v>
+        <v>How do I become a contact tracer?</v>
       </c>
       <c r="B141" t="str">
-        <v>You should [get tested](https://covid19.ca.gov/testing-and-treatment/). Contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing, and isolate yourself while waiting for your test results.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>The initial phase of California Connected, the state’s contact tracing program, will utilize existing resources and redirect state employees to begin contact tracing efforts. Offers of additional support from the private sector and qualified members of the public are appreciated, but contact tracers from outside state government may not be needed until a future phase. Thank you for wanting to share your expertise and resources with your fellow Californians.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C141" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4048,13 +4048,13 @@
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>How do I become a contact tracer?</v>
+        <v>County case metrics</v>
       </c>
       <c r="B142" t="str">
-        <v>The initial phase of California Connected, the state’s contact tracing program, will utilize existing resources and redirect state employees to begin contact tracing efforts. Offers of additional support from the private sector and qualified members of the public are appreciated, but contact tracers from outside state government may not be needed until a future phase. Thank you for wanting to share your expertise and resources with your fellow Californians.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>**Stable or down trending hospitalizations**\n\n*   Stable hospitalizations of COVID individuals on a 7-day average of daily percent change of less than 5% **OR** no more than 20 COVID hospitalizations on any single day in the past 14 days \n\n**Cases per population count and test positivity rate**\n\n*   Less than 25 new cases per 100,000 residents in the past 14 days **OR** less than 8% testing positive in the past 7 days\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
       </c>
       <c r="C142" t="str">
-        <v>https://covid19.ca.gov/contact-tracing/</v>
+        <v>https://covid19.ca.gov/roadmap-counties/</v>
       </c>
       <c r="D142" t="str">
         <v xml:space="preserve"> </v>
@@ -4074,10 +4074,10 @@
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>County case metrics</v>
+        <v>County preparedness</v>
       </c>
       <c r="B143" t="str">
-        <v>**Stable or down trending hospitalizations**\n\n*   Stable hospitalizations of COVID individuals on a 7-day average of daily percent change of less than 5% **OR** no more than 20 COVID hospitalizations on any single day in the past 14 days \n\n**Cases per population count and test positivity rate**\n\n*   Less than 25 new cases per 100,000 residents in the past 14 days **OR** less than 8% testing positive in the past 7 days\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>**Testing capacity** \n\n*   Minimum daily testing volume to test 1.5 per 1,000 residents, which can be met through a combination of testing of symptomatic individuals and targeted surveillance.  The county’s average daily testing volume for the past week must be provided.  If the county does not believe a testing volume of 1.5 per 1,000 residents is merited, justification must be provided. \n*   Testing availability for at least 75% of residents, as measured by a specimen collection site (including established health care providers) within 30 minutes driving time in urban areas, and 60 minutes in rural areas. \n\n**Contact tracing** \n\n*   Sufficient contact tracing so public health staff work can work with a patient to help them recall everyone with whom they have had close contact during the timeframe while they may have been infectious.  For counties that have no cases, there should be at least 15 staff per 100,000 county population trained and available for contact tracing; for counties with small populations, there must be at least one staff person trained and available.  \n\n**Hospital surge**\n\n*   County (or regional) hospital capacity to accommodate a minimum surge of 35% due to COVID-19 cases in addition to providing usual care for non-COVID-19 patients.  \n\n**SNF disease outbreak prevention and containment**\n\n*   Must have plans to prevent and mitigate infections in skilled nursing facilities (SNF)\n*   Skilled nursing facilities must have more than a 14 day supply of PPE on hand for staff, with an established process for ongoing procurement from non-state supply chains.  \n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
       </c>
       <c r="C143" t="str">
         <v>https://covid19.ca.gov/roadmap-counties/</v>
@@ -4100,10 +4100,10 @@
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>County preparedness</v>
+        <v>County response</v>
       </c>
       <c r="B144" t="str">
-        <v>**Testing capacity** \n\n*   Minimum daily testing volume to test 1.5 per 1,000 residents, which can be met through a combination of testing of symptomatic individuals and targeted surveillance.  The county’s average daily testing volume for the past week must be provided.  If the county does not believe a testing volume of 1.5 per 1,000 residents is merited, justification must be provided. \n*   Testing availability for at least 75% of residents, as measured by a specimen collection site (including established health care providers) within 30 minutes driving time in urban areas, and 60 minutes in rural areas. \n\n**Contact tracing** \n\n*   Sufficient contact tracing so public health staff work can work with a patient to help them recall everyone with whom they have had close contact during the timeframe while they may have been infectious.  For counties that have no cases, there should be at least 15 staff per 100,000 county population trained and available for contact tracing; for counties with small populations, there must be at least one staff person trained and available.  \n\n**Hospital surge**\n\n*   County (or regional) hospital capacity to accommodate a minimum surge of 35% due to COVID-19 cases in addition to providing usual care for non-COVID-19 patients.  \n\n**SNF disease outbreak prevention and containment**\n\n*   Must have plans to prevent and mitigate infections in skilled nursing facilities (SNF)\n*   Skilled nursing facilities must have more than a 14 day supply of PPE on hand for staff, with an established process for ongoing procurement from non-state supply chains.  \n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>*   Counties must produce plans for the following related to county-wide containment:\n    *   Availability of temporary housing units to shelter at least 15% of county residents experiencing homelessness in case of an outbreak among this population requiring isolation and quarantine of affected individuals. The county’s plans to support individuals, including those experiencing homelessness, who are not able to properly isolate in a home setting by providing them with temporary housing (including access to a private bathroom), for the duration of the necessary isolation or quarantine period must be described.\n\n*   County (or regional) hospital facilities have a robust plan to protect the hospital workforce, both clinical and nonclinical, with PPE.  \n*   Guidance for employers and essential critical infrastructure workplaces on how to structure the physical environment to protect essential workers.  \n*   Availability of supplies (disinfectant, essential protective gear) to protect essential workers. \n*   Each county must provide details on their plans to move further ahead in the Resilience Roadmap including which sectors and spaces will be opened, in what sequence, on what timeline.  Please specifically indicate where the plan differs from the state’s order.  Please note that this variance should not include sectors that are part of Stage 3.\n*   County metrics that would serve as triggers for either slowing the pace through Stage 2 or tightening modifications, including the frequency of measurement, the specific actions triggered by metric changes must be described, and how the county will inform the state of emerging concerns and how it will implement early containment measures. \n*   The county must provide details on the plan to move through opening sectors and spaces that are part of the State’s plan for Stage 2. A reminder, that this variance only covers those areas that are part of Stage 2, up to, but not including Stage 3. \n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
       </c>
       <c r="C144" t="str">
         <v>https://covid19.ca.gov/roadmap-counties/</v>
@@ -4126,10 +4126,10 @@
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>County response</v>
+        <v>Dine-in restaurants</v>
       </c>
       <c r="B145" t="str">
-        <v>*   Counties must produce plans for the following related to county-wide containment:\n    *   Availability of temporary housing units to shelter at least 15% of county residents experiencing homelessness in case of an outbreak among this population requiring isolation and quarantine of affected individuals. The county’s plans to support individuals, including those experiencing homelessness, who are not able to properly isolate in a home setting by providing them with temporary housing (including access to a private bathroom), for the duration of the necessary isolation or quarantine period must be described.\n\n*   County (or regional) hospital facilities have a robust plan to protect the hospital workforce, both clinical and nonclinical, with PPE.  \n*   Guidance for employers and essential critical infrastructure workplaces on how to structure the physical environment to protect essential workers.  \n*   Availability of supplies (disinfectant, essential protective gear) to protect essential workers. \n*   Each county must provide details on their plans to move further ahead in the Resilience Roadmap including which sectors and spaces will be opened, in what sequence, on what timeline.  Please specifically indicate where the plan differs from the state’s order.  Please note that this variance should not include sectors that are part of Stage 3.\n*   County metrics that would serve as triggers for either slowing the pace through Stage 2 or tightening modifications, including the frequency of measurement, the specific actions triggered by metric changes must be described, and how the county will inform the state of emerging concerns and how it will implement early containment measures. \n*   The county must provide details on the plan to move through opening sectors and spaces that are part of the State’s plan for Stage 2. A reminder, that this variance only covers those areas that are part of Stage 2, up to, but not including Stage 3. \n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>This [guidance for dine-in restaurants](https://covid19.ca.gov/pdf/guidance-dine-in-restaurants.pdf) provides guidelines to create a safer environment for workers.  \nReview the guidance, prepare a plan, and post the [checklist for dine-in restaurants](https://covid19.ca.gov/pdf/checklist-dine-in-restaurants.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
       </c>
       <c r="C145" t="str">
         <v>https://covid19.ca.gov/roadmap-counties/</v>
@@ -4152,10 +4152,10 @@
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>Dine-in restaurants</v>
+        <v>Hair salons and barbershops</v>
       </c>
       <c r="B146" t="str">
-        <v>This [guidance for dine-in restaurants](https://covid19.ca.gov/pdf/guidance-dine-in-restaurants.pdf) provides guidelines to create a safer environment for workers.  \nReview the guidance, prepare a plan, and post the [checklist for dine-in restaurants](https://covid19.ca.gov/pdf/checklist-dine-in-restaurants.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>This [guidance for hair salons and barbershops](https://covid19.ca.gov/pdf/guidance-hair-salons.pdf) provides guidelines to create a safer environment for workers.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
       </c>
       <c r="C146" t="str">
         <v>https://covid19.ca.gov/roadmap-counties/</v>
@@ -4178,10 +4178,10 @@
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>Hair salons and barbershops</v>
+        <v>Casinos</v>
       </c>
       <c r="B147" t="str">
-        <v>This [guidance for hair salons and barbershops](https://covid19.ca.gov/pdf/guidance-hair-salons.pdf) provides guidelines to create a safer environment for workers.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>In working with tribal governments, CDPH and DIR has released guidance on how to reopen casinos with reduced risk of transmission. Tribal governments should make determinations on when to reopen based on how they align with the current local public health conditions and the statewide stage of reopening and the Governor respectfully requests that until a surrounding or neighboring local jurisdiction has progressed into Stage 3, tribal casinos remain closed.\n\nFollow this [guidance for casinos](https://covid19.ca.gov/pdf/guidance-casinos.pdf) to create a safer environment for workers and patrons.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
       </c>
       <c r="C147" t="str">
         <v>https://covid19.ca.gov/roadmap-counties/</v>
@@ -4204,10 +4204,10 @@
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>Casinos</v>
+        <v>Movie theaters and family entertainment centers</v>
       </c>
       <c r="B148" t="str">
-        <v>In working with tribal governments, CDPH and DIR has released guidance on how to reopen casinos with reduced risk of transmission. Tribal governments should make determinations on when to reopen based on how they align with the current local public health conditions and the statewide stage of reopening and the Governor respectfully requests that until a surrounding or neighboring local jurisdiction has progressed into Stage 3, tribal casinos remain closed.\n\nFollow this [guidance for casinos](https://covid19.ca.gov/pdf/guidance-casinos.pdf) to create a safer environment for workers and patrons.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>Follow this guidance for [movie theaters and family entertainment centers](http://covid19.ca.gov/pdf/guidance-family-entertainment.pdf) to create a safer environment for workers and patrons.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
       </c>
       <c r="C148" t="str">
         <v>https://covid19.ca.gov/roadmap-counties/</v>
@@ -4230,10 +4230,10 @@
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v>Movie theaters and family entertainment centers</v>
+        <v>Restaurants, wineries, and bars</v>
       </c>
       <c r="B149" t="str">
-        <v>Follow this guidance for [movie theaters and family entertainment centers](http://covid19.ca.gov/pdf/guidance-family-entertainment.pdf) to create a safer environment for workers and patrons.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>Follow this [guidance for restaurants, wineries, and bars](http://covid19.ca.gov/pdf/guidance-restaurants-bars.pdf) to create a safer environment for workers and patrons.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
       </c>
       <c r="C149" t="str">
         <v>https://covid19.ca.gov/roadmap-counties/</v>
@@ -4256,10 +4256,10 @@
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>Restaurants, wineries, and bars</v>
+        <v>Zoos and museums</v>
       </c>
       <c r="B150" t="str">
-        <v>Follow this [guidance for restaurants, wineries, and bars](http://covid19.ca.gov/pdf/guidance-restaurants-bars.pdf) to create a safer environment for workers and patrons.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>Follow this [guidance for zoos, museums](http://covid19.ca.gov/pdf/guidance-zoos-museums.pdf), galleries, and aquariums to create a safer environment for workers and patrons.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
       </c>
       <c r="C150" t="str">
         <v>https://covid19.ca.gov/roadmap-counties/</v>
@@ -4282,10 +4282,10 @@
     </row>
     <row r="151">
       <c r="A151" t="str">
-        <v>Zoos and museums</v>
+        <v>Gyms and fitness centers</v>
       </c>
       <c r="B151" t="str">
-        <v>Follow this [guidance for zoos, museums](http://covid19.ca.gov/pdf/guidance-zoos-museums.pdf), galleries, and aquariums to create a safer environment for workers and patrons.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>Follow this [guidance for gyms and fitness centers](http://covid19.ca.gov/pdf/guidance-fitness.pdf) to create a safer environment for workers and patrons.  \n  \nRecreational team sports are not permitted and will be subject to separate guidance.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)&lt;!-- skill, clinic, youth, sports, league, recreational, team --&gt;</v>
       </c>
       <c r="C151" t="str">
         <v>https://covid19.ca.gov/roadmap-counties/</v>
@@ -4308,10 +4308,10 @@
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>Gyms and fitness centers</v>
+        <v>Hotels (for tourism and individual travel)</v>
       </c>
       <c r="B152" t="str">
-        <v>Follow this [guidance for gyms and fitness centers](http://covid19.ca.gov/pdf/guidance-fitness.pdf) to create a safer environment for workers and patrons.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>Follow this [guidance for hotels and short term rentals](https://covid19.ca.gov/pdf/guidance-hotels-lodging-rentals.pdf) for tourism and individual travel to create a safer environment for workers and patrons.\n\nThis guidance is applicable only within counties with variance attestation. Hotel and lodging services in all other counties should adhere to the guidance limitations provided by [statewide guidance](https://covid19.ca.gov/pdf/guidance-hotels.pdf), where hotels should only open for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or providing housing solutions, including measures to protect homeless populations.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)&lt;!-- motel, vacation, airbnb, vrbo, rental home --&gt;</v>
       </c>
       <c r="C152" t="str">
         <v>https://covid19.ca.gov/roadmap-counties/</v>
@@ -4334,10 +4334,10 @@
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v>Hotels (for tourism and individual travel)</v>
+        <v>Cardrooms and racetracks</v>
       </c>
       <c r="B153" t="str">
-        <v>Follow this [guidance for hotels and short term rentals](https://covid19.ca.gov/pdf/guidance-hotels-lodging-rentals.pdf) for tourism and individual travel to create a safer environment for workers and patrons.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>Follow this [guidance for cardrooms](https://covid19.ca.gov/pdf/guidance-cardrooms-racetracks.pdf), race tracks, and satellite wagering to create a safer environment for workers and patrons.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
       </c>
       <c r="C153" t="str">
         <v>https://covid19.ca.gov/roadmap-counties/</v>
@@ -4360,10 +4360,10 @@
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v>Cardrooms and racetracks</v>
+        <v>Campgrounds and outdoor recreation</v>
       </c>
       <c r="B154" t="str">
-        <v>Follow this [guidance for cardrooms](https://covid19.ca.gov/pdf/guidance-cardrooms-racetracks.pdf), race tracks, and satellite wagering to create a safer environment for workers and patrons.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>Follow this [guidance for campgrounds](http://covid19.ca.gov/pdf/guidance-campgrounds.pdf) to create a safer environment for workers and patrons.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)&lt;!-- park, visitor center, travel, museum, recreation, outdoor recreation, sports, RV, tent, camp, fish, beach, lake, river, event, outdoor event, event planning, wedding, hike, walk, bike, exercise, nature, birdwatching, public --&gt;</v>
       </c>
       <c r="C154" t="str">
         <v>https://covid19.ca.gov/roadmap-counties/</v>
@@ -4386,10 +4386,10 @@
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>Campgrounds and outdoor recreation</v>
+        <v>Personal care services</v>
       </c>
       <c r="B155" t="str">
-        <v>Follow this [guidance for campgrounds](http://covid19.ca.gov/pdf/guidance-campgrounds.pdf) to create a safer environment for workers and patrons.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>Follow this [guidance for personal care services](https://files.covid19.ca.gov/pdf/expanded-personal-services--en.pdf) like nail salons, tattoo parlors, and body waxing to create a safer environment for workers and patrons.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)&lt;!-- spa, esthetician, facial, electrolysis, waxing, massage office, massage clinic, massage therapist, massage parlor, masseuse, skin care, cosmetology services, electrology, massage therapy --&gt;</v>
       </c>
       <c r="C155" t="str">
         <v>https://covid19.ca.gov/roadmap-counties/</v>
@@ -4412,13 +4412,13 @@
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v>Personal care services</v>
+        <v>Northern California</v>
       </c>
       <c r="B156" t="str">
-        <v>Follow this [guidance for personal care services](https://covid19.ca.gov/pdf/expanded-personal-services.pdf) like nail salons, tattoo parlors, and body waxing to create a safer environment for workers and patrons.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>*   American Canyon (Napa County)\n*   Alturas (Modoc County)\n*   Bear Valley (Alpine County)\n*   Bieber (Lassen County)\n*   Bishop (Inyo County)\n*   Bridgeport (Mono County)\n*   Cedarville (Modoc County)\n*   Clearlake (Lake County)\n*   Coleville (Mono County)\n*   Crescent City (Del Norte County)\n*   Daly City (San Mateo County)\n*   Downieville (Sierra County)\n*   Doyle (Lassen County)\n*   East Palo Alto (San Mateo County)\n*   Half Moon Bay (San Mateo County)\n*   Hayfork (Trinity County)\n*   Herlong (Lassen County)\n*   Jackson (Amador County)\n*   Kirkwood (Alpine and Amador Counties)\n*   Lakeport (Lake County)\n*   Lone Pine (Inyo County)\n*   Loyalton (Sierra County)\n*   Mammoth Lakes (Mono County)\n*   Middletown (Lake County)\n*   Napa (Napa County)\n*   Oakland (Alameda County)\n*   Quincy (Plumas County)\n*   Redwood City (San Mateo County)\n*   Sacramento (Sacramento County)\n*   Salida (Stanislaus County)\n*   San Francisco (San Francisco)\n*   San Jose (Santa Clara County)\n*   San Mateo (San Mateo County)\n*   Stockton (San Joaquin County)\n*   Susanville (Lassen County)\n*   Weaverville (Trinity County)\n*   Westwood (Lassen County)\n*   Willow Creek (Humboldt County)\n*   Woodfords (Alpine County)\n*   Yosemite Valley (Mariposa County)\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C156" t="str">
-        <v>https://covid19.ca.gov/roadmap-counties/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D156" t="str">
         <v xml:space="preserve"> </v>
@@ -4438,10 +4438,10 @@
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>Northern California</v>
+        <v>Southern California</v>
       </c>
       <c r="B157" t="str">
-        <v>*   Alturas (Modoc County)\n*   Bear Valley (Alpine County)\n*   Bieber (Lassen County)\n*   Bishop (Inyo County)\n*   Bridgeport (Mono County)\n*   Cedarville (Modoc County)\n*   Clearlake (Lake County)\n*   Crescent City (Del Norte County)\n*   Daly City (San Mateo County)\n*   Downieville (Sierra County)\n*   Doyle (Lassen County)\n*   East Palo Alto (San Mateo County)\n*   Half Moon Bay (San Mateo County)\n*   Hayfork (Trinity County)\n*   Herlong (Lassen County)\n*   Jackson (Amador County)\n*   Kirkwood (Alpine and Amador Counties)\n*   Lakeport (Lake County)\n*   Lone Pine (Inyo County)\n*   Loyalton (Sierra County)\n*   Mammoth Lakes (Mono County)\n*   Middletown (Lake County)\n*   Napa (Napa County)\n*   Oakland (Alameda County)\n*   Quincy (Plumas County)\n*   Redwood City (San Mateo County)\n*   Sacramento (Sacramento County)\n*   Salida (Stanislaus County)\n*   San Francisco (San Francisco)\n*   San Jose (Santa Clara County)\n*   San Mateo (San Mateo County)\n*   Stockton (San Joaquin County)\n*   Susanville (Lassen County)\n*   Weaverville (Trinity County)\n*   Westwood (Lassen County)\n*   Willow Creek (Humboldt County)\n*   Woodfords (Alpine County)\n*   Yosemite Valley (Mariposa County)\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>*   Bell (Los Angeles County)\n*   Bakersfield (Kern County)\n*   Lake Elsinore (Riverside County)\n*   Long Beach (Los Angeles County)\n*   Los Angeles (Los Angeles County)\n*   Sherman Oaks (Los Angeles County)\n*   Van Nuys (Los Angeles County)\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C157" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4464,10 +4464,10 @@
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>Southern California</v>
+        <v>How do I get a drive-through test?</v>
       </c>
       <c r="B158" t="str">
-        <v>*   Bakersfield (Kern County)\n*   Lake Elsinore (Riverside County)\n*   Long Beach (Los Angeles County)\n*   Los Angeles (Los Angeles County)\n*   Sherman Oaks (Los Angeles County)\n*   Van Nuys (Los Angeles County)\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>There are two steps to this process: screening and testing. First, you will create an account and take the online screener. If your answers from the screener determine you are eligible at this time, you will receive details on how and where to get tested. Once tested, you’ll be informed via email or phone when your COVID-19 test results are available.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C158" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4490,10 +4490,10 @@
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>How do I get a drive-through test?</v>
+        <v>Why am I asked to create an account for drive-through testing using Verily’s Project Baseline?</v>
       </c>
       <c r="B159" t="str">
-        <v>There are two steps to this process: screening and testing. First, you will create an account and take the online screener. If your answers from the screener determine you are eligible at this time, you will receive details on how and where to get tested. Once tested, you’ll be informed via email or phone when your COVID-19 test results are available.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>For the Baseline COVID-19 Program to work, Verily needs a way to authenticate users to appropriately protect their information. Verily turned to Google for this service because Google Account provides best-in-class authentication. We ask that you link to an existing Google Account or create a new Google Account (which can be done with any email address). This lets Verily authenticate your account, and securely and privately contact you during the screening and testing process. All the data provided by Baseline COVID-19 Program users for screening is stored separately and not directly linked to a user’s Google Account.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C159" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4516,10 +4516,10 @@
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>Why am I asked to create an account for drive-through testing using Verily’s Project Baseline?</v>
+        <v>I have mild COVID-19 symptoms. How long do I have to isolate at home?</v>
       </c>
       <c r="B160" t="str">
-        <v>For the Baseline COVID-19 Program to work, Verily needs a way to authenticate users to appropriately protect their information. Verily turned to Google for this service because Google Account provides best-in-class authentication. We ask that you link to an existing Google Account or create a new Google Account (which can be done with any email address). This lets Verily authenticate your account, and securely and privately contact you during the screening and testing process. All the data provided by Baseline COVID-19 Program users for screening is stored separately and not directly linked to a user’s Google Account.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>Follow the Centers for Disease Control and Prevention (CDC) guidance on [ending self-isolation](https://www.cdc.gov/coronavirus/2019-ncov/hcp/disposition-in-home-patients.html).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C160" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4542,10 +4542,10 @@
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>I have mild COVID-19 symptoms. How long do I have to isolate at home?</v>
+        <v>How can I find a coronavirus testing location near me?</v>
       </c>
       <c r="B161" t="str">
-        <v>Follow the Centers for Disease Control and Prevention (CDC) guidance on [ending self-isolation](https://www.cdc.gov/coronavirus/2019-ncov/hcp/disposition-in-home-patients.html).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>Find a testing location\n-----------------------\n\n&gt; [See the map](https://arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401)\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C161" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4568,10 +4568,10 @@
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>How can I find a coronavirus testing location near me?</v>
+        <v>When should I seek emergency medical assistance (e. g. go to hospital for treatment, etc.) for COVID-19 / Coronavirus Symptoms?</v>
       </c>
       <c r="B162" t="str">
-        <v>Find a testing location\n-----------------------\n\n&gt; [See the map](https://arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401)\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>If you develop any of these warning signs for COVID-19, get emergency medical attention immediately:\n\n*   Trouble breathing\n*   Persistent pain or pressure in the chest\n*   New confusion \n*   Inability to awake or stay awake\n*   Bluish lips or face\n\nThere are other, less-common symptoms. Please call your medical provider if you have any symptoms that are severe or concerning to you.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call 911, tell the operator you have coronavirus symptoms so ambulance workers can be ready to treat you safely.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C162" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4594,13 +4594,13 @@
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>When should I seek emergency medical assistance (e. g. go to hospital for treatment, etc.) for COVID-19 / Coronavirus Symptoms?</v>
+        <v>What are the pay and benefits for California Health Corps professionals?</v>
       </c>
       <c r="B163" t="str">
-        <v>If you develop any of these warning signs for COVID-19, get emergency medical attention immediately:\n\n*   Trouble breathing\n*   Persistent pain or pressure in the chest\n*   New confusion \n*   Inability to awake or stay awake\n*   Bluish lips or face\n\nThere are other, less-common symptoms. Please call your medical provider if you have any symptoms that are severe or concerning to you.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call 911, tell the operator you have coronavirus symptoms so ambulance workers can be ready to treat you safely.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>Salary rates for most of the health care professionals being hired for this emergency are listed in the [CalHR Pay Scales](https://www.calhr.ca.gov/Pay%20Scales%20Library/PS_Sec_05.pdf) (pages 5.12 and 5.13). In addition, CalHR has established pay rates for medical roles that don’t have a corresponding regular classification and pay schedule, such as paramedics and EMTs. CalHR will determine specific salary and benefits after conducting a review of each application.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C163" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/healthcorps/</v>
       </c>
       <c r="D163" t="str">
         <v xml:space="preserve"> </v>
@@ -4620,10 +4620,10 @@
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>What are the pay and benefits for California Health Corps professionals?</v>
+        <v>Some healthcare professions are not listed. Are health professionals who are not listed (e.g., Medical Technicians, Lab Technicians, etc.) eligible for the California Health Corps?</v>
       </c>
       <c r="B164" t="str">
-        <v>Salary rates for most of the health care professionals being hired for this emergency are listed in the [CalHR Pay Scales](https://www.calhr.ca.gov/Pay%20Scales%20Library/PS_Sec_05.pdf) (pages 5.12 and 5.13). In addition, CalHR has established pay rates for medical roles that don’t have a corresponding regular classification and pay schedule, such as paramedics and EMTs. CalHR will determine specific salary and benefits after conducting a review of each application.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>California Health Corps are currently only accepting applications for the healthcare professions listed on the website. However, we are constantly re-evaluating our needs during this fluid situation and will open the registration for other professionals, if the need arises.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C164" t="str">
         <v>https://covid19.ca.gov/healthcorps/</v>
@@ -4646,10 +4646,10 @@
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>Some healthcare professions are not listed. Are health professionals who are not listed (e.g., Medical Technicians, Lab Technicians, etc.) eligible for the California Health Corps?</v>
+        <v>When can I expect to hear a response after completing my California Health Corps registration?</v>
       </c>
       <c r="B165" t="str">
-        <v>California Health Corps are currently only accepting applications for the healthcare professions listed on the website. However, we are constantly re-evaluating our needs during this fluid situation and will open the registration for other professionals, if the need arises.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>Currently we anticipate the process may take up to two weeks, since an incredible number of responses are received and need to prioritize certain parts of the state, where the needs are the greatest. We will begin to contact the volunteers after verification of credentials, and based on current and anticipated needs.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C165" t="str">
         <v>https://covid19.ca.gov/healthcorps/</v>
@@ -4672,10 +4672,10 @@
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>When can I expect to hear a response after completing my California Health Corps registration?</v>
+        <v>How do I return to the California Health Corps application after logging out?</v>
       </c>
       <c r="B166" t="str">
-        <v>Currently we anticipate the process may take up to two weeks, since an incredible number of responses are received and need to prioritize certain parts of the state, where the needs are the greatest. We will begin to contact the volunteers after verification of credentials, and based on current and anticipated needs.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>Visit [https://healthcarevolunteers.ca.gov/](https://healthcarevolunteers.ca.gov/) and use the account you created while applying to correct or update any information you want.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C166" t="str">
         <v>https://covid19.ca.gov/healthcorps/</v>
@@ -4698,10 +4698,10 @@
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>How do I return to the California Health Corps application after logging out?</v>
+        <v>Resources for the California Health Corps participants</v>
       </c>
       <c r="B167" t="str">
-        <v>Visit [https://healthcarevolunteers.ca.gov/](https://healthcarevolunteers.ca.gov/) and use the account you created while applying to correct or update any information you want.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>*   SNF Orientation: [SNF-Nursing-Staff-Orientation (PDF)](https://covid19.ca.gov/pdf/SNF-Nursing-Staff-Orientation.pdf)\n*   Program FAQ details: [CA-Health-Corps-FAQ (PDF)](https://covid19.ca.gov/pdf/CA-Health-Corps-FAQ.pdf)\n*   How to file a complaint: [How-to-file-a-complaint (PDF)](https://covid19.ca.gov/pdf/How-to-file-a-complaint.pdf)\n*   EMSA Pocket Travel Guide: [EMSA-Pocket-Travel-Guide (PDF)](https://covid19.ca.gov/pdf/EMSA-Pocket-Travel-Guide.pdf)\n*   Direct deposit: [std699-Direct-Deposit (PDF)](https://covid19.ca.gov/pdf/std699-Direct-Deposit.pdf)\n*   Travel Info: [CA-Health-Corps-Travel-Info (PDF)](https://covid19.ca.gov/pdf/CA-Health-Corps-Travel-Info.pdf)\n*   Travel expense claim: [Std262-Travel-Expense-Claim (PDF)](https://covid19.ca.gov/pdf/Std262-Travel-Expense-Claim.pdf)\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C167" t="str">
         <v>https://covid19.ca.gov/healthcorps/</v>
@@ -4724,10 +4724,10 @@
     </row>
     <row r="168">
       <c r="A168" t="str">
-        <v>Resources for the California Health Corps participants</v>
+        <v>Can a doctor with out of state Licence or foreign medical graduate without California license work for the California Health Corps?</v>
       </c>
       <c r="B168" t="str">
-        <v>*   SNF Orientation: [SNF-Nursing-Staff-Orientation (PDF)](https://covid19.ca.gov/pdf/SNF-Nursing-Staff-Orientation.pdf)\n*   Program FAQ details: [CA-Health-Corps-FAQ (PDF)](https://covid19.ca.gov/pdf/CA-Health-Corps-FAQ.pdf)\n*   How to file a complaint: [How-to-file-a-complaint (PDF)](https://covid19.ca.gov/pdf/How-to-file-a-complaint.pdf)\n*   EMSA Pocket Travel Guide: [EMSA-Pocket-Travel-Guide (PDF)](https://covid19.ca.gov/pdf/EMSA-Pocket-Travel-Guide.pdf)\n*   Direct deposit: [std699-Direct-Deposit (PDF)](https://covid19.ca.gov/pdf/std699-Direct-Deposit.pdf)\n*   Travel Info: [CA-Health-Corps-Travel-Info (PDF)](https://covid19.ca.gov/pdf/CA-Health-Corps-Travel-Info.pdf)\n*   Travel expense claim: [Std262-Travel-Expense-Claim (PDF)](https://covid19.ca.gov/pdf/Std262-Travel-Expense-Claim.pdf)\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>To be eligible for COVID-19 emergency medical staffing roles, you must:\n\n*   Have a valid California License for clinical practice (if you are a MD, DO, etc.) \n*   **OR** are a medical resident or nursing student \n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C168" t="str">
         <v>https://covid19.ca.gov/healthcorps/</v>
@@ -4750,13 +4750,13 @@
     </row>
     <row r="169">
       <c r="A169" t="str">
-        <v>Can a doctor with out of state Licence or foreign medical graduate without California license work for the California Health Corps?</v>
+        <v>Agriculture and livestock</v>
       </c>
       <c r="B169" t="str">
-        <v>To be eligible for COVID-19 emergency medical staffing roles, you must:\n\n*   Have a valid California License for clinical practice (if you are a MD, DO, etc.) \n*   **OR** are a medical resident or nursing student \n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>The [guidance for the agriculture and livestock industry](http://covid19.ca.gov/pdf/guidance-agriculture.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the agriculture and livestock industry](http://covid19.ca.gov/pdf/checklist-agriculture.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C169" t="str">
-        <v>https://covid19.ca.gov/healthcorps/</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D169" t="str">
         <v xml:space="preserve"> </v>
@@ -4776,10 +4776,10 @@
     </row>
     <row r="170">
       <c r="A170" t="str">
-        <v>Agriculture and livestock</v>
+        <v>Auto dealerships</v>
       </c>
       <c r="B170" t="str">
-        <v>The [guidance for the agriculture and livestock industry](http://covid19.ca.gov/pdf/guidance-agriculture.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the agriculture and livestock industry](http://covid19.ca.gov/pdf/checklist-agriculture.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the automobile dealerships and rental operators industry](http://covid19.ca.gov/pdf/guidance-auto-dealerships.pdf) provides guidelines to create a safer environment for workers.  \nReview the guidance, prepare a plan, and post the [checklist for the automobile dealerships and rental operators](http://covid19.ca.gov/pdf/checklist-auto-dealerships.pdf) industry in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C170" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4802,10 +4802,10 @@
     </row>
     <row r="171">
       <c r="A171" t="str">
-        <v>Auto dealerships</v>
+        <v>Childcare</v>
       </c>
       <c r="B171" t="str">
-        <v>The [guidance for the automobile dealerships and rental operators industry](http://covid19.ca.gov/pdf/guidance-auto-dealerships.pdf) provides guidelines to create a safer environment for workers.  \nReview the guidance, prepare a plan, and post the [checklist for the automobile dealerships and rental operators](http://covid19.ca.gov/pdf/checklist-auto-dealerships.pdf) industry in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>All childcare facilities can open with necessary modifications. The updated [guidance for childcare industry](https://files.covid19.ca.gov/pdf/guidance-childcare--en.pdf) provides guidelines to minimize the spread of COVID-19 and ensure the safety of children, providers, and families. As programs begin to reopen and other programs transition from emergency childcare for essential workers to enhanced regular operations, all providers must apply new and updated policies and requirements and must update their emergency preparedness plan.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C171" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4828,10 +4828,10 @@
     </row>
     <row r="172">
       <c r="A172" t="str">
-        <v>Childcare</v>
+        <v>Communications infrastructure</v>
       </c>
       <c r="B172" t="str">
-        <v>All childcare facilities can open with necessary modifications. The updated [guidance for childcare industry](http://covid19.ca.gov/pdf/guidance-childcare.pdf) provides guidelines to minimize the spread of COVID-19 and ensure the safety of children, providers, and families. As programs begin to reopen and other programs transition from emergency childcare for essential workers to enhanced regular operations, all providers must apply new and updated policies and requirements and must update their emergency preparedness plan.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the communications infrastructure industry](http://covid19.ca.gov/pdf/guidance-communications.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the communications infrastructure industry](http://covid19.ca.gov/pdf/checklist-communications.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C172" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4854,10 +4854,10 @@
     </row>
     <row r="173">
       <c r="A173" t="str">
-        <v>Communications infrastructure</v>
+        <v>Construction</v>
       </c>
       <c r="B173" t="str">
-        <v>The [guidance for the communications infrastructure industry](http://covid19.ca.gov/pdf/guidance-communications.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the communications infrastructure industry](http://covid19.ca.gov/pdf/checklist-communications.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [guidance for the construction industry](http://covid19.ca.gov/pdf/guidance-construction.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the construction industry](http://covid19.ca.gov/pdf/checklist-construction.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C173" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4880,10 +4880,10 @@
     </row>
     <row r="174">
       <c r="A174" t="str">
-        <v>Construction</v>
+        <v>Day camps</v>
       </c>
       <c r="B174" t="str">
-        <v>This [guidance for the construction industry](http://covid19.ca.gov/pdf/guidance-construction.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the construction industry](http://covid19.ca.gov/pdf/checklist-construction.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for day camps](http://covid19.ca.gov/pdf/guidance-daycamps.pdf) provides guidelines to create a plan for safe re-opening.  Implementation of these guidelines should be tailored for each setting. Implementation requires training and support for staff and adequate consideration of camper and family needs. All decisions about following these recommendations should be made in collaboration with local health officials and other authorities, and should depend on the levels of COVID-19 community transmission and the capacities of the local public health and healthcare systems, among other relevant factors.  \n  \nRecreational team sports are not permitted and will be subject to separate guidance.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)&lt;!-- skill, clinic, youth, sports, league, recreational, team --&gt;</v>
       </c>
       <c r="C174" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4906,10 +4906,10 @@
     </row>
     <row r="175">
       <c r="A175" t="str">
-        <v>Day camps</v>
+        <v>Delivery services</v>
       </c>
       <c r="B175" t="str">
-        <v>The [guidance for day camps](http://covid19.ca.gov/pdf/guidance-daycamps.pdf) provides guidelines to create a plan for safe re-opening.  Implementation of these guidelines should be tailored for each setting. Implementation requires training and support for staff and adequate consideration of camper and family needs. All decisions about following these recommendations should be made in collaboration with local health officials and other authorities, and should depend on the levels of COVID-19 community transmission and the capacities of the local public health and healthcare systems, among other relevant factors.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the delivery services industry](http://covid19.ca.gov/pdf/guidance-delivery-services.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the delivery services industry](http://covid19.ca.gov/pdf/checklist-delivery-services.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C175" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4932,10 +4932,10 @@
     </row>
     <row r="176">
       <c r="A176" t="str">
-        <v>Delivery services</v>
+        <v>Energy and utilities</v>
       </c>
       <c r="B176" t="str">
-        <v>The [guidance for the delivery services industry](http://covid19.ca.gov/pdf/guidance-delivery-services.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the delivery services industry](http://covid19.ca.gov/pdf/checklist-delivery-services.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the energy and utilities industry](http://covid19.ca.gov/pdf/guidance-energy.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post  the [checklist for the energy and utilities industry](http://covid19.ca.gov/pdf/checklist-energy.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C176" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4958,10 +4958,10 @@
     </row>
     <row r="177">
       <c r="A177" t="str">
-        <v>Energy and utilities</v>
+        <v>Family friendly practices for employers</v>
       </c>
       <c r="B177" t="str">
-        <v>The [guidance for the energy and utilities industry](http://covid19.ca.gov/pdf/guidance-energy.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post  the [checklist for the energy and utilities industry](http://covid19.ca.gov/pdf/checklist-energy.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for family friendly practices for employers](http://covid19.ca.gov/pdf/guidance-familyfriendlypracticesemployers.pdf) provides guidelines for family-friendly practices to keep employees safe and be responsive to their needs in order to ensure continued productivity. As workplaces reopen, employees will require both child care supports and workplace flexibility. Work-life balance policies will become even more important and continued investment in family-friendly workplace policies by employers is critical.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C177" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4984,10 +4984,10 @@
     </row>
     <row r="178">
       <c r="A178" t="str">
-        <v>Family friendly practices for employers</v>
+        <v>Food packing</v>
       </c>
       <c r="B178" t="str">
-        <v>The [guidance for family friendly practices for employers](http://covid19.ca.gov/pdf/guidance-familyfriendlypracticesemployers.pdf) provides guidelines for family-friendly practices to keep employees safe and be responsive to their needs in order to ensure continued productivity. As workplaces reopen, employees will require both child care supports and workplace flexibility. Work-life balance policies will become even more important and continued investment in family-friendly workplace policies by employers is critical.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for facilities that process or pack meat, dairy, or produce](http://covid19.ca.gov/pdf/guidance-food-packing.pdf) provides guidelines to create a safer environment for workers.  \nReview the guidance, prepare a plan, and post the [checklist for facilities that process or pack meat, dairy or produce](http://covid19.ca.gov/pdf/checklist-food-packing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C178" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5010,10 +5010,10 @@
     </row>
     <row r="179">
       <c r="A179" t="str">
-        <v>Food packing</v>
+        <v>Hotels and lodging</v>
       </c>
       <c r="B179" t="str">
-        <v>The [guidance for facilities that process or pack meat, dairy, or produce](http://covid19.ca.gov/pdf/guidance-food-packing.pdf) provides guidelines to create a safer environment for workers.  \nReview the guidance, prepare a plan, and post the [checklist for facilities that process or pack meat, dairy or produce](http://covid19.ca.gov/pdf/checklist-food-packing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [guidance for the hotels and lodging](http://covid19.ca.gov/pdf/guidance-hotels.pdf) provides guidelines to counties not [approved for variance](https://covid19.ca.gov/roadmap-counties/) create a safer environment for workers.\n\nUnless your county has been approved to move further in the roadmap, hotels should only open for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or providing housing solutions, including measures to protect homeless populations.\n\nSeparate guidance for hotels and lodging services in counties with variance attestation [can be found here](https://covid19.ca.gov/pdf/guidance-hotels-lodging-rentals.pdf).\n\nReview the guidance, prepare a plan, and post the [checklist for hotels and lodging](http://covid19.ca.gov/pdf/checklist-hotels.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C179" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5036,10 +5036,10 @@
     </row>
     <row r="180">
       <c r="A180" t="str">
-        <v>Hotels and lodging</v>
+        <v>Life sciences</v>
       </c>
       <c r="B180" t="str">
-        <v>This [guidance for the hotels and lodging](http://covid19.ca.gov/pdf/guidance-hotels.pdf) provides guidelines to create a safer environment for workers.\n\nUnless your county has been approved to move further in the roadmap, hotels should only open for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or providing housing solutions, including measures to protect homeless populations.\n\nReview the guidance, prepare a plan, and post the [checklist for hotels and lodging](http://covid19.ca.gov/pdf/checklist-hotels.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the life sciences industry](http://covid19.ca.gov/pdf/guidance-life-sciences.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the life sciences industry](http://covid19.ca.gov/pdf/checklist-life-sciences.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C180" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5062,10 +5062,10 @@
     </row>
     <row r="181">
       <c r="A181" t="str">
-        <v>Life sciences</v>
+        <v>Limited services</v>
       </c>
       <c r="B181" t="str">
-        <v>The [guidance for the life sciences industry](http://covid19.ca.gov/pdf/guidance-life-sciences.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the life sciences industry](http://covid19.ca.gov/pdf/checklist-life-sciences.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Limited Services are defined as those which do not generally require close contact. Follow this [guidance for Limited Services](https://covid19.ca.gov/pdf/guidance-limited-services.pdf) to create a safer environment for workers and patrons.\n\nFaith-based counseling can reopen within the following parameters:\n\n1.  Counselling services are permissible in-person where the service cannot reasonably be practiced remotely;\n2.  Counselling services should adopt state guidance on Limited Services, where applicable;\n3.  This designation does not permit gatherings beyond counselling to members of a single household.\n\nReview the guidance, prepare a plan, and post the [checklist for Limited Services](https://covid19.ca.gov/pdf/checklist-limited-services.pdf) in your workplace to show clients and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C181" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5088,10 +5088,10 @@
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>Limited services</v>
+        <v>Logistics and warehousing facilities</v>
       </c>
       <c r="B182" t="str">
-        <v>Limited Services are defined as those which do not generally require close contact. Follow this [guidance for Limited Services](https://covid19.ca.gov/pdf/guidance-limited-services.pdf) to create a safer environment for workers and patrons.\n\nFaith-based counseling can reopen within the following parameters:\n\n1.  Counselling services are permissible in-person where the service cannot reasonably be practiced remotely;\n2.  Counselling services should adopt state guidance on Limited Services, where applicable;\n3.  This designation does not permit gatherings beyond counselling to members of a single household.\n\nReview the guidance, prepare a plan, and post the [checklist for Limited Services](https://covid19.ca.gov/pdf/checklist-limited-services.pdf) in your workplace to show clients and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for businesses operating in the logistics/warehousing industry](http://covid19.ca.gov/pdf/guidance-logistics-warehousing.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post  the [checklist for the logistics/warehousing industry](http://covid19.ca.gov/pdf/checklist-logistics-warehousing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C182" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5114,10 +5114,10 @@
     </row>
     <row r="183">
       <c r="A183" t="str">
-        <v>Logistics and warehousing facilities</v>
+        <v>Manufacturing</v>
       </c>
       <c r="B183" t="str">
-        <v>The [guidance for businesses operating in the logistics/warehousing industry](http://covid19.ca.gov/pdf/guidance-logistics-warehousing.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post  the [checklist for the logistics/warehousing industry](http://covid19.ca.gov/pdf/checklist-logistics-warehousing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the manufacturing industry](http://covid19.ca.gov/pdf/guidance-manufacturing.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the manufacturing industry](http://covid19.ca.gov/pdf/checklist-manufacturing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C183" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5140,10 +5140,10 @@
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>Manufacturing</v>
+        <v>Mining and logging</v>
       </c>
       <c r="B184" t="str">
-        <v>The [guidance for the manufacturing industry](http://covid19.ca.gov/pdf/guidance-manufacturing.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the manufacturing industry](http://covid19.ca.gov/pdf/checklist-manufacturing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the mining and logging industries](http://covid19.ca.gov/pdf/guidance-mining-logging.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the mining and logging industries](http://covid19.ca.gov/pdf/checklist-mining-logging.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C184" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5166,10 +5166,10 @@
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>Mining and logging</v>
+        <v>Music, film, and TV production</v>
       </c>
       <c r="B185" t="str">
-        <v>The [guidance for the mining and logging industries](http://covid19.ca.gov/pdf/guidance-mining-logging.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the mining and logging industries](http://covid19.ca.gov/pdf/checklist-mining-logging.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Music, TV and film production may resume in California, recommended no sooner than June 12, 2020 and subject to approval by county public health officers within the jurisdictions of operations following their review of local epidemiological data including cases per 100,000 population, rate of test positivity, and local preparedness to support a health care surge, vulnerable populations, contact tracing and testing.  \n  \nTo reduce the risk of COVID-19 transmission, productions, cast, crew and other industry workers should abide by safety protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should adhere to [Office Workspace guidelines](https://covid19.ca.gov/industry-guidance/#top) published by the California Department of Public Health and the California Department of Industrial Relations, to reduce the risk of COVID-19 transmission.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C185" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5192,10 +5192,10 @@
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>Music, film, and TV production</v>
+        <v>Office workspaces</v>
       </c>
       <c r="B186" t="str">
-        <v>Music, TV and film production may resume in California, recommended no sooner than June 12, 2020 and subject to approval by county public health officers within the jurisdictions of operations following their review of local epidemiological data including cases per 100,000 population, rate of test positivity, and local preparedness to support a health care surge, vulnerable populations, contact tracing and testing.  \n  \nTo reduce the risk of COVID-19 transmission, productions, cast, crew and other industry workers should abide by safety protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should adhere to [Office Workspace guidelines](https://covid19.ca.gov/industry-guidance/#top) published by the California Department of Public Health and the California Department of Industrial Relations, to reduce the risk of COVID-19 transmission.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for office workspaces](http://covid19.ca.gov/pdf/guidance-office-workspaces.pdf) to create a safer environment for workers.\n\nFaith-based office workspaces can reopen within the following parameters:\n\n1.  Faith-based facilities are considered “offices” only for those employed by the organization and where the facility is their regular place of work.\n2.  The employer should implement state guidance relating to offices before reopening the facility for employees.\n3.  This designation does not permit gatherings of non-employees, such as the organization’s congregation.\n\nReview the guidance, prepare a plan, and post the [checklist for office workspaces](http://covid19.ca.gov/pdf/checklist-office-workspaces.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C186" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5218,10 +5218,10 @@
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>Office workspaces</v>
+        <v>Outdoor museums</v>
       </c>
       <c r="B187" t="str">
-        <v>Follow this [guidance for office workspaces](http://covid19.ca.gov/pdf/guidance-office-workspaces.pdf) to create a safer environment for workers.\n\nFaith-based office workspaces can reopen within the following parameters:\n\n1.  Faith-based facilities are considered “offices” only for those employed by the organization and where the facility is their regular place of work.\n2.  The employer should implement state guidance relating to offices before reopening the facility for employees.\n3.  This designation does not permit gatherings of non-employees, such as the organization’s congregation.\n\nReview the guidance, prepare a plan, and post the [checklist for office workspaces](http://covid19.ca.gov/pdf/checklist-office-workspaces.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for outdoor museums](https://covid19.ca.gov/pdf/guidance-outdoor-museums.pdf) to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for outdoor museums](http://covid19.ca.gov/pdf/checklist-outdoor-museums.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C187" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5244,10 +5244,10 @@
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>Outdoor museums</v>
+        <v>Places of worship</v>
       </c>
       <c r="B188" t="str">
-        <v>Follow this [guidance for outdoor museums](https://covid19.ca.gov/pdf/guidance-outdoor-museums.pdf) to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for outdoor museums](http://covid19.ca.gov/pdf/checklist-outdoor-museums.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [guidance for the places of worship](http://covid19.ca.gov/pdf/guidance-places-of-worship.pdf) provides guidelines to create a safer environment for workers.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)&lt;!-- wedding, funeral, event, assembly, choir, chorus, congregation, congregate, congregation, crowd, group --&gt;</v>
       </c>
       <c r="C188" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5270,10 +5270,10 @@
     </row>
     <row r="189">
       <c r="A189" t="str">
-        <v>Places of worship</v>
+        <v>Ports</v>
       </c>
       <c r="B189" t="str">
-        <v>This [guidance for the places of worship](http://covid19.ca.gov/pdf/guidance-places-of-worship.pdf) provides guidelines to create a safer environment for workers.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [guidance for the port industry](http://covid19.ca.gov/pdf/guidance-ports.pdf) provides guidelines to create a safer environment for workers. Review the guidance, prepare a plan, and post the [checklist for the port industry](http://covid19.ca.gov/pdf/checklist-ports.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C189" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5296,10 +5296,10 @@
     </row>
     <row r="190">
       <c r="A190" t="str">
-        <v>Ports</v>
+        <v>Professional sports (without live audiences)</v>
       </c>
       <c r="B190" t="str">
-        <v>This [guidance for the port industry](http://covid19.ca.gov/pdf/guidance-ports.pdf) provides guidelines to create a safer environment for workers. Review the guidance, prepare a plan, and post the [checklist for the port industry](http://covid19.ca.gov/pdf/checklist-ports.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Professional sports in California may resume training and competition without live audiences, recommended no sooner than June 12, 2020 and subject to approval by county public health officers within the jurisdiction of operations following their review of local epidemiological data including cases per 100,000 population, rate of test positivity, and local preparedness to support a health care surge, vulnerable populations, contact tracing and testing.  \n  \nTo reduce the risk of COVID-19 transmission, athletes, coaching staff, medical staff, broadcasting staff and others at sporting facilities or events should abide by COVID-19 protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should adhere to [Office Workspace guidelines](https://covid19.ca.gov/pdf/guidance-office-workspaces.pdf) published by the California Department of Public Health and the California Department of Industrial Relations, to reduce the risk of COVID-19 transmission. Retail staff should adhere to [Retail guidelines](https://covid19.ca.gov/pdf/guidance-retail.pdf) published by the California Department of Public Health and the California Department of Industrial Relations, to reduce the risk of COVID-19 transmission.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C190" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5322,10 +5322,10 @@
     </row>
     <row r="191">
       <c r="A191" t="str">
-        <v>Professional sports (without live audiences)</v>
+        <v>Public transit and intercity passenger rail</v>
       </c>
       <c r="B191" t="str">
-        <v>Professional sports in California may resume training and competition without live audiences, recommended no sooner than June 12, 2020 and subject to approval by county public health officers within the jurisdiction of operations following their review of local epidemiological data including cases per 100,000 population, rate of test positivity, and local preparedness to support a health care surge, vulnerable populations, contact tracing and testing.  \n  \nTo reduce the risk of COVID-19 transmission, athletes, coaching staff, medical staff, broadcasting staff and others at sporting facilities or events should abide by COVID-19 protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should adhere to [Office Workspace guidelines](https://covid19.ca.gov/pdf/guidance-office-workspaces.pdf) published by the California Department of Public Health and the California Department of Industrial Relations, to reduce the risk of COVID-19 transmission. Retail staff should adhere to [Retail guidelines](https://covid19.ca.gov/pdf/guidance-retail.pdf) published by the California Department of Public Health and the California Department of Industrial Relations, to reduce the risk of COVID-19 transmission.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [guidance for public transit agencies](http://covid19.ca.gov/pdf/guidance-transit-rail.pdf) provides guidelines to create a safer environment for workers.  \nReview the guidance, prepare a plan, and post the [checklist for public transit agencies](http://covid19.ca.gov/pdf/checklist-transit-rail.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C191" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5348,10 +5348,10 @@
     </row>
     <row r="192">
       <c r="A192" t="str">
-        <v>Public transit and intercity passenger rail</v>
+        <v>Real estate transaction</v>
       </c>
       <c r="B192" t="str">
-        <v>This [guidance for public transit agencies](http://covid19.ca.gov/pdf/guidance-transit-rail.pdf) provides guidelines to create a safer environment for workers.  \nReview the guidance, prepare a plan, and post the [checklist for public transit agencies](http://covid19.ca.gov/pdf/checklist-transit-rail.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [guidance for businesses operating in the real estate industry](http://covid19.ca.gov/pdf/guidance-real-estate.pdf) provides guidelines to create a safer environment for workers.  \nReview the guidance, prepare a plan, and post the [checklist for the real estate industry](http://covid19.ca.gov/pdf/checklist-real-estate.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C192" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5374,10 +5374,10 @@
     </row>
     <row r="193">
       <c r="A193" t="str">
-        <v>Real estate transaction</v>
+        <v>Retail</v>
       </c>
       <c r="B193" t="str">
-        <v>This [guidance for businesses operating in the real estate industry](http://covid19.ca.gov/pdf/guidance-real-estate.pdf) provides guidelines to create a safer environment for workers.  \nReview the guidance, prepare a plan, and post the [checklist for the real estate industry](http://covid19.ca.gov/pdf/checklist-real-estate.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for retailers](http://covid19.ca.gov/pdf/guidance-retail.pdf) to create a safer environment for workers and customers.\n\nRetailers and libraries can re-open, along with the manufacturing and logistics sectors that support retail. Drive-in and movie theaters can re-open with additional considerations.\n\nRetail doesn’t include personal services such as beauty salons, but does include the sale of goods such as:\n\n*   Bookstores\n*   Jewelry stores\n*   Toy stores\n*   Clothing and shoe stores\n*   Home and furnishing stores\n*   Sporting goods stores\n*   Florists\n\nRetail stores identified in the [essential workforce list](https://covid19.ca.gov/essential-workforce/) can open for in-store shopping. They include:\n\n*   Retail facilities specializing in medical goods and supplies\n*   Grocery stores, pharmacies, convenience stores, and other retail that sells food or beverage products, and animal/pet food\n*   Fuel centers such as gas stations and truck stops\n*   Hardware and building materials stores, consumer electronics, technology and appliances retail\n\nReview the guidance, prepare a plan, and post the [checklist for retail](http://covid19.ca.gov/pdf/checklist-retail.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C193" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5400,10 +5400,10 @@
     </row>
     <row r="194">
       <c r="A194" t="str">
-        <v>Retail</v>
+        <v>Schools</v>
       </c>
       <c r="B194" t="str">
-        <v>Follow this [guidance for retailers](http://covid19.ca.gov/pdf/guidance-retail.pdf) to create a safer environment for workers and customers.\n\nRetailers and libraries can re-open, along with the manufacturing and logistics sectors that support retail. Drive-in and movie theaters can re-open with additional considerations.\n\nRetail doesn’t include personal services such as beauty salons, but does include the sale of goods such as:\n\n*   Bookstores\n*   Jewelry stores\n*   Toy stores\n*   Clothing and shoe stores\n*   Home and furnishing stores\n*   Sporting goods stores\n*   Florists\n\nRetail stores identified in the [essential workforce list](https://covid19.ca.gov/essential-workforce/) can open for in-store shopping. They include:\n\n*   Retail facilities specializing in medical goods and supplies\n*   Grocery stores, pharmacies, convenience stores, and other retail that sells food or beverage products, and animal/pet food\n*   Fuel centers such as gas stations and truck stops\n*   Hardware and building materials stores, consumer electronics, technology and appliances retail\n\nReview the guidance, prepare a plan, and post the [checklist for retail](http://covid19.ca.gov/pdf/checklist-retail.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [interim guidance for schools and school-based programs](http://covid19.ca.gov/pdf/guidance-schools.pdf) provides guidelines to create a safer environment for student, family, and staff populations. This guidance will be updated as new data and practices emerge. The guidelines and considerations do not reflect the full scope of issues that school communities will need to address, which range from day-to-day site-based logistics to the social and emotional well-being of students and staff. Further guidance is forthcoming, including on school-based sports and extracurricular activities. All decisions about following this guidance should be made in collaboration with local health officials and other authorities.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C194" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5426,10 +5426,10 @@
     </row>
     <row r="195">
       <c r="A195" t="str">
-        <v>Schools</v>
+        <v>Support for working families</v>
       </c>
       <c r="B195" t="str">
-        <v>This [interim guidance for schools and school-based programs](http://covid19.ca.gov/pdf/guidance-schools.pdf) provides guidelines to create a safer environment for student, family, and staff populations. This guidance will be updated as new data and practices emerge. The guidelines and considerations do not reflect the full scope of issues that school communities will need to address, which range from day-to-day site-based logistics to the social and emotional well-being of students and staff. Further guidance is forthcoming, including on school-based sports and extracurricular activities. All decisions about following this guidance should be made in collaboration with local health officials and other authorities.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [support for working families](http://covid19.ca.gov/pdf/guidance-supportworkingfamilies.pdf) guidance provides information to help you locate child care, find assistance to pay for child care, and connect you to additional supports for your family. As stay-at-home orders are lifted for additional industries to promote California’s economic recovery, the need for child care and other supports for working families increases.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C195" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5452,10 +5452,10 @@
     </row>
     <row r="196">
       <c r="A196" t="str">
-        <v>Support for working families</v>
+        <v>Shopping centers</v>
       </c>
       <c r="B196" t="str">
-        <v>The [support for working families](http://covid19.ca.gov/pdf/guidance-supportworkingfamilies.pdf) guidance provides information to help you locate child care, find assistance to pay for child care, and connect you to additional supports for your family. As stay-at-home orders are lifted for additional industries to promote California’s economic recovery, the need for child care and other supports for working families increases.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for shopping centers](https://covid19.ca.gov/pdf/guidance-shopping-centers.pdf) to create a safer environment for workers and customers.  \n  \nInterior stores in shopping malls can do curbside pickup with modifications.  \n  \nReview the guidance, prepare a plan, and post the [checklist for shopping centers](https://covid19.ca.gov/pdf/checklist-shopping-centers.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C196" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5478,13 +5478,13 @@
     </row>
     <row r="197">
       <c r="A197" t="str">
-        <v>Shopping centers</v>
+        <v>Is there a convalescent blood plasma donation center near me?</v>
       </c>
       <c r="B197" t="str">
-        <v>Follow this [guidance for shopping centers](https://covid19.ca.gov/pdf/guidance-shopping-centers.pdf) to create a safer environment for workers and customers.  \n  \nInterior stores in shopping malls can do curbside pickup with modifications.  \n  \nReview the guidance, prepare a plan, and post the [checklist for shopping centers](https://covid19.ca.gov/pdf/checklist-shopping-centers.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Statewide industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Locate a donation center\n------------------------\n\nFind the blood center near you collecting COVID-19 blood plasma.\n\n[See the plasma donation center lookup](https://covid19.ca.gov/plasma#plasma-lookup)\n\nMore info: [Survivors of COVID-19: Donate your plasma](https://covid19.ca.gov/plasma/)</v>
       </c>
       <c r="C197" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/plasma/</v>
       </c>
       <c r="D197" t="str">
         <v xml:space="preserve"> </v>
@@ -5504,13 +5504,13 @@
     </row>
     <row r="198">
       <c r="A198" t="str">
-        <v>Is there a convalescent blood plasma donation center near me?</v>
+        <v>Where can I apply for unemployment?</v>
       </c>
       <c r="B198" t="str">
-        <v>Locate a donation center\n------------------------\n\nFind the blood center near you collecting COVID-19 blood plasma.\n\n[See the plasma donation center lookup](https://covid19.ca.gov/plasma#plasma-lookup)\n\nMore info: [Survivors of COVID-19: Donate your plasma](https://covid19.ca.gov/plasma/)</v>
+        <v>If you lost your job or had your hours reduced, and meet eligibility requirements, you may be eligible to receive Unemployment Insurance (UI) benefits from California’s Employment Development Department (EDD). Check the [guide to applying for unemployment benefits](https://unemployment.edd.ca.gov/guide).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C198" t="str">
-        <v>https://covid19.ca.gov/plasma/</v>
+        <v>Editorial</v>
       </c>
       <c r="D198" t="str">
         <v xml:space="preserve"> </v>
@@ -5530,10 +5530,10 @@
     </row>
     <row r="199">
       <c r="A199" t="str">
-        <v>Where can I apply for unemployment?</v>
+        <v xml:space="preserve">Can I go to the movies? </v>
       </c>
       <c r="B199" t="str">
-        <v>If you lost your job or had your hours reduced, and meet eligibility requirements, you may be eligible to receive Unemployment Insurance (UI) benefits from California’s Employment Development Department (EDD). Check the [guide to applying for unemployment benefits](https://unemployment.edd.ca.gov/guide).</v>
+        <v>Yes, movie theaters and drive-in movie theaters can open statewide with modifications to support physical distancing. &lt;!-- film, imax --&gt;</v>
       </c>
       <c r="C199" t="str">
         <v>Editorial</v>
@@ -5556,10 +5556,10 @@
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>Can I go to the movies? Are movie theaters open?</v>
+        <v>Are hotels allowed to open?</v>
       </c>
       <c r="B200" t="str">
-        <v>Yes, movie theaters and drive-in movie theaters can open statewide with modifications to support physical distancing.</v>
+        <v>[Counties that have received approval from the State](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/County_Variance_Attestation_Form.aspx) may open hotels, lodging and short term rentals for tourism and individual travel as long as they follow [state guidance](https://covid19.ca.gov/pdf/guidance-hotels-lodging-rentals.pdf) for public health and safety. Large meeting venues, banquet halls or convention centers should remain closed. All other counties [should only open hotels and lodging](https://covid19.ca.gov/pdf/guidance-hotels.pdf) for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or housing solutions, including measures to protect homeless populations. &lt;!-- motel, vacation, airbnb, vrbo, rental home --&gt;</v>
       </c>
       <c r="C200" t="str">
         <v>Editorial</v>
@@ -5582,10 +5582,10 @@
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>Are hotels allowed to open?</v>
+        <v>Are restaurants allowed to open?</v>
       </c>
       <c r="B201" t="str">
-        <v>[Counties that have received approval from the State](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/County_Variance_Attestation_Form.aspx) may open hotels, lodging and short term rentals for tourism and individual travel as long as they follow [state guidance](https://covid19.ca.gov/pdf/guidance-hotels-lodging-rentals.pdf) for public health and safety. Large meeting venues, banquet halls or convention centers should remain closed. All other counties [should only open hotels and lodging](https://covid19.ca.gov/pdf/guidance-hotels.pdf) for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or housing solutions, including measures to protect homeless populations.</v>
+        <v>Restaurants across the state can be open for take out or delivery services. [Restaurants, bars, wineries and lounges](https://covid19.ca.gov/pdf/guidance-restaurants-bars.pdf) may be open [only in counties that have received approval from the State](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/County_Variance_Attestation_Form.aspx). &lt;!-- food, pub, brew, craft distilleries --&gt;</v>
       </c>
       <c r="C201" t="str">
         <v>Editorial</v>
@@ -5608,10 +5608,10 @@
     </row>
     <row r="202">
       <c r="A202" t="str">
-        <v>Are restaurants allowed to open?</v>
+        <v>Can I get my nails done? Can I get a massage? Can I get a facial? Can I get a tattoo?</v>
       </c>
       <c r="B202" t="str">
-        <v>Restaurants across the state can be open for take out or delivery services. [Restaurants, bars, wineries and lounges](https://covid19.ca.gov/pdf/guidance-restaurants-bars.pdf) may be open [only in counties that have received approval from the State](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/County_Variance_Attestation_Form.aspx).</v>
+        <v>It depends. If your county has been approved to move further in the Resilience Roadmap, then personal care services like nail salons, massage clinics, skin care, tattoo parlors, and piercing shops may reopen in your area. See the list of [counties with a variance](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/County_Variance_Attestation_Form.aspx).\n\nMore info: [Stay home Q&amp;Q](https://covid19.ca.gov/stay-home-except-for-essential-needs/) &lt;!-- spa, esthetician, electrolysis, waxing, cosmetology services, electrology, body art --&gt;</v>
       </c>
       <c r="C202" t="str">
         <v>Editorial</v>
@@ -5634,10 +5634,10 @@
     </row>
     <row r="203">
       <c r="A203" t="str">
-        <v>What about nail salons? Can I get my nails done?</v>
+        <v>Can my pet test positive for coronavirus? Can I take my pet to the vet?</v>
       </c>
       <c r="B203" t="str">
-        <v>[Counties that are approved to progress further into the Resilience Roadmap](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/County_Variance_Attestation_Form.aspx) can decide to open the following industries but are strongly encouraged to wait until June 19, 2020:\n\nPersonal services, like nail salons, body waxing and tattoo parlors\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>While we are still learning about coronavirus, the risk of your pet testing positive for coronavirus is low. Because [there is still a risk](https://www.cdc.gov/coronavirus/2019-ncov/animals/pets-other-animals.html), keep your pets away from other pets and people outside of your household. Do not put face coverings on pets as this could harm your pet.\n\nYou can go to the vet or pet hospital if your pet is sick. Remember to wear a cloth face covering and to distance yourself at least 6 feet from other pets and owners.</v>
       </c>
       <c r="C203" t="str">
         <v>Editorial</v>
@@ -5658,35 +5658,9 @@
         <v>202</v>
       </c>
     </row>
-    <row r="204">
-      <c r="A204" t="str">
-        <v>Can my pet test positive for coronavirus? Can I take my pet to the vet?</v>
-      </c>
-      <c r="B204" t="str">
-        <v>While we are still learning about coronavirus, the risk of your pet testing positive for coronavirus is low. Because [there is still a risk](https://www.cdc.gov/coronavirus/2019-ncov/animals/pets-other-animals.html), keep your pets away from other pets and people outside of your household. Do not put face coverings on pets as this could harm your pet.\n\nYou can go to the vet or pet hospital if your pet is sick. Remember to wear a cloth face covering and to distance yourself at least 6 feet from other pets and owners.</v>
-      </c>
-      <c r="C204" t="str">
-        <v>Editorial</v>
-      </c>
-      <c r="D204" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E204" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F204" t="str">
-        <v>false</v>
-      </c>
-      <c r="G204" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H204" t="str">
-        <v>203</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H204"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H203"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
latest manual editorial items
</commit_message>
<xml_diff>
--- a/qnacrawler/merged.xlsx
+++ b/qnacrawler/merged.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H218"/>
+  <dimension ref="A1:H224"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -671,7 +671,7 @@
         <v>What is open with county variance?</v>
       </c>
       <c r="B12" t="str">
-        <v>The following may open only in [counties approved to move further in the Resilience Roadmap](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/County_Variance_Attestation_Form.aspx):\n\n*   Hotels (for tourism and individual travel)\n*   Campgrounds and outdoor recreation\n*   Racetracks\n*   Casinos\n\nCounties that have remained on the County Monitoring List for 3 or more consecutive days are required to **close** some industries. The closures will apply for a minimum of three weeks and are subject to an extension based on epidemiologic indicators.\n\nThe following sectors must **close** indoor operations and activities unless they can be modified to operate outside or by pick-up:\n\n*   Gyms and fitness centers, like yoga and dance studios\n*   Places of worship and cultural ceremonies, like weddings and funerals\n*   Indoor protests\n*   Offices for non-essential (non-critical infrastructure) sectors\n*   Personal care services, like nail salons, body waxing and tattoo parlors\n*   Hair salons and barbershops\n*   Shopping malls\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>The following may open only in [counties approved to move further in the Resilience Roadmap](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/County_Variance_Attestation_Form.aspx):\n\n*   Hotels (for tourism and individual travel)\n*   Campgrounds and outdoor recreation\n*   Racetracks\n*   Casinos\n\nCounties that have remained on the County Monitoring List for 3 or more consecutive days are required to **close** some industries.\n\nThe following sectors must **close** indoor operations and activities unless they can be modified to operate outside or by pick-up:\n\n*   Gyms and fitness centers, like yoga and dance studios\n*   Places of worship and cultural ceremonies, like weddings and funerals\n*   Indoor protests\n*   Offices for non-essential (non-critical infrastructure) sectors\n*   Personal care services, like nail salons and body waxing\n*   Hair salons and barbershops\n*   Shopping malls\n\nShops that offer tattoos, piercings and electrolysis may not be operated outdoors and must close.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C12" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -827,7 +827,7 @@
         <v>Can I get a haircut?</v>
       </c>
       <c r="B18" t="str">
-        <v>It depends. All indoor operations of hair salon and barbershops have closed in counties on the county monitoring list for 3 consecutive days. [Learn more about which counties are on the list](https://covid19.ca.gov/roadmap-counties/).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>It depends. Hair salons and barbershops are open in counties not on the [County Monitoring List](https://covid19.ca.gov/roadmap-counties/). However, all indoor operations for these businesses are closed in counties that are on this list. Outdoor hair services may be available.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C18" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -905,7 +905,7 @@
         <v>How do I vote?</v>
       </c>
       <c r="B21" t="str">
-        <v>Elections are an essential activity, and the [Governor has issued executive orders to ensure elections are safe and accessible](https://www.gov.ca.gov/2020/05/08/governor-newsom-issues-executive-order-to-protect-public-health-by-mailing-every-registered-voter-a-ballot-ahead-of-the-november-general-election/). Vote-by-mail ballots will be sent to all registered voters for the November 3, 2020 General Election. Additionally, many in-person voting opportunities will be available: counties are required to provide [three days of early voting](https://www.gov.ca.gov/2020/06/03/governor-newsom-signs-executive-order-on-safe-secure-and-accessible-general-election-in-november/) starting the Saturday before the election, and open ballot drop-box locations between October 6 and November 3, 2020. The Secretary of State and the California Department of Public Health are working on additional guidance to ensure that all Californians are able to participate in elections safely. Except where suspended by Executive Order, existing laws addressing the use of vote-by-mail ballots in California elections remain in effect.\n\nOf course, whenever you engage in any permissible activity—including the collection and drop-off of ballots, or other election-related activities (such as the collection of signatures to qualify candidates or measures for the ballot)—adhere to physical distancing and other applicable public health directives.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Elections are an essential activity. The Governor has issued [executive orders to ensure elections are safe and accessible](https://www.gov.ca.gov/2020/05/08/governor-newsom-issues-executive-order-to-protect-public-health-by-mailing-every-registered-voter-a-ballot-ahead-of-the-november-general-election/). Vote-by-mail ballots will be sent to all registered voters for the November 3, 2020 General Election. Most counties will provide [three days of early voting](https://www.gov.ca.gov/2020/06/03/governor-newsom-signs-executive-order-on-safe-secure-and-accessible-general-election-in-november/) in-person starting the Saturday before the election.Open ballot drop-box locations will be available between October 6 and November 3, 2020. Existing laws addressing the use of vote-by-mail ballots in California elections remain in effect except where suspended by Executive Order. Find [guidance for the safe administration of elections](https://elections.cdn.sos.ca.gov/ccrov/pdf/2020/july/20154jl.pdf) during COVID-19.\n\n Visit [online voter registration](https://registertovote.ca.gov/) to register to vote or check your voter registration status. \n\nPractice physical distancing and follow other applicable public health directives while engaged in election-related activities. These include collection and drop-off of ballots, and collection of signatures to qualify candidates or measures for the ballot.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C21" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1318,10 +1318,10 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>What if I don’t have health insurance and I need screening,  testing, or treatment for COVID-19?</v>
+        <v>What if I don’t have health insurance and I need screening, testing, or treatment for COVID-19?</v>
       </c>
       <c r="B37" t="str">
-        <v>The cost of coronavirus screening, testing, and treatment for the uninsured is paid for by the [government](https://www.hrsa.gov/CovidUninsuredClaim). You can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor through [telehealth](https://covid19.ca.gov/telehealth/). You can also get free [testing](https://covid19.ca.gov/testing-and-treatment/) through [Verily’s Project Baseline](https://www.projectbaseline.com/study/covid-19/eligibility/) or [OptumServe](https://lhi.care/covidtesting).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>The cost of medically necessary screening, testing, and treatment for the uninsured is paid for by the [government](https://www.hrsa.gov/CovidUninsuredClaim). You can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor through [telehealth](https://covid19.ca.gov/telehealth/). You can also get free medically necessary [testing](https://covid19.ca.gov/testing-and-treatment/) through [Verily’s Project Baseline](https://www.projectbaseline.com/study/covid-19/eligibility/) or [OptumServe](https://lhi.care/covidtesting).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C37" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1344,10 +1344,10 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>I want to get screened or tested for COVID-19. I have insurance, but what will this cost me out-of-pocket?</v>
+        <v>Does my health plan have to cover my COVID-19 test?</v>
       </c>
       <c r="B38" t="str">
-        <v>Nothing. The state agencies that regulate health care in California have mandated that all full-service insurance plans (including Medi-Cal) waive copayments, coinsurance, and deductibles for medically necessary screening and testing for COVID-19. This includes emergency room, urgent care, or provider office visits when the purpose of the visit is to be screened and tested for COVID-19.\n\n[Testing](https://covid19.ca.gov/testing-and-treatment/) for COVID-19 is covered by insurance, Medicare, and Medi-Cal. If you have no insurance, it’s paid for by the [government](https://www.hrsa.gov/CovidUninsuredClaim). As a first step, you can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor through [telehealth](https://covid19.ca.gov/telehealth/).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes, if you’re experiencing COVID-19 symptoms, you think you were exposed to someone who has COVID-19, or the test is otherwise medically necessary for your situation. \n\nIf you have symptoms of COVID-19 or you think you’ve been exposed to someone with COVID-19, under federal law, you can obtain a COVID-19 test anywhere and your health plan must pay for the test. \n\nIf you don’t have symptoms and don’t think you’ve been exposed to someone with COVID-19, but you are an [essential worker](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf) as defined for COVID-19 testing coverage, your health plan must cover your COVID-19 test. However, you must contact your health plan before getting testing. \n\nIf you don’t have symptoms, don’t think you’ve been exposed to someone with COVID-19, and aren’t an [essential worker](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf) as defined for COVID-19 testing coverage, and you think you need a test, please contact your health plan or health care provider for further guidance.\n\nAs a first step, you can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor through [telehealth](https://covid19.ca.gov/telehealth/).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C38" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1370,10 +1370,10 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>I have a concern or complaint about getting care for COVID-19 under my health insurance. What can I do?</v>
+        <v>How long will I have to wait to get a test?</v>
       </c>
       <c r="B39" t="str">
-        <v>If you are having trouble accessing care, or were inappropriately charged for medically necessary screening, testing, or treatment for COVID-19, follow up directly with your health plan by calling the member phone number listed on your health plan card. If your health plan doesn’t resolve the issue, contact the [](https://www.healthhelp.ca.gov/)[California Department of Managed Health Care (DMHC)](http://www.dmhc.ca.gov/?referral=healthhelp.ca.gov) Help Center for assistance at 1-888-466-2219.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Your wait time depends on why you are seeking a test. \n\n**If you have symptoms of COVID-19 or think you were exposed,** under federal law, you can go immediately to any available testing site. Find a testing site on our [Testing page,](https://covid19.ca.gov/testing-and-treatment/#top) or call your health plan so they can direct you to an available testing location. \n\n**If you don’t have symptoms or suspected exposure, and you are an** [**essential worker**](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf)**,** your health plan must offer you a test appointment within 48 hours. The testing site must be within 15 miles or 30 minutes of your residence or workplace. If the health plan can’t find you an available appointment within that time and distance, then you can go to any available testing site and your health plan will pay for the test. \n\n**If you don’t have symptoms or suspected exposure, and you are not an essential worker,** if your provider determines a COVID-19 test is medically necessary for you, your health plan must offer you a test appointment within 96 hours. The testing site must be within 15 miles or 30 minutes of your residence or workplace. If the health plan can’t find you an available appointment within that time and distance, you can go to any available testing site.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C39" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1396,10 +1396,10 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>Do Medicare or Medicare Advantage Plans cover coronavirus tests or coronavirus antibody tests?</v>
+        <v>I get my health care coverage through my employer, who has a “self-insured” plan. Do the California Department of Managed Health Care (DMHC) regulations apply to me?</v>
       </c>
       <c r="B40" t="str">
-        <v>Yes. Both [Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) cover [coronavirus tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test) tests, with no out-of-pocket costs. \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Self-insured plans are regulated by the federal government, rather than the state. If you have symptoms of COVID-19 or you were exposed to someone who you know or suspect has COVID-19, under federal law, your employer’s self-insured plan must cover your test. In all other instances, you should talk to your employer’s self-insured plan to find out whether they will cover COVID-19 testing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C40" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1422,10 +1422,10 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>Can I use telehealth if I am on Medicare?</v>
+        <v>How does my health plan know if I’m an essential worker?</v>
       </c>
       <c r="B41" t="str">
-        <v>Yes. Medicare has temporarily expanded its coverage of [telehealth services (medical care via phone, video chat, or online portal)](https://www.medicare.gov/coverage/telehealth) to respond to the current Public Health Emergency. You can now use a wide range of communication tools (including smartphone) from home to interact with a range of providers, like doctors, nurse practitioners, clinical psychologists, licensed clinical social workers, physical therapists, occupational therapists, and speech language pathologists. If you have original Medicare, you can get many services without a copayment through [telehealth,](https://covid19.ca.gov/telehealth/) including evaluation and management visits (common office visits), mental health counseling, and preventive health screenings.\n\nIf you have a [Medicare Advantage Plan](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans), you have access to these same benefits. Many plans offer additional [telehealth](https://covid19.ca.gov/telehealth/) benefits and expanded benefits, like meal delivery or medical transport services. Check with your plan about your coverage and costs.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Your health plan can ask you questions about why you want a COVID-19 test and about the nature of your work. They can ask these questions to help determine whether a COVID-19 test is medically necessary for you. \n\nHowever, your health plan can’t ask you to provide further documentation or evidence of your work status. For example, your health plan can’t ask you to provide written proof of where you work or the conditions of your workplace.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C41" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>I am nervous or scared. What can I do?</v>
+        <v>I have a concern or complaint about getting care for COVID-19 under my health insurance. What can I do?</v>
       </c>
       <c r="B42" t="str">
-        <v>You are not alone. The California Surgeon General released [two playbooks for managing stress](https://covid19.ca.gov/manage-stress-for-health/#top) and tips for care-givers and kids. If you feel like you need to talk to someone and want emotional support see this [list of resources](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/#top).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>If you are having trouble accessing care, or were inappropriately charged for medically necessary screening, testing, or treatment for COVID-19, follow up directly with your health plan by calling the member phone number listed on your health plan card. If your health plan doesn’t resolve the issue, contact the [California Department of Managed Health Care (DMHC)](http://www.dmhc.ca.gov/?referral=healthhelp.ca.gov) Help Center for assistance at 1-888-466-2219.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C42" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1474,10 +1474,10 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>My safety net eligibility (like CalFresh, Medi-Cal) is expiring and I am under the statewide stay home order for COVID-19. Do I need to renew my eligibility now?</v>
+        <v>Do Medicare or Medicare Advantage Plans cover coronavirus tests or coronavirus antibody tests?</v>
       </c>
       <c r="B43" t="str">
-        <v>****No, you will not need to renew until August 17, 2020.**** Governor Gavin Newsom issued an [executive order](https://www.gov.ca.gov/wp-content/uploads/2020/06/6.15.20-EO-N-69-20-text.pdf) to ensure that health care, food assistance, and in-home supportive services continue during the COVID-19 outbreak.\n\nThe order waives eligibility re-determinations for 150 days for participants in:\n\n*   Medi-Cal health coverage\n*   CalFresh food assistance\n*   CalWORKs\n*   Cash Assistance for Immigrants\n*   In-Home Supportive Services\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. Both [Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) cover [coronavirus tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test) tests, with no out-of-pocket costs. \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C43" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1500,10 +1500,10 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>What if I need to visit a health care provider?</v>
+        <v>Can I use telehealth if I am on Medicare?</v>
       </c>
       <c r="B44" t="str">
-        <v>If you have [coronavirus symptoms](https://covid19.ca.gov/symptoms-and-risks/#top), please contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) or use the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) self-checker.\n\nIf you have other illnesses or chronic conditions, use [telehealth](https://covid19.ca.gov/telehealth/) to get care from home.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call 911, tell the 911 operator your exact symptoms so the ambulance provider can be ready to treat you safely.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. Medicare has temporarily expanded its coverage of [telehealth services (medical care via phone, video chat, or online portal)](https://www.medicare.gov/coverage/telehealth) to respond to the current Public Health Emergency. You can now use a wide range of communication tools (including smartphone) from home to interact with a range of providers, like doctors, nurse practitioners, clinical psychologists, licensed clinical social workers, physical therapists, occupational therapists, and speech language pathologists. If you have original Medicare, you can get many services without a copayment through [telehealth,](https://covid19.ca.gov/telehealth/) including evaluation and management visits (common office visits), mental health counseling, and preventive health screenings.\n\nIf you have a [Medicare Advantage Plan](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans), you have access to these same benefits. Many plans offer additional [telehealth](https://covid19.ca.gov/telehealth/) benefits and expanded benefits, like meal delivery or medical transport services. Check with your plan about your coverage and costs.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C44" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1526,10 +1526,10 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>What about routine, elective, or non-urgent medical or dental appointments?</v>
+        <v>I am nervous or scared. What can I do?</v>
       </c>
       <c r="B45" t="str">
-        <v>Preventive care services and non-emergency surgeries, like organ replacements and tumor removals, can take place if hospitals have enough capacity and protective equipment to do so safely. Eye exams, and elective procedures should be cancelled or rescheduled. If possible, health care visits should be done remotely. [Dental services and preventive dental care](https://www.cdc.gov/coronavirus/2019-ncov/hcp/dental-settings.html) may be resumed. Contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) to see what services they are providing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>You are not alone. The California Surgeon General released [two playbooks for managing stress](https://covid19.ca.gov/manage-stress-for-health/#top) and tips for care-givers and kids. If you feel like you need to talk to someone and want emotional support see this [list of resources](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/#top).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C45" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1552,10 +1552,10 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>Can I get my prescriptions filled?</v>
+        <v>My safety net eligibility (like CalFresh, Medi-Cal) is expiring and I am under the statewide stay home order for COVID-19. Do I need to renew my eligibility now?</v>
       </c>
       <c r="B46" t="str">
-        <v>Yes. You may leave your home to get prescriptions or cannabis from dispensaries with medical permits.\n\nYou can contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) to get a new prescription or adjust your existing prescriptions. \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>****No, you will not need to renew until August 17, 2020.**** Governor Gavin Newsom issued an [executive order](https://www.gov.ca.gov/wp-content/uploads/2020/06/6.15.20-EO-N-69-20-text.pdf) to ensure that health care, food assistance, and in-home supportive services continue during the COVID-19 outbreak.\n\nThe order waives eligibility re-determinations for 150 days for participants in:\n\n*   Medi-Cal health coverage\n*   CalFresh food assistance\n*   CalWORKs\n*   Cash Assistance for Immigrants\n*   In-Home Supportive Services\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C46" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1578,10 +1578,10 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>I am an older Californian who is isolating at home and I need non-urgent assistance. What can I do?</v>
+        <v>What if I need to visit a health care provider?</v>
       </c>
       <c r="B47" t="str">
-        <v>You can call the statewide hotline for older Californians at [1-833-544-2374](tel:1-833-544-2374) for your non-urgent medical needs, to get meals delivered, to track down prescriptions, and more. The most important thing you can do is stay home for your health and wellbeing. If you are experiencing an emergency please call 911.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>If you have [coronavirus symptoms](https://covid19.ca.gov/symptoms-and-risks/#top), please contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) or use the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) self-checker.\n\nIf you have other illnesses or chronic conditions, use [telehealth](https://covid19.ca.gov/telehealth/) to get care from home.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call 911, tell the 911 operator your exact symptoms so the ambulance provider can be ready to treat you safely.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C47" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1604,10 +1604,10 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>How can I make sure the older Californians in my life are safe and healthy during the stay home order?</v>
+        <v>What about routine, elective, or non-urgent medical or dental appointments?</v>
       </c>
       <c r="B48" t="str">
-        <v>You should check in on your older neighbors and loved ones with a call, text, or physically-distanced door knock to make sure they are okay. You can also teach them how to use FaceTime, Zoom, Google Duo or Facebook video to communicate. The most important thing you can do is to keep in touch with older loved ones for their mental health and safety.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Preventive care services and non-emergency surgeries, like organ replacements and tumor removals, can take place if hospitals have enough capacity and protective equipment to do so safely. Eye exams, and elective procedures should be cancelled or rescheduled. If possible, health care visits should be done remotely. [Dental services and preventive dental care](https://www.cdc.gov/coronavirus/2019-ncov/hcp/dental-settings.html) may be resumed. Contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) to see what services they are providing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C48" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1630,10 +1630,10 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>Can I leave home to care for my elderly parents or friends who require assistance? Or a friend or family member who has disabilities?</v>
+        <v>Can I get my prescriptions filled?</v>
       </c>
       <c r="B49" t="str">
-        <v>Yes. Be sure that you protect them and yourself by following physical distancing guidelines such as wearing a mask, washing hands before and after, using hand sanitizer, maintaining at least six feet of distance when possible, and covering your cough or sneeze. If you have early signs of a cold, please stay away from your older loved ones.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)&lt;!-- disability, senior --&gt;</v>
+        <v>Yes. You may leave your home to get prescriptions or cannabis from dispensaries with medical permits.\n\nYou can contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) to get a new prescription or adjust your existing prescriptions. \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C49" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1656,10 +1656,10 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>Can I visit loved ones in the hospital, nursing home, skilled nursing facility, or other residential care facility?</v>
+        <v>I am an older Californian who is isolating at home and I need non-urgent assistance. What can I do?</v>
       </c>
       <c r="B50" t="str">
-        <v>Generally, no. There are limited exceptions, such as if you are going to the hospital with a minor who is under 18 or someone who is developmentally disabled and needs assistance. For most other situations, the order prohibits visitation to these kinds of facilities. This is difficult, but necessary to protect hospital staff and other patients. Check the [frequently asked questions for friends and family with a loved one in a skilled nursing or residential care facility](https://www.aging.ca.gov/download.ashx?lE0rcNUV0zaaXLD5JZ%2f6Uw%3d%3d) for more detailed information.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)&lt;!-- elderly, disability, senior --&gt;</v>
+        <v>You can call the statewide hotline for older Californians at [1-833-544-2374](tel:1-833-544-2374) for your non-urgent medical needs, to get meals delivered, to track down prescriptions, and more. The most important thing you can do is stay home for your health and wellbeing. If you are experiencing an emergency please call 911.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C50" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1682,10 +1682,10 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>Can a senior over 65, disabled, uninsured or undocumented immigrant get free COVID-19 / Coronavirus test or treatment?</v>
+        <v>How can I make sure the older Californians in my life are safe and healthy during the stay home order?</v>
       </c>
       <c r="B51" t="str">
-        <v>All patients with full-service Medi-Cal or commercial insurance in California will have [copays, coinsurance and deductibles waived](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf) for COVID-19 [testing](https://covid19.ca.gov/testing-and-treatment/) and screening.  [Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) cover [coronavirus tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test) tests, with no out-of-pocket costs. The cost of coronavirus screening, testing, and treatment for the uninsured is paid for by the [government](https://www.hrsa.gov/CovidUninsuredClaim). \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>You should check in on your older neighbors and loved ones with a call, text, or physically-distanced door knock to make sure they are okay. You can also teach them how to use FaceTime, Zoom, Google Duo or Facebook video to communicate. The most important thing you can do is to keep in touch with older loved ones for their mental health and safety.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C51" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1708,13 +1708,13 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>What do taxpayers need to do if they want to take advantage of relief from the California Department of Tax and Fee Administration?</v>
+        <v>Can I leave home to care for my elderly parents or friends who require assistance? Or a friend or family member who has disabilities?</v>
       </c>
       <c r="B52" t="str">
-        <v>Interested taxpayers should contact CDTFA by visiting the [CDTFA website](http://cdtfa.ca.gov/) or calling [800-400-7115](tel:800-400-7115).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Yes. Be sure that you protect them and yourself by following physical distancing guidelines such as wearing a mask, washing hands before and after, using hand sanitizer, maintaining at least six feet of distance when possible, and covering your cough or sneeze. If you have early signs of a cold, please stay away from your older loved ones.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)&lt;!-- disability, senior --&gt;</v>
       </c>
       <c r="C52" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/healthcare/</v>
       </c>
       <c r="D52" t="str">
         <v xml:space="preserve"> </v>
@@ -1734,13 +1734,13 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>When will taxpayers start on these payment plans?</v>
+        <v>Can I visit loved ones in the hospital, nursing home, skilled nursing facility, or other residential care facility?</v>
       </c>
       <c r="B53" t="str">
-        <v>Given that the April deadline to file and pay sales and use tax returns has been extended to late July for all but the largest taxpayers, CDTFA expects that most participating taxpayers will begin their payment arrangements in late July of this year.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Generally, no. There are limited exceptions, such as if you are going to the hospital with a minor who is under 18 or someone who is developmentally disabled and needs assistance. For most other situations, the order prohibits visitation to these kinds of facilities. This is difficult, but necessary to protect hospital staff and other patients. Check the [frequently asked questions for friends and family with a loved one in a skilled nursing or residential care facility](https://www.aging.ca.gov/download.ashx?lE0rcNUV0zaaXLD5JZ%2f6Uw%3d%3d) for more detailed information.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)&lt;!-- elderly, disability, senior --&gt;</v>
       </c>
       <c r="C53" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/healthcare/</v>
       </c>
       <c r="D53" t="str">
         <v xml:space="preserve"> </v>
@@ -1760,13 +1760,13 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>How will the payment plans work?</v>
+        <v>Can I get free COVID-19 testing or treatment if I am a senior over 65, disabled, uninsured, or an undocumented immigrant?</v>
       </c>
       <c r="B54" t="str">
-        <v>Qualifying sales and use taxpayers with deferred liabilities up to $50,000 will pay their tax due in 12 equal monthly installments. No interest or penalties will be assessed against the liability.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>All patients with full-service Medi-Cal or commercial insurance in California will have [copays, coinsurance and deductibles waived](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf) for COVID-19 [testing](https://covid19.ca.gov/testing-and-treatment/) and screening.  [Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) cover [coronavirus tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test) tests, with no out-of-pocket costs. The cost of medically necessary coronavirus screening, testing, and treatment for the uninsured is paid for by the [government](https://www.hrsa.gov/CovidUninsuredClaim). \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C54" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/healthcare/</v>
       </c>
       <c r="D54" t="str">
         <v xml:space="preserve"> </v>
@@ -1786,10 +1786,10 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>Is this only for tax payments due for the 1st quarter of 2020?</v>
+        <v>What do taxpayers need to do if they want to take advantage of relief from the California Department of Tax and Fee Administration?</v>
       </c>
       <c r="B55" t="str">
-        <v>If taxpayers choose to use this program to distribute the burden of their May or June prepayments or their July return, CDTFA will work to accommodate those taxpayers.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Interested taxpayers should contact CDTFA by visiting the [CDTFA website](http://cdtfa.ca.gov/) or calling [800-400-7115](tel:800-400-7115).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C55" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1812,10 +1812,10 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>What if taxpayers owe more than the $50,000 limit on the relief?</v>
+        <v>When will taxpayers start on these payment plans?</v>
       </c>
       <c r="B56" t="str">
-        <v>The maximum amount that any taxpayer can defer interest-free under this relief effort is $50,000.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Given that the April deadline to file and pay sales and use tax returns has been extended to late July for all but the largest taxpayers, CDTFA expects that most participating taxpayers will begin their payment arrangements in late July of this year.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C56" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1838,10 +1838,10 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>What if taxpayers with more than $5 million in annual taxable sales need this relief?</v>
+        <v>How will the payment plans work?</v>
       </c>
       <c r="B57" t="str">
-        <v>We recognize that some taxpayers, particularly in low margin businesses, with annual taxable sales over $5 million may also need this relief. Those taxpayers are encouraged to reach out to CDTFA, which will work with them to provide relief where appropriate.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Qualifying sales and use taxpayers with deferred liabilities up to $50,000 will pay their tax due in 12 equal monthly installments. No interest or penalties will be assessed against the liability.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C57" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1864,10 +1864,10 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>Is the deadline for filing California tax returns extended?</v>
+        <v>Is this only for tax payments due for the 1st quarter of 2020?</v>
       </c>
       <c r="B58" t="str">
-        <v>Yes. All California taxpayers (individuals and businesses) can file and pay by July 15, 2020. See [information from the CA Franchise Tax Board](https://www.ftb.ca.gov/about-ftb/newsroom/news-releases/2020-3-state-postpones-tax-deadlines-until-july-15-due-to-the-covid-19-pandemic.html) for more information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>If taxpayers choose to use this program to distribute the burden of their May or June prepayments or their July return, CDTFA will work to accommodate those taxpayers.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C58" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1890,10 +1890,10 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>What is a loan guarantee?</v>
+        <v>What if taxpayers owe more than the $50,000 limit on the relief?</v>
       </c>
       <c r="B59" t="str">
-        <v>A loan guarantee is a credit enhancement that helps mitigate the risk assumed by a lending institution when making a loan. With the Small Business Finance Center’s Disaster Relief Loan Guarantee Program, IBank agrees to guarantee up to 95% of the loan, removing the barriers to capital that often exist for small business borrowers that may not otherwise be eligible for traditional lending. This program also can assist those who may not be eligible for a U.S. Small Business Administration (SBA) loan.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The maximum amount that any taxpayer can defer interest-free under this relief effort is $50,000.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C59" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1916,10 +1916,10 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>Who is eligible to apply?</v>
+        <v>What if taxpayers with more than $5 million in annual taxable sales need this relief?</v>
       </c>
       <c r="B60" t="str">
-        <v>Small business entities that have been affected by loss, damage or other economic injury due to the COVID-19 pandemic and meet the program’s eligibility requirements. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>We recognize that some taxpayers, particularly in low margin businesses, with annual taxable sales over $5 million may also need this relief. Those taxpayers are encouraged to reach out to CDTFA, which will work with them to provide relief where appropriate.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C60" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1942,10 +1942,10 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>What do you consider a small business?</v>
+        <v>Is the deadline for filing California tax returns extended?</v>
       </c>
       <c r="B61" t="str">
-        <v>The business must have between 1-750 employees and be established as an entity, including:\n\n*   Sole Proprietor – Individual using legal name as business name that files a Schedule C, Schedule F, or has a fictitious business name or DBA statement\n    *   If the loan appears to be in the name of an individual, evidence of Sole Proprietorship will be required and may include a Schedule C, Schedule F, Seller’s Permit, and/or fictitious business name or DBA statement\n*   Limited Liability Company \n*   Cooperative\n*   Corporation\n*   Partnership\n*   S-Corporation\n*   Not-for-profit\n\nThe program will not accept an _individual_ as the borrower. It is permissible for an individual to be a guarantor or co-borrower on the loan, but the primary borrower must be a small business. It does not consider citizenship or immigration status for eligibility requirements**,** as long as the entity/individual meets the above criteria. Trucking owners/operators are eligible as long as they are registered as a legal business entity.\n\n**AND**\n\n*   The business activity must be eligible under the program and in one of the industries listed in the [North American Industry Classification System (NAICS) codes list](http://www.census.gov/eos/www/naics), and\n*   It must be located in a declared disaster area. A major disaster area declaration was made for the state of California on March 22, 2020 in regards to the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Yes. All California taxpayers (individuals and businesses) can file and pay by July 15, 2020. See [information from the CA Franchise Tax Board](https://www.ftb.ca.gov/about-ftb/newsroom/news-releases/2020-3-state-postpones-tax-deadlines-until-july-15-due-to-the-covid-19-pandemic.html) for more information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C61" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1968,10 +1968,10 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>What are excluded businesses?</v>
+        <v>What is a loan guarantee?</v>
       </c>
       <c r="B62" t="str">
-        <v>Businesses that are not eligible include passive real estate businesses (rental income, etc.).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>A loan guarantee is a credit enhancement that helps mitigate the risk assumed by a lending institution when making a loan. With the Small Business Finance Center’s Disaster Relief Loan Guarantee Program, IBank agrees to guarantee up to 95% of the loan, removing the barriers to capital that often exist for small business borrowers that may not otherwise be eligible for traditional lending. This program also can assist those who may not be eligible for a U.S. Small Business Administration (SBA) loan.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C62" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1994,10 +1994,10 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>Can I apply for a loan guarantee only if I am ineligible for federal disaster fund financing, such as a SBA loan?</v>
+        <v>Who is eligible to apply?</v>
       </c>
       <c r="B63" t="str">
-        <v>Yes, this program is designed for those who do not qualify for federal programs. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Small business entities that have been affected by loss, damage or other economic injury due to the COVID-19 pandemic and meet the program’s eligibility requirements. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C63" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2020,10 +2020,10 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>How much can I borrow?</v>
+        <v>What do you consider a small business?</v>
       </c>
       <c r="B64" t="str">
-        <v>The Small Business Finance Center’s Disaster Relief Loan Guarantee Program allows a maximum loan of $1.25 million and a maximum guarantee of $1 million. To serve as many California small businesses as possible, the COVID-19 disaster program is focused on serving small businesses, especially those in low-wealth and immigrant communities with needs from $500 to $50,000. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The business must have between 1-750 employees and be established as an entity, including:\n\n*   Sole Proprietor – Individual using legal name as business name that files a Schedule C, Schedule F, or has a fictitious business name or DBA statement\n    *   If the loan appears to be in the name of an individual, evidence of Sole Proprietorship will be required and may include a Schedule C, Schedule F, Seller’s Permit, and/or fictitious business name or DBA statement\n*   Limited Liability Company \n*   Cooperative\n*   Corporation\n*   Partnership\n*   S-Corporation\n*   Not-for-profit\n\nThe program will not accept an _individual_ as the borrower. It is permissible for an individual to be a guarantor or co-borrower on the loan, but the primary borrower must be a small business. It does not consider citizenship or immigration status for eligibility requirements**,** as long as the entity/individual meets the above criteria. Trucking owners/operators are eligible as long as they are registered as a legal business entity.\n\n**AND**\n\n*   The business activity must be eligible under the program and in one of the industries listed in the [North American Industry Classification System (NAICS) codes list](http://www.census.gov/eos/www/naics), and\n*   It must be located in a declared disaster area. A major disaster area declaration was made for the state of California on March 22, 2020 in regards to the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C64" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2046,10 +2046,10 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>What are the loan terms?</v>
+        <v>What are excluded businesses?</v>
       </c>
       <c r="B65" t="str">
-        <v>The length of the loan can be negotiated with your lender, but the guarantee is good for up to seven years. The interest rate and loan criteria will be determined by the lender and could depend on the credit strength of the business. The guarantee is designed to lower the interest rate in exchange for a higher guarantee to your lender. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Businesses that are not eligible include passive real estate businesses (rental income, etc.).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C65" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2072,10 +2072,10 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>How can I apply?</v>
+        <v>Can I apply for a loan guarantee only if I am ineligible for federal disaster fund financing, such as a SBA loan?</v>
       </c>
       <c r="B66" t="str">
-        <v>The Small Business Finance Center partners with Community Development Financial Institutions (CDFIs), Community Lending Institutions, and Financial Development Corporations (FDCs) to provide loan guarantees for small businesses.  To apply,\n\n*   View the [list of FDCs and participating lenders](http://www.ibank.ca.gov/small-business-finance-center/) interested in this Small Business Disaster Relief Loan Guarantee Program. \n*   Contact the lender on the list nearest to your business to apply.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Yes, this program is designed for those who do not qualify for federal programs. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C66" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2098,10 +2098,10 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>What is the timing for the funding of loans?</v>
+        <v>How much can I borrow?</v>
       </c>
       <c r="B67" t="str">
-        <v>The program is in place and businesses can apply immediately. Once you provide your lender with complete information, you could be funded in a matter of days.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The Small Business Finance Center’s Disaster Relief Loan Guarantee Program allows a maximum loan of $1.25 million and a maximum guarantee of $1 million. To serve as many California small businesses as possible, the COVID-19 disaster program is focused on serving small businesses, especially those in low-wealth and immigrant communities with needs from $500 to $50,000. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C67" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2124,10 +2124,10 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>What can the money be used for?</v>
+        <v>What are the loan terms?</v>
       </c>
       <c r="B68" t="str">
-        <v>The funds are meant to help small businesses through this challenging time. Loan proceeds can be used for business continuance or to cure “economic injury” as a result of COVID-19.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The length of the loan can be negotiated with your lender, but the guarantee is good for up to seven years. The interest rate and loan criteria will be determined by the lender and could depend on the credit strength of the business. The guarantee is designed to lower the interest rate in exchange for a higher guarantee to your lender. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C68" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2150,10 +2150,10 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>How will this program assist low-wealth and minority communities?</v>
+        <v>How can I apply?</v>
       </c>
       <c r="B69" t="str">
-        <v>By working with the Community Development Financial Institutions (CDFIs) throughout the state of California, this disaster relief program can play an important role in generating economic growth and opportunity in some of our most distressed communities. CDFIs and mission-based lenders play a vital role across the state and have experience steering lending and investment to where it is needed and will matter the most, in particular in low-wealth and immigrant communities. CDFIs and our partner Financial Development Corporations (FDCs) that process the loan guarantees are embedded in communities across the state, speak several languages, and are invested in the community successfully managing its way through this pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The Small Business Finance Center partners with Community Development Financial Institutions (CDFIs), Community Lending Institutions, and Financial Development Corporations (FDCs) to provide loan guarantees for small businesses.  To apply,\n\n*   View the [list of FDCs and participating lenders](http://www.ibank.ca.gov/small-business-finance-center/) interested in this Small Business Disaster Relief Loan Guarantee Program. \n*   Contact the lender on the list nearest to your business to apply.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C69" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2176,10 +2176,10 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>Are faith-based businesses eligible for this loan guarantee program?</v>
+        <v>What is the timing for the funding of loans?</v>
       </c>
       <c r="B70" t="str">
-        <v>Faith-based businesses (non-profit or otherwise) that have business activity outside of worship are eligible as long as they are a legal business that has been affected by the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The program is in place and businesses can apply immediately. Once you provide your lender with complete information, you could be funded in a matter of days.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C70" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2202,10 +2202,10 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>What SBA programs are available to small businesses right now?</v>
+        <v>What can the money be used for?</v>
       </c>
       <c r="B71" t="str">
-        <v>The U.S. SBA offers the **Paycheck Protection Program (PPP)** and **Economic Injury Disaster Loan and Advance (EIDL and EIDL Advance)**.\n\nMore about **Paycheck Protection Program (PPP)**:\n\nThe PPP is a loan program for small businesses, self-employed, independent contractors, nonprofits with a maximum of 500 employees, and it is intended to keep workers paid and employed. The loan amount is calculated based on payroll expenses with a maximum amount of $10 million at a rate of 1%. For all loans made on or after June 5, the minimum term is five years. For loans made before June 5, the two-year minimum maturity remains in effect unless both the borrower and the lender agree to extend it to five years. The loan is forgivable if 60% of the loan amount is used for payroll, and no employees are laid off, or if laid-off employees are rehired before December 31, 2020. In addition to payroll and benefits costs, allowable expenses include mortgage interest, rent, and utilities. Submit your application as soon as possible, even if you need to rehire employees that have been laid off.\n\nThe SBA is accepting PPP loan applications from approved lenders. The new deadline to apply for a PPP loan is August 8, 2020. You must apply directly through a lender. [Find a PPP lender in your area](https://www.sba.gov/paycheckprotection/find) to contact right away. See [SBA.gov](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program#section-header-0) for more details. \n\nMore about **Economic Injury Disaster Loan and Advance (EIDL and EIDL Advance):**\n\nAs of June 15, the U.S. SBA is accepting new applications from all eligible businesses, and will continue to process **EIDL Loan and Advance applications** already submitted on a first come, first-served basis. Check the U.S. SBA’s [Disaster Loan Applications website](https://www.sba.gov/page/disaster-loan-applications#section-header-0) for more information.\n\nThe EIDL is a direct loan for up to $2 million at a rate of 3.75% for small businesses and 2.75% for nonprofits. Applicants can get an **Advance** of up to $10,000 upon request within days of a successful application. This advance doesn’t have to be repaid. [Apply directly with the SBA](https://covid19relief.sba.gov/#/). For questions, you can contact SBA’s Customer Service Line at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or send an email to [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The funds are meant to help small businesses through this challenging time. Loan proceeds can be used for business continuance or to cure “economic injury” as a result of COVID-19.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C71" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2228,10 +2228,10 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>Which banks are offering the Paycheck Protection Program forgivable loans?</v>
+        <v>How will this program assist low-wealth and minority communities?</v>
       </c>
       <c r="B72" t="str">
-        <v>Interested borrowers can contact any SBA participating bank, credit union, or nonprofit lenders to apply for the [PPP](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program). For more information, contact your local bank or reach out to [SBA’s local district offices](https://www.sba.gov/local-assistance/find/?type=SBA%20District%20Office&amp;pageNumber=1) for assistance.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>By working with the Community Development Financial Institutions (CDFIs) throughout the state of California, this disaster relief program can play an important role in generating economic growth and opportunity in some of our most distressed communities. CDFIs and mission-based lenders play a vital role across the state and have experience steering lending and investment to where it is needed and will matter the most, in particular in low-wealth and immigrant communities. CDFIs and our partner Financial Development Corporations (FDCs) that process the loan guarantees are embedded in communities across the state, speak several languages, and are invested in the community successfully managing its way through this pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C72" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2254,10 +2254,10 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>Where do I find more information on allowable expenses for a forgivable loan under the Paycheck Protection Program?</v>
+        <v>Are faith-based businesses eligible for this loan guarantee program?</v>
       </c>
       <c r="B73" t="str">
-        <v>You can find this on the Paycheck Protection Program’s [Loan Forgiveness Application](https://www.sba.gov/sites/default/files/2020-06/PPP%20Loan%20Forgiveness%20Application%20%28Revised%206.16.2020%29-fillable_0-508.pdf). The application provides detailed [instructions](https://www.sba.gov/sites/default/files/2020-06/PPP%20Loan%20Forgiveness%20Application%20Instructions%20%28Revised%206.16.2020%29-508.pdf) on how to apply for forgiveness of PPP loans. Once your business has expended the PPP funds and is ready to pursue loan forgiveness, please review the Loan Forgiveness Application and consult with your accountant, lender, or one of California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) for assistance.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Faith-based businesses (non-profit or otherwise) that have business activity outside of worship are eligible as long as they are a legal business that has been affected by the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C73" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2280,10 +2280,10 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>How does a business know if it is eligible for an SBA loan or loan guarantee program?</v>
+        <v>What SBA programs are available to small businesses right now?</v>
       </c>
       <c r="B74" t="str">
-        <v>Small businesses with 500 employees or less are eligible to apply for the Paycheck Protection Program (PPP) and/or the Small Business Debt Relief Program. Small businesses are also eligible to apply for the Economic Injury Disaster Loan (EIDL) program and the EIDL Advance. Visit SBA’s comprehensive [COVID-19 support website](https://www.sba.gov/page/coronavirus-covid-19-small-business-guidance-loan-resources#section-header-4%20.) to find out more about SBA’s eligibility requirements for each program.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The U.S. SBA offers the **Paycheck Protection Program (PPP)** and **Economic Injury Disaster Loan and Advance (EIDL and EIDL Advance)**.\n\nMore about **Paycheck Protection Program (PPP)**:\n\nThe PPP is a loan program for small businesses, self-employed, independent contractors, nonprofits with a maximum of 500 employees, and it is intended to keep workers paid and employed. The loan amount is calculated based on payroll expenses with a maximum amount of $10 million at a rate of 1%. For all loans made on or after June 5, the minimum term is five years. For loans made before June 5, the two-year minimum maturity remains in effect unless both the borrower and the lender agree to extend it to five years. The loan is forgivable if 60% of the loan amount is used for payroll, and no employees are laid off, or if laid-off employees are rehired before December 31, 2020. In addition to payroll and benefits costs, allowable expenses include mortgage interest, rent, and utilities. Submit your application as soon as possible, even if you need to rehire employees that have been laid off.\n\nThe SBA is accepting PPP loan applications from approved lenders. The new deadline to apply for a PPP loan is August 8, 2020. You must apply directly through a lender. [Find a PPP lender in your area](https://www.sba.gov/paycheckprotection/find) to contact right away. See [SBA.gov](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program#section-header-0) for more details. \n\nMore about **Economic Injury Disaster Loan and Advance (EIDL and EIDL Advance):**\n\nAs of June 15, the U.S. SBA is accepting new applications from all eligible businesses, and will continue to process **EIDL Loan and Advance applications** already submitted on a first come, first-served basis. Check the U.S. SBA’s [Disaster Loan Applications website](https://www.sba.gov/page/disaster-loan-applications#section-header-0) for more information.\n\nThe EIDL is a direct loan for up to $2 million at a rate of 3.75% for small businesses and 2.75% for nonprofits. Applicants can get an **Advance** of up to $10,000 upon request within days of a successful application. This advance doesn’t have to be repaid. [Apply directly with the SBA](https://covid19relief.sba.gov/#/). For questions, you can contact SBA’s Customer Service Line at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or send an email to [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C74" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2306,10 +2306,10 @@
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>How do I reach SBA for any questions or assistance?</v>
+        <v>Which banks are offering the Paycheck Protection Program forgivable loans?</v>
       </c>
       <c r="B75" t="str">
-        <v>SBA has district offices in California that are open to answer questions. You can use the [SBA’s Local Assistance Directory](https://www.sba.gov/local-assistance) to locate the office nearest you. You can also contact the SBA by phone at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or by email at [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).  \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Interested borrowers can contact any SBA participating bank, credit union, or nonprofit lenders to apply for the [PPP](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program). For more information, contact your local bank or reach out to [SBA’s local district offices](https://www.sba.gov/local-assistance/find/?type=SBA%20District%20Office&amp;pageNumber=1) for assistance.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C75" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2332,10 +2332,10 @@
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>How does a small business know which SBA loan or loan guarantee program is the right one? Can a small business apply to more than one?</v>
+        <v>Where do I find more information on allowable expenses for a forgivable loan under the Paycheck Protection Program?</v>
       </c>
       <c r="B76" t="str">
-        <v>Call or email the SBA to find out which program is right for you. While businesses can apply for and receive more than one form of capital assistance through the SBA, they cannot be used for the same purpose. The SBA can advise you on your options. Call [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or email [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>You can find this on the Paycheck Protection Program’s [Loan Forgiveness Application](https://www.sba.gov/sites/default/files/2020-06/PPP%20Loan%20Forgiveness%20Application%20%28Revised%206.16.2020%29-fillable_0-508.pdf). The application provides detailed [instructions](https://www.sba.gov/sites/default/files/2020-06/PPP%20Loan%20Forgiveness%20Application%20Instructions%20%28Revised%206.16.2020%29-508.pdf) on how to apply for forgiveness of PPP loans. Once your business has expended the PPP funds and is ready to pursue loan forgiveness, please review the Loan Forgiveness Application and consult with your accountant, lender, or one of California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) for assistance.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C76" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2358,10 +2358,10 @@
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>How do I get SBA to cover my loan payments on my existing 7(a), 504, or microloan if I cannot pay due to COVID-19?</v>
+        <v>How does a business know if it is eligible for an SBA loan or loan guarantee program?</v>
       </c>
       <c r="B77" t="str">
-        <v>SBA has a [Debt Relief program](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/sba-debt-relief) and will pay the principal and interest of existing SBA loans. Please contact your lender for information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Small businesses with 500 employees or less are eligible to apply for the Paycheck Protection Program (PPP) and/or the Small Business Debt Relief Program. Small businesses are also eligible to apply for the Economic Injury Disaster Loan (EIDL) program and the EIDL Advance. Visit SBA’s comprehensive [COVID-19 support website](https://www.sba.gov/page/coronavirus-covid-19-small-business-guidance-loan-resources#section-header-4%20.) to find out more about SBA’s eligibility requirements for each program.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C77" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2384,10 +2384,10 @@
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>If I need help to figure out which program is best for me or to submit an application, where can I find support?</v>
+        <v>How do I reach SBA for any questions or assistance?</v>
       </c>
       <c r="B78" t="str">
-        <v>California’s network of small business support centers can help you figure out which loans and programs are best for your business, develop resiliency strategies, and find other resources. Go to California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) to find the closest center.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>SBA has district offices in California that are open to answer questions. You can use the [SBA’s Local Assistance Directory](https://www.sba.gov/local-assistance) to locate the office nearest you. You can also contact the SBA by phone at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or by email at [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).  \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C78" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2410,10 +2410,10 @@
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>How do I maintain a safe workplace?</v>
+        <v>How does a small business know which SBA loan or loan guarantee program is the right one? Can a small business apply to more than one?</v>
       </c>
       <c r="B79" t="str">
-        <v>As California [reopens](https://covid19.ca.gov/roadmap/), every business will need to create a safer, low-risk environment. If you own or manage a business, follow the [industry-specific guidance](https://covid19.ca.gov/industry-guidance/) that applies to protect your workers and customers.\n\nIf your business is approved to reopen, you should take steps to ensure the safety and health of your workers. It’s important that employees with COVID-19 know they should stay home. Your sick leave policies need to support that. \n\n*   Encourage sick employees to stay home if they are sick. See government programs supporting [COVID-19 sick leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) and [workers’ compensation](https://www.labor.ca.gov/coronavirus2019/#chart).\n*   Establish routine cleaning throughout the workplace.\n*   Reduce travel. If possible, encourage video conferencing and limit larger gatherings.\n*   See [Cal/OSHA interim guidelines for general industry](https://www.dir.ca.gov/dosh/coronavirus/General-Industry.html).\n*   Follow [CDC guidance on keeping the workplace safe (PDF)](https://www.cdc.gov/coronavirus/2019-ncov/downloads/workplace-school-and-home-guidance.pdf).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Call or email the SBA to find out which program is right for you. While businesses can apply for and receive more than one form of capital assistance through the SBA, they cannot be used for the same purpose. The SBA can advise you on your options. Call [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or email [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C79" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2436,10 +2436,10 @@
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>What precautions should healthcare workers and organizations take?</v>
+        <v>How do I get SBA to cover my loan payments on my existing 7(a), 504, or microloan if I cannot pay due to COVID-19?</v>
       </c>
       <c r="B80" t="str">
-        <v>See [Cal/OSHA’s guidance on protecting workers from coronavirus](https://www.dir.ca.gov/dosh/coronavirus/Health-Care-General-Industry.html).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>SBA has a [Debt Relief program](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/sba-debt-relief) and will pay the principal and interest of existing SBA loans. Please contact your lender for information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C80" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2462,10 +2462,10 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>How can I avoid laying off employees if my business is impacted by COVID-19?</v>
+        <v>If I need help to figure out which program is best for me or to submit an application, where can I find support?</v>
       </c>
       <c r="B81" t="str">
-        <v>Apply for the [Unemployment Insurance (UI) Work Sharing Program](https://www.edd.ca.gov/Unemployment/Work_Sharing_Program.htm).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>California’s network of small business support centers can help you figure out which loans and programs are best for your business, develop resiliency strategies, and find other resources. Go to California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) to find the closest center.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C81" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2488,13 +2488,13 @@
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>What action is the state taking to ensure all schools are providing meaningful instruction during the pandemic whether they are physically open or closed?</v>
+        <v>How do I maintain a safe workplace?</v>
       </c>
       <c r="B82" t="str">
-        <v>*   California has made $5.3 billion in investments to support safe reopening and rigorous distance learning.\n*   Funds prioritize low-income students, English language learners, and special education students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>As California [reopens](https://covid19.ca.gov/roadmap/), every business will need to create a safer, low-risk environment. If you own or manage a business, follow the [industry-specific guidance](https://covid19.ca.gov/industry-guidance/) that applies to protect your workers and customers.\n\nIf your business is approved to reopen, you should take steps to ensure the safety and health of your workers. It’s important that employees with COVID-19 know they should stay home. Your sick leave policies need to support that. \n\n*   Encourage sick employees to stay home if they are sick. See government programs supporting [COVID-19 sick leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) and [workers’ compensation](https://www.labor.ca.gov/coronavirus2019/#chart).\n*   Establish routine cleaning throughout the workplace.\n*   Reduce travel. If possible, encourage video conferencing and limit larger gatherings.\n*   See [Cal/OSHA interim guidelines for general industry](https://www.dir.ca.gov/dosh/coronavirus/General-Industry.html).\n*   Follow [CDC guidance on keeping the workplace safe (PDF)](https://www.cdc.gov/coronavirus/2019-ncov/downloads/workplace-school-and-home-guidance.pdf).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C82" t="str">
-        <v>https://covid19.ca.gov/education/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D82" t="str">
         <v xml:space="preserve"> </v>
@@ -2514,13 +2514,13 @@
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>What determines whether schools are conducting in-person learning or distance learning?</v>
+        <v>What precautions should healthcare workers and organizations take?</v>
       </c>
       <c r="B83" t="str">
-        <v>Using health data, schools can physically open when its county has been off the Monitoring List for 14 days and only if they follow strict health and safety requirements like masks and physical distancing. [Find the County Monitoring List here.](https://covid19.ca.gov/roadmap-counties/#track-data)\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>See [Cal/OSHA’s guidance on protecting workers from coronavirus](https://www.dir.ca.gov/dosh/coronavirus/Health-Care-General-Industry.html).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C83" t="str">
-        <v>https://covid19.ca.gov/education/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D83" t="str">
         <v xml:space="preserve"> </v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>What are the health and safety requirements for schools doing in-person learning?</v>
+        <v>How can I avoid laying off employees if my business is impacted by COVID-19?</v>
       </c>
       <c r="B84" t="str">
-        <v>*   Everyone entering the school must do daily health checks.\n*   If someone experiences symptoms while at school, they will be sent home.\n*   Masks are required for all staff and students 3rd grade and above. Younger students should be encouraged to wear masks.\n*   Staff members must maintain 6ft distance from each other and students. Students should maintain 6ft distance as practicable.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>Apply for the [Unemployment Insurance (UI) Work Sharing Program](https://www.edd.ca.gov/Unemployment/Work_Sharing_Program.htm).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C84" t="str">
-        <v>https://covid19.ca.gov/education/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D84" t="str">
         <v xml:space="preserve"> </v>
@@ -2566,10 +2566,10 @@
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>What happens if someone gets COVID-19 at my child’s school?</v>
+        <v>What action is the state taking to ensure all schools are providing meaningful instruction during the pandemic whether they are physically open or closed?</v>
       </c>
       <c r="B85" t="str">
-        <v>*   A classroom goes home when there is a confirmed case\n*   A school should switch to distance learning when there are multiple positive cases in multiple classroom cohorts\n*   A district should switch to distance learning if 25% of schools in the district are closed within a 14-day period\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>*   California has made $5.3 billion in investments to support safe reopening and rigorous distance learning.\n*   Funds prioritize low-income students, English language learners, and special education students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C85" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2592,10 +2592,10 @@
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>If my child’s school is engaged in distance learning, what should I expect?</v>
+        <v>What determines whether schools are conducting in-person learning or distance learning?</v>
       </c>
       <c r="B86" t="str">
-        <v>*   New statewide requirements include:\n    *   Access to devices and connectivity for all students\n    *   Daily live interaction with teachers and other students\n    *   Classes and assignments that are challenging and are equivalent to in-person instruction\n    *   Special requirements for English language learners and special education students\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>Using health data, schools can physically open when its county has been off the Monitoring List for 14 days and only if they follow strict health and safety requirements like masks and physical distancing. [Find the County Monitoring List here.](https://covid19.ca.gov/roadmap-counties/#track-data)\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C86" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2618,10 +2618,10 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>Is there financial help for student loans?</v>
+        <v>What are the health and safety requirements for schools doing in-person learning?</v>
       </c>
       <c r="B87" t="str">
-        <v>The [governor has ordered](https://www.gov.ca.gov/2020/04/23/governor-newsom-announces-additional-relief-for-californians-impacted-by-covid-19/) relief for students with federal loans. Check with your lender to see what options are available for you.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>*   Everyone entering the school must do daily health checks.\n*   If someone experiences symptoms while at school, they will be sent home.\n*   Masks are required for all staff and students 3rd grade and above. Younger students should be encouraged to wear masks.\n*   Staff members must maintain 6ft distance from each other and students. Students should maintain 6ft distance as practicable.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C87" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2644,10 +2644,10 @@
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>My school provides free grab-and-go meals. Are those still available?</v>
+        <v>What happens if someone gets COVID-19 at my child’s school?</v>
       </c>
       <c r="B88" t="str">
-        <v>Yes. It is essential to keep children fed. Check with your local school district for days and times meals are offered.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>*   A classroom goes home when there is a confirmed case\n*   A school should switch to distance learning when there are multiple positive cases in multiple classroom cohorts\n*   A district should switch to distance learning if 25% of schools in the district are closed within a 14-day period\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C88" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2670,10 +2670,10 @@
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>What if I don’t have internet access at home?</v>
+        <v>If my child’s school is engaged in distance learning, what should I expect?</v>
       </c>
       <c r="B89" t="str">
-        <v>Check with your local school district or college to see what resources are available for you.  List of providers offering free internet access currently:\n\n[Spectrum mobile](https://mobile.spectrum.com/support/article/360040980371/coronavirus-covid19-update)  has opened wifi hotspots and are working on assisting school districts with facilitating home internet access. \n\n[Comcast](https://corporate.comcast.com/covid-19) has opened free Xfinity WiFi hotspot access across the country. Xfinity has also paused data plans, late fees, and disconnects for the next 60 days. Families with limited income can receive internet services for free for the next 60 days (usually $9.95 per month). \n\n[AT&amp;T](https://about.att.com/pages/COVID-19.html)  has opened all public WiFi hotspots and will not charge customers for any late fees or overages. AT&amp;T also offers internet access for [$10/month for households on limited income](https://www.att.com/shop/internet/access/index.html?source=ECmj0000000000mbU&amp;wtExtndSource=access#!/#%2F).\n\n[Low-cost Internet access plans](https://www.cde.ca.gov/ls/he/hn/availableinternetplans.asp) are also available.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>*   New statewide requirements include:\n    *   Access to devices and connectivity for all students\n    *   Daily live interaction with teachers and other students\n    *   Classes and assignments that are challenging and are equivalent to in-person instruction\n    *   Special requirements for English language learners and special education students\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C89" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2696,10 +2696,10 @@
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>How will students with disabilities receive services during school closures?</v>
+        <v>Is there financial help for student loans?</v>
       </c>
       <c r="B90" t="str">
-        <v>The Department of Education has released [guidance on distance learning](https://www.cde.ca.gov/ls/he/hn/distancelearning.asp) to support schools. This guidance includes recommendations to ensure equity and access for all students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>The [governor has ordered](https://www.gov.ca.gov/2020/04/23/governor-newsom-announces-additional-relief-for-californians-impacted-by-covid-19/) relief for students with federal loans. Check with your lender to see what options are available for you.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C90" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2722,10 +2722,10 @@
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>Will there be standardized testing? When?</v>
+        <v>My school provides free grab-and-go meals. Are those still available?</v>
       </c>
       <c r="B91" t="str">
-        <v>Probably not: on March 18, 2020, Governor Newsom issued an [executive order](https://www.gov.ca.gov/2020/03/18/governor-newsom-issues-executive-order-to-suspend-standardized-testing-for-students-in-response-to-covid-19-outbreak/)  to waive this year’s statewide testing for K-12 schools.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>Yes. It is essential to keep children fed. Check with your local school district for days and times meals are offered.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C91" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2748,13 +2748,13 @@
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>Am I allowed to work during the outbreak?</v>
+        <v>What if I don’t have internet access at home?</v>
       </c>
       <c r="B92" t="str">
-        <v>It depends what your job is. Workers in [essential sectors (pdf)](https://covid19.ca.gov/img/EssentialCriticalInfrastructureWorkers.pdf) are allowed to work during the [stay home order](https://covid19.ca.gov/stay-home-except-for-essential-needs/#top). And anyone is allowed to work from their home that has arranged to do so with their employer.\n\nFor information on businesses and industry sectors that are allowed to reopen, visit [industry guidance](https://covid19.ca.gov/industry-guidance/).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>Check with your local school district or college to see what resources are available for you.  List of providers offering free internet access currently:\n\n[Spectrum mobile](https://mobile.spectrum.com/support/article/360040980371/coronavirus-covid19-update)  has opened wifi hotspots and are working on assisting school districts with facilitating home internet access. \n\n[Comcast](https://corporate.comcast.com/covid-19) has opened free Xfinity WiFi hotspot access across the country. Xfinity has also paused data plans, late fees, and disconnects for the next 60 days. Families with limited income can receive internet services for free for the next 60 days (usually $9.95 per month). \n\n[AT&amp;T](https://about.att.com/pages/COVID-19.html)  has opened all public WiFi hotspots and will not charge customers for any late fees or overages. AT&amp;T also offers internet access for [$10/month for households on limited income](https://www.att.com/shop/internet/access/index.html?source=ECmj0000000000mbU&amp;wtExtndSource=access#!/#%2F).\n\n[Low-cost Internet access plans](https://www.cde.ca.gov/ls/he/hn/availableinternetplans.asp) are also available.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C92" t="str">
-        <v>https://covid19.ca.gov/workers/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D92" t="str">
         <v xml:space="preserve"> </v>
@@ -2774,13 +2774,13 @@
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>What can I do if my work hours are reduced because of COVID-19?</v>
+        <v>How will students with disabilities receive services during school closures?</v>
       </c>
       <c r="B93" t="str">
-        <v>You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>The Department of Education has released [guidance on distance learning](https://www.cde.ca.gov/ls/he/hn/distancelearning.asp) to support schools. This guidance includes recommendations to ensure equity and access for all students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C93" t="str">
-        <v>https://covid19.ca.gov/workers/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D93" t="str">
         <v xml:space="preserve"> </v>
@@ -2800,13 +2800,13 @@
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>Do I need a note or certificate from a medical provider to file for unemployment?</v>
+        <v>Will there be standardized testing? When?</v>
       </c>
       <c r="B94" t="str">
-        <v>No, a medical certificate is not required.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>Probably not: on March 18, 2020, Governor Newsom issued an [executive order](https://www.gov.ca.gov/2020/03/18/governor-newsom-issues-executive-order-to-suspend-standardized-testing-for-students-in-response-to-covid-19-outbreak/)  to waive this year’s statewide testing for K-12 schools.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C94" t="str">
-        <v>https://covid19.ca.gov/workers/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D94" t="str">
         <v xml:space="preserve"> </v>
@@ -2826,10 +2826,10 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>How long will it take to process a claim for unemployment or insurance benefits and to receive a payment?</v>
+        <v>Am I allowed to work during the outbreak?</v>
       </c>
       <c r="B95" t="str">
-        <v>After your claim is submitted, it will take at least three weeks to be processed. It may take longer if your information doesn’t match wage records or your identity can’t be verified. \n\nThe Governor has [waived the one-week waiting period](https://www.gov.ca.gov/2020/03/12/governor-newsom-issues-new-executive-order-further-enhancing-state-and-local-governments-ability-to-respond-to-covid-19-pandemic/). This means you can collect benefits for the first week that you were out of work or had reduced hours.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>It depends what your job is. Workers in [essential sectors (pdf)](https://covid19.ca.gov/img/EssentialCriticalInfrastructureWorkers.pdf) are allowed to work during the [stay home order](https://covid19.ca.gov/stay-home-except-for-essential-needs/#top). And anyone is allowed to work from their home that has arranged to do so with their employer.\n\nFor information on businesses and industry sectors that are allowed to reopen, visit [industry guidance](https://covid19.ca.gov/industry-guidance/).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C95" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2852,10 +2852,10 @@
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>Can I file a workplace safety complaint?</v>
+        <v>What can I do if my work hours are reduced because of COVID-19?</v>
       </c>
       <c r="B96" t="str">
-        <v>Yes, you have the right to file a complaint. Find [information and instructions](https://www.dir.ca.gov/dosh/complaint.htm) for how to file a complaint. If you submit a complaint, your name must be kept confidential by law.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C96" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2878,10 +2878,10 @@
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>What can I do if I miss work because of school closures?</v>
+        <v>Do I need a note or certificate from a medical provider to file for unemployment?</v>
       </c>
       <c r="B97" t="str">
-        <v>*   You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n*   Other options may be available. See [Benefits for Workers Impacted by COVID-19](https://www.labor.ca.gov/coronavirus2019/#chart).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>No, a medical certificate is not required.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C97" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2904,10 +2904,10 @@
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>What if I can’t work because I’m taking care of someone who’s sick or quarantined?</v>
+        <v>How long will it take to process a claim for unemployment or insurance benefits and to receive a payment?</v>
       </c>
       <c r="B98" t="str">
-        <v>*   You may use [paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). The Labor and Workforce Development Agency has created a [chart detailing the available paid sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law. \n*   You can [file a Paid Family Leave (PFL) claim](https://www.edd.ca.gov/Disability/How_to_File_a_PFL_Claim_in_SDI_Online.htm).\n*   Unpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>After your claim is submitted, it will take at least three weeks to be processed. It may take longer if your information doesn’t match wage records or your identity can’t be verified. \n\nThe Governor has [waived the one-week waiting period](https://www.gov.ca.gov/2020/03/12/governor-newsom-issues-new-executive-order-further-enhancing-state-and-local-governments-ability-to-respond-to-covid-19-pandemic/). This means you can collect benefits for the first week that you were out of work or had reduced hours.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C98" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2930,10 +2930,10 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>What can I do if I can’t work because I’m sick or quarantined because of COVID-19?</v>
+        <v>Can I file a workplace safety complaint?</v>
       </c>
       <c r="B99" t="str">
-        <v>*   You may be able to use [paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). The Labor and Workforce Development Agency has created a [chart detailing the available paid sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law.\n*   If you’re unable to work due to having or being exposed to COVID-19, you can [file a Disability Insurance (DI) claim](https://www.edd.ca.gov/Disability/How_to_File_a_DI_Claim_in_SDI_Online.htm).\n*   You may also file a [Workers’ Compensation Claim](https://www.dir.ca.gov/dwc/FileAClaim.htm) if you suffered a COVID-19 illness that arose from an exposure during the course of your work. Check the California Department of Industrial Relations’ [COVID-19 Resources and Workers’ Compensation](https://www.dir.ca.gov/dwc/Covid-19/Index.html) for more information.\n*   Unpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>Yes, you have the right to file a complaint. Find [information and instructions](https://www.dir.ca.gov/dosh/complaint.htm) for how to file a complaint. If you submit a complaint, your name must be kept confidential by law.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C99" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2956,10 +2956,10 @@
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>What if I don’t have any available sick leave to use?</v>
+        <v>What can I do if I miss work because of school closures?</v>
       </c>
       <c r="B100" t="str">
-        <v>Check the Labor and Workforce Development Agency’s [chart detailing the available sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law.\n\nUnpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>*   You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n*   Other options may be available. See [Benefits for Workers Impacted by COVID-19](https://www.labor.ca.gov/coronavirus2019/#chart).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C100" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2982,13 +2982,13 @@
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>What effect will this have on my credit report?</v>
+        <v>What if I can’t work because I’m taking care of someone who’s sick or quarantined?</v>
       </c>
       <c r="B101" t="str">
-        <v>Financial institutions will not report derogatory information (like late payments) to credit reporting agencies but may report a forbearance. Typically this does not negatively affect a credit score on its own.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>*   You may use [paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). The Labor and Workforce Development Agency has created a [chart detailing the available paid sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law. \n*   You can [file a Paid Family Leave (PFL) claim](https://www.edd.ca.gov/Disability/How_to_File_a_PFL_Claim_in_SDI_Online.htm).\n*   Unpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C101" t="str">
-        <v>https://covid19.ca.gov/get-financial-help/</v>
+        <v>https://covid19.ca.gov/workers/</v>
       </c>
       <c r="D101" t="str">
         <v xml:space="preserve"> </v>
@@ -3008,13 +3008,13 @@
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>How long will these programs last?</v>
+        <v>What can I do if I can’t work because I’m sick or quarantined because of COVID-19?</v>
       </c>
       <c r="B102" t="str">
-        <v>It is still unclear how severe or how long the COVID-19 impact will be. Financial institutions have committed to necessary relief and will be assessing the ongoing conditions and need for continuing relief.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>*   You may be able to use [paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). The Labor and Workforce Development Agency has created a [chart detailing the available paid sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law.\n*   If you’re unable to work due to having or being exposed to COVID-19, you can [file a Disability Insurance (DI) claim](https://www.edd.ca.gov/Disability/How_to_File_a_DI_Claim_in_SDI_Online.htm).\n*   You may also file a [Workers’ Compensation Claim](https://www.dir.ca.gov/dwc/FileAClaim.htm) if you suffered a COVID-19 illness that arose from an exposure during the course of your work. Check the California Department of Industrial Relations’ [COVID-19 Resources and Workers’ Compensation](https://www.dir.ca.gov/dwc/Covid-19/Index.html) for more information.\n*   Unpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C102" t="str">
-        <v>https://covid19.ca.gov/get-financial-help/</v>
+        <v>https://covid19.ca.gov/workers/</v>
       </c>
       <c r="D102" t="str">
         <v xml:space="preserve"> </v>
@@ -3034,13 +3034,13 @@
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>What if my financial institution isn’t offering this relief?</v>
+        <v>What if I don’t have any available sick leave to use?</v>
       </c>
       <c r="B103" t="str">
-        <v>Call or check their website to be sure. At this time, JP Morgan Chase, US Bank, Wells Fargo and Citigroup, [and nearly 200 state-chartered banks](https://dbo.ca.gov/covid19-updates-fi/), credit unions are supporting these commitments. \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>Check the Labor and Workforce Development Agency’s [chart detailing the available sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law.\n\nUnpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C103" t="str">
-        <v>https://covid19.ca.gov/get-financial-help/</v>
+        <v>https://covid19.ca.gov/workers/</v>
       </c>
       <c r="D103" t="str">
         <v xml:space="preserve"> </v>
@@ -3060,10 +3060,10 @@
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>What if I already made a payment or was hit with a fee because of COVID-19?</v>
+        <v>What effect will this have on my credit report?</v>
       </c>
       <c r="B104" t="str">
-        <v>Talk to your financial institution. These measures go into effect as of March 25, 2020.  \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>Financial institutions will not report derogatory information (like late payments) to credit reporting agencies but may report a forbearance. Typically this does not negatively affect a credit score on its own.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C104" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -3086,10 +3086,10 @@
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>Is mortgage relief available to businesses?</v>
+        <v>How long will these programs last?</v>
       </c>
       <c r="B105" t="str">
-        <v>The relief is currently only available for residential mortgages.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>It is still unclear how severe or how long the COVID-19 impact will be. Financial institutions have committed to necessary relief and will be assessing the ongoing conditions and need for continuing relief.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C105" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -3112,10 +3112,10 @@
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>What if my mortgage servicer is not communicative or cooperative?</v>
+        <v>What if my financial institution isn’t offering this relief?</v>
       </c>
       <c r="B106" t="str">
-        <v>You can file a complaint with the Department of Business Oversight:\n\n*   File on their [website](https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fdbo.ca.gov%2Ffile-a-complaint%2F&amp;data=02%7C01%7CManuel.Alvarez%40dbo.ca.gov%7Ce2673837ec6f42fce84508d7d114ed59%7Cd6910b1745b44b7bbb66cb7936fabafe%7C1%7C0%7C637207760136603083&amp;sdata=VR6CdqCvrBGkfC%2Bm%2B6Yj9emco9ldVY5BLWSiLpe3f4c%3D&amp;reserved=0)\n*    Call their Consumer Services Office at [(866) 275-2677](tel:(866) 275-2677) or [(916) 327-7585](tel:(916) 327-7585) \n*   Or email Ask.DBO@dbo.ca.gov\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>Call or check their website to be sure. At this time, JP Morgan Chase, US Bank, Wells Fargo and Citigroup, [and nearly 200 state-chartered banks](https://dbo.ca.gov/covid19-updates-fi/), credit unions are supporting these commitments. \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C106" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -3138,10 +3138,10 @@
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>Can I get child care during the stay home order?</v>
+        <v>What if I already made a payment or was hit with a fee because of COVID-19?</v>
       </c>
       <c r="B107" t="str">
-        <v>[Child care options](https://covid19.ca.gov/childcare/) are available if you work at an [essential job](https://covid19.ca.gov/essential-workforce/) or a permitted job in the [current roadmap stage](https://covid19.ca.gov/roadmap/). If you are not working at a job like this, it is important to keep children at home. \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>Talk to your financial institution. These measures go into effect as of March 25, 2020.  \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C107" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -3164,13 +3164,13 @@
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>I am homeless and I may have come in contact with coronavirus. How can I self-isolate with nowhere to go and services closing down?</v>
+        <v>Is mortgage relief available to businesses?</v>
       </c>
       <c r="B108" t="str">
-        <v>A motel or hotel room may be available for you and your family. Contact your local homeless [continuum of care](https://www.bcsh.ca.gov/hcfc/documents/coc_poc.pdf) to connect you to this service.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>The relief is currently only available for residential mortgages.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C108" t="str">
-        <v>https://covid19.ca.gov/housing-and-homelessness/</v>
+        <v>https://covid19.ca.gov/get-financial-help/</v>
       </c>
       <c r="D108" t="str">
         <v xml:space="preserve"> </v>
@@ -3190,13 +3190,13 @@
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>Will there be a rent freeze or waiver for renters? Are evictions allowed during the stay at home order?</v>
+        <v>What if my mortgage servicer is not communicative or cooperative?</v>
       </c>
       <c r="B109" t="str">
-        <v>There is an [order](https://www.gov.ca.gov/2020/03/16/governor-newsom-issues-executive-order-to-protect-renters-and-homeowners-during-covid-19-pandemic/) in place to halt evictions and protect renters. If you are financially affected by COVID-19 and [can’t pay your full rent](https://bcsh.ca.gov/coronavirus19/graphic_rent.pdf), let your landlord know in writing within seven days of the rent due date. Save documentation as proof. The order does not relieve you from the obligation to pay rent. It also does not restrict the landlord from recovering rent that is due.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>You can file a complaint with the Department of Business Oversight:\n\n*   File on their [website](https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fdbo.ca.gov%2Ffile-a-complaint%2F&amp;data=02%7C01%7CManuel.Alvarez%40dbo.ca.gov%7Ce2673837ec6f42fce84508d7d114ed59%7Cd6910b1745b44b7bbb66cb7936fabafe%7C1%7C0%7C637207760136603083&amp;sdata=VR6CdqCvrBGkfC%2Bm%2B6Yj9emco9ldVY5BLWSiLpe3f4c%3D&amp;reserved=0)\n*    Call their Consumer Services Office at [(866) 275-2677](tel:(866) 275-2677) or [(916) 327-7585](tel:(916) 327-7585) \n*   Or email Ask.DBO@dbo.ca.gov\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C109" t="str">
-        <v>https://covid19.ca.gov/housing-and-homelessness/</v>
+        <v>https://covid19.ca.gov/get-financial-help/</v>
       </c>
       <c r="D109" t="str">
         <v xml:space="preserve"> </v>
@@ -3216,13 +3216,13 @@
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>Can landlords delay their payments while their tenants cannot pay rent?</v>
+        <v>Can I get child care during the stay home order?</v>
       </c>
       <c r="B110" t="str">
-        <v>Yes, there are protections in effect through September 30, 2020 for landlords. The [order](https://www.gov.ca.gov/2020/03/16/governor-newsom-issues-executive-order-to-protect-renters-and-homeowners-during-covid-19-pandemic/) requests lenders to halt foreclosures and related evictions during this time. Property owners should contact their financial institutions.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>[Child care options](https://covid19.ca.gov/childcare/) are available if you work at an [essential job](https://covid19.ca.gov/essential-workforce/) or a permitted job in the [current roadmap stage](https://covid19.ca.gov/roadmap/). If you are not working at a job like this, it is important to keep children at home. \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C110" t="str">
-        <v>https://covid19.ca.gov/housing-and-homelessness/</v>
+        <v>https://covid19.ca.gov/get-financial-help/</v>
       </c>
       <c r="D110" t="str">
         <v xml:space="preserve"> </v>
@@ -3242,10 +3242,10 @@
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>How do I get mortgage relief and/or forbearance?</v>
+        <v>I am homeless and I may have come in contact with coronavirus. How can I self-isolate with nowhere to go and services closing down?</v>
       </c>
       <c r="B111" t="str">
-        <v>You should contact and work directly with your mortgage servicer to learn about and apply for available relief. Please note that financial institutions and their servicers are experiencing high volumes of inquiries.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>A motel or hotel room may be available for you and your family. Contact your local homeless [continuum of care](https://www.bcsh.ca.gov/hcfc/documents/coc_poc.pdf) to connect you to this service.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C111" t="str">
         <v>https://covid19.ca.gov/housing-and-homelessness/</v>
@@ -3268,10 +3268,10 @@
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>How long will the forbearance last?</v>
+        <v>Will there be a rent freeze or waiver for renters? Are evictions allowed during the stay at home order?</v>
       </c>
       <c r="B112" t="str">
-        <v>The terms of a forbearance will be agreed to between you and your mortgage service. Financial institutions will confirm approval of and terms of the forbearance program.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>There is an [order](https://www.gov.ca.gov/2020/03/16/governor-newsom-issues-executive-order-to-protect-renters-and-homeowners-during-covid-19-pandemic/) in place to halt evictions and protect renters. If you are financially affected by COVID-19 and [can’t pay your full rent](https://bcsh.ca.gov/coronavirus19/graphic_rent.pdf), let your landlord know in writing within seven days of the rent due date. Save documentation as proof. The order does not relieve you from the obligation to pay rent. It also does not restrict the landlord from recovering rent that is due.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C112" t="str">
         <v>https://covid19.ca.gov/housing-and-homelessness/</v>
@@ -3294,13 +3294,13 @@
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>What if a provider says they have availability on MyChildCare.ca.gov but when I connect with them they have no space?</v>
+        <v>Can landlords delay their payments while their tenants cannot pay rent?</v>
       </c>
       <c r="B113" t="str">
-        <v>The information on [MyChildCare.ca.gov](http://mychildcare.ca.gov/) will be updated twice each week but it is possible that vacancies are filled between updates. Contact your [local childcare resource and referral agency](http://rrnetwork.org/family-services/find-child-care) to find more vacancies. \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
+        <v>Yes, there are protections in effect through September 30, 2020 for landlords. The [order](https://www.gov.ca.gov/2020/03/16/governor-newsom-issues-executive-order-to-protect-renters-and-homeowners-during-covid-19-pandemic/) requests lenders to halt foreclosures and related evictions during this time. Property owners should contact their financial institutions.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C113" t="str">
-        <v>https://covid19.ca.gov/childcare/</v>
+        <v>https://covid19.ca.gov/housing-and-homelessness/</v>
       </c>
       <c r="D113" t="str">
         <v xml:space="preserve"> </v>
@@ -3320,13 +3320,13 @@
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>How can I find out more about the provider listed in MyChildCare.ca.gov?</v>
+        <v>How do I get mortgage relief and/or forbearance?</v>
       </c>
       <c r="B114" t="str">
-        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) includes each provider’s facility/license number. This number can be searched at [CDSS Community Care Licensing Database](https://www.ccld.dss.ca.gov/carefacilitysearch/) to find more information about the provider, like information on inspections and complaints.  \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
+        <v>You should contact and work directly with your mortgage servicer to learn about and apply for available relief. Please note that financial institutions and their servicers are experiencing high volumes of inquiries.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C114" t="str">
-        <v>https://covid19.ca.gov/childcare/</v>
+        <v>https://covid19.ca.gov/housing-and-homelessness/</v>
       </c>
       <c r="D114" t="str">
         <v xml:space="preserve"> </v>
@@ -3346,13 +3346,13 @@
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>How can I find help paying for childcare?</v>
+        <v>How long will the forbearance last?</v>
       </c>
       <c r="B115" t="str">
-        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) provides information on all licensed center-based and family childcare homes. This includes both private-pay and subsidized childcare. Children of essential workers are now eligible to enroll in subsidized emergency childcare through June 30, 2020, or 60 calendar days after the date of the child’s enrollment, whichever is longer. This is subject to capacity and eligibility requirements. Your [local childcare resource and referral agency](https://rrnetwork.org/index.php?p=family-services/find-child-care) can answer more questions about childcare subsidies.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
+        <v>The terms of a forbearance will be agreed to between you and your mortgage service. Financial institutions will confirm approval of and terms of the forbearance program.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C115" t="str">
-        <v>https://covid19.ca.gov/childcare/</v>
+        <v>https://covid19.ca.gov/housing-and-homelessness/</v>
       </c>
       <c r="D115" t="str">
         <v xml:space="preserve"> </v>
@@ -3372,10 +3372,10 @@
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>Can I get childcare during the stay home order?</v>
+        <v>What if a provider says they have availability on MyChildCare.ca.gov but when I connect with them they have no space?</v>
       </c>
       <c r="B116" t="str">
-        <v>Yes, all childcare facilities can open with necessary modifications.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
+        <v>The information on [MyChildCare.ca.gov](http://mychildcare.ca.gov/) will be updated twice each week but it is possible that vacancies are filled between updates. Contact your [local childcare resource and referral agency](http://rrnetwork.org/family-services/find-child-care) to find more vacancies. \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
       </c>
       <c r="C116" t="str">
         <v>https://covid19.ca.gov/childcare/</v>
@@ -3398,10 +3398,10 @@
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>Can my babysitter still come to the house?</v>
+        <v>How can I find out more about the provider listed in MyChildCare.ca.gov?</v>
       </c>
       <c r="B117" t="str">
-        <v>Yes, a childcare worker can come to your home if necessary and should practice basic prevention guidelines (like handwashing for at least 20 seconds, physical distancing, and staying home if feeling ill).\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
+        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) includes each provider’s facility/license number. This number can be searched at [CDSS Community Care Licensing Database](https://www.ccld.dss.ca.gov/carefacilitysearch/) to find more information about the provider, like information on inspections and complaints.  \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
       </c>
       <c r="C117" t="str">
         <v>https://covid19.ca.gov/childcare/</v>
@@ -3424,13 +3424,13 @@
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>County websites:</v>
+        <v>How can I find help paying for childcare?</v>
       </c>
       <c r="B118" t="str">
-        <v>*   [Alameda County](http://www.acphd.org/2019-ncov.aspx)\n*   [Alpine County](http://alpinecountyca.gov/Index.aspx?NID=516)\n*   [Amador County](https://www.amadorgov.org/services/covid-19)\n*   [Butte County](https://www.buttecounty.net/publichealth)\n*   [Calaveras County](https://covid19.calaverasgov.us/)\n*   [Colusa County](https://www.countyofcolusa.org/99/Public-Health)\n*   [Contra Costa County](https://www.coronavirus.cchealth.org/)\n*   [Del Norte County](http://www.co.del-norte.ca.us/departments/health-human-services/public-health)\n*   [El Dorado County](https://www.edcgov.us/Government/hhsa/Pages/EDCCOVID-19.aspx)\n*   [Fresno County](https://www.co.fresno.ca.us/departments/public-health/covid-19)\n*   [Glenn County](https://www.countyofglenn.net/dept/health-human-services/public-health/covid-19)\n*   [Humboldt County](https://humboldtgov.org/2018/Humboldt-Health-Alert)\n*   [Imperial County](http://www.icphd.org/health-information-and-resources/healthy-facts/covid-19/)\n*   [Inyo County](https://www.inyocounty.us/coronavirus-covid-19-response)\n*   [Kern County](https://kernpublichealth.com/2019-novel-coronavirus/)\n*   [Kings County](https://www.countyofkings.com/departments/health-welfare/public-health/coronavirus-disease-2019-covid-19/-fsiteid-1)\n*   [Lake County](http://health.co.lake.ca.us/Coronavirus.htm)\n*   [Lassen County](http://www.co.lassen.ca.us/)\n*   [Los Angeles County](http://publichealth.lacounty.gov/media/Coronavirus/)\n*   [Madera County](https://www.maderacounty.com/government/public-health/health-updates/corona-virus)\n*   [Marin County](https://coronavirus.marinhhs.org/)\n*   [Mariposa County](http://www.mariposacounty.org/1592/COVID-19-Information)\n*   [Mendocino County](https://www.mendocinocounty.org/community/novel-coronavirus)\n*   [Merced County](https://www.co.merced.ca.us/3350/Coronavirus-Disease-2019)\n*   [Modoc County](http://www.co.modoc.ca.us/)\n*   [Mono County](https://coronavirus.monocounty.ca.gov/)\n*   [Monterey County](https://www.co.monterey.ca.us/government/departments-a-h/health/diseases/2019-novel-coronavirus-covid-19)\n*   [Napa County](https://www.countyofnapa.org/2739/Coronavirus)\n*   [Nevada County](https://www.mynevadacounty.com/2924/Coronavirus)\n*   [Orange County](https://www.ochealthinfo.com/phs/about/epidasmt/epi/dip/prevention/novel_coronavirus)\n*   [Placer County](https://www.placer.ca.gov/coronavirus)\n*   [Plumas County](https://www.plumascounty.us/2669/Novel-Coronavirus-2019-COVID-19)\n*   [Riverside County](https://www.rivcoph.org/coronavirus)\n*   [Sacramento County](https://dhs.saccounty.net/PUB/Pages/PUB-Home.aspx)\n*   [San Benito County](https://hhsa.cosb.us/publichealth/communicable-disease/coronavirus/)\n*   [San Bernardino County](http://wp.sbcounty.gov/dph/coronavirus/)\n*   [San Diego County](https://www.sandiegocounty.gov/coronavirus.html)\n*   [San Francisco City and County](https://sf.gov/topics/coronavirus-covid-19)\n*   [San Joaquin County](https://www.sjgov.org/covid19/)\n*   [San Luis Obispo County](https://www.emergencyslo.org/en/covid19.aspx)\n*   [San Mateo County](https://www.smchealth.org/coronavirus)\n*   [Santa Barbara County](https://publichealthsbc.org/)\n*   [Santa Clara County](https://www.sccgov.org/sites/phd/DiseaseInformation/novel-coronavirus/Pages/home.aspx)\n*   [Santa Cruz County](https://www.santacruzhealth.org/HSAHome/HSADivisions/PublicHealth/CommunicableDiseaseControl/Coronavirus.aspx)\n*   [Shasta County](https://www.co.shasta.ca.us/index/hhsa/health-safety/current-heath-concerns/coronavirus)\n*   [Sierra County](http://sierracounty.ca.gov/582/Coronavirus-COVID-19)\n*   [Siskiyou County](https://www.co.siskiyou.ca.us/publichealth/page/coronavirus-covid-19-what-siskiyou-county-residents-need-know)\n*   [Solano County](http://www.solanocounty.com/depts/ph/ncov.asp)\n*   [Sonoma County](https://socoemergency.org/emergency/novel-coronavirus/)\n*   [Stanislaus County](http://schsa.org/publichealth/pages/corona-virus/)\n*   [Sutter County](https://www.suttercounty.org/doc/government/depts/cao/em/coronavirus)\n*   [Tehama County](https://www.tehamacohealthservices.net/services/communicable-diseases/#current-events)\n*   [Trinity County](https://www.trinitycounty.org/)\n*   [Tulare County](https://tchhsa.org/eng/index.cfm/public-health/covid-19-updates-novel-coronavirus/)\n*   [Tuolumne County](https://www.tuolumnecounty.ca.gov/250/Public-Health)\n*   [Ventura County](https://www.vcemergency.com/)\n*   [Yolo County](https://www.yolocounty.org/health-human-services/adults/communicable-disease-investigation-and-control/novel-coronavirus-2019)\n*   [Yuba County](https://www.yuba.org/coronavirus/)\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) provides information on all licensed center-based and family childcare homes. This includes both private-pay and subsidized childcare. Children of essential workers are now eligible to enroll in subsidized emergency childcare through June 30, 2020, or 60 calendar days after the date of the child’s enrollment, whichever is longer. This is subject to capacity and eligibility requirements. Your [local childcare resource and referral agency](https://rrnetwork.org/index.php?p=family-services/find-child-care) can answer more questions about childcare subsidies.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
       </c>
       <c r="C118" t="str">
-        <v>https://covid19.ca.gov/state-local-resources/</v>
+        <v>https://covid19.ca.gov/childcare/</v>
       </c>
       <c r="D118" t="str">
         <v xml:space="preserve"> </v>
@@ -3450,13 +3450,13 @@
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>What are the restrictions in my area?</v>
+        <v>Can I get childcare during the stay home order?</v>
       </c>
       <c r="B119" t="str">
-        <v>While each county may have different restrictions, it is important to stay home as much as possible. If you do go out, stay 6 feet away from others who are not in your household and wear a cloth mask. Your actions save lives.\n\nSee what [industries are open or closed](https://covid19.ca.gov/roadmap-counties/#track-data) in your county.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>Yes, all childcare facilities can open with necessary modifications.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
       </c>
       <c r="C119" t="str">
-        <v>https://covid19.ca.gov/state-local-resources/</v>
+        <v>https://covid19.ca.gov/childcare/</v>
       </c>
       <c r="D119" t="str">
         <v xml:space="preserve"> </v>
@@ -3476,13 +3476,13 @@
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>How are we helping the homeless?</v>
+        <v>Can my babysitter still come to the house?</v>
       </c>
       <c r="B120" t="str">
-        <v>Each county and local government in California has [increased resources](https://covid19.ca.gov/housing-and-homelessness/#top) to protect people experiencing homelessness during COVID-19. [Financial protections](https://covid19.ca.gov/housing-and-homelessness/#top) were added to prevent others from losing their homes during the outbreak.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>Yes, a childcare worker can come to your home if necessary and should practice basic prevention guidelines (like handwashing for at least 20 seconds, physical distancing, and staying home if feeling ill).\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
       </c>
       <c r="C120" t="str">
-        <v>https://covid19.ca.gov/state-local-resources/</v>
+        <v>https://covid19.ca.gov/childcare/</v>
       </c>
       <c r="D120" t="str">
         <v xml:space="preserve"> </v>
@@ -3502,10 +3502,10 @@
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>How is the state protecting incarcerated people in California?</v>
+        <v>County websites:</v>
       </c>
       <c r="B121" t="str">
-        <v>[California Department of Corrections and Rehabilitation (CDCR)](https://www.cdcr.ca.gov/covid19/) is dedicated to the safety of everyone who lives in, works in, and visits state prisons. CDCR has given all staff and inmates 2 reusable cloth masks to wear while moving between cells, dorms, meetings with others, or health care appointments. CDCR also requires ongoing testing for all staff working in adult institutions, suspended non-essential transfer of inmates, and suspended volunteer services and in-person visiting.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>*   [Alameda County](http://www.acphd.org/2019-ncov.aspx)\n*   [Alpine County](http://alpinecountyca.gov/Index.aspx?NID=516)\n*   [Amador County](https://www.amadorgov.org/services/covid-19)\n*   [Butte County](https://www.buttecounty.net/publichealth)\n*   [Calaveras County](https://covid19.calaverasgov.us/)\n*   [Colusa County](https://www.countyofcolusa.org/99/Public-Health)\n*   [Contra Costa County](https://www.coronavirus.cchealth.org/)\n*   [Del Norte County](http://www.co.del-norte.ca.us/departments/health-human-services/public-health)\n*   [El Dorado County](https://www.edcgov.us/Government/hhsa/Pages/EDCCOVID-19.aspx)\n*   [Fresno County](https://www.co.fresno.ca.us/departments/public-health/covid-19)\n*   [Glenn County](https://www.countyofglenn.net/dept/health-human-services/public-health/covid-19)\n*   [Humboldt County](https://humboldtgov.org/2018/Humboldt-Health-Alert)\n*   [Imperial County](http://www.icphd.org/health-information-and-resources/healthy-facts/covid-19/)\n*   [Inyo County](https://www.inyocounty.us/coronavirus-covid-19-response)\n*   [Kern County](https://kernpublichealth.com/2019-novel-coronavirus/)\n*   [Kings County](https://www.countyofkings.com/departments/health-welfare/public-health/coronavirus-disease-2019-covid-19/-fsiteid-1)\n*   [Lake County](http://health.co.lake.ca.us/Coronavirus.htm)\n*   [Lassen County](http://www.co.lassen.ca.us/)\n*   [Los Angeles County](http://publichealth.lacounty.gov/media/Coronavirus/)\n*   [Madera County](https://www.maderacounty.com/government/public-health/health-updates/corona-virus)\n*   [Marin County](https://coronavirus.marinhhs.org/)\n*   [Mariposa County](http://www.mariposacounty.org/1592/COVID-19-Information)\n*   [Mendocino County](https://www.mendocinocounty.org/community/novel-coronavirus)\n*   [Merced County](https://www.co.merced.ca.us/3350/Coronavirus-Disease-2019)\n*   [Modoc County](http://www.co.modoc.ca.us/)\n*   [Mono County](https://coronavirus.monocounty.ca.gov/)\n*   [Monterey County](https://www.co.monterey.ca.us/government/departments-a-h/health/diseases/2019-novel-coronavirus-covid-19)\n*   [Napa County](https://www.countyofnapa.org/2739/Coronavirus)\n*   [Nevada County](https://www.mynevadacounty.com/2924/Coronavirus)\n*   [Orange County](https://www.ochealthinfo.com/phs/about/epidasmt/epi/dip/prevention/novel_coronavirus)\n*   [Placer County](https://www.placer.ca.gov/coronavirus)\n*   [Plumas County](https://www.plumascounty.us/2669/Novel-Coronavirus-2019-COVID-19)\n*   [Riverside County](https://www.rivcoph.org/coronavirus)\n*   [Sacramento County](https://dhs.saccounty.net/PUB/Pages/PUB-Home.aspx)\n*   [San Benito County](https://hhsa.cosb.us/publichealth/communicable-disease/coronavirus/)\n*   [San Bernardino County](http://wp.sbcounty.gov/dph/coronavirus/)\n*   [San Diego County](https://www.sandiegocounty.gov/coronavirus.html)\n*   [San Francisco City and County](https://sf.gov/topics/coronavirus-covid-19)\n*   [San Joaquin County](https://www.sjgov.org/covid19/)\n*   [San Luis Obispo County](https://www.emergencyslo.org/en/covid19.aspx)\n*   [San Mateo County](https://www.smchealth.org/coronavirus)\n*   [Santa Barbara County](https://publichealthsbc.org/)\n*   [Santa Clara County](https://www.sccgov.org/sites/phd/DiseaseInformation/novel-coronavirus/Pages/home.aspx)\n*   [Santa Cruz County](https://www.santacruzhealth.org/HSAHome/HSADivisions/PublicHealth/CommunicableDiseaseControl/Coronavirus.aspx)\n*   [Shasta County](https://www.co.shasta.ca.us/index/hhsa/health-safety/current-heath-concerns/coronavirus)\n*   [Sierra County](http://sierracounty.ca.gov/582/Coronavirus-COVID-19)\n*   [Siskiyou County](https://www.co.siskiyou.ca.us/publichealth/page/coronavirus-covid-19-what-siskiyou-county-residents-need-know)\n*   [Solano County](http://www.solanocounty.com/depts/ph/ncov.asp)\n*   [Sonoma County](https://socoemergency.org/emergency/novel-coronavirus/)\n*   [Stanislaus County](http://schsa.org/publichealth/pages/corona-virus/)\n*   [Sutter County](https://www.suttercounty.org/doc/government/depts/cao/em/coronavirus)\n*   [Tehama County](https://www.tehamacohealthservices.net/services/communicable-diseases/#current-events)\n*   [Trinity County](https://www.trinitycounty.org/)\n*   [Tulare County](https://tchhsa.org/eng/index.cfm/public-health/covid-19-updates-novel-coronavirus/)\n*   [Tuolumne County](https://www.tuolumnecounty.ca.gov/250/Public-Health)\n*   [Ventura County](https://www.vcemergency.com/)\n*   [Yolo County](https://www.yolocounty.org/health-human-services/adults/communicable-disease-investigation-and-control/novel-coronavirus-2019)\n*   [Yuba County](https://www.yuba.org/coronavirus/)\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C121" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3528,10 +3528,10 @@
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>Who can I contact about my child custody order and child visitation rights?</v>
+        <v>What are the restrictions in my area?</v>
       </c>
       <c r="B122" t="str">
-        <v>Court operations vary from county to county. You can use the [California Courts Self-Help Center](https://www.courts.ca.gov/selfhelp.htm) or reach out to your [local government office](https://www.courts.ca.gov/find-my-court.htm?query=browse_courts) for more information. \n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>While each county may have different restrictions, it is important to stay home as much as possible. If you do go out, stay 6 feet away from others who are not in your household and wear a cloth mask. Your actions save lives.\n\nSee what [industries are open or closed](https://covid19.ca.gov/roadmap-counties/#track-data) in your county.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C122" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3554,10 +3554,10 @@
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>Do I have to report to jury duty if summoned?</v>
+        <v>How are we helping the homeless?</v>
       </c>
       <c r="B123" t="str">
-        <v>Court operations vary from county to county. You can use the [California Courts Self-Help Center](https://www.courts.ca.gov/selfhelp.htm) or reach out to your [local government office](https://www.courts.ca.gov/find-my-court.htm?query=browse_courts) for more information about jury duty.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)&lt;!-- jury duty, summons, courts, court, court operations--&gt;</v>
+        <v>Each county and local government in California has [increased resources](https://covid19.ca.gov/housing-and-homelessness/#top) to protect people experiencing homelessness during COVID-19. [Financial protections](https://covid19.ca.gov/housing-and-homelessness/#top) were added to prevent others from losing their homes during the outbreak.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C123" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3580,13 +3580,13 @@
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>When is the disaster relief assistance available?</v>
+        <v>How is the state protecting incarcerated people in California?</v>
       </c>
       <c r="B124" t="str">
-        <v>Individuals may begin applying on May 18, 2020. Assistance will be available until the funding is spent or until June 30, 2020, at the latest. Applicants will be considered on a first-come, first-served basis. Applicants may only apply with the nonprofit organization(s) in their county of residency.\n\n**Please note:**\n\n*   Funding is limited, and disaster relief application services and assistance are not guaranteed.\n*   Nonprofit organizations will not be assisting individuals before May 18. Individuals _should not_ contact them ahead of time regarding disaster relief assistance.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>[California Department of Corrections and Rehabilitation (CDCR)](https://www.cdcr.ca.gov/covid19/) is dedicated to the safety of everyone who lives in, works in, and visits state prisons. CDCR has given all staff and inmates 2 reusable cloth masks to wear while moving between cells, dorms, meetings with others, or health care appointments. CDCR also requires ongoing testing for all staff working in adult institutions, suspended non-essential transfer of inmates, and suspended volunteer services and in-person visiting.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C124" t="str">
-        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
+        <v>https://covid19.ca.gov/state-local-resources/</v>
       </c>
       <c r="D124" t="str">
         <v xml:space="preserve"> </v>
@@ -3606,13 +3606,13 @@
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v>Who is eligible for this disaster relief assistance?</v>
+        <v>Who can I contact about my child custody order and child visitation rights?</v>
       </c>
       <c r="B125" t="str">
-        <v>Eligible individuals must be able to provide information that they:\n\n*   Are an undocumented adult (person over the age of 18)\n*   Are not eligible for federal COVID-19 assistance, like the CARES Act stimulus payments or pandemic unemployment benefits, and\n*   Have experienced hardship as a result of COVID-19.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>Court operations vary from county to county. You can use the [California Courts Self-Help Center](https://www.courts.ca.gov/selfhelp.htm) or reach out to your [local government office](https://www.courts.ca.gov/find-my-court.htm?query=browse_courts) for more information. \n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C125" t="str">
-        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
+        <v>https://covid19.ca.gov/state-local-resources/</v>
       </c>
       <c r="D125" t="str">
         <v xml:space="preserve"> </v>
@@ -3632,13 +3632,13 @@
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v>Can getting this assistance affect my ability to get a green card or to become a U.S. Citizen? Will receiving it make me a public charge?</v>
+        <v>Do I have to report to jury duty if summoned?</v>
       </c>
       <c r="B126" t="str">
-        <v>This disaster relief assistance is not means-tested and is one-time assistance. The federal government does not list this assistance as a public benefit for a public charge consideration. However, USCIS has not issued specific guidance related to this assistance.\n\nIf you have questions about your immigration status and this program, please consult an attorney. A list of free and low-cost immigration services providers is available in the [Guide for Immigrant Californians (PDF)](/wp-content/uploads/2020/04/LISTOS_COVID_19_immigrant_guidance_EN_dAf.pdf).\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>Court operations vary from county to county. You can use the [California Courts Self-Help Center](https://www.courts.ca.gov/selfhelp.htm) or reach out to your [local government office](https://www.courts.ca.gov/find-my-court.htm?query=browse_courts) for more information about jury duty.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)&lt;!-- jury duty, summons, courts, court, court operations--&gt;</v>
       </c>
       <c r="C126" t="str">
-        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
+        <v>https://covid19.ca.gov/state-local-resources/</v>
       </c>
       <c r="D126" t="str">
         <v xml:space="preserve"> </v>
@@ -3658,10 +3658,10 @@
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v>Is the personal information I provide to the nonprofits protected?</v>
+        <v>When is the disaster relief assistance available?</v>
       </c>
       <c r="B127" t="str">
-        <v>Your information is only used to confirm eligibility and provide the assistance. No personal information (like name or address) will be given to any government agency. Only general information like age, gender, and preferred language will be shared with the State of California.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>Individuals may begin applying on May 18, 2020. Assistance will be available until the funding is spent or until June 30, 2020, at the latest. Applicants will be considered on a first-come, first-served basis. Applicants may only apply with the nonprofit organization(s) in their county of residency.\n\n**Please note:**\n\n*   Funding is limited, and disaster relief application services and assistance are not guaranteed.\n*   Nonprofit organizations will not be assisting individuals before May 18. Individuals _should not_ contact them ahead of time regarding disaster relief assistance.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C127" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3684,10 +3684,10 @@
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v>How do I apply?</v>
+        <v>Who is eligible for this disaster relief assistance?</v>
       </c>
       <c r="B128" t="str">
-        <v>The California Department of Social Services (CDSS) has identified non-profit where you can apply for disaster assistance. Find the [nonprofit where you can apply in your area](https://cdss.ca.gov/inforesources/immigration/covid-19-drai).\n\nApply _no sooner than May 18, and only to the organization in your area._ They will assist you with applying, confirm your eligibility, and deliver a payment card if you are approved. Applications will be considered on a first-come, first-served basis.\n\nFunding is limited, and disaster relief application services and assistance are not guaranteed.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>Eligible individuals must be able to provide information that they:\n\n*   Are an undocumented adult (person over the age of 18)\n*   Are not eligible for federal COVID-19 assistance, like the CARES Act stimulus payments or pandemic unemployment benefits, and\n*   Have experienced hardship as a result of COVID-19.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C128" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3710,10 +3710,10 @@
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v>How many people in a household can receive this assistance?</v>
+        <v>Can getting this assistance affect my ability to get a green card or to become a U.S. Citizen? Will receiving it make me a public charge?</v>
       </c>
       <c r="B129" t="str">
-        <v>A maximum of two adults per household can qualify for this assistance, for a total of $1,000 per household. A household is defined as individuals who live, shop, and prepare meals together.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>This disaster relief assistance is not means-tested and is one-time assistance. The federal government does not list this assistance as a public benefit for a public charge consideration. However, USCIS has not issued specific guidance related to this assistance.\n\nIf you have questions about your immigration status and this program, please consult an attorney. A list of free and low-cost immigration services providers is available in the [Guide for Immigrant Californians (PDF)](https://files.covid19.ca.gov/pdf/COVID_immigrant_guidance--en.pdf).\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C129" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3736,10 +3736,10 @@
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v>How do eligible individuals receive this assistance?</v>
+        <v>Is the personal information I provide to the nonprofits protected?</v>
       </c>
       <c r="B130" t="str">
-        <v>You will get a payment card either in person or through the mail. The organization in your area can give you more information.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>Your information is only used to confirm eligibility and provide the assistance. No personal information (like name or address) will be given to any government agency. Only general information like age, gender, and preferred language will be shared with the State of California.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C130" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3762,10 +3762,10 @@
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v>How long do I have to apply?</v>
+        <v>How do I apply?</v>
       </c>
       <c r="B131" t="str">
-        <v>Payments will be distributed beginning on May 18, 2020. They will continue until the $75 million in funding is spent, or until June 30, 2020 at the latest. We expect that this disaster relief assistance will run out very quickly. Apply as soon as you can, but not before May 18.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>The California Department of Social Services (CDSS) has identified non-profit where you can apply for disaster assistance. Find the [nonprofit where you can apply in your area](https://cdss.ca.gov/inforesources/immigration/covid-19-drai).\n\nApply _no sooner than May 18, and only to the organization in your area._ They will assist you with applying, confirm your eligibility, and deliver a payment card if you are approved. Applications will be considered on a first-come, first-served basis.\n\nFunding is limited, and disaster relief application services and assistance are not guaranteed.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C131" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3788,10 +3788,10 @@
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v>If I am unable to apply for this program, are there other organizations that can help me?</v>
+        <v>How many people in a household can receive this assistance?</v>
       </c>
       <c r="B132" t="str">
-        <v>Yes. The California Immigrant Resilience Fund is raising $50 million to provide cash assistance to undocumented Californians who are ineligible for other COVID-19 programs. Visit the [California Immigrant Resilience Fund](http://www.immigrantfundca.org) website to see if you can benefit from this program.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>A maximum of two adults per household can qualify for this assistance, for a total of $1,000 per household. A household is defined as individuals who live, shop, and prepare meals together.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C132" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3814,10 +3814,10 @@
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v>What other government programs may I be eligible for during the COVID-19 pandemic?</v>
+        <v>How do eligible individuals receive this assistance?</v>
       </c>
       <c r="B133" t="str">
-        <v>Check the [Guide for Immigrant Californians (PDF)](/wp-content/uploads/2020/04/LISTOS_COVID_19_immigrant_guidance_EN_dAf.pdf). It has information about jobs, wages, benefits, and small business and housing support.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>You will get a payment card either in person or through the mail. The organization in your area can give you more information.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C133" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3840,13 +3840,13 @@
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v>Youth and Teens</v>
+        <v>How long do I have to apply?</v>
       </c>
       <c r="B134" t="str">
-        <v>*   [California Youth Crisis Line](https://calyouth.org/cycl/)**:** Youth ages 12-24 can call or text [800-843-5200](tel:800-843-5200) or [chat online](https://m2.icarol.com/ConsumerRegistration.aspx?org=53141&amp;pid=326&amp;cc=en-US) for 24/7 crisis support.\n*   [TEEN LINE](https://teenlineonline.org/talk-now/): Teens can talk to another teen by texting “TEEN” to [839863](sms:839863) from 6pm – 9pm, or call [800-852-8336](tel:800-852-8336) from 6pm – 10pm.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>Payments will be distributed beginning on May 18, 2020. They will continue until the $75 million in funding is spent, or until June 30, 2020 at the latest. We expect that this disaster relief assistance will run out very quickly. Apply as soon as you can, but not before May 18.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C134" t="str">
-        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
+        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
       </c>
       <c r="D134" t="str">
         <v xml:space="preserve"> </v>
@@ -3866,13 +3866,13 @@
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v>Veterans</v>
+        <v>If I am unable to apply for this program, are there other organizations that can help me?</v>
       </c>
       <c r="B135" t="str">
-        <v>[Veterans Crisis Line](https://www.veteranscrisisline.net): Call [800-273-8255](tel:800-273-8255) and Press 1 or text [838255](sms:838255) for 24/7 support.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>Yes. The California Immigrant Resilience Fund is raising $50 million to provide cash assistance to undocumented Californians who are ineligible for other COVID-19 programs. Visit the [California Immigrant Resilience Fund](http://www.immigrantfundca.org) website to see if you can benefit from this program.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C135" t="str">
-        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
+        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
       </c>
       <c r="D135" t="str">
         <v xml:space="preserve"> </v>
@@ -3892,13 +3892,13 @@
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v>First Responders and Law Enforcement</v>
+        <v>What other government programs may I be eligible for during the COVID-19 pandemic?</v>
       </c>
       <c r="B136" t="str">
-        <v>*   [Fire/EMS helpline](https://www.nvfc.org/fireems-helpline/): Call [888-731-FIRE](tel:888-731-FIRE) to get 24/7 help for a variety of behavioral health issues.\n*   [COPLINE](https://www.copline.org/): Call [800-267-5463](tel:800-267-5463) to find support 24/7 for law enforcement officers.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>Check the [Guide for Immigrant Californians (PDF)](/wp-content/uploads/2020/04/LISTOS_COVID_19_immigrant_guidance_EN_dAf.pdf). It has information about jobs, wages, benefits, and small business and housing support.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C136" t="str">
-        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
+        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
       </c>
       <c r="D136" t="str">
         <v xml:space="preserve"> </v>
@@ -3918,10 +3918,10 @@
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v>Older Californians</v>
+        <v>Youth and Teens</v>
       </c>
       <c r="B137" t="str">
-        <v>*   [Friendship Line](https://www.ioaging.org/services/all-inclusive-health-care/friendship-line): Call [888-670-1360](tel:888-670-1360) for 24/7 support if you are 60 years or older, or an adult living with disabilities.  \n*   California Aging and Adult Information Line: Call [800-510-2020](tel:800-510-2020) for help finding local assistance. \n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>*   [California Youth Crisis Line](https://calyouth.org/cycl/)**:** Youth ages 12-24 can call or text [800-843-5200](tel:800-843-5200) or [chat online](https://m2.icarol.com/ConsumerRegistration.aspx?org=53141&amp;pid=326&amp;cc=en-US) for 24/7 crisis support.\n*   [TEEN LINE](https://teenlineonline.org/talk-now/): Teens can talk to another teen by texting “TEEN” to [839863](sms:839863) from 6pm – 9pm, or call [800-852-8336](tel:800-852-8336) from 6pm – 10pm.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C137" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -3944,10 +3944,10 @@
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v>Deaf and Hard of Hearing Individuals</v>
+        <v>Veterans</v>
       </c>
       <c r="B138" t="str">
-        <v>[National Suicide Prevention Deaf and Hard of Hearing Hotline](https://suicidepreventionlifeline.org/help-yourself/for-deaf-hard-of-hearing/): Access 24/7 video relay service by dialing [800-273-8255](tel:800-273-8255) (TTY [800-799-4889](tel:800-799-4889)).\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>[Veterans Crisis Line](https://www.veteranscrisisline.net): Call [800-273-8255](tel:800-273-8255) and Press 1 or text [838255](sms:838255) for 24/7 support.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C138" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -3970,10 +3970,10 @@
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>Services for Substance Use Disorders</v>
+        <v>First Responders and Law Enforcement</v>
       </c>
       <c r="B139" t="str">
-        <v>*   [SAMHSA National Helpline](https://www.samhsa.gov/find-help/national-helpline): Call [800-662-HELP](tel:1-800-662-4357) for 24/7 information and referrals in English and Spanish. \n*   [SAMHSA Treatment Locator](https://findtreatment.samhsa.gov)**:**  Find drug or alcohol treatment programs. \n*   [Local county access lines](https://gcc01.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.dhcs.ca.gov%2Findividuals%2FPages%2FSUD_County_Access_Lines.aspx&amp;data=02%7C01%7CJanne.Olson-Morgan%40osg.ca.gov%7C122307be91754d12e5dc08d7d984f958%7C265c2dcd2a6e43aab2e826421a8c8526%7C0%7C0%7C637217037446186621&amp;sdata=5sx4UdIlVkRL%2BEJR7FrpK0gYAn20yE71TyBDFIw1kJM%3D&amp;reserved=0): Find your local number for help seeking substance use disorder services.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>*   [Fire/EMS helpline](https://www.nvfc.org/fireems-helpline/): Call [888-731-FIRE](tel:888-731-FIRE) to get 24/7 help for a variety of behavioral health issues.\n*   [COPLINE](https://www.copline.org/): Call [800-267-5463](tel:800-267-5463) to find support 24/7 for law enforcement officers.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C139" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -3996,10 +3996,10 @@
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>LGBTQ Individuals</v>
+        <v>Older Californians</v>
       </c>
       <c r="B140" t="str">
-        <v>*   [Trevor Project](https://www.thetrevorproject.org): Call [866-488-7386](tel:866-488-7386) or text START to [678678](sms:678678) for 24/7 information and suicide prevention resources for LGBTQ youth.\n*   [Lesbian, Gay, Bisexual and Transgender National Hotline](https://www.glbthotline.org/hotline.html): Call [800-273-8255](tel:800-273-8255) from 1pm – 9pm for support, information or help finding resources.\n*   [Victims of Crime Resource Center](https://1800victims.org/): Call or text [800-842-8467](tel:800-842-8467) or [chat online](https://1800victims.org/) for information about LGTBQ rights, legal protections, and local resources.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>*   [Friendship Line](https://www.ioaging.org/services/all-inclusive-health-care/friendship-line): Call [888-670-1360](tel:888-670-1360) for 24/7 support if you are 60 years or older, or an adult living with disabilities.  \n*   California Aging and Adult Information Line: Call [800-510-2020](tel:800-510-2020) for help finding local assistance. \n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C140" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -4022,13 +4022,13 @@
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>What is a close contact?</v>
+        <v>Deaf and Hard of Hearing Individuals</v>
       </c>
       <c r="B141" t="str">
-        <v>A close contact is someone who was within 6 feet of a person with COVID-19 for at least 15 minutes. This usually includes household members, intimate contacts, and caregivers, but can include others.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>[National Suicide Prevention Deaf and Hard of Hearing Hotline](https://suicidepreventionlifeline.org/help-yourself/for-deaf-hard-of-hearing/): Access 24/7 video relay service by dialing [800-273-8255](tel:800-273-8255) (TTY [800-799-4889](tel:800-799-4889)).\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C141" t="str">
-        <v>https://covid19.ca.gov/contact-tracing/</v>
+        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
       </c>
       <c r="D141" t="str">
         <v xml:space="preserve"> </v>
@@ -4048,13 +4048,13 @@
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>Will contact tracers track my location?</v>
+        <v>Services for Substance Use Disorders</v>
       </c>
       <c r="B142" t="str">
-        <v>California’s contact tracing program does not use any cell phone tracking technology. Someone from your local public health department will simply speak privately with you. All information is confidential and protected by California’s strict privacy laws. They may stay in touch to make sure your symptoms aren’t worsening.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>*   [SAMHSA National Helpline](https://www.samhsa.gov/find-help/national-helpline): Call [800-662-HELP](tel:1-800-662-4357) for 24/7 information and referrals in English and Spanish. \n*   [SAMHSA Treatment Locator](https://findtreatment.samhsa.gov)**:**  Find drug or alcohol treatment programs. \n*   [Local county access lines](https://gcc01.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.dhcs.ca.gov%2Findividuals%2FPages%2FSUD_County_Access_Lines.aspx&amp;data=02%7C01%7CJanne.Olson-Morgan%40osg.ca.gov%7C122307be91754d12e5dc08d7d984f958%7C265c2dcd2a6e43aab2e826421a8c8526%7C0%7C0%7C637217037446186621&amp;sdata=5sx4UdIlVkRL%2BEJR7FrpK0gYAn20yE71TyBDFIw1kJM%3D&amp;reserved=0): Find your local number for help seeking substance use disorder services.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C142" t="str">
-        <v>https://covid19.ca.gov/contact-tracing/</v>
+        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
       </c>
       <c r="D142" t="str">
         <v xml:space="preserve"> </v>
@@ -4074,13 +4074,13 @@
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>Is contact tracing help available in my language?</v>
+        <v>LGBTQ Individuals</v>
       </c>
       <c r="B143" t="str">
-        <v>Your [local health department](https://covid19.ca.gov/state-local-resources/#top) can communicate with you in many different languages.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>*   [Trevor Project](https://www.thetrevorproject.org): Call [866-488-7386](tel:866-488-7386) or text START to [678678](sms:678678) for 24/7 information and suicide prevention resources for LGBTQ youth.\n*   [Lesbian, Gay, Bisexual and Transgender National Hotline](https://www.glbthotline.org/hotline.html): Call [800-273-8255](tel:800-273-8255) from 1pm – 9pm for support, information or help finding resources.\n*   [Victims of Crime Resource Center](https://1800victims.org/): Call or text [800-842-8467](tel:800-842-8467) or [chat online](https://1800victims.org/) for information about LGTBQ rights, legal protections, and local resources.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C143" t="str">
-        <v>https://covid19.ca.gov/contact-tracing/</v>
+        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
       </c>
       <c r="D143" t="str">
         <v xml:space="preserve"> </v>
@@ -4100,10 +4100,10 @@
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>Who should get tested?</v>
+        <v>What is a close contact?</v>
       </c>
       <c r="B144" t="str">
-        <v>You should get tested if you:\n\n*   Are a close contact of anyone who has or may have COVID-19, or\n*   Think you may have been exposed, or\n*   Are having [COVID-19 symptoms](https://covid19.ca.gov/symptoms-and-risks/). \n\nFind a [testing site in your area](https://covid19.ca.gov/testing-and-treatment/).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>A close contact is someone who was within 6 feet of a person with COVID-19 for at least 15 minutes. This usually includes household members, intimate contacts, and caregivers, but can include others.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C144" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4126,10 +4126,10 @@
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>How do I find a testing location?</v>
+        <v>Will contact tracers track my location?</v>
       </c>
       <c r="B145" t="str">
-        <v>To learn more about testing and care, visit the [Testing and treatment page](https://covid19.ca.gov/testing-and-treatment/). You can search for testing locations there using your zip code. \n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>California’s contact tracing program does not use any cell phone tracking technology. Someone from your local public health department will simply speak privately with you. All information is confidential and protected by California’s strict privacy laws. They may stay in touch to make sure your symptoms aren’t worsening.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C145" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4152,10 +4152,10 @@
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>What if I have COVID-19 symptoms and have not been contacted by the health department?</v>
+        <v>Is contact tracing help available in my language?</v>
       </c>
       <c r="B146" t="str">
-        <v>[Get tested](https://covid19.ca.gov/testing-and-treatment/) immediately, contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing, and [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) yourself while waiting for your test results.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>Your [local health department](https://covid19.ca.gov/state-local-resources/#top) can communicate with you in many different languages.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C146" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4178,10 +4178,10 @@
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>What if I came in contact with someone who has COVID-19 symptoms, but my local health department is not aware of it?</v>
+        <v>Who should get tested?</v>
       </c>
       <c r="B147" t="str">
-        <v>You should [get tested](https://covid19.ca.gov/testing-and-treatment/). Contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing, and [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) yourself while waiting for your test results.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>You should get tested if you:\n\n*   Are a close contact of anyone who has or may have COVID-19, or\n*   Think you may have been exposed, or\n*   Are having [COVID-19 symptoms](https://covid19.ca.gov/symptoms-and-risks/). \n\nFind a [testing site in your area](https://covid19.ca.gov/testing-and-treatment/).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C147" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4204,10 +4204,10 @@
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>How do I become a contact tracer?</v>
+        <v>How do I find a testing location?</v>
       </c>
       <c r="B148" t="str">
-        <v>The initial phase of California Connected, the state’s contact tracing program, will utilize existing resources and redirect state employees to begin contact tracing efforts. Offers of additional support from the private sector and qualified members of the public are appreciated, but contact tracers from outside state government may not be needed until a future phase. Thank you for wanting to share your expertise and resources with your fellow Californians.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>To learn more about testing and care, visit the [Testing and treatment page](https://covid19.ca.gov/testing-and-treatment/). You can search for testing locations there using your zip code. \n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C148" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4230,13 +4230,13 @@
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v>Affected counties as of 7/16/20</v>
+        <v>What if I have COVID-19 symptoms and have not been contacted by the health department?</v>
       </c>
       <c r="B149" t="str">
-        <v>*   Alameda\n*   Colusa\n*   Contra Costa\n*   Fresno\n*   Glenn\n*   Imperial\n*   Kings\n*   Los Angeles\n*   Madera\n*   Marin\n*   Merced\n*   Monterey\n*   Napa\n*   Orange\n*   Placer\n*   Riverside\n*   Sacramento\n*   San Benito\n*   San Bernardino\n*   San Diego\n*   San Joaquin\n*   San Luis Obispo\n*   Santa Barbara\n*   Santa Clara\n*   Solano\n*   Sonoma\n*   Stanislaus\n*   Sutter\n*   Tulare\n*   Yolo\n*   Yuba\n*   Ventura\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>[Get tested](https://covid19.ca.gov/testing-and-treatment/) immediately, contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing, and [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) yourself while waiting for your test results.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C149" t="str">
-        <v>https://covid19.ca.gov/roadmap-counties/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D149" t="str">
         <v xml:space="preserve"> </v>
@@ -4256,13 +4256,13 @@
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>For attested counties not on Monitoring List</v>
+        <v>What if I came in contact with someone who has COVID-19 symptoms, but my local health department is not aware of it?</v>
       </c>
       <c r="B150" t="str">
-        <v>*   [Industries open statewide](https://covid19.ca.gov/industry-guidance/)\n*   Dine-in restaurants (outdoors only)\n*   Wineries and tasting rooms (outdoors only)\n*   Family entertainment centers (outdoors only)\n*   Zoos and museums (outdoors only)\n*   Cardrooms (outdoors only)\n*   Hair salons and barbershops\n*   Casinos\n*   Gyms and fitness centers\n*   Hotels (for tourism and individual travel)\n*   Campgrounds and outdoor recreation\n*   Personal care services, like nail salons, body waxing and tattoo parlors\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>You should [get tested](https://covid19.ca.gov/testing-and-treatment/). Contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing, and [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) yourself while waiting for your test results.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C150" t="str">
-        <v>https://covid19.ca.gov/roadmap-counties/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D150" t="str">
         <v xml:space="preserve"> </v>
@@ -4282,13 +4282,13 @@
     </row>
     <row r="151">
       <c r="A151" t="str">
-        <v>For counties on Monitoring List for 3 consecutive days</v>
+        <v>How do I become a contact tracer?</v>
       </c>
       <c r="B151" t="str">
-        <v>*   [Industries open statewide](https://covid19.ca.gov/industry-guidance/)\n*   Casinos\n*   Hotels (for tourism and individual travel)\n*   Campgrounds and outdoor recreation\n\nThe following industries must close indoor operations, but they may be modified to operate outside or by pick-up:\n\n*   Dine-in restaurants\n*   Wineries and tasting rooms\n*   Movie theaters \n*   Family entertainment centers (for example: bowling alleys, miniature golf, batting cages and arcades)\n*   Zoos and museums\n*   Cardrooms\n*   Hair salons and barbershops\n*   Gyms and fitness centers\n*   Personal care services, like nail salons, body waxing and tattoo parlors\n*   Places of worship and cultural ceremonies, like weddings and funerals\n*   Offices for non-critical infrastructure sectors\n*   Shopping malls \n\nNOTE: Imperial County is open to the essential workforce only (Stage One). Alameda County does not have an attestation and can only have open those industries which are open statewide.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>The initial phase of California Connected, the state’s contact tracing program, will utilize existing resources and redirect state employees to begin contact tracing efforts. Offers of additional support from the private sector and qualified members of the public are appreciated, but contact tracers from outside state government may not be needed until a future phase. Thank you for wanting to share your expertise and resources with your fellow Californians.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C151" t="str">
-        <v>https://covid19.ca.gov/roadmap-counties/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D151" t="str">
         <v xml:space="preserve"> </v>
@@ -4308,10 +4308,10 @@
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>For counties without attestations</v>
+        <v>County Monitoring List</v>
       </c>
       <c r="B152" t="str">
-        <v>*   [Industries open statewide](https://covid19.ca.gov/industry-guidance/)\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>*   Alameda\n*   Butte (on the list less than 3 days)\n*   Colusa\n*   Contra Costa\n*   Fresno\n*   Glenn\n*   Imperial\n*   Kern (on the list less than 3 days)\n*   Kings\n*   Los Angeles\n*   Madera\n*   Marin\n*   Merced\n*   Monterey\n*   Napa\n*   Orange\n*   Placer\n*   Riverside\n*   Sacramento\n*   San Benito\n*   San Bernardino\n*   San Diego\n*   San Francisco\n*   San Joaquin\n*   San Luis Obispo\n*   Santa Barbara\n*   Santa Clara\n*   Solano\n*   Sonoma\n*   Stanislaus\n*   Sutter\n*   Tulare\n*   Ventura\n*   Yolo\n*   Yuba\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
       </c>
       <c r="C152" t="str">
         <v>https://covid19.ca.gov/roadmap-counties/</v>
@@ -4334,13 +4334,13 @@
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v>Northern California</v>
+        <v>For attested counties not on Monitoring List</v>
       </c>
       <c r="B153" t="str">
-        <v>*   Alturas (Modoc County)\n*   American Canyon (Napa County)\n*   Antioch (Contra Costa County)\n*   Atascadero (San Luis Obispo County)\n*   Bear Valley (Alpine County)\n*   Bieber (Lassen County)\n*   Bishop (Inyo County)\n*   Calistoga (Napa County)\n*   Calpine (Sierra County)\n*   Cedarville (Modoc County)\n*   Ceres (Sanislaus County)\n*   Chowchilla (Madera County)\n*   Clearlake (Lake County)\n*   Coleville (Mono County)\n*   Corcoran (King County)\n*   Corona (King County)\n*   Crescent City (Del Norte County)\n*   Daly City (San Mateo County)\n*   Dinuba (Tulare County)\n*   Downieville (Sierra County)\n*   Doyle (Lassen County)\n*   East Palo Alto (San Mateo County)\n*   Elk Grove (Sacramento County)\n*   Exeter (Tulare County)\n*   Farmersville (Tulare County)\n*   French Camp (San Joaquin County)\n*   Fresno (Fresno County)\n*   Gridley (Butte County)\n*   Half Moon Bay (San Mateo County)\n*   Hanford (King County)\n*   Hayfork (Trinity County)\n*   Herlong (Lassen County)\n*   Jackson (Amador County)\n*   Kerman (Fresno County)\n*   Lakeport (Lake County)\n*   Lemoore (King County)\n*   Lewiston (Trinity County)\n*   Livingston (Merced County)\n*   Lone Pine (Inyo County)\n*   Loyalton (Sierra County)\n*   Magalia (Butte County)\n*   Mammoth Lakes (Mono County)\n*   Markleeville (Alpine County)\n*   Merced (Merced County)\n*   Middletown (Lake County)\n*   Napa (Napa County)\n*   North San Juan (Nevada County)\n*   Oakland (Alameda County)\n*   Placerville (El Dorado County)\n*   Portarville (Tulare County)\n*   Redding (Shasta County)\n*   Redwood City (San Mateo County)\n*   Reedley (Fresno County)\n*   Rio Linda (Sacramento County)\n*   Sacramento (Sacramento County)\n*   Salida (Stanislaus County)\n*   San Bruno (San Mateo County)\n*   San Francisco (San Francisco)\n*   San Jose (Santa Clara County)\n*   San Mateo (San Mateo County)\n*   Santa Rosa (Sonoma County)\n*   Selma (Fresno County)\n*   St. Helena (Napa County)\n*   Stockton (San Joaquin County)\n*   Susanville (Lassen County)\n*   Tracy (San Joaquin County)\n*   Tulare (Tulare County)\n*   Turlock (Stanislaus County)\n*   Upper Lake (Lake County)\n*   Vallejo (Solano County)\n*   Visalia (Tulare County)\n*   Weaverville (Trinity County)\n*   Westwood (Lassen County)\n\n*   Woodlake (Tulare County)\n*   Woodland (Yolo County)\n*   Willow Creek (Humboldt County)\n*   Yosemite Valley (Mariposa County)\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>*   [Industries open statewide](https://covid19.ca.gov/industry-guidance/)\n*   Dine-in restaurants (outdoors only)\n*   Wineries and tasting rooms (outdoors only)\n*   Family entertainment centers (outdoors only)\n*   Zoos and museums (outdoors only)\n*   Cardrooms (outdoors only)\n*   Casinos\n*   Gyms and fitness centers\n*   Hotels (for tourism and individual travel)\n*   Campgrounds and outdoor recreation\n*   Personal care services, like nail salons and body waxing\n*   Hair salons and barbershops\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
       </c>
       <c r="C153" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/roadmap-counties/</v>
       </c>
       <c r="D153" t="str">
         <v xml:space="preserve"> </v>
@@ -4360,13 +4360,13 @@
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v>Southern California</v>
+        <v>For counties on Monitoring List for 3 consecutive days</v>
       </c>
       <c r="B154" t="str">
-        <v>*   Alpine (San Diego County) \n*   Anaheim (Orange County)\n*   Apple Valley (San Bernardino County)\n*   Bakersfield (Kern County)\n*   Banning (Riverside County)\n*   Barstow (San Bernardino County)\n*   Beaumont (Riverside County)\n*   Bell (Los Angeles County)\n*   Blythe (Riverside County)\n*   Calexico (Imperial County)\n*   Cochella (Riverside County)\n*   Compton (Los Angeles County)\n*   Costa Mesa (Orange County)\n*   Delano (Kern County)\n*   Desert Hot Springs (Riverside County)\n*   El Centro (Imperial County)\n*   Fallbrook (San Diego)\n*   Fontana (San Bernardino County)\n*   Fullerton (Orange County)\n*   Gardena (Los Angeles County)\n*   Hemet (Riverside County)\n*   Hesperia (San Bernardino County)\n*   Indio (Riverside County)\n*   La Habra (Orange County)\n*   Lake Elsinore (Riverside County)\n*   Lamont (Kern County)\n*   Lancaster (Los Angeles County)\n*   Lemon Grove (San Diego County)\n*   Los Angeles (Los Angeles County)\n*   McFarland (Kern County)\n*   Oceanside (San Diego)\n*   Ontario (San Bernardino County)\n*   Palmdale (Los Angeles County)\n*   Paramount (Los Angeles County)\n*   Pasadena (Los Angeles County)\n*   Perris (Riverside County)\n*   Phelan (San Bernardino County)\n*   Pico Rivera (Los Angeles County)\n*   Pomona (Los Angeles County)\n*   Port Hueneme (Ventura County)\n*   Riverside (Riverside County)\n*   Rosamond (Kern County)\n*   San Jucinta (Riverside County)\n*   San Juan Capistrano (Orange County)\n*   Santa Maria (Santa Barbara County)\n*   Santa Paula (Ventura County)\n*   Shafter (Kern County)\n*   Valley Center (San Diego County)\n*   Victorville (San Bernardino County)\n*   Wasco (Kern County) \n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>*   [Industries open statewide](https://covid19.ca.gov/industry-guidance/)\n*   Casinos\n*   Hotels (for tourism and individual travel)\n*   Campgrounds and outdoor recreation\n\nThe following industries must close indoor operations, but they may be modified to operate outside or by pick-up:\n\n*   Dine-in restaurants\n*   Wineries and tasting rooms\n*   Movie theaters \n*   Family entertainment centers (for example: bowling alleys, miniature golf, batting cages and arcades)\n*   Zoos and museums\n*   Cardrooms\n*   Gyms and fitness centers\n*   Personal care services, like nail salons and body waxing\n*   Places of worship and cultural ceremonies, like weddings and funerals\n*   Offices for non-critical infrastructure sectors\n*   Shopping malls \n\nNOTE: Imperial County is open to the essential workforce only (Stage One). Alameda County does not have an attestation and can only have open those industries which are open statewide.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
       </c>
       <c r="C154" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/roadmap-counties/</v>
       </c>
       <c r="D154" t="str">
         <v xml:space="preserve"> </v>
@@ -4386,13 +4386,13 @@
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>How do I get a drive-through test?</v>
+        <v>For counties without attestations</v>
       </c>
       <c r="B155" t="str">
-        <v>There are two steps to this process: screening and testing. First, you will create an account and take the online screener. If your answers from the screener determine you are eligible at this time, you will receive details on how and where to get tested. Once tested, you’ll be informed via email or phone when your COVID-19 test results are available.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>*   [Industries open statewide](https://covid19.ca.gov/industry-guidance/)\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
       </c>
       <c r="C155" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/roadmap-counties/</v>
       </c>
       <c r="D155" t="str">
         <v xml:space="preserve"> </v>
@@ -4412,10 +4412,10 @@
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v>Why am I asked to create an account for drive-through testing using Verily’s Project Baseline?</v>
+        <v>Northern California</v>
       </c>
       <c r="B156" t="str">
-        <v>For the Baseline COVID-19 Program to work, Verily needs a way to authenticate users to appropriately protect their information. Verily turned to Google for this service because Google Account provides best-in-class authentication. We ask that you link to an existing Google Account or create a new Google Account (which can be done with any email address). This lets Verily authenticate your account, and securely and privately contact you during the screening and testing process. All the data provided by Baseline COVID-19 Program users for screening is stored separately and not directly linked to a user’s Google Account.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>*   Alturas (Modoc County)\n*   American Canyon (Napa County)\n*   Antioch (Contra Costa County)\n*   Atascadero (San Luis Obispo County)\n*   Bear Valley (Alpine County)\n*   Bieber (Lassen County)\n*   Bishop (Inyo County)\n*   Calistoga (Napa County)\n*   Calpine (Sierra County)\n*   Cedarville (Modoc County)\n*   Ceres (Sanislaus County)\n*   Chowchilla (Madera County)\n*   Clearlake (Lake County)\n*   Coleville (Mono County)\n*   Corcoran (King County)\n*   Corona (King County)\n*   Crescent City (Del Norte County)\n*   Daly City (San Mateo County)\n*   Dinuba (Tulare County)\n*   Downieville (Sierra County)\n*   Doyle (Lassen County)\n*   East Palo Alto (San Mateo County)\n*   Elk Grove (Sacramento County)\n*   Exeter (Tulare County)\n*   Farmersville (Tulare County)\n*   French Camp (San Joaquin County)\n*   Fresno (Fresno County)\n*   Gridley (Butte County)\n*   Half Moon Bay (San Mateo County)\n*   Hanford (King County)\n*   Hayfork (Trinity County)\n*   Herlong (Lassen County)\n*   Jackson (Amador County)\n*   Kerman (Fresno County)\n*   Lakeport (Lake County)\n*   Lemoore (King County)\n*   Lewiston (Trinity County)\n*   Livingston (Merced County)\n*   Lone Pine (Inyo County)\n*   Loyalton (Sierra County)\n*   Magalia (Butte County)\n*   Mammoth Lakes (Mono County)\n*   Markleeville (Alpine County)\n*   Mendota (Fresno County)\n*   Merced (Merced County)\n*   Middletown (Lake County)\n*   Napa (Napa County)\n*   North San Juan (Nevada County)\n*   Oakland (Alameda County)\n*   Placerville (El Dorado County)\n*   Porterville (Tulare County)\n*   Redding (Shasta County)\n*   Redwood City (San Mateo County)\n*   Reedley (Fresno County)\n*   Rio Linda (Sacramento County)\n*   Sacramento (Sacramento County)\n*   Salida (Stanislaus County)\n*   San Bruno (San Mateo County)\n*   San Francisco (San Francisco)\n*   San Jose (Santa Clara County)\n*   San Mateo (San Mateo County)\n*   Santa Rosa (Sonoma County)\n*   Selma (Fresno County)\n*   St. Helena (Napa County)\n*   Stockton (San Joaquin County)\n*   Susanville (Lassen County)\n*   Tracy (San Joaquin County)\n*   Tulare (Tulare County)\n*   Turlock (Stanislaus County)\n*   Upper Lake (Lake County)\n*   Vallejo (Solano County)\n*   Visalia (Tulare County)\n*   Willow Creek (Humboldt County)\n*   Weaverville (Trinity County)\n*   Westwood (Lassen County)\n\n*   Woodlake (Tulare County)\n*   Woodland (Yolo County)\n*   Yosemite Valley (Mariposa County)\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C156" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4438,10 +4438,10 @@
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>Do I need emergency treatment?</v>
+        <v>Southern California</v>
       </c>
       <c r="B157" t="str">
-        <v>If you develop any of these warning signs for COVID-19, get emergency medical attention immediately:\n\n*   Trouble breathing\n*   Persistent pain or pressure in the chest\n*   New confusion \n*   Inability to awake or stay awake\n*   Bluish lips or face\n\nThere are other, less-common symptoms. Please call your medical provider if you have any symptoms that are severe or concerning to you.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call 911, tell the operator you have coronavirus symptoms so ambulance workers can be ready to treat you safely.\n\nIf you’re not sure if this applies to you, you can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor through [telehealth](https://covid19.ca.gov/telehealth/).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>*   Alpine (San Diego County) \n*   Anaheim (Orange County)\n*   Apple Valley (San Bernardino County)\n*   Bakersfield (Kern County)\n*   Banning (Riverside County)\n*   Barstow (San Bernardino County)\n*   Beaumont (Riverside County)\n*   Bell (Los Angeles County)\n*   Blythe (Riverside County)\n*   Calexico (Imperial County)\n*   Coachella (Riverside County)\n*   Compton (Los Angeles County)\n*   Costa Mesa (Orange County)\n*   Delano (Kern County)\n*   Desert Hot Springs (Riverside County)\n*   El Centro (Imperial County)\n*   Fallbrook (San Diego)\n*   Fontana (San Bernardino County)\n*   Fullerton (Orange County)\n*   Gardena (Los Angeles County)\n*   Hemet (Riverside County)\n*   Hesperia (San Bernardino County)\n*   Indio (Riverside County)\n*   La Habra (Orange County)\n*   Lake Elsinore (Riverside County)\n*   Lamont (Kern County)\n*   Lancaster (Los Angeles County)\n*   Lemon Grove (San Diego County)\n*   Los Angeles (Los Angeles County)\n*   McFarland (Kern County)\n*   Oceanside (San Diego)\n*   Ontario (San Bernardino County)\n*   Palmdale (Los Angeles County)\n*   Paramount (Los Angeles County)\n*   Pasadena (Los Angeles County)\n*   Perris (Riverside County)\n*   Phelan (San Bernardino County)\n*   Pico Rivera (Los Angeles County)\n*   Pomona (Los Angeles County)\n*   Port Hueneme (Ventura County)\n*   Riverside (Riverside County)\n*   Rosamond (Kern County)\n*   San Jucinta (Riverside County)\n*   San Juan Capistrano (Orange County)\n*   Santa Maria (Santa Barbara County)\n*   Santa Paula (Ventura County)\n*   Shafter (Kern County)\n*   Valley Center (San Diego County)\n*   Victorville (San Bernardino County)\n*   Wasco (Kern County) \n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C157" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4464,10 +4464,10 @@
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>I have mild COVID-19 symptoms. How long do I have to isolate at home?</v>
+        <v>How do I get a drive-through test?</v>
       </c>
       <c r="B158" t="str">
-        <v>Follow the Centers for Disease Control and Prevention (CDC) guidance on [ending self-isolation](https://www.cdc.gov/coronavirus/2019-ncov/hcp/disposition-in-home-patients.html).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>There are two steps to this process: screening and testing. First, you will create an account and take the online screener. If your answers from the screener determine you are eligible at this time, you will receive details on how and where to get tested. Once tested, you’ll be informed via email or phone when your COVID-19 test results are available.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C158" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4490,10 +4490,10 @@
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>When can I be around other people after I had or likely had COVID-19?</v>
+        <v>Why am I asked to create an account for drive-through testing using Verily’s Project Baseline?</v>
       </c>
       <c r="B159" t="str">
-        <v>You can be with others after:\n\n*   3 days with no fever **and**\n*   Respiratory symptoms have improved (e.g. cough, shortness of breath) **and**\n*   10 days since symptoms first appeared\n\n[CDPH](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Expanding-Access-to-Testing-Updated-Interim-Guidance-on-Prioritization-for-COVID-19-Laboratory-Testing-0501.aspx) and [CDC](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/end-home-isolation.html) have detailed recommendations for quarantine/isolation, if you are sick with COVID-19 or tested positive for coronavirus.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>For the Baseline COVID-19 Program to work, Verily needs a way to authenticate users to appropriately protect their information. Verily turned to Google for this service because Google Account provides best-in-class authentication. We ask that you link to an existing Google Account or create a new Google Account (which can be done with any email address). This lets Verily authenticate your account, and securely and privately contact you during the screening and testing process. All the data provided by Baseline COVID-19 Program users for screening is stored separately and not directly linked to a user’s Google Account.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C159" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4516,10 +4516,10 @@
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>How can I find a coronavirus testing location near me?</v>
+        <v>Do I need emergency treatment?</v>
       </c>
       <c r="B160" t="str">
-        <v>Find a testing location\n-----------------------\n\n&gt; [See the map](https://arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401)\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>If you develop any of these warning signs for COVID-19, get emergency medical attention immediately:\n\n*   Trouble breathing\n*   Persistent pain or pressure in the chest\n*   New confusion \n*   Inability to awake or stay awake\n*   Bluish lips or face\n\nThere are other, less-common symptoms. Please call your medical provider if you have any symptoms that are severe or concerning to you.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call 911, tell the operator you have coronavirus symptoms so ambulance workers can be ready to treat you safely.\n\nIf you’re not sure if this applies to you, you can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor through [telehealth](https://covid19.ca.gov/telehealth/).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C160" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4542,10 +4542,10 @@
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>What is an antibody test? Where can I get an antibody test?</v>
+        <v>I have mild COVID-19 symptoms. How long do I have to isolate at home?</v>
       </c>
       <c r="B161" t="str">
-        <v>[Antibody tests](https://www.cdc.gov/coronavirus/2019-ncov/testing/serology-overview.html) detect past infections (but not current infections). They are used to detect past COVID-19 infections in an individual and can be used to determine if you are a good candidate to [donate blood plasma](https://covid19.ca.gov/plasma). It can take 1-3 weeks after infection for your body to make antibodies. \n\nYou can find locations for both viral and antibody [tests](https://www.arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401) on [California’s testing map](https://www.arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>Follow the Centers for Disease Control and Prevention (CDC) guidance on [ending self-isolation](https://www.cdc.gov/coronavirus/2019-ncov/hcp/disposition-in-home-patients.html).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C161" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4568,13 +4568,13 @@
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>What are the pay and benefits for California Health Corps professionals?</v>
+        <v>When can I be around other people after I had or likely had COVID-19?</v>
       </c>
       <c r="B162" t="str">
-        <v>Salary rates for most of the health care professionals being hired for this emergency are listed in the [CalHR Pay Scales](https://www.calhr.ca.gov/Pay%20Scales%20Library/PS_Sec_05.pdf) (pages 5.12 and 5.13). In addition, CalHR has established pay rates for medical roles that don’t have a corresponding regular classification and pay schedule, such as paramedics and EMTs. CalHR will determine specific salary and benefits after conducting a review of each application.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>You can be with others after:\n\n*   3 days with no fever **and**\n*   Respiratory symptoms have improved (e.g. cough, shortness of breath) **and**\n*   10 days since symptoms first appeared\n\n[CDPH](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Expanding-Access-to-Testing-Updated-Interim-Guidance-on-Prioritization-for-COVID-19-Laboratory-Testing-0501.aspx) and [CDC](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/end-home-isolation.html) have detailed recommendations for quarantine/isolation, if you are sick with COVID-19 or tested positive for coronavirus.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C162" t="str">
-        <v>https://covid19.ca.gov/healthcorps/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D162" t="str">
         <v xml:space="preserve"> </v>
@@ -4594,13 +4594,13 @@
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>Some healthcare professions are not listed. Are health professionals who are not listed (e.g., Medical Technicians, Lab Technicians, etc.) eligible for the California Health Corps?</v>
+        <v>How can I find a coronavirus testing location near me?</v>
       </c>
       <c r="B163" t="str">
-        <v>California Health Corps are currently only accepting applications for the healthcare professions listed on the website. However, we are constantly re-evaluating our needs during this fluid situation and will open the registration for other professionals, if the need arises.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>Find a testing location\n-----------------------\n\n&gt; [See the map](https://arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401)\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C163" t="str">
-        <v>https://covid19.ca.gov/healthcorps/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D163" t="str">
         <v xml:space="preserve"> </v>
@@ -4620,13 +4620,13 @@
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>When can I expect to hear a response after completing my California Health Corps registration?</v>
+        <v>What is an antibody test? Where can I get an antibody test?</v>
       </c>
       <c r="B164" t="str">
-        <v>Currently we anticipate the process may take up to two weeks, since an incredible number of responses are received and need to prioritize certain parts of the state, where the needs are the greatest. We will begin to contact the volunteers after verification of credentials, and based on current and anticipated needs.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>[Antibody tests](https://www.cdc.gov/coronavirus/2019-ncov/testing/serology-overview.html) detect past infections (but not current infections). They are used to detect past COVID-19 infections in an individual and can be used to determine if you are a good candidate to [donate blood plasma](https://covid19.ca.gov/plasma). It can take 1-3 weeks after infection for your body to make antibodies. \n\nYou can find locations for both viral and antibody [tests](https://www.arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401) on [California’s testing map](https://www.arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C164" t="str">
-        <v>https://covid19.ca.gov/healthcorps/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D164" t="str">
         <v xml:space="preserve"> </v>
@@ -4646,10 +4646,10 @@
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>How do I return to the California Health Corps application after logging out?</v>
+        <v>What are the pay and benefits for California Health Corps professionals?</v>
       </c>
       <c r="B165" t="str">
-        <v>Visit [https://healthcarevolunteers.ca.gov/](https://healthcarevolunteers.ca.gov/) and use the account you created while applying to correct or update any information you want.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>Salary rates for most of the health care professionals being hired for this emergency are listed in the [CalHR Pay Scales](https://www.calhr.ca.gov/Pay%20Scales%20Library/PS_Sec_05.pdf) (pages 5.12 and 5.13). In addition, CalHR has established pay rates for medical roles that don’t have a corresponding regular classification and pay schedule, such as paramedics and EMTs. CalHR will determine specific salary and benefits after conducting a review of each application.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C165" t="str">
         <v>https://covid19.ca.gov/healthcorps/</v>
@@ -4672,10 +4672,10 @@
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>Resources for the California Health Corps participants</v>
+        <v>Some healthcare professions are not listed. Are health professionals who are not listed (e.g., Medical Technicians, Lab Technicians, etc.) eligible for the California Health Corps?</v>
       </c>
       <c r="B166" t="str">
-        <v>*   SNF Orientation: [SNF-Nursing-Staff-Orientation (PDF)](https://covid19.ca.gov/pdf/SNF-Nursing-Staff-Orientation.pdf)\n*   Program FAQ details: [CA-Health-Corps-FAQ (PDF)](https://covid19.ca.gov/pdf/CA-Health-Corps-FAQ.pdf)\n*   How to file a complaint: [How-to-file-a-complaint (PDF)](https://covid19.ca.gov/pdf/How-to-file-a-complaint.pdf)\n*   Direct deposit: [std699-Direct-Deposit (PDF)](https://covid19.ca.gov/pdf/std699-Direct-Deposit.pdf)\n*   Travel expense claim: [Std262-Travel-Expense-Claim (PDF)](https://covid19.ca.gov/pdf/Std262-Travel-Expense-Claim.pdf)\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>California Health Corps are currently only accepting applications for the healthcare professions listed on the website. However, we are constantly re-evaluating our needs during this fluid situation and will open the registration for other professionals, if the need arises.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C166" t="str">
         <v>https://covid19.ca.gov/healthcorps/</v>
@@ -4698,10 +4698,10 @@
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>Can a doctor with out of state Licence or foreign medical graduate without California license work for the California Health Corps?</v>
+        <v>When can I expect to hear a response after completing my California Health Corps registration?</v>
       </c>
       <c r="B167" t="str">
-        <v>To be eligible for COVID-19 emergency medical staffing roles, you must:\n\n*   Have a valid California License for clinical practice (if you are a MD, DO, etc.) \n*   **OR** are a medical resident or nursing student \n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>Currently we anticipate the process may take up to two weeks, since an incredible number of responses are received and need to prioritize certain parts of the state, where the needs are the greatest. We will begin to contact the volunteers after verification of credentials, and based on current and anticipated needs.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C167" t="str">
         <v>https://covid19.ca.gov/healthcorps/</v>
@@ -4724,13 +4724,13 @@
     </row>
     <row r="168">
       <c r="A168" t="str">
-        <v>Agriculture and livestock</v>
+        <v>How do I return to the California Health Corps application after logging out?</v>
       </c>
       <c r="B168" t="str">
-        <v>The [guidance for the agriculture and livestock industry](http://covid19.ca.gov/pdf/guidance-agriculture.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the agriculture and livestock industry](http://covid19.ca.gov/pdf/checklist-agriculture.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Visit [https://healthcarevolunteers.ca.gov/](https://healthcarevolunteers.ca.gov/) and use the account you created while applying to correct or update any information you want.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C168" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/healthcorps/</v>
       </c>
       <c r="D168" t="str">
         <v xml:space="preserve"> </v>
@@ -4750,13 +4750,13 @@
     </row>
     <row r="169">
       <c r="A169" t="str">
-        <v>Auto dealerships</v>
+        <v>Resources for the California Health Corps participants</v>
       </c>
       <c r="B169" t="str">
-        <v>The [guidance for the automobile dealerships and rental operators industry](http://covid19.ca.gov/pdf/guidance-auto-dealerships.pdf) provides guidelines to create a safer environment for workers.  \nReview the guidance, prepare a plan, and post the [checklist for the automobile dealerships and rental operators](http://covid19.ca.gov/pdf/checklist-auto-dealerships.pdf) industry in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>*   SNF Orientation: [SNF-Nursing-Staff-Orientation (PDF)](https://covid19.ca.gov/pdf/SNF-Nursing-Staff-Orientation.pdf)\n*   Program FAQ details: [CA-Health-Corps-FAQ (PDF)](https://covid19.ca.gov/pdf/CA-Health-Corps-FAQ.pdf)\n*   How to file a complaint: [How-to-file-a-complaint (PDF)](https://covid19.ca.gov/pdf/How-to-file-a-complaint.pdf)\n*   Direct deposit: [std699-Direct-Deposit (PDF)](https://covid19.ca.gov/pdf/std699-Direct-Deposit.pdf)\n*   Travel expense claim: [Std262-Travel-Expense-Claim (PDF)](https://covid19.ca.gov/pdf/Std262-Travel-Expense-Claim.pdf)\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C169" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/healthcorps/</v>
       </c>
       <c r="D169" t="str">
         <v xml:space="preserve"> </v>
@@ -4776,13 +4776,13 @@
     </row>
     <row r="170">
       <c r="A170" t="str">
-        <v>Childcare – Updated July 17!</v>
+        <v>Can a doctor with out of state Licence or foreign medical graduate without California license work for the California Health Corps?</v>
       </c>
       <c r="B170" t="str">
-        <v>All childcare facilities can open with necessary modifications. The updated [guidance for childcare industry](https://files.covid19.ca.gov/pdf/guidance-childcare--en.pdf) provides guidelines to minimize the spread of COVID-19 and ensure the safety of children, providers, and families. As programs begin to reopen and other programs transition from emergency childcare for essential workers to enhanced regular operations, all providers must apply new and updated policies and requirements and must update their emergency preparedness plan.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>To be eligible for COVID-19 emergency medical staffing roles, you must:\n\n*   Have a valid California License for clinical practice (if you are a MD, DO, etc.) \n*   **OR** are a medical resident or nursing student \n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C170" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/healthcorps/</v>
       </c>
       <c r="D170" t="str">
         <v xml:space="preserve"> </v>
@@ -4802,10 +4802,10 @@
     </row>
     <row r="171">
       <c r="A171" t="str">
-        <v>Communications infrastructure</v>
+        <v>Agriculture and livestock</v>
       </c>
       <c r="B171" t="str">
-        <v>The [guidance for the communications infrastructure industry](http://covid19.ca.gov/pdf/guidance-communications.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the communications infrastructure industry](http://covid19.ca.gov/pdf/checklist-communications.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the agriculture and livestock industry](http://covid19.ca.gov/pdf/guidance-agriculture.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the agriculture and livestock industry](http://covid19.ca.gov/pdf/checklist-agriculture.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C171" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4828,10 +4828,10 @@
     </row>
     <row r="172">
       <c r="A172" t="str">
-        <v>Construction</v>
+        <v>Auto dealerships</v>
       </c>
       <c r="B172" t="str">
-        <v>This [guidance for the construction industry](http://covid19.ca.gov/pdf/guidance-construction.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the construction industry](http://covid19.ca.gov/pdf/checklist-construction.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the automobile dealerships and rental operators industry](http://covid19.ca.gov/pdf/guidance-auto-dealerships.pdf) provides guidelines to create a safer environment for workers.  \nReview the guidance, prepare a plan, and post the [checklist for the automobile dealerships and rental operators](http://covid19.ca.gov/pdf/checklist-auto-dealerships.pdf) industry in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C172" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4854,10 +4854,10 @@
     </row>
     <row r="173">
       <c r="A173" t="str">
-        <v>Day camps – Updated July 17!</v>
+        <v>Childcare – Updated July 20</v>
       </c>
       <c r="B173" t="str">
-        <v>The updated [guidance for day camps](http://covid19.ca.gov/pdf/guidance-daycamps.pdf) provides guidelines to create a plan for safe re-opening.  Implementation of these guidelines should be tailored for each setting. Implementation requires training and support for staff and adequate consideration of camper and family needs. All decisions about following these recommendations should be made in collaboration with local health officials and other authorities, and should depend on the levels of COVID-19 community transmission and the capacities of the local public health and healthcare systems, among other relevant factors.  \n  \nRecreational team sports are not permitted and will be subject to separate guidance.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>All childcare facilities can open with necessary modifications. The updated [guidance for the childcare industry](https://files.covid19.ca.gov/pdf/guidance-childcare--en.pdf) provides guidelines to minimize the spread of COVID-19 and ensure the safety of children, providers, and families. As programs begin to reopen and other programs transition from emergency childcare for essential workers to enhanced regular operations, all providers must apply new and updated policies and requirements and must update their emergency preparedness plan.\n\nReview the guidance, prepare a plan, and post the [checklist for childcare](https://files.covid19.ca.gov/pdf/checklist-childcare--en.pdf) in your facility to show employees and families that you’ve reduced the risk and are open for operation.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C173" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4880,10 +4880,10 @@
     </row>
     <row r="174">
       <c r="A174" t="str">
-        <v>Delivery services</v>
+        <v>Communications infrastructure</v>
       </c>
       <c r="B174" t="str">
-        <v>The [guidance for the delivery services industry](http://covid19.ca.gov/pdf/guidance-delivery-services.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the delivery services industry](http://covid19.ca.gov/pdf/checklist-delivery-services.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the communications infrastructure industry](http://covid19.ca.gov/pdf/guidance-communications.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the communications infrastructure industry](http://covid19.ca.gov/pdf/checklist-communications.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C174" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4906,10 +4906,10 @@
     </row>
     <row r="175">
       <c r="A175" t="str">
-        <v>Energy and utilities</v>
+        <v>Construction</v>
       </c>
       <c r="B175" t="str">
-        <v>The [guidance for the energy and utilities industry](http://covid19.ca.gov/pdf/guidance-energy.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post  the [checklist for the energy and utilities industry](http://covid19.ca.gov/pdf/checklist-energy.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [guidance for the construction industry](http://covid19.ca.gov/pdf/guidance-construction.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the construction industry](http://covid19.ca.gov/pdf/checklist-construction.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C175" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4932,10 +4932,10 @@
     </row>
     <row r="176">
       <c r="A176" t="str">
-        <v>Family friendly practices for employers</v>
+        <v>Day camps – Updated July 20</v>
       </c>
       <c r="B176" t="str">
-        <v>The [guidance for family friendly practices for employers](http://covid19.ca.gov/pdf/guidance-familyfriendlypracticesemployers.pdf) provides guidelines for family-friendly practices to keep employees safe and be responsive to their needs in order to ensure continued productivity. As workplaces reopen, employees will require both child care supports and workplace flexibility. Work-life balance policies will become even more important and continued investment in family-friendly workplace policies by employers is critical.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The updated [guidance for day camps](http://covid19.ca.gov/pdf/guidance-daycamps.pdf) provides guidelines to create a plan for safe re-opening. Implementation of these guidelines should be tailored for each setting. Implementation requires training and support for staff and adequate consideration of camper and family needs. All decisions about following these recommendations should be made in collaboration with local health officials and other authorities, and should depend on the levels of COVID-19 community transmission and the capacities of the local public health and healthcare systems, among other relevant factors.\n\nReview the guidance, prepare a plan, and post the [checklist for day camps](https://files.covid19.ca.gov/pdf/checklist-daycamps--en.pdf) in your facility to show employees, campers, and families that you’ve reduced the risk and are open for operation.  \n  \nRecreational team sports are not permitted and will be subject to separate guidance.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C176" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4958,10 +4958,10 @@
     </row>
     <row r="177">
       <c r="A177" t="str">
-        <v>Food packing</v>
+        <v>Delivery services</v>
       </c>
       <c r="B177" t="str">
-        <v>The [guidance for facilities that process or pack meat, dairy, or produce](http://covid19.ca.gov/pdf/guidance-food-packing.pdf) provides guidelines to create a safer environment for workers.  \nReview the guidance, prepare a plan, and post the [checklist for facilities that process or pack meat, dairy or produce](http://covid19.ca.gov/pdf/checklist-food-packing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the delivery services industry](http://covid19.ca.gov/pdf/guidance-delivery-services.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the delivery services industry](http://covid19.ca.gov/pdf/checklist-delivery-services.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C177" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4984,10 +4984,10 @@
     </row>
     <row r="178">
       <c r="A178" t="str">
-        <v>Hotels and lodging</v>
+        <v>Energy and utilities</v>
       </c>
       <c r="B178" t="str">
-        <v>This [guidance for the hotels and lodging](http://covid19.ca.gov/pdf/guidance-hotels.pdf) provides guidelines to counties not [approved for variance](https://covid19.ca.gov/roadmap-counties/) create a safer environment for workers and customers.\n\nUnless your county has been approved to move further in the roadmap, hotels should only open for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or providing housing solutions, including measures to protect homeless populations.\n\nSeparate guidance for hotels and lodging services in counties with variance attestation [can be found here](https://covid19.ca.gov/pdf/guidance-hotels-lodging-rentals.pdf).\n\nReview the guidance, prepare a plan, and post the [checklist for hotels and lodging](http://covid19.ca.gov/pdf/checklist-hotels.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the energy and utilities industry](http://covid19.ca.gov/pdf/guidance-energy.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post  the [checklist for the energy and utilities industry](http://covid19.ca.gov/pdf/checklist-energy.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C178" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5010,10 +5010,10 @@
     </row>
     <row r="179">
       <c r="A179" t="str">
-        <v>Life sciences</v>
+        <v>Family friendly practices for employers</v>
       </c>
       <c r="B179" t="str">
-        <v>The [guidance for the life sciences industry](http://covid19.ca.gov/pdf/guidance-life-sciences.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the life sciences industry](http://covid19.ca.gov/pdf/checklist-life-sciences.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for family friendly practices for employers](http://covid19.ca.gov/pdf/guidance-familyfriendlypracticesemployers.pdf) provides guidelines for family-friendly practices to keep employees safe and be responsive to their needs in order to ensure continued productivity. As workplaces reopen, employees will require both child care supports and workplace flexibility. Work-life balance policies will become even more important and continued investment in family-friendly workplace policies by employers is critical.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C179" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5036,10 +5036,10 @@
     </row>
     <row r="180">
       <c r="A180" t="str">
-        <v>Limited services</v>
+        <v>Food packing</v>
       </c>
       <c r="B180" t="str">
-        <v>Limited Services are defined as those which do not generally require close contact. Follow this [guidance for Limited Services](https://covid19.ca.gov/pdf/guidance-limited-services.pdf) to create a safer environment for workers and patrons.\n\nFaith-based counseling can reopen within the following parameters:\n\n1.  Counselling services are permissible in-person where the service cannot reasonably be practiced remotely;\n2.  Counselling services should adopt state guidance on Limited Services, where applicable;\n3.  This designation does not permit gatherings beyond counselling to members of a single household.\n\nReview the guidance, prepare a plan, and post the [checklist for Limited Services](https://covid19.ca.gov/pdf/checklist-limited-services.pdf) in your workplace to show clients and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)&lt;!-- laundromat, dry cleaner, laundry, auto repair, car wash, landscaper, door to door, sales, pet groom, dog walk, entry to private residences, community 2 facilities, residential, janitorial, cleaning services, house keep, house clean, HVAC, appliance repair, electrician, plumbers, mechanical trade, handyperson, handyman, general contractors, lessees, subcontractors --&gt;</v>
+        <v>The [guidance for facilities that process or pack meat, dairy, or produce](http://covid19.ca.gov/pdf/guidance-food-packing.pdf) provides guidelines to create a safer environment for workers.  \nReview the guidance, prepare a plan, and post the [checklist for facilities that process or pack meat, dairy or produce](http://covid19.ca.gov/pdf/checklist-food-packing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C180" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5062,10 +5062,10 @@
     </row>
     <row r="181">
       <c r="A181" t="str">
-        <v>Logistics and warehousing facilities</v>
+        <v>Hotels and lodging</v>
       </c>
       <c r="B181" t="str">
-        <v>The [guidance for businesses operating in the logistics/warehousing industry](http://covid19.ca.gov/pdf/guidance-logistics-warehousing.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post  the [checklist for the logistics/warehousing industry](http://covid19.ca.gov/pdf/checklist-logistics-warehousing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [guidance for the hotels and lodging](http://covid19.ca.gov/pdf/guidance-hotels.pdf) provides guidelines to counties not [approved for variance](https://covid19.ca.gov/roadmap-counties/) create a safer environment for workers and customers.\n\nUnless your county has been approved to move further in the roadmap, hotels should only open for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or providing housing solutions, including measures to protect homeless populations.\n\nSeparate guidance for hotels and lodging services in counties with variance attestation [can be found here](https://covid19.ca.gov/pdf/guidance-hotels-lodging-rentals.pdf).\n\nReview the guidance, prepare a plan, and post the [checklist for hotels and lodging](http://covid19.ca.gov/pdf/checklist-hotels.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C181" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5088,10 +5088,10 @@
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>Manufacturing</v>
+        <v>Life sciences</v>
       </c>
       <c r="B182" t="str">
-        <v>The [guidance for the manufacturing industry](http://covid19.ca.gov/pdf/guidance-manufacturing.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the manufacturing industry](http://covid19.ca.gov/pdf/checklist-manufacturing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the life sciences industry](http://covid19.ca.gov/pdf/guidance-life-sciences.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the life sciences industry](http://covid19.ca.gov/pdf/checklist-life-sciences.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C182" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5114,10 +5114,10 @@
     </row>
     <row r="183">
       <c r="A183" t="str">
-        <v>Mining and logging</v>
+        <v>Limited services</v>
       </c>
       <c r="B183" t="str">
-        <v>The [guidance for the mining and logging industries](http://covid19.ca.gov/pdf/guidance-mining-logging.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the mining and logging industries](http://covid19.ca.gov/pdf/checklist-mining-logging.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Limited Services are defined as those which do not generally require close contact. Follow this [guidance for Limited Services](https://covid19.ca.gov/pdf/guidance-limited-services.pdf) to create a safer environment for workers and patrons.\n\nFaith-based counseling can reopen within the following parameters:\n\n1.  Counselling services are permissible in-person where the service cannot reasonably be practiced remotely;\n2.  Counselling services should adopt state guidance on Limited Services, where applicable;\n3.  This designation does not permit gatherings beyond counselling to members of a single household.\n\nReview the guidance, prepare a plan, and post the [checklist for Limited Services](https://covid19.ca.gov/pdf/checklist-limited-services.pdf) in your workplace to show clients and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)&lt;!-- laundromat, dry cleaner, laundry, auto repair, car wash, landscaper, door to door, sales, pet groom, dog walk, entry to private residences, community 2 facilities, residential, janitorial, cleaning services, house keep, house clean, HVAC, appliance repair, electrician, plumbers, mechanical trade, handyperson, handyman, general contractors, lessees, subcontractors --&gt;</v>
       </c>
       <c r="C183" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5140,10 +5140,10 @@
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>Music, film, and TV production</v>
+        <v>Logistics and warehousing facilities</v>
       </c>
       <c r="B184" t="str">
-        <v>Music, TV and film production may resume in California, recommended no sooner than June 12, 2020 and subject to approval by county public health officers within the jurisdictions of operations following their review of local epidemiological data including cases per 100,000 population, rate of test positivity, and local preparedness to support a health care surge, vulnerable populations, contact tracing and testing.  \n  \nTo reduce the risk of COVID-19 transmission, productions, cast, crew and other industry workers should abide by safety protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should adhere to [Office Workspace guidelines](https://covid19.ca.gov/industry-guidance/#top) published by the California Department of Public Health and the California Department of Industrial Relations, to reduce the risk of COVID-19 transmission.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for businesses operating in the logistics/warehousing industry](http://covid19.ca.gov/pdf/guidance-logistics-warehousing.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post  the [checklist for the logistics/warehousing industry](http://covid19.ca.gov/pdf/checklist-logistics-warehousing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C184" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5166,10 +5166,10 @@
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>Office workspaces</v>
+        <v>Manufacturing</v>
       </c>
       <c r="B185" t="str">
-        <v>Follow this [guidance for office workspaces](http://covid19.ca.gov/pdf/guidance-office-workspaces.pdf) to create a safer environment for workers.\n\nFaith-based office workspaces can reopen within the following parameters:\n\n1.  Faith-based facilities are considered “offices” only for those employed by the organization and where the facility is their regular place of work.\n2.  The employer should implement state guidance relating to offices before reopening the facility for employees.\n3.  This designation does not permit gatherings of non-employees, such as the organization’s congregation.\n\nReview the guidance, prepare a plan, and post the [checklist for office workspaces](http://covid19.ca.gov/pdf/checklist-office-workspaces.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the manufacturing industry](http://covid19.ca.gov/pdf/guidance-manufacturing.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the manufacturing industry](http://covid19.ca.gov/pdf/checklist-manufacturing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C185" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5192,10 +5192,10 @@
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>Outdoor museums</v>
+        <v>Mining and logging</v>
       </c>
       <c r="B186" t="str">
-        <v>Follow this [guidance for outdoor museums](https://covid19.ca.gov/pdf/guidance-outdoor-museums.pdf) to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for outdoor museums](http://covid19.ca.gov/pdf/checklist-outdoor-museums.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the mining and logging industries](http://covid19.ca.gov/pdf/guidance-mining-logging.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the mining and logging industries](http://covid19.ca.gov/pdf/checklist-mining-logging.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C186" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5218,10 +5218,10 @@
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>Places of worship and cultural ceremonies</v>
+        <v>Music, film, and TV production</v>
       </c>
       <c r="B187" t="str">
-        <v>This [guidance for places of worship](http://covid19.ca.gov/pdf/guidance-places-of-worship.pdf) and cultural ceremonies, like weddings and funerals, provides guidelines to create a safer environment for workers and visitors. Guidance last updated July 6, 2020. Review the guidance, prepare a plan, and post the [checklist for places of worship](https://files.covid19.ca.gov/pdf/checklist-places-of-worship.pdf) and cultural ceremonies in your workplace to show workers and visitors that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Music, TV and film production may resume in California, recommended no sooner than June 12, 2020 and subject to approval by county public health officers within the jurisdictions of operations following their review of local epidemiological data including cases per 100,000 population, rate of test positivity, and local preparedness to support a health care surge, vulnerable populations, contact tracing and testing.  \n  \nTo reduce the risk of COVID-19 transmission, productions, cast, crew and other industry workers should abide by safety protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should adhere to [Office Workspace guidelines](https://covid19.ca.gov/industry-guidance/#top) published by the California Department of Public Health and the California Department of Industrial Relations, to reduce the risk of COVID-19 transmission.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C187" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5244,10 +5244,10 @@
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>Ports</v>
+        <v>Office workspaces</v>
       </c>
       <c r="B188" t="str">
-        <v>This [guidance for the port industry](http://covid19.ca.gov/pdf/guidance-ports.pdf) provides guidelines to create a safer environment for workers. Review the guidance, prepare a plan, and post the [checklist for the port industry](http://covid19.ca.gov/pdf/checklist-ports.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for office workspaces](http://covid19.ca.gov/pdf/guidance-office-workspaces.pdf) to create a safer environment for workers.\n\nFaith-based office workspaces can reopen within the following parameters:\n\n1.  Faith-based facilities are considered “offices” only for those employed by the organization and where the facility is their regular place of work.\n2.  The employer should implement state guidance relating to offices before reopening the facility for employees.\n3.  This designation does not permit gatherings of non-employees, such as the organization’s congregation.\n\nReview the guidance, prepare a plan, and post the [checklist for office workspaces](http://covid19.ca.gov/pdf/checklist-office-workspaces.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C188" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5270,10 +5270,10 @@
     </row>
     <row r="189">
       <c r="A189" t="str">
-        <v>Professional sports (without live audiences)</v>
+        <v>Outdoor museums</v>
       </c>
       <c r="B189" t="str">
-        <v>Professional sports in California may resume training and competition without live audiences, recommended no sooner than June 12, 2020 and subject to approval by county public health officers within the jurisdiction of operations following their review of local epidemiological data including cases per 100,000 population, rate of test positivity, and local preparedness to support a health care surge, vulnerable populations, contact tracing and testing.  \n  \nTo reduce the risk of COVID-19 transmission, athletes, coaching staff, medical staff, broadcasting staff and others at sporting facilities or events should abide by COVID-19 protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should adhere to [Office Workspace guidelines](https://covid19.ca.gov/pdf/guidance-office-workspaces.pdf) published by the California Department of Public Health and the California Department of Industrial Relations, to reduce the risk of COVID-19 transmission. Retail staff should adhere to [Retail guidelines](https://covid19.ca.gov/pdf/guidance-retail.pdf) published by the California Department of Public Health and the California Department of Industrial Relations, to reduce the risk of COVID-19 transmission.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for outdoor museums](https://covid19.ca.gov/pdf/guidance-outdoor-museums.pdf) to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for outdoor museums](http://covid19.ca.gov/pdf/checklist-outdoor-museums.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C189" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5296,10 +5296,10 @@
     </row>
     <row r="190">
       <c r="A190" t="str">
-        <v>Public transit and intercity passenger rail</v>
+        <v>Places of worship and cultural ceremonies</v>
       </c>
       <c r="B190" t="str">
-        <v>This [guidance for public transit agencies](http://covid19.ca.gov/pdf/guidance-transit-rail.pdf) provides guidelines to create a safer environment for workers and customers.  \nReview the guidance, prepare a plan, and post the [checklist for public transit agencies](http://covid19.ca.gov/pdf/checklist-transit-rail.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [guidance for places of worship](http://covid19.ca.gov/pdf/guidance-places-of-worship.pdf) and cultural ceremonies, like weddings and funerals, provides guidelines to create a safer environment for workers and visitors. Guidance last updated July 6, 2020. Review the guidance, prepare a plan, and post the [checklist for places of worship](https://files.covid19.ca.gov/pdf/checklist-places-of-worship.pdf) and cultural ceremonies in your workplace to show workers and visitors that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C190" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5322,10 +5322,10 @@
     </row>
     <row r="191">
       <c r="A191" t="str">
-        <v>Real estate transaction</v>
+        <v>Ports</v>
       </c>
       <c r="B191" t="str">
-        <v>This [guidance for businesses operating in the real estate industry](http://covid19.ca.gov/pdf/guidance-real-estate.pdf) provides guidelines to create a safer environment for workers.  \nReview the guidance, prepare a plan, and post the [checklist for the real estate industry](http://covid19.ca.gov/pdf/checklist-real-estate.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [guidance for the port industry](http://covid19.ca.gov/pdf/guidance-ports.pdf) provides guidelines to create a safer environment for workers. Review the guidance, prepare a plan, and post the [checklist for the port industry](http://covid19.ca.gov/pdf/checklist-ports.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C191" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5348,10 +5348,10 @@
     </row>
     <row r="192">
       <c r="A192" t="str">
-        <v>Retail</v>
+        <v>Professional sports (without live audiences)</v>
       </c>
       <c r="B192" t="str">
-        <v>Follow this [guidance for retailers](http://covid19.ca.gov/pdf/guidance-retail.pdf) to create a safer environment for workers and customers.\n\nRetailers and libraries can re-open, along with the manufacturing and logistics sectors that support retail. Drive-in and movie theaters can re-open with additional considerations.\n\nRetail doesn’t include personal services such as beauty salons, but does include the sale of goods such as:\n\n*   Bookstores\n*   Jewelry stores\n*   Toy stores\n*   Clothing and shoe stores\n*   Home and furnishing stores\n*   Sporting goods stores\n*   Florists\n\nRetail stores identified in the [essential workforce list](https://covid19.ca.gov/essential-workforce/) can open for in-store shopping. They include:\n\n*   Retail facilities specializing in medical goods and supplies\n*   Grocery stores, pharmacies, convenience stores, and other retail that sells food or beverage products, and animal/pet food\n*   Fuel centers such as gas stations and truck stops\n*   Hardware and building materials stores, consumer electronics, technology and appliances retail\n\nReview the guidance, prepare a plan, and post the [checklist for retail](http://covid19.ca.gov/pdf/checklist-retail.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Professional sports in California may resume training and competition without live audiences, recommended no sooner than June 12, 2020 and subject to approval by county public health officers within the jurisdiction of operations following their review of local epidemiological data including cases per 100,000 population, rate of test positivity, and local preparedness to support a health care surge, vulnerable populations, contact tracing and testing.  \n  \nTo reduce the risk of COVID-19 transmission, athletes, coaching staff, medical staff, broadcasting staff and others at sporting facilities or events should abide by COVID-19 protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should adhere to [Office Workspace guidelines](https://covid19.ca.gov/pdf/guidance-office-workspaces.pdf) published by the California Department of Public Health and the California Department of Industrial Relations, to reduce the risk of COVID-19 transmission. Retail staff should adhere to [Retail guidelines](https://covid19.ca.gov/pdf/guidance-retail.pdf) published by the California Department of Public Health and the California Department of Industrial Relations, to reduce the risk of COVID-19 transmission.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C192" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5374,10 +5374,10 @@
     </row>
     <row r="193">
       <c r="A193" t="str">
-        <v>Schools – Updated July 17!</v>
+        <v>Public transit and intercity passenger rail</v>
       </c>
       <c r="B193" t="str">
-        <v>This [updated guidance for schools and school-based programs](http://covid19.ca.gov/pdf/guidance-schools.pdf) provides guidelines for in-person learning and distance learning. This guidance will be updated as new data and practices emerge. The guidelines and considerations do not reflect the full scope of issues that school communities will need to address, which range from day-to-day site-based logistics to the social and emotional well-being of students and staff. Further guidance is forthcoming, including on school-based sports and extracurricular activities. All decisions about following this guidance should be made in collaboration with local health officials and other authorities.\n\nSchools have been closed for in-person instruction since mid-March 2020 due to the COVID-19 pandemic. School closures to in-person instruction were part of a broader set of recommendations intended to reduce the spread of COVID-19. For more detailed direction on measures to be taken when a student, teacher, or staff member has symptoms or is diagnosed with COVID-19, please see the [COVID-19 and Reopening Framework for K-12 Schools in California](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Schools%20Reopening%20Recommendations.pdf).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [guidance for public transit agencies](http://covid19.ca.gov/pdf/guidance-transit-rail.pdf) provides guidelines to create a safer environment for workers and customers.  \nReview the guidance, prepare a plan, and post the [checklist for public transit agencies](http://covid19.ca.gov/pdf/checklist-transit-rail.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C193" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5400,10 +5400,10 @@
     </row>
     <row r="194">
       <c r="A194" t="str">
-        <v>Support for working families</v>
+        <v>Real estate transaction</v>
       </c>
       <c r="B194" t="str">
-        <v>The [support for working families](http://files.covid19.ca.gov/pdf/guidance-supportworkingfamilies--en.pdf) guidance provides information to help you locate child care, find assistance to pay for child care, and connect you to additional supports for your family. As stay-at-home orders are lifted for additional industries to promote California’s economic recovery, the need for child care and other supports for working families increases.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [guidance for businesses operating in the real estate industry](http://covid19.ca.gov/pdf/guidance-real-estate.pdf) provides guidelines to create a safer environment for workers.  \nReview the guidance, prepare a plan, and post the [checklist for the real estate industry](http://covid19.ca.gov/pdf/checklist-real-estate.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C194" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5426,10 +5426,10 @@
     </row>
     <row r="195">
       <c r="A195" t="str">
-        <v>Shopping centers</v>
+        <v>Retail</v>
       </c>
       <c r="B195" t="str">
-        <v>Follow this [guidance for shopping centers](https://covid19.ca.gov/pdf/guidance-shopping-centers.pdf) to create a safer environment for workers and customers.  \n  \nInterior stores in shopping malls can do curbside pickup with modifications.  \n  \nReview the guidance, prepare a plan, and post the [checklist for shopping centers](https://covid19.ca.gov/pdf/checklist-shopping-centers.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for retailers](http://covid19.ca.gov/pdf/guidance-retail.pdf) to create a safer environment for workers and customers.\n\nRetailers and libraries can re-open, along with the manufacturing and logistics sectors that support retail. Drive-in and movie theaters can re-open with additional considerations.\n\nRetail doesn’t include personal services such as beauty salons, but does include the sale of goods such as:\n\n*   Bookstores\n*   Jewelry stores\n*   Toy stores\n*   Clothing and shoe stores\n*   Home and furnishing stores\n*   Sporting goods stores\n*   Florists\n\nRetail stores identified in the [essential workforce list](https://covid19.ca.gov/essential-workforce/) can open for in-store shopping. They include:\n\n*   Retail facilities specializing in medical goods and supplies\n*   Grocery stores, pharmacies, convenience stores, and other retail that sells food or beverage products, and animal/pet food\n*   Fuel centers such as gas stations and truck stops\n*   Hardware and building materials stores, consumer electronics, technology and appliances retail\n\nReview the guidance, prepare a plan, and post the [checklist for retail](http://covid19.ca.gov/pdf/checklist-retail.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C195" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5452,10 +5452,10 @@
     </row>
     <row r="196">
       <c r="A196" t="str">
-        <v>Take-out restaurants</v>
+        <v>Schools – Updated July 20</v>
       </c>
       <c r="B196" t="str">
-        <v>Follow this [guidance for restaurants providing take-out, drive-through, and delivery](https://files.covid19.ca.gov/pdf/guidance-takeout-restaurants.pdf) to create a safer environment for workers and patrons. Review the guidance and prepare a plan in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [updated guidance for schools and school-based programs](http://covid19.ca.gov/pdf/guidance-schools.pdf) provides guidelines for in-person learning and distance learning. This guidance will be updated as new data and practices emerge. The guidelines and considerations do not reflect the full scope of issues that school communities will need to address, which range from day-to-day site-based logistics to the social and emotional well-being of students and staff. Further guidance is forthcoming, including on school-based sports and extracurricular activities. All decisions about following this guidance should be made in collaboration with local health officials and other authorities. Review the guidance, prepare a plan, and post the [checklist for schools](https://files.covid19.ca.gov/pdf/checklist-schools--en.pdf) in your facility to show employees, students, and families that you’ve reduced the risk and are open for operation.\n\nSchools have been closed for in-person instruction since mid-March 2020 due to the COVID-19 pandemic. School closures to in-person instruction were part of a broader set of recommendations intended to reduce the spread of COVID-19. For more detailed direction on measures to be taken when a student, teacher, or staff member has symptoms or is diagnosed with COVID-19, please see the [COVID-19 and Reopening Framework for K-12 Schools in California](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Schools%20Reopening%20Recommendations.pdf).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C196" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5478,10 +5478,10 @@
     </row>
     <row r="197">
       <c r="A197" t="str">
-        <v>Dine-in restaurants</v>
+        <v>Support for working families</v>
       </c>
       <c r="B197" t="str">
-        <v>This [guidance for dine-in restaurants](https://covid19.ca.gov/pdf/guidance-dine-in-restaurants.pdf) provides guidelines to create a safer environment for workers and customers.  \nReview the guidance, prepare a plan, and post the [checklist for dine-in restaurants](https://covid19.ca.gov/pdf/checklist-dine-in-restaurants.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [support for working families](http://files.covid19.ca.gov/pdf/guidance-supportworkingfamilies--en.pdf) guidance provides information to help you locate child care, find assistance to pay for child care, and connect you to additional supports for your family. As stay-at-home orders are lifted for additional industries to promote California’s economic recovery, the need for child care and other supports for working families increases.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C197" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5504,10 +5504,10 @@
     </row>
     <row r="198">
       <c r="A198" t="str">
-        <v>Hair salons and barbershops</v>
+        <v>Shopping centers</v>
       </c>
       <c r="B198" t="str">
-        <v>This [guidance for hair salons and barbershops](https://covid19.ca.gov/pdf/guidance-hair-salons.pdf) provides guidelines to create a safer environment for workers and customers. Review the guidance, prepare a plan, and post the [checklist for hair salons](https://files.covid19.ca.gov/pdf/checklist-hair-salons.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for shopping centers](https://covid19.ca.gov/pdf/guidance-shopping-centers.pdf) to create a safer environment for workers and customers.  \n  \nInterior stores in shopping malls can do curbside pickup with modifications.  \n  \nReview the guidance, prepare a plan, and post the [checklist for shopping centers](https://covid19.ca.gov/pdf/checklist-shopping-centers.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C198" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5530,10 +5530,10 @@
     </row>
     <row r="199">
       <c r="A199" t="str">
-        <v>Casinos</v>
+        <v>Take-out restaurants</v>
       </c>
       <c r="B199" t="str">
-        <v>In working with tribal governments, CDPH and DIR have released guidance on how to reopen casinos with reduced risk of transmission. Tribal governments should make determinations on when to reopen based on how they align with the current local public health conditions and the statewide stage of reopening and the Governor respectfully requests that until a surrounding or neighboring local jurisdiction has progressed into Stage 3, tribal casinos remain closed.\n\nFollow this [guidance for casinos](https://covid19.ca.gov/pdf/guidance-casinos.pdf) to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for casinos](https://files.covid19.ca.gov/pdf/checklist-casinos.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for restaurants providing take-out, drive-through, and delivery](https://files.covid19.ca.gov/pdf/guidance-takeout-restaurants.pdf) to create a safer environment for workers and patrons. Review the guidance and prepare a plan in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C199" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5556,10 +5556,10 @@
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>Movie theaters and family entertainment centers</v>
+        <v>Dine-in restaurants</v>
       </c>
       <c r="B200" t="str">
-        <v>Follow this guidance for [movie theaters and family entertainment centers](http://covid19.ca.gov/pdf/guidance-family-entertainment.pdf) to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for movie theaters and family entertainment centers](https://files.covid19.ca.gov/pdf/checklist-family-entertainment.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [guidance for dine-in restaurants](https://covid19.ca.gov/pdf/guidance-dine-in-restaurants.pdf) provides guidelines to create a safer environment for workers and customers.  \nReview the guidance, prepare a plan, and post the [checklist for dine-in restaurants](https://covid19.ca.gov/pdf/checklist-dine-in-restaurants.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C200" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5582,10 +5582,10 @@
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>Restaurants, wineries, and bars</v>
+        <v>Hair salons and barbershops</v>
       </c>
       <c r="B201" t="str">
-        <v>Follow this [guidance for restaurants, wineries, and bars](http://covid19.ca.gov/pdf/guidance-restaurants-bars.pdf) to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for restaurants, wineries, and bars](https://files.covid19.ca.gov/pdf/checklist-restaurants-bars.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [guidance for hair salons and barbershops](https://covid19.ca.gov/pdf/guidance-hair-salons.pdf) provides guidelines to create a safer environment for workers and customers. Review the guidance, prepare a plan, and post the [checklist for hair salons](https://files.covid19.ca.gov/pdf/checklist-hair-salons.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nFor counties that have been on the Monitoring List for 3 consecutive days, find guidance for providing hair services outdoors in the list of [guidance for counties on the Monitoring List](https://covid19.ca.gov/industry-guidance/#guidance-monitor).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C201" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5608,10 +5608,10 @@
     </row>
     <row r="202">
       <c r="A202" t="str">
-        <v>Zoos and museums</v>
+        <v>Casinos</v>
       </c>
       <c r="B202" t="str">
-        <v>Follow this [guidance for zoos, museums](http://covid19.ca.gov/pdf/guidance-zoos-museums.pdf), galleries, and aquariums to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for zoos, museums](https://files.covid19.ca.gov/pdf/checklist-zoos-museums.pdf), galleries, and aquariums in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>In working with tribal governments, CDPH and DIR have released guidance on how to reopen casinos with reduced risk of transmission. Tribal governments should make determinations on when to reopen based on how they align with the current local public health conditions and the statewide stage of reopening and the Governor respectfully requests that until a surrounding or neighboring local jurisdiction has progressed into Stage 3, tribal casinos remain closed.\n\nFollow this [guidance for casinos](https://covid19.ca.gov/pdf/guidance-casinos.pdf) to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for casinos](https://files.covid19.ca.gov/pdf/checklist-casinos.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C202" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5634,10 +5634,10 @@
     </row>
     <row r="203">
       <c r="A203" t="str">
-        <v>Gyms and fitness centers</v>
+        <v>Movie theaters and family entertainment centers</v>
       </c>
       <c r="B203" t="str">
-        <v>Follow this [guidance for gyms and fitness centers](https://files.covid19.ca.gov/pdf/guidance-fitness--en.pdf), including yoga and dance studios, to create a safer environment for workers and patrons. Guidance last updated July 1, 2020. Review the guidance, prepare a plan, and post the [checklist for gyms and fitness centers](https://files.covid19.ca.gov/pdf/checklist-fitness.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.  \n  \nRecreational team sports are not permitted and will be subject to separate guidance.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this guidance for [movie theaters and family entertainment centers](http://covid19.ca.gov/pdf/guidance-family-entertainment.pdf) to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for movie theaters and family entertainment centers](https://files.covid19.ca.gov/pdf/checklist-family-entertainment.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C203" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5660,10 +5660,10 @@
     </row>
     <row r="204">
       <c r="A204" t="str">
-        <v>Hotels (for tourism and individual travel)</v>
+        <v>Restaurants, wineries, and bars</v>
       </c>
       <c r="B204" t="str">
-        <v>Follow this [guidance for hotels and short term rentals](https://covid19.ca.gov/pdf/guidance-hotels-lodging-rentals.pdf) for tourism and individual travel to create a safer environment for workers and patrons.\n\nThis guidance is applicable only within counties with variance attestation. Hotel and lodging services in all other counties should adhere to the guidance limitations provided by [statewide guidance](https://covid19.ca.gov/pdf/guidance-hotels.pdf), where hotels should only open for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or providing housing solutions, including measures to protect homeless populations.\n\nReview the guidance, prepare a plan, and post the [checklist for hotels and lodging](http://covid19.ca.gov/pdf/checklist-hotels.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)&lt;!-- motel, vacation, airbnb, vrbo, rental home --&gt;</v>
+        <v>Follow this [guidance for restaurants, wineries, and bars](http://covid19.ca.gov/pdf/guidance-restaurants-bars.pdf) to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for restaurants, wineries, and bars](https://files.covid19.ca.gov/pdf/checklist-restaurants-bars.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C204" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5686,10 +5686,10 @@
     </row>
     <row r="205">
       <c r="A205" t="str">
-        <v>Cardrooms and racetracks</v>
+        <v>Zoos and museums</v>
       </c>
       <c r="B205" t="str">
-        <v>Follow this [guidance for cardrooms](https://covid19.ca.gov/pdf/guidance-cardrooms-racetracks.pdf), race tracks, and satellite wagering to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for cardrooms](https://files.covid19.ca.gov/pdf/checklist-cardrooms-racetracks.pdf), race tracks, and satellite wagering in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for zoos, museums](http://covid19.ca.gov/pdf/guidance-zoos-museums.pdf), galleries, and aquariums to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for zoos, museums](https://files.covid19.ca.gov/pdf/checklist-zoos-museums.pdf), galleries, and aquariums in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C205" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5712,10 +5712,10 @@
     </row>
     <row r="206">
       <c r="A206" t="str">
-        <v>Campgrounds and outdoor recreation</v>
+        <v>Gyms and fitness centers</v>
       </c>
       <c r="B206" t="str">
-        <v>Follow this [guidance for campgrounds](http://covid19.ca.gov/pdf/guidance-campgrounds.pdf) to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the checklist for campgrounds in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)&lt;!-- park, visitor center, travel, museum, recreation, outdoor recreation, sports, RV, tent, camp, fish, beach, lake, river, event, wedding, hike, walk, bike, exercise, nature, birdwatch, guided, tour, hunt, boat, cabin, bonfire, campsite, amphitheater, sport, court, rental, public, trail, marina, bonfire, campsite,  --&gt;</v>
+        <v>Follow this [guidance for gyms and fitness centers](https://files.covid19.ca.gov/pdf/guidance-fitness--en.pdf), including yoga and dance studios, to create a safer environment for workers and patrons. Guidance last updated July 1, 2020. Review the guidance, prepare a plan, and post the [checklist for gyms and fitness centers](https://files.covid19.ca.gov/pdf/checklist-fitness.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.  \n  \nRecreational team sports are not permitted and will be subject to separate guidance.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C206" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5738,10 +5738,10 @@
     </row>
     <row r="207">
       <c r="A207" t="str">
-        <v>Personal care services</v>
+        <v>Hotels (for tourism and individual travel)</v>
       </c>
       <c r="B207" t="str">
-        <v>Follow this [guidance for personal care services](https://files.covid19.ca.gov/pdf/expanded-personal-services--en.pdf) like nail salons, tattoo parlors, and body waxing to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for personal care services](https://files.covid19.ca.gov/pdf/checklist-expanded-personal-care-services.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for hotels and short term rentals](https://covid19.ca.gov/pdf/guidance-hotels-lodging-rentals.pdf) for tourism and individual travel to create a safer environment for workers and patrons.\n\nThis guidance is applicable only within counties with variance attestation. Hotel and lodging services in all other counties should adhere to the guidance limitations provided by [statewide guidance](https://covid19.ca.gov/pdf/guidance-hotels.pdf), where hotels should only open for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or providing housing solutions, including measures to protect homeless populations.\n\nReview the guidance, prepare a plan, and post the [checklist for hotels and lodging](http://covid19.ca.gov/pdf/checklist-hotels.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)&lt;!-- motel, vacation, airbnb, vrbo, rental home --&gt;</v>
       </c>
       <c r="C207" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5764,10 +5764,10 @@
     </row>
     <row r="208">
       <c r="A208" t="str">
-        <v>Outdoor dining</v>
+        <v>Cardrooms and racetracks</v>
       </c>
       <c r="B208" t="str">
-        <v>Follow this [guidance for restaurants providing outdoor dining, take-out, drive-through, and delivery](https://files.covid19.ca.gov/pdf/guidance-outdoor-restaurants.pdf) to create a safer environment for workers and patrons. Review the guidance and prepare a plan in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for cardrooms](https://covid19.ca.gov/pdf/guidance-cardrooms-racetracks.pdf), race tracks, and satellite wagering to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for cardrooms](https://files.covid19.ca.gov/pdf/checklist-cardrooms-racetracks.pdf), race tracks, and satellite wagering in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C208" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5790,13 +5790,13 @@
     </row>
     <row r="209">
       <c r="A209" t="str">
-        <v>Is there a convalescent blood plasma donation center near me?</v>
+        <v>Campgrounds and outdoor recreation</v>
       </c>
       <c r="B209" t="str">
-        <v>Locate a donation center\n------------------------\n\nFind the blood center near you collecting COVID-19 blood plasma.\n\n[See the plasma donation center lookup](https://covid19.ca.gov/plasma#plasma-lookup)\n\nMore info: [Survivors of COVID-19: Donate your plasma](https://covid19.ca.gov/plasma/)</v>
+        <v>Follow this [guidance for campgrounds](http://covid19.ca.gov/pdf/guidance-campgrounds.pdf) to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the checklist for campgrounds in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)&lt;!-- park, visitor center, travel, museum, recreation, outdoor recreation, sports, RV, tent, camp, fish, beach, lake, river, event, wedding, hike, walk, bike, exercise, nature, birdwatch, guided, tour, hunt, boat, cabin, bonfire, campsite, amphitheater, sport, court, rental, public, trail, marina, bonfire, campsite,  --&gt;</v>
       </c>
       <c r="C209" t="str">
-        <v>https://covid19.ca.gov/plasma/</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D209" t="str">
         <v xml:space="preserve"> </v>
@@ -5816,13 +5816,13 @@
     </row>
     <row r="210">
       <c r="A210" t="str">
-        <v>Where can I apply for unemployment?</v>
+        <v>Personal care services</v>
       </c>
       <c r="B210" t="str">
-        <v>If you lost your job or had your hours reduced, and meet eligibility requirements, you may be eligible to receive Unemployment Insurance (UI) benefits from California’s Employment Development Department (EDD). Check the [guide to applying for unemployment benefits](https://unemployment.edd.ca.gov/guide).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>Follow this [guidance for personal care services](https://files.covid19.ca.gov/pdf/expanded-personal-services--en.pdf) like nail salons, tattoo parlors, and body waxing to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for personal care services](https://files.covid19.ca.gov/pdf/checklist-expanded-personal-care-services.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nFor counties that have been on the Monitoring List for 3 consecutive days, find guidance for providing some personal care services outdoors in the list of [guidance for counties on the Monitoring List](https://covid19.ca.gov/industry-guidance/#guidance-monitor).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C210" t="str">
-        <v>Editorial</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D210" t="str">
         <v xml:space="preserve"> </v>
@@ -5842,13 +5842,13 @@
     </row>
     <row r="211">
       <c r="A211" t="str">
-        <v>Are hotels allowed to open?</v>
+        <v>Outdoor dining</v>
       </c>
       <c r="B211" t="str">
-        <v>[Counties that have received approval from the State](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/County_Variance_Attestation_Form.aspx) may open hotels, lodging and short term rentals for tourism and individual travel as long as they follow [state guidance](https://covid19.ca.gov/pdf/guidance-hotels-lodging-rentals.pdf) for public health and safety. Large meeting venues, banquet halls or convention centers should remain closed. All other counties [should only open hotels and lodging](https://covid19.ca.gov/pdf/guidance-hotels.pdf) for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or housing solutions, including measures to protect homeless populations. &lt;!-- motel, vacation, airbnb, vrbo, rental home --&gt;</v>
+        <v>Follow this [guidance for restaurants providing outdoor dining, take-out, drive-through, and delivery](https://files.covid19.ca.gov/pdf/guidance-outdoor-restaurants.pdf) to create a safer environment for workers and patrons. Review the guidance and prepare a plan in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C211" t="str">
-        <v>Editorial</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D211" t="str">
         <v xml:space="preserve"> </v>
@@ -5868,13 +5868,13 @@
     </row>
     <row r="212">
       <c r="A212" t="str">
-        <v>Can my pet test positive for coronavirus? Can I take my pet to the vet?</v>
+        <v>Outdoor services for hair salons and barbershops</v>
       </c>
       <c r="B212" t="str">
-        <v>While we are still learning about coronavirus, the risk of your pet testing positive for coronavirus is low. Because [there is still a risk](https://www.cdc.gov/coronavirus/2019-ncov/animals/pets-other-animals.html), keep your pets away from other pets and people outside of your household. Do not put face coverings on pets as this could harm your pet.\n\nYou can go to the vet or pet hospital if your pet is sick. Remember to wear a cloth face covering and to distance yourself at least 6 feet from other pets and owners.</v>
+        <v>Follow this [guidance for hair salons and barbershops providing services outdoors](https://files.covid19.ca.gov/pdf/guidance-outdoor-hair-salons--en.pdf) to support an outdoor safe, clean environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for hair salons providing services outdoors](https://files.covid19.ca.gov/pdf/checklist-outdoor-hair-salons--en.pdf) at your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C212" t="str">
-        <v>Editorial</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D212" t="str">
         <v xml:space="preserve"> </v>
@@ -5894,13 +5894,13 @@
     </row>
     <row r="213">
       <c r="A213" t="str">
-        <v>What is Larry David's advice?</v>
+        <v>Outdoor services for personal care services</v>
       </c>
       <c r="B213" t="str">
-        <v>&lt;blockquote class="twitter-tweet"&gt;&lt;p lang="en" dir="ltr"&gt;“You’re hurting old people like me. Well, not me... I’ll never see you.”&lt;br&gt;&lt;br&gt;Larry David wants everyone to stay home to protect older Californians from &lt;a href="https://twitter.com/hashtag/COVID19?src=hash&amp;amp;ref_src=twsrc%5Etfw"&gt;#COVID19&lt;/a&gt;! &lt;br&gt;He does not do these things. &lt;br&gt;Listen to Larry.&lt;a href="https://twitter.com/hashtag/StayHomeSaveLives?src=hash&amp;amp;ref_src=twsrc%5Etfw"&gt;#StayHomeSaveLives&lt;/a&gt;&lt;a href="https://t.co/snYe5v55Rw"&gt;https://t.co/snYe5v55Rw&lt;/a&gt; &lt;a href="https://t.co/C5cKOaAufE"&gt;pic.twitter.com/C5cKOaAufE&lt;/a&gt;&lt;/p&gt;&amp;mdash; Office of the Governor of California (@CAgovernor) &lt;a href="https://twitter.com/CAgovernor/status/1245110728199045120?ref_src=twsrc%5Etfw"&gt;March 31, 2020&lt;/a&gt;&lt;/blockquote&gt; &lt;script async src="https://platform.twitter.com/widgets.js" charset="utf-8"&gt;&lt;/script&gt;</v>
+        <v>Follow this [guidance for personal care services provided outdoors](https://files.covid19.ca.gov/pdf/guidance-outdoor-personal-care--en.pdf) to support an outdoor safe, clean environment for workers and patrons. This guidance applies to services that require touching a client’s face, like facials and waxing. This guidance also applies to esthetic services, skin care, cosmetology, nail services, and massage therapy. Review the guidance, prepare a plan, and post the [checklist for personal care services provided outdoors](https://files.covid19.ca.gov/pdf/checklist-outdoor-personal-care--en.pdf) at your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C213" t="str">
-        <v>Editorial</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D213" t="str">
         <v xml:space="preserve"> </v>
@@ -5920,13 +5920,13 @@
     </row>
     <row r="214">
       <c r="A214" t="str">
-        <v>Can I get my nails done? Can I get a massage? Can I get a facial? Can I get a tattoo?</v>
+        <v>Is there a convalescent blood plasma donation center near me?</v>
       </c>
       <c r="B214" t="str">
-        <v>It depends. All indoor operations of nail salons, tattoo parlors, and massage places have closed in counties on the county monitoring list for 3 consecutive days. [Learn more about which counties are on the list](https://covid19.ca.gov/roadmap-counties/).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) &lt;!-- spa, esthetician, electrolysis, waxing, cosmetology services, electrology, body art --&gt;</v>
+        <v>Locate a donation center\n------------------------\n\nFind the blood center near you collecting COVID-19 blood plasma.\n\n[See the plasma donation center lookup](https://covid19.ca.gov/plasma#plasma-lookup)\n\nMore info: [Survivors of COVID-19: Donate your plasma](https://covid19.ca.gov/plasma/)</v>
       </c>
       <c r="C214" t="str">
-        <v>Editorial</v>
+        <v>https://covid19.ca.gov/plasma/</v>
       </c>
       <c r="D214" t="str">
         <v xml:space="preserve"> </v>
@@ -5946,10 +5946,10 @@
     </row>
     <row r="215">
       <c r="A215" t="str">
-        <v xml:space="preserve">Can I go to the movies? </v>
+        <v>Where can I apply for unemployment?</v>
       </c>
       <c r="B215" t="str">
-        <v xml:space="preserve">Effective July 13, 2020, indoor movie theaters are closed in all counties. Drive-in movie theaters with modifications to support physical distancing may be open.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) </v>
+        <v>If you lost your job or had your hours reduced, and meet eligibility requirements, you may be eligible to receive Unemployment Insurance (UI) benefits from California’s Employment Development Department (EDD). Check the [guide to applying for unemployment benefits](https://unemployment.edd.ca.gov/guide).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C215" t="str">
         <v>Editorial</v>
@@ -5972,10 +5972,10 @@
     </row>
     <row r="216">
       <c r="A216" t="str">
-        <v>Can I go to a restaurant? Can I go to a winery or a brewery?</v>
+        <v>Are hotels allowed to open?</v>
       </c>
       <c r="B216" t="str">
-        <v xml:space="preserve">Indoor operations of all dine-in restaurants are closed in all counties. Restaurants across the state can be open for take out, drive through, delivery, and outdoor dining. \n\nIndoor operations for wineries and tasting rooms are closed in all counties. All bars, brewpubs, breweries, and pubs are closed statewide for both indoor and outdoor operations, unless they offer sit-down, outdoor dine-in meals. Alcohol can only be sold in the same transaction as a meal.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) </v>
+        <v>[Counties that have received approval from the State](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/County_Variance_Attestation_Form.aspx) may open hotels, lodging and short term rentals for tourism and individual travel as long as they follow [state guidance](https://covid19.ca.gov/pdf/guidance-hotels-lodging-rentals.pdf) for public health and safety. Large meeting venues, banquet halls or convention centers should remain closed. All other counties [should only open hotels and lodging](https://covid19.ca.gov/pdf/guidance-hotels.pdf) for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or housing solutions, including measures to protect homeless populations. &lt;!-- motel, vacation, airbnb, vrbo, rental home --&gt;</v>
       </c>
       <c r="C216" t="str">
         <v>Editorial</v>
@@ -5998,10 +5998,10 @@
     </row>
     <row r="217">
       <c r="A217" t="str">
-        <v>Are restaurants allowed to open?</v>
+        <v>Can my pet test positive for coronavirus? Can I take my pet to the vet?</v>
       </c>
       <c r="B217" t="str">
-        <v xml:space="preserve">Restaurants across the state can be open for [take out, drive through, and delivery](https://files.covid19.ca.gov/pdf/guidance-takeout-restaurants.pdf). Indoor operations for dine-in restaurants are closed in all counties. Bars, brewpubs, breweries, and pubs must close both indoor and outdoor operations unless they are offering [sit-down, outdoor dine-in meals](https://files.covid19.ca.gov/pdf/guidance-outdoor-restaurants.pdf). Alcohol can only be sold in the same transaction as a meal.\n\nMore info: [Industry guidance](https://covid19.ca.gov/industry-guidance/) and [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) </v>
+        <v>While we are still learning about coronavirus, the risk of your pet testing positive for coronavirus is low. Because [there is still a risk](https://www.cdc.gov/coronavirus/2019-ncov/animals/pets-other-animals.html), keep your pets away from other pets and people outside of your household. Do not put face coverings on pets as this could harm your pet.\n\nYou can go to the vet or pet hospital if your pet is sick. Remember to wear a cloth face covering and to distance yourself at least 6 feet from other pets and owners.</v>
       </c>
       <c r="C217" t="str">
         <v>Editorial</v>
@@ -6024,10 +6024,10 @@
     </row>
     <row r="218">
       <c r="A218" t="str">
-        <v>Where can I find the list of essential critical infrastructure sectors?</v>
+        <v>What is Larry David's advice?</v>
       </c>
       <c r="B218" t="str">
-        <v xml:space="preserve">Visit [Essential workforce](https://covid19.ca.gov/essential-workforce/) to learn about what workers and sectors are included. </v>
+        <v>&lt;blockquote class="twitter-tweet"&gt;&lt;p lang="en" dir="ltr"&gt;“You’re hurting old people like me. Well, not me... I’ll never see you.”&lt;br&gt;&lt;br&gt;Larry David wants everyone to stay home to protect older Californians from &lt;a href="https://twitter.com/hashtag/COVID19?src=hash&amp;amp;ref_src=twsrc%5Etfw"&gt;#COVID19&lt;/a&gt;! &lt;br&gt;He does not do these things. &lt;br&gt;Listen to Larry.&lt;a href="https://twitter.com/hashtag/StayHomeSaveLives?src=hash&amp;amp;ref_src=twsrc%5Etfw"&gt;#StayHomeSaveLives&lt;/a&gt;&lt;a href="https://t.co/snYe5v55Rw"&gt;https://t.co/snYe5v55Rw&lt;/a&gt; &lt;a href="https://t.co/C5cKOaAufE"&gt;pic.twitter.com/C5cKOaAufE&lt;/a&gt;&lt;/p&gt;&amp;mdash; Office of the Governor of California (@CAgovernor) &lt;a href="https://twitter.com/CAgovernor/status/1245110728199045120?ref_src=twsrc%5Etfw"&gt;March 31, 2020&lt;/a&gt;&lt;/blockquote&gt; &lt;script async src="https://platform.twitter.com/widgets.js" charset="utf-8"&gt;&lt;/script&gt;</v>
       </c>
       <c r="C218" t="str">
         <v>Editorial</v>
@@ -6048,9 +6048,165 @@
         <v>217</v>
       </c>
     </row>
+    <row r="219">
+      <c r="A219" t="str">
+        <v xml:space="preserve">Can I go to the movies? </v>
+      </c>
+      <c r="B219" t="str">
+        <v xml:space="preserve">Effective July 13, 2020, indoor movie theaters are closed in all counties. Drive-in movie theaters with modifications to support physical distancing may be open.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) </v>
+      </c>
+      <c r="C219" t="str">
+        <v>Editorial</v>
+      </c>
+      <c r="D219" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E219" t="str">
+        <v>[]</v>
+      </c>
+      <c r="F219" t="str">
+        <v>false</v>
+      </c>
+      <c r="G219" t="str">
+        <v>[]</v>
+      </c>
+      <c r="H219" t="str">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="str">
+        <v>Can I go to a restaurant? Can I go to a winery or a brewery?</v>
+      </c>
+      <c r="B220" t="str">
+        <v xml:space="preserve">Indoor operations of all dine-in restaurants are closed in all counties. Restaurants across the state can be open for take out, drive through, delivery, and outdoor dining. \n\nIndoor operations for wineries and tasting rooms are closed in all counties. All bars, brewpubs, breweries, and pubs are closed statewide for both indoor and outdoor operations, unless they offer sit-down, outdoor dine-in meals. Alcohol can only be sold in the same transaction as a meal.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) </v>
+      </c>
+      <c r="C220" t="str">
+        <v>Editorial</v>
+      </c>
+      <c r="D220" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E220" t="str">
+        <v>[]</v>
+      </c>
+      <c r="F220" t="str">
+        <v>false</v>
+      </c>
+      <c r="G220" t="str">
+        <v>[]</v>
+      </c>
+      <c r="H220" t="str">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="str">
+        <v>Are restaurants allowed to open?</v>
+      </c>
+      <c r="B221" t="str">
+        <v xml:space="preserve">Restaurants across the state can be open for [take out, drive through, and delivery](https://files.covid19.ca.gov/pdf/guidance-takeout-restaurants.pdf). Indoor operations for dine-in restaurants are closed in all counties. Bars, brewpubs, breweries, and pubs must close both indoor and outdoor operations unless they are offering [sit-down, outdoor dine-in meals](https://files.covid19.ca.gov/pdf/guidance-outdoor-restaurants.pdf). Alcohol can only be sold in the same transaction as a meal.\n\nMore info: [Industry guidance](https://covid19.ca.gov/industry-guidance/) and [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) </v>
+      </c>
+      <c r="C221" t="str">
+        <v>Editorial</v>
+      </c>
+      <c r="D221" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E221" t="str">
+        <v>[]</v>
+      </c>
+      <c r="F221" t="str">
+        <v>false</v>
+      </c>
+      <c r="G221" t="str">
+        <v>[]</v>
+      </c>
+      <c r="H221" t="str">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="str">
+        <v>Where can I find the list of essential critical infrastructure sectors?</v>
+      </c>
+      <c r="B222" t="str">
+        <v xml:space="preserve">Visit [Essential workforce](https://covid19.ca.gov/essential-workforce/) to learn about what workers and sectors are included. </v>
+      </c>
+      <c r="C222" t="str">
+        <v>Editorial</v>
+      </c>
+      <c r="D222" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E222" t="str">
+        <v>[]</v>
+      </c>
+      <c r="F222" t="str">
+        <v>false</v>
+      </c>
+      <c r="G222" t="str">
+        <v>[]</v>
+      </c>
+      <c r="H222" t="str">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="str">
+        <v>Can I get my nails done? Can I get a massage? Can I get a facial?</v>
+      </c>
+      <c r="B223" t="str">
+        <v>It depends. Services like nails, waxing, facials, and massage therapy can be open in counties not on the Monitoring List. For counties on the Monitoring List for 3 consecutive days, some services may be provided outdoors, like nails, waxing, facials, and massage. All indoor operations of nail salons, skin care, waxing, and massage are closed in counties on the Monitoring List for 3 consecutive days. [Learn more about which counties are on the list](https://covid19.ca.gov/roadmap-counties/).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) &lt;!-- spa, esthetician, electrolysis, waxing, cosmetology services, electrology, body art --&gt;</v>
+      </c>
+      <c r="C223" t="str">
+        <v>Editorial</v>
+      </c>
+      <c r="D223" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E223" t="str">
+        <v>[]</v>
+      </c>
+      <c r="F223" t="str">
+        <v>false</v>
+      </c>
+      <c r="G223" t="str">
+        <v>[]</v>
+      </c>
+      <c r="H223" t="str">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="str">
+        <v>Can I get a tattoo or piercing? Can I get electrolysis?</v>
+      </c>
+      <c r="B224" t="str">
+        <v>It depends. Tattoo, piercing, and electrolysis services can be open in counties not on the Monitoring List. All indoor and outdoor services for tattooing, piercing, and electrolysis are closed in counties on the Monitoring List for 3 consecutive days. [Learn more about which counties are on the list](https://covid19.ca.gov/roadmap-counties/).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) &lt;!-- spa, esthetician, electrolysis, waxing, cosmetology services, electrology, body art --&gt;</v>
+      </c>
+      <c r="C224" t="str">
+        <v>Editorial</v>
+      </c>
+      <c r="D224" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E224" t="str">
+        <v>[]</v>
+      </c>
+      <c r="F224" t="str">
+        <v>false</v>
+      </c>
+      <c r="G224" t="str">
+        <v>[]</v>
+      </c>
+      <c r="H224" t="str">
+        <v>223</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H218"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H224"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update quick answer dataset
</commit_message>
<xml_diff>
--- a/qnacrawler/merged.xlsx
+++ b/qnacrawler/merged.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H224"/>
+  <dimension ref="A1:H229"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -463,7 +463,7 @@
         <v>Who are high risk people for COVID-19?</v>
       </c>
       <c r="B4" t="str">
-        <v>### Some people are at higher risk to get very sick from COVID-19, including:\n\n*   people over 65 years old\n*   people with compromised immune systems\n*   Individuals who have serious chronic medical conditions like:\n    *   Heart disease\n    *   Diabetes\n    *   Lung disease\n*   [Smokers](https://www.nejm.org/doi/full/10.1056/NEJMoa2002032)\n\nMore info: [Symptoms and risks](https://covid19.ca.gov/symptoms-and-risks/)</v>
+        <v>#### Some people are at [higher risk](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-at-increased-risk.html) to get very sick from COVID-19, including:\n\nMore info: [Symptoms and risks](https://covid19.ca.gov/symptoms-and-risks/)</v>
       </c>
       <c r="C4" t="str">
         <v>https://covid19.ca.gov/symptoms-and-risks/</v>
@@ -850,10 +850,10 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>I want to express my political views.  How can I make my voice heard without raising public health concerns?</v>
+        <v>Are safety protocols being enforced? How do I report a business that isn’t complying?</v>
       </c>
       <c r="B19" t="str">
-        <v>There are many ways for you to express your political views without holding a physical, in-person gathering.  For example, you may continue to call or write elected officials, write letters to the editor of news publications, display lawn or window signs, or use online and other electronic media (including Zoom rooms, Twitter feeds, Facebook pages, and other digital forums) to express your views.  \n\nAdditionally, as noted above, you may leave your home for any reason as long as you comply with any other applicable public health directives. When you are otherwise out in public, public health directives do not prevent you from engaging in political expression—such as by wearing or carrying a sign.\n\nIf collective action in physical space is important to you, consider whether you and other participants can safely protest from within your cars.  The State Public Health Officer does not consider in-car activities to be gatherings, if participants stay in their cars and otherwise remain apart from individuals who are not part of their households.  Many activists have organized car-based protests (honking horns, flying flags, displaying signs, and so on) to express their political views while complying with State public health directives.  \n\nWhenever you are considering a protest (including an in-car protest), make sure you comply with all other applicable laws, including any local public-health measures that may be more restrictive than statewide directives and any other applicable local laws.\n\nIf you do wish to engage in in-person protest outside of your car with a group of any size, you must follow the guidelines for political protest gatherings below.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>They are being enforced, and you can report it. Report unsafe conditions or businesses that shouldn’t be open to your local Alcohol Beverage Control, Labor Commissioner’s office, or regional Cal/OSHA office, depending on the type of business. To find these local contacts, see Appendix B of the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C19" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -876,10 +876,10 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>Can I engage in political protest gatherings?</v>
+        <v>I want to express my political views.  How can I make my voice heard without raising public health concerns?</v>
       </c>
       <c r="B20" t="str">
-        <v>Yes, although in-person protests present special public health concerns. \n\nEven with adherence to physical distancing, bringing members of different households together to engage in in-person protest carries a higher risk of widespread transmission of COVID-19.  Such gatherings may result in increased rates of infection, hospitalization, and death, especially among more vulnerable populations. In particular, activities like chanting, shouting, singing, and group recitation negate the risk-reduction achieved through 6 feet of physical distancing. For this reason, people engaging in these activities should wear face coverings at all times.\n\nTherefore, it is strongly recommended that those exercising their right to engage in political expression (including, for example, their right to petition the government) should utilize alternative channels, such as the many online and broadcasting platforms available in the digital age, in place of in-person gatherings. \n\nHowever, state public health directives do not prohibit in-person _outdoor_ protests as long as you maintain a physical distance of 6 feet between persons or groups of persons from different households at all times. When you can’t maintain a safe physical distance of 6 feet from people not in your household, you must wear a face covering or mask. Local Health Officers are advised to consider appropriate limitations on outdoor attendance capacities, factoring their jurisdiction’s key COVID-19 health indicators. Failure to maintain adequate physical distancing may result in an order to disperse or other enforcement action. Masks and face coverings are strongly recommended.\n\nIn counties that have been on the [County Monitoring List](https://covid19.ca.gov/roadmap-counties/) for three consecutive days, indoor protests are not currently permitted. State public health directives do not prohibit in-person _indoor_ protests as long as (1) attendance is limited to 25% of the relevant area’s maximum occupancy, as defined by the relevant local permitting authority or other relevant authority, or a maximum of 100 attendees, whichever is lower, (2) physical distancing of 6 feet between persons or groups of persons from different households is maintained at all times, and (3) singing and chanting activities are discontinued. Failure to maintain adequate physical distancing may result in an order to disperse or other enforcement action. Masks and face coverings are required in compliance with CDPH directives.\n\nParticipants must maintain a physical distance of 6 feet from any uniformed peace officers and other public safety personnel present, unless otherwise directed, and follow all other requirements and directives imposed by local health officers and law enforcement, or other applicable authorities.\n\nThis limitation on attendance will be reviewed regularly. This review will assess the impacts of these imposed limits on public health and provide further direction as part of a phased-in restoration of gatherings that implicate the First Amendment.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>There are many ways for you to express your political views without holding a physical, in-person gathering.  For example, you may continue to call or write elected officials, write letters to the editor of news publications, display lawn or window signs, or use online and other electronic media (including Zoom rooms, Twitter feeds, Facebook pages, and other digital forums) to express your views.  \n\nAdditionally, as noted above, you may leave your home for any reason as long as you comply with any other applicable public health directives. When you are otherwise out in public, public health directives do not prevent you from engaging in political expression—such as by wearing or carrying a sign.\n\nIf collective action in physical space is important to you, consider whether you and other participants can safely protest from within your cars.  The State Public Health Officer does not consider in-car activities to be gatherings, if participants stay in their cars and otherwise remain apart from individuals who are not part of their households.  Many activists have organized car-based protests (honking horns, flying flags, displaying signs, and so on) to express their political views while complying with State public health directives.  \n\nWhenever you are considering a protest (including an in-car protest), make sure you comply with all other applicable laws, including any local public-health measures that may be more restrictive than statewide directives and any other applicable local laws.\n\nIf you do wish to engage in in-person protest outside of your car with a group of any size, you must follow the guidelines for political protest gatherings below.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C20" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -902,10 +902,10 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>How do I vote?</v>
+        <v>Can I engage in political protest gatherings?</v>
       </c>
       <c r="B21" t="str">
-        <v>Elections are an essential activity. The Governor has issued [executive orders to ensure elections are safe and accessible](https://www.gov.ca.gov/2020/05/08/governor-newsom-issues-executive-order-to-protect-public-health-by-mailing-every-registered-voter-a-ballot-ahead-of-the-november-general-election/). Vote-by-mail ballots will be sent to all registered voters for the November 3, 2020 General Election. Most counties will provide [three days of early voting](https://www.gov.ca.gov/2020/06/03/governor-newsom-signs-executive-order-on-safe-secure-and-accessible-general-election-in-november/) in-person starting the Saturday before the election.Open ballot drop-box locations will be available between October 6 and November 3, 2020. Existing laws addressing the use of vote-by-mail ballots in California elections remain in effect except where suspended by Executive Order. Find [guidance for the safe administration of elections](https://elections.cdn.sos.ca.gov/ccrov/pdf/2020/july/20154jl.pdf) during COVID-19.\n\n Visit [online voter registration](https://registertovote.ca.gov/) to register to vote or check your voter registration status. \n\nPractice physical distancing and follow other applicable public health directives while engaged in election-related activities. These include collection and drop-off of ballots, and collection of signatures to qualify candidates or measures for the ballot.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes, although in-person protests present special public health concerns. \n\nEven with adherence to physical distancing, bringing members of different households together to engage in in-person protest carries a higher risk of widespread transmission of COVID-19.  Such gatherings may result in increased rates of infection, hospitalization, and death, especially among more vulnerable populations. In particular, activities like chanting, shouting, singing, and group recitation negate the risk-reduction achieved through 6 feet of physical distancing. For this reason, people engaging in these activities should wear face coverings at all times.\n\nTherefore, it is strongly recommended that those exercising their right to engage in political expression (including, for example, their right to petition the government) should utilize alternative channels, such as the many online and broadcasting platforms available in the digital age, in place of in-person gatherings. \n\nHowever, state public health directives do not prohibit in-person _outdoor_ protests as long as you maintain a physical distance of 6 feet between persons or groups of persons from different households at all times. When you can’t maintain a safe physical distance of 6 feet from people not in your household, you must wear a face covering or mask. Local Health Officers are advised to consider appropriate limitations on outdoor attendance capacities, factoring their jurisdiction’s key COVID-19 health indicators. Failure to maintain adequate physical distancing may result in an order to disperse or other enforcement action. Masks and face coverings are strongly recommended.\n\nIn counties that have been on the [County Monitoring List](https://covid19.ca.gov/roadmap-counties/) for three consecutive days, indoor protests are not currently permitted. State public health directives do not prohibit in-person _indoor_ protests as long as (1) attendance is limited to 25% of the relevant area’s maximum occupancy, as defined by the relevant local permitting authority or other relevant authority, or a maximum of 100 attendees, whichever is lower, (2) physical distancing of 6 feet between persons or groups of persons from different households is maintained at all times, and (3) singing and chanting activities are discontinued. Failure to maintain adequate physical distancing may result in an order to disperse or other enforcement action. Masks and face coverings are required in compliance with CDPH directives.\n\nParticipants must maintain a physical distance of 6 feet from any uniformed peace officers and other public safety personnel present, unless otherwise directed, and follow all other requirements and directives imposed by local health officers and law enforcement, or other applicable authorities.\n\nThis limitation on attendance will be reviewed regularly. This review will assess the impacts of these imposed limits on public health and provide further direction as part of a phased-in restoration of gatherings that implicate the First Amendment.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C21" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -928,10 +928,10 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>Can I go to church?</v>
+        <v>How do I vote?</v>
       </c>
       <c r="B22" t="str">
-        <v>Yes. Places of worship such as churches, mosques, temples, and synagogues can open throughout the state, with [modifications for safety (PDF)](https://covid19.ca.gov/pdf/guidance-places-of-worship.pdf). In counties on the [County Monitoring List](https://covid19.ca.gov/roadmap-counties/), indoor services in places of worship must be discontinued but outdoor and online services are permitted.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Elections are an essential activity. The Governor has issued [executive orders to ensure elections are safe and accessible](https://www.gov.ca.gov/2020/05/08/governor-newsom-issues-executive-order-to-protect-public-health-by-mailing-every-registered-voter-a-ballot-ahead-of-the-november-general-election/). Vote-by-mail ballots will be sent to all registered voters for the November 3, 2020 General Election. Most counties will provide [three days of early voting](https://www.gov.ca.gov/2020/06/03/governor-newsom-signs-executive-order-on-safe-secure-and-accessible-general-election-in-november/) in-person starting the Saturday before the election.Open ballot drop-box locations will be available between October 6 and November 3, 2020. Existing laws addressing the use of vote-by-mail ballots in California elections remain in effect except where suspended by Executive Order. Find [guidance for the safe administration of elections](https://elections.cdn.sos.ca.gov/ccrov/pdf/2020/july/20154jl.pdf) during COVID-19.\n\n Visit [online voter registration](https://registertovote.ca.gov/) to register to vote or check your voter registration status. \n\nPractice physical distancing and follow other applicable public health directives while engaged in election-related activities. These include collection and drop-off of ballots, and collection of signatures to qualify candidates or measures for the ballot.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C22" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -954,10 +954,10 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Can I practice my religious faith?</v>
+        <v>Can I go to church?</v>
       </c>
       <c r="B23" t="str">
-        <v>Yes. Practicing your faith is a constitutionally-protected activity and may manifest in many different forms.\n\nAlthough in-person religious gatherings—like other in-person gatherings—have been restricted to prevent the transmission of COVID-19, on May 25, 2020, the State Public Health Officer began to ease restrictions on in-person religious gatherings. In particular, the State Public Health Officer now authorizes County Departments of Public Health to allow collective activities at places of worship, subject to conditions to support a safe, clean environment for employees, interns and trainees, volunteers, scholars, and all other types of workers as well as congregants, worshippers, and visitors.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- church, mosque, synagogue, temple, wedding, funeral, baptism --&gt;</v>
+        <v>Yes. Places of worship such as churches, mosques, temples, and synagogues can open throughout the state, with [modifications for safety (PDF)](https://files.covid19.ca.gov/pdf/guidance-places-of-worship.pdf). In counties on the [County Monitoring List](https://covid19.ca.gov/roadmap-counties/), indoor services in places of worship must be discontinued but outdoor and online services are permitted.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C23" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -980,10 +980,10 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>What conditions must be met to resume religious services and cultural ceremonies at places of worship?</v>
+        <v>Can I practice my religious faith?</v>
       </c>
       <c r="B24" t="str">
-        <v>Information on conditions imposed by the state can be found at [guidance for places of worship (PDF)](https://covid19.ca.gov/pdf/guidance-places-of-worship.pdf). Additional conditions may be imposed by local public health officials. This guidance does not obligate places of worship to resume in-person activity. It is strongly recommended that places of worship continue to facilitate remote services and other alternatives to in-person religious practice for those who are vulnerable to COVID19.\n\nEven with adherence to physical distancing, convening in a congregational setting of multiple households to practice a personal faith carries a higher risk of widespread transmission of COVID-19, and may result in increased rates of infection, hospitalization, and death, especially among more vulnerable populations. In particular, activities like singing and group recitation dramatically increase the risk of COVID-19 transmission. For this reason, singing and chanting activities must be discontinued at indoor services, and congregants engaging in group recitation should wear face coverings at all times.\n\nPlaces of worship must therefore limit _indoor_ attendance to 25% of building capacity or a maximum of 100 attendees, whichever is lower, and singing and chanting activities must be discontinued in indoor services. In counties on the County Monitoring List for three consecutive days, places of worship must discontinue indoor services.\n\nLocal Health Officers are advised to consider appropriate limitations on _outdoor_ attendance capacities, factoring their jurisdiction’s key COVID-19 health indicators. At a minimum, outdoor attendance should be limited naturally through implementation of strict physical distancing measures of a minimum of 6 feet between attendees from different households, in addition to other relevant protocols within this document.\n\nThis limitation will be regularly reviewed by the California Department of Public Health.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes. Practicing your faith is a constitutionally-protected activity and may manifest in many different forms.\n\nAlthough in-person religious gatherings—like other in-person gatherings—have been restricted to prevent the transmission of COVID-19, on May 25, 2020, the State Public Health Officer began to ease restrictions on in-person religious gatherings. In particular, the State Public Health Officer now authorizes County Departments of Public Health to allow collective activities at places of worship, subject to conditions to support a safe, clean environment for employees, interns and trainees, volunteers, scholars, and all other types of workers as well as congregants, worshippers, and visitors.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- church, mosque, synagogue, temple, wedding, funeral, baptism --&gt;</v>
       </c>
       <c r="C24" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1006,10 +1006,10 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>Can children attend group activities (like Sunday school or Hebrew school) at places of worship?</v>
+        <v>What conditions must be met to resume religious services and cultural ceremonies at places of worship?</v>
       </c>
       <c r="B25" t="str">
-        <v>At this time, no. Children should remain in the care of those in their household unit and not interact with children of other parties at all times while visiting facilities. Places of worship must discontinue activities and services for children (for example, shared play areas) where physical distancing of at least 6 feet cannot be maintained.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Information on conditions imposed by the state can be found at [guidance for places of worship (PDF)](https://files.covid19.ca.gov/pdf/guidance-places-of-worship.pdf). Additional conditions may be imposed by local public health officials. This guidance does not obligate places of worship to resume in-person activity. It is strongly recommended that places of worship continue to facilitate remote services and other alternatives to in-person religious practice for those who are vulnerable to COVID19.\n\nEven with adherence to physical distancing, convening in a congregational setting of multiple households to practice a personal faith carries a higher risk of widespread transmission of COVID-19, and may result in increased rates of infection, hospitalization, and death, especially among more vulnerable populations. In particular, activities like singing and group recitation dramatically increase the risk of COVID-19 transmission. For this reason, singing and chanting activities must be discontinued at indoor services, and congregants engaging in group recitation should wear face coverings at all times.\n\nPlaces of worship must therefore limit _indoor_ attendance to 25% of building capacity or a maximum of 100 attendees, whichever is lower, and singing and chanting activities must be discontinued in indoor services. In counties on the County Monitoring List for three consecutive days, places of worship must discontinue indoor services.\n\nLocal Health Officers are advised to consider appropriate limitations on _outdoor_ attendance capacities, factoring their jurisdiction’s key COVID-19 health indicators. At a minimum, outdoor attendance should be limited naturally through implementation of strict physical distancing measures of a minimum of 6 feet between attendees from different households, in addition to other relevant protocols within this document.\n\nThis limitation will be regularly reviewed by the California Department of Public Health.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C25" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1032,10 +1032,10 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>When will these conditions change for places of worship?</v>
+        <v>Can children attend group activities (like Sunday school or Hebrew school) at places of worship?</v>
       </c>
       <c r="B26" t="str">
-        <v>The California Department of Public Health, in consultation with county Departments of Public Health, will regularly review and assess the impacts of these imposed limits on public health and provide further direction as part of a phased-in restoration of activities in places of worship.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>At this time, no. Children should remain in the care of those in their household unit and not interact with children of other parties at all times while visiting facilities. Places of worship must discontinue activities and services for children (for example, shared play areas) where physical distancing of at least 6 feet cannot be maintained.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C26" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1058,10 +1058,10 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>Can I still exercise? Take my kids to the park for fresh air? Take a walk around the block?</v>
+        <v>When will these conditions change for places of worship?</v>
       </c>
       <c r="B27" t="str">
-        <v>It’s okay to go outside to go for a walk, to exercise, and participate in healthy activities as long as you **maintain a safe physical distance of 6 feet and gather only with members of your household.** You can also participate in activities at [outdoor recreational facilities](https://covid19.ca.gov/pdf/guidance-campgrounds.pdf) that are allowed to open. [Parks may be closed](https://covid19.ca.gov/public-recreation/) to help slow the spread of the virus. Check with local officials about park closures in your area. Californians should not travel significant distances for recreation and should stay close to home.\n\nBelow is a list of some outdoor recreational activities.\n\n*   Badminton (singles)\n*   Throwing a baseball/softball\n*   BMX biking\n*   Canoeing (singles)\n*   Crabbing\n*   Cycling\n*   Exploring rock pools\n*   Gardening (not in groups)\n*   Golfing (doubles, only if cart has protective partition)\n*   Hiking (trails/ paths allowing distancing)\n*   Horse riding (singles)\n*   Jogging and running\n*   Kite boarding and kitesurfing\n*   Meditation\n*   Outdoor photography\n*   Picnics (with your household members only)\n*   Quad biking\n*   Rock climbing\n*   Roller skating and rollerblading\n*   Rowing (singles)\n*   Scootering (not in groups)\n*   Skateboarding (not in groups)\n*   Soft martial arts – tai chi, chi kung (not in groups)\n*   Surfing\n*   Tennis and table tennis (singles)\n*   Throwing a football, kicking a soccer ball (not in groups)\n*   Trail running\n*   Trampolining\n*   Tree climbing\n*   Volleyball (singles)\n*   Walk the dog\n*   Wash the car\n*   Watch the sunrise or sunset\n*   Yoga\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>The California Department of Public Health, in consultation with county Departments of Public Health, will regularly review and assess the impacts of these imposed limits on public health and provide further direction as part of a phased-in restoration of activities in places of worship.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C27" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>Can I walk my dog? Take my pet to the vet?</v>
+        <v>Can I still exercise? Take my kids to the park for fresh air? Take a walk around the block?</v>
       </c>
       <c r="B28" t="str">
-        <v>You can walk your dog. You can go to the vet or pet hospital if your pet is sick. Remember to wear a face covering and distance yourself at least 6 feet from other pets and owners.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>It’s okay to go outside to go for a walk, to exercise, and participate in healthy activities as long as you **maintain a safe physical distance of 6 feet and gather only with members of your household.** You can also participate in activities at [outdoor recreational facilities](https://files.covid19.ca.gov/pdf/guidance-campgrounds.pdf) that are allowed to open. [Parks may be closed](https://covid19.ca.gov/public-recreation/) to help slow the spread of the virus. Check with local officials about park closures in your area. Californians should not travel significant distances for recreation and should stay close to home.\n\nBelow is a list of some outdoor recreational activities.\n\n*   Badminton (singles)\n*   Throwing a baseball/softball\n*   BMX biking\n*   Canoeing (singles)\n*   Crabbing\n*   Cycling\n*   Exploring rock pools\n*   Gardening (not in groups)\n*   Golfing (doubles, only if cart has protective partition)\n*   Hiking (trails/ paths allowing distancing)\n*   Horse riding (singles)\n*   Jogging and running\n*   Kite boarding and kitesurfing\n*   Meditation\n*   Outdoor photography\n*   Picnics (with your household members only)\n*   Quad biking\n*   Rock climbing\n*   Roller skating and rollerblading\n*   Rowing (singles)\n*   Scootering (not in groups)\n*   Skateboarding (not in groups)\n*   Soft martial arts – tai chi, chi kung (not in groups)\n*   Surfing\n*   Tennis and table tennis (singles)\n*   Throwing a football, kicking a soccer ball (not in groups)\n*   Trail running\n*   Trampolining\n*   Tree climbing\n*   Volleyball (singles)\n*   Walk the dog\n*   Wash the car\n*   Watch the sunrise or sunset\n*   Yoga\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C28" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1110,10 +1110,10 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>Can I visit State Parks? What outdoor spaces are open?</v>
+        <v>Can I walk my dog? Take my pet to the vet?</v>
       </c>
       <c r="B29" t="str">
-        <v>State Parks, campgrounds, museums, and visitor centers [may continue to be closed](https://www.parks.ca.gov/?page_id=30350) to help slow the spread of the virus. Starting June 12, some counties may open campgrounds and RV parks. Be sure to check [parks in your area before you travel](https://covid19.ca.gov/public-recreation/). Californians should not travel significant distances for pleasure or recreation and should stay close to home. If you do travel, take steps to keep everyone safe like wearing a face covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently.\n\nYou can walk, run, hike and bike in your local neighborhoods as long as they continue to practice physical distancing of 6 feet. This means avoiding crowded trails and parking lots.\n\nFor information on National Parks, please the [National Park Service website](https://www.nps.gov/aboutus/news/public-health-update.htm).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- park, visitor center, travel, museum, RV parks, recreation, outdoor recreation, sports, RV, tent camping, tent camp, fish, beach, lake, river, event, outdoor event, event planning, hike, walk, bike, exercise, nature, bird watching, public →&lt;/p&gt;--&gt;</v>
+        <v>You can walk your dog. You can go to the vet or pet hospital if your pet is sick. Remember to wear a face covering and distance yourself at least 6 feet from other pets and owners.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C29" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1136,10 +1136,10 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>Can I travel?</v>
+        <v>Can I visit State Parks? What outdoor spaces are open?</v>
       </c>
       <c r="B30" t="str">
-        <v>You can travel for urgent matters or if such travel is essential to your permitted work. Even though businesses around the state are opening up, avoid travelling long distances for vacations or pleasure as much as possible. This is to slow the spread of the coronavirus. Do not travel if you are sick, or if someone in your household has had coronavirus in the last two weeks. Do not travel with someone who is sick.\n\nYou should check with the local health department where you are starting from, along your route, and at your planned destination for information. Know that local rules are constantly changing and may change even after you start your trip. [Check for travel updates](https://www.visitcalifornia.com/latest-covid-19-coronavirus) before you leave your home.\n\nBefore travelling away from your community, consider these questions from the [Center for Disease Control (CDC) travel guidance](https://www.cdc.gov/coronavirus/2019-ncov/travelers/travel-in-the-us.html):\n\n*   Is coronavirus spreading where you are traveling?\n*   Are you or those you are traveling with more likely to get very sick from coronavirus?\n*   Will you be able to keep 6 feet of physical distance from others during or after your trip?\n\nIf you do travel, take steps to keep everyone safe like wearing a face covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently.  \n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- wedding, travel, gathering, tourism, funeral, motel, vacation, airbnb, vrbo, rental home --&gt;</v>
+        <v>State Parks, campgrounds, museums, and visitor centers [may continue to be closed](https://www.parks.ca.gov/?page_id=30350) to help slow the spread of the virus. Starting June 12, some counties may open campgrounds and RV parks. Be sure to check [parks in your area before you travel](https://covid19.ca.gov/public-recreation/). Californians should not travel significant distances for pleasure or recreation and should stay close to home. If you do travel, take steps to keep everyone safe like wearing a face covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently.\n\nYou can walk, run, hike and bike in your local neighborhoods as long as they continue to practice physical distancing of 6 feet. This means avoiding crowded trails and parking lots.\n\nFor information on National Parks, please the [National Park Service website](https://www.nps.gov/aboutus/news/public-health-update.htm).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- park, visitor center, travel, museum, RV parks, recreation, outdoor recreation, sports, RV, tent camping, tent camp, fish, beach, lake, river, event, outdoor event, event planning, hike, walk, bike, exercise, nature, bird watching, public →&lt;/p&gt;--&gt;</v>
       </c>
       <c r="C30" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1162,10 +1162,10 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>Can I go to the Department of Motor Vehicles (DMV)?</v>
+        <v>Can I travel?</v>
       </c>
       <c r="B31" t="str">
-        <v>Beginning June 11, [all DMV offices](https://www.dmv.ca.gov/portal/news-and-media/dmv-reopens-remaining-field-offices-to-public/) are open to the public to help with appointments that require an in-person visit. You will be required to wear a mask and must remain 6 feet apart in line. In-person appointments are limited to:\n\n*   Paying registration for a vehicle impounded because of registration-related issues\n*   Reinstating a suspended or revoked driver license\n*   Applying for a reduced-fee or no-fee identification card\n*   Processing commercial driver license transactions\n*   Applying for a disabled person parking placards\n*   Adding an ambulance certificate or firefighter endorsement to a driver license\n*   Verifying a transit training document to drive a transit bus\n*   Processing DMV Express customers for REAL ID transactions, if time and space allows\n*   On June 26, the DMV will begin behind-the-wheel driving tests. The DMV will reschedule all cancelled driving test appointments. New behind-the-wheel driving tests will not be available until all cancelled appointments are completed. \n    *   [For the health and safety of drivers and DMV staff](https://www.dmv.ca.gov/portal/news-and-media/dmv-resumes-behind-the-wheel-drive-tests-with-new-protocols-on-friday/), you must wear a face covering and will have your temperature checked before the test.\n\nDMV services that do not require an in-person office visit can be accessed through the [DMV Virtual Field Office](https://virtual.dmv.ca.gov/), including driver’s license renewals, vehicle registrations, title changes, and more.\n\nDMV has extended deadlines for:\n\n*   Drivers 70 years of age and older with licenses expiring between March 1 through December 31, 2020 are valid for one year from the original expiration date.\n*   Drivers 69 years of age and younger with licenses expiring between March 1 through July 31, 2020 can request a free temporary [extension online](https://www.dmv.ca.gov/portal/dmv-virtual-office/temporary-driver-license-extension/), though one is not needed to drive.\n*   Expiring commercial licenses, endorsements, and certificates are valid through June 30, 2020.\n*   In-person renewals for vehicle registrations that expire between the dates of March 16, 2020, and May 31, 2020.\n*   In-person renewals for those with safe driving records whose last DMV visit was 15 years ago.\n*   Driver license permits expiring between June through August 2020 are extended six months or to a date 24 months from the date of application, whichever is earlier.\n*   Commercial learner’s permits expiring between March and June 2020 are now valid through June 30, 2020.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>You can travel for urgent matters or if such travel is essential to your permitted work. Even though businesses around the state are opening up, avoid travelling long distances for vacations or pleasure as much as possible. This is to slow the spread of the coronavirus. Do not travel if you are sick, or if someone in your household has had coronavirus in the last two weeks. Do not travel with someone who is sick.\n\nYou should check with the local health department where you are starting from, along your route, and at your planned destination for information. Know that local rules are constantly changing and may change even after you start your trip. [Check for travel updates](https://www.visitcalifornia.com/latest-covid-19-coronavirus) before you leave your home.\n\nBefore travelling away from your community, consider these questions from the [Center for Disease Control (CDC) travel guidance](https://www.cdc.gov/coronavirus/2019-ncov/travelers/travel-in-the-us.html):\n\n*   Is coronavirus spreading where you are traveling?\n*   Are you or those you are traveling with more likely to get very sick from coronavirus?\n*   Will you be able to keep 6 feet of physical distance from others during or after your trip?\n\nIf you do travel, take steps to keep everyone safe like wearing a face covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently.  \n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- wedding, travel, gathering, tourism, funeral, motel, vacation, airbnb, vrbo, rental home --&gt;</v>
       </c>
       <c r="C31" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1188,10 +1188,10 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>Can I get my car smog checked?</v>
+        <v>Can I go to the Department of Motor Vehicles (DMV)?</v>
       </c>
       <c r="B32" t="str">
-        <v>It depends. Some smog check locations may be closed. The [Bureau of Automotive Repair](https://www.bar.ca.gov/COVID-19_Impacts_on_BAR_Programs_and_Services.aspx) advises drivers to still pay DMV vehicle registration fees to avoid any late fees. However, you will not receive your new registration or year sticker until the smog information has been received by DMV. Once state and local orders or directives are no longer in effect, you can then obtain the required smog check certificate to complete the DMV vehicle registration process.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Beginning June 11, [all DMV offices](https://www.dmv.ca.gov/portal/news-and-media/dmv-reopens-remaining-field-offices-to-public/) are open to the public to help with appointments that require an in-person visit. You will be required to wear a mask and must remain 6 feet apart in line. In-person appointments are limited to:\n\n*   Paying registration for a vehicle impounded because of registration-related issues\n*   Reinstating a suspended or revoked driver license\n*   Applying for a reduced-fee or no-fee identification card\n*   Processing commercial driver license transactions\n*   Applying for a disabled person parking placards\n*   Adding an ambulance certificate or firefighter endorsement to a driver license\n*   Verifying a transit training document to drive a transit bus\n*   Processing DMV Express customers for REAL ID transactions, if time and space allows\n*   On June 26, the DMV will begin behind-the-wheel driving tests. The DMV will reschedule all cancelled driving test appointments. New behind-the-wheel driving tests will not be available until all cancelled appointments are completed. \n    *   [For the health and safety of drivers and DMV staff](https://www.dmv.ca.gov/portal/news-and-media/dmv-resumes-behind-the-wheel-drive-tests-with-new-protocols-on-friday/), you must wear a face covering and will have your temperature checked before the test.\n\nDMV services that do not require an in-person office visit can be accessed through the [DMV Virtual Field Office](https://virtual.dmv.ca.gov/), including driver’s license renewals, vehicle registrations, title changes, and more.\n\nDMV has extended deadlines for:\n\n*   Drivers 70 years of age and older with licenses expiring between March 1 through December 31, 2020 are valid for one year from the original expiration date.\n*   Drivers 69 years of age and younger with licenses expiring between March 1 through July 31, 2020 can request a free temporary [extension online](https://www.dmv.ca.gov/portal/dmv-virtual-office/temporary-driver-license-extension/), though one is not needed to drive.\n*   Expiring commercial licenses, endorsements, and certificates are valid through June 30, 2020.\n*   In-person renewals for vehicle registrations that expire between the dates of March 16, 2020, and May 31, 2020.\n*   In-person renewals for those with safe driving records whose last DMV visit was 15 years ago.\n*   Driver license permits expiring between June through August 2020 are extended six months or to a date 24 months from the date of application, whichever is earlier.\n*   Commercial learner’s permits expiring between March and June 2020 are now valid through June 30, 2020.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C32" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1214,13 +1214,13 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>Should I wear a face covering or mask to protect against COVID-19?</v>
+        <v>Can I get my car smog checked?</v>
       </c>
       <c r="B33" t="str">
-        <v>Yes. Californians must wear face coverings when in public spaces, especially indoors and other areas where physical distancing is not possible. Face coverings help reduce the spread of COVID-19. \n\nThe California Department of Public Health (CDPH) has released a [Guidance](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Guidance-for-Face-Coverings_06-18-2020.pdf) for the use of face covering.\n\nThe guidance reminds Californians that the best defense against COVID-19 continues to be: \n\n*   Maintain six feet of physical distance from others \n*   Wash hands frequently\n*   Avoid touching eyes, nose and mouth with unwashed hands\n*   Avoid being around people with COVID-19 symptoms\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>It depends. Some smog check locations may be closed. The [Bureau of Automotive Repair](https://www.bar.ca.gov/COVID-19_Impacts_on_BAR_Programs_and_Services.aspx) advises drivers to still pay DMV vehicle registration fees to avoid any late fees. However, you will not receive your new registration or year sticker until the smog information has been received by DMV. Once state and local orders or directives are no longer in effect, you can then obtain the required smog check certificate to complete the DMV vehicle registration process.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C33" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
       </c>
       <c r="D33" t="str">
         <v xml:space="preserve"> </v>
@@ -1240,10 +1240,10 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>How well do face coverings prevent spread of COVID-19?</v>
+        <v>Should I wear a face covering or mask to protect against COVID-19?</v>
       </c>
       <c r="B34" t="str">
-        <v>There is scientific evidence to suggest that use of face coverings by the public during a pandemic could help reduce disease transmission. Their primary role is to reduce the release of infectious particles into the air when someone speaks, coughs, or sneezes, including someone who has COVID-19 but feels well. Face coverings are not a substitute for physical distancing, washing hands, and staying home when ill, but they may be helpful when combined with these primary interventions.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. Californians must wear face coverings when in public spaces, especially indoors and other areas where physical distancing is not possible. Face coverings help reduce the spread of COVID-19. \n\nThe California Department of Public Health (CDPH) has released a [Guidance](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Guidance-for-Face-Coverings_06-18-2020.pdf) for the use of face covering.\n\nThe guidance reminds Californians that the best defense against COVID-19 continues to be: \n\n*   Maintain six feet of physical distance from others \n*   Wash hands frequently\n*   Avoid touching eyes, nose and mouth with unwashed hands\n*   Avoid being around people with COVID-19 symptoms\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C34" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1266,10 +1266,10 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>What is a face covering?</v>
+        <v>How well do face coverings prevent spread of COVID-19?</v>
       </c>
       <c r="B35" t="str">
-        <v>A face covering is [material that covers the nose and mouth](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/diy-cloth-face-coverings.html). It can be secured to the head with ties or straps or simply wrapped around the lower face. It can be made of a variety of materials, such as cotton, silk, or linen. A face covering may be factory-made or sewn by hand, or can be improvised from household items such as scarfs, T-shirts, sweatshirts, or towels.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>There is scientific evidence to suggest that use of face coverings by the public during a pandemic could help reduce disease transmission. Their primary role is to reduce the release of infectious particles into the air when someone speaks, coughs, or sneezes, including someone who has COVID-19 but feels well. Face coverings are not a substitute for physical distancing, washing hands, and staying home when ill, but they may be helpful when combined with these primary interventions.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C35" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1292,10 +1292,10 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>How should I care for a face covering?</v>
+        <v>What is a face covering?</v>
       </c>
       <c r="B36" t="str">
-        <v>It’s a good idea to [wash your face covering](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/diy-cloth-face-coverings.html) frequently, ideally after each use. Have a bag or bin to keep face coverings in until they can be laundered with detergent and hot water and dried on a hot cycle. If you must re-wear your face covering before washing, wash your hands immediately after putting it back on and avoid touching your face. Discard coverings that:\n\n*   No longer cover the nose and mouth\n*   Have stretched out or damaged ties or straps\n*   Cannot stay on the face\n*   Have holes or tears in the fabric\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>A face covering is [material that covers the nose and mouth](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/diy-cloth-face-coverings.html). It can be secured to the head with ties or straps or simply wrapped around the lower face. It can be made of a variety of materials, such as cotton, silk, or linen. A face covering may be factory-made or sewn by hand, or can be improvised from household items such as scarfs, T-shirts, sweatshirts, or towels.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C36" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1318,10 +1318,10 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>What if I don’t have health insurance and I need screening, testing, or treatment for COVID-19?</v>
+        <v>How should I care for a face covering?</v>
       </c>
       <c r="B37" t="str">
-        <v>The cost of medically necessary screening, testing, and treatment for the uninsured is paid for by the [government](https://www.hrsa.gov/CovidUninsuredClaim). You can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor through [telehealth](https://covid19.ca.gov/telehealth/). You can also get free medically necessary [testing](https://covid19.ca.gov/testing-and-treatment/) through [Verily’s Project Baseline](https://www.projectbaseline.com/study/covid-19/eligibility/) or [OptumServe](https://lhi.care/covidtesting).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>It’s a good idea to [wash your face covering](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/diy-cloth-face-coverings.html) frequently, ideally after each use. Have a bag or bin to keep face coverings in until they can be laundered with detergent and hot water and dried on a hot cycle. If you must re-wear your face covering before washing, wash your hands immediately after putting it back on and avoid touching your face. Discard coverings that:\n\n*   No longer cover the nose and mouth\n*   Have stretched out or damaged ties or straps\n*   Cannot stay on the face\n*   Have holes or tears in the fabric\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C37" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1344,10 +1344,10 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>Does my health plan have to cover my COVID-19 test?</v>
+        <v>What if I don’t have health insurance and I need screening, testing, or treatment for COVID-19?</v>
       </c>
       <c r="B38" t="str">
-        <v>Yes, if you’re experiencing COVID-19 symptoms, you think you were exposed to someone who has COVID-19, or the test is otherwise medically necessary for your situation. \n\nIf you have symptoms of COVID-19 or you think you’ve been exposed to someone with COVID-19, under federal law, you can obtain a COVID-19 test anywhere and your health plan must pay for the test. \n\nIf you don’t have symptoms and don’t think you’ve been exposed to someone with COVID-19, but you are an [essential worker](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf) as defined for COVID-19 testing coverage, your health plan must cover your COVID-19 test. However, you must contact your health plan before getting testing. \n\nIf you don’t have symptoms, don’t think you’ve been exposed to someone with COVID-19, and aren’t an [essential worker](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf) as defined for COVID-19 testing coverage, and you think you need a test, please contact your health plan or health care provider for further guidance.\n\nAs a first step, you can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor through [telehealth](https://covid19.ca.gov/telehealth/).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>The cost of medically necessary screening, testing, and treatment for the uninsured is paid for by the [government](https://www.hrsa.gov/CovidUninsuredClaim). You can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor through [telehealth](https://covid19.ca.gov/telehealth/). You can also get free medically necessary [testing](https://covid19.ca.gov/testing-and-treatment/) through [Verily’s Project Baseline](https://www.projectbaseline.com/study/covid-19/eligibility/) or [OptumServe](https://lhi.care/covidtesting).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C38" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1370,10 +1370,10 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>How long will I have to wait to get a test?</v>
+        <v>Does my health plan have to cover my COVID-19 test?</v>
       </c>
       <c r="B39" t="str">
-        <v>Your wait time depends on why you are seeking a test. \n\n**If you have symptoms of COVID-19 or think you were exposed,** under federal law, you can go immediately to any available testing site. Find a testing site on our [Testing page,](https://covid19.ca.gov/testing-and-treatment/#top) or call your health plan so they can direct you to an available testing location. \n\n**If you don’t have symptoms or suspected exposure, and you are an** [**essential worker**](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf)**,** your health plan must offer you a test appointment within 48 hours. The testing site must be within 15 miles or 30 minutes of your residence or workplace. If the health plan can’t find you an available appointment within that time and distance, then you can go to any available testing site and your health plan will pay for the test. \n\n**If you don’t have symptoms or suspected exposure, and you are not an essential worker,** if your provider determines a COVID-19 test is medically necessary for you, your health plan must offer you a test appointment within 96 hours. The testing site must be within 15 miles or 30 minutes of your residence or workplace. If the health plan can’t find you an available appointment within that time and distance, you can go to any available testing site.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes, if you’re experiencing COVID-19 symptoms, you think you were exposed to someone who has COVID-19, or the test is otherwise medically necessary for your situation. \n\nIf you have symptoms of COVID-19 or you think you’ve been exposed to someone with COVID-19, under federal law, you can obtain a COVID-19 test anywhere and your health plan must pay for the test. \n\nIf you don’t have symptoms and don’t think you’ve been exposed to someone with COVID-19, but you are an [essential worker](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf) as defined for COVID-19 testing coverage, your health plan must cover your COVID-19 test. However, you must contact your health plan before getting testing. \n\nIf you don’t have symptoms, don’t think you’ve been exposed to someone with COVID-19, and aren’t an [essential worker](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf) as defined for COVID-19 testing coverage, and you think you need a test, please contact your health plan or health care provider for further guidance.\n\nAs a first step, you can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor through [telehealth](https://covid19.ca.gov/telehealth/).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C39" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1396,10 +1396,10 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>I get my health care coverage through my employer, who has a “self-insured” plan. Do the California Department of Managed Health Care (DMHC) regulations apply to me?</v>
+        <v>How long will I have to wait to get a test?</v>
       </c>
       <c r="B40" t="str">
-        <v>Self-insured plans are regulated by the federal government, rather than the state. If you have symptoms of COVID-19 or you were exposed to someone who you know or suspect has COVID-19, under federal law, your employer’s self-insured plan must cover your test. In all other instances, you should talk to your employer’s self-insured plan to find out whether they will cover COVID-19 testing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Your wait time depends on why you are seeking a test. \n\n**If you have symptoms of COVID-19 or think you were exposed,** under federal law, you can go immediately to any available testing site. Find a testing site on our [Testing page,](https://covid19.ca.gov/testing-and-treatment/#top) or call your health plan so they can direct you to an available testing location. \n\n**If you don’t have symptoms or suspected exposure, and you are an** [**essential worker**](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf)**,** your health plan must offer you a test appointment within 48 hours. The testing site must be within 15 miles or 30 minutes of your residence or workplace. If the health plan can’t find you an available appointment within that time and distance, then you can go to any available testing site and your health plan will pay for the test. \n\n**If you don’t have symptoms or suspected exposure, and you are not an essential worker,** if your provider determines a COVID-19 test is medically necessary for you, your health plan must offer you a test appointment within 96 hours. The testing site must be within 15 miles or 30 minutes of your residence or workplace. If the health plan can’t find you an available appointment within that time and distance, you can go to any available testing site.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C40" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1422,10 +1422,10 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>How does my health plan know if I’m an essential worker?</v>
+        <v>I get my health care coverage through my employer, who has a “self-insured” plan. Do the California Department of Managed Health Care (DMHC) regulations apply to me?</v>
       </c>
       <c r="B41" t="str">
-        <v>Your health plan can ask you questions about why you want a COVID-19 test and about the nature of your work. They can ask these questions to help determine whether a COVID-19 test is medically necessary for you. \n\nHowever, your health plan can’t ask you to provide further documentation or evidence of your work status. For example, your health plan can’t ask you to provide written proof of where you work or the conditions of your workplace.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Self-insured plans are regulated by the federal government, rather than the state. If you have symptoms of COVID-19 or you were exposed to someone who you know or suspect has COVID-19, under federal law, your employer’s self-insured plan must cover your test. In all other instances, you should talk to your employer’s self-insured plan to find out whether they will cover COVID-19 testing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C41" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>I have a concern or complaint about getting care for COVID-19 under my health insurance. What can I do?</v>
+        <v>How does my health plan know if I’m an essential worker?</v>
       </c>
       <c r="B42" t="str">
-        <v>If you are having trouble accessing care, or were inappropriately charged for medically necessary screening, testing, or treatment for COVID-19, follow up directly with your health plan by calling the member phone number listed on your health plan card. If your health plan doesn’t resolve the issue, contact the [California Department of Managed Health Care (DMHC)](http://www.dmhc.ca.gov/?referral=healthhelp.ca.gov) Help Center for assistance at 1-888-466-2219.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Your health plan can ask you questions about why you want a COVID-19 test and about the nature of your work. They can ask these questions to help determine whether a COVID-19 test is medically necessary for you. \n\nHowever, your health plan can’t ask you to provide further documentation or evidence of your work status. For example, your health plan can’t ask you to provide written proof of where you work or the conditions of your workplace.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C42" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1474,10 +1474,10 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>Do Medicare or Medicare Advantage Plans cover coronavirus tests or coronavirus antibody tests?</v>
+        <v>I have a concern or complaint about getting care for COVID-19 under my health insurance. What can I do?</v>
       </c>
       <c r="B43" t="str">
-        <v>Yes. Both [Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) cover [coronavirus tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test) tests, with no out-of-pocket costs. \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>If you are having trouble accessing care, or were inappropriately charged for medically necessary screening, testing, or treatment for COVID-19, follow up directly with your health plan by calling the member phone number listed on your health plan card. If your health plan doesn’t resolve the issue, contact the [California Department of Managed Health Care (DMHC)](http://www.dmhc.ca.gov/?referral=healthhelp.ca.gov) Help Center for assistance at 1-888-466-2219.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C43" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1500,10 +1500,10 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>Can I use telehealth if I am on Medicare?</v>
+        <v>Do Medicare or Medicare Advantage Plans cover coronavirus tests or coronavirus antibody tests?</v>
       </c>
       <c r="B44" t="str">
-        <v>Yes. Medicare has temporarily expanded its coverage of [telehealth services (medical care via phone, video chat, or online portal)](https://www.medicare.gov/coverage/telehealth) to respond to the current Public Health Emergency. You can now use a wide range of communication tools (including smartphone) from home to interact with a range of providers, like doctors, nurse practitioners, clinical psychologists, licensed clinical social workers, physical therapists, occupational therapists, and speech language pathologists. If you have original Medicare, you can get many services without a copayment through [telehealth,](https://covid19.ca.gov/telehealth/) including evaluation and management visits (common office visits), mental health counseling, and preventive health screenings.\n\nIf you have a [Medicare Advantage Plan](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans), you have access to these same benefits. Many plans offer additional [telehealth](https://covid19.ca.gov/telehealth/) benefits and expanded benefits, like meal delivery or medical transport services. Check with your plan about your coverage and costs.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. Both [Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) cover [coronavirus tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test) tests, with no out-of-pocket costs. \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C44" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1526,10 +1526,10 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>I am nervous or scared. What can I do?</v>
+        <v>Can I use telehealth if I am on Medicare?</v>
       </c>
       <c r="B45" t="str">
-        <v>You are not alone. The California Surgeon General released [two playbooks for managing stress](https://covid19.ca.gov/manage-stress-for-health/#top) and tips for care-givers and kids. If you feel like you need to talk to someone and want emotional support see this [list of resources](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/#top).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. Medicare has temporarily expanded its coverage of [telehealth services (medical care via phone, video chat, or online portal)](https://www.medicare.gov/coverage/telehealth) to respond to the current Public Health Emergency. You can now use a wide range of communication tools (including smartphone) from home to interact with a range of providers, like doctors, nurse practitioners, clinical psychologists, licensed clinical social workers, physical therapists, occupational therapists, and speech language pathologists. If you have original Medicare, you can get many services without a copayment through [telehealth,](https://covid19.ca.gov/telehealth/) including evaluation and management visits (common office visits), mental health counseling, and preventive health screenings.\n\nIf you have a [Medicare Advantage Plan](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans), you have access to these same benefits. Many plans offer additional [telehealth](https://covid19.ca.gov/telehealth/) benefits and expanded benefits, like meal delivery or medical transport services. Check with your plan about your coverage and costs.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C45" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1552,10 +1552,10 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>My safety net eligibility (like CalFresh, Medi-Cal) is expiring and I am under the statewide stay home order for COVID-19. Do I need to renew my eligibility now?</v>
+        <v>I am nervous or scared. What can I do?</v>
       </c>
       <c r="B46" t="str">
-        <v>****No, you will not need to renew until August 17, 2020.**** Governor Gavin Newsom issued an [executive order](https://www.gov.ca.gov/wp-content/uploads/2020/06/6.15.20-EO-N-69-20-text.pdf) to ensure that health care, food assistance, and in-home supportive services continue during the COVID-19 outbreak.\n\nThe order waives eligibility re-determinations for 150 days for participants in:\n\n*   Medi-Cal health coverage\n*   CalFresh food assistance\n*   CalWORKs\n*   Cash Assistance for Immigrants\n*   In-Home Supportive Services\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>You are not alone. The California Surgeon General released [two playbooks for managing stress](https://covid19.ca.gov/manage-stress-for-health/#top) and tips for care-givers and kids. If you feel like you need to talk to someone and want emotional support see this [list of resources](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/#top).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C46" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1578,10 +1578,10 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>What if I need to visit a health care provider?</v>
+        <v>My safety net eligibility (like CalFresh, Medi-Cal) is expiring and I am under the statewide stay home order for COVID-19. Do I need to renew my eligibility now?</v>
       </c>
       <c r="B47" t="str">
-        <v>If you have [coronavirus symptoms](https://covid19.ca.gov/symptoms-and-risks/#top), please contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) or use the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) self-checker.\n\nIf you have other illnesses or chronic conditions, use [telehealth](https://covid19.ca.gov/telehealth/) to get care from home.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call 911, tell the 911 operator your exact symptoms so the ambulance provider can be ready to treat you safely.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>****No, you will not need to renew until August 17, 2020.**** Governor Gavin Newsom issued an [executive order](https://www.gov.ca.gov/wp-content/uploads/2020/06/6.15.20-EO-N-69-20-text.pdf) to ensure that health care, food assistance, and in-home supportive services continue during the COVID-19 outbreak.\n\nThe order waives eligibility re-determinations for 150 days for participants in:\n\n*   Medi-Cal health coverage\n*   CalFresh food assistance\n*   CalWORKs\n*   Cash Assistance for Immigrants\n*   In-Home Supportive Services\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C47" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1604,10 +1604,10 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>What about routine, elective, or non-urgent medical or dental appointments?</v>
+        <v>What if I need to visit a health care provider?</v>
       </c>
       <c r="B48" t="str">
-        <v>Preventive care services and non-emergency surgeries, like organ replacements and tumor removals, can take place if hospitals have enough capacity and protective equipment to do so safely. Eye exams, and elective procedures should be cancelled or rescheduled. If possible, health care visits should be done remotely. [Dental services and preventive dental care](https://www.cdc.gov/coronavirus/2019-ncov/hcp/dental-settings.html) may be resumed. Contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) to see what services they are providing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>If you have [coronavirus symptoms](https://covid19.ca.gov/symptoms-and-risks/#top), please contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) or use the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) self-checker.\n\nIf you have other illnesses or chronic conditions, use [telehealth](https://covid19.ca.gov/telehealth/) to get care from home.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call 911, tell the 911 operator your exact symptoms so the ambulance provider can be ready to treat you safely.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C48" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1630,10 +1630,10 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>Can I get my prescriptions filled?</v>
+        <v>What about routine, elective, or non-urgent medical or dental appointments?</v>
       </c>
       <c r="B49" t="str">
-        <v>Yes. You may leave your home to get prescriptions or cannabis from dispensaries with medical permits.\n\nYou can contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) to get a new prescription or adjust your existing prescriptions. \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Preventive care services and non-emergency surgeries, like organ replacements and tumor removals, can take place if hospitals have enough capacity and protective equipment to do so safely. Eye exams, and elective procedures should be cancelled or rescheduled. If possible, health care visits should be done remotely. [Dental services and preventive dental care](https://www.cdc.gov/coronavirus/2019-ncov/hcp/dental-settings.html) may be resumed. Contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) to see what services they are providing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C49" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1656,10 +1656,10 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>I am an older Californian who is isolating at home and I need non-urgent assistance. What can I do?</v>
+        <v>Can I get my prescriptions filled?</v>
       </c>
       <c r="B50" t="str">
-        <v>You can call the statewide hotline for older Californians at [1-833-544-2374](tel:1-833-544-2374) for your non-urgent medical needs, to get meals delivered, to track down prescriptions, and more. The most important thing you can do is stay home for your health and wellbeing. If you are experiencing an emergency please call 911.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. You may leave your home to get prescriptions or cannabis from dispensaries with medical permits.\n\nYou can contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) to get a new prescription or adjust your existing prescriptions. \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C50" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1682,10 +1682,10 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>How can I make sure the older Californians in my life are safe and healthy during the stay home order?</v>
+        <v>I am an older Californian who is isolating at home and I need non-urgent assistance. What can I do?</v>
       </c>
       <c r="B51" t="str">
-        <v>You should check in on your older neighbors and loved ones with a call, text, or physically-distanced door knock to make sure they are okay. You can also teach them how to use FaceTime, Zoom, Google Duo or Facebook video to communicate. The most important thing you can do is to keep in touch with older loved ones for their mental health and safety.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>You can call the statewide hotline for older Californians at [1-833-544-2374](tel:1-833-544-2374) for your non-urgent medical needs, to get meals delivered, to track down prescriptions, and more. The most important thing you can do is stay home for your health and wellbeing. If you are experiencing an emergency please call 911.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C51" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1708,10 +1708,10 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>Can I leave home to care for my elderly parents or friends who require assistance? Or a friend or family member who has disabilities?</v>
+        <v>How can I make sure the older Californians in my life are safe and healthy during the stay home order?</v>
       </c>
       <c r="B52" t="str">
-        <v>Yes. Be sure that you protect them and yourself by following physical distancing guidelines such as wearing a mask, washing hands before and after, using hand sanitizer, maintaining at least six feet of distance when possible, and covering your cough or sneeze. If you have early signs of a cold, please stay away from your older loved ones.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)&lt;!-- disability, senior --&gt;</v>
+        <v>You should check in on your older neighbors and loved ones with a call, text, or physically-distanced door knock to make sure they are okay. You can also teach them how to use FaceTime, Zoom, Google Duo or Facebook video to communicate. The most important thing you can do is to keep in touch with older loved ones for their mental health and safety.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C52" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1734,10 +1734,10 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>Can I visit loved ones in the hospital, nursing home, skilled nursing facility, or other residential care facility?</v>
+        <v>Can I leave home to care for my elderly parents or friends who require assistance? Or a friend or family member who has disabilities?</v>
       </c>
       <c r="B53" t="str">
-        <v>Generally, no. There are limited exceptions, such as if you are going to the hospital with a minor who is under 18 or someone who is developmentally disabled and needs assistance. For most other situations, the order prohibits visitation to these kinds of facilities. This is difficult, but necessary to protect hospital staff and other patients. Check the [frequently asked questions for friends and family with a loved one in a skilled nursing or residential care facility](https://www.aging.ca.gov/download.ashx?lE0rcNUV0zaaXLD5JZ%2f6Uw%3d%3d) for more detailed information.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)&lt;!-- elderly, disability, senior --&gt;</v>
+        <v>Yes. Be sure that you protect them and yourself by following physical distancing guidelines such as wearing a mask, washing hands before and after, using hand sanitizer, maintaining at least six feet of distance when possible, and covering your cough or sneeze. If you have early signs of a cold, please stay away from your older loved ones.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)&lt;!-- disability, senior --&gt;</v>
       </c>
       <c r="C53" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1760,10 +1760,10 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>Can I get free COVID-19 testing or treatment if I am a senior over 65, disabled, uninsured, or an undocumented immigrant?</v>
+        <v>Can I visit loved ones in the hospital, nursing home, skilled nursing facility, or other residential care facility?</v>
       </c>
       <c r="B54" t="str">
-        <v>All patients with full-service Medi-Cal or commercial insurance in California will have [copays, coinsurance and deductibles waived](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf) for COVID-19 [testing](https://covid19.ca.gov/testing-and-treatment/) and screening.  [Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) cover [coronavirus tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test) tests, with no out-of-pocket costs. The cost of medically necessary coronavirus screening, testing, and treatment for the uninsured is paid for by the [government](https://www.hrsa.gov/CovidUninsuredClaim). \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Generally, no. There are limited exceptions, such as if you are going to the hospital with a minor who is under 18 or someone who is developmentally disabled and needs assistance. For most other situations, the order prohibits visitation to these kinds of facilities. This is difficult, but necessary to protect hospital staff and other patients. Check the [frequently asked questions for friends and family with a loved one in a skilled nursing or residential care facility](https://www.aging.ca.gov/download.ashx?lE0rcNUV0zaaXLD5JZ%2f6Uw%3d%3d) for more detailed information.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)&lt;!-- elderly, disability, senior --&gt;</v>
       </c>
       <c r="C54" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1786,13 +1786,13 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>What do taxpayers need to do if they want to take advantage of relief from the California Department of Tax and Fee Administration?</v>
+        <v>Can I get free COVID-19 testing or treatment if I am a senior over 65, disabled, uninsured, or an undocumented immigrant?</v>
       </c>
       <c r="B55" t="str">
-        <v>Interested taxpayers should contact CDTFA by visiting the [CDTFA website](http://cdtfa.ca.gov/) or calling [800-400-7115](tel:800-400-7115).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>All patients with full-service Medi-Cal or commercial insurance in California will have [copays, coinsurance and deductibles waived](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf) for COVID-19 [testing](https://covid19.ca.gov/testing-and-treatment/) and screening.  [Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) cover [coronavirus tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test) tests, with no out-of-pocket costs. The cost of medically necessary coronavirus screening, testing, and treatment for the uninsured is paid for by the [government](https://www.hrsa.gov/CovidUninsuredClaim). \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C55" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/healthcare/</v>
       </c>
       <c r="D55" t="str">
         <v xml:space="preserve"> </v>
@@ -1812,10 +1812,10 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>When will taxpayers start on these payment plans?</v>
+        <v>What do taxpayers need to do if they want to take advantage of relief from the California Department of Tax and Fee Administration?</v>
       </c>
       <c r="B56" t="str">
-        <v>Given that the April deadline to file and pay sales and use tax returns has been extended to late July for all but the largest taxpayers, CDTFA expects that most participating taxpayers will begin their payment arrangements in late July of this year.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Interested taxpayers should contact CDTFA by visiting the [CDTFA website](http://cdtfa.ca.gov/) or calling [800-400-7115](tel:800-400-7115).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C56" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1838,10 +1838,10 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>How will the payment plans work?</v>
+        <v>When will taxpayers start on these payment plans?</v>
       </c>
       <c r="B57" t="str">
-        <v>Qualifying sales and use taxpayers with deferred liabilities up to $50,000 will pay their tax due in 12 equal monthly installments. No interest or penalties will be assessed against the liability.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Given that the April deadline to file and pay sales and use tax returns has been extended to late July for all but the largest taxpayers, CDTFA expects that most participating taxpayers will begin their payment arrangements in late July of this year.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C57" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1864,10 +1864,10 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>Is this only for tax payments due for the 1st quarter of 2020?</v>
+        <v>How will the payment plans work?</v>
       </c>
       <c r="B58" t="str">
-        <v>If taxpayers choose to use this program to distribute the burden of their May or June prepayments or their July return, CDTFA will work to accommodate those taxpayers.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Qualifying sales and use taxpayers with deferred liabilities up to $50,000 will pay their tax due in 12 equal monthly installments. No interest or penalties will be assessed against the liability.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C58" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1890,10 +1890,10 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>What if taxpayers owe more than the $50,000 limit on the relief?</v>
+        <v>Is this only for tax payments due for the 1st quarter of 2020?</v>
       </c>
       <c r="B59" t="str">
-        <v>The maximum amount that any taxpayer can defer interest-free under this relief effort is $50,000.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>If taxpayers choose to use this program to distribute the burden of their May or June prepayments or their July return, CDTFA will work to accommodate those taxpayers.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C59" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1916,10 +1916,10 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>What if taxpayers with more than $5 million in annual taxable sales need this relief?</v>
+        <v>What if taxpayers owe more than the $50,000 limit on the relief?</v>
       </c>
       <c r="B60" t="str">
-        <v>We recognize that some taxpayers, particularly in low margin businesses, with annual taxable sales over $5 million may also need this relief. Those taxpayers are encouraged to reach out to CDTFA, which will work with them to provide relief where appropriate.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The maximum amount that any taxpayer can defer interest-free under this relief effort is $50,000.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C60" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1942,10 +1942,10 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>Is the deadline for filing California tax returns extended?</v>
+        <v>What if taxpayers with more than $5 million in annual taxable sales need this relief?</v>
       </c>
       <c r="B61" t="str">
-        <v>Yes. All California taxpayers (individuals and businesses) can file and pay by July 15, 2020. See [information from the CA Franchise Tax Board](https://www.ftb.ca.gov/about-ftb/newsroom/news-releases/2020-3-state-postpones-tax-deadlines-until-july-15-due-to-the-covid-19-pandemic.html) for more information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>We recognize that some taxpayers, particularly in low margin businesses, with annual taxable sales over $5 million may also need this relief. Those taxpayers are encouraged to reach out to CDTFA, which will work with them to provide relief where appropriate.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C61" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1968,10 +1968,10 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>What is a loan guarantee?</v>
+        <v>Is the deadline for filing California tax returns extended?</v>
       </c>
       <c r="B62" t="str">
-        <v>A loan guarantee is a credit enhancement that helps mitigate the risk assumed by a lending institution when making a loan. With the Small Business Finance Center’s Disaster Relief Loan Guarantee Program, IBank agrees to guarantee up to 95% of the loan, removing the barriers to capital that often exist for small business borrowers that may not otherwise be eligible for traditional lending. This program also can assist those who may not be eligible for a U.S. Small Business Administration (SBA) loan.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Yes. All California taxpayers (individuals and businesses) can file and pay by July 15, 2020. See [information from the CA Franchise Tax Board](https://www.ftb.ca.gov/about-ftb/newsroom/news-releases/2020-3-state-postpones-tax-deadlines-until-july-15-due-to-the-covid-19-pandemic.html) for more information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C62" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1994,10 +1994,10 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>Who is eligible to apply?</v>
+        <v>What is a loan guarantee?</v>
       </c>
       <c r="B63" t="str">
-        <v>Small business entities that have been affected by loss, damage or other economic injury due to the COVID-19 pandemic and meet the program’s eligibility requirements. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>A loan guarantee is a credit enhancement that helps mitigate the risk assumed by a lending institution when making a loan. With the Small Business Finance Center’s Disaster Relief Loan Guarantee Program, IBank agrees to guarantee up to 95% of the loan, removing the barriers to capital that often exist for small business borrowers that may not otherwise be eligible for traditional lending. This program also can assist those who may not be eligible for a U.S. Small Business Administration (SBA) loan.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C63" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2020,10 +2020,10 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>What do you consider a small business?</v>
+        <v>Who is eligible to apply?</v>
       </c>
       <c r="B64" t="str">
-        <v>The business must have between 1-750 employees and be established as an entity, including:\n\n*   Sole Proprietor – Individual using legal name as business name that files a Schedule C, Schedule F, or has a fictitious business name or DBA statement\n    *   If the loan appears to be in the name of an individual, evidence of Sole Proprietorship will be required and may include a Schedule C, Schedule F, Seller’s Permit, and/or fictitious business name or DBA statement\n*   Limited Liability Company \n*   Cooperative\n*   Corporation\n*   Partnership\n*   S-Corporation\n*   Not-for-profit\n\nThe program will not accept an _individual_ as the borrower. It is permissible for an individual to be a guarantor or co-borrower on the loan, but the primary borrower must be a small business. It does not consider citizenship or immigration status for eligibility requirements**,** as long as the entity/individual meets the above criteria. Trucking owners/operators are eligible as long as they are registered as a legal business entity.\n\n**AND**\n\n*   The business activity must be eligible under the program and in one of the industries listed in the [North American Industry Classification System (NAICS) codes list](http://www.census.gov/eos/www/naics), and\n*   It must be located in a declared disaster area. A major disaster area declaration was made for the state of California on March 22, 2020 in regards to the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Small business entities that have been affected by loss, damage or other economic injury due to the COVID-19 pandemic and meet the program’s eligibility requirements. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C64" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2046,10 +2046,10 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>What are excluded businesses?</v>
+        <v>What do you consider a small business?</v>
       </c>
       <c r="B65" t="str">
-        <v>Businesses that are not eligible include passive real estate businesses (rental income, etc.).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The business must have between 1-750 employees and be established as an entity, including:\n\n*   Sole Proprietor – Individual using legal name as business name that files a Schedule C, Schedule F, or has a fictitious business name or DBA statement\n    *   If the loan appears to be in the name of an individual, evidence of Sole Proprietorship will be required and may include a Schedule C, Schedule F, Seller’s Permit, and/or fictitious business name or DBA statement\n*   Limited Liability Company \n*   Cooperative\n*   Corporation\n*   Partnership\n*   S-Corporation\n*   Not-for-profit\n\nThe program will not accept an _individual_ as the borrower. It is permissible for an individual to be a guarantor or co-borrower on the loan, but the primary borrower must be a small business. It does not consider citizenship or immigration status for eligibility requirements**,** as long as the entity/individual meets the above criteria. Trucking owners/operators are eligible as long as they are registered as a legal business entity.\n\n**AND**\n\n*   The business activity must be eligible under the program and in one of the industries listed in the [North American Industry Classification System (NAICS) codes list](http://www.census.gov/eos/www/naics), and\n*   It must be located in a declared disaster area. A major disaster area declaration was made for the state of California on March 22, 2020 in regards to the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C65" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2072,10 +2072,10 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>Can I apply for a loan guarantee only if I am ineligible for federal disaster fund financing, such as a SBA loan?</v>
+        <v>What are excluded businesses?</v>
       </c>
       <c r="B66" t="str">
-        <v>Yes, this program is designed for those who do not qualify for federal programs. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Businesses that are not eligible include passive real estate businesses (rental income, etc.).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C66" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2098,10 +2098,10 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>How much can I borrow?</v>
+        <v>Can I apply for a loan guarantee only if I am ineligible for federal disaster fund financing, such as a SBA loan?</v>
       </c>
       <c r="B67" t="str">
-        <v>The Small Business Finance Center’s Disaster Relief Loan Guarantee Program allows a maximum loan of $1.25 million and a maximum guarantee of $1 million. To serve as many California small businesses as possible, the COVID-19 disaster program is focused on serving small businesses, especially those in low-wealth and immigrant communities with needs from $500 to $50,000. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Yes, this program is designed for those who do not qualify for federal programs. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C67" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2124,10 +2124,10 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>What are the loan terms?</v>
+        <v>How much can I borrow?</v>
       </c>
       <c r="B68" t="str">
-        <v>The length of the loan can be negotiated with your lender, but the guarantee is good for up to seven years. The interest rate and loan criteria will be determined by the lender and could depend on the credit strength of the business. The guarantee is designed to lower the interest rate in exchange for a higher guarantee to your lender. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The Small Business Finance Center’s Disaster Relief Loan Guarantee Program allows a maximum loan of $1.25 million and a maximum guarantee of $1 million. To serve as many California small businesses as possible, the COVID-19 disaster program is focused on serving small businesses, especially those in low-wealth and immigrant communities with needs from $500 to $50,000. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C68" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2150,10 +2150,10 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>How can I apply?</v>
+        <v>What are the loan terms?</v>
       </c>
       <c r="B69" t="str">
-        <v>The Small Business Finance Center partners with Community Development Financial Institutions (CDFIs), Community Lending Institutions, and Financial Development Corporations (FDCs) to provide loan guarantees for small businesses.  To apply,\n\n*   View the [list of FDCs and participating lenders](http://www.ibank.ca.gov/small-business-finance-center/) interested in this Small Business Disaster Relief Loan Guarantee Program. \n*   Contact the lender on the list nearest to your business to apply.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The length of the loan can be negotiated with your lender, but the guarantee is good for up to seven years. The interest rate and loan criteria will be determined by the lender and could depend on the credit strength of the business. The guarantee is designed to lower the interest rate in exchange for a higher guarantee to your lender. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C69" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2176,10 +2176,10 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>What is the timing for the funding of loans?</v>
+        <v>How can I apply?</v>
       </c>
       <c r="B70" t="str">
-        <v>The program is in place and businesses can apply immediately. Once you provide your lender with complete information, you could be funded in a matter of days.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The Small Business Finance Center partners with Community Development Financial Institutions (CDFIs), Community Lending Institutions, and Financial Development Corporations (FDCs) to provide loan guarantees for small businesses.  To apply,\n\n*   View the [list of FDCs and participating lenders](http://www.ibank.ca.gov/small-business-finance-center/) interested in this Small Business Disaster Relief Loan Guarantee Program. \n*   Contact the lender on the list nearest to your business to apply.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C70" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2202,10 +2202,10 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>What can the money be used for?</v>
+        <v>What is the timing for the funding of loans?</v>
       </c>
       <c r="B71" t="str">
-        <v>The funds are meant to help small businesses through this challenging time. Loan proceeds can be used for business continuance or to cure “economic injury” as a result of COVID-19.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The program is in place and businesses can apply immediately. Once you provide your lender with complete information, you could be funded in a matter of days.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C71" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2228,10 +2228,10 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>How will this program assist low-wealth and minority communities?</v>
+        <v>What can the money be used for?</v>
       </c>
       <c r="B72" t="str">
-        <v>By working with the Community Development Financial Institutions (CDFIs) throughout the state of California, this disaster relief program can play an important role in generating economic growth and opportunity in some of our most distressed communities. CDFIs and mission-based lenders play a vital role across the state and have experience steering lending and investment to where it is needed and will matter the most, in particular in low-wealth and immigrant communities. CDFIs and our partner Financial Development Corporations (FDCs) that process the loan guarantees are embedded in communities across the state, speak several languages, and are invested in the community successfully managing its way through this pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The funds are meant to help small businesses through this challenging time. Loan proceeds can be used for business continuance or to cure “economic injury” as a result of COVID-19.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C72" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2254,10 +2254,10 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>Are faith-based businesses eligible for this loan guarantee program?</v>
+        <v>How will this program assist low-wealth and minority communities?</v>
       </c>
       <c r="B73" t="str">
-        <v>Faith-based businesses (non-profit or otherwise) that have business activity outside of worship are eligible as long as they are a legal business that has been affected by the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>By working with the Community Development Financial Institutions (CDFIs) throughout the state of California, this disaster relief program can play an important role in generating economic growth and opportunity in some of our most distressed communities. CDFIs and mission-based lenders play a vital role across the state and have experience steering lending and investment to where it is needed and will matter the most, in particular in low-wealth and immigrant communities. CDFIs and our partner Financial Development Corporations (FDCs) that process the loan guarantees are embedded in communities across the state, speak several languages, and are invested in the community successfully managing its way through this pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C73" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2280,10 +2280,10 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>What SBA programs are available to small businesses right now?</v>
+        <v>Are faith-based businesses eligible for this loan guarantee program?</v>
       </c>
       <c r="B74" t="str">
-        <v>The U.S. SBA offers the **Paycheck Protection Program (PPP)** and **Economic Injury Disaster Loan and Advance (EIDL and EIDL Advance)**.\n\nMore about **Paycheck Protection Program (PPP)**:\n\nThe PPP is a loan program for small businesses, self-employed, independent contractors, nonprofits with a maximum of 500 employees, and it is intended to keep workers paid and employed. The loan amount is calculated based on payroll expenses with a maximum amount of $10 million at a rate of 1%. For all loans made on or after June 5, the minimum term is five years. For loans made before June 5, the two-year minimum maturity remains in effect unless both the borrower and the lender agree to extend it to five years. The loan is forgivable if 60% of the loan amount is used for payroll, and no employees are laid off, or if laid-off employees are rehired before December 31, 2020. In addition to payroll and benefits costs, allowable expenses include mortgage interest, rent, and utilities. Submit your application as soon as possible, even if you need to rehire employees that have been laid off.\n\nThe SBA is accepting PPP loan applications from approved lenders. The new deadline to apply for a PPP loan is August 8, 2020. You must apply directly through a lender. [Find a PPP lender in your area](https://www.sba.gov/paycheckprotection/find) to contact right away. See [SBA.gov](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program#section-header-0) for more details. \n\nMore about **Economic Injury Disaster Loan and Advance (EIDL and EIDL Advance):**\n\nAs of June 15, the U.S. SBA is accepting new applications from all eligible businesses, and will continue to process **EIDL Loan and Advance applications** already submitted on a first come, first-served basis. Check the U.S. SBA’s [Disaster Loan Applications website](https://www.sba.gov/page/disaster-loan-applications#section-header-0) for more information.\n\nThe EIDL is a direct loan for up to $2 million at a rate of 3.75% for small businesses and 2.75% for nonprofits. Applicants can get an **Advance** of up to $10,000 upon request within days of a successful application. This advance doesn’t have to be repaid. [Apply directly with the SBA](https://covid19relief.sba.gov/#/). For questions, you can contact SBA’s Customer Service Line at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or send an email to [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Faith-based businesses (non-profit or otherwise) that have business activity outside of worship are eligible as long as they are a legal business that has been affected by the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C74" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2306,10 +2306,10 @@
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>Which banks are offering the Paycheck Protection Program forgivable loans?</v>
+        <v>What SBA programs are available to small businesses right now?</v>
       </c>
       <c r="B75" t="str">
-        <v>Interested borrowers can contact any SBA participating bank, credit union, or nonprofit lenders to apply for the [PPP](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program). For more information, contact your local bank or reach out to [SBA’s local district offices](https://www.sba.gov/local-assistance/find/?type=SBA%20District%20Office&amp;pageNumber=1) for assistance.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The U.S. SBA offers the **Paycheck Protection Program (PPP)** and **Economic Injury Disaster Loan (EIDL)**.\n\nMore about **Paycheck Protection Program (PPP)**:\n\nThe PPP is a loan program for small businesses, self-employed, independent contractors, nonprofits with a maximum of 500 employees, and it is intended to keep workers paid and employed. The loan amount is calculated based on payroll expenses with a maximum amount of $10 million at a rate of 1%. For all loans made on or after June 5, the minimum term is five years. For loans made before June 5, the two-year minimum maturity remains in effect unless both the borrower and the lender agree to extend it to five years. The loan is forgivable if 60% of the loan amount is used for payroll, and no employees are laid off, or if laid-off employees are rehired before December 31, 2020. In addition to payroll and benefits costs, allowable expenses include mortgage interest, rent, and utilities. Submit your application as soon as possible, even if you need to rehire employees that have been laid off.\n\nThe SBA is accepting PPP loan applications from approved lenders. The new deadline to apply for a PPP loan is August 8, 2020. You must apply directly through a lender. [Find a PPP lender in your area](https://www.sba.gov/paycheckprotection/find) to contact right away. See [SBA.gov](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program#section-header-0) for more details. \n\nMore about **Economic Injury Disaster Loan (EIDL):**\n\nThe U.S. SBA is accepting new applications from all eligible businesses, and will continue to process **EIDL Loan applications** already submitted on a first come, first-served basis. Check the U.S. SBA’s [Disaster Loan Applications website](https://www.sba.gov/page/disaster-loan-applications#section-header-0) for more information.\n\nThe EIDL is a direct loan for up to $2 million at a rate of 3.75% for small businesses and 2.75% for nonprofits. [Apply directly with the SBA](https://covid19relief.sba.gov/#/). For questions, you can contact SBA’s Customer Service Line at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or send an email to [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nThe **Economic Injury Disaster Loan (**EIDL) **Advance** has been [discontinued](https://www.sba.gov/page/disaster-loan-applications#section-header-0). EIDL loan applications will still be processed even though the Advance is no longer available.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C75" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2332,10 +2332,10 @@
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>Where do I find more information on allowable expenses for a forgivable loan under the Paycheck Protection Program?</v>
+        <v>Which banks are offering the Paycheck Protection Program forgivable loans?</v>
       </c>
       <c r="B76" t="str">
-        <v>You can find this on the Paycheck Protection Program’s [Loan Forgiveness Application](https://www.sba.gov/sites/default/files/2020-06/PPP%20Loan%20Forgiveness%20Application%20%28Revised%206.16.2020%29-fillable_0-508.pdf). The application provides detailed [instructions](https://www.sba.gov/sites/default/files/2020-06/PPP%20Loan%20Forgiveness%20Application%20Instructions%20%28Revised%206.16.2020%29-508.pdf) on how to apply for forgiveness of PPP loans. Once your business has expended the PPP funds and is ready to pursue loan forgiveness, please review the Loan Forgiveness Application and consult with your accountant, lender, or one of California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) for assistance.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Interested borrowers can contact any SBA participating bank, credit union, or nonprofit lenders to apply for the [PPP](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program). For more information, contact your local bank or reach out to [SBA’s local district offices](https://www.sba.gov/local-assistance/find/?type=SBA%20District%20Office&amp;pageNumber=1) for assistance.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C76" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2358,10 +2358,10 @@
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>How does a business know if it is eligible for an SBA loan or loan guarantee program?</v>
+        <v>Where do I find more information on allowable expenses for a forgivable loan under the Paycheck Protection Program?</v>
       </c>
       <c r="B77" t="str">
-        <v>Small businesses with 500 employees or less are eligible to apply for the Paycheck Protection Program (PPP) and/or the Small Business Debt Relief Program. Small businesses are also eligible to apply for the Economic Injury Disaster Loan (EIDL) program and the EIDL Advance. Visit SBA’s comprehensive [COVID-19 support website](https://www.sba.gov/page/coronavirus-covid-19-small-business-guidance-loan-resources#section-header-4%20.) to find out more about SBA’s eligibility requirements for each program.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>You can find this on the Paycheck Protection Program’s [Loan Forgiveness Application](https://www.sba.gov/sites/default/files/2020-06/PPP%20Loan%20Forgiveness%20Application%20%28Revised%206.16.2020%29-fillable_0-508.pdf). The application provides detailed [instructions](https://www.sba.gov/sites/default/files/2020-06/PPP%20Loan%20Forgiveness%20Application%20Instructions%20%28Revised%206.16.2020%29-508.pdf) on how to apply for forgiveness of PPP loans. Once your business has expended the PPP funds and is ready to pursue loan forgiveness, please review the Loan Forgiveness Application and consult with your accountant, lender, or one of California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) for assistance.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C77" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2384,10 +2384,10 @@
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>How do I reach SBA for any questions or assistance?</v>
+        <v>How does a business know if it is eligible for an SBA loan or loan guarantee program?</v>
       </c>
       <c r="B78" t="str">
-        <v>SBA has district offices in California that are open to answer questions. You can use the [SBA’s Local Assistance Directory](https://www.sba.gov/local-assistance) to locate the office nearest you. You can also contact the SBA by phone at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or by email at [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).  \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Small businesses with 500 employees or less are eligible to apply for the Paycheck Protection Program (PPP) and/or the Small Business Debt Relief Program. Small businesses are also eligible to apply for the Economic Injury Disaster Loan (EIDL) program. Visit SBA’s comprehensive [COVID-19 support website](https://www.sba.gov/page/coronavirus-covid-19-small-business-guidance-loan-resources#section-header-4%20.) to find out more about SBA’s eligibility requirements for each program.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C78" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2410,10 +2410,10 @@
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>How does a small business know which SBA loan or loan guarantee program is the right one? Can a small business apply to more than one?</v>
+        <v>How do I reach SBA for any questions or assistance?</v>
       </c>
       <c r="B79" t="str">
-        <v>Call or email the SBA to find out which program is right for you. While businesses can apply for and receive more than one form of capital assistance through the SBA, they cannot be used for the same purpose. The SBA can advise you on your options. Call [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or email [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>SBA has district offices in California that are open to answer questions. You can use the [SBA’s Local Assistance Directory](https://www.sba.gov/local-assistance) to locate the office nearest you. You can also contact the SBA by phone at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or by email at [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).  \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C79" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2436,10 +2436,10 @@
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>How do I get SBA to cover my loan payments on my existing 7(a), 504, or microloan if I cannot pay due to COVID-19?</v>
+        <v>How does a small business know which SBA loan or loan guarantee program is the right one? Can a small business apply to more than one?</v>
       </c>
       <c r="B80" t="str">
-        <v>SBA has a [Debt Relief program](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/sba-debt-relief) and will pay the principal and interest of existing SBA loans. Please contact your lender for information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Call or email the SBA to find out which program is right for you. While businesses can apply for and receive more than one form of capital assistance through the SBA, they cannot be used for the same purpose. The SBA can advise you on your options. Call [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or email [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C80" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2462,10 +2462,10 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>If I need help to figure out which program is best for me or to submit an application, where can I find support?</v>
+        <v>How do I get SBA to cover my loan payments on my existing 7(a), 504, or microloan if I cannot pay due to COVID-19?</v>
       </c>
       <c r="B81" t="str">
-        <v>California’s network of small business support centers can help you figure out which loans and programs are best for your business, develop resiliency strategies, and find other resources. Go to California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) to find the closest center.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>SBA has a [Debt Relief program](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/sba-debt-relief) and will pay the principal and interest of existing SBA loans. Please contact your lender for information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C81" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2488,10 +2488,10 @@
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>How do I maintain a safe workplace?</v>
+        <v>If I need help to figure out which program is best for me or to submit an application, where can I find support?</v>
       </c>
       <c r="B82" t="str">
-        <v>As California [reopens](https://covid19.ca.gov/roadmap/), every business will need to create a safer, low-risk environment. If you own or manage a business, follow the [industry-specific guidance](https://covid19.ca.gov/industry-guidance/) that applies to protect your workers and customers.\n\nIf your business is approved to reopen, you should take steps to ensure the safety and health of your workers. It’s important that employees with COVID-19 know they should stay home. Your sick leave policies need to support that. \n\n*   Encourage sick employees to stay home if they are sick. See government programs supporting [COVID-19 sick leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) and [workers’ compensation](https://www.labor.ca.gov/coronavirus2019/#chart).\n*   Establish routine cleaning throughout the workplace.\n*   Reduce travel. If possible, encourage video conferencing and limit larger gatherings.\n*   See [Cal/OSHA interim guidelines for general industry](https://www.dir.ca.gov/dosh/coronavirus/General-Industry.html).\n*   Follow [CDC guidance on keeping the workplace safe (PDF)](https://www.cdc.gov/coronavirus/2019-ncov/downloads/workplace-school-and-home-guidance.pdf).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>California’s network of small business support centers can help you figure out which loans and programs are best for your business, develop resiliency strategies, and find other resources. Go to California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) to find the closest center.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C82" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2514,10 +2514,10 @@
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>What precautions should healthcare workers and organizations take?</v>
+        <v>How do I maintain a safe workplace?</v>
       </c>
       <c r="B83" t="str">
-        <v>See [Cal/OSHA’s guidance on protecting workers from coronavirus](https://www.dir.ca.gov/dosh/coronavirus/Health-Care-General-Industry.html).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>As California reopens, every business will need to create a safer, low-risk environment. If you own or manage a business, follow the [industry-specific guidance](https://covid19.ca.gov/industry-guidance/) that applies to protect your workers and customers.\n\nIf your business is approved to reopen, you should take steps to ensure the safety and health of your workers. It’s important that employees with COVID-19 know they should stay home. Your sick leave policies need to support that. \n\n*   Encourage sick employees to stay home if they are sick. See government programs supporting [COVID-19 sick leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) and [workers’ compensation](https://www.labor.ca.gov/coronavirus2019/#chart).\n*   Establish routine cleaning throughout the workplace.\n*   Reduce travel. If possible, encourage video conferencing and limit larger gatherings.\n*   See [Cal/OSHA interim guidelines for general industry](https://www.dir.ca.gov/dosh/coronavirus/General-Industry.html).\n*   Follow [CDC guidance on keeping the workplace safe (PDF)](https://www.cdc.gov/coronavirus/2019-ncov/downloads/workplace-school-and-home-guidance.pdf).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C83" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2540,10 +2540,10 @@
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>How can I avoid laying off employees if my business is impacted by COVID-19?</v>
+        <v>What precautions should healthcare workers and organizations take?</v>
       </c>
       <c r="B84" t="str">
-        <v>Apply for the [Unemployment Insurance (UI) Work Sharing Program](https://www.edd.ca.gov/Unemployment/Work_Sharing_Program.htm).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>See [Cal/OSHA’s guidance on protecting workers from coronavirus](https://www.dir.ca.gov/dosh/coronavirus/Health-Care-General-Industry.html).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C84" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2566,13 +2566,13 @@
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>What action is the state taking to ensure all schools are providing meaningful instruction during the pandemic whether they are physically open or closed?</v>
+        <v>How can I avoid laying off employees if my business is impacted by COVID-19?</v>
       </c>
       <c r="B85" t="str">
-        <v>*   California has made $5.3 billion in investments to support safe reopening and rigorous distance learning.\n*   Funds prioritize low-income students, English language learners, and special education students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>Apply for the [Unemployment Insurance (UI) Work Sharing Program](https://www.edd.ca.gov/Unemployment/Work_Sharing_Program.htm).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C85" t="str">
-        <v>https://covid19.ca.gov/education/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D85" t="str">
         <v xml:space="preserve"> </v>
@@ -2592,10 +2592,10 @@
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>What determines whether schools are conducting in-person learning or distance learning?</v>
+        <v>What action is the state taking to ensure all schools are providing meaningful instruction during the pandemic whether they are physically open or closed?</v>
       </c>
       <c r="B86" t="str">
-        <v>Using health data, schools can physically open when its county has been off the Monitoring List for 14 days and only if they follow strict health and safety requirements like masks and physical distancing. [Find the County Monitoring List here.](https://covid19.ca.gov/roadmap-counties/#track-data)\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>*   California has made $5.3 billion in investments to support safe reopening and rigorous distance learning.\n*   Funds prioritize low-income students, English language learners, and special education students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C86" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2618,10 +2618,10 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>What are the health and safety requirements for schools doing in-person learning?</v>
+        <v>What determines whether schools are conducting in-person learning or distance learning?</v>
       </c>
       <c r="B87" t="str">
-        <v>*   Everyone entering the school must do daily health checks.\n*   If someone experiences symptoms while at school, they will be sent home.\n*   Masks are required for all staff and students 3rd grade and above. Younger students should be encouraged to wear masks.\n*   Staff members must maintain 6ft distance from each other and students. Students should maintain 6ft distance as practicable.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>Using health data, schools can physically open when its county has been off the Monitoring List for 14 days and only if they follow strict health and safety requirements like masks and physical distancing. [Find the County Monitoring List here.](https://covid19.ca.gov/roadmap-counties/#track-data)\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C87" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2644,10 +2644,10 @@
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>What happens if someone gets COVID-19 at my child’s school?</v>
+        <v>What are the health and safety requirements for schools doing in-person learning?</v>
       </c>
       <c r="B88" t="str">
-        <v>*   A classroom goes home when there is a confirmed case\n*   A school should switch to distance learning when there are multiple positive cases in multiple classroom cohorts\n*   A district should switch to distance learning if 25% of schools in the district are closed within a 14-day period\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>*   Everyone entering the school must do daily health checks.\n*   If someone experiences symptoms while at school, they will be sent home.\n*   Masks are required for all staff and students 3rd grade and above. Younger students should be encouraged to wear masks.\n*   Staff members must maintain 6ft distance from each other and students. Students should maintain 6ft distance as practicable.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C88" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2670,10 +2670,10 @@
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>If my child’s school is engaged in distance learning, what should I expect?</v>
+        <v>What happens if someone gets COVID-19 at my child’s school?</v>
       </c>
       <c r="B89" t="str">
-        <v>*   New statewide requirements include:\n    *   Access to devices and connectivity for all students\n    *   Daily live interaction with teachers and other students\n    *   Classes and assignments that are challenging and are equivalent to in-person instruction\n    *   Special requirements for English language learners and special education students\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>*   A classroom goes home when there is a confirmed case\n*   A school should switch to distance learning when there are multiple positive cases in multiple classroom cohorts\n*   A district should switch to distance learning if 25% of schools in the district are closed within a 14-day period\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C89" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2696,10 +2696,10 @@
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>Is there financial help for student loans?</v>
+        <v>If my child’s school is engaged in distance learning, what should I expect?</v>
       </c>
       <c r="B90" t="str">
-        <v>The [governor has ordered](https://www.gov.ca.gov/2020/04/23/governor-newsom-announces-additional-relief-for-californians-impacted-by-covid-19/) relief for students with federal loans. Check with your lender to see what options are available for you.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>*   New statewide requirements include:\n    *   Access to devices and connectivity for all students\n    *   Daily live interaction with teachers and other students\n    *   Classes and assignments that are challenging and are equivalent to in-person instruction\n    *   Special requirements for English language learners and special education students\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C90" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2722,10 +2722,10 @@
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>My school provides free grab-and-go meals. Are those still available?</v>
+        <v>Is there financial help for student loans?</v>
       </c>
       <c r="B91" t="str">
-        <v>Yes. It is essential to keep children fed. Check with your local school district for days and times meals are offered.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>The [governor has ordered](https://www.gov.ca.gov/2020/04/23/governor-newsom-announces-additional-relief-for-californians-impacted-by-covid-19/) relief for students with federal loans. Check with your lender to see what options are available for you.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C91" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2748,10 +2748,10 @@
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>What if I don’t have internet access at home?</v>
+        <v>My school provides free grab-and-go meals. Are those still available?</v>
       </c>
       <c r="B92" t="str">
-        <v>Check with your local school district or college to see what resources are available for you.  List of providers offering free internet access currently:\n\n[Spectrum mobile](https://mobile.spectrum.com/support/article/360040980371/coronavirus-covid19-update)  has opened wifi hotspots and are working on assisting school districts with facilitating home internet access. \n\n[Comcast](https://corporate.comcast.com/covid-19) has opened free Xfinity WiFi hotspot access across the country. Xfinity has also paused data plans, late fees, and disconnects for the next 60 days. Families with limited income can receive internet services for free for the next 60 days (usually $9.95 per month). \n\n[AT&amp;T](https://about.att.com/pages/COVID-19.html)  has opened all public WiFi hotspots and will not charge customers for any late fees or overages. AT&amp;T also offers internet access for [$10/month for households on limited income](https://www.att.com/shop/internet/access/index.html?source=ECmj0000000000mbU&amp;wtExtndSource=access#!/#%2F).\n\n[Low-cost Internet access plans](https://www.cde.ca.gov/ls/he/hn/availableinternetplans.asp) are also available.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>Yes. It is essential to keep children fed. Check with your local school district for days and times meals are offered.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C92" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2774,10 +2774,10 @@
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>How will students with disabilities receive services during school closures?</v>
+        <v>What if I don’t have internet access at home?</v>
       </c>
       <c r="B93" t="str">
-        <v>The Department of Education has released [guidance on distance learning](https://www.cde.ca.gov/ls/he/hn/distancelearning.asp) to support schools. This guidance includes recommendations to ensure equity and access for all students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>Check with your local school district or college to see what resources are available for you.  List of providers offering free internet access currently:\n\n[Spectrum mobile](https://mobile.spectrum.com/support/article/360040980371/coronavirus-covid19-update)  has opened wifi hotspots and are working on assisting school districts with facilitating home internet access. \n\n[Comcast](https://corporate.comcast.com/covid-19) has opened free Xfinity WiFi hotspot access across the country. Xfinity has also paused data plans, late fees, and disconnects for the next 60 days. Families with limited income can receive internet services for free for the next 60 days (usually $9.95 per month). \n\n[AT&amp;T](https://about.att.com/pages/COVID-19.html)  has opened all public WiFi hotspots and will not charge customers for any late fees or overages. AT&amp;T also offers internet access for [$10/month for households on limited income](https://www.att.com/shop/internet/access/index.html?source=ECmj0000000000mbU&amp;wtExtndSource=access#!/#%2F).\n\n[Low-cost Internet access plans](https://www.cde.ca.gov/ls/he/hn/availableinternetplans.asp) are also available.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C93" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2800,10 +2800,10 @@
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>Will there be standardized testing? When?</v>
+        <v>How will students with disabilities receive services during school closures?</v>
       </c>
       <c r="B94" t="str">
-        <v>Probably not: on March 18, 2020, Governor Newsom issued an [executive order](https://www.gov.ca.gov/2020/03/18/governor-newsom-issues-executive-order-to-suspend-standardized-testing-for-students-in-response-to-covid-19-outbreak/)  to waive this year’s statewide testing for K-12 schools.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>The Department of Education has released [guidance on distance learning](https://www.cde.ca.gov/ls/he/hn/distancelearning.asp) to support schools. This guidance includes recommendations to ensure equity and access for all students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C94" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2826,13 +2826,13 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>Am I allowed to work during the outbreak?</v>
+        <v>Will there be standardized testing? When?</v>
       </c>
       <c r="B95" t="str">
-        <v>It depends what your job is. Workers in [essential sectors (pdf)](https://covid19.ca.gov/img/EssentialCriticalInfrastructureWorkers.pdf) are allowed to work during the [stay home order](https://covid19.ca.gov/stay-home-except-for-essential-needs/#top). And anyone is allowed to work from their home that has arranged to do so with their employer.\n\nFor information on businesses and industry sectors that are allowed to reopen, visit [industry guidance](https://covid19.ca.gov/industry-guidance/).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>Probably not: on March 18, 2020, Governor Newsom issued an [executive order](https://www.gov.ca.gov/2020/03/18/governor-newsom-issues-executive-order-to-suspend-standardized-testing-for-students-in-response-to-covid-19-outbreak/)  to waive this year’s statewide testing for K-12 schools.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C95" t="str">
-        <v>https://covid19.ca.gov/workers/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D95" t="str">
         <v xml:space="preserve"> </v>
@@ -2852,10 +2852,10 @@
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>What can I do if my work hours are reduced because of COVID-19?</v>
+        <v>Am I allowed to work during the outbreak?</v>
       </c>
       <c r="B96" t="str">
-        <v>You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>It depends what your job is. Workers in [essential sectors (PDF)](https://files.covid19.ca.gov/pdf/EssentialCriticalInfrastructureWorkers.pdf) are allowed to work during the [stay home order](https://covid19.ca.gov/stay-home-except-for-essential-needs/#top). And anyone is allowed to work from their home that has arranged to do so with their employer.\n\nFor information on businesses and industry sectors that are allowed to reopen, visit [industry guidance](https://covid19.ca.gov/industry-guidance/).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C96" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2878,10 +2878,10 @@
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>Do I need a note or certificate from a medical provider to file for unemployment?</v>
+        <v>What can I do if my work hours are reduced because of COVID-19?</v>
       </c>
       <c r="B97" t="str">
-        <v>No, a medical certificate is not required.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C97" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2904,10 +2904,10 @@
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>How long will it take to process a claim for unemployment or insurance benefits and to receive a payment?</v>
+        <v>Do I need a note or certificate from a medical provider to file for unemployment?</v>
       </c>
       <c r="B98" t="str">
-        <v>After your claim is submitted, it will take at least three weeks to be processed. It may take longer if your information doesn’t match wage records or your identity can’t be verified. \n\nThe Governor has [waived the one-week waiting period](https://www.gov.ca.gov/2020/03/12/governor-newsom-issues-new-executive-order-further-enhancing-state-and-local-governments-ability-to-respond-to-covid-19-pandemic/). This means you can collect benefits for the first week that you were out of work or had reduced hours.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>No, a medical certificate is not required.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C98" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2930,10 +2930,10 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>Can I file a workplace safety complaint?</v>
+        <v>How long will it take to process a claim for unemployment or insurance benefits and to receive a payment?</v>
       </c>
       <c r="B99" t="str">
-        <v>Yes, you have the right to file a complaint. Find [information and instructions](https://www.dir.ca.gov/dosh/complaint.htm) for how to file a complaint. If you submit a complaint, your name must be kept confidential by law.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>After your claim is submitted, it will take at least three weeks to be processed. It may take longer if your information doesn’t match wage records or your identity can’t be verified. \n\nThe Governor has [waived the one-week waiting period](https://www.gov.ca.gov/2020/03/12/governor-newsom-issues-new-executive-order-further-enhancing-state-and-local-governments-ability-to-respond-to-covid-19-pandemic/). This means you can collect benefits for the first week that you were out of work or had reduced hours.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C99" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2956,10 +2956,10 @@
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>What can I do if I miss work because of school closures?</v>
+        <v>Can I file a workplace safety complaint?</v>
       </c>
       <c r="B100" t="str">
-        <v>*   You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n*   Other options may be available. See [Benefits for Workers Impacted by COVID-19](https://www.labor.ca.gov/coronavirus2019/#chart).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>Yes, you have the right to file a complaint. Find [information and instructions](https://www.dir.ca.gov/dosh/complaint.htm) for how to file a complaint. If you submit a complaint, your name must be kept confidential by law.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C100" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2982,10 +2982,10 @@
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>What if I can’t work because I’m taking care of someone who’s sick or quarantined?</v>
+        <v>What can I do if I miss work because of school closures?</v>
       </c>
       <c r="B101" t="str">
-        <v>*   You may use [paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). The Labor and Workforce Development Agency has created a [chart detailing the available paid sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law. \n*   You can [file a Paid Family Leave (PFL) claim](https://www.edd.ca.gov/Disability/How_to_File_a_PFL_Claim_in_SDI_Online.htm).\n*   Unpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>*   You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n*   Other options may be available. See [Benefits for Workers Impacted by COVID-19](https://www.labor.ca.gov/coronavirus2019/#chart).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C101" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -3008,10 +3008,10 @@
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>What can I do if I can’t work because I’m sick or quarantined because of COVID-19?</v>
+        <v>What if I can’t work because I’m taking care of someone who’s sick or quarantined?</v>
       </c>
       <c r="B102" t="str">
-        <v>*   You may be able to use [paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). The Labor and Workforce Development Agency has created a [chart detailing the available paid sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law.\n*   If you’re unable to work due to having or being exposed to COVID-19, you can [file a Disability Insurance (DI) claim](https://www.edd.ca.gov/Disability/How_to_File_a_DI_Claim_in_SDI_Online.htm).\n*   You may also file a [Workers’ Compensation Claim](https://www.dir.ca.gov/dwc/FileAClaim.htm) if you suffered a COVID-19 illness that arose from an exposure during the course of your work. Check the California Department of Industrial Relations’ [COVID-19 Resources and Workers’ Compensation](https://www.dir.ca.gov/dwc/Covid-19/Index.html) for more information.\n*   Unpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>*   You may use [paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). The Labor and Workforce Development Agency has created a [chart detailing the available paid sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law. \n*   You can [file a Paid Family Leave (PFL) claim](https://www.edd.ca.gov/Disability/How_to_File_a_PFL_Claim_in_SDI_Online.htm).\n*   Unpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C102" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -3034,10 +3034,10 @@
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>What if I don’t have any available sick leave to use?</v>
+        <v>What can I do if I can’t work because I’m sick or quarantined because of COVID-19?</v>
       </c>
       <c r="B103" t="str">
-        <v>Check the Labor and Workforce Development Agency’s [chart detailing the available sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law.\n\nUnpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>*   You may be able to use [paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). The Labor and Workforce Development Agency has created a [chart detailing the available paid sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law.\n*   If you’re unable to work due to having or being exposed to COVID-19, you can [file a Disability Insurance (DI) claim](https://www.edd.ca.gov/Disability/How_to_File_a_DI_Claim_in_SDI_Online.htm).\n*   You may also file a [Workers’ Compensation Claim](https://www.dir.ca.gov/dwc/FileAClaim.htm) if you suffered a COVID-19 illness that arose from an exposure during the course of your work. Check the California Department of Industrial Relations’ [COVID-19 Resources and Workers’ Compensation](https://www.dir.ca.gov/dwc/Covid-19/Index.html) for more information.\n*   Unpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C103" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -3060,13 +3060,13 @@
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>What effect will this have on my credit report?</v>
+        <v>What if I don’t have any available sick leave to use?</v>
       </c>
       <c r="B104" t="str">
-        <v>Financial institutions will not report derogatory information (like late payments) to credit reporting agencies but may report a forbearance. Typically this does not negatively affect a credit score on its own.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>Check the Labor and Workforce Development Agency’s [chart detailing the available sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law.\n\nUnpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C104" t="str">
-        <v>https://covid19.ca.gov/get-financial-help/</v>
+        <v>https://covid19.ca.gov/workers/</v>
       </c>
       <c r="D104" t="str">
         <v xml:space="preserve"> </v>
@@ -3086,10 +3086,10 @@
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>How long will these programs last?</v>
+        <v>What effect will this have on my credit report?</v>
       </c>
       <c r="B105" t="str">
-        <v>It is still unclear how severe or how long the COVID-19 impact will be. Financial institutions have committed to necessary relief and will be assessing the ongoing conditions and need for continuing relief.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>Financial institutions will not report derogatory information (like late payments) to credit reporting agencies but may report a forbearance. Typically this does not negatively affect a credit score on its own.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C105" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -3112,10 +3112,10 @@
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>What if my financial institution isn’t offering this relief?</v>
+        <v>How long will these programs last?</v>
       </c>
       <c r="B106" t="str">
-        <v>Call or check their website to be sure. At this time, JP Morgan Chase, US Bank, Wells Fargo and Citigroup, [and nearly 200 state-chartered banks](https://dbo.ca.gov/covid19-updates-fi/), credit unions are supporting these commitments. \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>It is still unclear how severe or how long the COVID-19 impact will be. Financial institutions have committed to necessary relief and will be assessing the ongoing conditions and need for continuing relief.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C106" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -3138,10 +3138,10 @@
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>What if I already made a payment or was hit with a fee because of COVID-19?</v>
+        <v>What if my financial institution isn’t offering this relief?</v>
       </c>
       <c r="B107" t="str">
-        <v>Talk to your financial institution. These measures go into effect as of March 25, 2020.  \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>Call or check their website to be sure. At this time, JP Morgan Chase, US Bank, Wells Fargo and Citigroup, [and nearly 200 state-chartered banks](https://dbo.ca.gov/covid19-updates-fi/), credit unions are supporting these commitments. \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C107" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -3164,10 +3164,10 @@
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>Is mortgage relief available to businesses?</v>
+        <v>What if I already made a payment or was hit with a fee because of COVID-19?</v>
       </c>
       <c r="B108" t="str">
-        <v>The relief is currently only available for residential mortgages.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>Talk to your financial institution. These measures go into effect as of March 25, 2020.  \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C108" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -3190,10 +3190,10 @@
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>What if my mortgage servicer is not communicative or cooperative?</v>
+        <v>Is mortgage relief available to businesses?</v>
       </c>
       <c r="B109" t="str">
-        <v>You can file a complaint with the Department of Business Oversight:\n\n*   File on their [website](https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fdbo.ca.gov%2Ffile-a-complaint%2F&amp;data=02%7C01%7CManuel.Alvarez%40dbo.ca.gov%7Ce2673837ec6f42fce84508d7d114ed59%7Cd6910b1745b44b7bbb66cb7936fabafe%7C1%7C0%7C637207760136603083&amp;sdata=VR6CdqCvrBGkfC%2Bm%2B6Yj9emco9ldVY5BLWSiLpe3f4c%3D&amp;reserved=0)\n*    Call their Consumer Services Office at [(866) 275-2677](tel:(866) 275-2677) or [(916) 327-7585](tel:(916) 327-7585) \n*   Or email Ask.DBO@dbo.ca.gov\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>The relief is currently only available for residential mortgages.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C109" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -3216,10 +3216,10 @@
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>Can I get child care during the stay home order?</v>
+        <v>What if my mortgage servicer is not communicative or cooperative?</v>
       </c>
       <c r="B110" t="str">
-        <v>[Child care options](https://covid19.ca.gov/childcare/) are available if you work at an [essential job](https://covid19.ca.gov/essential-workforce/) or a permitted job in the [current roadmap stage](https://covid19.ca.gov/roadmap/). If you are not working at a job like this, it is important to keep children at home. \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>You can file a complaint with the Department of Business Oversight:\n\n*   File on their [website](https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fdbo.ca.gov%2Ffile-a-complaint%2F&amp;data=02%7C01%7CManuel.Alvarez%40dbo.ca.gov%7Ce2673837ec6f42fce84508d7d114ed59%7Cd6910b1745b44b7bbb66cb7936fabafe%7C1%7C0%7C637207760136603083&amp;sdata=VR6CdqCvrBGkfC%2Bm%2B6Yj9emco9ldVY5BLWSiLpe3f4c%3D&amp;reserved=0)\n*    Call their Consumer Services Office at [(866) 275-2677](tel:(866) 275-2677) or [(916) 327-7585](tel:(916) 327-7585) \n*   Or email Ask.DBO@dbo.ca.gov\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C110" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -3242,13 +3242,13 @@
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>I am homeless and I may have come in contact with coronavirus. How can I self-isolate with nowhere to go and services closing down?</v>
+        <v>Can I get child care during the stay home order?</v>
       </c>
       <c r="B111" t="str">
-        <v>A motel or hotel room may be available for you and your family. Contact your local homeless [continuum of care](https://www.bcsh.ca.gov/hcfc/documents/coc_poc.pdf) to connect you to this service.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>[Child care options](https://covid19.ca.gov/childcare/) are available if you work at an [essential job](https://covid19.ca.gov/essential-workforce/) or a permitted job in the [current roadmap stage](https://covid19.ca.gov/roadmap/). If you are not working at a job like this, it is important to keep children at home. \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C111" t="str">
-        <v>https://covid19.ca.gov/housing-and-homelessness/</v>
+        <v>https://covid19.ca.gov/get-financial-help/</v>
       </c>
       <c r="D111" t="str">
         <v xml:space="preserve"> </v>
@@ -3268,10 +3268,10 @@
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>Will there be a rent freeze or waiver for renters? Are evictions allowed during the stay at home order?</v>
+        <v>I am homeless and I may have come in contact with coronavirus. How can I self-isolate with nowhere to go and services closing down?</v>
       </c>
       <c r="B112" t="str">
-        <v>There is an [order](https://www.gov.ca.gov/2020/03/16/governor-newsom-issues-executive-order-to-protect-renters-and-homeowners-during-covid-19-pandemic/) in place to halt evictions and protect renters. If you are financially affected by COVID-19 and [can’t pay your full rent](https://bcsh.ca.gov/coronavirus19/graphic_rent.pdf), let your landlord know in writing within seven days of the rent due date. Save documentation as proof. The order does not relieve you from the obligation to pay rent. It also does not restrict the landlord from recovering rent that is due.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>A motel or hotel room may be available for you and your family. Contact your local homeless [continuum of care](https://www.bcsh.ca.gov/hcfc/documents/coc_poc.pdf) to connect you to this service.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C112" t="str">
         <v>https://covid19.ca.gov/housing-and-homelessness/</v>
@@ -3294,10 +3294,10 @@
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>Can landlords delay their payments while their tenants cannot pay rent?</v>
+        <v>Will there be a rent freeze or waiver for renters? Are evictions allowed during the stay at home order?</v>
       </c>
       <c r="B113" t="str">
-        <v>Yes, there are protections in effect through September 30, 2020 for landlords. The [order](https://www.gov.ca.gov/2020/03/16/governor-newsom-issues-executive-order-to-protect-renters-and-homeowners-during-covid-19-pandemic/) requests lenders to halt foreclosures and related evictions during this time. Property owners should contact their financial institutions.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>There is an [order](https://www.gov.ca.gov/2020/06/30/governor-newsom-signs-executive-order-on-actions-in-response-to-covid-19-6-30-20/) in place to halt evictions and protect renters. If you are financially affected by COVID-19 and [can’t pay your full rent](https://bcsh.ca.gov/coronavirus19/graphic_rent.pdf), let your landlord know in writing within seven days of the rent due date. Save documentation as proof. The order does not relieve you from the obligation to pay rent. It also does not restrict the landlord from recovering rent that is due.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C113" t="str">
         <v>https://covid19.ca.gov/housing-and-homelessness/</v>
@@ -3320,10 +3320,10 @@
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>How do I get mortgage relief and/or forbearance?</v>
+        <v>Can landlords delay their payments while their tenants cannot pay rent?</v>
       </c>
       <c r="B114" t="str">
-        <v>You should contact and work directly with your mortgage servicer to learn about and apply for available relief. Please note that financial institutions and their servicers are experiencing high volumes of inquiries.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>Yes, there are protections in effect through September 30, 2020 for landlords. The [order](https://www.gov.ca.gov/2020/03/16/governor-newsom-issues-executive-order-to-protect-renters-and-homeowners-during-covid-19-pandemic/) requests lenders to halt foreclosures and related evictions during this time. Property owners should contact their financial institutions.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C114" t="str">
         <v>https://covid19.ca.gov/housing-and-homelessness/</v>
@@ -3346,10 +3346,10 @@
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>How long will the forbearance last?</v>
+        <v>How do I get mortgage relief and/or forbearance?</v>
       </c>
       <c r="B115" t="str">
-        <v>The terms of a forbearance will be agreed to between you and your mortgage service. Financial institutions will confirm approval of and terms of the forbearance program.\n\nMore info: [Housing and Homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>You should contact and work directly with your mortgage servicer to learn about and apply for available relief. Please note that financial institutions and their servicers are experiencing high volumes of inquiries.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C115" t="str">
         <v>https://covid19.ca.gov/housing-and-homelessness/</v>
@@ -3372,13 +3372,13 @@
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>What if a provider says they have availability on MyChildCare.ca.gov but when I connect with them they have no space?</v>
+        <v>How long will the forbearance last?</v>
       </c>
       <c r="B116" t="str">
-        <v>The information on [MyChildCare.ca.gov](http://mychildcare.ca.gov/) will be updated twice each week but it is possible that vacancies are filled between updates. Contact your [local childcare resource and referral agency](http://rrnetwork.org/family-services/find-child-care) to find more vacancies. \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
+        <v>The terms of a forbearance will be agreed to between you and your mortgage service. Financial institutions will confirm approval of and terms of the forbearance program.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C116" t="str">
-        <v>https://covid19.ca.gov/childcare/</v>
+        <v>https://covid19.ca.gov/housing-and-homelessness/</v>
       </c>
       <c r="D116" t="str">
         <v xml:space="preserve"> </v>
@@ -3398,10 +3398,10 @@
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>How can I find out more about the provider listed in MyChildCare.ca.gov?</v>
+        <v>What if a provider says they have availability on MyChildCare.ca.gov but when I connect with them they have no space?</v>
       </c>
       <c r="B117" t="str">
-        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) includes each provider’s facility/license number. This number can be searched at [CDSS Community Care Licensing Database](https://www.ccld.dss.ca.gov/carefacilitysearch/) to find more information about the provider, like information on inspections and complaints.  \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
+        <v>The information on [MyChildCare.ca.gov](http://mychildcare.ca.gov/) will be updated twice each week but it is possible that vacancies are filled between updates. Contact your [local childcare resource and referral agency](http://rrnetwork.org/family-services/find-child-care) to find more vacancies. \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
       </c>
       <c r="C117" t="str">
         <v>https://covid19.ca.gov/childcare/</v>
@@ -3424,10 +3424,10 @@
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>How can I find help paying for childcare?</v>
+        <v>How can I find out more about the provider listed in MyChildCare.ca.gov?</v>
       </c>
       <c r="B118" t="str">
-        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) provides information on all licensed center-based and family childcare homes. This includes both private-pay and subsidized childcare. Children of essential workers are now eligible to enroll in subsidized emergency childcare through June 30, 2020, or 60 calendar days after the date of the child’s enrollment, whichever is longer. This is subject to capacity and eligibility requirements. Your [local childcare resource and referral agency](https://rrnetwork.org/index.php?p=family-services/find-child-care) can answer more questions about childcare subsidies.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
+        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) includes each provider’s facility/license number. This number can be searched at [CDSS Community Care Licensing Database](https://www.ccld.dss.ca.gov/carefacilitysearch/) to find more information about the provider, like information on inspections and complaints.  \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
       </c>
       <c r="C118" t="str">
         <v>https://covid19.ca.gov/childcare/</v>
@@ -3450,10 +3450,10 @@
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>Can I get childcare during the stay home order?</v>
+        <v>How can I find help paying for childcare?</v>
       </c>
       <c r="B119" t="str">
-        <v>Yes, all childcare facilities can open with necessary modifications.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
+        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) provides information on all licensed center-based and family childcare homes. This includes both private-pay and subsidized childcare. Children of essential workers are now eligible to enroll in subsidized emergency childcare through June 30, 2020, or 60 calendar days after the date of the child’s enrollment, whichever is longer. This is subject to capacity and eligibility requirements. Your [local childcare resource and referral agency](https://rrnetwork.org/index.php?p=family-services/find-child-care) can answer more questions about childcare subsidies.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
       </c>
       <c r="C119" t="str">
         <v>https://covid19.ca.gov/childcare/</v>
@@ -3476,10 +3476,10 @@
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>Can my babysitter still come to the house?</v>
+        <v>Can I get childcare during the stay home order?</v>
       </c>
       <c r="B120" t="str">
-        <v>Yes, a childcare worker can come to your home if necessary and should practice basic prevention guidelines (like handwashing for at least 20 seconds, physical distancing, and staying home if feeling ill).\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
+        <v>Yes, all childcare facilities can open with necessary modifications.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
       </c>
       <c r="C120" t="str">
         <v>https://covid19.ca.gov/childcare/</v>
@@ -3502,13 +3502,13 @@
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>County websites:</v>
+        <v>Can my babysitter still come to the house?</v>
       </c>
       <c r="B121" t="str">
-        <v>*   [Alameda County](http://www.acphd.org/2019-ncov.aspx)\n*   [Alpine County](http://alpinecountyca.gov/Index.aspx?NID=516)\n*   [Amador County](https://www.amadorgov.org/services/covid-19)\n*   [Butte County](https://www.buttecounty.net/publichealth)\n*   [Calaveras County](https://covid19.calaverasgov.us/)\n*   [Colusa County](https://www.countyofcolusa.org/99/Public-Health)\n*   [Contra Costa County](https://www.coronavirus.cchealth.org/)\n*   [Del Norte County](http://www.co.del-norte.ca.us/departments/health-human-services/public-health)\n*   [El Dorado County](https://www.edcgov.us/Government/hhsa/Pages/EDCCOVID-19.aspx)\n*   [Fresno County](https://www.co.fresno.ca.us/departments/public-health/covid-19)\n*   [Glenn County](https://www.countyofglenn.net/dept/health-human-services/public-health/covid-19)\n*   [Humboldt County](https://humboldtgov.org/2018/Humboldt-Health-Alert)\n*   [Imperial County](http://www.icphd.org/health-information-and-resources/healthy-facts/covid-19/)\n*   [Inyo County](https://www.inyocounty.us/coronavirus-covid-19-response)\n*   [Kern County](https://kernpublichealth.com/2019-novel-coronavirus/)\n*   [Kings County](https://www.countyofkings.com/departments/health-welfare/public-health/coronavirus-disease-2019-covid-19/-fsiteid-1)\n*   [Lake County](http://health.co.lake.ca.us/Coronavirus.htm)\n*   [Lassen County](http://www.co.lassen.ca.us/)\n*   [Los Angeles County](http://publichealth.lacounty.gov/media/Coronavirus/)\n*   [Madera County](https://www.maderacounty.com/government/public-health/health-updates/corona-virus)\n*   [Marin County](https://coronavirus.marinhhs.org/)\n*   [Mariposa County](http://www.mariposacounty.org/1592/COVID-19-Information)\n*   [Mendocino County](https://www.mendocinocounty.org/community/novel-coronavirus)\n*   [Merced County](https://www.co.merced.ca.us/3350/Coronavirus-Disease-2019)\n*   [Modoc County](http://www.co.modoc.ca.us/)\n*   [Mono County](https://coronavirus.monocounty.ca.gov/)\n*   [Monterey County](https://www.co.monterey.ca.us/government/departments-a-h/health/diseases/2019-novel-coronavirus-covid-19)\n*   [Napa County](https://www.countyofnapa.org/2739/Coronavirus)\n*   [Nevada County](https://www.mynevadacounty.com/2924/Coronavirus)\n*   [Orange County](https://www.ochealthinfo.com/phs/about/epidasmt/epi/dip/prevention/novel_coronavirus)\n*   [Placer County](https://www.placer.ca.gov/coronavirus)\n*   [Plumas County](https://www.plumascounty.us/2669/Novel-Coronavirus-2019-COVID-19)\n*   [Riverside County](https://www.rivcoph.org/coronavirus)\n*   [Sacramento County](https://dhs.saccounty.net/PUB/Pages/PUB-Home.aspx)\n*   [San Benito County](https://hhsa.cosb.us/publichealth/communicable-disease/coronavirus/)\n*   [San Bernardino County](http://wp.sbcounty.gov/dph/coronavirus/)\n*   [San Diego County](https://www.sandiegocounty.gov/coronavirus.html)\n*   [San Francisco City and County](https://sf.gov/topics/coronavirus-covid-19)\n*   [San Joaquin County](https://www.sjgov.org/covid19/)\n*   [San Luis Obispo County](https://www.emergencyslo.org/en/covid19.aspx)\n*   [San Mateo County](https://www.smchealth.org/coronavirus)\n*   [Santa Barbara County](https://publichealthsbc.org/)\n*   [Santa Clara County](https://www.sccgov.org/sites/phd/DiseaseInformation/novel-coronavirus/Pages/home.aspx)\n*   [Santa Cruz County](https://www.santacruzhealth.org/HSAHome/HSADivisions/PublicHealth/CommunicableDiseaseControl/Coronavirus.aspx)\n*   [Shasta County](https://www.co.shasta.ca.us/index/hhsa/health-safety/current-heath-concerns/coronavirus)\n*   [Sierra County](http://sierracounty.ca.gov/582/Coronavirus-COVID-19)\n*   [Siskiyou County](https://www.co.siskiyou.ca.us/publichealth/page/coronavirus-covid-19-what-siskiyou-county-residents-need-know)\n*   [Solano County](http://www.solanocounty.com/depts/ph/ncov.asp)\n*   [Sonoma County](https://socoemergency.org/emergency/novel-coronavirus/)\n*   [Stanislaus County](http://schsa.org/publichealth/pages/corona-virus/)\n*   [Sutter County](https://www.suttercounty.org/doc/government/depts/cao/em/coronavirus)\n*   [Tehama County](https://www.tehamacohealthservices.net/services/communicable-diseases/#current-events)\n*   [Trinity County](https://www.trinitycounty.org/)\n*   [Tulare County](https://tchhsa.org/eng/index.cfm/public-health/covid-19-updates-novel-coronavirus/)\n*   [Tuolumne County](https://www.tuolumnecounty.ca.gov/250/Public-Health)\n*   [Ventura County](https://www.vcemergency.com/)\n*   [Yolo County](https://www.yolocounty.org/health-human-services/adults/communicable-disease-investigation-and-control/novel-coronavirus-2019)\n*   [Yuba County](https://www.yuba.org/coronavirus/)\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>Yes, a childcare worker can come to your home if necessary and should practice basic prevention guidelines (like handwashing for at least 20 seconds, physical distancing, and staying home if feeling ill).\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
       </c>
       <c r="C121" t="str">
-        <v>https://covid19.ca.gov/state-local-resources/</v>
+        <v>https://covid19.ca.gov/childcare/</v>
       </c>
       <c r="D121" t="str">
         <v xml:space="preserve"> </v>
@@ -3528,10 +3528,10 @@
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>What are the restrictions in my area?</v>
+        <v>County websites:</v>
       </c>
       <c r="B122" t="str">
-        <v>While each county may have different restrictions, it is important to stay home as much as possible. If you do go out, stay 6 feet away from others who are not in your household and wear a cloth mask. Your actions save lives.\n\nSee what [industries are open or closed](https://covid19.ca.gov/roadmap-counties/#track-data) in your county.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>*   [Alameda County](http://www.acphd.org/2019-ncov.aspx)\n*   [Alpine County](http://alpinecountyca.gov/Index.aspx?NID=516)\n*   [Amador County](https://www.amadorgov.org/services/covid-19)\n*   [Butte County](https://www.buttecounty.net/publichealth)\n*   [Calaveras County](https://covid19.calaverasgov.us/)\n*   [Colusa County](https://www.countyofcolusa.org/99/Public-Health)\n*   [Contra Costa County](https://www.coronavirus.cchealth.org/)\n*   [Del Norte County](http://www.co.del-norte.ca.us/departments/health-human-services/public-health)\n*   [El Dorado County](https://www.edcgov.us/Government/hhsa/Pages/EDCCOVID-19.aspx)\n*   [Fresno County](https://www.co.fresno.ca.us/departments/public-health/covid-19)\n*   [Glenn County](https://www.countyofglenn.net/dept/health-human-services/public-health/covid-19)\n*   [Humboldt County](https://humboldtgov.org/2018/Humboldt-Health-Alert)\n*   [Imperial County](http://www.icphd.org/health-information-and-resources/healthy-facts/covid-19/)\n*   [Inyo County](https://www.inyocounty.us/coronavirus-covid-19-response)\n*   [Kern County](https://kernpublichealth.com/2019-novel-coronavirus/)\n*   [Kings County](https://www.countyofkings.com/departments/health-welfare/public-health/coronavirus-disease-2019-covid-19/-fsiteid-1)\n*   [Lake County](http://health.co.lake.ca.us/Coronavirus.htm)\n*   [Lassen County](http://www.co.lassen.ca.us/)\n*   [Los Angeles County](http://publichealth.lacounty.gov/media/Coronavirus/)\n*   [Madera County](https://www.maderacounty.com/government/public-health/health-updates/corona-virus)\n*   [Marin County](https://coronavirus.marinhhs.org/)\n*   [Mariposa County](http://www.mariposacounty.org/1592/COVID-19-Information)\n*   [Mendocino County](https://www.mendocinocounty.org/community/novel-coronavirus)\n*   [Merced County](https://www.co.merced.ca.us/3350/Coronavirus-Disease-2019)\n*   [Modoc County](http://www.co.modoc.ca.us/)\n*   [Mono County](https://coronavirus.monocounty.ca.gov/)\n*   [Monterey County](https://www.co.monterey.ca.us/government/departments-a-h/health/diseases/2019-novel-coronavirus-covid-19)\n*   [Napa County](https://www.countyofnapa.org/2739/Coronavirus)\n*   [Nevada County](https://www.mynevadacounty.com/2924/Coronavirus)\n*   [Orange County](https://www.ochealthinfo.com/phs/about/epidasmt/epi/dip/prevention/novel_coronavirus)\n*   [Placer County](https://www.placer.ca.gov/coronavirus)\n*   [Plumas County](https://www.plumascounty.us/2669/Novel-Coronavirus-2019-COVID-19)\n*   [Riverside County](https://www.rivcoph.org/coronavirus)\n*   [Sacramento County](https://dhs.saccounty.net/PUB/Pages/PUB-Home.aspx)\n*   [San Benito County](https://hhsa.cosb.us/publichealth/communicable-disease/coronavirus/)\n*   [San Bernardino County](http://wp.sbcounty.gov/dph/coronavirus/)\n*   [San Diego County](https://www.sandiegocounty.gov/coronavirus.html)\n*   [San Francisco City and County](https://sf.gov/topics/coronavirus-covid-19)\n*   [San Joaquin County](https://www.sjgov.org/covid19/)\n*   [San Luis Obispo County](https://www.emergencyslo.org/en/covid19.aspx)\n*   [San Mateo County](https://www.smchealth.org/coronavirus)\n*   [Santa Barbara County](https://publichealthsbc.org/)\n*   [Santa Clara County](https://www.sccgov.org/sites/phd/DiseaseInformation/novel-coronavirus/Pages/home.aspx)\n*   [Santa Cruz County](https://www.santacruzhealth.org/HSAHome/HSADivisions/PublicHealth/CommunicableDiseaseControl/Coronavirus.aspx)\n*   [Shasta County](https://www.co.shasta.ca.us/index/hhsa/health-safety/current-heath-concerns/coronavirus)\n*   [Sierra County](http://sierracounty.ca.gov/582/Coronavirus-COVID-19)\n*   [Siskiyou County](https://www.co.siskiyou.ca.us/publichealth/page/coronavirus-covid-19-what-siskiyou-county-residents-need-know)\n*   [Solano County](http://www.solanocounty.com/depts/ph/ncov.asp)\n*   [Sonoma County](https://socoemergency.org/emergency/novel-coronavirus/)\n*   [Stanislaus County](http://schsa.org/publichealth/pages/corona-virus/)\n*   [Sutter County](https://www.suttercounty.org/doc/government/depts/cao/em/coronavirus)\n*   [Tehama County](https://www.tehamacohealthservices.net/services/communicable-diseases/#current-events)\n*   [Trinity County](https://www.trinitycounty.org/)\n*   [Tulare County](https://tchhsa.org/eng/index.cfm/public-health/covid-19-updates-novel-coronavirus/)\n*   [Tuolumne County](https://www.tuolumnecounty.ca.gov/250/Public-Health)\n*   [Ventura County](https://www.vcemergency.com/)\n*   [Yolo County](https://www.yolocounty.org/health-human-services/adults/communicable-disease-investigation-and-control/novel-coronavirus-2019)\n*   [Yuba County](https://www.yuba.org/coronavirus/)\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C122" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3554,10 +3554,10 @@
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>How are we helping the homeless?</v>
+        <v>What are the restrictions in my area?</v>
       </c>
       <c r="B123" t="str">
-        <v>Each county and local government in California has [increased resources](https://covid19.ca.gov/housing-and-homelessness/#top) to protect people experiencing homelessness during COVID-19. [Financial protections](https://covid19.ca.gov/housing-and-homelessness/#top) were added to prevent others from losing their homes during the outbreak.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>While each county may have different restrictions, it is important to stay home as much as possible. If you do go out, stay 6 feet away from others who are not in your household and wear a mask or face covering. Your actions save lives.\n\nSee what [industries are open or closed](https://covid19.ca.gov/roadmap-counties/#track-data) in your county.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C123" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3580,10 +3580,10 @@
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>How is the state protecting incarcerated people in California?</v>
+        <v>How are we helping the homeless?</v>
       </c>
       <c r="B124" t="str">
-        <v>[California Department of Corrections and Rehabilitation (CDCR)](https://www.cdcr.ca.gov/covid19/) is dedicated to the safety of everyone who lives in, works in, and visits state prisons. CDCR has given all staff and inmates 2 reusable cloth masks to wear while moving between cells, dorms, meetings with others, or health care appointments. CDCR also requires ongoing testing for all staff working in adult institutions, suspended non-essential transfer of inmates, and suspended volunteer services and in-person visiting.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>Each county and local government in California has [increased resources](https://covid19.ca.gov/housing-and-homelessness/#top) to protect people experiencing homelessness during COVID-19. [Financial protections](https://covid19.ca.gov/housing-and-homelessness/#top) were added to prevent others from losing their homes during the outbreak.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C124" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3606,10 +3606,10 @@
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v>Who can I contact about my child custody order and child visitation rights?</v>
+        <v>How is the state protecting incarcerated people in California?</v>
       </c>
       <c r="B125" t="str">
-        <v>Court operations vary from county to county. You can use the [California Courts Self-Help Center](https://www.courts.ca.gov/selfhelp.htm) or reach out to your [local government office](https://www.courts.ca.gov/find-my-court.htm?query=browse_courts) for more information. \n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>[California Department of Corrections and Rehabilitation (CDCR)](https://www.cdcr.ca.gov/covid19/) is dedicated to the safety of everyone who lives in, works in, and visits state prisons. CDCR has given all staff and inmates 2 reusable cloth masks to wear while moving between cells, dorms, meetings with others, or health care appointments. CDCR also requires ongoing testing for all staff working in adult institutions, suspended non-essential transfer of inmates, and suspended volunteer services and in-person visiting.\n\nSee [CDCR’s COVID-19 Response Efforts](https://www.cdcr.ca.gov/covid19/covid-19-response-efforts/) for more detailed information.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C125" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3632,10 +3632,10 @@
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v>Do I have to report to jury duty if summoned?</v>
+        <v>Who can I contact about my child custody order and child visitation rights?</v>
       </c>
       <c r="B126" t="str">
-        <v>Court operations vary from county to county. You can use the [California Courts Self-Help Center](https://www.courts.ca.gov/selfhelp.htm) or reach out to your [local government office](https://www.courts.ca.gov/find-my-court.htm?query=browse_courts) for more information about jury duty.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)&lt;!-- jury duty, summons, courts, court, court operations--&gt;</v>
+        <v>Court operations vary from county to county. You can use the [California Courts Self-Help Center](https://www.courts.ca.gov/selfhelp.htm) or reach out to your [local government office](https://www.courts.ca.gov/find-my-court.htm?query=browse_courts) for more information. \n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C126" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3658,13 +3658,13 @@
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v>When is the disaster relief assistance available?</v>
+        <v>Do I have to report to jury duty if summoned?</v>
       </c>
       <c r="B127" t="str">
-        <v>Individuals may begin applying on May 18, 2020. Assistance will be available until the funding is spent or until June 30, 2020, at the latest. Applicants will be considered on a first-come, first-served basis. Applicants may only apply with the nonprofit organization(s) in their county of residency.\n\n**Please note:**\n\n*   Funding is limited, and disaster relief application services and assistance are not guaranteed.\n*   Nonprofit organizations will not be assisting individuals before May 18. Individuals _should not_ contact them ahead of time regarding disaster relief assistance.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>Court operations vary from county to county. You can use the [California Courts Self-Help Center](https://www.courts.ca.gov/selfhelp.htm) or reach out to your [local government office](https://www.courts.ca.gov/find-my-court.htm?query=browse_courts) for more information about jury duty.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)&lt;!-- jury duty, summons, courts, court, court operations--&gt;</v>
       </c>
       <c r="C127" t="str">
-        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
+        <v>https://covid19.ca.gov/state-local-resources/</v>
       </c>
       <c r="D127" t="str">
         <v xml:space="preserve"> </v>
@@ -3684,10 +3684,10 @@
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v>Who is eligible for this disaster relief assistance?</v>
+        <v>When is the disaster relief assistance available?</v>
       </c>
       <c r="B128" t="str">
-        <v>Eligible individuals must be able to provide information that they:\n\n*   Are an undocumented adult (person over the age of 18)\n*   Are not eligible for federal COVID-19 assistance, like the CARES Act stimulus payments or pandemic unemployment benefits, and\n*   Have experienced hardship as a result of COVID-19.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>Individuals may begin applying on May 18, 2020. Assistance will be available until the funding is spent or until June 30, 2020, at the latest. Applicants will be considered on a first-come, first-served basis. Applicants may only apply with the nonprofit organization(s) in their county of residency.\n\n**Please note:**\n\n*   Funding is limited, and disaster relief application services and assistance are not guaranteed.\n*   Nonprofit organizations will not be assisting individuals before May 18. Individuals _should not_ contact them ahead of time regarding disaster relief assistance.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C128" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3710,10 +3710,10 @@
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v>Can getting this assistance affect my ability to get a green card or to become a U.S. Citizen? Will receiving it make me a public charge?</v>
+        <v>Who is eligible for this disaster relief assistance?</v>
       </c>
       <c r="B129" t="str">
-        <v>This disaster relief assistance is not means-tested and is one-time assistance. The federal government does not list this assistance as a public benefit for a public charge consideration. However, USCIS has not issued specific guidance related to this assistance.\n\nIf you have questions about your immigration status and this program, please consult an attorney. A list of free and low-cost immigration services providers is available in the [Guide for Immigrant Californians (PDF)](https://files.covid19.ca.gov/pdf/COVID_immigrant_guidance--en.pdf).\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>Eligible individuals must be able to provide information that they:\n\n*   Are an undocumented adult (person over the age of 18)\n*   Are not eligible for federal COVID-19 assistance, like the CARES Act stimulus payments or pandemic unemployment benefits, and\n*   Have experienced hardship as a result of COVID-19.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C129" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3736,10 +3736,10 @@
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v>Is the personal information I provide to the nonprofits protected?</v>
+        <v>Can getting this assistance affect my ability to get a green card or to become a U.S. Citizen? Will receiving it make me a public charge?</v>
       </c>
       <c r="B130" t="str">
-        <v>Your information is only used to confirm eligibility and provide the assistance. No personal information (like name or address) will be given to any government agency. Only general information like age, gender, and preferred language will be shared with the State of California.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>This disaster relief assistance is not means-tested and is one-time assistance. The federal government does not list this assistance as a public benefit for a public charge consideration. However, USCIS has not issued specific guidance related to this assistance.\n\nIf you have questions about your immigration status and this program, please consult an attorney. A list of free and low-cost immigration services providers is available in the [Guide for Immigrant Californians (PDF)](https://files.covid19.ca.gov/pdf/COVID_immigrant_guidance--en.pdf).\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C130" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3762,10 +3762,10 @@
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v>How do I apply?</v>
+        <v>Is the personal information I provide to the nonprofits protected?</v>
       </c>
       <c r="B131" t="str">
-        <v>The California Department of Social Services (CDSS) has identified non-profit where you can apply for disaster assistance. Find the [nonprofit where you can apply in your area](https://cdss.ca.gov/inforesources/immigration/covid-19-drai).\n\nApply _no sooner than May 18, and only to the organization in your area._ They will assist you with applying, confirm your eligibility, and deliver a payment card if you are approved. Applications will be considered on a first-come, first-served basis.\n\nFunding is limited, and disaster relief application services and assistance are not guaranteed.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>Your information is only used to confirm eligibility and provide the assistance. No personal information (like name or address) will be given to any government agency. Only general information like age, gender, and preferred language will be shared with the State of California.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C131" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3788,10 +3788,10 @@
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v>How many people in a household can receive this assistance?</v>
+        <v>How do I apply?</v>
       </c>
       <c r="B132" t="str">
-        <v>A maximum of two adults per household can qualify for this assistance, for a total of $1,000 per household. A household is defined as individuals who live, shop, and prepare meals together.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>The California Department of Social Services (CDSS) has identified non-profit where you can apply for disaster assistance. Find the [nonprofit where you can apply in your area](https://cdss.ca.gov/inforesources/immigration/covid-19-drai).\n\nApply _no sooner than May 18, and only to the organization in your area._ They will assist you with applying, confirm your eligibility, and deliver a payment card if you are approved. Applications will be considered on a first-come, first-served basis.\n\nFunding is limited, and disaster relief application services and assistance are not guaranteed.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C132" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3814,10 +3814,10 @@
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v>How do eligible individuals receive this assistance?</v>
+        <v>How many people in a household can receive this assistance?</v>
       </c>
       <c r="B133" t="str">
-        <v>You will get a payment card either in person or through the mail. The organization in your area can give you more information.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>A maximum of two adults per household can qualify for this assistance, for a total of $1,000 per household. A household is defined as individuals who live, shop, and prepare meals together.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C133" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3840,10 +3840,10 @@
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v>How long do I have to apply?</v>
+        <v>How do eligible individuals receive this assistance?</v>
       </c>
       <c r="B134" t="str">
-        <v>Payments will be distributed beginning on May 18, 2020. They will continue until the $75 million in funding is spent, or until June 30, 2020 at the latest. We expect that this disaster relief assistance will run out very quickly. Apply as soon as you can, but not before May 18.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>You will get a payment card either in person or through the mail. The organization in your area can give you more information.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C134" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3866,10 +3866,10 @@
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v>If I am unable to apply for this program, are there other organizations that can help me?</v>
+        <v>How long do I have to apply?</v>
       </c>
       <c r="B135" t="str">
-        <v>Yes. The California Immigrant Resilience Fund is raising $50 million to provide cash assistance to undocumented Californians who are ineligible for other COVID-19 programs. Visit the [California Immigrant Resilience Fund](http://www.immigrantfundca.org) website to see if you can benefit from this program.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>Payments will be distributed beginning on May 18, 2020. They will continue until the $75 million in funding is spent, or until June 30, 2020 at the latest. We expect that this disaster relief assistance will run out very quickly. Apply as soon as you can, but not before May 18.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C135" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3892,10 +3892,10 @@
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v>What other government programs may I be eligible for during the COVID-19 pandemic?</v>
+        <v>If I am unable to apply for this program, are there other organizations that can help me?</v>
       </c>
       <c r="B136" t="str">
-        <v>Check the [Guide for Immigrant Californians (PDF)](/wp-content/uploads/2020/04/LISTOS_COVID_19_immigrant_guidance_EN_dAf.pdf). It has information about jobs, wages, benefits, and small business and housing support.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>Yes. The California Immigrant Resilience Fund is raising $50 million to provide cash assistance to undocumented Californians who are ineligible for other COVID-19 programs. Visit the [California Immigrant Resilience Fund](http://www.immigrantfundca.org) website to see if you can benefit from this program.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C136" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3918,13 +3918,13 @@
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v>Youth and Teens</v>
+        <v>What other government programs may I be eligible for during the COVID-19 pandemic?</v>
       </c>
       <c r="B137" t="str">
-        <v>*   [California Youth Crisis Line](https://calyouth.org/cycl/)**:** Youth ages 12-24 can call or text [800-843-5200](tel:800-843-5200) or [chat online](https://m2.icarol.com/ConsumerRegistration.aspx?org=53141&amp;pid=326&amp;cc=en-US) for 24/7 crisis support.\n*   [TEEN LINE](https://teenlineonline.org/talk-now/): Teens can talk to another teen by texting “TEEN” to [839863](sms:839863) from 6pm – 9pm, or call [800-852-8336](tel:800-852-8336) from 6pm – 10pm.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>Check the [Guide for Immigrant Californians (PDF)](/wp-content/uploads/2020/04/LISTOS_COVID_19_immigrant_guidance_EN_dAf.pdf). It has information about jobs, wages, benefits, and small business and housing support.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C137" t="str">
-        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
+        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
       </c>
       <c r="D137" t="str">
         <v xml:space="preserve"> </v>
@@ -3944,10 +3944,10 @@
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v>Veterans</v>
+        <v>Youth and Teens</v>
       </c>
       <c r="B138" t="str">
-        <v>[Veterans Crisis Line](https://www.veteranscrisisline.net): Call [800-273-8255](tel:800-273-8255) and Press 1 or text [838255](sms:838255) for 24/7 support.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>*   [California Youth Crisis Line](https://calyouth.org/cycl/)**:** Youth ages 12-24 can call or text [800-843-5200](tel:800-843-5200) or [chat online](https://m2.icarol.com/ConsumerRegistration.aspx?org=53141&amp;pid=326&amp;cc=en-US) for 24/7 crisis support.\n*   [TEEN LINE](https://teenlineonline.org/talk-now/): Teens can talk to another teen by texting “TEEN” to [839863](sms:839863) from 6pm – 9pm, or call [800-852-8336](tel:800-852-8336) from 6pm – 10pm.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C138" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -3970,10 +3970,10 @@
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>First Responders and Law Enforcement</v>
+        <v>Veterans</v>
       </c>
       <c r="B139" t="str">
-        <v>*   [Fire/EMS helpline](https://www.nvfc.org/fireems-helpline/): Call [888-731-FIRE](tel:888-731-FIRE) to get 24/7 help for a variety of behavioral health issues.\n*   [COPLINE](https://www.copline.org/): Call [800-267-5463](tel:800-267-5463) to find support 24/7 for law enforcement officers.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>[Veterans Crisis Line](https://www.veteranscrisisline.net): Call [800-273-8255](tel:800-273-8255) and Press 1 or text [838255](sms:838255) for 24/7 support.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C139" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -3996,10 +3996,10 @@
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>Older Californians</v>
+        <v>First Responders and Law Enforcement</v>
       </c>
       <c r="B140" t="str">
-        <v>*   [Friendship Line](https://www.ioaging.org/services/all-inclusive-health-care/friendship-line): Call [888-670-1360](tel:888-670-1360) for 24/7 support if you are 60 years or older, or an adult living with disabilities.  \n*   California Aging and Adult Information Line: Call [800-510-2020](tel:800-510-2020) for help finding local assistance. \n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>*   [Fire/EMS helpline](https://www.nvfc.org/fireems-helpline/): Call [888-731-FIRE](tel:888-731-FIRE) to get 24/7 help for a variety of behavioral health issues.\n*   [COPLINE](https://www.copline.org/): Call [800-267-5463](tel:800-267-5463) to find support 24/7 for law enforcement officers.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C140" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -4022,10 +4022,10 @@
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>Deaf and Hard of Hearing Individuals</v>
+        <v>Older Californians</v>
       </c>
       <c r="B141" t="str">
-        <v>[National Suicide Prevention Deaf and Hard of Hearing Hotline](https://suicidepreventionlifeline.org/help-yourself/for-deaf-hard-of-hearing/): Access 24/7 video relay service by dialing [800-273-8255](tel:800-273-8255) (TTY [800-799-4889](tel:800-799-4889)).\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>*   [Friendship Line](https://www.ioaging.org/services/all-inclusive-health-care/friendship-line): Call [888-670-1360](tel:888-670-1360) for 24/7 support if you are 60 years or older, or an adult living with disabilities.  \n*   California Aging and Adult Information Line: Call [800-510-2020](tel:800-510-2020) for help finding local assistance. \n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C141" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -4048,10 +4048,10 @@
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>Services for Substance Use Disorders</v>
+        <v>Deaf and Hard of Hearing Individuals</v>
       </c>
       <c r="B142" t="str">
-        <v>*   [SAMHSA National Helpline](https://www.samhsa.gov/find-help/national-helpline): Call [800-662-HELP](tel:1-800-662-4357) for 24/7 information and referrals in English and Spanish. \n*   [SAMHSA Treatment Locator](https://findtreatment.samhsa.gov)**:**  Find drug or alcohol treatment programs. \n*   [Local county access lines](https://gcc01.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.dhcs.ca.gov%2Findividuals%2FPages%2FSUD_County_Access_Lines.aspx&amp;data=02%7C01%7CJanne.Olson-Morgan%40osg.ca.gov%7C122307be91754d12e5dc08d7d984f958%7C265c2dcd2a6e43aab2e826421a8c8526%7C0%7C0%7C637217037446186621&amp;sdata=5sx4UdIlVkRL%2BEJR7FrpK0gYAn20yE71TyBDFIw1kJM%3D&amp;reserved=0): Find your local number for help seeking substance use disorder services.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>[National Suicide Prevention Deaf and Hard of Hearing Hotline](https://suicidepreventionlifeline.org/help-yourself/for-deaf-hard-of-hearing/): Access 24/7 video relay service by dialing [800-273-8255](tel:800-273-8255) (TTY [800-799-4889](tel:800-799-4889)).\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C142" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -4074,10 +4074,10 @@
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>LGBTQ Individuals</v>
+        <v>Services for Substance Use Disorders</v>
       </c>
       <c r="B143" t="str">
-        <v>*   [Trevor Project](https://www.thetrevorproject.org): Call [866-488-7386](tel:866-488-7386) or text START to [678678](sms:678678) for 24/7 information and suicide prevention resources for LGBTQ youth.\n*   [Lesbian, Gay, Bisexual and Transgender National Hotline](https://www.glbthotline.org/hotline.html): Call [800-273-8255](tel:800-273-8255) from 1pm – 9pm for support, information or help finding resources.\n*   [Victims of Crime Resource Center](https://1800victims.org/): Call or text [800-842-8467](tel:800-842-8467) or [chat online](https://1800victims.org/) for information about LGTBQ rights, legal protections, and local resources.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>*   [SAMHSA National Helpline](https://www.samhsa.gov/find-help/national-helpline): Call [800-662-HELP](tel:1-800-662-4357) for 24/7 information and referrals in English and Spanish. \n*   [SAMHSA Treatment Locator](https://findtreatment.samhsa.gov)**:**  Find drug or alcohol treatment programs. \n*   [Local county access lines](https://gcc01.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.dhcs.ca.gov%2Findividuals%2FPages%2FSUD_County_Access_Lines.aspx&amp;data=02%7C01%7CJanne.Olson-Morgan%40osg.ca.gov%7C122307be91754d12e5dc08d7d984f958%7C265c2dcd2a6e43aab2e826421a8c8526%7C0%7C0%7C637217037446186621&amp;sdata=5sx4UdIlVkRL%2BEJR7FrpK0gYAn20yE71TyBDFIw1kJM%3D&amp;reserved=0): Find your local number for help seeking substance use disorder services.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C143" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -4100,13 +4100,13 @@
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>What is a close contact?</v>
+        <v>LGBTQ Individuals</v>
       </c>
       <c r="B144" t="str">
-        <v>A close contact is someone who was within 6 feet of a person with COVID-19 for at least 15 minutes. This usually includes household members, intimate contacts, and caregivers, but can include others.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>*   [Trevor Project](https://www.thetrevorproject.org): Call [866-488-7386](tel:866-488-7386) or text START to [678678](sms:678678) for 24/7 information and suicide prevention resources for LGBTQ youth.\n*   [Lesbian, Gay, Bisexual and Transgender National Hotline](https://www.glbthotline.org/hotline.html): Call [800-273-8255](tel:800-273-8255) from 1pm – 9pm for support, information or help finding resources.\n*   [Victims of Crime Resource Center](https://1800victims.org/): Call or text [800-842-8467](tel:800-842-8467) or [chat online](https://1800victims.org/) for information about LGTBQ rights, legal protections, and local resources.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C144" t="str">
-        <v>https://covid19.ca.gov/contact-tracing/</v>
+        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
       </c>
       <c r="D144" t="str">
         <v xml:space="preserve"> </v>
@@ -4126,10 +4126,10 @@
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>Will contact tracers track my location?</v>
+        <v>What is a close contact?</v>
       </c>
       <c r="B145" t="str">
-        <v>California’s contact tracing program does not use any cell phone tracking technology. Someone from your local public health department will simply speak privately with you. All information is confidential and protected by California’s strict privacy laws. They may stay in touch to make sure your symptoms aren’t worsening.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>A close contact is someone who was within 6 feet of a person with COVID-19 for at least 15 minutes. This usually includes household members, intimate contacts, and caregivers, but can include others.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C145" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4152,10 +4152,10 @@
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>Is contact tracing help available in my language?</v>
+        <v>Will contact tracers track my location?</v>
       </c>
       <c r="B146" t="str">
-        <v>Your [local health department](https://covid19.ca.gov/state-local-resources/#top) can communicate with you in many different languages.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>California’s contact tracing program does not use any cell phone tracking technology. Someone from your local public health department will simply speak privately with you. All information is confidential and protected by California’s strict privacy laws. They may stay in touch to make sure your symptoms aren’t worsening.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C146" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4178,10 +4178,10 @@
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>Who should get tested?</v>
+        <v>Is contact tracing help available in my language?</v>
       </c>
       <c r="B147" t="str">
-        <v>You should get tested if you:\n\n*   Are a close contact of anyone who has or may have COVID-19, or\n*   Think you may have been exposed, or\n*   Are having [COVID-19 symptoms](https://covid19.ca.gov/symptoms-and-risks/). \n\nFind a [testing site in your area](https://covid19.ca.gov/testing-and-treatment/).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>Your [local health department](https://covid19.ca.gov/state-local-resources/#top) can communicate with you in many different languages.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C147" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4204,10 +4204,10 @@
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>How do I find a testing location?</v>
+        <v>Who should get tested?</v>
       </c>
       <c r="B148" t="str">
-        <v>To learn more about testing and care, visit the [Testing and treatment page](https://covid19.ca.gov/testing-and-treatment/). You can search for testing locations there using your zip code. \n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>You should get tested if you:\n\n*   Are a close contact of anyone who has or may have COVID-19, or\n*   Think you may have been exposed, or\n*   Are having [COVID-19 symptoms](https://covid19.ca.gov/symptoms-and-risks/). \n\nFind a [testing site in your area](https://covid19.ca.gov/testing-and-treatment/).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C148" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4230,10 +4230,10 @@
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v>What if I have COVID-19 symptoms and have not been contacted by the health department?</v>
+        <v>How do I find a testing location?</v>
       </c>
       <c r="B149" t="str">
-        <v>[Get tested](https://covid19.ca.gov/testing-and-treatment/) immediately, contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing, and [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) yourself while waiting for your test results.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>To learn more about testing and care, visit the [Testing and treatment page](https://covid19.ca.gov/testing-and-treatment/). You can search for testing locations there using your zip code. \n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C149" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4256,10 +4256,10 @@
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>What if I came in contact with someone who has COVID-19 symptoms, but my local health department is not aware of it?</v>
+        <v>What if I have COVID-19 symptoms and have not been contacted by the health department?</v>
       </c>
       <c r="B150" t="str">
-        <v>You should [get tested](https://covid19.ca.gov/testing-and-treatment/). Contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing, and [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) yourself while waiting for your test results.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>[Get tested](https://covid19.ca.gov/testing-and-treatment/) immediately, contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing, and [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) yourself until:\n\n*   at least 10 days have passed since symptoms started, **AND**\n*    your fever has been gone for 24 hours without the aid of medication, **AND** \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested. Read more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C150" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4282,10 +4282,10 @@
     </row>
     <row r="151">
       <c r="A151" t="str">
-        <v>How do I become a contact tracer?</v>
+        <v>What if I came in contact with someone who has COVID-19 symptoms, but my local health department is not aware of it?</v>
       </c>
       <c r="B151" t="str">
-        <v>The initial phase of California Connected, the state’s contact tracing program, will utilize existing resources and redirect state employees to begin contact tracing efforts. Offers of additional support from the private sector and qualified members of the public are appreciated, but contact tracers from outside state government may not be needed until a future phase. Thank you for wanting to share your expertise and resources with your fellow Californians.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>You should [get tested](https://covid19.ca.gov/testing-and-treatment/). Contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing, and [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) yourself while waiting for your test results.\n\n**If you tested positive but have no symptoms**, you should [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) at home for at least 10 days.\n\n**If you develop symptoms**, you should stay home until:\n\n*   at least 10 days have passed since symptoms started, **AND**\n*   your fever has been gone for 24 hours without the aid of medication, **AND** \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested.\n\n**If you had close contact with someone who tested positive but you tested negative**, you should still [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) at home for at least 14 days.\n\nRead more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C151" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4308,13 +4308,13 @@
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>County Monitoring List</v>
+        <v>How do I become a contact tracer?</v>
       </c>
       <c r="B152" t="str">
-        <v>*   Alameda\n*   Butte (on the list less than 3 days)\n*   Colusa\n*   Contra Costa\n*   Fresno\n*   Glenn\n*   Imperial\n*   Kern (on the list less than 3 days)\n*   Kings\n*   Los Angeles\n*   Madera\n*   Marin\n*   Merced\n*   Monterey\n*   Napa\n*   Orange\n*   Placer\n*   Riverside\n*   Sacramento\n*   San Benito\n*   San Bernardino\n*   San Diego\n*   San Francisco\n*   San Joaquin\n*   San Luis Obispo\n*   Santa Barbara\n*   Santa Clara\n*   Solano\n*   Sonoma\n*   Stanislaus\n*   Sutter\n*   Tulare\n*   Ventura\n*   Yolo\n*   Yuba\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>The initial phase of California Connected, the state’s contact tracing program, will utilize existing resources and redirect state employees to begin contact tracing efforts. Offers of additional support from the private sector and qualified members of the public are appreciated, but contact tracers from outside state government may not be needed until a future phase. Thank you for wanting to share your expertise and resources with your fellow Californians.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C152" t="str">
-        <v>https://covid19.ca.gov/roadmap-counties/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D152" t="str">
         <v xml:space="preserve"> </v>
@@ -4334,13 +4334,13 @@
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v>For attested counties not on Monitoring List</v>
+        <v>Is there extra sick leave available for workers who have COVID-19 symptoms or are waiting for test results?</v>
       </c>
       <c r="B153" t="str">
-        <v>*   [Industries open statewide](https://covid19.ca.gov/industry-guidance/)\n*   Dine-in restaurants (outdoors only)\n*   Wineries and tasting rooms (outdoors only)\n*   Family entertainment centers (outdoors only)\n*   Zoos and museums (outdoors only)\n*   Cardrooms (outdoors only)\n*   Casinos\n*   Gyms and fitness centers\n*   Hotels (for tourism and individual travel)\n*   Campgrounds and outdoor recreation\n*   Personal care services, like nail salons and body waxing\n*   Hair salons and barbershops\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>Yes. There are extra federal, state, and in some cases, local sick leaves available for people experiencing COVID-19 symptoms, seeking a medical diagnosis or in quarantine:\n\n*   **Federal paid sick leave:** Up to 80 hours under the Families First Coronavirus Response Act ([FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-employee-paid-leave)) for businesses with less than 500 workers. See [more information on FFCRA in its FAQs](https://www.dol.gov/agencies/whd/pandemic/ffcra-questions).\n*   **California COVID-19 supplemental paid sick leave:** Food businesses with more than 500 workers must give up to 80 hours of [paid sick leave](https://www.gov.ca.gov/wp-content/uploads/2020/04/4.16.20-EO-N-51-20.pdf).  See [more information on supplemental paid sick leave](https://www.dir.ca.gov/dlse/FAQ-for-PSL.html). \n*   **Local paid sick leave ordinances:** Certain local areas also have paid sick leave ordinances.  Consult with the local enforcement agency in your area.\n\nTo understand what resources may be available, see the side-by-side comparison of [COVID-19 sick leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) and [benefits for workers impacted by COVID-19](https://www.labor.ca.gov/coronavirus2019/#chart).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C153" t="str">
-        <v>https://covid19.ca.gov/roadmap-counties/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D153" t="str">
         <v xml:space="preserve"> </v>
@@ -4360,13 +4360,13 @@
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v>For counties on Monitoring List for 3 consecutive days</v>
+        <v>Can I return to work once my isolation or quarantine is over?</v>
       </c>
       <c r="B154" t="str">
-        <v>*   [Industries open statewide](https://covid19.ca.gov/industry-guidance/)\n*   Casinos\n*   Hotels (for tourism and individual travel)\n*   Campgrounds and outdoor recreation\n\nThe following industries must close indoor operations, but they may be modified to operate outside or by pick-up:\n\n*   Dine-in restaurants\n*   Wineries and tasting rooms\n*   Movie theaters \n*   Family entertainment centers (for example: bowling alleys, miniature golf, batting cages and arcades)\n*   Zoos and museums\n*   Cardrooms\n*   Gyms and fitness centers\n*   Personal care services, like nail salons and body waxing\n*   Places of worship and cultural ceremonies, like weddings and funerals\n*   Offices for non-critical infrastructure sectors\n*   Shopping malls \n\nNOTE: Imperial County is open to the essential workforce only (Stage One). Alameda County does not have an attestation and can only have open those industries which are open statewide.\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>Yes, but when you return depends on your situation.\n\n**If you have symptoms**, you should stay home until:\n\n*   at least 10 days have passed since symptoms started, **AND**\n*    your fever has been gone for 24 hours without the aid of medication, **AND** \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested.\n\n**If you have tested positive but have no symptoms**, you should [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) at home for at least 10 days.\n\n**If you had close contact with someone who tested positive but you have tested negative**, you should still [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) at home for at least 14 days.\n\nGet tested as soon as possible if you have symptoms or have come in contact with someone who has tested positive or has symptoms.\n\nRead more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C154" t="str">
-        <v>https://covid19.ca.gov/roadmap-counties/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D154" t="str">
         <v xml:space="preserve"> </v>
@@ -4386,13 +4386,13 @@
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>For counties without attestations</v>
+        <v>What steps are required when a business has an employee who tests positive?</v>
       </c>
       <c r="B155" t="str">
-        <v>*   [Industries open statewide](https://covid19.ca.gov/industry-guidance/)\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>If an employer discovers a worker has tested positive for COVID-19 or has symptoms, they should send the worker home. Then the employer should [follow guidance](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf) about isolation or quarantine, testing, and when it is appropriate for the worker to return to work. Employers should support the need for workers to stay home for the protection of others with flexible leave policies. For more details, see “What to do if there is a Case of COVID-19 in the Workplace” in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf) and check with your local health department.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C155" t="str">
-        <v>https://covid19.ca.gov/roadmap-counties/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D155" t="str">
         <v xml:space="preserve"> </v>
@@ -4412,13 +4412,13 @@
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v>Northern California</v>
+        <v>Can people who recover from COVID-19 be re-infected?</v>
       </c>
       <c r="B156" t="str">
-        <v>*   Alturas (Modoc County)\n*   American Canyon (Napa County)\n*   Antioch (Contra Costa County)\n*   Atascadero (San Luis Obispo County)\n*   Bear Valley (Alpine County)\n*   Bieber (Lassen County)\n*   Bishop (Inyo County)\n*   Calistoga (Napa County)\n*   Calpine (Sierra County)\n*   Cedarville (Modoc County)\n*   Ceres (Sanislaus County)\n*   Chowchilla (Madera County)\n*   Clearlake (Lake County)\n*   Coleville (Mono County)\n*   Corcoran (King County)\n*   Corona (King County)\n*   Crescent City (Del Norte County)\n*   Daly City (San Mateo County)\n*   Dinuba (Tulare County)\n*   Downieville (Sierra County)\n*   Doyle (Lassen County)\n*   East Palo Alto (San Mateo County)\n*   Elk Grove (Sacramento County)\n*   Exeter (Tulare County)\n*   Farmersville (Tulare County)\n*   French Camp (San Joaquin County)\n*   Fresno (Fresno County)\n*   Gridley (Butte County)\n*   Half Moon Bay (San Mateo County)\n*   Hanford (King County)\n*   Hayfork (Trinity County)\n*   Herlong (Lassen County)\n*   Jackson (Amador County)\n*   Kerman (Fresno County)\n*   Lakeport (Lake County)\n*   Lemoore (King County)\n*   Lewiston (Trinity County)\n*   Livingston (Merced County)\n*   Lone Pine (Inyo County)\n*   Loyalton (Sierra County)\n*   Magalia (Butte County)\n*   Mammoth Lakes (Mono County)\n*   Markleeville (Alpine County)\n*   Mendota (Fresno County)\n*   Merced (Merced County)\n*   Middletown (Lake County)\n*   Napa (Napa County)\n*   North San Juan (Nevada County)\n*   Oakland (Alameda County)\n*   Placerville (El Dorado County)\n*   Porterville (Tulare County)\n*   Redding (Shasta County)\n*   Redwood City (San Mateo County)\n*   Reedley (Fresno County)\n*   Rio Linda (Sacramento County)\n*   Sacramento (Sacramento County)\n*   Salida (Stanislaus County)\n*   San Bruno (San Mateo County)\n*   San Francisco (San Francisco)\n*   San Jose (Santa Clara County)\n*   San Mateo (San Mateo County)\n*   Santa Rosa (Sonoma County)\n*   Selma (Fresno County)\n*   St. Helena (Napa County)\n*   Stockton (San Joaquin County)\n*   Susanville (Lassen County)\n*   Tracy (San Joaquin County)\n*   Tulare (Tulare County)\n*   Turlock (Stanislaus County)\n*   Upper Lake (Lake County)\n*   Vallejo (Solano County)\n*   Visalia (Tulare County)\n*   Willow Creek (Humboldt County)\n*   Weaverville (Trinity County)\n*   Westwood (Lassen County)\n\n*   Woodlake (Tulare County)\n*   Woodland (Yolo County)\n*   Yosemite Valley (Mariposa County)\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>We don’t yet know. The duration of immunity to coronavirus infection is not yet understood. Patients infected with other similar coronaviruses are unlikely to be re-infected in the months after they recover. However, more information is needed to know whether similar immune protection will be observed for patients with COVID-19.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C156" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D156" t="str">
         <v xml:space="preserve"> </v>
@@ -4438,13 +4438,13 @@
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>Southern California</v>
+        <v>County Monitoring List</v>
       </c>
       <c r="B157" t="str">
-        <v>*   Alpine (San Diego County) \n*   Anaheim (Orange County)\n*   Apple Valley (San Bernardino County)\n*   Bakersfield (Kern County)\n*   Banning (Riverside County)\n*   Barstow (San Bernardino County)\n*   Beaumont (Riverside County)\n*   Bell (Los Angeles County)\n*   Blythe (Riverside County)\n*   Calexico (Imperial County)\n*   Coachella (Riverside County)\n*   Compton (Los Angeles County)\n*   Costa Mesa (Orange County)\n*   Delano (Kern County)\n*   Desert Hot Springs (Riverside County)\n*   El Centro (Imperial County)\n*   Fallbrook (San Diego)\n*   Fontana (San Bernardino County)\n*   Fullerton (Orange County)\n*   Gardena (Los Angeles County)\n*   Hemet (Riverside County)\n*   Hesperia (San Bernardino County)\n*   Indio (Riverside County)\n*   La Habra (Orange County)\n*   Lake Elsinore (Riverside County)\n*   Lamont (Kern County)\n*   Lancaster (Los Angeles County)\n*   Lemon Grove (San Diego County)\n*   Los Angeles (Los Angeles County)\n*   McFarland (Kern County)\n*   Oceanside (San Diego)\n*   Ontario (San Bernardino County)\n*   Palmdale (Los Angeles County)\n*   Paramount (Los Angeles County)\n*   Pasadena (Los Angeles County)\n*   Perris (Riverside County)\n*   Phelan (San Bernardino County)\n*   Pico Rivera (Los Angeles County)\n*   Pomona (Los Angeles County)\n*   Port Hueneme (Ventura County)\n*   Riverside (Riverside County)\n*   Rosamond (Kern County)\n*   San Jucinta (Riverside County)\n*   San Juan Capistrano (Orange County)\n*   Santa Maria (Santa Barbara County)\n*   Santa Paula (Ventura County)\n*   Shafter (Kern County)\n*   Valley Center (San Diego County)\n*   Victorville (San Bernardino County)\n*   Wasco (Kern County) \n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>1.  Alameda\n2.  Butte\n3.  Colusa\n4.  Contra Costa\n5.  Fresno\n6.  Glenn\n7.  Imperial\n8.  Kern\n9.  Kings\n10.  Los Angeles\n11.  Madera\n12.  Marin\n13.  Merced\n14.  Mono\n15.  Monterey\n16.  Napa\n17.  Orange\n18.  Placer\n19.  Riverside\n20.  Sacramento\n21.  San Benito\n22.  San Bernardino\n23.  San Diego\n24.  San Francisco\n25.  San Joaquin\n26.  San Luis Obispo\n27.  San Mateo **(3 days or less)**\n28.  Santa Barbara\n29.  Santa Clara\n30.  Santa Cruz\n31.  Solano\n32.  Sonoma\n33.  Stanislaus\n34.  Sutter\n35.  Tulare\n36.  Ventura\n37.  Yolo\n38.  Yuba\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
       </c>
       <c r="C157" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/roadmap-counties/</v>
       </c>
       <c r="D157" t="str">
         <v xml:space="preserve"> </v>
@@ -4464,13 +4464,13 @@
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>How do I get a drive-through test?</v>
+        <v>For attested counties not on Monitoring List</v>
       </c>
       <c r="B158" t="str">
-        <v>There are two steps to this process: screening and testing. First, you will create an account and take the online screener. If your answers from the screener determine you are eligible at this time, you will receive details on how and where to get tested. Once tested, you’ll be informed via email or phone when your COVID-19 test results are available.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>*   [Industries open statewide](https://covid19.ca.gov/industry-guidance/)\n*   Dine-in restaurants (outdoors only)\n*   Wineries and tasting rooms (outdoors only)\n*   Family entertainment centers (outdoors only)\n*   Zoos and museums (outdoors only)\n*   Cardrooms (outdoors only)\n*   Casinos\n*   Gyms and fitness centers\n*   Hotels (for tourism and individual travel)\n*   Campgrounds and outdoor recreation\n*   Personal care services, like nail salons and body waxing\n*   Hair salons and barbershops\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
       </c>
       <c r="C158" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/roadmap-counties/</v>
       </c>
       <c r="D158" t="str">
         <v xml:space="preserve"> </v>
@@ -4490,13 +4490,13 @@
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>Why am I asked to create an account for drive-through testing using Verily’s Project Baseline?</v>
+        <v>For counties on Monitoring List for 3 consecutive days</v>
       </c>
       <c r="B159" t="str">
-        <v>For the Baseline COVID-19 Program to work, Verily needs a way to authenticate users to appropriately protect their information. Verily turned to Google for this service because Google Account provides best-in-class authentication. We ask that you link to an existing Google Account or create a new Google Account (which can be done with any email address). This lets Verily authenticate your account, and securely and privately contact you during the screening and testing process. All the data provided by Baseline COVID-19 Program users for screening is stored separately and not directly linked to a user’s Google Account.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>*   [Industries open statewide](https://covid19.ca.gov/industry-guidance/)\n*   Casinos\n*   Hotels (for tourism and individual travel)\n*   Campgrounds and outdoor recreation\n\nThe following industries must close indoor operations, but they may be modified to operate outside or by pick-up:\n\n*   Dine-in restaurants\n*   Wineries and tasting rooms\n*   Movie theaters \n*   Family entertainment centers (for example: bowling alleys, miniature golf, batting cages and arcades)\n*   Zoos and museums\n*   Cardrooms\n*   Gyms and fitness centers\n*   Personal care services, like nail salons and body waxing\n*   Places of worship and cultural ceremonies, like weddings and funerals\n*   Offices for non-critical infrastructure sectors\n*   Shopping malls \n\nNOTE: Imperial County is open to the essential workforce only (Stage One).\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
       </c>
       <c r="C159" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/roadmap-counties/</v>
       </c>
       <c r="D159" t="str">
         <v xml:space="preserve"> </v>
@@ -4516,13 +4516,13 @@
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>Do I need emergency treatment?</v>
+        <v>For counties without attestations</v>
       </c>
       <c r="B160" t="str">
-        <v>If you develop any of these warning signs for COVID-19, get emergency medical attention immediately:\n\n*   Trouble breathing\n*   Persistent pain or pressure in the chest\n*   New confusion \n*   Inability to awake or stay awake\n*   Bluish lips or face\n\nThere are other, less-common symptoms. Please call your medical provider if you have any symptoms that are severe or concerning to you.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call 911, tell the operator you have coronavirus symptoms so ambulance workers can be ready to treat you safely.\n\nIf you’re not sure if this applies to you, you can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor through [telehealth](https://covid19.ca.gov/telehealth/).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>*   [Industries open statewide](https://covid19.ca.gov/industry-guidance/)\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
       </c>
       <c r="C160" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/roadmap-counties/</v>
       </c>
       <c r="D160" t="str">
         <v xml:space="preserve"> </v>
@@ -4542,10 +4542,10 @@
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>I have mild COVID-19 symptoms. How long do I have to isolate at home?</v>
+        <v>Drive-through testing in Northern California</v>
       </c>
       <c r="B161" t="str">
-        <v>Follow the Centers for Disease Control and Prevention (CDC) guidance on [ending self-isolation](https://www.cdc.gov/coronavirus/2019-ncov/hcp/disposition-in-home-patients.html).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>*   Alturas (Modoc County)\n*   American Canyon (Napa County)\n*   Antioch (Contra Costa County)\n*   Atascadero (San Luis Obispo County)\n*   Bear Valley (Alpine County)\n*   Bieber (Lassen County)\n*   Bishop (Inyo County)\n*   Calistoga (Napa County)\n*   Calpine (Sierra County)\n*   Cedarville (Modoc County)\n*   Ceres (Sanislaus County)\n*   Chowchilla (Madera County)\n*   Clearlake (Lake County)\n*   Coleville (Mono County)\n*   Corcoran (King County)\n*   Corona (King County)\n*   Crescent City (Del Norte County)\n*   Daly City (San Mateo County)\n*   Dinuba (Tulare County)\n*   Downieville (Sierra County)\n*   Doyle (Lassen County)\n*   East Palo Alto (San Mateo County)\n*   Elk Grove (Sacramento County)\n*   Exeter (Tulare County)\n*   Farmersville (Tulare County)\n*   French Camp (San Joaquin County)\n*   Fresno (Fresno County)\n*   Gridley (Butte County)\n*   Half Moon Bay (San Mateo County)\n*   Hanford (King County)\n*   Hayfork (Trinity County)\n*   Herlong (Lassen County)\n*   Huron (Fresno County)\n*   Jackson (Amador County)\n*   Kerman (Fresno County)\n*   Lakeport (Lake County)\n*   Lemoore (King County)\n*   Lewiston (Trinity County)\n*   Livingston (Merced County)\n*   Lone Pine (Inyo County)\n*   Loyalton (Sierra County)\n*   Magalia (Butte County)\n*   Mammoth Lakes (Mono County)\n*   Markleeville (Alpine County)\n*   Mendota (Fresno County)\n*   Merced (Merced County)\n*   Middletown (Lake County)\n*   Napa (Napa County)\n*   North San Juan (Nevada County)\n*   Oakland (Alameda County)\n*   Placerville (El Dorado County)\n*   Porterville (Tulare County)\n*   Redding (Shasta County)\n*   Redwood City (San Mateo County)\n*   Reedley (Fresno County)\n*   Rio Linda (Sacramento County)\n*   Sacramento (Sacramento County)\n*   Salida (Stanislaus County)\n*   San Bruno (San Mateo County)\n*   San Francisco (San Francisco)\n*   San Jose (Santa Clara County)\n*   San Mateo (San Mateo County)\n*   Santa Rosa (Sonoma County)\n*   Selma (Fresno County)\n*   St. Helena (Napa County)\n*   Stockton (San Joaquin County)\n*   Susanville (Lassen County)\n*   Tracy (San Joaquin County)\n*   Tulare (Tulare County)\n*   Turlock (Stanislaus County)\n*   Upper Lake (Lake County)\n*   Vallejo (Solano County)\n*   Visalia (Tulare County)\n*   Weaverville (Trinity County)\n*   Westwood (Lassen County)\n\n*   Woodlake (Tulare County)\n*   Woodland (Yolo County)\n*   Yosemite Valley (Mariposa County)\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C161" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4568,10 +4568,10 @@
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>When can I be around other people after I had or likely had COVID-19?</v>
+        <v>Drive-through testing in Southern California</v>
       </c>
       <c r="B162" t="str">
-        <v>You can be with others after:\n\n*   3 days with no fever **and**\n*   Respiratory symptoms have improved (e.g. cough, shortness of breath) **and**\n*   10 days since symptoms first appeared\n\n[CDPH](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Expanding-Access-to-Testing-Updated-Interim-Guidance-on-Prioritization-for-COVID-19-Laboratory-Testing-0501.aspx) and [CDC](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/end-home-isolation.html) have detailed recommendations for quarantine/isolation, if you are sick with COVID-19 or tested positive for coronavirus.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>*   Alpine (San Diego County) \n*   Anaheim (Orange County)\n*   Apple Valley (San Bernardino County)\n*   Bakersfield (Kern County)\n*   Banning (Riverside County)\n*   Barstow (San Bernardino County)\n*   Beaumont (Riverside County)\n*   Bell (Los Angeles County)\n*   Blythe (Riverside County)\n*   Calexico (Imperial County)\n*   Coachella (Riverside County)\n*   Compton (Los Angeles County)\n*   Costa Mesa (Orange County)\n*   Delano (Kern County)\n*   Desert Hot Springs (Riverside County)\n*   El Centro (Imperial County)\n*   Fallbrook (San Diego)\n*   Fontana (San Bernardino County)\n*   Fullerton (Orange County)\n*   Gardena (Los Angeles County)\n*   Hemet (Riverside County)\n*   Hesperia (San Bernardino County)\n*   Indio (Riverside County)\n*   La Habra (Orange County)\n*   Lake Elsinore (Riverside County)\n*   Lamont (Kern County)\n*   Lancaster (Los Angeles County)\n*   Lemon Grove (San Diego County)\n*   Los Angeles (Los Angeles County)\n*   McFarland (Kern County)\n*   Oceanside (San Diego)\n*   Ontario (San Bernardino County)\n*   Palmdale (Los Angeles County)\n*   Paramount (Los Angeles County)\n*   Pasadena (Los Angeles County)\n*   Perris (Riverside County)\n*   Phelan (San Bernardino County)\n*   Pico Rivera (Los Angeles County)\n*   Pomona (Los Angeles County)\n*   Port Hueneme (Ventura County)\n*   Riverside (Riverside County)\n*   Rosamond (Kern County)\n*   San Jucinta (Riverside County)\n*   San Juan Capistrano (Orange County)\n*   Santa Maria (Santa Barbara County)\n*   Santa Paula (Ventura County)\n*   Shafter (Kern County)\n*   Valley Center (San Diego County)\n*   Victorville (San Bernardino County)\n*   Wasco (Kern County) \n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C162" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4594,10 +4594,10 @@
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>How can I find a coronavirus testing location near me?</v>
+        <v>How do I get a drive-through test by Verily’s Project Baseline?</v>
       </c>
       <c r="B163" t="str">
-        <v>Find a testing location\n-----------------------\n\n&gt; [See the map](https://arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401)\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>There are two steps to this process: screening and testing. First, you will create an account and take the online screener. If you are eligible, you will get details on how and where to get tested. Once tested, you’ll get an email or phone call with your COVID-19 test results.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C163" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4620,10 +4620,10 @@
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>What is an antibody test? Where can I get an antibody test?</v>
+        <v>Why am I asked to create an account for Verily?</v>
       </c>
       <c r="B164" t="str">
-        <v>[Antibody tests](https://www.cdc.gov/coronavirus/2019-ncov/testing/serology-overview.html) detect past infections (but not current infections). They are used to detect past COVID-19 infections in an individual and can be used to determine if you are a good candidate to [donate blood plasma](https://covid19.ca.gov/plasma). It can take 1-3 weeks after infection for your body to make antibodies. \n\nYou can find locations for both viral and antibody [tests](https://www.arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401) on [California’s testing map](https://www.arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>Verily needs a way to authenticate and protect user information. They turned to Google for this service, because Google accounts have best-in-class authentication. Simply link to an existing Google account or create a new one (which you can do with any email address). Then Verily can contact you securely during the screening and testing process. All data r collected by Verily is kept private and is not linked to a user’s Google account.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C164" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4646,13 +4646,13 @@
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>What are the pay and benefits for California Health Corps professionals?</v>
+        <v>Do I need emergency treatment?</v>
       </c>
       <c r="B165" t="str">
-        <v>Salary rates for most of the health care professionals being hired for this emergency are listed in the [CalHR Pay Scales](https://www.calhr.ca.gov/Pay%20Scales%20Library/PS_Sec_05.pdf) (pages 5.12 and 5.13). In addition, CalHR has established pay rates for medical roles that don’t have a corresponding regular classification and pay schedule, such as paramedics and EMTs. CalHR will determine specific salary and benefits after conducting a review of each application.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>If you develop any of these symptoms of COVID-19, get medical attention immediately:\n\n*   Trouble breathing\n*   Persistent pain or pressure in the chest\n*   New confusion \n*   Inability to awake or stay awake\n*   Bluish lips or face\n\nThere are other, less-common symptoms. Please call your medical provider if you have any symptoms that are severe or concern you.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call 911, tell the operator you have coronavirus symptoms. This is so ambulance workers can be ready to treat you safely.\n\nNot sure if this applies to you? Check your symptoms with the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C165" t="str">
-        <v>https://covid19.ca.gov/healthcorps/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D165" t="str">
         <v xml:space="preserve"> </v>
@@ -4672,13 +4672,13 @@
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>Some healthcare professions are not listed. Are health professionals who are not listed (e.g., Medical Technicians, Lab Technicians, etc.) eligible for the California Health Corps?</v>
+        <v>When can I be around other people after I had or likely had COVID-19?</v>
       </c>
       <c r="B166" t="str">
-        <v>California Health Corps are currently only accepting applications for the healthcare professions listed on the website. However, we are constantly re-evaluating our needs during this fluid situation and will open the registration for other professionals, if the need arises.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>You can be with others after:\n\n*   10 days since symptoms first appeared **and**\n*   At least 24 hours with no fever without fever-reducing medication **and**\n*   After symptoms have improved\n\nCDC has [detailed recommendations](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/end-home-isolation.html) for people who had tested positive but had no symptoms.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C166" t="str">
-        <v>https://covid19.ca.gov/healthcorps/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D166" t="str">
         <v xml:space="preserve"> </v>
@@ -4698,13 +4698,13 @@
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>When can I expect to hear a response after completing my California Health Corps registration?</v>
+        <v>When can I be around other people after I tested positive for COVID-19 but had no symptoms?</v>
       </c>
       <c r="B167" t="str">
-        <v>Currently we anticipate the process may take up to two weeks, since an incredible number of responses are received and need to prioritize certain parts of the state, where the needs are the greatest. We will begin to contact the volunteers after verification of credentials, and based on current and anticipated needs.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>If you continue to have no symptoms, you can be with others after 10 days have passed since your test.\n\nCDC has [detailed recommendations](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/end-home-isolation.html) for people who had tested positive for coronavirus but had no symptoms.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C167" t="str">
-        <v>https://covid19.ca.gov/healthcorps/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D167" t="str">
         <v xml:space="preserve"> </v>
@@ -4724,13 +4724,13 @@
     </row>
     <row r="168">
       <c r="A168" t="str">
-        <v>How do I return to the California Health Corps application after logging out?</v>
+        <v>Should employees be required to provide proof of a negative coronavirus test before returning to work after they had COVID-19?</v>
       </c>
       <c r="B168" t="str">
-        <v>Visit [https://healthcarevolunteers.ca.gov/](https://healthcarevolunteers.ca.gov/) and use the account you created while applying to correct or update any information you want.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>No. Proof of a negative test should not be required prior to returning to the workplace after documented COVID infection, since PCR tests can remain positive long after an individual is no longer infectious. CDPH [COVID-19 Testing Guidance](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Updated-COVID-19-Testing-Guidance.aspx) recommends symptom- or protocol-based criteria be used to determine when an employee is safe to return to the workplace.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C168" t="str">
-        <v>https://covid19.ca.gov/healthcorps/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D168" t="str">
         <v xml:space="preserve"> </v>
@@ -4750,13 +4750,13 @@
     </row>
     <row r="169">
       <c r="A169" t="str">
-        <v>Resources for the California Health Corps participants</v>
+        <v>Can two people that both tested positive hang out/stay together?</v>
       </c>
       <c r="B169" t="str">
-        <v>*   SNF Orientation: [SNF-Nursing-Staff-Orientation (PDF)](https://covid19.ca.gov/pdf/SNF-Nursing-Staff-Orientation.pdf)\n*   Program FAQ details: [CA-Health-Corps-FAQ (PDF)](https://covid19.ca.gov/pdf/CA-Health-Corps-FAQ.pdf)\n*   How to file a complaint: [How-to-file-a-complaint (PDF)](https://covid19.ca.gov/pdf/How-to-file-a-complaint.pdf)\n*   Direct deposit: [std699-Direct-Deposit (PDF)](https://covid19.ca.gov/pdf/std699-Direct-Deposit.pdf)\n*   Travel expense claim: [Std262-Travel-Expense-Claim (PDF)](https://covid19.ca.gov/pdf/Std262-Travel-Expense-Claim.pdf)\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>No. You should take preventive measures to protect yourself and others. We do not know yet if or when a person can be reinfected with COVID-19. \n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C169" t="str">
-        <v>https://covid19.ca.gov/healthcorps/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D169" t="str">
         <v xml:space="preserve"> </v>
@@ -4776,13 +4776,13 @@
     </row>
     <row r="170">
       <c r="A170" t="str">
-        <v>Can a doctor with out of state Licence or foreign medical graduate without California license work for the California Health Corps?</v>
+        <v>If I test positive for COVID-19 in a viral test, what should I do to protect others in my household?</v>
       </c>
       <c r="B170" t="str">
-        <v>To be eligible for COVID-19 emergency medical staffing roles, you must:\n\n*   Have a valid California License for clinical practice (if you are a MD, DO, etc.) \n*   **OR** are a medical resident or nursing student \n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>You should [self-isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) from others in your household who have not tested positive. Sleep and stay in a separate room from them, and use a separate bathroom, if possible. Multiple infected people in the same household can use the same room for isolation.\n\nMembers of your household should get tested right away. They should [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) for at least 14 days. Symptoms can develop even after testing negative within 14 days after exposure. Multiple people in the same household should not quarantine in the same room, since some may be infected.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C170" t="str">
-        <v>https://covid19.ca.gov/healthcorps/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D170" t="str">
         <v xml:space="preserve"> </v>
@@ -4802,13 +4802,13 @@
     </row>
     <row r="171">
       <c r="A171" t="str">
-        <v>Agriculture and livestock</v>
+        <v>How can I find a coronavirus testing location near me?</v>
       </c>
       <c r="B171" t="str">
-        <v>The [guidance for the agriculture and livestock industry](http://covid19.ca.gov/pdf/guidance-agriculture.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the agriculture and livestock industry](http://covid19.ca.gov/pdf/checklist-agriculture.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>&gt; [Find a testing location](https://arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401)\n&gt; -----------------------------------------------------------------------------------------------------------\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C171" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D171" t="str">
         <v xml:space="preserve"> </v>
@@ -4828,13 +4828,13 @@
     </row>
     <row r="172">
       <c r="A172" t="str">
-        <v>Auto dealerships</v>
+        <v>What is an antibody test? Where can I get an antibody test?</v>
       </c>
       <c r="B172" t="str">
-        <v>The [guidance for the automobile dealerships and rental operators industry](http://covid19.ca.gov/pdf/guidance-auto-dealerships.pdf) provides guidelines to create a safer environment for workers.  \nReview the guidance, prepare a plan, and post the [checklist for the automobile dealerships and rental operators](http://covid19.ca.gov/pdf/checklist-auto-dealerships.pdf) industry in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v xml:space="preserve"> [Antibody tests](https://www.cdc.gov/coronavirus/2019-ncov/testing/serology-overview.html) detect past infections. They can determine if you are a good candidate to [donate blood plasma](https://covid19.ca.gov/plasma). It can take 1-3 weeks after infection for your body to make antibodies.\n\nYou can find locations for both viral and antibody tests on [California’s testing map](https://www.arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C172" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D172" t="str">
         <v xml:space="preserve"> </v>
@@ -4854,13 +4854,13 @@
     </row>
     <row r="173">
       <c r="A173" t="str">
-        <v>Childcare – Updated July 20</v>
+        <v>What are the pay and benefits for California Health Corps professionals?</v>
       </c>
       <c r="B173" t="str">
-        <v>All childcare facilities can open with necessary modifications. The updated [guidance for the childcare industry](https://files.covid19.ca.gov/pdf/guidance-childcare--en.pdf) provides guidelines to minimize the spread of COVID-19 and ensure the safety of children, providers, and families. As programs begin to reopen and other programs transition from emergency childcare for essential workers to enhanced regular operations, all providers must apply new and updated policies and requirements and must update their emergency preparedness plan.\n\nReview the guidance, prepare a plan, and post the [checklist for childcare](https://files.covid19.ca.gov/pdf/checklist-childcare--en.pdf) in your facility to show employees and families that you’ve reduced the risk and are open for operation.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Salary rates for most of the health care professionals being hired for this emergency are listed in the [CalHR Pay Scales](https://www.calhr.ca.gov/Pay%20Scales%20Library/PS_Sec_05.pdf) (pages 5.12 and 5.13). In addition, CalHR has established pay rates for medical roles that don’t have a corresponding regular classification and pay schedule, such as paramedics and EMTs. CalHR will determine specific salary and benefits after conducting a review of each application.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C173" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/healthcorps/</v>
       </c>
       <c r="D173" t="str">
         <v xml:space="preserve"> </v>
@@ -4880,13 +4880,13 @@
     </row>
     <row r="174">
       <c r="A174" t="str">
-        <v>Communications infrastructure</v>
+        <v>Some healthcare professions are not listed. Are health professionals who are not listed (e.g., Medical Technicians, Lab Technicians, etc.) eligible for the California Health Corps?</v>
       </c>
       <c r="B174" t="str">
-        <v>The [guidance for the communications infrastructure industry](http://covid19.ca.gov/pdf/guidance-communications.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the communications infrastructure industry](http://covid19.ca.gov/pdf/checklist-communications.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>California Health Corps are currently only accepting applications for the healthcare professions listed on the website. However, we are constantly re-evaluating our needs during this fluid situation and will open the registration for other professionals, if the need arises.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C174" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/healthcorps/</v>
       </c>
       <c r="D174" t="str">
         <v xml:space="preserve"> </v>
@@ -4906,13 +4906,13 @@
     </row>
     <row r="175">
       <c r="A175" t="str">
-        <v>Construction</v>
+        <v>When can I expect to hear a response after completing my California Health Corps registration?</v>
       </c>
       <c r="B175" t="str">
-        <v>This [guidance for the construction industry](http://covid19.ca.gov/pdf/guidance-construction.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the construction industry](http://covid19.ca.gov/pdf/checklist-construction.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Currently we anticipate the process may take up to two weeks, since an incredible number of responses are received and need to prioritize certain parts of the state, where the needs are the greatest. We will begin to contact the volunteers after verification of credentials, and based on current and anticipated needs.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C175" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/healthcorps/</v>
       </c>
       <c r="D175" t="str">
         <v xml:space="preserve"> </v>
@@ -4932,13 +4932,13 @@
     </row>
     <row r="176">
       <c r="A176" t="str">
-        <v>Day camps – Updated July 20</v>
+        <v>How do I return to the California Health Corps application after logging out?</v>
       </c>
       <c r="B176" t="str">
-        <v>The updated [guidance for day camps](http://covid19.ca.gov/pdf/guidance-daycamps.pdf) provides guidelines to create a plan for safe re-opening. Implementation of these guidelines should be tailored for each setting. Implementation requires training and support for staff and adequate consideration of camper and family needs. All decisions about following these recommendations should be made in collaboration with local health officials and other authorities, and should depend on the levels of COVID-19 community transmission and the capacities of the local public health and healthcare systems, among other relevant factors.\n\nReview the guidance, prepare a plan, and post the [checklist for day camps](https://files.covid19.ca.gov/pdf/checklist-daycamps--en.pdf) in your facility to show employees, campers, and families that you’ve reduced the risk and are open for operation.  \n  \nRecreational team sports are not permitted and will be subject to separate guidance.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Visit [https://healthcarevolunteers.ca.gov/](https://healthcarevolunteers.ca.gov/) and use the account you created while applying to correct or update any information you want.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C176" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/healthcorps/</v>
       </c>
       <c r="D176" t="str">
         <v xml:space="preserve"> </v>
@@ -4958,13 +4958,13 @@
     </row>
     <row r="177">
       <c r="A177" t="str">
-        <v>Delivery services</v>
+        <v>Resources for the California Health Corps participants</v>
       </c>
       <c r="B177" t="str">
-        <v>The [guidance for the delivery services industry](http://covid19.ca.gov/pdf/guidance-delivery-services.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the delivery services industry](http://covid19.ca.gov/pdf/checklist-delivery-services.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>*   SNF Orientation: [SNF-Nursing-Staff-Orientation (PDF)](https://files.covid19.ca.gov/pdf/SNF-Nursing-Staff-Orientation.pdf)\n*   Program FAQ details: [CA-Health-Corps-FAQ (PDF)](https://files.covid19.ca.gov/pdf/CA-Health-Corps-FAQ.pdf)\n*   How to file a complaint: [How-to-file-a-complaint (PDF)](https://files.covid19.ca.gov/pdf/How-to-file-a-complaint.pdf)\n*   Direct deposit: [std699-Direct-Deposit (PDF)](https://files.covid19.ca.gov/pdf/std699-Direct-Deposit.pdf)\n*   Travel expense claim: [Std262-Travel-Expense-Claim (PDF)](https://files.covid19.ca.gov/pdf/Std262-Travel-Expense-Claim.pdf)\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C177" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/healthcorps/</v>
       </c>
       <c r="D177" t="str">
         <v xml:space="preserve"> </v>
@@ -4984,13 +4984,13 @@
     </row>
     <row r="178">
       <c r="A178" t="str">
-        <v>Energy and utilities</v>
+        <v>Can a doctor with out of state Licence or foreign medical graduate without California license work for the California Health Corps?</v>
       </c>
       <c r="B178" t="str">
-        <v>The [guidance for the energy and utilities industry](http://covid19.ca.gov/pdf/guidance-energy.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post  the [checklist for the energy and utilities industry](http://covid19.ca.gov/pdf/checklist-energy.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>To be eligible for COVID-19 emergency medical staffing roles, you must:\n\n*   Have a valid California License for clinical practice (if you are a MD, DO, etc.) \n*   **OR** are a medical resident or nursing student \n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C178" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/healthcorps/</v>
       </c>
       <c r="D178" t="str">
         <v xml:space="preserve"> </v>
@@ -5010,10 +5010,10 @@
     </row>
     <row r="179">
       <c r="A179" t="str">
-        <v>Family friendly practices for employers</v>
+        <v>Agriculture and livestock</v>
       </c>
       <c r="B179" t="str">
-        <v>The [guidance for family friendly practices for employers](http://covid19.ca.gov/pdf/guidance-familyfriendlypracticesemployers.pdf) provides guidelines for family-friendly practices to keep employees safe and be responsive to their needs in order to ensure continued productivity. As workplaces reopen, employees will require both child care supports and workplace flexibility. Work-life balance policies will become even more important and continued investment in family-friendly workplace policies by employers is critical.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the agriculture and livestock industry](https://files.covid19.ca.gov/pdf/guidance-agriculture.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the agriculture and livestock industry](https://files.covid19.ca.gov/pdf/checklist-agriculture.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C179" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5036,10 +5036,10 @@
     </row>
     <row r="180">
       <c r="A180" t="str">
-        <v>Food packing</v>
+        <v>Auto dealerships</v>
       </c>
       <c r="B180" t="str">
-        <v>The [guidance for facilities that process or pack meat, dairy, or produce](http://covid19.ca.gov/pdf/guidance-food-packing.pdf) provides guidelines to create a safer environment for workers.  \nReview the guidance, prepare a plan, and post the [checklist for facilities that process or pack meat, dairy or produce](http://covid19.ca.gov/pdf/checklist-food-packing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the automobile dealerships and rental operators industry](https://files.covid19.ca.gov/pdf/guidance-auto-dealerships.pdf) provides guidelines to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for the automobile dealerships and rental operators](https://files.covid19.ca.gov/pdf/checklist-auto-dealerships.pdf) industry in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C180" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5062,10 +5062,10 @@
     </row>
     <row r="181">
       <c r="A181" t="str">
-        <v>Hotels and lodging</v>
+        <v>Childcare</v>
       </c>
       <c r="B181" t="str">
-        <v>This [guidance for the hotels and lodging](http://covid19.ca.gov/pdf/guidance-hotels.pdf) provides guidelines to counties not [approved for variance](https://covid19.ca.gov/roadmap-counties/) create a safer environment for workers and customers.\n\nUnless your county has been approved to move further in the roadmap, hotels should only open for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or providing housing solutions, including measures to protect homeless populations.\n\nSeparate guidance for hotels and lodging services in counties with variance attestation [can be found here](https://covid19.ca.gov/pdf/guidance-hotels-lodging-rentals.pdf).\n\nReview the guidance, prepare a plan, and post the [checklist for hotels and lodging](http://covid19.ca.gov/pdf/checklist-hotels.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>All childcare facilities can open with necessary modifications. The updated [guidance for the childcare industry](https://files.covid19.ca.gov/pdf/guidance-childcare--en.pdf) provides guidelines to minimize the spread of COVID-19 and ensure the safety of children, providers, and families. As programs begin to reopen and other programs transition from emergency childcare for essential workers to enhanced regular operations, all providers must apply new and updated policies and requirements and must update their emergency preparedness plan.\n\nReview the guidance, prepare a plan, and post the [checklist for childcare](https://files.covid19.ca.gov/pdf/checklist-childcare--en.pdf) in your facility to show employees and families that you’ve reduced the risk and are open for operation.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C181" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5088,10 +5088,10 @@
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>Life sciences</v>
+        <v>Communications infrastructure</v>
       </c>
       <c r="B182" t="str">
-        <v>The [guidance for the life sciences industry](http://covid19.ca.gov/pdf/guidance-life-sciences.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the life sciences industry](http://covid19.ca.gov/pdf/checklist-life-sciences.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the communications infrastructure industry](https://files.covid19.ca.gov/pdf/guidance-communications.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the communications infrastructure industry](https://files.covid19.ca.gov/pdf/checklist-communications.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C182" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5114,10 +5114,10 @@
     </row>
     <row r="183">
       <c r="A183" t="str">
-        <v>Limited services</v>
+        <v>Construction</v>
       </c>
       <c r="B183" t="str">
-        <v>Limited Services are defined as those which do not generally require close contact. Follow this [guidance for Limited Services](https://covid19.ca.gov/pdf/guidance-limited-services.pdf) to create a safer environment for workers and patrons.\n\nFaith-based counseling can reopen within the following parameters:\n\n1.  Counselling services are permissible in-person where the service cannot reasonably be practiced remotely;\n2.  Counselling services should adopt state guidance on Limited Services, where applicable;\n3.  This designation does not permit gatherings beyond counselling to members of a single household.\n\nReview the guidance, prepare a plan, and post the [checklist for Limited Services](https://covid19.ca.gov/pdf/checklist-limited-services.pdf) in your workplace to show clients and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)&lt;!-- laundromat, dry cleaner, laundry, auto repair, car wash, landscaper, door to door, sales, pet groom, dog walk, entry to private residences, community 2 facilities, residential, janitorial, cleaning services, house keep, house clean, HVAC, appliance repair, electrician, plumbers, mechanical trade, handyperson, handyman, general contractors, lessees, subcontractors --&gt;</v>
+        <v>This [guidance for the construction industry](https://files.covid19.ca.gov/pdf/guidance-construction.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the construction industry](https://files.covid19.ca.gov/pdf/checklist-construction.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C183" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5140,10 +5140,10 @@
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>Logistics and warehousing facilities</v>
+        <v>Day camps</v>
       </c>
       <c r="B184" t="str">
-        <v>The [guidance for businesses operating in the logistics/warehousing industry](http://covid19.ca.gov/pdf/guidance-logistics-warehousing.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post  the [checklist for the logistics/warehousing industry](http://covid19.ca.gov/pdf/checklist-logistics-warehousing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The updated [guidance for day camps](https://files.covid19.ca.gov/pdf/guidance-daycamps.pdf) provides guidelines to create a plan for safe re-opening. Implementation of these guidelines should be tailored for each setting. Implementation requires training and support for staff and adequate consideration of camper and family needs. All decisions about following these recommendations should be made in collaboration with local health officials and other authorities, and should depend on the levels of COVID-19 community transmission and the capacities of the local public health and healthcare systems, among other relevant factors.\n\nReview the guidance, prepare a plan, and post the [checklist for day camps](https://files.covid19.ca.gov/pdf/checklist-daycamps--en.pdf) in your facility to show employees, campers, and families that you’ve reduced the risk and are open for operation.  \n  \nRecreational team sports are **not** permitted and will be subject to separate guidance.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C184" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5166,10 +5166,10 @@
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>Manufacturing</v>
+        <v>Delivery services</v>
       </c>
       <c r="B185" t="str">
-        <v>The [guidance for the manufacturing industry](http://covid19.ca.gov/pdf/guidance-manufacturing.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the manufacturing industry](http://covid19.ca.gov/pdf/checklist-manufacturing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the delivery services industry](https://files.covid19.ca.gov/pdf/guidance-delivery-services.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the delivery services industry](https://files.covid19.ca.gov/pdf/checklist-delivery-services.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C185" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5192,10 +5192,10 @@
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>Mining and logging</v>
+        <v>Energy and utilities</v>
       </c>
       <c r="B186" t="str">
-        <v>The [guidance for the mining and logging industries](http://covid19.ca.gov/pdf/guidance-mining-logging.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the mining and logging industries](http://covid19.ca.gov/pdf/checklist-mining-logging.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the energy and utilities industry](https://files.covid19.ca.gov/pdf/guidance-energy.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the energy and utilities industry](https://files.covid19.ca.gov/pdf/checklist-energy.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C186" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5218,10 +5218,10 @@
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>Music, film, and TV production</v>
+        <v>Family friendly practices for employers</v>
       </c>
       <c r="B187" t="str">
-        <v>Music, TV and film production may resume in California, recommended no sooner than June 12, 2020 and subject to approval by county public health officers within the jurisdictions of operations following their review of local epidemiological data including cases per 100,000 population, rate of test positivity, and local preparedness to support a health care surge, vulnerable populations, contact tracing and testing.  \n  \nTo reduce the risk of COVID-19 transmission, productions, cast, crew and other industry workers should abide by safety protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should adhere to [Office Workspace guidelines](https://covid19.ca.gov/industry-guidance/#top) published by the California Department of Public Health and the California Department of Industrial Relations, to reduce the risk of COVID-19 transmission.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for family friendly practices for employers](https://files.covid19.ca.gov/pdf/guidance-familyfriendlypracticesemployers.pdf) provides guidelines for family-friendly practices to keep employees safe and be responsive to their needs in order to ensure continued productivity. As workplaces reopen, employees will require both child care supports and workplace flexibility. Work-life balance policies will become even more important and continued investment in family-friendly workplace policies by employers is critical.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C187" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5244,10 +5244,10 @@
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>Office workspaces</v>
+        <v>Food packing</v>
       </c>
       <c r="B188" t="str">
-        <v>Follow this [guidance for office workspaces](http://covid19.ca.gov/pdf/guidance-office-workspaces.pdf) to create a safer environment for workers.\n\nFaith-based office workspaces can reopen within the following parameters:\n\n1.  Faith-based facilities are considered “offices” only for those employed by the organization and where the facility is their regular place of work.\n2.  The employer should implement state guidance relating to offices before reopening the facility for employees.\n3.  This designation does not permit gatherings of non-employees, such as the organization’s congregation.\n\nReview the guidance, prepare a plan, and post the [checklist for office workspaces](http://covid19.ca.gov/pdf/checklist-office-workspaces.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for facilities that process or pack meat, dairy, or produce](https://files.covid19.ca.gov/pdf/guidance-food-packing.pdf) provides guidelines to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for facilities that process or pack meat, dairy or produce](https://files.covid19.ca.gov/pdf/checklist-food-packing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C188" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5270,10 +5270,10 @@
     </row>
     <row r="189">
       <c r="A189" t="str">
-        <v>Outdoor museums</v>
+        <v>Hotels and lodging</v>
       </c>
       <c r="B189" t="str">
-        <v>Follow this [guidance for outdoor museums](https://covid19.ca.gov/pdf/guidance-outdoor-museums.pdf) to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for outdoor museums](http://covid19.ca.gov/pdf/checklist-outdoor-museums.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Unless your county has been approved to move further in the reopening roadmap, hotels should only open for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or providing housing solutions, including measures to protect homeless populations. Follow this [guidance for hotels and lodging](https://files.covid19.ca.gov/pdf/guidance-hotels.pdf) to create a safer environment for workers and customers.\n\n[Counties that have approval](https://covid19.ca.gov/roadmap-counties/) to move further can reopen hotels, lodging, and short-term rentals for tourism and individual travel. Follow this [guidance for hotels and short term rentals](https://files.covid19.ca.gov/pdf/guidance-hotels-lodging-rentals.pdf) for tourism and individual travel to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for hotels, lodging, and short-term rentals](https://files.covid19.ca.gov/pdf/checklist-hotels.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C189" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5296,10 +5296,10 @@
     </row>
     <row r="190">
       <c r="A190" t="str">
-        <v>Places of worship and cultural ceremonies</v>
+        <v>Life sciences</v>
       </c>
       <c r="B190" t="str">
-        <v>This [guidance for places of worship](http://covid19.ca.gov/pdf/guidance-places-of-worship.pdf) and cultural ceremonies, like weddings and funerals, provides guidelines to create a safer environment for workers and visitors. Guidance last updated July 6, 2020. Review the guidance, prepare a plan, and post the [checklist for places of worship](https://files.covid19.ca.gov/pdf/checklist-places-of-worship.pdf) and cultural ceremonies in your workplace to show workers and visitors that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the life sciences industry](https://files.covid19.ca.gov/pdf/guidance-life-sciences.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the life sciences industry](https://files.covid19.ca.gov/pdf/checklist-life-sciences.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C190" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5322,10 +5322,10 @@
     </row>
     <row r="191">
       <c r="A191" t="str">
-        <v>Ports</v>
+        <v>Limited services</v>
       </c>
       <c r="B191" t="str">
-        <v>This [guidance for the port industry](http://covid19.ca.gov/pdf/guidance-ports.pdf) provides guidelines to create a safer environment for workers. Review the guidance, prepare a plan, and post the [checklist for the port industry](http://covid19.ca.gov/pdf/checklist-ports.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Limited Services are defined as those which do not generally require close contact. Follow this [guidance for Limited Services](https://files.covid19.ca.gov/pdf/guidance-limited-services.pdf) to create a safer environment for workers and patrons.\n\nFaith-based counseling can reopen within the following parameters:\n\n1.  Counseling services are permissible in-person where the service cannot reasonably be practiced remotely;\n2.  Counseling services should adopt state guidance on Limited Services, where applicable;\n3.  This designation does not permit gatherings beyond counseling to members of a single household.\n\nReview the guidance, prepare a plan, and post the [checklist for Limited Services](https://files.covid19.ca.gov/pdf/checklist-limited-services.pdf) in your workplace to show clients and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)&lt;!-- laundromat, dry cleaner, laundry, auto repair, car wash, landscaper, door to door, sales, pet groom, dog walk, entry to private residences, community 2 facilities, residential, janitorial, cleaning services, house keep, house clean, HVAC, appliance repair, electrician, plumbers, mechanical trade, handyperson, handyman, general contractors, lessees, subcontractors --&gt;</v>
       </c>
       <c r="C191" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5348,10 +5348,10 @@
     </row>
     <row r="192">
       <c r="A192" t="str">
-        <v>Professional sports (without live audiences)</v>
+        <v>Logistics and warehousing facilities</v>
       </c>
       <c r="B192" t="str">
-        <v>Professional sports in California may resume training and competition without live audiences, recommended no sooner than June 12, 2020 and subject to approval by county public health officers within the jurisdiction of operations following their review of local epidemiological data including cases per 100,000 population, rate of test positivity, and local preparedness to support a health care surge, vulnerable populations, contact tracing and testing.  \n  \nTo reduce the risk of COVID-19 transmission, athletes, coaching staff, medical staff, broadcasting staff and others at sporting facilities or events should abide by COVID-19 protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should adhere to [Office Workspace guidelines](https://covid19.ca.gov/pdf/guidance-office-workspaces.pdf) published by the California Department of Public Health and the California Department of Industrial Relations, to reduce the risk of COVID-19 transmission. Retail staff should adhere to [Retail guidelines](https://covid19.ca.gov/pdf/guidance-retail.pdf) published by the California Department of Public Health and the California Department of Industrial Relations, to reduce the risk of COVID-19 transmission.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for businesses operating in the logistics/warehousing industry](https://files.covid19.ca.gov/pdf/guidance-logistics-warehousing.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post  the [checklist for the logistics/warehousing industry](https://files.covid19.ca.gov/pdf/checklist-logistics-warehousing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C192" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5374,10 +5374,10 @@
     </row>
     <row r="193">
       <c r="A193" t="str">
-        <v>Public transit and intercity passenger rail</v>
+        <v>Manufacturing</v>
       </c>
       <c r="B193" t="str">
-        <v>This [guidance for public transit agencies](http://covid19.ca.gov/pdf/guidance-transit-rail.pdf) provides guidelines to create a safer environment for workers and customers.  \nReview the guidance, prepare a plan, and post the [checklist for public transit agencies](http://covid19.ca.gov/pdf/checklist-transit-rail.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the manufacturing industry](https://files.covid19.ca.gov/pdf/guidance-manufacturing.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the manufacturing industry](https://files.covid19.ca.gov/pdf/checklist-manufacturing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C193" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5400,10 +5400,10 @@
     </row>
     <row r="194">
       <c r="A194" t="str">
-        <v>Real estate transaction</v>
+        <v>Mining and logging</v>
       </c>
       <c r="B194" t="str">
-        <v>This [guidance for businesses operating in the real estate industry](http://covid19.ca.gov/pdf/guidance-real-estate.pdf) provides guidelines to create a safer environment for workers.  \nReview the guidance, prepare a plan, and post the [checklist for the real estate industry](http://covid19.ca.gov/pdf/checklist-real-estate.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [guidance for the mining and logging industries](https://files.covid19.ca.gov/pdf/guidance-mining-logging.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the mining and logging industries](https://files.covid19.ca.gov/pdf/checklist-mining-logging.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C194" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5426,10 +5426,10 @@
     </row>
     <row r="195">
       <c r="A195" t="str">
-        <v>Retail</v>
+        <v>Music, film, and TV production</v>
       </c>
       <c r="B195" t="str">
-        <v>Follow this [guidance for retailers](http://covid19.ca.gov/pdf/guidance-retail.pdf) to create a safer environment for workers and customers.\n\nRetailers and libraries can re-open, along with the manufacturing and logistics sectors that support retail. Drive-in and movie theaters can re-open with additional considerations.\n\nRetail doesn’t include personal services such as beauty salons, but does include the sale of goods such as:\n\n*   Bookstores\n*   Jewelry stores\n*   Toy stores\n*   Clothing and shoe stores\n*   Home and furnishing stores\n*   Sporting goods stores\n*   Florists\n\nRetail stores identified in the [essential workforce list](https://covid19.ca.gov/essential-workforce/) can open for in-store shopping. They include:\n\n*   Retail facilities specializing in medical goods and supplies\n*   Grocery stores, pharmacies, convenience stores, and other retail that sells food or beverage products, and animal/pet food\n*   Fuel centers such as gas stations and truck stops\n*   Hardware and building materials stores, consumer electronics, technology and appliances retail\n\nReview the guidance, prepare a plan, and post the [checklist for retail](http://covid19.ca.gov/pdf/checklist-retail.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Music, TV, and film production may resume, subject to approval by county public health officers. They will review local epidemiological data, including cases per 100,000 people, rate of test positivity, local preparedness to support a health care surge, vulnerable populations, contact tracing and testing.  \n  \nTo reduce the risk of COVID-19 transmission, productions, cast, crew and other industry workers should abide by safety protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should follow the [guidance for office workspaces](https://files.covid19.ca.gov/pdf/guidance-office-workspaces.pdf).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C195" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5452,10 +5452,10 @@
     </row>
     <row r="196">
       <c r="A196" t="str">
-        <v>Schools – Updated July 20</v>
+        <v>Office workspaces</v>
       </c>
       <c r="B196" t="str">
-        <v>This [updated guidance for schools and school-based programs](http://covid19.ca.gov/pdf/guidance-schools.pdf) provides guidelines for in-person learning and distance learning. This guidance will be updated as new data and practices emerge. The guidelines and considerations do not reflect the full scope of issues that school communities will need to address, which range from day-to-day site-based logistics to the social and emotional well-being of students and staff. Further guidance is forthcoming, including on school-based sports and extracurricular activities. All decisions about following this guidance should be made in collaboration with local health officials and other authorities. Review the guidance, prepare a plan, and post the [checklist for schools](https://files.covid19.ca.gov/pdf/checklist-schools--en.pdf) in your facility to show employees, students, and families that you’ve reduced the risk and are open for operation.\n\nSchools have been closed for in-person instruction since mid-March 2020 due to the COVID-19 pandemic. School closures to in-person instruction were part of a broader set of recommendations intended to reduce the spread of COVID-19. For more detailed direction on measures to be taken when a student, teacher, or staff member has symptoms or is diagnosed with COVID-19, please see the [COVID-19 and Reopening Framework for K-12 Schools in California](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Schools%20Reopening%20Recommendations.pdf).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for office workspaces](https://files.covid19.ca.gov/pdf/guidance-office-workspaces.pdf) to create a safer environment for workers.\n\nFaith-based office workspaces can reopen within the following parameters:\n\n1.  Faith-based facilities are considered “offices” only for those employed by the organization and where the facility is their regular place of work.\n2.  The employer should implement state guidance relating to offices before reopening the facility for employees.\n3.  This designation does not permit gatherings of non-employees, such as the organization’s congregation.\n\n**For counties on the** [**Monitoring List**](https://covid19.ca.gov/roadmap-counties/#affected-counties)**:**\n\n**Indoor** operations of offices for non-essential non-critical infrastructure must be closed. \n\nReview the guidance, prepare a plan, and post the [checklist for office workspaces](https://files.covid19.ca.gov/pdf/checklist-office-workspaces.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C196" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5478,10 +5478,10 @@
     </row>
     <row r="197">
       <c r="A197" t="str">
-        <v>Support for working families</v>
+        <v>Outdoor museums</v>
       </c>
       <c r="B197" t="str">
-        <v>The [support for working families](http://files.covid19.ca.gov/pdf/guidance-supportworkingfamilies--en.pdf) guidance provides information to help you locate child care, find assistance to pay for child care, and connect you to additional supports for your family. As stay-at-home orders are lifted for additional industries to promote California’s economic recovery, the need for child care and other supports for working families increases.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for outdoor museums](https://files.covid19.ca.gov/pdf/guidance-outdoor-museums.pdf), open air galleries, botanical gardens, and other outdoor exhibition spaces to create a safer environment for workers and patrons. This guidance is not intended for zoos, amusement parks, or indoor gallery and museum spaces.\n\nReview the guidance, prepare a plan, and post the [checklist for outdoor museums](https://files.covid19.ca.gov/pdf/checklist-outdoor-museums.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C197" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5504,10 +5504,10 @@
     </row>
     <row r="198">
       <c r="A198" t="str">
-        <v>Shopping centers</v>
+        <v>Places of worship and cultural ceremonies</v>
       </c>
       <c r="B198" t="str">
-        <v>Follow this [guidance for shopping centers](https://covid19.ca.gov/pdf/guidance-shopping-centers.pdf) to create a safer environment for workers and customers.  \n  \nInterior stores in shopping malls can do curbside pickup with modifications.  \n  \nReview the guidance, prepare a plan, and post the [checklist for shopping centers](https://covid19.ca.gov/pdf/checklist-shopping-centers.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [guidance for places of worship](https://files.covid19.ca.gov/pdf/guidance-places-of-worship.pdf) and providers of religious services and cultural ceremonies, like weddings and funerals, provides guidelines to create a safer environment for workers and visitors.\n\n**For counties on the** [**Monitoring List**](https://covid19.ca.gov/roadmap-counties/#affected-counties)**:**\n\n**Indoor** operations must be closed. \n\nReview the guidance, prepare a plan, and post the [checklist for places of worship](https://files.covid19.ca.gov/pdf/checklist-places-of-worship.pdf) and cultural ceremonies in your workplace to show workers and visitors that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C198" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5530,10 +5530,10 @@
     </row>
     <row r="199">
       <c r="A199" t="str">
-        <v>Take-out restaurants</v>
+        <v>Ports</v>
       </c>
       <c r="B199" t="str">
-        <v>Follow this [guidance for restaurants providing take-out, drive-through, and delivery](https://files.covid19.ca.gov/pdf/guidance-takeout-restaurants.pdf) to create a safer environment for workers and patrons. Review the guidance and prepare a plan in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [guidance for the port industry](https://files.covid19.ca.gov/pdf/guidance-ports.pdf) provides guidelines to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for the port industry](https://files.covid19.ca.gov/pdf/checklist-ports.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C199" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5556,10 +5556,10 @@
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>Dine-in restaurants</v>
+        <v>Professional sports (without live audiences)</v>
       </c>
       <c r="B200" t="str">
-        <v>This [guidance for dine-in restaurants](https://covid19.ca.gov/pdf/guidance-dine-in-restaurants.pdf) provides guidelines to create a safer environment for workers and customers.  \nReview the guidance, prepare a plan, and post the [checklist for dine-in restaurants](https://covid19.ca.gov/pdf/checklist-dine-in-restaurants.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Professional sports may resume training and competition without live audiences, subject to approval by county public health officers. They will review local epidemiological data, including cases per 100,000 people, rate of test positivity, local preparedness to support a health care surge, vulnerable populations, contact tracing and testing.  \n  \nTo reduce the risk of COVID-19 transmission, athletes, coaching staff, medical staff, broadcasting staff and others at sporting facilities or events should abide by COVID-19 protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should follow the [guidance for office workspaces](https://files.covid19.ca.gov/pdf/guidance-office-workspaces.pdf).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C200" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5582,10 +5582,10 @@
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>Hair salons and barbershops</v>
+        <v>Public transit and intercity passenger rail</v>
       </c>
       <c r="B201" t="str">
-        <v>This [guidance for hair salons and barbershops](https://covid19.ca.gov/pdf/guidance-hair-salons.pdf) provides guidelines to create a safer environment for workers and customers. Review the guidance, prepare a plan, and post the [checklist for hair salons](https://files.covid19.ca.gov/pdf/checklist-hair-salons.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nFor counties that have been on the Monitoring List for 3 consecutive days, find guidance for providing hair services outdoors in the list of [guidance for counties on the Monitoring List](https://covid19.ca.gov/industry-guidance/#guidance-monitor).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [guidance for public transit agencies](https://files.covid19.ca.gov/pdf/guidance-transit-rail.pdf) provides guidelines to create a safer environment for workers and customers.\n\nReview the guidance, prepare a plan, and post the [checklist for public transit agencies](https://files.covid19.ca.gov/pdf/checklist-transit-rail.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C201" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5608,10 +5608,10 @@
     </row>
     <row r="202">
       <c r="A202" t="str">
-        <v>Casinos</v>
+        <v>Real estate transaction</v>
       </c>
       <c r="B202" t="str">
-        <v>In working with tribal governments, CDPH and DIR have released guidance on how to reopen casinos with reduced risk of transmission. Tribal governments should make determinations on when to reopen based on how they align with the current local public health conditions and the statewide stage of reopening and the Governor respectfully requests that until a surrounding or neighboring local jurisdiction has progressed into Stage 3, tribal casinos remain closed.\n\nFollow this [guidance for casinos](https://covid19.ca.gov/pdf/guidance-casinos.pdf) to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for casinos](https://files.covid19.ca.gov/pdf/checklist-casinos.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [guidance for businesses operating in the real estate industry](https://files.covid19.ca.gov/pdf/guidance-real-estate.pdf) provides guidelines to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for the real estate industry](https://files.covid19.ca.gov/pdf/checklist-real-estate.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C202" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5634,10 +5634,10 @@
     </row>
     <row r="203">
       <c r="A203" t="str">
-        <v>Movie theaters and family entertainment centers</v>
+        <v>Retail</v>
       </c>
       <c r="B203" t="str">
-        <v>Follow this guidance for [movie theaters and family entertainment centers](http://covid19.ca.gov/pdf/guidance-family-entertainment.pdf) to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for movie theaters and family entertainment centers](https://files.covid19.ca.gov/pdf/checklist-family-entertainment.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for retailers](https://files.covid19.ca.gov/pdf/guidance-retail.pdf) to create a safer environment for workers and customers.\n\nReview the guidance, prepare a plan, and post the [checklist for retail](https://files.covid19.ca.gov/pdf/checklist-retail.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nRetailers and libraries can re-open, along with the manufacturing and logistics sectors that support retail. Drive-in and movie theaters can re-open with additional considerations.\n\nRetail doesn’t include personal services such as beauty salons, but does include the sale of goods such as:\n\n*   Bookstores\n*   Jewelry stores\n*   Toy stores\n*   Clothing and shoe stores\n*   Home and furnishing stores\n*   Sporting goods stores\n*   Florists\n\nRetail stores identified in the [essential workforce list](https://covid19.ca.gov/essential-workforce/) can open for in-store shopping. They include:\n\n*   Retail facilities specializing in medical goods and supplies\n*   Grocery stores, pharmacies, convenience stores, and other retail that sells food or beverage products, and animal/pet food\n*   Fuel centers such as gas stations and truck stops\n*   Hardware and building materials stores, consumer electronics, technology and appliances retail\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C203" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5660,10 +5660,10 @@
     </row>
     <row r="204">
       <c r="A204" t="str">
-        <v>Restaurants, wineries, and bars</v>
+        <v>Schools</v>
       </c>
       <c r="B204" t="str">
-        <v>Follow this [guidance for restaurants, wineries, and bars](http://covid19.ca.gov/pdf/guidance-restaurants-bars.pdf) to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for restaurants, wineries, and bars](https://files.covid19.ca.gov/pdf/checklist-restaurants-bars.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [updated guidance for schools and school-based programs](https://files.covid19.ca.gov/pdf/guidance-schools.pdf) provides guidelines for in-person learning and distance learning. This guidance will be updated as new data and practices emerge. The guidelines and considerations do not reflect the full scope of issues that school communities will need to address, which range from day-to-day site-based logistics to the social and emotional well-being of students and staff. Further guidance is forthcoming, including on school-based sports and extracurricular activities. All decisions about following this guidance should be made in collaboration with local health officials and other authorities. Review the guidance, prepare a plan, and post the [checklist for schools](https://files.covid19.ca.gov/pdf/checklist-schools--en.pdf) in your facility to show employees, students, and families that you’ve reduced the risk and are open for operation.\n\nSchools have been closed for in-person instruction since mid-March 2020 due to the COVID-19 pandemic. School closures to in-person instruction were part of a broader set of recommendations intended to reduce the spread of COVID-19. For more detailed direction on measures to be taken when a student, teacher, or staff member has symptoms or is diagnosed with COVID-19, please see the [COVID-19 and Reopening Framework for K-12 Schools in California](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Schools%20Reopening%20Recommendations.pdf).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C204" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5686,10 +5686,10 @@
     </row>
     <row r="205">
       <c r="A205" t="str">
-        <v>Zoos and museums</v>
+        <v>Support for working families</v>
       </c>
       <c r="B205" t="str">
-        <v>Follow this [guidance for zoos, museums](http://covid19.ca.gov/pdf/guidance-zoos-museums.pdf), galleries, and aquariums to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for zoos, museums](https://files.covid19.ca.gov/pdf/checklist-zoos-museums.pdf), galleries, and aquariums in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [support for working families](https://files.covid19.ca.gov/pdf/guidance-supportworkingfamilies--en.pdf) guidance provides information to help you locate child care, find assistance to pay for child care, and connect you to additional supports for your family. As stay-at-home orders are lifted for additional industries to promote California’s economic recovery, the need for child care and other supports for working families increases.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C205" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5712,10 +5712,10 @@
     </row>
     <row r="206">
       <c r="A206" t="str">
-        <v>Gyms and fitness centers</v>
+        <v>Shopping centers</v>
       </c>
       <c r="B206" t="str">
-        <v>Follow this [guidance for gyms and fitness centers](https://files.covid19.ca.gov/pdf/guidance-fitness--en.pdf), including yoga and dance studios, to create a safer environment for workers and patrons. Guidance last updated July 1, 2020. Review the guidance, prepare a plan, and post the [checklist for gyms and fitness centers](https://files.covid19.ca.gov/pdf/checklist-fitness.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.  \n  \nRecreational team sports are not permitted and will be subject to separate guidance.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for shopping centers](https://files.covid19.ca.gov/pdf/guidance-shopping-centers.pdf), destination shopping centers, strip and outlet malls, and swap meets to create a safer environment for workers and customers. Interior stores in shopping malls can do curbside pickup with modifications. \n\n**For counties on the** [**Monitoring List**](https://covid19.ca.gov/roadmap-counties/#affected-counties)**:**\n\n**Indoor** operations must be closed. \n\nReview the guidance, prepare a plan, and post the [checklist for shopping centers](https://files.covid19.ca.gov/pdf/checklist-shopping-centers.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C206" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5738,10 +5738,10 @@
     </row>
     <row r="207">
       <c r="A207" t="str">
-        <v>Hotels (for tourism and individual travel)</v>
+        <v>Take-out restaurants</v>
       </c>
       <c r="B207" t="str">
-        <v>Follow this [guidance for hotels and short term rentals](https://covid19.ca.gov/pdf/guidance-hotels-lodging-rentals.pdf) for tourism and individual travel to create a safer environment for workers and patrons.\n\nThis guidance is applicable only within counties with variance attestation. Hotel and lodging services in all other counties should adhere to the guidance limitations provided by [statewide guidance](https://covid19.ca.gov/pdf/guidance-hotels.pdf), where hotels should only open for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or providing housing solutions, including measures to protect homeless populations.\n\nReview the guidance, prepare a plan, and post the [checklist for hotels and lodging](http://covid19.ca.gov/pdf/checklist-hotels.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)&lt;!-- motel, vacation, airbnb, vrbo, rental home --&gt;</v>
+        <v>Follow this [guidance for restaurants providing take-out, drive-through, and delivery](https://files.covid19.ca.gov/pdf/guidance-takeout-restaurants.pdf) to create a safer environment for workers and patrons. Review the guidance and prepare a plan for your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C207" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5764,10 +5764,10 @@
     </row>
     <row r="208">
       <c r="A208" t="str">
-        <v>Cardrooms and racetracks</v>
+        <v>Dine-in restaurants</v>
       </c>
       <c r="B208" t="str">
-        <v>Follow this [guidance for cardrooms](https://covid19.ca.gov/pdf/guidance-cardrooms-racetracks.pdf), race tracks, and satellite wagering to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for cardrooms](https://files.covid19.ca.gov/pdf/checklist-cardrooms-racetracks.pdf), race tracks, and satellite wagering in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>This [guidance for dine-in restaurants](https://files.covid19.ca.gov/pdf/guidance-dine-in-restaurants.pdf) provides guidelines to create a safer environment for workers and customers. **Indoor** operations for dine-in restaurants must be closed in **all** counties. Bars, brewpubs, breweries, and pubs must close both **indoor and outdoor** operations in **all** counties unless they are offering sit-down, outdoor dine-in meals. Alcohol can only be sold in the same transaction as a meal.\n\n**For counties on the** [**Monitoring List**](https://covid19.ca.gov/roadmap-counties/#affected-counties)**:**\n\n**Indoor** operations must be closed. Follow this [guidance for restaurants providing outdoor dining, take-out, drive-through, and delivery](https://files.covid19.ca.gov/pdf/guidance-outdoor-restaurants.pdf) to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for dine-in restaurants](https://files.covid19.ca.gov/pdf/checklist-dine-in-restaurants.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C208" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5790,10 +5790,10 @@
     </row>
     <row r="209">
       <c r="A209" t="str">
-        <v>Campgrounds and outdoor recreation</v>
+        <v>Hair salons and barbershops</v>
       </c>
       <c r="B209" t="str">
-        <v>Follow this [guidance for campgrounds](http://covid19.ca.gov/pdf/guidance-campgrounds.pdf) to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the checklist for campgrounds in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)&lt;!-- park, visitor center, travel, museum, recreation, outdoor recreation, sports, RV, tent, camp, fish, beach, lake, river, event, wedding, hike, walk, bike, exercise, nature, birdwatch, guided, tour, hunt, boat, cabin, bonfire, campsite, amphitheater, sport, court, rental, public, trail, marina, bonfire, campsite,  --&gt;</v>
+        <v>This [guidance for hair salons and barbershops](https://files.covid19.ca.gov/pdf/guidance-hair-salons.pdf) provides guidelines to create a safer environment for workers and customers. Review the guidance, prepare a plan, and post the [checklist for hair salons](https://files.covid19.ca.gov/pdf/checklist-hair-salons.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\n**For counties on the** [**Monitoring List**](https://covid19.ca.gov/roadmap-counties/#affected-counties)**:**\n\nHair services provided **indoors** must be closed. Follow this [guidance for hair salons and barbershops providing outdoor services](https://files.covid19.ca.gov/pdf/guidance-outdoor-hair-salons--en.pdf) to support an outdoor safe, clean environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for hair salons providing services outdoors](https://files.covid19.ca.gov/pdf/checklist-outdoor-hair-salons--en.pdf) at your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C209" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5816,10 +5816,10 @@
     </row>
     <row r="210">
       <c r="A210" t="str">
-        <v>Personal care services</v>
+        <v>Casinos</v>
       </c>
       <c r="B210" t="str">
-        <v>Follow this [guidance for personal care services](https://files.covid19.ca.gov/pdf/expanded-personal-services--en.pdf) like nail salons, tattoo parlors, and body waxing to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for personal care services](https://files.covid19.ca.gov/pdf/checklist-expanded-personal-care-services.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nFor counties that have been on the Monitoring List for 3 consecutive days, find guidance for providing some personal care services outdoors in the list of [guidance for counties on the Monitoring List](https://covid19.ca.gov/industry-guidance/#guidance-monitor).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>In working with tribal governments, CDPH and DIR have released guidance on how to reopen casinos with reduced risk of transmission. Tribal governments should make determinations on when to reopen based on how they align with the current local public health conditions and the statewide stage of reopening and the Governor respectfully requests that until a surrounding or neighboring local jurisdiction has progressed into Stage 3, tribal casinos remain closed.\n\nFollow this [guidance for casinos](https://files.covid19.ca.gov/pdf/guidance-casinos.pdf) to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for casinos](https://files.covid19.ca.gov/pdf/checklist-casinos.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C210" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5842,10 +5842,10 @@
     </row>
     <row r="211">
       <c r="A211" t="str">
-        <v>Outdoor dining</v>
+        <v>Movie theaters and family entertainment centers</v>
       </c>
       <c r="B211" t="str">
-        <v>Follow this [guidance for restaurants providing outdoor dining, take-out, drive-through, and delivery](https://files.covid19.ca.gov/pdf/guidance-outdoor-restaurants.pdf) to create a safer environment for workers and patrons. Review the guidance and prepare a plan in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this guidance for [movie theaters and family entertainment centers](https://files.covid19.ca.gov/pdf/guidance-family-entertainment.pdf), like bowling alleys, miniature golf, batting cages, and arcades, to create a safer environment for workers and patrons. **Indoor** operations must be closed in **all** counties.\n\nReview the guidance, prepare a plan, and post the [checklist for movie theaters and family entertainment centers](https://files.covid19.ca.gov/pdf/checklist-family-entertainment.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C211" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5868,10 +5868,10 @@
     </row>
     <row r="212">
       <c r="A212" t="str">
-        <v>Outdoor services for hair salons and barbershops</v>
+        <v>Restaurants, wineries, and bars</v>
       </c>
       <c r="B212" t="str">
-        <v>Follow this [guidance for hair salons and barbershops providing services outdoors](https://files.covid19.ca.gov/pdf/guidance-outdoor-hair-salons--en.pdf) to support an outdoor safe, clean environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for hair salons providing services outdoors](https://files.covid19.ca.gov/pdf/checklist-outdoor-hair-salons--en.pdf) at your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for restaurants, wineries, and bars](https://files.covid19.ca.gov/pdf/guidance-restaurants-bars.pdf) to create a safer environment for workers and patrons. **Indoor** operations for dine-in restaurants, wineries, and tasting rooms must be closed in **all** counties. Bars, brewpubs, breweries, and pubs must close both **indoor and outdoor** operations in **all** counties unless they are offering sit-down, outdoor dine-in meals. Alcohol can only be sold in the same transaction as a meal.\n\n**For counties on the** [**Monitoring List**](https://covid19.ca.gov/roadmap-counties/#affected-counties)**:**\n\n**Indoor** operations must be closed. Follow this [guidance for restaurants providing outdoor dining, take-out, drive-through, and delivery](https://files.covid19.ca.gov/pdf/guidance-outdoor-restaurants.pdf) to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for restaurants, wineries, and bars](https://files.covid19.ca.gov/pdf/checklist-restaurants-bars.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C212" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5894,10 +5894,10 @@
     </row>
     <row r="213">
       <c r="A213" t="str">
-        <v>Outdoor services for personal care services</v>
+        <v>Zoos and museums</v>
       </c>
       <c r="B213" t="str">
-        <v>Follow this [guidance for personal care services provided outdoors](https://files.covid19.ca.gov/pdf/guidance-outdoor-personal-care--en.pdf) to support an outdoor safe, clean environment for workers and patrons. This guidance applies to services that require touching a client’s face, like facials and waxing. This guidance also applies to esthetic services, skin care, cosmetology, nail services, and massage therapy. Review the guidance, prepare a plan, and post the [checklist for personal care services provided outdoors](https://files.covid19.ca.gov/pdf/checklist-outdoor-personal-care--en.pdf) at your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for zoos, museums](https://files.covid19.ca.gov/pdf/guidance-zoos-museums.pdf), galleries, botanical gardens, and aquariums to create a safer environment for workers and patrons. **Indoor** operations must be closed in **all** counties. Review the guidance, prepare a plan, and post the [checklist for zoos, museums](https://files.covid19.ca.gov/pdf/checklist-zoos-museums.pdf), galleries, and aquariums in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nIf your county hasn’t been approved to move further in the reopening roadmap, follow this [guidance for outdoor museums](https://files.covid19.ca.gov/pdf/guidance-outdoor-museums.pdf), open air galleries, botanical gardens, and other outdoor exhibition spaces to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for outdoor museums](https://files.covid19.ca.gov/pdf/checklist-outdoor-museums.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C213" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5920,13 +5920,13 @@
     </row>
     <row r="214">
       <c r="A214" t="str">
-        <v>Is there a convalescent blood plasma donation center near me?</v>
+        <v>Gyms and fitness centers</v>
       </c>
       <c r="B214" t="str">
-        <v>Locate a donation center\n------------------------\n\nFind the blood center near you collecting COVID-19 blood plasma.\n\n[See the plasma donation center lookup](https://covid19.ca.gov/plasma#plasma-lookup)\n\nMore info: [Survivors of COVID-19: Donate your plasma](https://covid19.ca.gov/plasma/)</v>
+        <v>Follow this [guidance for gyms and fitness centers](https://files.covid19.ca.gov/pdf/guidance-fitness--en.pdf), including yoga and dance studios, to create a safer environment for workers and patrons. Recreational team sports are **not** permitted and will be subject to separate guidance.\n\n**For counties on the** [**Monitoring List**](https://covid19.ca.gov/roadmap-counties/#affected-counties)**:**\n\n**Indoor** operations must be closed. \n\nReview the guidance, prepare a plan, and post the [checklist for gyms and fitness centers](https://files.covid19.ca.gov/pdf/checklist-fitness.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C214" t="str">
-        <v>https://covid19.ca.gov/plasma/</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D214" t="str">
         <v xml:space="preserve"> </v>
@@ -5946,13 +5946,13 @@
     </row>
     <row r="215">
       <c r="A215" t="str">
-        <v>Where can I apply for unemployment?</v>
+        <v>Hotels (for tourism and individual travel)</v>
       </c>
       <c r="B215" t="str">
-        <v>If you lost your job or had your hours reduced, and meet eligibility requirements, you may be eligible to receive Unemployment Insurance (UI) benefits from California’s Employment Development Department (EDD). Check the [guide to applying for unemployment benefits](https://unemployment.edd.ca.gov/guide).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>Follow this [guidance for hotels and short term rentals](https://files.covid19.ca.gov/pdf/guidance-hotels-lodging-rentals.pdf) for tourism and individual travel to create a safer environment for workers and patrons.\n\nIf your county hasn’t been approved to move further in the reopening roadmap, hotels should only open for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or providing housing solutions, including measures to protect homeless populations. Follow this [guidance for hotels and lodging](https://files.covid19.ca.gov/pdf/guidance-hotels.pdf) to create a safer environment for workers and customers.\n\nReview the guidance, prepare a plan, and post the [checklist for hotels, lodging, and short-term rentals](https://files.covid19.ca.gov/pdf/checklist-hotels.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C215" t="str">
-        <v>Editorial</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D215" t="str">
         <v xml:space="preserve"> </v>
@@ -5972,13 +5972,13 @@
     </row>
     <row r="216">
       <c r="A216" t="str">
-        <v>Are hotels allowed to open?</v>
+        <v>Cardrooms and racetracks</v>
       </c>
       <c r="B216" t="str">
-        <v>[Counties that have received approval from the State](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/County_Variance_Attestation_Form.aspx) may open hotels, lodging and short term rentals for tourism and individual travel as long as they follow [state guidance](https://covid19.ca.gov/pdf/guidance-hotels-lodging-rentals.pdf) for public health and safety. Large meeting venues, banquet halls or convention centers should remain closed. All other counties [should only open hotels and lodging](https://covid19.ca.gov/pdf/guidance-hotels.pdf) for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or housing solutions, including measures to protect homeless populations. &lt;!-- motel, vacation, airbnb, vrbo, rental home --&gt;</v>
+        <v>Follow this [guidance for cardrooms](https://files.covid19.ca.gov/pdf/guidance-cardrooms-racetracks.pdf), racetracks, and satellite wagering to create a safer environment for workers and patrons. **Indoor** operations at cardrooms must be closed in **all** counties. Racetracks may only operate without spectators.\n\nReview the guidance, prepare a plan, and post the [checklist for cardrooms](https://files.covid19.ca.gov/pdf/checklist-cardrooms-racetracks.pdf), racetracks, and satellite wagering in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C216" t="str">
-        <v>Editorial</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D216" t="str">
         <v xml:space="preserve"> </v>
@@ -5998,13 +5998,13 @@
     </row>
     <row r="217">
       <c r="A217" t="str">
-        <v>Can my pet test positive for coronavirus? Can I take my pet to the vet?</v>
+        <v>Campgrounds and outdoor recreation</v>
       </c>
       <c r="B217" t="str">
-        <v>While we are still learning about coronavirus, the risk of your pet testing positive for coronavirus is low. Because [there is still a risk](https://www.cdc.gov/coronavirus/2019-ncov/animals/pets-other-animals.html), keep your pets away from other pets and people outside of your household. Do not put face coverings on pets as this could harm your pet.\n\nYou can go to the vet or pet hospital if your pet is sick. Remember to wear a cloth face covering and to distance yourself at least 6 feet from other pets and owners.</v>
+        <v>Follow this [guidance for campgrounds](https://files.covid19.ca.gov/pdf/guidance-campgrounds.pdf), RV parks, and outdoor recreation to create a safer environment for workers and patrons. Review the guidance and prepare a plan for your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C217" t="str">
-        <v>Editorial</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D217" t="str">
         <v xml:space="preserve"> </v>
@@ -6024,13 +6024,13 @@
     </row>
     <row r="218">
       <c r="A218" t="str">
-        <v>What is Larry David's advice?</v>
+        <v>Personal care services</v>
       </c>
       <c r="B218" t="str">
-        <v>&lt;blockquote class="twitter-tweet"&gt;&lt;p lang="en" dir="ltr"&gt;“You’re hurting old people like me. Well, not me... I’ll never see you.”&lt;br&gt;&lt;br&gt;Larry David wants everyone to stay home to protect older Californians from &lt;a href="https://twitter.com/hashtag/COVID19?src=hash&amp;amp;ref_src=twsrc%5Etfw"&gt;#COVID19&lt;/a&gt;! &lt;br&gt;He does not do these things. &lt;br&gt;Listen to Larry.&lt;a href="https://twitter.com/hashtag/StayHomeSaveLives?src=hash&amp;amp;ref_src=twsrc%5Etfw"&gt;#StayHomeSaveLives&lt;/a&gt;&lt;a href="https://t.co/snYe5v55Rw"&gt;https://t.co/snYe5v55Rw&lt;/a&gt; &lt;a href="https://t.co/C5cKOaAufE"&gt;pic.twitter.com/C5cKOaAufE&lt;/a&gt;&lt;/p&gt;&amp;mdash; Office of the Governor of California (@CAgovernor) &lt;a href="https://twitter.com/CAgovernor/status/1245110728199045120?ref_src=twsrc%5Etfw"&gt;March 31, 2020&lt;/a&gt;&lt;/blockquote&gt; &lt;script async src="https://platform.twitter.com/widgets.js" charset="utf-8"&gt;&lt;/script&gt;</v>
+        <v>Follow this [guidance for personal care services](https://files.covid19.ca.gov/pdf/expanded-personal-services--en.pdf) like nail salons, tattoo parlors, and body waxing to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for personal care services](https://files.covid19.ca.gov/pdf/checklist-expanded-personal-care-services.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\n**For counties on the** [**Monitoring List**](https://covid19.ca.gov/roadmap-counties/#affected-counties)**:**\n\n*   **Indoor** operations of nail salons, skin care, waxing, and massage must be closed. \n*   **All indoor and outdoor** services for tattooing, piercing, and electrolysis must be closed.\n*   Some services may be provided **outdoors**, like nails and massage. Follow this [guidance for personal care services provided outdoors](https://files.covid19.ca.gov/pdf/guidance-outdoor-personal-care--en.pdf) to support an outdoor safe, clean environment for workers and patrons. This guidance applies to services that require touching a client’s face, like facials and waxing. This guidance also applies to esthetic services, skin care, cosmetology, nail services, and massage therapy. Review the guidance, prepare a plan, and post the [checklist for personal care services provided outdoors](https://files.covid19.ca.gov/pdf/checklist-outdoor-personal-care--en.pdf) at your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C218" t="str">
-        <v>Editorial</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D218" t="str">
         <v xml:space="preserve"> </v>
@@ -6050,13 +6050,13 @@
     </row>
     <row r="219">
       <c r="A219" t="str">
-        <v xml:space="preserve">Can I go to the movies? </v>
+        <v>Is there a convalescent blood plasma donation center near me?</v>
       </c>
       <c r="B219" t="str">
-        <v xml:space="preserve">Effective July 13, 2020, indoor movie theaters are closed in all counties. Drive-in movie theaters with modifications to support physical distancing may be open.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) </v>
+        <v>Locate a donation center\n------------------------\n\nFind the blood center near you collecting COVID-19 blood plasma.\n\n[See the plasma donation center lookup](https://covid19.ca.gov/plasma#plasma-lookup)\n\nMore info: [Survivors of COVID-19: Donate your plasma](https://covid19.ca.gov/plasma/)</v>
       </c>
       <c r="C219" t="str">
-        <v>Editorial</v>
+        <v>https://covid19.ca.gov/plasma/</v>
       </c>
       <c r="D219" t="str">
         <v xml:space="preserve"> </v>
@@ -6076,10 +6076,10 @@
     </row>
     <row r="220">
       <c r="A220" t="str">
-        <v>Can I go to a restaurant? Can I go to a winery or a brewery?</v>
+        <v>Where can I apply for unemployment?</v>
       </c>
       <c r="B220" t="str">
-        <v xml:space="preserve">Indoor operations of all dine-in restaurants are closed in all counties. Restaurants across the state can be open for take out, drive through, delivery, and outdoor dining. \n\nIndoor operations for wineries and tasting rooms are closed in all counties. All bars, brewpubs, breweries, and pubs are closed statewide for both indoor and outdoor operations, unless they offer sit-down, outdoor dine-in meals. Alcohol can only be sold in the same transaction as a meal.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) </v>
+        <v>If you lost your job or had your hours reduced, and meet eligibility requirements, you may be eligible to receive Unemployment Insurance (UI) benefits from California’s Employment Development Department (EDD). Check the [guide to applying for unemployment benefits](https://unemployment.edd.ca.gov/guide).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C220" t="str">
         <v>Editorial</v>
@@ -6102,10 +6102,10 @@
     </row>
     <row r="221">
       <c r="A221" t="str">
-        <v>Are restaurants allowed to open?</v>
+        <v>Are hotels allowed to open?</v>
       </c>
       <c r="B221" t="str">
-        <v xml:space="preserve">Restaurants across the state can be open for [take out, drive through, and delivery](https://files.covid19.ca.gov/pdf/guidance-takeout-restaurants.pdf). Indoor operations for dine-in restaurants are closed in all counties. Bars, brewpubs, breweries, and pubs must close both indoor and outdoor operations unless they are offering [sit-down, outdoor dine-in meals](https://files.covid19.ca.gov/pdf/guidance-outdoor-restaurants.pdf). Alcohol can only be sold in the same transaction as a meal.\n\nMore info: [Industry guidance](https://covid19.ca.gov/industry-guidance/) and [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) </v>
+        <v>[Counties that have received approval from the State](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/County_Variance_Attestation_Form.aspx) may open hotels, lodging and short term rentals for tourism and individual travel as long as they follow [state guidance](https://covid19.ca.gov/pdf/guidance-hotels-lodging-rentals.pdf) for public health and safety. Large meeting venues, banquet halls or convention centers should remain closed. All other counties [should only open hotels and lodging](https://covid19.ca.gov/pdf/guidance-hotels.pdf) for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or housing solutions, including measures to protect homeless populations. &lt;!-- motel, vacation, airbnb, vrbo, rental home --&gt;</v>
       </c>
       <c r="C221" t="str">
         <v>Editorial</v>
@@ -6128,10 +6128,10 @@
     </row>
     <row r="222">
       <c r="A222" t="str">
-        <v>Where can I find the list of essential critical infrastructure sectors?</v>
+        <v>Can my pet test positive for coronavirus? Can I take my pet to the vet?</v>
       </c>
       <c r="B222" t="str">
-        <v xml:space="preserve">Visit [Essential workforce](https://covid19.ca.gov/essential-workforce/) to learn about what workers and sectors are included. </v>
+        <v>While we are still learning about coronavirus, the risk of your pet testing positive for coronavirus is low. Because [there is still a risk](https://www.cdc.gov/coronavirus/2019-ncov/animals/pets-other-animals.html), keep your pets away from other pets and people outside of your household. Do not put face coverings on pets as this could harm your pet.\n\nYou can go to the vet or pet hospital if your pet is sick. Remember to wear a cloth face covering and to distance yourself at least 6 feet from other pets and owners.</v>
       </c>
       <c r="C222" t="str">
         <v>Editorial</v>
@@ -6154,10 +6154,10 @@
     </row>
     <row r="223">
       <c r="A223" t="str">
-        <v>Can I get my nails done? Can I get a massage? Can I get a facial?</v>
+        <v>What is Larry David's advice?</v>
       </c>
       <c r="B223" t="str">
-        <v>It depends. Services like nails, waxing, facials, and massage therapy can be open in counties not on the Monitoring List. For counties on the Monitoring List for 3 consecutive days, some services may be provided outdoors, like nails, waxing, facials, and massage. All indoor operations of nail salons, skin care, waxing, and massage are closed in counties on the Monitoring List for 3 consecutive days. [Learn more about which counties are on the list](https://covid19.ca.gov/roadmap-counties/).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) &lt;!-- spa, esthetician, electrolysis, waxing, cosmetology services, electrology, body art --&gt;</v>
+        <v>&lt;blockquote class="twitter-tweet"&gt;&lt;p lang="en" dir="ltr"&gt;“You’re hurting old people like me. Well, not me... I’ll never see you.”&lt;br&gt;&lt;br&gt;Larry David wants everyone to stay home to protect older Californians from &lt;a href="https://twitter.com/hashtag/COVID19?src=hash&amp;amp;ref_src=twsrc%5Etfw"&gt;#COVID19&lt;/a&gt;! &lt;br&gt;He does not do these things. &lt;br&gt;Listen to Larry.&lt;a href="https://twitter.com/hashtag/StayHomeSaveLives?src=hash&amp;amp;ref_src=twsrc%5Etfw"&gt;#StayHomeSaveLives&lt;/a&gt;&lt;a href="https://t.co/snYe5v55Rw"&gt;https://t.co/snYe5v55Rw&lt;/a&gt; &lt;a href="https://t.co/C5cKOaAufE"&gt;pic.twitter.com/C5cKOaAufE&lt;/a&gt;&lt;/p&gt;&amp;mdash; Office of the Governor of California (@CAgovernor) &lt;a href="https://twitter.com/CAgovernor/status/1245110728199045120?ref_src=twsrc%5Etfw"&gt;March 31, 2020&lt;/a&gt;&lt;/blockquote&gt; &lt;script async src="https://platform.twitter.com/widgets.js" charset="utf-8"&gt;&lt;/script&gt;</v>
       </c>
       <c r="C223" t="str">
         <v>Editorial</v>
@@ -6180,10 +6180,10 @@
     </row>
     <row r="224">
       <c r="A224" t="str">
-        <v>Can I get a tattoo or piercing? Can I get electrolysis?</v>
+        <v xml:space="preserve">Can I go to the movies? </v>
       </c>
       <c r="B224" t="str">
-        <v>It depends. Tattoo, piercing, and electrolysis services can be open in counties not on the Monitoring List. All indoor and outdoor services for tattooing, piercing, and electrolysis are closed in counties on the Monitoring List for 3 consecutive days. [Learn more about which counties are on the list](https://covid19.ca.gov/roadmap-counties/).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) &lt;!-- spa, esthetician, electrolysis, waxing, cosmetology services, electrology, body art --&gt;</v>
+        <v xml:space="preserve">Effective July 13, 2020, indoor movie theaters are closed in all counties. Drive-in movie theaters with modifications to support physical distancing may be open.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) </v>
       </c>
       <c r="C224" t="str">
         <v>Editorial</v>
@@ -6204,9 +6204,139 @@
         <v>223</v>
       </c>
     </row>
+    <row r="225">
+      <c r="A225" t="str">
+        <v>Can I go to a restaurant? Can I go to a winery or a brewery?</v>
+      </c>
+      <c r="B225" t="str">
+        <v xml:space="preserve">Indoor operations of all dine-in restaurants are closed in all counties. Restaurants across the state can be open for take out, drive through, delivery, and outdoor dining. \n\nIndoor operations for wineries and tasting rooms are closed in all counties. All bars, brewpubs, breweries, and pubs are closed statewide for both indoor and outdoor operations, unless they offer sit-down, outdoor dine-in meals. Alcohol can only be sold in the same transaction as a meal.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) </v>
+      </c>
+      <c r="C225" t="str">
+        <v>Editorial</v>
+      </c>
+      <c r="D225" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E225" t="str">
+        <v>[]</v>
+      </c>
+      <c r="F225" t="str">
+        <v>false</v>
+      </c>
+      <c r="G225" t="str">
+        <v>[]</v>
+      </c>
+      <c r="H225" t="str">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="str">
+        <v>Are restaurants allowed to open?</v>
+      </c>
+      <c r="B226" t="str">
+        <v xml:space="preserve">Restaurants across the state can be open for [take out, drive through, and delivery](https://files.covid19.ca.gov/pdf/guidance-takeout-restaurants.pdf). Indoor operations for dine-in restaurants are closed in all counties. Bars, brewpubs, breweries, and pubs must close both indoor and outdoor operations unless they are offering [sit-down, outdoor dine-in meals](https://files.covid19.ca.gov/pdf/guidance-outdoor-restaurants.pdf). Alcohol can only be sold in the same transaction as a meal.\n\nMore info: [Industry guidance](https://covid19.ca.gov/industry-guidance/) and [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) </v>
+      </c>
+      <c r="C226" t="str">
+        <v>Editorial</v>
+      </c>
+      <c r="D226" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E226" t="str">
+        <v>[]</v>
+      </c>
+      <c r="F226" t="str">
+        <v>false</v>
+      </c>
+      <c r="G226" t="str">
+        <v>[]</v>
+      </c>
+      <c r="H226" t="str">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="str">
+        <v>Where can I find the list of essential critical infrastructure sectors?</v>
+      </c>
+      <c r="B227" t="str">
+        <v xml:space="preserve">Visit [Essential workforce](https://covid19.ca.gov/essential-workforce/) to learn about what workers and sectors are included. </v>
+      </c>
+      <c r="C227" t="str">
+        <v>Editorial</v>
+      </c>
+      <c r="D227" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E227" t="str">
+        <v>[]</v>
+      </c>
+      <c r="F227" t="str">
+        <v>false</v>
+      </c>
+      <c r="G227" t="str">
+        <v>[]</v>
+      </c>
+      <c r="H227" t="str">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="str">
+        <v>Can I get my nails done? Can I get a massage? Can I get a facial?</v>
+      </c>
+      <c r="B228" t="str">
+        <v>It depends. Services like nails, waxing, facials, and massage therapy can be open in counties not on the Monitoring List. For counties on the Monitoring List for 3 consecutive days, some services may be provided outdoors, like nails, waxing, facials, and massage. All indoor operations of nail salons, skin care, waxing, and massage are closed in counties on the Monitoring List for 3 consecutive days. [Learn more about which counties are on the list](https://covid19.ca.gov/roadmap-counties/).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) &lt;!-- spa, esthetician, electrolysis, waxing, cosmetology services, electrology, body art --&gt;</v>
+      </c>
+      <c r="C228" t="str">
+        <v>Editorial</v>
+      </c>
+      <c r="D228" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E228" t="str">
+        <v>[]</v>
+      </c>
+      <c r="F228" t="str">
+        <v>false</v>
+      </c>
+      <c r="G228" t="str">
+        <v>[]</v>
+      </c>
+      <c r="H228" t="str">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="str">
+        <v>Can I get a tattoo or piercing? Can I get electrolysis?</v>
+      </c>
+      <c r="B229" t="str">
+        <v>It depends. Tattoo, piercing, and electrolysis services can be open in counties not on the Monitoring List. All indoor and outdoor services for tattooing, piercing, and electrolysis are closed in counties on the Monitoring List for 3 consecutive days. [Learn more about which counties are on the list](https://covid19.ca.gov/roadmap-counties/).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) &lt;!-- spa, esthetician, electrolysis, waxing, cosmetology services, electrology, body art --&gt;</v>
+      </c>
+      <c r="C229" t="str">
+        <v>Editorial</v>
+      </c>
+      <c r="D229" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E229" t="str">
+        <v>[]</v>
+      </c>
+      <c r="F229" t="str">
+        <v>false</v>
+      </c>
+      <c r="G229" t="str">
+        <v>[]</v>
+      </c>
+      <c r="H229" t="str">
+        <v>228</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H224"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H229"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
less custom questions, remove old crawl url
</commit_message>
<xml_diff>
--- a/qnacrawler/merged.xlsx
+++ b/qnacrawler/merged.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H239"/>
+  <dimension ref="A1:H220"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -564,7 +564,7 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>What is the relationship between the order and these questions and answers?</v>
+        <v>What is the relationship between the stay home order and these questions and answers?</v>
       </c>
       <c r="B8" t="str">
         <v>The Governor has ordered Californians to obey the directives of the State Public Health Officer. Those directives take many forms; they include specific materials linked on this page, as well as these questions and answers. These questions and answers are directives from the State Public Health Officer, and have the same force and effect as other State Public Health Officer directives.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
@@ -593,7 +593,7 @@
         <v>When does the stay home order go into effect and how long will we stay home? What areas of the state are covered?</v>
       </c>
       <c r="B9" t="str">
-        <v>The order went into effect on Thursday, March 19, 2020. The order is in place until further notice. It covers the whole state of California.\n\nAs of May 8, the stay home order was modified. In addition to essential activity, retail is allowed, along with the infrastructure to support it. As of May 12, offices, limited services, and outdoor museums are also permitted to open.\n\nSix key health and scientific [indicators](https://www.gov.ca.gov/2020/04/14/governor-newsom-outlines-six-critical-indicators-the-state-will-consider-before-modifying-the-stay-at-home-order-and-other-covid-19-interventions/) will be considered before modifying the state’s stay home order to allow additional activity.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>The order went into effect on Thursday, March 19, 2020. The order is in place until further notice. It covers the whole state of California.\n\nAs of May 8, the stay home order was modified. In addition to essential activity, retail is allowed, along with the infrastructure to support it. As of May 12, offices, limited services, and outdoor museums are also permitted to open.\n\n**\[Add new Executive Order language here.\]**\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C9" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -616,10 +616,10 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>What’s open statewide?</v>
+        <v>Is it safe to shop at open businesses?</v>
       </c>
       <c r="B10" t="str">
-        <v>**Essential services** that protect public health, public safety, and provide essential needs will remain open, such as:\n\n*   Gas stations \n*   Pharmacies\n*   Food: Grocery stores, farmers markets, food banks, convenience stores, take-out and delivery restaurants \n*   Banks \n*   Laundromats/laundry services \n*   Childcare\n*   Essential state and local government functions will also remain open, including law enforcement and offices that provide government programs and services.\n\n**Retailers** can open statewide. All will require modifications to support social distancing. This includes:\n\n*   Shopping malls (outdoor)\n*   Libraries\n*   Drive-in theaters (with modifications)\n*   Bookstores\n*   Jewelry stores\n*   Toy stores\n*   Clothing and shoe stores\n*   Home and furnishing stores\n*   Sporting goods stores\n*   Florists\n\n**Offices** (critical infrastructure indoors and outdoors; non-critical infrastructure outdoor only)\n\n**Limited services** which do not generally require close customer contact, such as: \n\n*   Pet grooming\n*   Dog walking\n*   Car washes\n*   Appliance repair\n*   Residential and janitorial cleaning\n*   Limited services for places of worship\n*   Plumbing\n\n**Outdoor museums**\n\n**Music, film, and TV production**\n\n**Professional sports (without live audiences)**\n\n**Schools and day camps**\n\n**Higher education** (lectures and student activities – see [guidance](https://files.covid19.ca.gov/pdf/guidance-higher-education--en.pdf))\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>The risk of COVID-19 infection is still real for all Californians and continues to be fatal. That is why every business permitted to open should take every step humanly possible to reduce the risk of infection by following these [state guidelines](https://covid19.ca.gov/industry-guidance/#top).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C10" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -642,10 +642,10 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>What’s closed statewide?</v>
+        <v>Can the stay home order be changed?</v>
       </c>
       <c r="B11" t="str">
-        <v>Statewide, the following are closed:\n\n*   Bars, brewpubs, breweries, and pubs, both indoors and outdoors, unless they are offering sit-down, outdoor dine-in meals. Alcohol can only be sold in the same transaction as a meal.\n*   Public events and gatherings, like live audience sports \n*   Convention centers\n*   Theme parks and festivals\n*   Indoor playgrounds, like bounce centers, ball pits and laser tag\n*   Saunas and steam rooms\n*   Recreational team sports\n\nStatewide, the following must close indoor operations:\n\n*   Dine-in restaurants\n*   Wineries and tasting rooms\n*   Movie theaters\n*   Family entertainment centers\n*   Zoos and museums\n*   Cardrooms\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes. The State Public Health Officer may issue new orders as the public health situation changes.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C11" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -668,10 +668,10 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>What is open with county variance?</v>
+        <v>How does the stay home order interact with local orders to shelter in place? Does it supersede them?</v>
       </c>
       <c r="B12" t="str">
-        <v>The following may open only in [counties approved to move further in the Resilience Roadmap](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/County_Variance_Attestation_Form.aspx):\n\n*   Hotels (for tourism and individual travel)\n*   Campgrounds and outdoor recreation\n*   Racetracks\n*   Casinos\n\nCounties that have remained on the County Monitoring List for 3 or more consecutive days are required to **close** some industries.\n\nThe following sectors must **close** indoor operations and activities unless they can be modified to operate outside or by pick-up:\n\n*   Gyms and fitness centers, like yoga and dance studios\n*   Places of worship and cultural ceremonies, like weddings and funerals\n*   Indoor protests\n*   Offices for non-essential (non-critical infrastructure) sectors\n*   Personal care services, like nail salons and body waxing\n*   Hair salons and barbershops\n*   Shopping malls\n*   Higher education (lectures and student activities – see [guidance](https://files.covid19.ca.gov/pdf/guidance-higher-education--en.pdf))\n\nShops that offer tattoos, piercings and electrolysis may not be operated outdoors and must close.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>This is a statewide order. Counties can have more restrictive criteria and different closures. See [your county’s status](https://covid19.ca.gov/safer-economy).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C12" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -694,10 +694,10 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Is it safe to shop at open businesses?</v>
+        <v>If I am not an Essential Critical Infrastructure Worker, can I still leave the house?</v>
       </c>
       <c r="B13" t="str">
-        <v>The risk of COVID-19 infection is still real for all Californians and continues to be fatal. That is why every business permitted to open should take every step humanly possible to reduce the risk of infection by following these [state guidelines](https://covid19.ca.gov/industry-guidance/#top).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes. As described in more detail elsewhere in applicable state public health directives (including on this page), there are a wide range of circumstances in which you may leave your home or other place of residence, even if you are not an Essential Critical Infrastructure Worker. For example, you may leave your home to work at any business or other entity that is allowed to open, to engage in in-person worship and protest activities consistent with public health directives, to patronize local businesses, or to care for friends or family members who require assistance (as set forth under [Health care](https://covid19.ca.gov/healthcare/#top)). And errands like these are not the only reasons you may leave your home: you may also leave your home with or without a specific destination in mind (for example, to walk your dog, to engage in physical recreation, or simply to get some fresh air) as long as you maintain physical distancing and comply with any other applicable public health directives.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C13" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -720,10 +720,10 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Can the Order be changed?</v>
+        <v>Are gatherings permitted?</v>
       </c>
       <c r="B14" t="str">
-        <v>Yes. The State Public Health Officer may issue new orders as the public health situation changes.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>State public health directives prohibit professional, social and community gatherings. Gatherings are defined as meetings or other events that bring together persons from multiple households at the same time for a shared or group experience in a single room, space, or place such as an auditorium, stadium, arena, large conference room, meeting hall, or other indoor or outdoor space. They pose an especially high danger of transmission and spread of COVID-19.\n\nOn May 25, 2020, in an effort to balance First Amendment interests with public health, the State Public Health Officer created an exception to the prohibition against mass gatherings for faith-based services and cultural ceremonies as well as protests. Those types of gatherings are now permitted indoors so long as they do not exceed 100 attendees or 25% of the capacity of the space in which the gathering is held, whichever is lower. State public health directives now do not prohibit in-person outdoor faith-based services or protests as long as face coverings are worn and physical distancing of 6 feet between persons or groups of persons from different households is maintained at all times. All other gatherings are prohibited until further notice, except as otherwise specifically permitted in state public health directives (including in applicable industry guidance).\n\nCrowds and limited physical distancing increase the risk for COVID-19. If you attended a protest, remember that confidential, free testing is available. [Find a testing location near you](https://urldefense.proofpoint.com/v2/url?u=https-3A__covid19.ca.gov_testing-2Dand-2Dtreatment_-23top&amp;d=DwMGaQ&amp;c=Lr0a7ed3egkbwePCNW4ROg&amp;r=yRsi0eKVK6Khc58oFC32XROAJ-JqVGBGabDv9P6148k&amp;m=Iul4bdNDGFuRu3rXHrxPHNWT2PT2bXFITW3YP1tzG94&amp;s=4qpOZ7lX1S5M_STTblq_XAQNu05ccIFwIyu4bvl9U3c&amp;e=). If you test negative it does not mean that you may not develop COVID-19 later on. Therefore, it is advisable that you self-isolate for 14 days if possible.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- wedding, protest, funeral, banquet, event, outdoor, conference, symposium, rally, rallies, assembly, assemblies, convention, congregation, congregate, congregation, crowd, group, forum, worship --&gt;</v>
       </c>
       <c r="C14" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -746,10 +746,10 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>How does this order interact with local orders to shelter in place? Does it supersede them?</v>
+        <v>Can I get a haircut?</v>
       </c>
       <c r="B15" t="str">
-        <v>This is a statewide order. Counties may move further into the Resilience Roadmap if they meet certain criteria.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes. Hair salons and barbershops are now open throughout the state with modifications for safety.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C15" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -772,10 +772,10 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>If I am not an Essential Critical Infrastructure Worker, can I still leave the house?</v>
+        <v>Are safety protocols being enforced? How do I report a business that isn’t complying?</v>
       </c>
       <c r="B16" t="str">
-        <v>Yes. As described in more detail elsewhere in applicable state public health directives (including on this page), there are a wide range of circumstances in which you may leave your home or other place of residence, even if you are not an Essential Critical Infrastructure Worker. For example, you may leave your home to work at any business or other entity that is allowed to open, to engage in in-person worship and protest activities consistent with public health directives, to patronize local businesses, or to care for friends or family members who require assistance (as set forth under [Health care](https://covid19.ca.gov/healthcare/#top)). And errands like these are not the only reasons you may leave your home: you may also leave your home with or without a specific destination in mind (for example, to walk your dog, to engage in physical recreation, or simply to get some fresh air) as long as you maintain physical distancing and comply with any other applicable public health directives.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>They are being enforced, and you can report it. Report unsafe conditions or businesses that shouldn’t be open to your local Alcohol Beverage Control, Labor Commissioner’s office, or regional Cal/OSHA office, depending on the type of business. To find these local contacts, see Appendix B of the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- Adding keywords mask masks report reporting enforce enforcement compliance for quick answers purposes --&gt;</v>
       </c>
       <c r="C16" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -798,10 +798,10 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Are gatherings permitted?</v>
+        <v>I want to express my political views.  How can I make my voice heard without raising public health concerns?</v>
       </c>
       <c r="B17" t="str">
-        <v>State public health directives prohibit professional, social and community gatherings. Gatherings are defined as meetings or other events that bring together persons from multiple households at the same time for a shared or group experience in a single room, space, or place such as an auditorium, stadium, arena, large conference room, meeting hall, or other indoor or outdoor space. They pose an especially high danger of transmission and spread of COVID-19.\n\nOn May 25, 2020, in an effort to balance First Amendment interests with public health, the State Public Health Officer created an exception to the prohibition against mass gatherings for faith-based services and cultural ceremonies as well as protests. Those types of gatherings are now permitted indoors so long as they do not exceed 100 attendees or 25% of the capacity of the space in which the gathering is held, whichever is lower. State public health directives now do not prohibit in-person outdoor faith-based services or protests as long as face coverings are worn and physical distancing of 6 feet between persons or groups of persons from different households is maintained at all times. All other gatherings are prohibited until further notice, except as otherwise specifically permitted in state public health directives (including in applicable industry guidance).\n\nCrowds and limited physical distancing increase the risk for COVID-19. If you attended a protest, remember that confidential, free testing is available. [Find a testing location near you](https://urldefense.proofpoint.com/v2/url?u=https-3A__covid19.ca.gov_testing-2Dand-2Dtreatment_-23top&amp;d=DwMGaQ&amp;c=Lr0a7ed3egkbwePCNW4ROg&amp;r=yRsi0eKVK6Khc58oFC32XROAJ-JqVGBGabDv9P6148k&amp;m=Iul4bdNDGFuRu3rXHrxPHNWT2PT2bXFITW3YP1tzG94&amp;s=4qpOZ7lX1S5M_STTblq_XAQNu05ccIFwIyu4bvl9U3c&amp;e=). If you test negative it does not mean that you may not develop COVID-19 later on. Therefore, it is advisable that you self-isolate for 14 days if possible.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- wedding, protest, funeral, banquet, event, outdoor, conference, symposium, rally, rallies, assembly, assemblies, convention, congregation, congregate, congregation, crowd, group, forum, worship --&gt;</v>
+        <v>There are many ways for you to express your political views without holding a physical, in-person gathering.  For example, you may continue to call or write elected officials, write letters to the editor of news publications, display lawn or window signs, or use online and other electronic media (including Zoom rooms, Twitter feeds, Facebook pages, and other digital forums) to express your views.  \n\nAdditionally, as noted above, you may leave your home for any reason as long as you comply with any other applicable public health directives. When you are otherwise out in public, public health directives do not prevent you from engaging in political expression—such as by wearing or carrying a sign.\n\nIf collective action in physical space is important to you, consider whether you and other participants can safely protest from within your cars.  The State Public Health Officer does not consider in-car activities to be gatherings, if participants stay in their cars and otherwise remain apart from individuals who are not part of their households.  Many activists have organized car-based protests (honking horns, flying flags, displaying signs, and so on) to express their political views while complying with State public health directives.  \n\nWhenever you are considering a protest (including an in-car protest), make sure you comply with all other applicable laws, including any local public-health measures that may be more restrictive than statewide directives and any other applicable local laws.\n\nIf you do wish to engage in in-person protest outside of your car with a group of any size, you must follow the guidelines for political protest gatherings below.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C17" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -824,10 +824,10 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Can I get a haircut?</v>
+        <v>Can I engage in political protest gatherings?</v>
       </c>
       <c r="B18" t="str">
-        <v>It depends. Hair salons and barbershops are open in counties not on the [County Monitoring List](https://covid19.ca.gov/roadmap-counties/). However, all indoor operations for these businesses are closed in counties that are on this list. Outdoor hair services may be available.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes, although in-person protests present special public health concerns. \n\nEven with adherence to physical distancing, bringing members of different households together to engage in in-person protest carries a higher risk of widespread transmission of COVID-19.  Such gatherings may result in increased rates of infection, hospitalization, and death, especially among more vulnerable populations. In particular, activities like chanting, shouting, singing, and group recitation negate the risk-reduction achieved through 6 feet of physical distancing. For this reason, people engaging in these activities should wear face coverings at all times.\n\nTherefore, it is strongly recommended that those exercising their right to engage in political expression (including, for example, their right to petition the government) should utilize alternative channels, such as the many online and broadcasting platforms available in the digital age, in place of in-person gatherings. \n\nHowever, state public health directives do not prohibit in-person _outdoor_ protests as long as you maintain a physical distance of 6 feet between persons or groups of persons from different households at all times. When you can’t maintain a safe physical distance of 6 feet from people not in your household, you must wear a face covering or mask. Local Health Officers are advised to consider appropriate limitations on outdoor attendance capacities, factoring their jurisdiction’s key COVID-19 health indicators. Failure to follow these requirements may result in an order to disperse or other enforcement action. Masks and face coverings are strongly recommended.\n\nIn counties in the [Widespread (purple) tier](https://covid19.ca.gov/safer-economy/) indoor protests are not currently permitted. In other counties, state public health directives do not prohibit in-person _indoor_ protests as long as (1) attendance is limited as as required by the [relevant local restrictions](https://covid19.ca.gov/safer-economy) places of worship (2) physical distancing of 6 feet between persons or groups of persons from different households is maintained at all times, and (3) singing and chanting activities are discontinued. Failure to follow these requirements may result in an order to disperse or other enforcement action. Masks and face coverings are required in compliance with CDPH directives.\n\nParticipants must maintain a physical distance of 6 feet from any uniformed peace officers and other public safety personnel present, unless otherwise directed, and follow all other requirements and directives imposed by local health officers and law enforcement, or other applicable authorities.\n\nThis limitation on attendance will be reviewed regularly. This review will assess the impacts of these imposed limits on public health and provide further direction as part of a phased-in restoration of gatherings that implicate the First Amendment.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C18" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -850,10 +850,10 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Are safety protocols being enforced? How do I report a business that isn’t complying?</v>
+        <v>How do I vote?</v>
       </c>
       <c r="B19" t="str">
-        <v>They are being enforced, and you can report it. Report unsafe conditions or businesses that shouldn’t be open to your local Alcohol Beverage Control, Labor Commissioner’s office, or regional Cal/OSHA office, depending on the type of business. To find these local contacts, see Appendix B of the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- Adding keywords mask masks report reporting enforce enforcement compliance for quick answers purposes --&gt;</v>
+        <v>**[Elections are an essential activity](https://files.covid19.ca.gov/pdf/CDPH-to-SOS-Letter-from-Acting-HO-Aug-18-1.pdf).** The Governor has issued [executive orders to ensure elections are safe and accessible](https://www.gov.ca.gov/2020/05/08/governor-newsom-issues-executive-order-to-protect-public-health-by-mailing-every-registered-voter-a-ballot-ahead-of-the-november-general-election/). Vote-by-mail ballots will be sent to all registered voters for the November 3, 2020 General Election. Most counties will provide [three days of early voting](https://www.gov.ca.gov/2020/06/03/governor-newsom-signs-executive-order-on-safe-secure-and-accessible-general-election-in-november/) in-person starting the Saturday before the election. Open ballot drop-box locations will be available between October 6 and November 3, 2020. Existing laws addressing the use of vote-by-mail ballots in California elections remain in effect except where suspended by Executive Order. Find [guidance for the safe administration of elections](https://elections.cdn.sos.ca.gov/ccrov/pdf/2020/july/20154jl.pdf) during COVID-19.\n\n Visit [online voter registration](https://registertovote.ca.gov/) to register to vote or check your voter registration status. \n\nPractice physical distancing and follow other applicable public health directives while engaged in election-related activities. These include collection and drop-off of ballots, and collection of signatures to qualify candidates or measures for the ballot.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C19" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -876,10 +876,10 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>I want to express my political views.  How can I make my voice heard without raising public health concerns?</v>
+        <v>Can I go to church?</v>
       </c>
       <c r="B20" t="str">
-        <v>There are many ways for you to express your political views without holding a physical, in-person gathering.  For example, you may continue to call or write elected officials, write letters to the editor of news publications, display lawn or window signs, or use online and other electronic media (including Zoom rooms, Twitter feeds, Facebook pages, and other digital forums) to express your views.  \n\nAdditionally, as noted above, you may leave your home for any reason as long as you comply with any other applicable public health directives. When you are otherwise out in public, public health directives do not prevent you from engaging in political expression—such as by wearing or carrying a sign.\n\nIf collective action in physical space is important to you, consider whether you and other participants can safely protest from within your cars.  The State Public Health Officer does not consider in-car activities to be gatherings, if participants stay in their cars and otherwise remain apart from individuals who are not part of their households.  Many activists have organized car-based protests (honking horns, flying flags, displaying signs, and so on) to express their political views while complying with State public health directives.  \n\nWhenever you are considering a protest (including an in-car protest), make sure you comply with all other applicable laws, including any local public-health measures that may be more restrictive than statewide directives and any other applicable local laws.\n\nIf you do wish to engage in in-person protest outside of your car with a group of any size, you must follow the guidelines for political protest gatherings below.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes. Places of worship such as churches, mosques, temples, and synagogues can open throughout the state, with [modifications for safety (PDF)](https://files.covid19.ca.gov/pdf/guidance-places-of-worship--en.pdf).In counties in the [Widespread (purple)](https://covid19.ca.gov/safer-economy) indoor services in places of worship must be discontinued but outdoor and online services are permitted.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C20" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -902,10 +902,10 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>Can I engage in political protest gatherings?</v>
+        <v>Can I practice my religious faith?</v>
       </c>
       <c r="B21" t="str">
-        <v>Yes, although in-person protests present special public health concerns. \n\nEven with adherence to physical distancing, bringing members of different households together to engage in in-person protest carries a higher risk of widespread transmission of COVID-19.  Such gatherings may result in increased rates of infection, hospitalization, and death, especially among more vulnerable populations. In particular, activities like chanting, shouting, singing, and group recitation negate the risk-reduction achieved through 6 feet of physical distancing. For this reason, people engaging in these activities should wear face coverings at all times.\n\nTherefore, it is strongly recommended that those exercising their right to engage in political expression (including, for example, their right to petition the government) should utilize alternative channels, such as the many online and broadcasting platforms available in the digital age, in place of in-person gatherings. \n\nHowever, state public health directives do not prohibit in-person _outdoor_ protests as long as you maintain a physical distance of 6 feet between persons or groups of persons from different households at all times. When you can’t maintain a safe physical distance of 6 feet from people not in your household, you must wear a face covering or mask. Local Health Officers are advised to consider appropriate limitations on outdoor attendance capacities, factoring their jurisdiction’s key COVID-19 health indicators. Failure to maintain adequate physical distancing may result in an order to disperse or other enforcement action. Masks and face coverings are strongly recommended.\n\nIn counties that have been on the [County Monitoring List](https://covid19.ca.gov/roadmap-counties/) for three consecutive days, indoor protests are not currently permitted. State public health directives do not prohibit in-person _indoor_ protests as long as (1) attendance is limited to 25% of the relevant area’s maximum occupancy, as defined by the relevant local permitting authority or other relevant authority, or a maximum of 100 attendees, whichever is lower, (2) physical distancing of 6 feet between persons or groups of persons from different households is maintained at all times, and (3) singing and chanting activities are discontinued. Failure to maintain adequate physical distancing may result in an order to disperse or other enforcement action. Masks and face coverings are required in compliance with CDPH directives.\n\nParticipants must maintain a physical distance of 6 feet from any uniformed peace officers and other public safety personnel present, unless otherwise directed, and follow all other requirements and directives imposed by local health officers and law enforcement, or other applicable authorities.\n\nThis limitation on attendance will be reviewed regularly. This review will assess the impacts of these imposed limits on public health and provide further direction as part of a phased-in restoration of gatherings that implicate the First Amendment.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes. Practicing your faith is a constitutionally-protected activity and may manifest in many different forms.\n\nAlthough in-person religious gatherings—like other in-person gatherings—have been restricted to prevent the transmission of COVID-19, on May 25, 2020, the State Public Health Officer began to ease restrictions on in-person religious gatherings. In particular, the State Public Health Officer now authorizes County Departments of Public Health to allow collective activities at places of worship, subject to conditions to support a safe, clean environment for employees, interns and trainees, volunteers, scholars, and all other types of workers as well as congregants, worshippers, and visitors.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- church, mosque, synagogue, temple, wedding, funeral, baptism --&gt;</v>
       </c>
       <c r="C21" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -928,10 +928,10 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>How do I vote?</v>
+        <v>What conditions must be met to resume religious services and cultural ceremonies at places of worship?</v>
       </c>
       <c r="B22" t="str">
-        <v>**[Elections are an essential activity](https://files.covid19.ca.gov/pdf/CDPH-to-SOS-Letter-from-Acting-HO-Aug-18-1.pdf).** The Governor has issued [executive orders to ensure elections are safe and accessible](https://www.gov.ca.gov/2020/05/08/governor-newsom-issues-executive-order-to-protect-public-health-by-mailing-every-registered-voter-a-ballot-ahead-of-the-november-general-election/). Vote-by-mail ballots will be sent to all registered voters for the November 3, 2020 General Election. Most counties will provide [three days of early voting](https://www.gov.ca.gov/2020/06/03/governor-newsom-signs-executive-order-on-safe-secure-and-accessible-general-election-in-november/) in-person starting the Saturday before the election. Open ballot drop-box locations will be available between October 6 and November 3, 2020. Existing laws addressing the use of vote-by-mail ballots in California elections remain in effect except where suspended by Executive Order. Find [guidance for the safe administration of elections](https://elections.cdn.sos.ca.gov/ccrov/pdf/2020/july/20154jl.pdf) during COVID-19.\n\n Visit [online voter registration](https://registertovote.ca.gov/) to register to vote or check your voter registration status. \n\nPractice physical distancing and follow other applicable public health directives while engaged in election-related activities. These include collection and drop-off of ballots, and collection of signatures to qualify candidates or measures for the ballot.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Information on conditions imposed by the state can be found at [guidance for places of worship (PDF)](https://files.covid19.ca.gov/pdf/guidance-places-of-worship--en.pdf). Additional conditions may be imposed by local public health officials. This guidance does not obligate places of worship to resume in-person activity. It is strongly recommended that places of worship continue to facilitate remote services and other alternatives to in-person religious practice for those who are vulnerable to COVID19.\n\nEven with adherence to physical distancing, convening in a congregational setting of multiple households to practice a personal faith carries a higher risk of widespread transmission of COVID-19, and may result in increased rates of infection, hospitalization, and death, especially among more vulnerable populations. In particular, activities like singing and group recitation dramatically increase the risk of COVID-19 transmission. For this reason, singing and chanting activities must be discontinued at indoor services, and congregants engaging in group recitation should wear face coverings at all times.\n\nPlaces of worship may only open indoor operations when permitted by [relevant local restrictions](https://covid19.ca.gov/safer-economy) and must comply with all applicable attendance limitations and guidance requirements.\n\nLocal Health Officers are advised to consider appropriate limitations on _outdoor_ attendance capacities, factoring their jurisdiction’s key COVID-19 health indicators. At a minimum, outdoor attendance should be limited naturally through implementation of strict physical distancing measures of a minimum of 6 feet between attendees from different households, in addition to other relevant protocols within this document.\n\nThis limitation will be regularly reviewed by the California Department of Public Health.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C22" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -954,10 +954,10 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Can I go to church?</v>
+        <v>Can children attend group activities (like Sunday school or Hebrew school) at places of worship?</v>
       </c>
       <c r="B23" t="str">
-        <v>Yes. Places of worship such as churches, mosques, temples, and synagogues can open throughout the state, with [modifications for safety (PDF)](https://files.covid19.ca.gov/pdf/guidance-places-of-worship--en.pdf). In counties on the [County Monitoring List](https://covid19.ca.gov/roadmap-counties/), indoor services in places of worship must be discontinued but outdoor and online services are permitted.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes.  Outdoor activities are permitted, and indoor activities are permitted if they comply with the [cohort guidance](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/small-groups-child-youth.aspx).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C23" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -980,10 +980,10 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>Can I practice my religious faith?</v>
+        <v>When will current conditions change for places of worship?</v>
       </c>
       <c r="B24" t="str">
-        <v>Yes. Practicing your faith is a constitutionally-protected activity and may manifest in many different forms.\n\nAlthough in-person religious gatherings—like other in-person gatherings—have been restricted to prevent the transmission of COVID-19, on May 25, 2020, the State Public Health Officer began to ease restrictions on in-person religious gatherings. In particular, the State Public Health Officer now authorizes County Departments of Public Health to allow collective activities at places of worship, subject to conditions to support a safe, clean environment for employees, interns and trainees, volunteers, scholars, and all other types of workers as well as congregants, worshippers, and visitors.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- church, mosque, synagogue, temple, wedding, funeral, baptism --&gt;</v>
+        <v>The California Department of Public Health, in consultation with county Departments of Public Health, will regularly review and assess the impacts of these imposed limits on public health and provide further direction as part of a phased-in restoration of activities in places of worship.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C24" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1006,10 +1006,10 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>What conditions must be met to resume religious services and cultural ceremonies at places of worship?</v>
+        <v>Can I still exercise? Take my kids to the park for fresh air? Take a walk around the block?</v>
       </c>
       <c r="B25" t="str">
-        <v>Information on conditions imposed by the state can be found at [guidance for places of worship (PDF)](https://files.covid19.ca.gov/pdf/guidance-places-of-worship--en.pdf). Additional conditions may be imposed by local public health officials. This guidance does not obligate places of worship to resume in-person activity. It is strongly recommended that places of worship continue to facilitate remote services and other alternatives to in-person religious practice for those who are vulnerable to COVID19.\n\nEven with adherence to physical distancing, convening in a congregational setting of multiple households to practice a personal faith carries a higher risk of widespread transmission of COVID-19, and may result in increased rates of infection, hospitalization, and death, especially among more vulnerable populations. In particular, activities like singing and group recitation dramatically increase the risk of COVID-19 transmission. For this reason, singing and chanting activities must be discontinued at indoor services, and congregants engaging in group recitation should wear face coverings at all times.\n\nPlaces of worship must therefore limit _indoor_ attendance to 25% of building capacity or a maximum of 100 attendees, whichever is lower, and singing and chanting activities must be discontinued in indoor services. In counties on the County Monitoring List for three consecutive days, places of worship must discontinue indoor services.\n\nLocal Health Officers are advised to consider appropriate limitations on _outdoor_ attendance capacities, factoring their jurisdiction’s key COVID-19 health indicators. At a minimum, outdoor attendance should be limited naturally through implementation of strict physical distancing measures of a minimum of 6 feet between attendees from different households, in addition to other relevant protocols within this document.\n\nThis limitation will be regularly reviewed by the California Department of Public Health.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>It’s okay to go outside to go for a walk, to exercise, and participate in healthy activities as long as you **maintain a safe physical distance of 6 feet and gather only with members of your household.** You can also participate in activities at [outdoor recreational facilities](https://files.covid19.ca.gov/pdf/guidance-campgrounds-outdoor-recreation--en.pdf) that are allowed to open. [Parks may be closed](https://covid19.ca.gov/public-recreation/) to help slow the spread of the virus. Young people can participate in sports as permitted by the [youth sports guidance (PDF)](https://files.covid19.ca.gov/pdf/guidance-youth-sports--en.pdf). Check with local officials about park closures in your area. Californians should not travel significant distances for recreation and should stay close to home.\n\nBelow is a list of some outdoor recreational activities.\n\n*   Badminton (singles)\n*   Throwing a baseball/softball\n*   BMX biking\n*   Canoeing (singles)\n*   Crabbing\n*   Cycling\n*   Exploring rock pools\n*   Gardening (not in groups)\n*   Golfing (doubles, only if cart has protective partition)\n*   Hiking (trails/ paths allowing distancing)\n*   Horse riding (singles)\n*   Jogging and running\n*   Kite boarding and kitesurfing\n*   Meditation\n*   Outdoor photography\n*   Picnics (with your household members only)\n*   Quad biking\n*   Rock climbing\n*   Roller skating and rollerblading\n*   Rowing (singles)\n*   Scootering (not in groups)\n*   Skateboarding (not in groups)\n*   Soft martial arts – tai chi, chi kung (not in groups)\n*   Surfing\n*   Tennis and table tennis (singles)\n*   Throwing a football, kicking a soccer ball (not in groups)\n*   Trail running\n*   Trampolining\n*   Tree climbing\n*   Volleyball (singles)\n*   Walk the dog\n*   Wash the car\n*   Watch the sunrise or sunset\n*   Yoga\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C25" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1032,10 +1032,10 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Can children attend group activities (like Sunday school or Hebrew school) at places of worship?</v>
+        <v>Can I walk my dog? Take my pet to the vet?</v>
       </c>
       <c r="B26" t="str">
-        <v>At this time, no. Children should remain in the care of those in their household unit and not interact with children of other parties at all times while visiting facilities. Places of worship must discontinue activities and services for children (for example, shared play areas) where physical distancing of at least 6 feet cannot be maintained.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>You can walk your dog. You can go to the vet or pet hospital if your pet is sick. Remember to wear a face covering and distance yourself at least 6 feet from other pets and owners.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C26" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1058,10 +1058,10 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>When will these conditions change for places of worship?</v>
+        <v>Can I visit State Parks? What outdoor spaces are open?</v>
       </c>
       <c r="B27" t="str">
-        <v>The California Department of Public Health, in consultation with county Departments of Public Health, will regularly review and assess the impacts of these imposed limits on public health and provide further direction as part of a phased-in restoration of activities in places of worship.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>State Parks, campgrounds, museums, and visitor centers [may continue to be closed](https://www.parks.ca.gov/?page_id=30350) to help slow the spread of the virus. Starting June 12, some counties may open campgrounds and RV parks. Be sure to check [parks in your area before you travel](https://covid19.ca.gov/public-recreation/). Californians should not travel significant distances for pleasure or recreation and should stay close to home. If you do travel, take steps to keep everyone safe like wearing a face covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently.\n\nYou can walk, run, hike and bike in your local neighborhoods as long as they continue to practice physical distancing of 6 feet. This means avoiding crowded trails and parking lots.\n\nFor information on National Parks, please the [National Park Service website](https://www.nps.gov/aboutus/news/public-health-update.htm).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- park, visitor center, travel, museum, RV parks, recreation, outdoor recreation, sports, RV, tent camping, tent camp, fish, beach, lake, river, event, outdoor event, event planning, hike, walk, bike, exercise, nature, bird watching, public →&lt;/p&gt;--&gt;</v>
       </c>
       <c r="C27" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>Can I still exercise? Take my kids to the park for fresh air? Take a walk around the block?</v>
+        <v>Can I travel?</v>
       </c>
       <c r="B28" t="str">
-        <v>It’s okay to go outside to go for a walk, to exercise, and participate in healthy activities as long as you **maintain a safe physical distance of 6 feet and gather only with members of your household.** You can also participate in activities at [outdoor recreational facilities](https://files.covid19.ca.gov/pdf/guidance-campgrounds-outdoor-recreation--en.pdf) that are allowed to open. [Parks may be closed](https://covid19.ca.gov/public-recreation/) to help slow the spread of the virus. Check with local officials about park closures in your area. Californians should not travel significant distances for recreation and should stay close to home.\n\nBelow is a list of some outdoor recreational activities.\n\n*   Badminton (singles)\n*   Throwing a baseball/softball\n*   BMX biking\n*   Canoeing (singles)\n*   Crabbing\n*   Cycling\n*   Exploring rock pools\n*   Gardening (not in groups)\n*   Golfing (doubles, only if cart has protective partition)\n*   Hiking (trails/ paths allowing distancing)\n*   Horse riding (singles)\n*   Jogging and running\n*   Kite boarding and kitesurfing\n*   Meditation\n*   Outdoor photography\n*   Picnics (with your household members only)\n*   Quad biking\n*   Rock climbing\n*   Roller skating and rollerblading\n*   Rowing (singles)\n*   Scootering (not in groups)\n*   Skateboarding (not in groups)\n*   Soft martial arts – tai chi, chi kung (not in groups)\n*   Surfing\n*   Tennis and table tennis (singles)\n*   Throwing a football, kicking a soccer ball (not in groups)\n*   Trail running\n*   Trampolining\n*   Tree climbing\n*   Volleyball (singles)\n*   Walk the dog\n*   Wash the car\n*   Watch the sunrise or sunset\n*   Yoga\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>You can travel for urgent matters or if such travel is essential to your permitted work. Even though businesses around the state are opening up, avoid travelling long distances for vacations or pleasure as much as possible. This is to slow the spread of the coronavirus. Do not travel if you are sick, or if someone in your household has had coronavirus in the last two weeks. Do not travel with someone who is sick.\n\nYou should check with the local health department where you are starting from, along your route, and at your planned destination for information. Know that local rules are constantly changing and may change even after you start your trip. [Check for travel updates](https://www.visitcalifornia.com/latest-covid-19-coronavirus) before you leave your home.\n\nBefore travelling away from your community, consider these questions from the [Center for Disease Control (CDC) travel guidance](https://www.cdc.gov/coronavirus/2019-ncov/travelers/travel-in-the-us.html):\n\n*   Is coronavirus spreading where you are traveling?\n*   Are you or those you are traveling with more likely to get very sick from coronavirus?\n*   Will you be able to keep 6 feet of physical distance from others during or after your trip?\n\nIf you do travel, take steps to keep everyone safe like wearing a face covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently.  \n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- wedding, travel, gathering, tourism, funeral, motel, vacation, airbnb, vrbo, rental home --&gt;</v>
       </c>
       <c r="C28" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1110,10 +1110,10 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>Can I walk my dog? Take my pet to the vet?</v>
+        <v>Are there travel restrictions within California?</v>
       </c>
       <c r="B29" t="str">
-        <v>You can walk your dog. You can go to the vet or pet hospital if your pet is sick. Remember to wear a face covering and distance yourself at least 6 feet from other pets and owners.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>To prevent further spread of COVID-19, Californians should not travel significant distances and should stay close to home as much as possible.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C29" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1136,10 +1136,10 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>Can I visit State Parks? What outdoor spaces are open?</v>
+        <v>Are there travel restrictions into or out of California?</v>
       </c>
       <c r="B30" t="str">
-        <v>State Parks, campgrounds, museums, and visitor centers [may continue to be closed](https://www.parks.ca.gov/?page_id=30350) to help slow the spread of the virus. Starting June 12, some counties may open campgrounds and RV parks. Be sure to check [parks in your area before you travel](https://covid19.ca.gov/public-recreation/). Californians should not travel significant distances for pleasure or recreation and should stay close to home. If you do travel, take steps to keep everyone safe like wearing a face covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently.\n\nYou can walk, run, hike and bike in your local neighborhoods as long as they continue to practice physical distancing of 6 feet. This means avoiding crowded trails and parking lots.\n\nFor information on National Parks, please the [National Park Service website](https://www.nps.gov/aboutus/news/public-health-update.htm).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- park, visitor center, travel, museum, RV parks, recreation, outdoor recreation, sports, RV, tent camping, tent camp, fish, beach, lake, river, event, outdoor event, event planning, hike, walk, bike, exercise, nature, bird watching, public →&lt;/p&gt;--&gt;</v>
+        <v>There are currently no restrictions for entering California if you are coming from another state in the U.S. The federal government has placed restrictions on certain international travelers. With specific exceptions, foreign nationals who visited certain countries during the past 14 days are prohibited from entry to the United States. All international travelers, including US citizens and permanent residents, should quarantine for 14 days after coming to California from any other country. All travelers should take safety precautions when considering traveling.·       \n\n*   Don’t travel if you have been sick in the past 14 days or if you live with someone with COVID-19·        \n*   Don’t travel with someone who is sick\n*   Wear a mask in public\n*   Wash your hands\n*   Keep 6 feet from anyone you don’t live with\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C30" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1162,10 +1162,10 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>Can I travel?</v>
+        <v>Are swimming pools open?</v>
       </c>
       <c r="B31" t="str">
-        <v>You can travel for urgent matters or if such travel is essential to your permitted work. Even though businesses around the state are opening up, avoid travelling long distances for vacations or pleasure as much as possible. This is to slow the spread of the coronavirus. Do not travel if you are sick, or if someone in your household has had coronavirus in the last two weeks. Do not travel with someone who is sick.\n\nYou should check with the local health department where you are starting from, along your route, and at your planned destination for information. Know that local rules are constantly changing and may change even after you start your trip. [Check for travel updates](https://www.visitcalifornia.com/latest-covid-19-coronavirus) before you leave your home.\n\nBefore travelling away from your community, consider these questions from the [Center for Disease Control (CDC) travel guidance](https://www.cdc.gov/coronavirus/2019-ncov/travelers/travel-in-the-us.html):\n\n*   Is coronavirus spreading where you are traveling?\n*   Are you or those you are traveling with more likely to get very sick from coronavirus?\n*   Will you be able to keep 6 feet of physical distance from others during or after your trip?\n\nIf you do travel, take steps to keep everyone safe like wearing a face covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently.  \n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- wedding, travel, gathering, tourism, funeral, motel, vacation, airbnb, vrbo, rental home --&gt;</v>
+        <v>Outdoor swimming pools are allowed to open in all counties in California. Outdoor pools must close slides, rides, or other attractions. \n\nIndoor swimming pools are closed in counties in the [Widespread (purple) or Substantial (red) tiers](https://covid19.ca.gov/safer-economy).\n\nWater parks, both indoor and outdoor, remain closed throughout the state.\n\nWhen out of the water, masks or face coverings should be worn. Physical distancing should be practiced at all times. Group gatherings are not allowed. Bring your own towel, and don’t share items that are worn on the face (like goggles, nose clips, or snorkels). Pool operators should follow heightened cleaning and safety guidance in response to COVID-19. See sector guidance for [gyms and fitness centers](https://files.covid19.ca.gov/pdf/guidance-fitness--en.pdf) and [campgrounds and outdoor recreation](https://files.covid19.ca.gov/pdf/guidance-campgrounds-outdoor-recreation--en.pdf).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C31" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1188,10 +1188,10 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>Are there travel restrictions within California?</v>
+        <v>Can I go to the Department of Motor Vehicles (DMV)?</v>
       </c>
       <c r="B32" t="str">
-        <v>To prevent further spread of COVID-19, Californians should not travel significant distances and should stay close to home as much as possible.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes, but first check if an in-person visit is required. Several deadlines have been extended, and many DMV services can be accessed online.\n\n##### **Extended deadlines**\n\nDMV has extended deadlines for:\n\n*   Drivers 70 years of age and older with licenses expiring between March 1 through December 31, 2020. Your license is valid for one year from the original expiration date.\n*   Drivers 69 years of age and younger with licenses expiring between March 1 through July 31, 2020. Though the extension has now expired, you can [renew your license online.](https://www.dmv.ca.gov/portal/driver-licenses-identification-cards/driver-license-id-card-online-renewal/) An in-person visit is not required.\n*   Expiring commercial licenses, endorsements, and certificates. They are valid through September 30, 2020.\n*   In-person renewals for vehicle registrations that expire between the dates of March 16, 2020, and May 31, 2020.\n*   In-person renewals for those with safe driving records whose last DMV visit was 15 years ago.\n*   Driver license permits expiring between March and November 2020. They are extended six months or to a date 24 months from the date of application, whichever is earlier.\n*   Commercial learner’s permits expiring between March and September 2020. They are now valid through September 30, 2020.\n\n##### Online services\n\nDMV offers many services that can be handled online, including simple vehicle registration, renewing a driver’s license, getting a duplicate license, and more. See:\n\n*   [DMV Online Services](https://www.dmv.ca.gov/portal/dmv-online/)\n\nSome DMV services that used to require an in-person office visit can now be accessed online, including driver’s license renewals, vehicle registrations, title transfers, temporary driver’s license extensions, commercial driver’s license renewals, and more. See:\n\n*   [DMV Virtual Field Office](https://virtual.dmv.ca.gov/)\n\n##### **In-person visits**\n\nBeginning June 11, [all DMV offices](https://www.dmv.ca.gov/portal/news-and-media/dmv-reopens-remaining-field-offices-to-public/) are open to the public for appointments that require an in-person visit. You will be required to wear a mask and must remain 6 feet apart in line.\n\nIn-person appointments are limited to:\n\n*   Paying registration for a vehicle impounded because of registration-related issues\n*   Reinstating a suspended or revoked driver license\n*   Applying for a reduced-fee or no-fee identification card\n*   Processing commercial driver license transactions\n*   Applying for a disabled person parking placards\n*   Adding an ambulance certificate or firefighter endorsement to a driver license\n*   Verifying a transit training document to drive a transit bus\n*   Processing DMV Express customers for REAL ID transactions, if time and space allows\n*   Behind-the-wheel driving tests\n    *   On June 26, the DMV began behind-the-wheel driving tests. All cancelled driving test appointments will be rescheduled. New tests will not be available until all cancelled appointments are completed. \n    *   For the health and safety of drivers and DMV staff, [you must wear a face covering and will have your temperature checked](https://www.dmv.ca.gov/portal/dmv-expands-its-health-screening-and-temperature-check-protocols-to-protect-customers-and-employees/) before the test.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C32" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1214,10 +1214,10 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>Are there travel restrictions into or out of California?</v>
+        <v>Can I get my car smog checked?</v>
       </c>
       <c r="B33" t="str">
-        <v>There are currently no restrictions for entering California if you are coming from another state in the U.S. The federal government has placed restrictions on certain international travelers. With specific exceptions, foreign nationals who visited certain countries during the past 14 days are prohibited from entry to the United States. All international travelers, including US citizens and permanent residents, should quarantine for 14 days after coming to California from any other country. All travelers should take safety precautions when considering traveling.·       \n\n*   Don’t travel if you have been sick in the past 14 days or if you live with someone with COVID-19·        \n*   Don’t travel with someone who is sick\n*   Wear a mask in public\n*   Wash your hands\n*   Keep 6 feet from anyone you don’t live with\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>It depends. Some smog check locations may be closed. The [Bureau of Automotive Repair](https://www.bar.ca.gov/COVID-19_Impacts_on_BAR_Programs_and_Services.aspx) advises drivers to still pay DMV vehicle registration fees to avoid any late fees. However, you will not receive your new registration or year sticker until the smog information has been received by DMV. Once state and local orders or directives are no longer in effect, you can then obtain the required smog check certificate to complete the DMV vehicle registration process.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C33" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1240,13 +1240,13 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>Are swimming pools open?</v>
+        <v>What if I don’t have health insurance and I need COVID-19 diagnosis, testing or treatment?</v>
       </c>
       <c r="B34" t="str">
-        <v>Outdoor swimming pools are allowed to open in all counties in California. Outdoor pools must close slides, rides, or other attractions. \n\nIndoor swimming pools are closed in counties on the Monitoring List. \n\nWater parks, both indoor and outdoor, remain closed throughout the state.\n\nSaunas, steam rooms, and hot tubs, whether indoor or outdoor, remain closed throughout the state.  \n\nWhen out of the water, masks or face coverings should be worn. Physical distancing should be practiced at all times. Group gatherings are not allowed. Bring your own towel, and don’t share items that are worn on the face (like goggles, nose clips, or snorkels). Pool operators should follow heightened cleaning and safety guidance in response to COVID-19. See sector guidance for [gyms and fitness centers](https://files.covid19.ca.gov/pdf/guidance-fitness--en.pdf) and [campgrounds and outdoor recreation](https://files.covid19.ca.gov/pdf/guidance-campgrounds-outdoor-recreation--en.pdf).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>The cost of needed COVID-19 diagnosis, testing and treatment for the uninsured is [paid for by the government](https://www.hrsa.gov/CovidUninsuredClaim). Check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by talking to your doctor. Medically necessary [testing](https://covid19.ca.gov/testing-and-treatment/) is also free through Verily’s Project Baseline or OptumServe\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C34" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/healthcare/</v>
       </c>
       <c r="D34" t="str">
         <v xml:space="preserve"> </v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>Can I go to the Department of Motor Vehicles (DMV)?</v>
+        <v>Does my health plan have to cover my COVID-19 test?</v>
       </c>
       <c r="B35" t="str">
-        <v>Beginning June 11, [all DMV offices](https://www.dmv.ca.gov/portal/news-and-media/dmv-reopens-remaining-field-offices-to-public/) are open to the public to help with appointments that require an in-person visit. You will be required to wear a mask and must remain 6 feet apart in line. In-person appointments are limited to:\n\n*   Paying registration for a vehicle impounded because of registration-related issues\n*   Reinstating a suspended or revoked driver license\n*   Applying for a reduced-fee or no-fee identification card\n*   Processing commercial driver license transactions\n*   Applying for a disabled person parking placards\n*   Adding an ambulance certificate or firefighter endorsement to a driver license\n*   Verifying a transit training document to drive a transit bus\n*   Processing DMV Express customers for REAL ID transactions, if time and space allows\n*   On June 26, the DMV will begin behind-the-wheel driving tests. The DMV will reschedule all cancelled driving test appointments. New behind-the-wheel driving tests will not be available until all cancelled appointments are completed. \n    *   [For the health and safety of drivers and DMV staff](https://www.dmv.ca.gov/portal/news-and-media/dmv-resumes-behind-the-wheel-drive-tests-with-new-protocols-on-friday/), you must wear a face covering and will have your temperature checked before the test.\n\nDMV services that do not require an in-person office visit can be accessed through the [DMV Virtual Field Office](https://virtual.dmv.ca.gov/), including driver’s license renewals, vehicle registrations, title changes, and more.\n\nDMV has extended deadlines for:\n\n*   Drivers 70 years of age and older with licenses expiring between March 1 through December 31, 2020 are valid for one year from the original expiration date.\n*   Drivers 69 years of age and younger with licenses expiring between March 1 through July 31, 2020 can request a free temporary [extension online](https://www.dmv.ca.gov/portal/dmv-virtual-office/temporary-driver-license-extension/), though one is not needed to drive.\n*   Expiring commercial licenses, endorsements, and certificates are valid through June 30, 2020.\n*   In-person renewals for vehicle registrations that expire between the dates of March 16, 2020, and May 31, 2020.\n*   In-person renewals for those with safe driving records whose last DMV visit was 15 years ago.\n*   Driver license permits expiring between June through August 2020 are extended six months or to a date 24 months from the date of application, whichever is earlier.\n*   Commercial learner’s permits expiring between March and June 2020 are now valid through June 30, 2020.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes, if you:\n\n*   Have COVID-19 symptoms,\n*   Were exposed to someone who has COVID-19, or\n*   The test is medically necessary for your situation. \n\nIf you have COVID-19 symptoms or think you’ve been exposed, under federal law, you can get a test anywhere and your health plan must pay for it.\n\nIf you are an [essential worker](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf), your health plan must cover your COVID-19 test. But you must contact your health plan before getting tested. \n\nIf none of these things above are true but you’d still like a test, contact your health plan or health care provider.\n\nAs a first step, you can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C35" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/healthcare/</v>
       </c>
       <c r="D35" t="str">
         <v xml:space="preserve"> </v>
@@ -1292,13 +1292,13 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>Can I get my car smog checked?</v>
+        <v>How long will I have to wait to get a coronavirus test?</v>
       </c>
       <c r="B36" t="str">
-        <v>It depends. Some smog check locations may be closed. The [Bureau of Automotive Repair](https://www.bar.ca.gov/COVID-19_Impacts_on_BAR_Programs_and_Services.aspx) advises drivers to still pay DMV vehicle registration fees to avoid any late fees. However, you will not receive your new registration or year sticker until the smog information has been received by DMV. Once state and local orders or directives are no longer in effect, you can then obtain the required smog check certificate to complete the DMV vehicle registration process.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Your wait time depends on why you are seeking a test. \n\n**If you have COVID-19 symptoms or think you were exposed,** under federal law, you can go immediately to any testing site. Find a testing site on our [Testing page](https://covid19.ca.gov/testing-and-treatment/#top), or call your health plan for an available testing location.\n\n**If you are an [essential worker](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf),** your health plan must offer you a test appointment within 48 hours. The testing site must be within 15 miles or 30 minutes of your home or workplace. If your health plan can’t find you such an appointment, then you can go to any available testing site. Your health plan will pay for the test. \n\n**If neither of these cases above are true,** your provider may still decide that a COVID-19 test is medically necessary for you. In that case, your health plan must offer you a test appointment within 96 hours. The testing site must be within 15 miles or 30 minutes of your home or workplace. If your health plan can’t find you such an appointment, then you can go to any available testing site.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C36" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/healthcare/</v>
       </c>
       <c r="D36" t="str">
         <v xml:space="preserve"> </v>
@@ -1318,10 +1318,10 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>What if I don’t have health insurance and I need COVID-19 diagnosis, testing or treatment?</v>
+        <v>I get my health care coverage through my employer, who has a “self-insured” plan. Do the California Department of Managed Health Care (DMHC) regulations apply to me?</v>
       </c>
       <c r="B37" t="str">
-        <v>The cost of needed COVID-19 diagnosis, testing and treatment for the uninsured is [paid for by the government](https://www.hrsa.gov/CovidUninsuredClaim). Check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by talking to your doctor. Medically necessary [testing](https://covid19.ca.gov/testing-and-treatment/) is also free through Verily’s Project Baseline or OptumServe\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Self-insured plans are regulated by the federal government, not the state. If you have COVID-19 symptoms or were exposed to someone with symptoms, under federal law, your self-insured plan must cover your test. In all other instances, you should talk to your plan to find out whether they will cover COVID-19 testing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C37" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1344,10 +1344,10 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>Does my health plan have to cover my COVID-19 test?</v>
+        <v>How does my health plan know if I’m an essential worker?</v>
       </c>
       <c r="B38" t="str">
-        <v>Yes, if you’re experiencing COVID-19 symptoms, you think you were exposed to someone who has COVID-19, or the test is otherwise medically necessary for your situation. \n\nIf you have symptoms of COVID-19 or you think you’ve been exposed to someone with COVID-19, under federal law, you can obtain a COVID-19 test anywhere and your health plan must pay for the test. \n\nIf you don’t have symptoms and don’t think you’ve been exposed to someone with COVID-19, but you are an [essential worker](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf) as defined for COVID-19 testing coverage, your health plan must cover your COVID-19 test. However, you must contact your health plan before getting testing. \n\nIf you don’t have symptoms, don’t think you’ve been exposed to someone with COVID-19, and aren’t an [essential worker](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf) as defined for COVID-19 testing coverage, and you think you need a test, please contact your health plan or health care provider for further guidance.\n\nAs a first step, you can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor through [telehealth](https://covid19.ca.gov/telehealth/).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Your health plan can ask you questions about why you want a COVID-19 test and about the nature of your work. This helps them determine whether a COVID-19 test is medically necessary for you.\n\nBut they can’t ask you to provide further documentation or evidence of your work status. For example, they can’t ask you to provide written proof of where you work or the conditions of your workplace.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C38" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1370,10 +1370,10 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>How long will I have to wait to get a test?</v>
+        <v>I have a concern or complaint about getting care for COVID-19 under my health insurance. What can I do?</v>
       </c>
       <c r="B39" t="str">
-        <v>Your wait time depends on why you are seeking a test. \n\n**If you have symptoms of COVID-19 or think you were exposed,** under federal law, you can go immediately to any available testing site. Find a testing site on our [Testing page,](https://covid19.ca.gov/testing-and-treatment/#top) or call your health plan so they can direct you to an available testing location. \n\n**If you don’t have symptoms or suspected exposure, and you are an** [**essential worker**](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf)**,** your health plan must offer you a test appointment within 48 hours. The testing site must be within 15 miles or 30 minutes of your residence or workplace. If the health plan can’t find you an available appointment within that time and distance, then you can go to any available testing site and your health plan will pay for the test. \n\n**If you don’t have symptoms or suspected exposure, and you are not an essential worker,** if your provider determines a COVID-19 test is medically necessary for you, your health plan must offer you a test appointment within 96 hours. The testing site must be within 15 miles or 30 minutes of your residence or workplace. If the health plan can’t find you an available appointment within that time and distance, you can go to any available testing site.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>If you can’t access care, or were charged in error, follow up with your health plan. Call the member phone number listed on your health plan card. If they don’t fix the problem, call the [California Department of Managed Health Care (DMHC)](http://www.dmhc.ca.gov/?referral=healthhelp.ca.gov) Help Center at [1-888-466-2219](tel:888-466-2219).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C39" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1396,10 +1396,10 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>I get my health care coverage through my employer, who has a “self-insured” plan. Do the California Department of Managed Health Care (DMHC) regulations apply to me?</v>
+        <v>Do Medicare or Medicare Advantage Plans cover coronavirus tests or coronavirus antibody tests?</v>
       </c>
       <c r="B40" t="str">
-        <v>Self-insured plans are regulated by the federal government, rather than the state. If you have symptoms of COVID-19 or you were exposed to someone who you know or suspect has COVID-19, under federal law, your employer’s self-insured plan must cover your test. In all other instances, you should talk to your employer’s self-insured plan to find out whether they will cover COVID-19 testing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. Both [Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) cover [diagnostic](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test), with no out-of-pocket costs.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C40" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1422,10 +1422,10 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>How does my health plan know if I’m an essential worker?</v>
+        <v>Can I use telehealth if I am on Medicare?</v>
       </c>
       <c r="B41" t="str">
-        <v>Your health plan can ask you questions about why you want a COVID-19 test and about the nature of your work. They can ask these questions to help determine whether a COVID-19 test is medically necessary for you. \n\nHowever, your health plan can’t ask you to provide further documentation or evidence of your work status. For example, your health plan can’t ask you to provide written proof of where you work or the conditions of your workplace.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. Medicare has expanded its [telehealth services](https://www.medicare.gov/coverage/telehealth) to respond to the public health emergency. You can now use your smartphone, video chat, or online portal from home to talk with a range of providers, like doctors, nurse practitioners, clinical psychologists, licensed clinical social workers, physical therapists, occupational therapists, and speech language pathologists. If you have original Medicare, you can get many services for free through [telehealth](https://covid19.ca.gov/telehealth/). This includes common office visits, mental health counseling, and preventive health screenings.\n\nIf you have a [Medicare Advantage Plan](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans), you have access to these same benefits. Many plans offer more [telehealth](https://covid19.ca.gov/telehealth/) and other benefits, like meal delivery or medical transport. Check with your plan about coverage and costs.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C41" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>I have a concern or complaint about getting care for COVID-19 under my health insurance. What can I do?</v>
+        <v>I am uninsured and diagnosed with COVID-19. What testing and treatment for me are paid for by the federal government?</v>
       </c>
       <c r="B42" t="str">
-        <v>If you are having trouble accessing care, or were inappropriately charged for medically necessary screening, testing, or treatment for COVID-19, follow up directly with your health plan by calling the member phone number listed on your health plan card. If your health plan doesn’t resolve the issue, contact the [California Department of Managed Health Care (DMHC)](http://www.dmhc.ca.gov/?referral=healthhelp.ca.gov) Help Center for assistance at 1-888-466-2219.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>The following services are covered:\n\n*   Specimen collection, diagnostic and antibody testing\n*   Testing-related visits, including in the following settings: \n    *   Office \n    *   Urgent care \n    *   Emergency room, or \n    *   Telehealth\n*   Treatment, including:\n    *   Office visit\n    *   [Telehealth](https://covid19.ca.gov/telehealth/#top)\n    *   Emergency room \n    *   Inpatient \n    *   Outpatient/observation \n    *   Skilled nursing facility \n    *   Long-term acute care (LTAC) \n    *   Acute inpatient rehab \n    *   Home health \n    *   Durable Medical Equipment (DME), like oxygen and ventilator\n    *   Emergency ambulance transportation \n    *   Non-emergent patient transfers via ambulance, and\n    *   FDA-approved drugs administered as part of an inpatient stay\n    *   FDA-approved vaccine, when available\n\nFor more details, see the [HRSA website](https://www.hrsa.gov/CovidUninsuredClaim) and their [frequently asked questions](https://www.hrsa.gov/coviduninsuredclaim/frequently-asked-questions).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C42" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1474,10 +1474,10 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>Do Medicare or Medicare Advantage Plans cover coronavirus tests or coronavirus antibody tests?</v>
+        <v>Does Medi-Cal provide free COVID-19 diagnosis, testing and treatments for the uninsured?</v>
       </c>
       <c r="B43" t="str">
-        <v>Yes. Both [Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) cover [coronavirus tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test) tests, with no out-of-pocket costs. \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. [Medi-Cal is available](https://www.dhcs.ca.gov/services/medi-cal/eligibility/Pages/COVID-19-Presumptive-Eligibility-Program.aspx#:~:text=Presumptive%20Eligibility%20(PE)%20for%20COVID,associated%20office%2C%20clinic%2C%20or%20emergency) to those with no insurance or whose insurance does not cover COVID-19 diagnosis, testing, and treatment. COVID-19 diagnosis, testing and treatment are considered emergency services. This allows all Medi-Cal beneficiaries, regardless of their scope of coverage under Medi-Cal or their immigration status, to receive at no cost all medically necessary testing, testing-related, and treatment services, which may include inpatient or outpatient services related to a COVID-19 diagnosis.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C43" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1500,10 +1500,10 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>Can I use telehealth if I am on Medicare?</v>
+        <v>My Medi-Cal eligibility is expiring. Do I need to renew it now?</v>
       </c>
       <c r="B44" t="str">
-        <v>Yes. Medicare has temporarily expanded its coverage of [telehealth services (medical care via phone, video chat, or online portal)](https://www.medicare.gov/coverage/telehealth) to respond to the current Public Health Emergency. You can now use a wide range of communication tools (including smartphone) from home to interact with a range of providers, like doctors, nurse practitioners, clinical psychologists, licensed clinical social workers, physical therapists, occupational therapists, and speech language pathologists. If you have original Medicare, you can get many services without a copayment through [telehealth,](https://covid19.ca.gov/telehealth/) including evaluation and management visits (common office visits), mental health counseling, and preventive health screenings.\n\nIf you have a [Medicare Advantage Plan](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans), you have access to these same benefits. Many plans offer additional [telehealth](https://covid19.ca.gov/telehealth/) benefits and expanded benefits, like meal delivery or medical transport services. Check with your plan about your coverage and costs.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>**No.** [DHCS instructed counties](https://www.dhcs.ca.gov/services/medi-cal/eligibility/letters/Documents/I20-14.pdf) to freeze the Medi-Cal eligibility redeterminations for the duration of the COVID-19 public health emergency.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C44" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1526,10 +1526,10 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>What COVID-19 testing and treatments are covered by the federal government’s free uninsured program?</v>
+        <v>I don’t have health insurance and/or a regular doctor. How can I get quick access to medical advice?</v>
       </c>
       <c r="B45" t="str">
-        <v>The following services are covered by the federal government if you are  uninsured and diagnosed with a primary COVID-19 diagnosis:\n\n*   Specimen collection, diagnostic and antibody testing\n*   Testing-related visits, including in the following settings: office, urgent care, emergency room, or telehealth\n*   Treatment, including office visit, [telehealth](https://covid19.ca.gov/telehealth/#top), emergency room, inpatient, outpatient/observation, skilled nursing facility, long-term acute care (LTAC), acute inpatient rehab, home health, Durable Medical Equipment (DME) like oxygen and ventilator, emergency ambulance transportation, non-emergent patient transfers via ambulance, and FDA-approved drugs as they become available for COVID-19 treatment and administered as part of an inpatient stay\n*   FDA-approved vaccine, when available\n\nFor additional details, see the [Health Resources &amp; Services Administration (HRSA) website](https://www.hrsa.gov/CovidUninsuredClaim) and their [Frequently Asked Questions](https://www.hrsa.gov/coviduninsuredclaim/frequently-asked-questions).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Call Medi-Nurse. Medi-Nurse is a [free, 24/7 nurse advice line](https://www.dhcs.ca.gov/Pages/DHCS-COVID%E2%80%9119-Medi-Nurse-Line.aspx) available at [1-877-409-9052](tel:877-409-9052). You can speak directly with a healthcare professional about your symptoms, get advice on testing and treatment in your area, or ask how to apply for health insurance.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C45" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1552,10 +1552,10 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>Does Medi-Cal provide free COVID-19 diagnosis, testing and treatments for the uninsured?</v>
+        <v>I am nervous or scared. What can I do?</v>
       </c>
       <c r="B46" t="str">
-        <v>Yes. [Medi-Cal is available](https://www.dhcs.ca.gov/services/medi-cal/eligibility/Pages/COVID-19-Presumptive-Eligibility-Program.aspx#:~:text=Presumptive%20Eligibility%20(PE)%20for%20COVID,associated%20office%2C%20clinic%2C%20or%20emergency) to individuals with no insurance or who currently have private insurance that does not cover COVID-19 diagnostic testing and testing-related services. Due to the current public health emergency, COVID-19 testing, evaluation, and treatment services are deemed emergency services. This allows all Medi-Cal beneficiaries, regardless of their scope of coverage under Medi-Cal or their immigration status, to receive at no cost all medically necessary testing, testing-related, and treatment services, which may include inpatient or outpatient services related to a COVID-19 diagnosis.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>You are not alone. The California Surgeon General released [two playbooks for managing stress](https://covid19.ca.gov/manage-stress-for-health/#top) and tips for care-givers and kids. If you feel like you need to talk to someone and want emotional support see this [list of resources](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/#top).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C46" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1578,10 +1578,10 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>I am nervous or scared. What can I do?</v>
+        <v>What if I need to visit a health care provider?</v>
       </c>
       <c r="B47" t="str">
-        <v>You are not alone. The California Surgeon General released [two playbooks for managing stress](https://covid19.ca.gov/manage-stress-for-health/#top) and tips for care-givers and kids. If you feel like you need to talk to someone and want emotional support see this [list of resources](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/#top).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>If you have [coronavirus symptoms](https://covid19.ca.gov/symptoms-and-risks/#top), please contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) or use the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html).\n\nIf you have other illnesses or chronic conditions, use [telehealth](https://covid19.ca.gov/telehealth/) to get care from home.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call [911](tel:911), tell the operator your symptoms so the ambulance provider can be ready to treat you safely.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C47" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1604,10 +1604,10 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>My safety net eligibility (like CalFresh, Medi-Cal) is expiring and I am under the statewide stay home order for COVID-19. Do I need to renew my eligibility now?</v>
+        <v>What about routine, elective, or non-urgent medical or dental appointments?</v>
       </c>
       <c r="B48" t="str">
-        <v>****No, you will not need to renew until August 17, 2020.**** Governor Gavin Newsom issued an [executive order](https://www.gov.ca.gov/wp-content/uploads/2020/06/6.15.20-EO-N-69-20-text.pdf) to ensure that health care, food assistance, and in-home supportive services continue during the COVID-19 outbreak.\n\nThe order waives eligibility re-determinations for 150 days for participants in:\n\n*   Medi-Cal health coverage\n*   CalFresh food assistance\n*   CalWORKs\n*   Cash Assistance for Immigrants\n*   In-Home Supportive Services\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Non-emergency surgeries, like organ replacements and tumor removals, can take place. Your doctor will know if your hospital has enough capacity and protective equipment. Elective procedures should be cancelled or rescheduled. If possible, health care visits should be done remotely. [Dental services and preventive dental care](https://www.cdc.gov/coronavirus/2019-ncov/hcp/dental-settings.html) may be resumed. Contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) to see what services they are providing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C48" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1630,10 +1630,10 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>What if I need to visit a health care provider?</v>
+        <v>Can I get my prescriptions filled?</v>
       </c>
       <c r="B49" t="str">
-        <v>If you have [coronavirus symptoms](https://covid19.ca.gov/symptoms-and-risks/#top), please contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) or use the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) self-checker.\n\nIf you have other illnesses or chronic conditions, use [telehealth](https://covid19.ca.gov/telehealth/) to get care from home.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call 911, tell the 911 operator your exact symptoms so the ambulance provider can be ready to treat you safely.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. Pharmacies and medical cannabis dispensaries are open.\n\nCall your doctor to get a new prescription or adjust your existing prescriptions.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C49" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1656,10 +1656,10 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>What about routine, elective, or non-urgent medical or dental appointments?</v>
+        <v>I am an older Californian who is isolating at home and I need non-urgent help. What can I do?</v>
       </c>
       <c r="B50" t="str">
-        <v>Preventive care services and non-emergency surgeries, like organ replacements and tumor removals, can take place if hospitals have enough capacity and protective equipment to do so safely. Eye exams, and elective procedures should be cancelled or rescheduled. If possible, health care visits should be done remotely. [Dental services and preventive dental care](https://www.cdc.gov/coronavirus/2019-ncov/hcp/dental-settings.html) may be resumed. Contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) to see what services they are providing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Call the statewide hotline for older Californians at [1-833-544-2374](tel:833-544-2374). They can help you with non-urgent medical needs, meal delivery, tracking down prescriptions, and more. The most important thing you can do is stay home for your health and wellbeing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C50" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1682,10 +1682,10 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>Can I get my prescriptions filled?</v>
+        <v>How can I make sure the older Californians in my life are safe and healthy during the stay home order?</v>
       </c>
       <c r="B51" t="str">
-        <v>Yes. You may leave your home to get prescriptions or cannabis from dispensaries with medical permits.\n\nYou can contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) to get a new prescription or adjust your existing prescriptions. \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Check in on your older neighbors and loved ones to make sure they are okay. Give them a call, text, or physically-distanced door knock. You can also teach them how to use FaceTime, Zoom, Google Duo, or Facebook video to communicate. It’s important to keep in touch with older loved ones for their mental health and safety.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C51" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1708,10 +1708,10 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>I am an older Californian who is isolating at home and I need non-urgent assistance. What can I do?</v>
+        <v>Can I care for my elderly parents or friends who need help? Or a friend or family member who has disabilities?</v>
       </c>
       <c r="B52" t="str">
-        <v>You can call the statewide hotline for older Californians at [1-833-544-2374](tel:1-833-544-2374) for your non-urgent medical needs, to get meals delivered, to track down prescriptions, and more. The most important thing you can do is stay home for your health and wellbeing. If you are experiencing an emergency please call 911.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. Protect them and yourself by following physical distancing guidelines. Wear a [mask](https://covid19.ca.gov/masks-and-ppe/#top), wash your hands often, maintain at least six feet of distance between you, and cover your cough or sneeze. If you have early signs of a cold, please stay away from your older loved ones.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C52" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1734,10 +1734,10 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>How can I make sure the older Californians in my life are safe and healthy during the stay home order?</v>
+        <v>Can I visit loved ones in the hospital, nursing home, or residential care facility?</v>
       </c>
       <c r="B53" t="str">
-        <v>You should check in on your older neighbors and loved ones with a call, text, or physically-distanced door knock to make sure they are okay. You can also teach them how to use FaceTime, Zoom, Google Duo or Facebook video to communicate. The most important thing you can do is to keep in touch with older loved ones for their mental health and safety.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Generally, no. There are exceptions, such as if you are taking a minor or someone who is developmentally disabled to the hospital. For most other situations, the order prohibits visitation to these kinds of facilities. This is difficult, but necessary to protect hospital staff and other patients. See more about this in [frequently asked questions for friends and family with a loved one in a skilled nursing or residential care facility](https://www.aging.ca.gov/download.ashx?lE0rcNUV0zaaXLD5JZ%2f6Uw%3d%3d).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C53" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1760,10 +1760,10 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>Can I leave home to care for my elderly parents or friends who require assistance? Or a friend or family member who has disabilities?</v>
+        <v>Can I get free COVID-19 testing or treatment if I am a senior over 65, disabled, uninsured, or an undocumented immigrant?</v>
       </c>
       <c r="B54" t="str">
-        <v>Yes. Be sure that you protect them and yourself by following physical distancing guidelines such as wearing a mask, washing hands before and after, using hand sanitizer, maintaining at least six feet of distance when possible, and covering your cough or sneeze. If you have early signs of a cold, please stay away from your older loved ones.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)&lt;!-- disability, senior --&gt;</v>
+        <v>[Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) provide free COVID-19 [diagnostic](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test). Needed COVID-19 diagnosis, testing, and treatment for the uninsured is [paid for by the government](https://www.hrsa.gov/CovidUninsuredClaim). \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C54" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1786,13 +1786,13 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>Can I visit loved ones in the hospital, nursing home, skilled nursing facility, or other residential care facility?</v>
+        <v>What do taxpayers need to do if they want to take advantage of relief from the California Department of Tax and Fee Administration?</v>
       </c>
       <c r="B55" t="str">
-        <v>Generally, no. There are limited exceptions, such as if you are going to the hospital with a minor who is under 18 or someone who is developmentally disabled and needs assistance. For most other situations, the order prohibits visitation to these kinds of facilities. This is difficult, but necessary to protect hospital staff and other patients. Check the [frequently asked questions for friends and family with a loved one in a skilled nursing or residential care facility](https://www.aging.ca.gov/download.ashx?lE0rcNUV0zaaXLD5JZ%2f6Uw%3d%3d) for more detailed information.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)&lt;!-- elderly, disability, senior --&gt;</v>
+        <v>Interested taxpayers should contact CDTFA by visiting the [CDTFA website](http://cdtfa.ca.gov/) or calling [800-400-7115](tel:800-400-7115).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C55" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D55" t="str">
         <v xml:space="preserve"> </v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>Can I get free COVID-19 testing or treatment if I am a senior over 65, disabled, uninsured, or an undocumented immigrant?</v>
+        <v>When will taxpayers start on these payment plans?</v>
       </c>
       <c r="B56" t="str">
-        <v>[Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) provide free COVID-19 [diagnostic](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Guidance-for-Health-Care-Providers.aspx) and [antibody tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test). Needed COVID-19 diagnosis, testing, and treatment for the uninsured is [paid for by the government](https://www.hrsa.gov/CovidUninsuredClaim). \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Given that the April deadline to file and pay sales and use tax returns has been extended to late July for all but the largest taxpayers, CDTFA expects that most participating taxpayers will begin their payment arrangements in late July of this year.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C56" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D56" t="str">
         <v xml:space="preserve"> </v>
@@ -1838,10 +1838,10 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>What do taxpayers need to do if they want to take advantage of relief from the California Department of Tax and Fee Administration?</v>
+        <v>How will the payment plans work?</v>
       </c>
       <c r="B57" t="str">
-        <v>Interested taxpayers should contact CDTFA by visiting the [CDTFA website](http://cdtfa.ca.gov/) or calling [800-400-7115](tel:800-400-7115).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Qualifying sales and use taxpayers with deferred liabilities up to $50,000 will pay their tax due in 12 equal monthly installments. No interest or penalties will be assessed against the liability.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C57" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1864,10 +1864,10 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>When will taxpayers start on these payment plans?</v>
+        <v>Is this only for tax payments due for the 1st quarter of 2020?</v>
       </c>
       <c r="B58" t="str">
-        <v>Given that the April deadline to file and pay sales and use tax returns has been extended to late July for all but the largest taxpayers, CDTFA expects that most participating taxpayers will begin their payment arrangements in late July of this year.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>If taxpayers choose to use this program to distribute the burden of their May or June prepayments or their July return, CDTFA will work to accommodate those taxpayers.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C58" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1890,10 +1890,10 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>How will the payment plans work?</v>
+        <v>What if taxpayers owe more than the $50,000 limit on the relief?</v>
       </c>
       <c r="B59" t="str">
-        <v>Qualifying sales and use taxpayers with deferred liabilities up to $50,000 will pay their tax due in 12 equal monthly installments. No interest or penalties will be assessed against the liability.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The maximum amount that any taxpayer can defer interest-free under this relief effort is $50,000.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C59" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1916,10 +1916,10 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>Is this only for tax payments due for the 1st quarter of 2020?</v>
+        <v>What if taxpayers with more than $5 million in annual taxable sales need this relief?</v>
       </c>
       <c r="B60" t="str">
-        <v>If taxpayers choose to use this program to distribute the burden of their May or June prepayments or their July return, CDTFA will work to accommodate those taxpayers.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>We recognize that some taxpayers, particularly in low margin businesses, with annual taxable sales over $5 million may also need this relief. Those taxpayers are encouraged to reach out to CDTFA, which will work with them to provide relief where appropriate.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C60" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1942,10 +1942,10 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>What if taxpayers owe more than the $50,000 limit on the relief?</v>
+        <v>Is the deadline for filing California tax returns extended?</v>
       </c>
       <c r="B61" t="str">
-        <v>The maximum amount that any taxpayer can defer interest-free under this relief effort is $50,000.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Yes. All California taxpayers (individuals and businesses) can file and pay by July 15, 2020. See [information from the CA Franchise Tax Board](https://www.ftb.ca.gov/about-ftb/newsroom/news-releases/2020-3-state-postpones-tax-deadlines-until-july-15-due-to-the-covid-19-pandemic.html) for more information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C61" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1968,10 +1968,10 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>What if taxpayers with more than $5 million in annual taxable sales need this relief?</v>
+        <v>What is a loan guarantee?</v>
       </c>
       <c r="B62" t="str">
-        <v>We recognize that some taxpayers, particularly in low margin businesses, with annual taxable sales over $5 million may also need this relief. Those taxpayers are encouraged to reach out to CDTFA, which will work with them to provide relief where appropriate.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>A loan guarantee is a credit enhancement that helps mitigate the risk assumed by a lending institution when making a loan. With the Small Business Finance Center’s Disaster Relief Loan Guarantee Program, IBank agrees to guarantee up to 95% of the loan, removing the barriers to capital that often exist for small business borrowers that may not otherwise be eligible for traditional lending. This program also can assist those who may not be eligible for a U.S. Small Business Administration (SBA) loan.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C62" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1994,10 +1994,10 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>Is the deadline for filing California tax returns extended?</v>
+        <v>Who is eligible to apply for a loan guarantee?</v>
       </c>
       <c r="B63" t="str">
-        <v>Yes. All California taxpayers (individuals and businesses) can file and pay by July 15, 2020. See [information from the CA Franchise Tax Board](https://www.ftb.ca.gov/about-ftb/newsroom/news-releases/2020-3-state-postpones-tax-deadlines-until-july-15-due-to-the-covid-19-pandemic.html) for more information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Small business entities that have been affected by loss, damage or other economic injury due to the COVID-19 pandemic and meet the program’s eligibility requirements. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C63" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2020,10 +2020,10 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>What is a loan guarantee?</v>
+        <v>What do you consider a small business?</v>
       </c>
       <c r="B64" t="str">
-        <v>A loan guarantee is a credit enhancement that helps mitigate the risk assumed by a lending institution when making a loan. With the Small Business Finance Center’s Disaster Relief Loan Guarantee Program, IBank agrees to guarantee up to 95% of the loan, removing the barriers to capital that often exist for small business borrowers that may not otherwise be eligible for traditional lending. This program also can assist those who may not be eligible for a U.S. Small Business Administration (SBA) loan.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The business must have between 1-750 employees and be established as an entity, including:\n\n*   Sole Proprietor – Individual using legal name as business name that files a Schedule C, Schedule F, or has a fictitious business name or DBA statement\n    *   If the loan appears to be in the name of an individual, evidence of Sole Proprietorship will be required and may include a Schedule C, Schedule F, Seller’s Permit, and/or fictitious business name or DBA statement\n*   Limited Liability Company \n*   Cooperative\n*   Corporation\n*   Partnership\n*   S-Corporation\n*   Not-for-profit\n\nThe program will not accept an _individual_ as the borrower. It is permissible for an individual to be a guarantor or co-borrower on the loan, but the primary borrower must be a small business. It does not consider citizenship or immigration status for eligibility requirements**,** as long as the entity/individual meets the above criteria. Trucking owners/operators are eligible as long as they are registered as a legal business entity.\n\n**AND**\n\n*   The business activity must be eligible under the program and in one of the industries listed in the [North American Industry Classification System (NAICS) codes list](http://www.census.gov/eos/www/naics), and\n*   It must be located in a declared disaster area. A major disaster area declaration was made for the state of California on March 22, 2020 in regards to the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C64" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2046,10 +2046,10 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>Who is eligible to apply?</v>
+        <v>What are excluded businesses?</v>
       </c>
       <c r="B65" t="str">
-        <v>Small business entities that have been affected by loss, damage or other economic injury due to the COVID-19 pandemic and meet the program’s eligibility requirements. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Businesses that are not eligible include passive real estate businesses (rental income, etc.).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C65" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2072,10 +2072,10 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>What do you consider a small business?</v>
+        <v>Can I apply for a loan guarantee only if I am ineligible for federal disaster fund financing, such as a SBA loan?</v>
       </c>
       <c r="B66" t="str">
-        <v>The business must have between 1-750 employees and be established as an entity, including:\n\n*   Sole Proprietor – Individual using legal name as business name that files a Schedule C, Schedule F, or has a fictitious business name or DBA statement\n    *   If the loan appears to be in the name of an individual, evidence of Sole Proprietorship will be required and may include a Schedule C, Schedule F, Seller’s Permit, and/or fictitious business name or DBA statement\n*   Limited Liability Company \n*   Cooperative\n*   Corporation\n*   Partnership\n*   S-Corporation\n*   Not-for-profit\n\nThe program will not accept an _individual_ as the borrower. It is permissible for an individual to be a guarantor or co-borrower on the loan, but the primary borrower must be a small business. It does not consider citizenship or immigration status for eligibility requirements**,** as long as the entity/individual meets the above criteria. Trucking owners/operators are eligible as long as they are registered as a legal business entity.\n\n**AND**\n\n*   The business activity must be eligible under the program and in one of the industries listed in the [North American Industry Classification System (NAICS) codes list](http://www.census.gov/eos/www/naics), and\n*   It must be located in a declared disaster area. A major disaster area declaration was made for the state of California on March 22, 2020 in regards to the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Yes, this program is designed for those who do not qualify for federal programs. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C66" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2098,10 +2098,10 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>What are excluded businesses?</v>
+        <v>How much can I borrow?</v>
       </c>
       <c r="B67" t="str">
-        <v>Businesses that are not eligible include passive real estate businesses (rental income, etc.).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The Small Business Finance Center’s Disaster Relief Loan Guarantee Program allows a maximum loan of $1.25 million and a maximum guarantee of $1 million. To serve as many California small businesses as possible, the COVID-19 disaster program is focused on serving small businesses, especially those in low-wealth and immigrant communities with needs from $500 to $50,000. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C67" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2124,10 +2124,10 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>Can I apply for a loan guarantee only if I am ineligible for federal disaster fund financing, such as a SBA loan?</v>
+        <v>What are the loan terms?</v>
       </c>
       <c r="B68" t="str">
-        <v>Yes, this program is designed for those who do not qualify for federal programs. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The length of the loan can be negotiated with your lender, but the guarantee is good for up to seven years. The interest rate and loan criteria will be determined by the lender and could depend on the credit strength of the business. The guarantee is designed to lower the interest rate in exchange for a higher guarantee to your lender. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C68" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2150,10 +2150,10 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>How much can I borrow?</v>
+        <v>How can I apply for a loan guarantee?</v>
       </c>
       <c r="B69" t="str">
-        <v>The Small Business Finance Center’s Disaster Relief Loan Guarantee Program allows a maximum loan of $1.25 million and a maximum guarantee of $1 million. To serve as many California small businesses as possible, the COVID-19 disaster program is focused on serving small businesses, especially those in low-wealth and immigrant communities with needs from $500 to $50,000. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The Small Business Finance Center partners with Community Development Financial Institutions (CDFIs), Community Lending Institutions, and Financial Development Corporations (FDCs) to provide loan guarantees for small businesses.  To apply,\n\n*   View the [list of FDCs and participating lenders](http://www.ibank.ca.gov/small-business-finance-center/) interested in this Small Business Disaster Relief Loan Guarantee Program. \n*   Contact the lender on the list nearest to your business to apply.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C69" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2176,10 +2176,10 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>What are the loan terms?</v>
+        <v>What is the timing for the funding of loans?</v>
       </c>
       <c r="B70" t="str">
-        <v>The length of the loan can be negotiated with your lender, but the guarantee is good for up to seven years. The interest rate and loan criteria will be determined by the lender and could depend on the credit strength of the business. The guarantee is designed to lower the interest rate in exchange for a higher guarantee to your lender. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The program is in place and businesses can apply immediately. Once you provide your lender with complete information, you could be funded in a matter of days.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C70" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2202,10 +2202,10 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>How can I apply?</v>
+        <v>What can the money be used for?</v>
       </c>
       <c r="B71" t="str">
-        <v>The Small Business Finance Center partners with Community Development Financial Institutions (CDFIs), Community Lending Institutions, and Financial Development Corporations (FDCs) to provide loan guarantees for small businesses.  To apply,\n\n*   View the [list of FDCs and participating lenders](http://www.ibank.ca.gov/small-business-finance-center/) interested in this Small Business Disaster Relief Loan Guarantee Program. \n*   Contact the lender on the list nearest to your business to apply.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The funds are meant to help small businesses through this challenging time. Loan proceeds can be used for business continuance or to cure “economic injury” as a result of COVID-19.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C71" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2228,10 +2228,10 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>What is the timing for the funding of loans?</v>
+        <v>How will this program assist low-wealth and minority communities?</v>
       </c>
       <c r="B72" t="str">
-        <v>The program is in place and businesses can apply immediately. Once you provide your lender with complete information, you could be funded in a matter of days.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>By working with the Community Development Financial Institutions (CDFIs) throughout the state of California, this disaster relief program can play an important role in generating economic growth and opportunity in some of our most distressed communities. CDFIs and mission-based lenders play a vital role across the state and have experience steering lending and investment to where it is needed and will matter the most, in particular in low-wealth and immigrant communities. CDFIs and our partner Financial Development Corporations (FDCs) that process the loan guarantees are embedded in communities across the state, speak several languages, and are invested in the community successfully managing its way through this pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C72" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2254,10 +2254,10 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>What can the money be used for?</v>
+        <v>Are faith-based businesses eligible for this loan guarantee program?</v>
       </c>
       <c r="B73" t="str">
-        <v>The funds are meant to help small businesses through this challenging time. Loan proceeds can be used for business continuance or to cure “economic injury” as a result of COVID-19.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Faith-based businesses (non-profit or otherwise) that have business activity outside of worship are eligible as long as they are a legal business that has been affected by the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C73" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2280,10 +2280,10 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>How will this program assist low-wealth and minority communities?</v>
+        <v>What SBA programs are available to small businesses right now?</v>
       </c>
       <c r="B74" t="str">
-        <v>By working with the Community Development Financial Institutions (CDFIs) throughout the state of California, this disaster relief program can play an important role in generating economic growth and opportunity in some of our most distressed communities. CDFIs and mission-based lenders play a vital role across the state and have experience steering lending and investment to where it is needed and will matter the most, in particular in low-wealth and immigrant communities. CDFIs and our partner Financial Development Corporations (FDCs) that process the loan guarantees are embedded in communities across the state, speak several languages, and are invested in the community successfully managing its way through this pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The U.S. SBA offers the **Economic Injury Disaster Loan (EIDL)**.\n\nThe U.S. SBA is accepting new applications from all eligible businesses, and will continue to process **EIDL Loan applications** already submitted on a first come, first-served basis. Check the U.S. SBA’s [Disaster Loan Applications website](https://www.sba.gov/page/disaster-loan-applications#section-header-0) for more information.\n\nThe EIDL is a direct loan for up to $2 million at a rate of 3.75% for small businesses and 2.75% for nonprofits. [Apply directly with the SBA](https://covid19relief.sba.gov/#/). For questions, you can contact SBA’s Customer Service Line at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or send an email to [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nThe **Economic Injury Disaster Loan (**EIDL) **Advance** has been [discontinued](https://www.sba.gov/page/disaster-loan-applications#section-header-0). EIDL loan applications will still be processed even though the Advance is no longer available.\n\nThe [**Paycheck Protection Program (PPP)**](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program#section-header-0) closed August 8, 2020. The U.S. SBA is no longer accepting PPP applications from approved lenders.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C74" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2306,10 +2306,10 @@
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>Are faith-based businesses eligible for this loan guarantee program?</v>
+        <v>Where do I find more information on allowable expenses for a forgivable loan under the Paycheck Protection Program?</v>
       </c>
       <c r="B75" t="str">
-        <v>Faith-based businesses (non-profit or otherwise) that have business activity outside of worship are eligible as long as they are a legal business that has been affected by the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>You can find this on the Paycheck Protection Program’s [Loan Forgiveness Application](https://www.sba.gov/sites/default/files/2020-06/PPP%20Loan%20Forgiveness%20Application%20%28Revised%206.16.2020%29-fillable_0-508.pdf). The application provides detailed [instructions](https://www.sba.gov/sites/default/files/2020-06/PPP%20Loan%20Forgiveness%20Application%20Instructions%20%28Revised%206.16.2020%29-508.pdf) on how to apply for forgiveness of PPP loans. Once your business has expended the PPP funds and is ready to pursue loan forgiveness, please review the Loan Forgiveness Application and consult with your accountant, lender, or one of California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) for assistance. See SBA’s [loan details and forgiveness](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program#section-header-5) information, and check the [frequently asked questions](https://www.sba.gov/sites/default/files/2020-08/PPP%20--%20Loan%20Forgiveness%20FAQs%20%28August%2011%2C%202020%29.pdf) on PPP loan forgiveness.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C75" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2332,10 +2332,10 @@
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>What SBA programs are available to small businesses right now?</v>
+        <v>How does a business know if it is eligible for an SBA loan or loan guarantee program?</v>
       </c>
       <c r="B76" t="str">
-        <v>The U.S. SBA offers the **Economic Injury Disaster Loan (EIDL)**.\n\nThe U.S. SBA is accepting new applications from all eligible businesses, and will continue to process **EIDL Loan applications** already submitted on a first come, first-served basis. Check the U.S. SBA’s [Disaster Loan Applications website](https://www.sba.gov/page/disaster-loan-applications#section-header-0) for more information.\n\nThe EIDL is a direct loan for up to $2 million at a rate of 3.75% for small businesses and 2.75% for nonprofits. [Apply directly with the SBA](https://covid19relief.sba.gov/#/). For questions, you can contact SBA’s Customer Service Line at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or send an email to [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nThe **Economic Injury Disaster Loan (**EIDL) **Advance** has been [discontinued](https://www.sba.gov/page/disaster-loan-applications#section-header-0). EIDL loan applications will still be processed even though the Advance is no longer available.\n\nThe [**Paycheck Protection Program (PPP)**](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program#section-header-0) closed August 8, 2020. The U.S. SBA is no longer accepting PPP applications from approved lenders.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Small businesses with 500 employees or less are eligible to apply for the Small Business Debt Relief Program. Small businesses are also eligible to apply for the Economic Injury Disaster Loan (EIDL) program. Visit SBA’s comprehensive [COVID-19 support website](https://www.sba.gov/page/coronavirus-covid-19-small-business-guidance-loan-resources#section-header-4%20.) to find out more about SBA’s eligibility requirements for each program.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C76" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2358,10 +2358,10 @@
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>Where do I find more information on allowable expenses for a forgivable loan under the Paycheck Protection Program?</v>
+        <v>How do I reach SBA for any questions or assistance?</v>
       </c>
       <c r="B77" t="str">
-        <v>You can find this on the Paycheck Protection Program’s [Loan Forgiveness Application](https://www.sba.gov/sites/default/files/2020-06/PPP%20Loan%20Forgiveness%20Application%20%28Revised%206.16.2020%29-fillable_0-508.pdf). The application provides detailed [instructions](https://www.sba.gov/sites/default/files/2020-06/PPP%20Loan%20Forgiveness%20Application%20Instructions%20%28Revised%206.16.2020%29-508.pdf) on how to apply for forgiveness of PPP loans. Once your business has expended the PPP funds and is ready to pursue loan forgiveness, please review the Loan Forgiveness Application and consult with your accountant, lender, or one of California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) for assistance. See SBA’s [loan details and forgiveness](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program#section-header-5) information, and check the [frequently asked questions](https://www.sba.gov/sites/default/files/2020-08/PPP%20--%20Loan%20Forgiveness%20FAQs%20%28August%2011%2C%202020%29.pdf) on PPP loan forgiveness.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>SBA has district offices in California that are open to answer questions. You can use the [SBA’s Local Assistance Directory](https://www.sba.gov/local-assistance) to locate the office nearest you. You can also contact the SBA by phone at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or by email at [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).  \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C77" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2384,10 +2384,10 @@
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>How does a business know if it is eligible for an SBA loan or loan guarantee program?</v>
+        <v>How does a small business know which SBA loan or loan guarantee program is the right one? Can a small business apply to more than one?</v>
       </c>
       <c r="B78" t="str">
-        <v>Small businesses with 500 employees or less are eligible to apply for the Small Business Debt Relief Program. Small businesses are also eligible to apply for the Economic Injury Disaster Loan (EIDL) program. Visit SBA’s comprehensive [COVID-19 support website](https://www.sba.gov/page/coronavirus-covid-19-small-business-guidance-loan-resources#section-header-4%20.) to find out more about SBA’s eligibility requirements for each program.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Call or email the SBA to find out which program is right for you. While businesses can apply for and receive more than one form of capital assistance through the SBA, they cannot be used for the same purpose. The SBA can advise you on your options. Call [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or email [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C78" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2410,10 +2410,10 @@
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>How do I reach SBA for any questions or assistance?</v>
+        <v>How do I get SBA to cover my loan payments on my existing 7(a), 504, or microloan if I cannot pay due to COVID-19?</v>
       </c>
       <c r="B79" t="str">
-        <v>SBA has district offices in California that are open to answer questions. You can use the [SBA’s Local Assistance Directory](https://www.sba.gov/local-assistance) to locate the office nearest you. You can also contact the SBA by phone at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or by email at [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).  \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>SBA has a [Debt Relief program](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/sba-debt-relief) and will pay the principal and interest of existing SBA loans. Please contact your lender for information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C79" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2436,10 +2436,10 @@
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>How does a small business know which SBA loan or loan guarantee program is the right one? Can a small business apply to more than one?</v>
+        <v>If I need help to figure out which program is best for me or to submit an application, where can I find support?</v>
       </c>
       <c r="B80" t="str">
-        <v>Call or email the SBA to find out which program is right for you. While businesses can apply for and receive more than one form of capital assistance through the SBA, they cannot be used for the same purpose. The SBA can advise you on your options. Call [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or email [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>California’s network of small business support centers can help you figure out which loans and programs are best for your business, develop resiliency strategies, and find other resources. Go to California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) to find the closest center.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C80" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2462,10 +2462,10 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>How do I get SBA to cover my loan payments on my existing 7(a), 504, or microloan if I cannot pay due to COVID-19?</v>
+        <v>How do I maintain a safe workplace?</v>
       </c>
       <c r="B81" t="str">
-        <v>SBA has a [Debt Relief program](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/sba-debt-relief) and will pay the principal and interest of existing SBA loans. Please contact your lender for information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>As California reopens, every business will need to create a safer, low-risk environment. If you own or manage a business, follow the [industry-specific guidance](https://covid19.ca.gov/industry-guidance/) that applies to protect your workers and customers.\n\nIf your business is approved to reopen, you should take steps to ensure the safety and health of your workers. It’s important that employees with COVID-19 know they should stay home. Your sick leave policies need to support that. \n\n*   Encourage sick employees to stay home if they are sick. See government programs supporting [COVID-19 sick leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) and [workers’ compensation](https://www.labor.ca.gov/coronavirus2019/#chart).\n*   Establish routine cleaning throughout the workplace.\n*   Reduce travel. If possible, encourage video conferencing and limit larger gatherings.\n*   See [Cal/OSHA interim guidelines for general industry](https://www.dir.ca.gov/dosh/coronavirus/General-Industry.html).\n*   Follow [CDC guidance on keeping the workplace safe (PDF)](https://www.cdc.gov/coronavirus/2019-ncov/downloads/workplace-school-and-home-guidance.pdf).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C81" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2488,10 +2488,10 @@
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>If I need help to figure out which program is best for me or to submit an application, where can I find support?</v>
+        <v>Should a business owner notify customers if an employee has been exposed to COVID-19?</v>
       </c>
       <c r="B82" t="str">
-        <v>California’s network of small business support centers can help you figure out which loans and programs are best for your business, develop resiliency strategies, and find other resources. Go to California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) to find the closest center.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The business owner isn’t required to notify customers if an employee was exposed to COVID-19. The local health department will use contact tracing to notify those who were in close contact with the COVID-19 positive worker.\n\nWhen an employer discovers a worker who has tested positive or has symptoms of COVID-19, the employer should:\n\n*   make sure the worker does not remain at work, and\n*   work with the local health department to support isolation or quarantine, testing, and about when the worker may return to work. \n\nEmployers must follow the [Employer playbook](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf) which includes detailed information on:\n\n*   When and how an employer must report a COVID-19 positive employee.\n*   What is defined as an outbreak.\n*   Notifying all workers who may have been exposed to the worker with COVID-19. This is especially important for those with high-risk medical conditions (e.g., immune compromise or pregnancy).\n*   Guidance for employers who may be considering whether to suspend operations due to COVID-19 spread in the workplace.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C82" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2514,10 +2514,10 @@
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>How do I maintain a safe workplace?</v>
+        <v>What precautions should healthcare workers and organizations take?</v>
       </c>
       <c r="B83" t="str">
-        <v>As California reopens, every business will need to create a safer, low-risk environment. If you own or manage a business, follow the [industry-specific guidance](https://covid19.ca.gov/industry-guidance/) that applies to protect your workers and customers.\n\nIf your business is approved to reopen, you should take steps to ensure the safety and health of your workers. It’s important that employees with COVID-19 know they should stay home. Your sick leave policies need to support that. \n\n*   Encourage sick employees to stay home if they are sick. See government programs supporting [COVID-19 sick leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) and [workers’ compensation](https://www.labor.ca.gov/coronavirus2019/#chart).\n*   Establish routine cleaning throughout the workplace.\n*   Reduce travel. If possible, encourage video conferencing and limit larger gatherings.\n*   See [Cal/OSHA interim guidelines for general industry](https://www.dir.ca.gov/dosh/coronavirus/General-Industry.html).\n*   Follow [CDC guidance on keeping the workplace safe (PDF)](https://www.cdc.gov/coronavirus/2019-ncov/downloads/workplace-school-and-home-guidance.pdf).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>See [Cal/OSHA’s guidance on protecting workers from coronavirus](https://www.dir.ca.gov/dosh/coronavirus/Health-Care-General-Industry.html).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C83" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2540,10 +2540,10 @@
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>Should a business owner notify customers if an employee has been exposed to COVID-19?</v>
+        <v>How can I avoid laying off employees if my business is impacted by COVID-19?</v>
       </c>
       <c r="B84" t="str">
-        <v>The business owner isn’t required to notify customers if an employee was exposed to COVID-19. The local health department will use contact tracing to notify those who were in close contact with the COVID-19 positive worker.\n\nWhen an employer discovers a worker who has tested positive or has symptoms of COVID-19, the employer should:\n\n*   make sure the worker does not remain at work, and\n*   work with the local health department to support isolation or quarantine, testing, and about when the worker may return to work. \n\nEmployers must follow the [Employer playbook](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf) which includes detailed information on:\n\n*   When and how an employer must report a COVID-19 positive employee.\n*   What is defined as an outbreak.\n*   Notifying all workers who may have been exposed to the worker with COVID-19. This is especially important for those with high-risk medical conditions (e.g., immune compromise or pregnancy).\n*   Guidance for employers who may be considering whether to suspend operations due to COVID-19 spread in the workplace.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Apply for the [Unemployment Insurance (UI) Work Sharing Program](https://www.edd.ca.gov/Unemployment/Work_Sharing_Program.htm).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)&lt;!-- workshare, furlough, reduce hours --&gt;</v>
       </c>
       <c r="C84" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2566,13 +2566,13 @@
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>What precautions should healthcare workers and organizations take?</v>
+        <v>What action is the state taking to ensure all schools are providing meaningful instruction during the pandemic whether they are physically open or closed?</v>
       </c>
       <c r="B85" t="str">
-        <v>See [Cal/OSHA’s guidance on protecting workers from coronavirus](https://www.dir.ca.gov/dosh/coronavirus/Health-Care-General-Industry.html).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>*   California has made $5.3 billion in investments to support safe reopening and rigorous distance learning.\n*   Funds prioritize low-income students, English language learners, and special education students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C85" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D85" t="str">
         <v xml:space="preserve"> </v>
@@ -2592,13 +2592,13 @@
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>How can I avoid laying off employees if my business is impacted by COVID-19?</v>
+        <v>What determines whether schools are conducting in-person learning or distance learning?</v>
       </c>
       <c r="B86" t="str">
-        <v>Apply for the [Unemployment Insurance (UI) Work Sharing Program](https://www.edd.ca.gov/Unemployment/Work_Sharing_Program.htm).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)&lt;!-- workshare, furlough, reduce hours --&gt;</v>
+        <v>Using health data, schools can reopen for in-person instruction once their county has been in the Substantial (red) tier for at least two weeks. Schools must follow the **[Blueprint for a Safer Economy](https://covid19.ca.gov/safer-economy)** to reopen or if they have to close again.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C86" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D86" t="str">
         <v xml:space="preserve"> </v>
@@ -2618,10 +2618,10 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>What action is the state taking to ensure all schools are providing meaningful instruction during the pandemic whether they are physically open or closed?</v>
+        <v>What are the health and safety requirements for schools doing in-person learning?</v>
       </c>
       <c r="B87" t="str">
-        <v>*   California has made $5.3 billion in investments to support safe reopening and rigorous distance learning.\n*   Funds prioritize low-income students, English language learners, and special education students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>*   Everyone entering the school must do daily health checks.\n*   If someone experiences symptoms while at school, they will be sent home.\n*   Masks are required for all staff and students 3rd grade and above. Younger students should be encouraged to wear masks.\n*   Staff members must maintain 6ft distance from each other and students. Students should maintain 6ft distance as practicable.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C87" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2644,10 +2644,10 @@
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>What determines whether schools are conducting in-person learning or distance learning?</v>
+        <v>What happens if someone gets COVID-19 at my child’s school?</v>
       </c>
       <c r="B88" t="str">
-        <v>Using health data, schools can physically open when its county has been off the Monitoring List for 14 days and only if they follow strict health and safety requirements like masks and physical distancing. [Find the County Monitoring List here.](https://covid19.ca.gov/roadmap-counties/#track-data)\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>*   A classroom goes home when there is a confirmed case\n*   A school should switch to distance learning when there are multiple positive cases in multiple classroom cohorts\n*   A district should switch to distance learning if 25% of schools in the district are closed within a 14-day period\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C88" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2670,10 +2670,10 @@
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>What are the health and safety requirements for schools doing in-person learning?</v>
+        <v>If my child’s school is engaged in distance learning, what should I expect?</v>
       </c>
       <c r="B89" t="str">
-        <v>*   Everyone entering the school must do daily health checks.\n*   If someone experiences symptoms while at school, they will be sent home.\n*   Masks are required for all staff and students 3rd grade and above. Younger students should be encouraged to wear masks.\n*   Staff members must maintain 6ft distance from each other and students. Students should maintain 6ft distance as practicable.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>*   New statewide requirements include:\n    *   Access to devices and connectivity for all students\n    *   Daily live interaction with teachers and other students\n    *   Classes and assignments that are challenging and are equivalent to in-person instruction\n    *   Special requirements for English language learners and special education students\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C89" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2696,10 +2696,10 @@
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>What happens if someone gets COVID-19 at my child’s school?</v>
+        <v>My school provides free grab-and-go meals. Are those still available?</v>
       </c>
       <c r="B90" t="str">
-        <v>*   A classroom goes home when there is a confirmed case\n*   A school should switch to distance learning when there are multiple positive cases in multiple classroom cohorts\n*   A district should switch to distance learning if 25% of schools in the district are closed within a 14-day period\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>Yes. It is essential to keep children fed. Check with your local school district for days and times meals are offered.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C90" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2722,10 +2722,10 @@
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>If my child’s school is engaged in distance learning, what should I expect?</v>
+        <v>When can colleges or universities in counties resume indoor lectures?</v>
       </c>
       <c r="B91" t="str">
-        <v>*   New statewide requirements include:\n    *   Access to devices and connectivity for all students\n    *   Daily live interaction with teachers and other students\n    *   Classes and assignments that are challenging and are equivalent to in-person instruction\n    *   Special requirements for English language learners and special education students\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>Certain indoor operations in institutions of higher education must remain closed in counties in the Widespread (purple) tier. In other counties, those indoor operations can reopen consistent with the [Blueprint for a Safer Economy](https://covid19.ca.gov/safer-economy/) requirements for movie theaters and places of worship.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C91" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2748,10 +2748,10 @@
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>My school provides free grab-and-go meals. Are those still available?</v>
+        <v>Is there financial help for student loans?</v>
       </c>
       <c r="B92" t="str">
-        <v>Yes. It is essential to keep children fed. Check with your local school district for days and times meals are offered.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>The [governor has ordered](https://www.gov.ca.gov/2020/04/23/governor-newsom-announces-additional-relief-for-californians-impacted-by-covid-19/) relief for students with federal loans. Check with your lender to see what options are available for you.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C92" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2774,10 +2774,10 @@
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>Is there financial help for student loans?</v>
+        <v>What if I don’t have internet access at home?</v>
       </c>
       <c r="B93" t="str">
-        <v>The [governor has ordered](https://www.gov.ca.gov/2020/04/23/governor-newsom-announces-additional-relief-for-californians-impacted-by-covid-19/) relief for students with federal loans. Check with your lender to see what options are available for you.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>Check with your local school district or college to see what resources are available for you.  List of providers offering free internet access currently:\n\n[Spectrum mobile](https://mobile.spectrum.com/support/article/360040980371/coronavirus-covid19-update)  has opened wifi hotspots and are working on assisting school districts with facilitating home internet access. \n\n[Comcast](https://corporate.comcast.com/covid-19) has opened free Xfinity WiFi hotspot access across the country. Xfinity has also paused data plans, late fees, and disconnects for the next 60 days. Families with limited income can receive internet services for free for the next 60 days (usually $9.95 per month). \n\n[AT&amp;T](https://about.att.com/pages/COVID-19.html)  has opened all public WiFi hotspots and will not charge customers for any late fees or overages. AT&amp;T also offers internet access for [$10/month for households on limited income](https://www.att.com/shop/internet/access/index.html?source=ECmj0000000000mbU&amp;wtExtndSource=access#!/#%2F).\n\n[Low-cost Internet access plans](https://www.cde.ca.gov/ls/he/hn/availableinternetplans.asp) are also available.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C93" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2800,10 +2800,10 @@
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>What if I don’t have internet access at home?</v>
+        <v>How will students with disabilities receive services during school closures?</v>
       </c>
       <c r="B94" t="str">
-        <v>Check with your local school district or college to see what resources are available for you.  List of providers offering free internet access currently:\n\n[Spectrum mobile](https://mobile.spectrum.com/support/article/360040980371/coronavirus-covid19-update)  has opened wifi hotspots and are working on assisting school districts with facilitating home internet access. \n\n[Comcast](https://corporate.comcast.com/covid-19) has opened free Xfinity WiFi hotspot access across the country. Xfinity has also paused data plans, late fees, and disconnects for the next 60 days. Families with limited income can receive internet services for free for the next 60 days (usually $9.95 per month). \n\n[AT&amp;T](https://about.att.com/pages/COVID-19.html)  has opened all public WiFi hotspots and will not charge customers for any late fees or overages. AT&amp;T also offers internet access for [$10/month for households on limited income](https://www.att.com/shop/internet/access/index.html?source=ECmj0000000000mbU&amp;wtExtndSource=access#!/#%2F).\n\n[Low-cost Internet access plans](https://www.cde.ca.gov/ls/he/hn/availableinternetplans.asp) are also available.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>The Department of Education has released [guidance on distance learning](https://www.cde.ca.gov/ls/he/hn/distancelearning.asp) to support schools. This guidance includes recommendations to ensure equity and access for all students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C94" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2826,10 +2826,10 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>How will students with disabilities receive services during school closures?</v>
+        <v>Will there be standardized testing for students? When?</v>
       </c>
       <c r="B95" t="str">
-        <v>The Department of Education has released [guidance on distance learning](https://www.cde.ca.gov/ls/he/hn/distancelearning.asp) to support schools. This guidance includes recommendations to ensure equity and access for all students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>Probably not: on March 18, 2020, Governor Newsom issued an [executive order](https://www.gov.ca.gov/2020/03/18/governor-newsom-issues-executive-order-to-suspend-standardized-testing-for-students-in-response-to-covid-19-outbreak/)  to waive this year’s statewide testing for K-12 schools.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C95" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2852,13 +2852,13 @@
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>Will there be standardized testing? When?</v>
+        <v>Am I allowed to work during the outbreak?</v>
       </c>
       <c r="B96" t="str">
-        <v>Probably not: on March 18, 2020, Governor Newsom issued an [executive order](https://www.gov.ca.gov/2020/03/18/governor-newsom-issues-executive-order-to-suspend-standardized-testing-for-students-in-response-to-covid-19-outbreak/)  to waive this year’s statewide testing for K-12 schools.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>It depends what your job is. Any member of the [essential workforce](https://files.covid19.ca.gov/pdf/EssentialCriticalInfrastructureWorkers.pdf) is allowed to work during the [stay home order](https://covid19.ca.gov/stay-home-except-for-essential-needs/#top). And anyone is allowed to work from their home that has arranged to do so with their employer.\n\nFor information on businesses and industry sectors that are allowed to reopen, visit [industry guidance](https://covid19.ca.gov/industry-guidance/).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C96" t="str">
-        <v>https://covid19.ca.gov/education/</v>
+        <v>https://covid19.ca.gov/workers/</v>
       </c>
       <c r="D96" t="str">
         <v xml:space="preserve"> </v>
@@ -2878,10 +2878,10 @@
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>Am I allowed to work during the outbreak?</v>
+        <v>What can I do if my work hours are reduced or I am furloughed because of COVID-19?</v>
       </c>
       <c r="B97" t="str">
-        <v>It depends what your job is. Workers in [essential sectors (PDF)](https://files.covid19.ca.gov/pdf/EssentialCriticalInfrastructureWorkers.pdf) are allowed to work during the [stay home order](https://covid19.ca.gov/stay-home-except-for-essential-needs/#top). And anyone is allowed to work from their home that has arranged to do so with their employer.\n\nFor information on businesses and industry sectors that are allowed to reopen, visit [industry guidance](https://covid19.ca.gov/industry-guidance/).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C97" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2904,10 +2904,10 @@
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>What can I do if my work hours are reduced because of COVID-19?</v>
+        <v>Do I need a note or certificate from a medical provider to file for unemployment?</v>
       </c>
       <c r="B98" t="str">
-        <v>You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>No, a medical certificate is not required.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C98" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2930,10 +2930,10 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>Do I need a note or certificate from a medical provider to file for unemployment?</v>
+        <v>How long will it take to process a claim for unemployment or insurance benefits and to receive a payment?</v>
       </c>
       <c r="B99" t="str">
-        <v>No, a medical certificate is not required.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>After your claim is submitted, it will take at least three weeks to be processed. It may take longer if your information doesn’t match wage records or your identity can’t be verified. \n\nThe Governor has [waived the one-week waiting period](https://www.gov.ca.gov/2020/03/12/governor-newsom-issues-new-executive-order-further-enhancing-state-and-local-governments-ability-to-respond-to-covid-19-pandemic/). This means you can collect benefits for the first week that you were out of work or had reduced hours.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C99" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2956,10 +2956,10 @@
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>How long will it take to process a claim for unemployment or insurance benefits and to receive a payment?</v>
+        <v>Can I file a workplace safety complaint?</v>
       </c>
       <c r="B100" t="str">
-        <v>After your claim is submitted, it will take at least three weeks to be processed. It may take longer if your information doesn’t match wage records or your identity can’t be verified. \n\nThe Governor has [waived the one-week waiting period](https://www.gov.ca.gov/2020/03/12/governor-newsom-issues-new-executive-order-further-enhancing-state-and-local-governments-ability-to-respond-to-covid-19-pandemic/). This means you can collect benefits for the first week that you were out of work or had reduced hours.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>Yes, you have the right to file a complaint. Find [information and instructions](https://www.dir.ca.gov/dosh/complaint.htm) for how to file a complaint. If you submit a complaint, your name must be kept confidential by law.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C100" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2982,10 +2982,10 @@
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>Can I file a workplace safety complaint?</v>
+        <v>What can I do if I miss work because of school closures?</v>
       </c>
       <c r="B101" t="str">
-        <v>Yes, you have the right to file a complaint. Find [information and instructions](https://www.dir.ca.gov/dosh/complaint.htm) for how to file a complaint. If you submit a complaint, your name must be kept confidential by law.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>*   You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n*   You may be eligible for up to 80 hours of paid sick leave at two-thirds of your regular rate under the Families First Coronavirus Response Act ([FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-employee-paid-leave)) if your employer has less than 500 workers. You may also be eligible for up to 10 additional weeks of paid expanded family and medical leave at two-thirds of your regular rate. \n    *   Check [quick tips about FFCRA paid leave](https://www.dol.gov/sites/dolgov/files/WHD/Pandemic/Quick%20Tip%20Poster%20FFCRA.pdf) from the U.S. Department of Labor. \n    *   Use the [FFCRA tool](https://www.dol.gov/agencies/whd/ffcra/benefits-eligibility-webtool) to find out if you may be eligible. \n    *   See detailed information in the [questions and answers about FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-questions). \n*   Other options may be available. See the [chart of benefits for workers impacted by COVID-19](https://www.labor.ca.gov/coronavirus2019/#chart).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C101" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -3008,10 +3008,10 @@
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>What can I do if I miss work because of school closures?</v>
+        <v>What if I can’t work because I’m taking care of someone who’s sick or quarantined?</v>
       </c>
       <c r="B102" t="str">
-        <v>*   You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n*   Other options may be available. See [Benefits for Workers Impacted by COVID-19](https://www.labor.ca.gov/coronavirus2019/#chart).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>*   You may be eligible for up to 80 hours of paid expanded family and medical leave at two-thirds of your regular rate under the Families First Coronavirus Response Act ([FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-employee-paid-leave)) if your employer has less than 500 workers. \n    *   Check the [quick tips about FFCRA paid leave](https://www.dol.gov/sites/dolgov/files/WHD/Pandemic/Quick%20Tip%20Poster%20FFCRA.pdf) from the U.S. Department of Labor. \n    *   Use this [tool](https://www.dol.gov/agencies/whd/ffcra/benefits-eligibility-webtool) to see if you’re eligible for FFCRA paid expanded family and medical leave. \n    *   Find detailed information in the [questions and answers about FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-questions). \n*   You may use other [paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). See the [chart of paid sick and family leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) available under state and federal law. \n*   You can [file a Paid Family Leave (PFL) claim](https://www.edd.ca.gov/Disability/How_to_File_a_PFL_Claim_in_SDI_Online.htm). \n    *   See if you may be [eligible for paid family leave](https://edd.ca.gov/Disability/Am_I_Eligible_for_PFL_Benefits.htm). \n    *   Find details about the [paid family leave process](https://www.edd.ca.gov/Disability/PFL_Claim_Process.htm). \n    *   Check the [frequently asked questions](https://www.edd.ca.gov/Disability/FAQs.htm) about paid family leave. \n    *   See the [chart of paid family and sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) available under state and federal law. \n*   Unpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf) about employment and COVID-19.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C102" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -3034,10 +3034,10 @@
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>What if I can’t work because I’m taking care of someone who’s sick or quarantined?</v>
+        <v>What can I do if I can’t work because I’m sick or quarantined because of COVID-19?</v>
       </c>
       <c r="B103" t="str">
-        <v>*   You may use [paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). The Labor and Workforce Development Agency has created a [chart detailing the available paid sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law. \n*   You can [file a Paid Family Leave (PFL) claim](https://www.edd.ca.gov/Disability/How_to_File_a_PFL_Claim_in_SDI_Online.htm).\n*   Unpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>Extra federal, state, and in some cases, local sick leave are available if you are having COVID-19 symptoms, seeking a medical diagnosis, or are in quarantine. Check the side-by-side [comparison of COVID-19 paid leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) to learn what options may be available to you.\n\n*   You may be eligible for up to 80 hours of paid sick leave under the Families First Coronavirus Response Act ([FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-employee-paid-leave)) if your employer has less than 500 workers. \n    *   Check the [quick tips about FFCRA paid leave](https://www.dol.gov/sites/dolgov/files/WHD/Pandemic/Quick%20Tip%20Poster%20FFCRA.pdf) from the U.S. Department of Labor. \n    *   Use this [tool](https://www.dol.gov/agencies/whd/ffcra/benefits-eligibility-webtool) to see if you’re eligible for FFCRA paid sick leave. \n    *   Find detailed information in the [questions and answers about FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-questions).\n*   You may be eligible for up to 80 hours of California COVID-19 supplemental paid sick leave if you work for a business in the food sector with more than 500 workers. See [frequently asked questions](https://www.dir.ca.gov/dlse/FAQ-for-PSL.html) about supplemental paid sick leave for food sector workers.\n*   Some local areas have paid sick leave ordinances, such as San Jose, San Francisco, and Los Angeles. Check with the local labor law enforcement agency in your area.\n\nCheck the chart of all [benefits for workers impacted by COVID-19](https://www.labor.ca.gov/coronavirus2019/#chart) to learn about other resources that may be available.\n\n*   You may be able to use paid sick leave. See the [frequently asked questions about paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). \n*   You can [file a Disability Insurance (DI) claim](https://www.edd.ca.gov/Disability/How_to_File_a_DI_Claim_in_SDI_Online.htm) if you’re unable to work due to having or being exposed to COVID-19. \n    *   See if you may be [eligible for disability insurance benefits](https://edd.ca.gov/Disability/Am_I_Eligible_for_DI_Benefits.htm). \n    *   Check the [frequently asked questions](https://www.edd.ca.gov/Disability/FAQs.htm) about state disability insurance. \n*   You can file a [Workers’ Compensation claim](https://www.dir.ca.gov/dwc/FileAClaim.htm) if you suffered a COVID-19 illness that arose from an exposure during the course of your work. Find more information on [COVID-19 Resources and Workers’ Compensation](https://www.dir.ca.gov/dwc/Covid-19/Index.html).\n*   You may be able to use job-protected unpaid leave. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf) about employment and COVID-19.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C103" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -3060,10 +3060,10 @@
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>What can I do if I can’t work because I’m sick or quarantined because of COVID-19?</v>
+        <v>What if I don’t have any available sick leave to use?</v>
       </c>
       <c r="B104" t="str">
-        <v>*   You may be able to use [paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). The Labor and Workforce Development Agency has created a [chart detailing the available paid sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law.\n*   If you’re unable to work due to having or being exposed to COVID-19, you can [file a Disability Insurance (DI) claim](https://www.edd.ca.gov/Disability/How_to_File_a_DI_Claim_in_SDI_Online.htm).\n*   You may also file a [Workers’ Compensation Claim](https://www.dir.ca.gov/dwc/FileAClaim.htm) if you suffered a COVID-19 illness that arose from an exposure during the course of your work. Check the California Department of Industrial Relations’ [COVID-19 Resources and Workers’ Compensation](https://www.dir.ca.gov/dwc/Covid-19/Index.html) for more information.\n*   Unpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>Check the Labor and Workforce Development Agency’s [chart detailing the available sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law.\n\nUnpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C104" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -3086,10 +3086,10 @@
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>What if I don’t have any available sick leave to use?</v>
+        <v>When can I return to work once my isolation or quarantine is over?</v>
       </c>
       <c r="B105" t="str">
-        <v>Check the Labor and Workforce Development Agency’s [chart detailing the available sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law.\n\nUnpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>When you can return to work depends on your situation. \n\nIf you have symptoms, you should stay home until:\n\n*   at least 10 days have passed since symptoms started, AND\n*    your fever has been gone for 24 hours without the aid of medication, AND \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested.\n\nIf you have tested positive but have no symptoms, you should [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) at home for at least 10 days.\n\nIf you had close contact with someone who tested positive but you have tested negative, you should still [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) at home for at least 14 days.\n\nGet tested as soon as possible if you have symptoms or have come in contact with someone who has tested positive or has symptoms.\n\nRead more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C105" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -3112,7 +3112,7 @@
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>What effect will this have on my credit report?</v>
+        <v>What effect will late payments have on my credit report?</v>
       </c>
       <c r="B106" t="str">
         <v>Financial institutions will not report derogatory information (like late payments) to credit reporting agencies but may report a forbearance. Typically this does not negatively affect a credit score on its own.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
@@ -3138,7 +3138,7 @@
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>How long will these programs last?</v>
+        <v>How long will financial relief programs last?</v>
       </c>
       <c r="B107" t="str">
         <v>It is still unclear how severe or how long the COVID-19 impact will be. Financial institutions have committed to necessary relief and will be assessing the ongoing conditions and need for continuing relief.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
@@ -3164,7 +3164,7 @@
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>What if my financial institution isn’t offering this relief?</v>
+        <v>What if my financial institution isn’t offering payment relief?</v>
       </c>
       <c r="B108" t="str">
         <v>Call or check their website to be sure. At this time, JP Morgan Chase, US Bank, Wells Fargo and Citigroup, [and nearly 200 state-chartered banks](https://dbo.ca.gov/covid19-updates-fi/), credit unions are supporting these commitments. \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
@@ -3190,10 +3190,10 @@
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>What if I already made a payment or was hit with a fee because of COVID-19?</v>
+        <v>Is mortgage relief available to businesses?</v>
       </c>
       <c r="B109" t="str">
-        <v>Talk to your financial institution. These measures go into effect as of March 25, 2020.  \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>The relief is currently only available for residential mortgages.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C109" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -3216,10 +3216,10 @@
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>Is mortgage relief available to businesses?</v>
+        <v>What if my mortgage servicer is not communicative or cooperative?</v>
       </c>
       <c r="B110" t="str">
-        <v>The relief is currently only available for residential mortgages.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>You can file a complaint with the Department of Business Oversight:\n\n*   File on their [website](https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fdbo.ca.gov%2Ffile-a-complaint%2F&amp;data=02%7C01%7CManuel.Alvarez%40dbo.ca.gov%7Ce2673837ec6f42fce84508d7d114ed59%7Cd6910b1745b44b7bbb66cb7936fabafe%7C1%7C0%7C637207760136603083&amp;sdata=VR6CdqCvrBGkfC%2Bm%2B6Yj9emco9ldVY5BLWSiLpe3f4c%3D&amp;reserved=0)\n*    Call their Consumer Services Office at [(866) 275-2677](tel:(866) 275-2677) or [(916) 327-7585](tel:(916) 327-7585) \n*   Or email Ask.DBO@dbo.ca.gov\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C110" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -3242,10 +3242,10 @@
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>What if my mortgage servicer is not communicative or cooperative?</v>
+        <v>Can I get child care during the stay home order?</v>
       </c>
       <c r="B111" t="str">
-        <v>You can file a complaint with the Department of Business Oversight:\n\n*   File on their [website](https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fdbo.ca.gov%2Ffile-a-complaint%2F&amp;data=02%7C01%7CManuel.Alvarez%40dbo.ca.gov%7Ce2673837ec6f42fce84508d7d114ed59%7Cd6910b1745b44b7bbb66cb7936fabafe%7C1%7C0%7C637207760136603083&amp;sdata=VR6CdqCvrBGkfC%2Bm%2B6Yj9emco9ldVY5BLWSiLpe3f4c%3D&amp;reserved=0)\n*    Call their Consumer Services Office at [(866) 275-2677](tel:(866) 275-2677) or [(916) 327-7585](tel:(916) 327-7585) \n*   Or email Ask.DBO@dbo.ca.gov\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>Yes, all [childcare](https://covid19.ca.gov/childcare/) facilities can open with necessary modifications.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C111" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>Can I get child care during the stay home order?</v>
+        <v>I am homeless and I may have come in contact with coronavirus. How can I self-isolate with nowhere to go and services closing down?</v>
       </c>
       <c r="B112" t="str">
-        <v>[Child care options](https://covid19.ca.gov/childcare/) are available if you work at an [essential job](https://covid19.ca.gov/essential-workforce/) or a permitted job in the [current roadmap stage](https://covid19.ca.gov/roadmap/). If you are not working at a job like this, it is important to keep children at home. \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>A motel or hotel room may be available for you and your family. Contact your local homeless [continuum of care](https://www.bcsh.ca.gov/hcfc/documents/coc_poc.pdf) to connect you to this service.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C112" t="str">
-        <v>https://covid19.ca.gov/get-financial-help/</v>
+        <v>https://covid19.ca.gov/housing-and-homelessness/</v>
       </c>
       <c r="D112" t="str">
         <v xml:space="preserve"> </v>
@@ -3294,10 +3294,10 @@
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>I am homeless and I may have come in contact with coronavirus. How can I self-isolate with nowhere to go and services closing down?</v>
+        <v>Will there be a rent freeze or waiver for renters? Are evictions allowed during the stay at home order?</v>
       </c>
       <c r="B113" t="str">
-        <v>A motel or hotel room may be available for you and your family. Contact your local homeless [continuum of care](https://www.bcsh.ca.gov/hcfc/documents/coc_poc.pdf) to connect you to this service.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>There is an [order](https://www.gov.ca.gov/2020/06/30/governor-newsom-signs-executive-order-on-actions-in-response-to-covid-19-6-30-20/) in place to halt evictions and protect renters. If you are financially affected by COVID-19 and [can’t pay your full rent](https://bcsh.ca.gov/coronavirus19/graphic_rent.pdf), let your landlord know in writing within seven days of the rent due date. Save documentation as proof. The order does not relieve you from the obligation to pay rent. It also does not restrict the landlord from recovering rent that is due.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C113" t="str">
         <v>https://covid19.ca.gov/housing-and-homelessness/</v>
@@ -3320,10 +3320,10 @@
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>Will there be a rent freeze or waiver for renters? Are evictions allowed during the stay at home order?</v>
+        <v>Can landlords delay their payments while their tenants cannot pay rent?</v>
       </c>
       <c r="B114" t="str">
-        <v>There is an [order](https://www.gov.ca.gov/2020/06/30/governor-newsom-signs-executive-order-on-actions-in-response-to-covid-19-6-30-20/) in place to halt evictions and protect renters. If you are financially affected by COVID-19 and [can’t pay your full rent](https://bcsh.ca.gov/coronavirus19/graphic_rent.pdf), let your landlord know in writing within seven days of the rent due date. Save documentation as proof. The order does not relieve you from the obligation to pay rent. It also does not restrict the landlord from recovering rent that is due.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>Yes, there are protections in effect through September 30, 2020 for landlords. The [order](https://www.gov.ca.gov/2020/03/16/governor-newsom-issues-executive-order-to-protect-renters-and-homeowners-during-covid-19-pandemic/) requests lenders to halt foreclosures and related evictions during this time. Property owners should contact their financial institutions.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C114" t="str">
         <v>https://covid19.ca.gov/housing-and-homelessness/</v>
@@ -3346,10 +3346,10 @@
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>Can landlords delay their payments while their tenants cannot pay rent?</v>
+        <v>How do I get mortgage relief and/or forbearance?</v>
       </c>
       <c r="B115" t="str">
-        <v>Yes, there are protections in effect through September 30, 2020 for landlords. The [order](https://www.gov.ca.gov/2020/03/16/governor-newsom-issues-executive-order-to-protect-renters-and-homeowners-during-covid-19-pandemic/) requests lenders to halt foreclosures and related evictions during this time. Property owners should contact their financial institutions.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>You should contact and work directly with your mortgage servicer to learn about and apply for available relief. Please note that financial institutions and their servicers are experiencing high volumes of inquiries.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C115" t="str">
         <v>https://covid19.ca.gov/housing-and-homelessness/</v>
@@ -3372,10 +3372,10 @@
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>How do I get mortgage relief and/or forbearance?</v>
+        <v>How long will the forbearance last?</v>
       </c>
       <c r="B116" t="str">
-        <v>You should contact and work directly with your mortgage servicer to learn about and apply for available relief. Please note that financial institutions and their servicers are experiencing high volumes of inquiries.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>The terms of a forbearance will be agreed to between you and your mortgage service. Financial institutions will confirm approval of and terms of the forbearance program.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C116" t="str">
         <v>https://covid19.ca.gov/housing-and-homelessness/</v>
@@ -3398,13 +3398,13 @@
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>How long will the forbearance last?</v>
+        <v>What if a provider says they have availability on MyChildCare.ca.gov but when I connect with them they have no space?</v>
       </c>
       <c r="B117" t="str">
-        <v>The terms of a forbearance will be agreed to between you and your mortgage service. Financial institutions will confirm approval of and terms of the forbearance program.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>The information on [MyChildCare.ca.gov](http://mychildcare.ca.gov/) will be updated twice each week but it is possible that vacancies are filled between updates. Contact your [local childcare resource and referral agency](http://rrnetwork.org/family-services/find-child-care) to find more vacancies. \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
       </c>
       <c r="C117" t="str">
-        <v>https://covid19.ca.gov/housing-and-homelessness/</v>
+        <v>https://covid19.ca.gov/childcare/</v>
       </c>
       <c r="D117" t="str">
         <v xml:space="preserve"> </v>
@@ -3424,10 +3424,10 @@
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>What if a provider says they have availability on MyChildCare.ca.gov but when I connect with them they have no space?</v>
+        <v>How can I find out more about the provider listed in MyChildCare.ca.gov?</v>
       </c>
       <c r="B118" t="str">
-        <v>The information on [MyChildCare.ca.gov](http://mychildcare.ca.gov/) will be updated twice each week but it is possible that vacancies are filled between updates. Contact your [local childcare resource and referral agency](http://rrnetwork.org/family-services/find-child-care) to find more vacancies. \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
+        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) includes each provider’s facility/license number. This number can be searched at [CDSS Community Care Licensing Database](https://www.ccld.dss.ca.gov/carefacilitysearch/) to find more information about the provider, like information on inspections and complaints.  \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
       </c>
       <c r="C118" t="str">
         <v>https://covid19.ca.gov/childcare/</v>
@@ -3450,10 +3450,10 @@
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>How can I find out more about the provider listed in MyChildCare.ca.gov?</v>
+        <v>How can I find help paying for childcare?</v>
       </c>
       <c r="B119" t="str">
-        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) includes each provider’s facility/license number. This number can be searched at [CDSS Community Care Licensing Database](https://www.ccld.dss.ca.gov/carefacilitysearch/) to find more information about the provider, like information on inspections and complaints.  \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
+        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) provides information on all licensed center-based and family childcare homes. This includes both private-pay and subsidized childcare. Children of essential workers are now eligible to enroll in subsidized emergency childcare through June 30, 2020, or 60 calendar days after the date of the child’s enrollment, whichever is longer. This is subject to capacity and eligibility requirements. Your [local childcare resource and referral agency](https://rrnetwork.org/index.php?p=family-services/find-child-care) can answer more questions about childcare subsidies.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
       </c>
       <c r="C119" t="str">
         <v>https://covid19.ca.gov/childcare/</v>
@@ -3476,10 +3476,10 @@
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>How can I find help paying for childcare?</v>
+        <v>Can I get childcare during the stay home order?</v>
       </c>
       <c r="B120" t="str">
-        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) provides information on all licensed center-based and family childcare homes. This includes both private-pay and subsidized childcare. Children of essential workers are now eligible to enroll in subsidized emergency childcare through June 30, 2020, or 60 calendar days after the date of the child’s enrollment, whichever is longer. This is subject to capacity and eligibility requirements. Your [local childcare resource and referral agency](https://rrnetwork.org/index.php?p=family-services/find-child-care) can answer more questions about childcare subsidies.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
+        <v>Yes, all childcare facilities can open with necessary modifications.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
       </c>
       <c r="C120" t="str">
         <v>https://covid19.ca.gov/childcare/</v>
@@ -3502,10 +3502,10 @@
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>Can I get childcare during the stay home order?</v>
+        <v>Can my babysitter still come to the house?</v>
       </c>
       <c r="B121" t="str">
-        <v>Yes, all childcare facilities can open with necessary modifications.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
+        <v>Yes, a childcare worker can come to your home if necessary and should practice basic prevention guidelines (like handwashing for at least 20 seconds, physical distancing, and staying home if feeling ill).\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
       </c>
       <c r="C121" t="str">
         <v>https://covid19.ca.gov/childcare/</v>
@@ -3528,13 +3528,13 @@
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>Can my babysitter still come to the house?</v>
+        <v>Fin your county websites</v>
       </c>
       <c r="B122" t="str">
-        <v>Yes, a childcare worker can come to your home if necessary and should practice basic prevention guidelines (like handwashing for at least 20 seconds, physical distancing, and staying home if feeling ill).\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
+        <v>*   [Alameda County](http://www.acphd.org/2019-ncov.aspx)\n*   [Alpine County](http://alpinecountyca.gov/Index.aspx?NID=516)\n*   [Amador County](https://www.amadorgov.org/services/covid-19)\n*   [Butte County](https://www.buttecounty.net/publichealth)\n*   [Calaveras County](https://covid19.calaverasgov.us/)\n*   [Colusa County](https://www.countyofcolusa.org/99/Public-Health)\n*   [Contra Costa County](https://www.coronavirus.cchealth.org/)\n*   [Del Norte County](http://www.co.del-norte.ca.us/departments/health-human-services/public-health)\n*   [El Dorado County](https://www.edcgov.us/Government/hhsa/Pages/EDCCOVID-19.aspx)\n*   [Fresno County](https://www.co.fresno.ca.us/departments/public-health/covid-19)\n*   [Glenn County](https://www.countyofglenn.net/dept/health-human-services/public-health/covid-19)\n*   [Humboldt County](https://humboldtgov.org/2018/Humboldt-Health-Alert)\n*   [Imperial County](http://www.icphd.org/health-information-and-resources/healthy-facts/covid-19/)\n*   [Inyo County](https://www.inyocounty.us/coronavirus-covid-19-response)\n*   [Kern County](https://kernpublichealth.com/2019-novel-coronavirus/)\n*   [Kings County](https://www.countyofkings.com/departments/health-welfare/public-health/coronavirus-disease-2019-covid-19/-fsiteid-1)\n*   [Lake County](http://health.co.lake.ca.us/Coronavirus.htm)\n*   [Lassen County](http://www.co.lassen.ca.us/)\n*   [Los Angeles County](http://publichealth.lacounty.gov/media/Coronavirus/)\n*   [Madera County](https://www.maderacounty.com/government/public-health/health-updates/corona-virus)\n*   [Marin County](https://coronavirus.marinhhs.org/)\n*   [Mariposa County](http://www.mariposacounty.org/1592/COVID-19-Information)\n*   [Mendocino County](https://www.mendocinocounty.org/community/novel-coronavirus)\n*   [Merced County](https://www.co.merced.ca.us/3350/Coronavirus-Disease-2019)\n*   [Modoc County](http://www.co.modoc.ca.us/)\n*   [Mono County](https://coronavirus.monocounty.ca.gov/)\n*   [Monterey County](https://www.co.monterey.ca.us/government/departments-a-h/health/diseases/2019-novel-coronavirus-covid-19)\n*   [Napa County](https://www.countyofnapa.org/2739/Coronavirus)\n*   [Nevada County](https://www.mynevadacounty.com/2924/Coronavirus)\n*   [Orange County](https://www.ochealthinfo.com/phs/about/epidasmt/epi/dip/prevention/novel_coronavirus)\n*   [Placer County](https://www.placer.ca.gov/coronavirus)\n*   [Plumas County](https://www.plumascounty.us/2669/Novel-Coronavirus-2019-COVID-19)\n*   [Riverside County](https://www.rivcoph.org/coronavirus)\n*   [Sacramento County](https://dhs.saccounty.net/PUB/Pages/PUB-Home.aspx)\n*   [San Benito County](https://hhsa.cosb.us/publichealth/communicable-disease/coronavirus/)\n*   [San Bernardino County](http://wp.sbcounty.gov/dph/coronavirus/)\n*   [San Diego County](https://www.sandiegocounty.gov/coronavirus.html)\n*   [San Francisco City and County](https://sf.gov/topics/coronavirus-covid-19)\n*   [San Joaquin County](https://www.sjgov.org/covid19/)\n*   [San Luis Obispo County](https://www.emergencyslo.org/en/covid19.aspx)\n*   [San Mateo County](https://www.smchealth.org/coronavirus)\n*   [Santa Barbara County](https://publichealthsbc.org/)\n*   [Santa Clara County](https://www.sccgov.org/sites/phd/DiseaseInformation/novel-coronavirus/Pages/home.aspx)\n*   [Santa Cruz County](https://www.santacruzhealth.org/HSAHome/HSADivisions/PublicHealth/CommunicableDiseaseControl/Coronavirus.aspx)\n*   [Shasta County](https://www.co.shasta.ca.us/index/hhsa/health-safety/current-heath-concerns/coronavirus)\n*   [Sierra County](http://sierracounty.ca.gov/582/Coronavirus-COVID-19)\n*   [Siskiyou County](https://www.co.siskiyou.ca.us/publichealth/page/covid-19-what-siskiyou-county-residents-need-know-now)\n*   [Solano County](http://www.solanocounty.com/depts/ph/ncov.asp)\n*   [Sonoma County](https://socoemergency.org/emergency/novel-coronavirus/)\n*   [Stanislaus County](http://schsa.org/publichealth/pages/corona-virus/)\n*   [Sutter County](https://www.suttercounty.org/doc/government/depts/cao/em/coronavirus)\n*   [Tehama County](https://www.tehamacohealthservices.net/services/communicable-diseases/#current-events)\n*   [Trinity County](https://www.trinitycounty.org/)\n*   [Tulare County](https://tchhsa.org/eng/index.cfm/public-health/covid-19-updates-novel-coronavirus/)\n*   [Tuolumne County](https://www.tuolumnecounty.ca.gov/250/Public-Health)\n*   [Ventura County](https://www.vcemergency.com/)\n*   [Yolo County](https://www.yolocounty.org/health-human-services/adults/communicable-disease-investigation-and-control/novel-coronavirus-2019)\n*   [Yuba County](https://www.yuba.org/coronavirus/)\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C122" t="str">
-        <v>https://covid19.ca.gov/childcare/</v>
+        <v>https://covid19.ca.gov/state-local-resources/</v>
       </c>
       <c r="D122" t="str">
         <v xml:space="preserve"> </v>
@@ -3554,10 +3554,10 @@
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>County websites:</v>
+        <v>What are the restrictions in my area?</v>
       </c>
       <c r="B123" t="str">
-        <v>*   [Alameda County](http://www.acphd.org/2019-ncov.aspx)\n*   [Alpine County](http://alpinecountyca.gov/Index.aspx?NID=516)\n*   [Amador County](https://www.amadorgov.org/services/covid-19)\n*   [Butte County](https://www.buttecounty.net/publichealth)\n*   [Calaveras County](https://covid19.calaverasgov.us/)\n*   [Colusa County](https://www.countyofcolusa.org/99/Public-Health)\n*   [Contra Costa County](https://www.coronavirus.cchealth.org/)\n*   [Del Norte County](http://www.co.del-norte.ca.us/departments/health-human-services/public-health)\n*   [El Dorado County](https://www.edcgov.us/Government/hhsa/Pages/EDCCOVID-19.aspx)\n*   [Fresno County](https://www.co.fresno.ca.us/departments/public-health/covid-19)\n*   [Glenn County](https://www.countyofglenn.net/dept/health-human-services/public-health/covid-19)\n*   [Humboldt County](https://humboldtgov.org/2018/Humboldt-Health-Alert)\n*   [Imperial County](http://www.icphd.org/health-information-and-resources/healthy-facts/covid-19/)\n*   [Inyo County](https://www.inyocounty.us/coronavirus-covid-19-response)\n*   [Kern County](https://kernpublichealth.com/2019-novel-coronavirus/)\n*   [Kings County](https://www.countyofkings.com/departments/health-welfare/public-health/coronavirus-disease-2019-covid-19/-fsiteid-1)\n*   [Lake County](http://health.co.lake.ca.us/Coronavirus.htm)\n*   [Lassen County](http://www.co.lassen.ca.us/)\n*   [Los Angeles County](http://publichealth.lacounty.gov/media/Coronavirus/)\n*   [Madera County](https://www.maderacounty.com/government/public-health/health-updates/corona-virus)\n*   [Marin County](https://coronavirus.marinhhs.org/)\n*   [Mariposa County](http://www.mariposacounty.org/1592/COVID-19-Information)\n*   [Mendocino County](https://www.mendocinocounty.org/community/novel-coronavirus)\n*   [Merced County](https://www.co.merced.ca.us/3350/Coronavirus-Disease-2019)\n*   [Modoc County](http://www.co.modoc.ca.us/)\n*   [Mono County](https://coronavirus.monocounty.ca.gov/)\n*   [Monterey County](https://www.co.monterey.ca.us/government/departments-a-h/health/diseases/2019-novel-coronavirus-covid-19)\n*   [Napa County](https://www.countyofnapa.org/2739/Coronavirus)\n*   [Nevada County](https://www.mynevadacounty.com/2924/Coronavirus)\n*   [Orange County](https://www.ochealthinfo.com/phs/about/epidasmt/epi/dip/prevention/novel_coronavirus)\n*   [Placer County](https://www.placer.ca.gov/coronavirus)\n*   [Plumas County](https://www.plumascounty.us/2669/Novel-Coronavirus-2019-COVID-19)\n*   [Riverside County](https://www.rivcoph.org/coronavirus)\n*   [Sacramento County](https://dhs.saccounty.net/PUB/Pages/PUB-Home.aspx)\n*   [San Benito County](https://hhsa.cosb.us/publichealth/communicable-disease/coronavirus/)\n*   [San Bernardino County](http://wp.sbcounty.gov/dph/coronavirus/)\n*   [San Diego County](https://www.sandiegocounty.gov/coronavirus.html)\n*   [San Francisco City and County](https://sf.gov/topics/coronavirus-covid-19)\n*   [San Joaquin County](https://www.sjgov.org/covid19/)\n*   [San Luis Obispo County](https://www.emergencyslo.org/en/covid19.aspx)\n*   [San Mateo County](https://www.smchealth.org/coronavirus)\n*   [Santa Barbara County](https://publichealthsbc.org/)\n*   [Santa Clara County](https://www.sccgov.org/sites/phd/DiseaseInformation/novel-coronavirus/Pages/home.aspx)\n*   [Santa Cruz County](https://www.santacruzhealth.org/HSAHome/HSADivisions/PublicHealth/CommunicableDiseaseControl/Coronavirus.aspx)\n*   [Shasta County](https://www.co.shasta.ca.us/index/hhsa/health-safety/current-heath-concerns/coronavirus)\n*   [Sierra County](http://sierracounty.ca.gov/582/Coronavirus-COVID-19)\n*   [Siskiyou County](https://www.co.siskiyou.ca.us/publichealth/page/covid-19-what-siskiyou-county-residents-need-know-now)\n*   [Solano County](http://www.solanocounty.com/depts/ph/ncov.asp)\n*   [Sonoma County](https://socoemergency.org/emergency/novel-coronavirus/)\n*   [Stanislaus County](http://schsa.org/publichealth/pages/corona-virus/)\n*   [Sutter County](https://www.suttercounty.org/doc/government/depts/cao/em/coronavirus)\n*   [Tehama County](https://www.tehamacohealthservices.net/services/communicable-diseases/#current-events)\n*   [Trinity County](https://www.trinitycounty.org/)\n*   [Tulare County](https://tchhsa.org/eng/index.cfm/public-health/covid-19-updates-novel-coronavirus/)\n*   [Tuolumne County](https://www.tuolumnecounty.ca.gov/250/Public-Health)\n*   [Ventura County](https://www.vcemergency.com/)\n*   [Yolo County](https://www.yolocounty.org/health-human-services/adults/communicable-disease-investigation-and-control/novel-coronavirus-2019)\n*   [Yuba County](https://www.yuba.org/coronavirus/)\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>While each county may have different restrictions, it is important to stay home as much as possible. If you do go out, stay 6 feet away from others who are not in your household and wear a mask or face covering. Your actions save lives.\n\nSee what [industries are open or closed](https://covid19.ca.gov/safer-economy) in your county.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C123" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3580,10 +3580,10 @@
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>What are the restrictions in my area?</v>
+        <v>How are we helping the homeless?</v>
       </c>
       <c r="B124" t="str">
-        <v>While each county may have different restrictions, it is important to stay home as much as possible. If you do go out, stay 6 feet away from others who are not in your household and wear a mask or face covering. Your actions save lives.\n\nSee what [industries are open or closed](https://covid19.ca.gov/roadmap-counties/#track-data) in your county.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>Each county and local government in California has [increased resources](https://covid19.ca.gov/housing-and-homelessness/#top) to protect people experiencing homelessness during COVID-19. [Financial protections](https://covid19.ca.gov/housing-and-homelessness/#top) were added to prevent others from losing their homes during the outbreak.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C124" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3606,10 +3606,10 @@
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v>How are we helping the homeless?</v>
+        <v>How is the state protecting incarcerated people in California?</v>
       </c>
       <c r="B125" t="str">
-        <v>Each county and local government in California has [increased resources](https://covid19.ca.gov/housing-and-homelessness/#top) to protect people experiencing homelessness during COVID-19. [Financial protections](https://covid19.ca.gov/housing-and-homelessness/#top) were added to prevent others from losing their homes during the outbreak.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>[California Department of Corrections and Rehabilitation (CDCR)](https://www.cdcr.ca.gov/covid19/) is dedicated to the safety of everyone who lives in, works in, and visits state prisons. CDCR has given all staff and inmates 2 reusable cloth masks to wear while moving between cells, dorms, meetings with others, or health care appointments. CDCR also requires ongoing testing for all staff working in adult institutions, suspended non-essential transfer of inmates, and suspended volunteer services and in-person visiting.\n\nSee [CDCR’s COVID-19 Response Efforts](https://www.cdcr.ca.gov/covid19/covid-19-response-efforts/) for more detailed information.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C125" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3632,10 +3632,10 @@
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v>How is the state protecting incarcerated people in California?</v>
+        <v>Who can I contact about my child custody order and child visitation rights?</v>
       </c>
       <c r="B126" t="str">
-        <v>[California Department of Corrections and Rehabilitation (CDCR)](https://www.cdcr.ca.gov/covid19/) is dedicated to the safety of everyone who lives in, works in, and visits state prisons. CDCR has given all staff and inmates 2 reusable cloth masks to wear while moving between cells, dorms, meetings with others, or health care appointments. CDCR also requires ongoing testing for all staff working in adult institutions, suspended non-essential transfer of inmates, and suspended volunteer services and in-person visiting.\n\nSee [CDCR’s COVID-19 Response Efforts](https://www.cdcr.ca.gov/covid19/covid-19-response-efforts/) for more detailed information.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>Court operations vary from county to county. You can use the [California Courts Self-Help Center](https://www.courts.ca.gov/selfhelp.htm) or reach out to your [local government office](https://www.courts.ca.gov/find-my-court.htm?query=browse_courts) for more information. \n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C126" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3658,10 +3658,10 @@
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v>Who can I contact about my child custody order and child visitation rights?</v>
+        <v>Do I have to report to jury duty if summoned?</v>
       </c>
       <c r="B127" t="str">
-        <v>Court operations vary from county to county. You can use the [California Courts Self-Help Center](https://www.courts.ca.gov/selfhelp.htm) or reach out to your [local government office](https://www.courts.ca.gov/find-my-court.htm?query=browse_courts) for more information. \n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>Court operations vary from county to county. You can use the [California Courts Self-Help Center](https://www.courts.ca.gov/selfhelp.htm) or reach out to your [local government office](https://www.courts.ca.gov/find-my-court.htm?query=browse_courts) for more information about jury duty.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)&lt;!-- jury duty, summons, courts, court, court operations--&gt;</v>
       </c>
       <c r="C127" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3684,13 +3684,13 @@
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v>Do I have to report to jury duty if summoned?</v>
+        <v>I am an immigrant Californian. Are there organizations that can help me?</v>
       </c>
       <c r="B128" t="str">
-        <v>Court operations vary from county to county. You can use the [California Courts Self-Help Center](https://www.courts.ca.gov/selfhelp.htm) or reach out to your [local government office](https://www.courts.ca.gov/find-my-court.htm?query=browse_courts) for more information about jury duty.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)&lt;!-- jury duty, summons, courts, court, court operations--&gt;</v>
+        <v>Yes. The California Immigrant Resilience Fund is raising $50 million to provide cash assistance to undocumented Californians who are ineligible for other COVID-19 programs. Visit the [California Immigrant Resilience Fund](http://www.immigrantfundca.org) website to see if you can benefit from this program.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C128" t="str">
-        <v>https://covid19.ca.gov/state-local-resources/</v>
+        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
       </c>
       <c r="D128" t="str">
         <v xml:space="preserve"> </v>
@@ -3710,10 +3710,10 @@
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v>When is the disaster relief assistance available?</v>
+        <v>What other government programs are immigrants eligible for during the COVID-19 pandemic?</v>
       </c>
       <c r="B129" t="str">
-        <v>Individuals may begin applying on May 18, 2020. Assistance will be available until the funding is spent or until June 30, 2020, at the latest. Applicants will be considered on a first-come, first-served basis. Applicants may only apply with the nonprofit organization(s) in their county of residency.\n\n**Please note:**\n\n*   Funding is limited, and disaster relief application services and assistance are not guaranteed.\n*   Nonprofit organizations will not be assisting individuals before May 18. Individuals should not contact them ahead of time regarding disaster relief assistance.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>Check the [Guide for Immigrant Californians (PDF)](/wp-content/uploads/2020/04/LISTOS_COVID_19_immigrant_guidance_EN_dAf.pdf). It has information about jobs, wages, benefits, and small business and housing support.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C129" t="str">
         <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
@@ -3736,13 +3736,13 @@
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v>Who is eligible for this disaster relief assistance?</v>
+        <v>Youth and Teens</v>
       </c>
       <c r="B130" t="str">
-        <v>Eligible individuals must be able to provide information that they:\n\n*   Are an undocumented adult (person over the age of 18)\n*   Are not eligible for federal COVID-19 assistance, like the CARES Act stimulus payments or pandemic unemployment benefits, and\n*   Have experienced hardship as a result of COVID-19.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>*   [California Youth Crisis Line](https://calyouth.org/cycl/)**:** Youth ages 12-24 can call or text [800-843-5200](tel:800-843-5200) or [chat online](https://m2.icarol.com/ConsumerRegistration.aspx?org=53141&amp;pid=326&amp;cc=en-US) for 24/7 crisis support.\n*   [TEEN LINE](https://teenlineonline.org/talk-now/): Teens can talk to another teen by texting “TEEN” to [839863](sms:839863) from 6pm – 9pm, or call [800-852-8336](tel:800-852-8336) from 6pm – 10pm.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C130" t="str">
-        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
+        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
       </c>
       <c r="D130" t="str">
         <v xml:space="preserve"> </v>
@@ -3762,13 +3762,13 @@
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v>Can getting this assistance affect my ability to get a green card or to become a U.S. Citizen? Will receiving it make me a public charge?</v>
+        <v>Veterans</v>
       </c>
       <c r="B131" t="str">
-        <v>This disaster relief assistance is not means-tested and is one-time assistance. The federal government does not list this assistance as a public benefit for a public charge consideration. However, USCIS has not issued specific guidance related to this assistance.\n\nIf you have questions about your immigration status and this program, please consult an attorney. A list of free and low-cost immigration services providers is available in the [Guide for Immigrant Californians (PDF)](https://files.covid19.ca.gov/pdf/COVID_immigrant_guidance--en.pdf).\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>[Veterans Crisis Line](https://www.veteranscrisisline.net): Call [800-273-8255](tel:800-273-8255) and Press 1 or text [838255](sms:838255) for 24/7 support.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C131" t="str">
-        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
+        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
       </c>
       <c r="D131" t="str">
         <v xml:space="preserve"> </v>
@@ -3788,13 +3788,13 @@
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v>Is the personal information I provide to the nonprofits protected?</v>
+        <v>First Responders and Law Enforcement</v>
       </c>
       <c r="B132" t="str">
-        <v>Your information is only used to confirm eligibility and provide the assistance. No personal information (like name or address) will be given to any government agency. Only general information like age, gender, and preferred language will be shared with the State of California.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>*   [Fire/EMS helpline](https://www.nvfc.org/fireems-helpline/): Call [888-731-FIRE](tel:888-731-FIRE) to get 24/7 help for a variety of behavioral health issues.\n*   [COPLINE](https://www.copline.org/): Call [800-267-5463](tel:800-267-5463) to find support 24/7 for law enforcement officers.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C132" t="str">
-        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
+        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
       </c>
       <c r="D132" t="str">
         <v xml:space="preserve"> </v>
@@ -3814,13 +3814,13 @@
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v>How do I apply?</v>
+        <v>Older Californians</v>
       </c>
       <c r="B133" t="str">
-        <v>The California Department of Social Services (CDSS) has identified non-profit where you can apply for disaster assistance. Find the [nonprofit where you can apply in your area](https://cdss.ca.gov/inforesources/immigration/covid-19-drai).\n\nApply no sooner than May 18, and only to the organization in your area. They will assist you with applying, confirm your eligibility, and deliver a payment card if you are approved. Applications will be considered on a first-come, first-served basis.\n\nFunding is limited, and disaster relief application services and assistance are not guaranteed.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>*   [Friendship Line](https://www.ioaging.org/services/all-inclusive-health-care/friendship-line): Call [888-670-1360](tel:888-670-1360) for 24/7 support if you are 60 years or older, or an adult living with disabilities.  \n*   California Aging and Adult Information Line: Call [800-510-2020](tel:800-510-2020) for help finding local assistance. \n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C133" t="str">
-        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
+        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
       </c>
       <c r="D133" t="str">
         <v xml:space="preserve"> </v>
@@ -3840,13 +3840,13 @@
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v>How many people in a household can receive this assistance?</v>
+        <v>Deaf and Hard of Hearing Individuals</v>
       </c>
       <c r="B134" t="str">
-        <v>A maximum of two adults per household can qualify for this assistance, for a total of $1,000 per household. A household is defined as individuals who live, shop, and prepare meals together.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>[National Suicide Prevention Deaf and Hard of Hearing Hotline](https://suicidepreventionlifeline.org/help-yourself/for-deaf-hard-of-hearing/): Access 24/7 video relay service by dialing [800-273-8255](tel:800-273-8255) (TTY [800-799-4889](tel:800-799-4889)).\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C134" t="str">
-        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
+        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
       </c>
       <c r="D134" t="str">
         <v xml:space="preserve"> </v>
@@ -3866,13 +3866,13 @@
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v>How do eligible individuals receive this assistance?</v>
+        <v>Services for Substance Use Disorders</v>
       </c>
       <c r="B135" t="str">
-        <v>You will get a payment card either in person or through the mail. The organization in your area can give you more information.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>*   [SAMHSA National Helpline](https://www.samhsa.gov/find-help/national-helpline): Call [800-662-HELP](tel:1-800-662-4357) for 24/7 information and referrals in English and Spanish. \n*   [SAMHSA Treatment Locator](https://findtreatment.samhsa.gov)**:**  Find drug or alcohol treatment programs. \n*   [Local county access lines](https://gcc01.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.dhcs.ca.gov%2Findividuals%2FPages%2FSUD_County_Access_Lines.aspx&amp;data=02%7C01%7CJanne.Olson-Morgan%40osg.ca.gov%7C122307be91754d12e5dc08d7d984f958%7C265c2dcd2a6e43aab2e826421a8c8526%7C0%7C0%7C637217037446186621&amp;sdata=5sx4UdIlVkRL%2BEJR7FrpK0gYAn20yE71TyBDFIw1kJM%3D&amp;reserved=0): Find your local number for help seeking substance use disorder services.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C135" t="str">
-        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
+        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
       </c>
       <c r="D135" t="str">
         <v xml:space="preserve"> </v>
@@ -3892,13 +3892,13 @@
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v>How long do I have to apply?</v>
+        <v>LGBTQ Individuals</v>
       </c>
       <c r="B136" t="str">
-        <v>Payments will be distributed beginning on May 18, 2020. They will continue until the $75 million in funding is spent, or until June 30, 2020 at the latest. We expect that this disaster relief assistance will run out very quickly. Apply as soon as you can, but not before May 18.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>*   [Trevor Project](https://www.thetrevorproject.org): Call [866-488-7386](tel:866-488-7386) or text START to [678678](sms:678678) for 24/7 information and suicide prevention resources for LGBTQ youth.\n*   [Lesbian, Gay, Bisexual and Transgender National Hotline](https://www.glbthotline.org/hotline.html): Call [800-273-8255](tel:800-273-8255) from 1pm – 9pm for support, information or help finding resources.\n*   [Victims of Crime Resource Center](https://1800victims.org/): Call or text [800-842-8467](tel:800-842-8467) or [chat online](https://1800victims.org/) for information about LGTBQ rights, legal protections, and local resources.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C136" t="str">
-        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
+        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
       </c>
       <c r="D136" t="str">
         <v xml:space="preserve"> </v>
@@ -3918,13 +3918,13 @@
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v>If I am unable to apply for this program, are there other organizations that can help me?</v>
+        <v>What is a close contact?</v>
       </c>
       <c r="B137" t="str">
-        <v>Yes. The California Immigrant Resilience Fund is raising $50 million to provide cash assistance to undocumented Californians who are ineligible for other COVID-19 programs. Visit the [California Immigrant Resilience Fund](http://www.immigrantfundca.org) website to see if you can benefit from this program.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>A [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) is someone who was within 6 feet of a person with COVID-19 for at least 15 minutes starting from 2 days before symptoms appeared (or, for asymptomatic patients, 2 days prior to their test) until the time the patient is isolated. This usually includes household members, intimate contacts, and caregivers, but can include others.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C137" t="str">
-        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D137" t="str">
         <v xml:space="preserve"> </v>
@@ -3944,13 +3944,13 @@
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v>What other government programs may I be eligible for during the COVID-19 pandemic?</v>
+        <v>Will contact tracers track my location?</v>
       </c>
       <c r="B138" t="str">
-        <v>Check the [Guide for Immigrant Californians (PDF)](/wp-content/uploads/2020/04/LISTOS_COVID_19_immigrant_guidance_EN_dAf.pdf). It has information about jobs, wages, benefits, and small business and housing support.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>California’s contact tracing program does not use any cell phone tracking technology. Someone from your local public health department will simply speak privately with you. All information is confidential and protected by California’s strict privacy laws. They may stay in touch to make sure your symptoms aren’t worsening.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C138" t="str">
-        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D138" t="str">
         <v xml:space="preserve"> </v>
@@ -3970,13 +3970,13 @@
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>Youth and Teens</v>
+        <v>Is contact tracing help available in my language?</v>
       </c>
       <c r="B139" t="str">
-        <v>*   [California Youth Crisis Line](https://calyouth.org/cycl/)**:** Youth ages 12-24 can call or text [800-843-5200](tel:800-843-5200) or [chat online](https://m2.icarol.com/ConsumerRegistration.aspx?org=53141&amp;pid=326&amp;cc=en-US) for 24/7 crisis support.\n*   [TEEN LINE](https://teenlineonline.org/talk-now/): Teens can talk to another teen by texting “TEEN” to [839863](sms:839863) from 6pm – 9pm, or call [800-852-8336](tel:800-852-8336) from 6pm – 10pm.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>Your [local health department](https://covid19.ca.gov/get-local-information/) can communicate with you in many different languages.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C139" t="str">
-        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D139" t="str">
         <v xml:space="preserve"> </v>
@@ -3996,13 +3996,13 @@
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>Veterans</v>
+        <v>Who should get tested for coronavirus?</v>
       </c>
       <c r="B140" t="str">
-        <v>[Veterans Crisis Line](https://www.veteranscrisisline.net): Call [800-273-8255](tel:800-273-8255) and Press 1 or text [838255](sms:838255) for 24/7 support.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>You should get tested if you:\n\n*   Had [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) with anyone who has tested positive for COVID-19\n*   Have COVID-19 symptoms\n*   Get a call from a contact tracer\n*   Are at [high risk](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Updated-COVID-19-Testing-Guidance.aspx)\n\nFind a [testing site in your area](https://covid19.ca.gov/testing-and-treatment/).\n\nIf you think you may have been exposed, call your doctor.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C140" t="str">
-        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D140" t="str">
         <v xml:space="preserve"> </v>
@@ -4022,13 +4022,13 @@
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>First Responders and Law Enforcement</v>
+        <v>How do I find a coronavirus testing location?</v>
       </c>
       <c r="B141" t="str">
-        <v>*   [Fire/EMS helpline](https://www.nvfc.org/fireems-helpline/): Call [888-731-FIRE](tel:888-731-FIRE) to get 24/7 help for a variety of behavioral health issues.\n*   [COPLINE](https://www.copline.org/): Call [800-267-5463](tel:800-267-5463) to find support 24/7 for law enforcement officers.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>To learn more about testing and care, visit the [Testing and treatment page](https://covid19.ca.gov/testing-and-treatment/). You can search for testing locations there using your zip code. \n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C141" t="str">
-        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D141" t="str">
         <v xml:space="preserve"> </v>
@@ -4048,13 +4048,13 @@
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>Older Californians</v>
+        <v>What if I have COVID-19 symptoms and have not been contacted by the health department?</v>
       </c>
       <c r="B142" t="str">
-        <v>*   [Friendship Line](https://www.ioaging.org/services/all-inclusive-health-care/friendship-line): Call [888-670-1360](tel:888-670-1360) for 24/7 support if you are 60 years or older, or an adult living with disabilities.  \n*   California Aging and Adult Information Line: Call [800-510-2020](tel:800-510-2020) for help finding local assistance. \n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>[Get tested](https://covid19.ca.gov/testing-and-treatment/) immediately. Contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing, and [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) yourself until:\n\n*   at least 10 days have passed since symptoms started, **AND**\n*   your fever has been gone for 24 hours without the aid of medication, **AND** \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested. Read more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C142" t="str">
-        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D142" t="str">
         <v xml:space="preserve"> </v>
@@ -4074,13 +4074,13 @@
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>Deaf and Hard of Hearing Individuals</v>
+        <v>What if I came in contact with someone who has COVID-19 symptoms, but my local health department is not aware of it?</v>
       </c>
       <c r="B143" t="str">
-        <v>[National Suicide Prevention Deaf and Hard of Hearing Hotline](https://suicidepreventionlifeline.org/help-yourself/for-deaf-hard-of-hearing/): Access 24/7 video relay service by dialing [800-273-8255](tel:800-273-8255) (TTY [800-799-4889](tel:800-799-4889)).\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>You should [get tested](https://covid19.ca.gov/testing-and-treatment/). Contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing. [Quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) yourself while waiting for your test results.\n\n**If you tested positive but have no symptoms**, you should [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) at home for at least 10 days.\n\n**If you develop symptoms**, you should stay home until:\n\n*   at least 10 days have passed since symptoms started, **AND**\n*   your fever has been gone for 24 hours without the aid of medication, **AND** \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested.\n\n**If you had [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) with someone who tested positive but you tested negative**, you should still [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) at home for at least 14 days.\n\nRead more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C143" t="str">
-        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D143" t="str">
         <v xml:space="preserve"> </v>
@@ -4100,13 +4100,13 @@
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>Services for Substance Use Disorders</v>
+        <v>How do I become a contact tracer?</v>
       </c>
       <c r="B144" t="str">
-        <v>*   [SAMHSA National Helpline](https://www.samhsa.gov/find-help/national-helpline): Call [800-662-HELP](tel:1-800-662-4357) for 24/7 information and referrals in English and Spanish. \n*   [SAMHSA Treatment Locator](https://findtreatment.samhsa.gov)**:**  Find drug or alcohol treatment programs. \n*   [Local county access lines](https://gcc01.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.dhcs.ca.gov%2Findividuals%2FPages%2FSUD_County_Access_Lines.aspx&amp;data=02%7C01%7CJanne.Olson-Morgan%40osg.ca.gov%7C122307be91754d12e5dc08d7d984f958%7C265c2dcd2a6e43aab2e826421a8c8526%7C0%7C0%7C637217037446186621&amp;sdata=5sx4UdIlVkRL%2BEJR7FrpK0gYAn20yE71TyBDFIw1kJM%3D&amp;reserved=0): Find your local number for help seeking substance use disorder services.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>California Connected is using existing state employees for contact tracing. We appreciate offers of additional support from the private sector and qualified members of the public, but they are not needed at this time.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C144" t="str">
-        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D144" t="str">
         <v xml:space="preserve"> </v>
@@ -4126,13 +4126,13 @@
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>LGBTQ Individuals</v>
+        <v>Is there extra sick leave available for workers who have COVID-19 symptoms or are waiting for test results?</v>
       </c>
       <c r="B145" t="str">
-        <v>*   [Trevor Project](https://www.thetrevorproject.org): Call [866-488-7386](tel:866-488-7386) or text START to [678678](sms:678678) for 24/7 information and suicide prevention resources for LGBTQ youth.\n*   [Lesbian, Gay, Bisexual and Transgender National Hotline](https://www.glbthotline.org/hotline.html): Call [800-273-8255](tel:800-273-8255) from 1pm – 9pm for support, information or help finding resources.\n*   [Victims of Crime Resource Center](https://1800victims.org/): Call or text [800-842-8467](tel:800-842-8467) or [chat online](https://1800victims.org/) for information about LGTBQ rights, legal protections, and local resources.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>Yes. There are extra federal, state, and in some cases, local sick leaves available for workers in this situation:\n\n*   **Federal paid sick leave:** Up to 80 hours under the Families First Coronavirus Response Act ([FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-employee-paid-leave)) for businesses with less than 500 workers. See [more information on FFCRA in its FAQs](https://www.dol.gov/agencies/whd/pandemic/ffcra-questions).\n*   **California COVID-19 supplemental paid sick leave:** Food businesses with more than 500 workers must give up to 80 hours of [paid sick leave](https://www.gov.ca.gov/wp-content/uploads/2020/04/4.16.20-EO-N-51-20.pdf).  See [more information on supplemental paid sick leave](https://www.dir.ca.gov/dlse/FAQ-for-PSL.html). \n*   **Local paid sick leave ordinances:** Certain local areas also have paid sick leave ordinances.  Consult with the local enforcement agency in your area.\n\nTo understand what may be available, see the comparison of [COVID-19 sick leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) and [benefits for workers impacted by COVID-19](https://www.labor.ca.gov/coronavirus2019/#chart).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C145" t="str">
-        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D145" t="str">
         <v xml:space="preserve"> </v>
@@ -4152,10 +4152,10 @@
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>What is a close contact?</v>
+        <v>Can I return to work once my isolation or quarantine is over?</v>
       </c>
       <c r="B146" t="str">
-        <v>A [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) is someone who was within 6 feet of a person with COVID-19 for at least 15 minutes starting from 2 days before symptoms appeared (or, for asymptomatic patients, 2 days prior to their test) until the time the patient is isolated. This usually includes household members, intimate contacts, and caregivers, but can include others.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>Yes, but when you return depends on your situation.\n\n**If you have symptoms**, you should stay home until:\n\n*   at least 10 days have passed since symptoms started, **AND**\n*    your fever has been gone for 24 hours without the aid of medication, **AND** \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested.\n\n**If you have tested positive but have no symptoms**, you should [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) at home for at least 10 days.\n\n**If you had [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) with someone who tested positive but you have tested negative**, you should still [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) at home for at least 14 days.\n\nGet tested as soon as possible if you have symptoms, or have come in contact with someone who has tested positive or has symptoms.\n\nRead more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C146" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4178,10 +4178,10 @@
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>Will contact tracers track my location?</v>
+        <v>What steps are required when a business has an employee who tests positive?</v>
       </c>
       <c r="B147" t="str">
-        <v>California’s contact tracing program does not use any cell phone tracking technology. Someone from your local public health department will simply speak privately with you. All information is confidential and protected by California’s strict privacy laws. They may stay in touch to make sure your symptoms aren’t worsening.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>If an employer discovers a worker has tested positive for COVID-19 or has symptoms, they should send the worker home. Then [follow guidance](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf) about isolation, quarantine, testing, and when the worker should return to work. Employers should have flexible leave policies. This supports the need for workers to stay home for the protection of others. \n\nThe employer must notify the local health department about the confirmed COVID-19 workers. They must tell their:\n\n*   job titles, \n*   work areas, \n*   [close contacts](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) in the workplace, \n*   dates of symptom onset, and \n*   shifts worked while infectious.\n\nSee “What to do if there is a Case of COVID-19 in the Workplace” in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf). \n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C147" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4204,10 +4204,10 @@
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>Is contact tracing help available in my language?</v>
+        <v>Can people who recover from COVID-19 be re-infected?</v>
       </c>
       <c r="B148" t="str">
-        <v>Your [local health department](https://covid19.ca.gov/get-local-information/) can communicate with you in many different languages.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>We don’t yet know. The duration of immunity to coronavirus infection is not yet understood. Patients infected with similar viruses are unlikely to be re-infected in the months after they recover. But we don’t yet know if  similar immune protection happens in patients with COVID-19.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C148" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4230,10 +4230,10 @@
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v>Who should get tested?</v>
+        <v>How do I apply for a contact tracer position?</v>
       </c>
       <c r="B149" t="str">
-        <v>You should get tested if you:\n\n*   Had [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) with anyone who has tested positive for COVID-19\n*   Have COVID-19 symptoms\n*   Get a call from a contact tracer\n*   Are at [high risk](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Updated-COVID-19-Testing-Guidance.aspx)\n\nFind a [testing site in your area](https://covid19.ca.gov/testing-and-treatment/).\n\nIf you think you may have been exposed, call your doctor.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>California Connected is using existing state employees for contact tracing. We appreciate offers of additional support from the private sector and qualified members of the public, but they are not needed at this time.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C149" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4256,10 +4256,10 @@
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>How do I find a testing location?</v>
+        <v>How do I sign-up for a contact tracer position?</v>
       </c>
       <c r="B150" t="str">
-        <v>To learn more about testing and care, visit the [Testing and treatment page](https://covid19.ca.gov/testing-and-treatment/). You can search for testing locations there using your zip code. \n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>California Connected is using existing state employees for contact tracing. We appreciate offers of additional support from the private sector and qualified members of the public, but they are not needed at this time.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C150" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4282,13 +4282,13 @@
     </row>
     <row r="151">
       <c r="A151" t="str">
-        <v>What if I have COVID-19 symptoms and have not been contacted by the health department?</v>
+        <v>Drive-through testing in Northern California</v>
       </c>
       <c r="B151" t="str">
-        <v>[Get tested](https://covid19.ca.gov/testing-and-treatment/) immediately. Contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing, and [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) yourself until:\n\n*   at least 10 days have passed since symptoms started, **AND**\n*   your fever has been gone for 24 hours without the aid of medication, **AND** \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested. Read more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>*   Alturas (Modoc County)\n*   American Canyon (Napa County)\n*   Antioch (Contra Costa County)\n*   Atascadero (San Luis Obispo County)\n*   Bear Valley (Alpine County)\n*   Bieber (Lassen County)\n*   Bishop (Inyo County)\n*   Calistoga (Napa County)\n*   Calpine (Sierra County)\n*   Cedarville (Modoc County)\n*   Ceres (Sanislaus County)\n*   Chowchilla (Madera County)\n*   Clearlake (Lake County)\n*   Coleville (Mono County)\n*   Corcoran (King County)\n*   Corona (King County)\n*   Crescent City (Del Norte County)\n*   Daly City (San Mateo County)\n*   Dinuba (Tulare County)\n*   Downieville (Sierra County)\n*   Doyle (Lassen County)\n*   East Palo Alto (San Mateo County)\n*   Elk Grove (Sacramento County)\n*   Exeter (Tulare County)\n*   Farmersville (Tulare County)\n*   French Camp (San Joaquin County)\n*   Fresno (Fresno County)\n*   Gridley (Butte County)\n*   Half Moon Bay (San Mateo County)\n*   Hanford (King County)\n*   Hayfork (Trinity County)\n*   Herlong (Lassen County)\n*   Huron (Fresno County)\n*   Jackson (Amador County)\n*   Kerman (Fresno County)\n*   Lakeport (Lake County)\n*   Lee Vining (Mono County)\n*   Lemoore (King County)\n*   Lewiston (Trinity County)\n*   Livingston (Merced County)\n*   Lone Pine (Inyo County)\n*   Los Banos (Merced County)\n*   Loyalton (Sierra County)\n*   Magalia (Butte County)\n*   Mammoth Lakes (Mono County)\n*   Markleeville (Alpine County)\n*   Mendota (Fresno County)\n*   Merced (Merced County)\n*   Middletown (Lake County)\n*   Napa (Napa County)\n*   North San Juan (Nevada County)\n*   Oakland (Alameda County)\n*   Placerville (El Dorado County)\n*   Porterville (Tulare County)\n*   Redding (Shasta County)\n*   Redwood City (San Mateo County)\n*   Reedley (Fresno County)\n*   Rio Linda (Sacramento County)\n*   Sacramento (Sacramento County)\n*   Salida (Stanislaus County)\n*   San Bruno (San Mateo County)\n*   San Francisco (San Francisco)\n*   San Jose (Santa Clara County)\n*   San Mateo (San Mateo County)\n*   Santa Rosa (Sonoma County)\n*   Selma (Fresno County)\n*   St. Helena (Napa County)\n*   Stockton (San Joaquin County)\n*   Susanville (Lassen County)\n*   Tracy (San Joaquin County)\n*   Tulare (Tulare County)\n*   Turlock (Stanislaus County)\n*   Upper Lake (Lake County)\n*   Vallejo (Solano County)\n*   Visalia (Tulare County)\n*   Wawona (Mariposa County)\n*   Weaverville (Trinity County)\n*   Westwood (Lassen County)\n\n*   Woodlake (Tulare County)\n*   Woodland (Yolo County)\n*   Yosemite Valley (Mariposa County)\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C151" t="str">
-        <v>https://covid19.ca.gov/contact-tracing/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D151" t="str">
         <v xml:space="preserve"> </v>
@@ -4308,13 +4308,13 @@
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>What if I came in contact with someone who has COVID-19 symptoms, but my local health department is not aware of it?</v>
+        <v>Drive-through testing in Southern California</v>
       </c>
       <c r="B152" t="str">
-        <v>You should [get tested](https://covid19.ca.gov/testing-and-treatment/). Contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing. [Quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) yourself while waiting for your test results.\n\n**If you tested positive but have no symptoms**, you should [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) at home for at least 10 days.\n\n**If you develop symptoms**, you should stay home until:\n\n*   at least 10 days have passed since symptoms started, **AND**\n*   your fever has been gone for 24 hours without the aid of medication, **AND** \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested.\n\n**If you had [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) with someone who tested positive but you tested negative**, you should still [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) at home for at least 14 days.\n\nRead more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>*   Alpine (San Diego County) \n*   Anaheim (Orange County)\n*   Apple Valley (San Bernardino County)\n*   Bakersfield (Kern County)\n*   Banning (Riverside County)\n*   Barstow (San Bernardino County)\n*   Beaumont (Riverside County)\n*   Bell (Los Angeles County)\n*   Blythe (Riverside County)\n*   Calexico (Imperial County)\n*   Coachella (Riverside County)\n*   Compton (Los Angeles County)\n*   Costa Mesa (Orange County)\n*   Delano (Kern County)\n*   Desert Hot Springs (Riverside County)\n*   El Centro (Imperial County)\n*   Fallbrook (San Diego)\n*   Fontana (San Bernardino County)\n*   Fullerton (Orange County)\n*   Gardena (Los Angeles County)\n*   Hemet (Riverside County)\n*   Hesperia (San Bernardino County)\n*   Indio (Riverside County)\n*   La Habra (Orange County)\n*   Lake Elsinore (Riverside County)\n*   Lamont (Kern County)\n*   Lancaster (Los Angeles County)\n*   Lemon Grove (San Diego County)\n*   Los Angeles (Los Angeles County)\n*   McFarland (Kern County)\n*   Oceanside (San Diego)\n*   Ontario (San Bernardino County)\n*   Palmdale (Los Angeles County)\n*   Paramount (Los Angeles County)\n*   Pasadena (Los Angeles County)\n*   Perris (Riverside County)\n*   Phelan (San Bernardino County)\n*   Pico Rivera (Los Angeles County)\n*   Pomona (Los Angeles County)\n*   Port Hueneme (Ventura County)\n*   Riverside (Riverside County)\n*   Rosamond (Kern County)\n*   San Jucinta (Riverside County)\n*   San Juan Capistrano (Orange County)\n*   Santa Maria (Santa Barbara County)\n*   Santa Paula (Ventura County)\n*   Shafter (Kern County)\n*   Valley Center (San Diego County)\n*   Victorville (San Bernardino County)\n*   Wasco (Kern County) \n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C152" t="str">
-        <v>https://covid19.ca.gov/contact-tracing/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D152" t="str">
         <v xml:space="preserve"> </v>
@@ -4334,13 +4334,13 @@
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v>How do I become a contact tracer?</v>
+        <v>How do I get a drive-through test by Verily’s Project Baseline?</v>
       </c>
       <c r="B153" t="str">
-        <v>California Connected is using existing state employees for contact tracing. We appreciate offers of additional support from the private sector and qualified members of the public, but they are not needed at this time.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>There are two steps to this process: screening and testing. First, you will create an account and take the online screener. If you are eligible, you will get details on how and where to get tested. Once tested, you’ll get an email or phone call with your COVID-19 test results.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C153" t="str">
-        <v>https://covid19.ca.gov/contact-tracing/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D153" t="str">
         <v xml:space="preserve"> </v>
@@ -4360,13 +4360,13 @@
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v>Is there extra sick leave available for workers who have COVID-19 symptoms or are waiting for test results?</v>
+        <v>Why am I asked to create an account for Verily?</v>
       </c>
       <c r="B154" t="str">
-        <v>Yes. There are extra federal, state, and in some cases, local sick leaves available for workers in this situation:\n\n*   **Federal paid sick leave:** Up to 80 hours under the Families First Coronavirus Response Act ([FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-employee-paid-leave)) for businesses with less than 500 workers. See [more information on FFCRA in its FAQs](https://www.dol.gov/agencies/whd/pandemic/ffcra-questions).\n*   **California COVID-19 supplemental paid sick leave:** Food businesses with more than 500 workers must give up to 80 hours of [paid sick leave](https://www.gov.ca.gov/wp-content/uploads/2020/04/4.16.20-EO-N-51-20.pdf).  See [more information on supplemental paid sick leave](https://www.dir.ca.gov/dlse/FAQ-for-PSL.html). \n*   **Local paid sick leave ordinances:** Certain local areas also have paid sick leave ordinances.  Consult with the local enforcement agency in your area.\n\nTo understand what may be available, see the comparison of [COVID-19 sick leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) and [benefits for workers impacted by COVID-19](https://www.labor.ca.gov/coronavirus2019/#chart).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>Verily needs a way to authenticate and protect user information. They turned to Google for this service, because Google accounts have best-in-class authentication. Simply link to an existing Google account or create a new one (which you can do with any email address). Then Verily can contact you securely during the screening and testing process. All data r collected by Verily is kept private and is not linked to a user’s Google account.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C154" t="str">
-        <v>https://covid19.ca.gov/contact-tracing/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D154" t="str">
         <v xml:space="preserve"> </v>
@@ -4386,13 +4386,13 @@
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>Can I return to work once my isolation or quarantine is over?</v>
+        <v>Do I need emergency treatment?</v>
       </c>
       <c r="B155" t="str">
-        <v>Yes, but when you return depends on your situation.\n\n**If you have symptoms**, you should stay home until:\n\n*   at least 10 days have passed since symptoms started, **AND**\n*    your fever has been gone for 24 hours without the aid of medication, **AND** \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested.\n\n**If you have tested positive but have no symptoms**, you should [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) at home for at least 10 days.\n\n**If you had [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) with someone who tested positive but you have tested negative**, you should still [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) at home for at least 14 days.\n\nGet tested as soon as possible if you have symptoms, or have come in contact with someone who has tested positive or has symptoms.\n\nRead more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>If you develop any of these symptoms of COVID-19, get medical attention immediately:\n\n*   Trouble breathing\n*   Persistent pain or pressure in the chest\n*   New confusion \n*   Inability to awake or stay awake\n*   Bluish lips or face\n\nThere are other, less-common symptoms. Please call your medical provider if you have any symptoms that are severe or concern you.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call [911](tel:911), tell the operator you have coronavirus symptoms. This is so ambulance workers can be ready to treat you safely.\n\nNot sure if this applies to you? Check your symptoms with the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C155" t="str">
-        <v>https://covid19.ca.gov/contact-tracing/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D155" t="str">
         <v xml:space="preserve"> </v>
@@ -4412,13 +4412,13 @@
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v>What steps are required when a business has an employee who tests positive?</v>
+        <v>When can I be around other people after I had or likely had COVID-19?</v>
       </c>
       <c r="B156" t="str">
-        <v>If an employer discovers a worker has tested positive for COVID-19 or has symptoms, they should send the worker home. Then [follow guidance](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf) about isolation, quarantine, testing, and when the worker should return to work. Employers should have flexible leave policies. This supports the need for workers to stay home for the protection of others. \n\nThe employer must notify the local health department about the confirmed COVID-19 workers. They must tell their:\n\n*   job titles, \n*   work areas, \n*   [close contacts](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) in the workplace, \n*   dates of symptom onset, and \n*   shifts worked while infectious.\n\nSee “What to do if there is a Case of COVID-19 in the Workplace” in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf). \n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>You can be with others after:\n\n*   10 days since symptoms first appeared **and**\n*   At least 24 hours with no fever without fever-reducing medication **and**\n*   After symptoms have improved\n\nCDC has [detailed recommendations](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/end-home-isolation.html) for people who had tested positive but had no symptoms.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C156" t="str">
-        <v>https://covid19.ca.gov/contact-tracing/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D156" t="str">
         <v xml:space="preserve"> </v>
@@ -4438,13 +4438,13 @@
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>Can people who recover from COVID-19 be re-infected?</v>
+        <v>When can I be around other people after I tested positive for COVID-19 but had no symptoms?</v>
       </c>
       <c r="B157" t="str">
-        <v>We don’t yet know. The duration of immunity to coronavirus infection is not yet understood. Patients infected with similar viruses are unlikely to be re-infected in the months after they recover. But we don’t yet know if  similar immune protection happens in patients with COVID-19.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>If you continue to have no symptoms, you can be with others after 10 days have passed since your test.\n\nCDC has [detailed recommendations](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/end-home-isolation.html) for people who had tested positive for coronavirus but had no symptoms.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C157" t="str">
-        <v>https://covid19.ca.gov/contact-tracing/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D157" t="str">
         <v xml:space="preserve"> </v>
@@ -4464,13 +4464,13 @@
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>County Monitoring List</v>
+        <v>Should employees be required to provide proof of a negative coronavirus test before returning to work after they had COVID-19?</v>
       </c>
       <c r="B158" t="str">
-        <v>1.  Alameda\n2.  Amador – 7/25/2020\n3.  Butte\n4.  Calaveras – 8/13/2020\n5.  Colusa\n6.  Contra Costa\n7.  Fresno\n8.  Glenn\n9.  Imperial\n10.  Inyo – 8/6/2020\n11.  Kern\n12.  Kings\n13.  Los Angeles\n14.  Madera\n15.  Marin\n16.  Mendocino – 7/25/2020\n17.  Merced\n18.  Mono\n19.  Monterey\n20.  Napa\n21.  Orange\n22.  Riverside\n23.  Sacramento\n24.  San Benito\n25.  San Bernardino\n26.  San Francisco\n27.  San Joaquin\n28.  San Luis Obispo\n29.  San Mateo\n30.  Santa Barbara\n31.  Santa Clara\n32.  Sierra – 8/15/2020\n33.  Solano\n34.  Sonoma\n35.  Stanislaus\n36.  Sutter\n37.  Tulare\n38.  Ventura\n39.  Yolo\n40.  Yuba\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>No. Proof of a negative test should not be required prior to returning to the workplace after documented COVID infection, since PCR tests can remain positive long after an individual is no longer infectious. CDPH [COVID-19 Testing Guidance](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Updated-COVID-19-Testing-Guidance.aspx) recommends symptom- or protocol-based criteria be used to determine when an employee is safe to return to the workplace.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C158" t="str">
-        <v>https://covid19.ca.gov/roadmap-counties/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D158" t="str">
         <v xml:space="preserve"> </v>
@@ -4490,13 +4490,13 @@
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>For attested counties not on Monitoring List</v>
+        <v>Can two people that both tested positive hang out/stay together?</v>
       </c>
       <c r="B159" t="str">
-        <v>*   [Industries open statewide](https://covid19.ca.gov/industry-guidance/)\n*   Dine-in restaurants (outdoors only)\n*   Wineries and tasting rooms (outdoors only)\n*   Family entertainment centers (outdoors only)\n*   Zoos and museums (outdoors only)\n*   Cardrooms (outdoors only)\n*   Casinos\n*   Gyms and fitness centers\n*   Hotels (for tourism and individual travel)\n*   Campgrounds and outdoor recreation\n*   Personal care services, like nail salons and body waxing\n*   Hair salons and barbershops\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>No. You should take preventive measures to protect yourself and others. We do not know yet if or when a person can be reinfected with COVID-19. \n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C159" t="str">
-        <v>https://covid19.ca.gov/roadmap-counties/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D159" t="str">
         <v xml:space="preserve"> </v>
@@ -4516,13 +4516,13 @@
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>For counties on Monitoring List for 3 consecutive days</v>
+        <v>If I test positive for COVID-19 in a viral test, what should I do to protect others in my household?</v>
       </c>
       <c r="B160" t="str">
-        <v>*   [Industries open statewide](https://covid19.ca.gov/industry-guidance/)\n*   Casinos\n*   Hotels (for tourism and individual travel)\n*   Campgrounds and outdoor recreation\n\nThe following industries must close indoor operations, but they may be modified to operate outside or by pick-up:\n\n*   Dine-in restaurants\n*   Wineries and tasting rooms\n*   Movie theaters \n*   Family entertainment centers (for example: bowling alleys, miniature golf, batting cages and arcades)\n*   Zoos and museums\n*   Cardrooms\n*   Gyms and fitness centers\n*   Personal care services, like nail salons and body waxing\n*   Places of worship and cultural ceremonies, like weddings and funerals\n*   Offices for non-critical infrastructure sectors\n*   Shopping malls \n\nNOTE: Imperial County is open to the essential workforce only (Stage One).\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>You should [self-isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) from others in your household who have not tested positive. Sleep and stay in a separate room from them, and use a separate bathroom, if possible. Multiple infected people in the same household can use the same room for isolation.\n\nMembers of your household should get tested right away. They should [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) for at least 14 days. Symptoms can develop even after testing negative within 14 days after exposure. Multiple people in the same household should not quarantine in the same room, since some may be infected.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C160" t="str">
-        <v>https://covid19.ca.gov/roadmap-counties/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D160" t="str">
         <v xml:space="preserve"> </v>
@@ -4542,13 +4542,13 @@
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>For counties without attestations</v>
+        <v>How can I find a coronavirus testing location near me?</v>
       </c>
       <c r="B161" t="str">
-        <v>*   [Industries open statewide](https://covid19.ca.gov/industry-guidance/)\n\nMore info: [County variance info](https://covid19.ca.gov/roadmap-counties/)</v>
+        <v>&gt; [Find a testing location](https://arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401)\n&gt; -----------------------------------------------------------------------------------------------------------\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C161" t="str">
-        <v>https://covid19.ca.gov/roadmap-counties/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D161" t="str">
         <v xml:space="preserve"> </v>
@@ -4568,10 +4568,10 @@
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>Drive-through testing in Northern California</v>
+        <v>What is an antibody test? Where can I get an antibody test?</v>
       </c>
       <c r="B162" t="str">
-        <v>*   Alturas (Modoc County)\n*   American Canyon (Napa County)\n*   Antioch (Contra Costa County)\n*   Atascadero (San Luis Obispo County)\n*   Bear Valley (Alpine County)\n*   Bieber (Lassen County)\n*   Bishop (Inyo County)\n*   Calistoga (Napa County)\n*   Calpine (Sierra County)\n*   Cedarville (Modoc County)\n*   Ceres (Sanislaus County)\n*   Chowchilla (Madera County)\n*   Clearlake (Lake County)\n*   Coleville (Mono County)\n*   Corcoran (King County)\n*   Corona (King County)\n*   Crescent City (Del Norte County)\n*   Daly City (San Mateo County)\n*   Dinuba (Tulare County)\n*   Downieville (Sierra County)\n*   Doyle (Lassen County)\n*   East Palo Alto (San Mateo County)\n*   Elk Grove (Sacramento County)\n*   Exeter (Tulare County)\n*   Farmersville (Tulare County)\n*   French Camp (San Joaquin County)\n*   Fresno (Fresno County)\n*   Gridley (Butte County)\n*   Half Moon Bay (San Mateo County)\n*   Hanford (King County)\n*   Hayfork (Trinity County)\n*   Herlong (Lassen County)\n*   Huron (Fresno County)\n*   Jackson (Amador County)\n*   Kerman (Fresno County)\n*   Lakeport (Lake County)\n*   Lee Vining (Mono County)\n*   Lemoore (King County)\n*   Lewiston (Trinity County)\n*   Livingston (Merced County)\n*   Lone Pine (Inyo County)\n*   Los Banos (Merced County)\n*   Loyalton (Sierra County)\n*   Magalia (Butte County)\n*   Mammoth Lakes (Mono County)\n*   Markleeville (Alpine County)\n*   Mendota (Fresno County)\n*   Merced (Merced County)\n*   Middletown (Lake County)\n*   Napa (Napa County)\n*   North San Juan (Nevada County)\n*   Oakland (Alameda County)\n*   Placerville (El Dorado County)\n*   Porterville (Tulare County)\n*   Redding (Shasta County)\n*   Redwood City (San Mateo County)\n*   Reedley (Fresno County)\n*   Rio Linda (Sacramento County)\n*   Sacramento (Sacramento County)\n*   Salida (Stanislaus County)\n*   San Bruno (San Mateo County)\n*   San Francisco (San Francisco)\n*   San Jose (Santa Clara County)\n*   San Mateo (San Mateo County)\n*   Santa Rosa (Sonoma County)\n*   Selma (Fresno County)\n*   St. Helena (Napa County)\n*   Stockton (San Joaquin County)\n*   Susanville (Lassen County)\n*   Tracy (San Joaquin County)\n*   Tulare (Tulare County)\n*   Turlock (Stanislaus County)\n*   Upper Lake (Lake County)\n*   Vallejo (Solano County)\n*   Visalia (Tulare County)\n*   Wawona (Mariposa County)\n*   Weaverville (Trinity County)\n*   Westwood (Lassen County)\n\n*   Woodlake (Tulare County)\n*   Woodland (Yolo County)\n*   Yosemite Valley (Mariposa County)\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>[**Antibody tests**](https://www.cdc.gov/coronavirus/2019-ncov/testing/serology-overview.html) detect past infections. They can determine if you are a good candidate to [donate blood plasma](https://covid19.ca.gov/plasma/). It can take 1-3 weeks after infection for your body to make antibodies.\n\nYou can find locations for both viral and antibody tests on [California’s testing map](https://www.arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C162" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4594,13 +4594,13 @@
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>Drive-through testing in Southern California</v>
+        <v>What are the pay and benefits for California Health Corps professionals?</v>
       </c>
       <c r="B163" t="str">
-        <v>*   Alpine (San Diego County) \n*   Anaheim (Orange County)\n*   Apple Valley (San Bernardino County)\n*   Bakersfield (Kern County)\n*   Banning (Riverside County)\n*   Barstow (San Bernardino County)\n*   Beaumont (Riverside County)\n*   Bell (Los Angeles County)\n*   Blythe (Riverside County)\n*   Calexico (Imperial County)\n*   Coachella (Riverside County)\n*   Compton (Los Angeles County)\n*   Costa Mesa (Orange County)\n*   Delano (Kern County)\n*   Desert Hot Springs (Riverside County)\n*   El Centro (Imperial County)\n*   Fallbrook (San Diego)\n*   Fontana (San Bernardino County)\n*   Fullerton (Orange County)\n*   Gardena (Los Angeles County)\n*   Hemet (Riverside County)\n*   Hesperia (San Bernardino County)\n*   Indio (Riverside County)\n*   La Habra (Orange County)\n*   Lake Elsinore (Riverside County)\n*   Lamont (Kern County)\n*   Lancaster (Los Angeles County)\n*   Lemon Grove (San Diego County)\n*   Los Angeles (Los Angeles County)\n*   McFarland (Kern County)\n*   Oceanside (San Diego)\n*   Ontario (San Bernardino County)\n*   Palmdale (Los Angeles County)\n*   Paramount (Los Angeles County)\n*   Pasadena (Los Angeles County)\n*   Perris (Riverside County)\n*   Phelan (San Bernardino County)\n*   Pico Rivera (Los Angeles County)\n*   Pomona (Los Angeles County)\n*   Port Hueneme (Ventura County)\n*   Riverside (Riverside County)\n*   Rosamond (Kern County)\n*   San Jucinta (Riverside County)\n*   San Juan Capistrano (Orange County)\n*   Santa Maria (Santa Barbara County)\n*   Santa Paula (Ventura County)\n*   Shafter (Kern County)\n*   Valley Center (San Diego County)\n*   Victorville (San Bernardino County)\n*   Wasco (Kern County) \n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>Salary rates for most of the health care professionals being hired for this emergency are listed in the [CalHR Pay Scales](https://www.calhr.ca.gov/Pay%20Scales%20Library/PS_Sec_05.pdf) (pages 5.12 and 5.13). In addition, CalHR has established pay rates for medical roles that don’t have a corresponding regular classification and pay schedule, such as paramedics and EMTs. CalHR will determine specific salary and benefits after conducting a review of each application.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C163" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/healthcorps/</v>
       </c>
       <c r="D163" t="str">
         <v xml:space="preserve"> </v>
@@ -4620,13 +4620,13 @@
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>How do I get a drive-through test by Verily’s Project Baseline?</v>
+        <v>Some healthcare professions are not listed. Are health professionals who are not listed (e.g., Medical Technicians, Lab Technicians, etc.) eligible for the California Health Corps?</v>
       </c>
       <c r="B164" t="str">
-        <v>There are two steps to this process: screening and testing. First, you will create an account and take the online screener. If you are eligible, you will get details on how and where to get tested. Once tested, you’ll get an email or phone call with your COVID-19 test results.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>California Health Corps are currently only accepting applications for the healthcare professions listed on the website. However, we are constantly re-evaluating our needs during this fluid situation and will open the registration for other professionals, if the need arises.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C164" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/healthcorps/</v>
       </c>
       <c r="D164" t="str">
         <v xml:space="preserve"> </v>
@@ -4646,13 +4646,13 @@
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>Why am I asked to create an account for Verily?</v>
+        <v>When can I expect to hear a response after completing my California Health Corps registration?</v>
       </c>
       <c r="B165" t="str">
-        <v>Verily needs a way to authenticate and protect user information. They turned to Google for this service, because Google accounts have best-in-class authentication. Simply link to an existing Google account or create a new one (which you can do with any email address). Then Verily can contact you securely during the screening and testing process. All data r collected by Verily is kept private and is not linked to a user’s Google account.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>Currently we anticipate the process may take up to two weeks, since an incredible number of responses are received and need to prioritize certain parts of the state, where the needs are the greatest. We will begin to contact the volunteers after verification of credentials, and based on current and anticipated needs.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C165" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/healthcorps/</v>
       </c>
       <c r="D165" t="str">
         <v xml:space="preserve"> </v>
@@ -4672,13 +4672,13 @@
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>Do I need emergency treatment?</v>
+        <v>How do I return to the California Health Corps application after logging out?</v>
       </c>
       <c r="B166" t="str">
-        <v>If you develop any of these symptoms of COVID-19, get medical attention immediately:\n\n*   Trouble breathing\n*   Persistent pain or pressure in the chest\n*   New confusion \n*   Inability to awake or stay awake\n*   Bluish lips or face\n\nThere are other, less-common symptoms. Please call your medical provider if you have any symptoms that are severe or concern you.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call 911, tell the operator you have coronavirus symptoms. This is so ambulance workers can be ready to treat you safely.\n\nNot sure if this applies to you? Check your symptoms with the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>Visit [https://healthcarevolunteers.ca.gov/](https://healthcarevolunteers.ca.gov/) and use the account you created while applying to correct or update any information you want.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C166" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/healthcorps/</v>
       </c>
       <c r="D166" t="str">
         <v xml:space="preserve"> </v>
@@ -4698,13 +4698,13 @@
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>When can I be around other people after I had or likely had COVID-19?</v>
+        <v>Resources for the California Health Corps participants</v>
       </c>
       <c r="B167" t="str">
-        <v>You can be with others after:\n\n*   10 days since symptoms first appeared **and**\n*   At least 24 hours with no fever without fever-reducing medication **and**\n*   After symptoms have improved\n\nCDC has [detailed recommendations](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/end-home-isolation.html) for people who had tested positive but had no symptoms.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>*   Health Corps FAQ: [FAQ-Health-Corps (PDF)](https://files.covid19.ca.gov/pdf/FAQ-Health-Corps.pdf)\n*   Travel Reimbursement FAQ: [FAQ-Travel-Reimbursement (PDF)](https://files.covid19.ca.gov/pdf/FAQ-Travel-Reimbursement.pdf)\n*   SNF Orientation: [SNF-Nursing-Staff-Orientation (PDF)](https://files.covid19.ca.gov/pdf/SNF-Nursing-Staff-Orientation.pdf)\n*   How to file a complaint: [How-to-file-a-complaint (PDF)](https://files.covid19.ca.gov/pdf/How-to-file-a-complaint.pdf)\n*   Direct deposit: [std699-Direct-Deposit (PDF)](https://files.covid19.ca.gov/pdf/std699-Direct-Deposit.pdf)\n*   Travel expense claim: [Std262-Travel-Expense-Claim (PDF)](https://files.covid19.ca.gov/pdf/Std262-Travel-Expense-Claim.pdf)\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C167" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/healthcorps/</v>
       </c>
       <c r="D167" t="str">
         <v xml:space="preserve"> </v>
@@ -4724,13 +4724,13 @@
     </row>
     <row r="168">
       <c r="A168" t="str">
-        <v>When can I be around other people after I tested positive for COVID-19 but had no symptoms?</v>
+        <v>Can a doctor with out of state license or foreign medical graduate without California license work for the California Health Corps?</v>
       </c>
       <c r="B168" t="str">
-        <v>If you continue to have no symptoms, you can be with others after 10 days have passed since your test.\n\nCDC has [detailed recommendations](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/end-home-isolation.html) for people who had tested positive for coronavirus but had no symptoms.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>To be eligible for COVID-19 emergency medical staffing roles, you must:\n\n*   Have a valid California License for clinical practice (if you are a MD, DO, etc.) \n*   **OR** are a medical resident or nursing student \n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C168" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/healthcorps/</v>
       </c>
       <c r="D168" t="str">
         <v xml:space="preserve"> </v>
@@ -4750,13 +4750,13 @@
     </row>
     <row r="169">
       <c r="A169" t="str">
-        <v>Should employees be required to provide proof of a negative coronavirus test before returning to work after they had COVID-19?</v>
+        <v>Agriculture and livestock</v>
       </c>
       <c r="B169" t="str">
-        <v>No. Proof of a negative test should not be required prior to returning to the workplace after documented COVID infection, since PCR tests can remain positive long after an individual is no longer infectious. CDPH [COVID-19 Testing Guidance](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Updated-COVID-19-Testing-Guidance.aspx) recommends symptom- or protocol-based criteria be used to determine when an employee is safe to return to the workplace.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>Follow this [guidance for the agriculture and livestock industry](https://files.covid19.ca.gov/pdf/guidance-agriculture--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the agriculture and livestock industry](https://files.covid19.ca.gov/pdf/checklist-agriculture.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C169" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D169" t="str">
         <v xml:space="preserve"> </v>
@@ -4776,13 +4776,13 @@
     </row>
     <row r="170">
       <c r="A170" t="str">
-        <v>Can two people that both tested positive hang out/stay together?</v>
+        <v>Auto dealerships</v>
       </c>
       <c r="B170" t="str">
-        <v>No. You should take preventive measures to protect yourself and others. We do not know yet if or when a person can be reinfected with COVID-19. \n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>Follow this [guidance for the automobile dealerships and rental operators industry](https://files.covid19.ca.gov/pdf/guidance-auto-dealerships--en.pdf) to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for the automobile dealerships and rental operators](https://files.covid19.ca.gov/pdf/checklist-auto-dealerships.pdf) industry in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C170" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D170" t="str">
         <v xml:space="preserve"> </v>
@@ -4802,13 +4802,13 @@
     </row>
     <row r="171">
       <c r="A171" t="str">
-        <v>If I test positive for COVID-19 in a viral test, what should I do to protect others in my household?</v>
+        <v>Campgrounds and outdoor recreation</v>
       </c>
       <c r="B171" t="str">
-        <v>You should [self-isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) from others in your household who have not tested positive. Sleep and stay in a separate room from them, and use a separate bathroom, if possible. Multiple infected people in the same household can use the same room for isolation.\n\nMembers of your household should get tested right away. They should [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) for at least 14 days. Symptoms can develop even after testing negative within 14 days after exposure. Multiple people in the same household should not quarantine in the same room, since some may be infected.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>Follow this [guidance for campgrounds](https://files.covid19.ca.gov/pdf/guidance-campgrounds-outdoor-recreation--en.pdf), RV parks, and outdoor recreation to create a safer environment for workers and patrons.\n\nReview the guidance and prepare a plan for your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C171" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D171" t="str">
         <v xml:space="preserve"> </v>
@@ -4828,13 +4828,13 @@
     </row>
     <row r="172">
       <c r="A172" t="str">
-        <v>How can I find a coronavirus testing location near me?</v>
+        <v>Cardrooms and racetracks</v>
       </c>
       <c r="B172" t="str">
-        <v>&gt; [Find a testing location](https://arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401)\n&gt; -----------------------------------------------------------------------------------------------------------\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>**Tier status:**\n\nWidespread (purple): Outdoor only with modifications\n\nSubstantial (red): Outdoor only with modifications\n\nModerate (orange)\n\n*   Indoor with modifications\n*   Capacity must be limited to 25%\n\nMinimal (yellow)\n\n*   Indoor with modifications\n*   Capacity must be limited to 50%\n\nFollow this [guidance for cardrooms](https://files.covid19.ca.gov/pdf/guidance-cardrooms-racetracks--en.pdf), racetracks, and satellite wagering to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for cardrooms](https://files.covid19.ca.gov/pdf/checklist-cardrooms-racetracks.pdf), racetracks, and satellite wagering in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C172" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D172" t="str">
         <v xml:space="preserve"> </v>
@@ -4854,13 +4854,13 @@
     </row>
     <row r="173">
       <c r="A173" t="str">
-        <v>What is an antibody test? Where can I get an antibody test?</v>
+        <v>Childcare</v>
       </c>
       <c r="B173" t="str">
-        <v>[**Antibody tests**](https://www.cdc.gov/coronavirus/2019-ncov/testing/serology-overview.html) detect past infections. They can determine if you are a good candidate to [donate blood plasma](https://covid19.ca.gov/plasma/). It can take 1-3 weeks after infection for your body to make antibodies.\n\nYou can find locations for both viral and antibody tests on [California’s testing map](https://www.arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>Childcare facilities\n\n*   Follow the [guidance for the childcare industry](https://files.covid19.ca.gov/pdf/guidance-childcare--en.pdf) to minimize the spread of COVID-19. \n*   Follow the [case and contact management guidance](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/contact-management-childcare-facilities.aspx), which includes:\n    *   What to do when kids or staff develop symptoms while in the facility.\n    *   What to do for kids and adults who may have been exposed to someone with COVID-19.\n    *   When closure of a facility should be considered, and when it can reopen.\n*   See the answers to [frequently asked questions about waivers](https://www.cdss.ca.gov/Portals/9/CCLD/PINs/2020/CCP/PIN-20-22-CCP.pdf) that are available to providers.\n*   Review the guidance, prepare a plan, and post the [checklist for childcare](https://files.covid19.ca.gov/pdf/checklist-childcare--en.pdf) in your facility to show employees and families that you’ve reduced the risk and are open for operation.\n\nCohorts of kids and adults in controlled, supervised settings\n\nA **cohort** is a stable group of no more than 14 children or youth and no more than two supervising adults in a supervised environment. The group stays together for all activities, including meals and recreation. And this group avoids contact with anyone not in their group.\n\nFollow the [guidance for cohorts of children](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/small-groups-child-youth.aspx) and youth in controlled, supervised and indoor environments. See the answers to [frequently asked questions](https://files.covid19.ca.gov/pdf/guidance-schools-cohort-FAQ.pdf) about cohort guidance.\n\nKids and adults in supervised care environments must be in groups as small as possible. Kids and supervising adults in one group must not physically interact with:\n\n*   kids and supervising adults in other groups\n*   other facility staff\n*   parents of kids in other groups\n\nPracticing a cohort structure\n\n*   decreases opportunities for exposure to or transmission of the virus\n*   facilitates more efficient contact tracing in the event of a positive case\n*   allows for targeted testing, quarantine, and isolation of a single group instead of an entire population of kids and supervising adults\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C173" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D173" t="str">
         <v xml:space="preserve"> </v>
@@ -4880,13 +4880,13 @@
     </row>
     <row r="174">
       <c r="A174" t="str">
-        <v>What are the pay and benefits for California Health Corps professionals?</v>
+        <v>Cohorts for children and youth in supervised settings</v>
       </c>
       <c r="B174" t="str">
-        <v>Salary rates for most of the health care professionals being hired for this emergency are listed in the [CalHR Pay Scales](https://www.calhr.ca.gov/Pay%20Scales%20Library/PS_Sec_05.pdf) (pages 5.12 and 5.13). In addition, CalHR has established pay rates for medical roles that don’t have a corresponding regular classification and pay schedule, such as paramedics and EMTs. CalHR will determine specific salary and benefits after conducting a review of each application.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>A **cohort** is a stable group of no more than 14 children or youth and no more than two supervising adults in a supervised environment. The group stays together for all activities, including meals and recreation. And this group avoids contact with anyone not in their group.\n\nThe [guidance related to cohorts](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/small-groups-child-youth.aspx) sets minimum guidelines for providing specialized, targeted support services, necessary in-person child supervision and limited instruction, and facilitation of distance learning in small group environments in ways that maintain the focus on health and safety to minimize transmission. This guidance enables schools to provide specialized services for students with disabilities and English learners, and in-person support for at-risk and high-need students. \n\nSee the answers to [frequently asked questions](https://files.covid19.ca.gov/pdf/guidance-schools-cohort-FAQ.pdf) about cohort guidance. \n\nLocal educational agencies, nonprofits, or other authorized providers must follow the guidance for cohorts of children and youth in controlled, supervised and indoor environments. These environments include, but are not limited to, the following:\n\n*   public and private schools\n*   licensed and license-exempt child care settings \n*   organized and supervised care environments, like “distance learning hubs”\n*   recreation programs\n*   before and after school programs\n*   youth groups\n*   day camps\n\nKids and adults in supervised care environments must be in groups as small as possible. Kids and supervising adults in one group must not physically interact with:\n\n*   kids and supervising adults in other groups\n*   other facility staff\n*   parents of kids in other groups\n\nPracticing a cohort structure:\n\n*   decreases opportunities for exposure to or transmission of the virus\n*   facilitates more efficient contact tracing in the event of a positive case\n*   allows for targeted testing, quarantine, and isolation of a single group instead of an entire population of kids and supervising adults\n\nChildcare facilities\n\n*   Follow the [case and contact management guidance](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/contact-management-childcare-facilities.aspx), which includes:\n    *   What to do when kids or staff develop symptoms while in the facility.\n    *   What to do for kids and adults who may have been exposed to someone with COVID-19.\n    *   When closure of a facility should be considered, and when it can reopen.\n*   See the answers to [frequently asked questions about waivers](https://www.cdss.ca.gov/Portals/9/CCLD/PINs/2020/CCP/PIN-20-22-CCP.pdf) that are available to providers. \n\nGuidance and directives related to [schools](https://covid19.ca.gov/industry-guidance/#schools-guidance), [childcare](https://covid19.ca.gov/industry-guidance/#childcare-guidance), [day camps](https://covid19.ca.gov/industry-guidance/#daycamps-guidance), [youth sports](https://covid19.ca.gov/industry-guidance/#youthsports-guidance), and [institutions of higher education](https://covid19.ca.gov/industry-guidance/#higher-education) are not superseded by this guidance for cohorts of children and youth and still apply to those specified settings.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C174" t="str">
-        <v>https://covid19.ca.gov/healthcorps/</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D174" t="str">
         <v xml:space="preserve"> </v>
@@ -4906,13 +4906,13 @@
     </row>
     <row r="175">
       <c r="A175" t="str">
-        <v>Some healthcare professions are not listed. Are health professionals who are not listed (e.g., Medical Technicians, Lab Technicians, etc.) eligible for the California Health Corps?</v>
+        <v>Communications infrastructure</v>
       </c>
       <c r="B175" t="str">
-        <v>California Health Corps are currently only accepting applications for the healthcare professions listed on the website. However, we are constantly re-evaluating our needs during this fluid situation and will open the registration for other professionals, if the need arises.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>Follow this [guidance for the communications infrastructure industry](https://files.covid19.ca.gov/pdf/guidance-communications--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the communications infrastructure industry](https://files.covid19.ca.gov/pdf/checklist-communications.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C175" t="str">
-        <v>https://covid19.ca.gov/healthcorps/</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D175" t="str">
         <v xml:space="preserve"> </v>
@@ -4932,13 +4932,13 @@
     </row>
     <row r="176">
       <c r="A176" t="str">
-        <v>When can I expect to hear a response after completing my California Health Corps registration?</v>
+        <v>Construction</v>
       </c>
       <c r="B176" t="str">
-        <v>Currently we anticipate the process may take up to two weeks, since an incredible number of responses are received and need to prioritize certain parts of the state, where the needs are the greatest. We will begin to contact the volunteers after verification of credentials, and based on current and anticipated needs.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>Follow this [guidance for the construction industry](https://files.covid19.ca.gov/pdf/guidance-construction--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the construction industry](https://files.covid19.ca.gov/pdf/checklist-construction.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C176" t="str">
-        <v>https://covid19.ca.gov/healthcorps/</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D176" t="str">
         <v xml:space="preserve"> </v>
@@ -4958,13 +4958,13 @@
     </row>
     <row r="177">
       <c r="A177" t="str">
-        <v>How do I return to the California Health Corps application after logging out?</v>
+        <v>Day camps</v>
       </c>
       <c r="B177" t="str">
-        <v>Visit [https://healthcarevolunteers.ca.gov/](https://healthcarevolunteers.ca.gov/) and use the account you created while applying to correct or update any information you want.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>Follow this [guidance for day camps](https://files.covid19.ca.gov/pdf/guidance-day-camps--en.pdf) to create a plan for safe re-opening. Implementation of these guidelines should be tailored for each setting. Implementation requires training and support for staff and adequate consideration of camper and family needs. All decisions about following these recommendations should be made in collaboration with local health officials and other authorities, and should depend on the levels of COVID-19 community transmission and the capacities of the local public health and healthcare systems, among other relevant factors. \n\nReview the guidance, prepare a plan, and post the [checklist for day camps](https://files.covid19.ca.gov/pdf/checklist-daycamps--en.pdf) in your facility to show employees, campers, and families that you’ve reduced the risk and are open for operation.\n\nCohorts of kids and adults in controlled, supervised settings\n\nA **cohort** is a stable group of no more than 14 children or youth and no more than two supervising adults in a supervised environment. The group stays together for all activities, including meals and recreation. And this group avoids contact with anyone not in their group.\n\nDay camp operators must follow the [guidance for cohorts of children](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/small-groups-child-youth.aspx) and youth in controlled, supervised and indoor environments. See the answers to [frequently asked questions](https://files.covid19.ca.gov/pdf/guidance-schools-cohort-FAQ.pdf) about cohort guidance.\n\nKids and adults in supervised care environments must be in groups as small as possible. Kids and supervising adults in one group must not physically interact with:\n\n*   kids and supervising adults in other groups\n*   other facility staff\n*   parents of kids in other groups\n\nPracticing a cohort structure\n\n*   decreases opportunities for exposure to or transmission of the virus\n*   facilitates more efficient contact tracing in the event of a positive case\n*   allows for targeted testing, quarantine, and isolation of a single group instead of an entire population of kids and supervising adults\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C177" t="str">
-        <v>https://covid19.ca.gov/healthcorps/</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D177" t="str">
         <v xml:space="preserve"> </v>
@@ -4984,13 +4984,13 @@
     </row>
     <row r="178">
       <c r="A178" t="str">
-        <v>Resources for the California Health Corps participants</v>
+        <v>Delivery services</v>
       </c>
       <c r="B178" t="str">
-        <v>*   Health Corps FAQ: [FAQ-Health-Corps (PDF)](https://files.covid19.ca.gov/pdf/FAQ-Health-Corps.pdf)\n*   Travel Reimbursement FAQ: [FAQ-Travel-Reimbursement (PDF)](https://files.covid19.ca.gov/pdf/FAQ-Travel-Reimbursement.pdf)\n*   SNF Orientation: [SNF-Nursing-Staff-Orientation (PDF)](https://files.covid19.ca.gov/pdf/SNF-Nursing-Staff-Orientation.pdf)\n*   How to file a complaint: [How-to-file-a-complaint (PDF)](https://files.covid19.ca.gov/pdf/How-to-file-a-complaint.pdf)\n*   Direct deposit: [std699-Direct-Deposit (PDF)](https://files.covid19.ca.gov/pdf/std699-Direct-Deposit.pdf)\n*   Travel expense claim: [Std262-Travel-Expense-Claim (PDF)](https://files.covid19.ca.gov/pdf/Std262-Travel-Expense-Claim.pdf)\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>Follow this [guidance for the delivery services industry](https://files.covid19.ca.gov/pdf/guidance-delivery-services--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the delivery services industry](https://files.covid19.ca.gov/pdf/checklist-delivery-services.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C178" t="str">
-        <v>https://covid19.ca.gov/healthcorps/</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D178" t="str">
         <v xml:space="preserve"> </v>
@@ -5010,13 +5010,13 @@
     </row>
     <row r="179">
       <c r="A179" t="str">
-        <v>Can a doctor with out of state Licence or foreign medical graduate without California license work for the California Health Corps?</v>
+        <v>Energy and utilities</v>
       </c>
       <c r="B179" t="str">
-        <v>To be eligible for COVID-19 emergency medical staffing roles, you must:\n\n*   Have a valid California License for clinical practice (if you are a MD, DO, etc.) \n*   **OR** are a medical resident or nursing student \n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>Follow this [guidance for the energy and utilities industry](https://files.covid19.ca.gov/pdf/guidance-energy--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the energy and utilities industry](https://files.covid19.ca.gov/pdf/checklist-energy.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C179" t="str">
-        <v>https://covid19.ca.gov/healthcorps/</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D179" t="str">
         <v xml:space="preserve"> </v>
@@ -5036,10 +5036,10 @@
     </row>
     <row r="180">
       <c r="A180" t="str">
-        <v>Agriculture and livestock</v>
+        <v>Family friendly practices for employers</v>
       </c>
       <c r="B180" t="str">
-        <v>The [guidance for the agriculture and livestock industry](https://files.covid19.ca.gov/pdf/guidance-agriculture--en.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the agriculture and livestock industry](https://files.covid19.ca.gov/pdf/checklist-agriculture.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for family friendly practices for employers](https://files.covid19.ca.gov/pdf/guidance-family-friendly-practices-employers--en.pdf) to keep employees safe and be responsive to their needs in order to ensure continued productivity. As workplaces reopen, employees will require both child care supports and workplace flexibility. Work-life balance policies will become even more important and continued investment in family-friendly workplace policies by employers is critical.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C180" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5062,10 +5062,10 @@
     </row>
     <row r="181">
       <c r="A181" t="str">
-        <v>Auto dealerships</v>
+        <v>Food packing</v>
       </c>
       <c r="B181" t="str">
-        <v>The [guidance for the automobile dealerships and rental operators industry](https://files.covid19.ca.gov/pdf/guidance-auto-dealerships--en.pdf) provides guidelines to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for the automobile dealerships and rental operators](https://files.covid19.ca.gov/pdf/checklist-auto-dealerships.pdf) industry in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for facilities that process or pack meat, dairy, or produce](https://files.covid19.ca.gov/pdf/guidance-food-packing--en.pdf) to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for facilities that process or pack meat, dairy or produce](https://files.covid19.ca.gov/pdf/checklist-food-packing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C181" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5088,10 +5088,10 @@
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>Childcare</v>
+        <v>Gyms and fitness centers</v>
       </c>
       <c r="B182" t="str">
-        <v>All childcare facilities can open with necessary modifications. The updated [guidance for the childcare industry](https://files.covid19.ca.gov/pdf/guidance-childcare--en.pdf) provides guidelines to minimize the spread of COVID-19 and ensure the safety of children, providers, and families. As programs begin to reopen and other programs transition from emergency childcare for essential workers to enhanced regular operations, all providers must apply new and updated policies and requirements and must update their emergency preparedness plan.\n\nReview the guidance, prepare a plan, and post the [checklist for childcare](https://files.covid19.ca.gov/pdf/checklist-childcare--en.pdf) in your facility to show employees and families that you’ve reduced the risk and are open for operation.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple):\n\n*   Outdoor only with modifications\n*   Saunas and steam rooms must close\n\nSubstantial (red): \n\n*   Indoor with modifications\n*   Capacity must be limited to 10%\n\nModerate (orange)\n\n*   Indoor with modifications\n*   Capacity must be limited to 25%\n*   Indoor pools can open\n\nMinimal (yellow)\n\n*   Indoor with modifications\n*   Capacity must be limited to 50%\n*   Indoor pools can open\n*   Saunas, spas, and steam rooms can open\n\nFollow this [guidance for gyms and fitness centers](https://files.covid19.ca.gov/pdf/guidance-fitness--en.pdf), including yoga and dance studios, to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for gyms and fitness centers](https://files.covid19.ca.gov/pdf/checklist-fitness.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C182" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5114,10 +5114,10 @@
     </row>
     <row r="183">
       <c r="A183" t="str">
-        <v>Communications infrastructure</v>
+        <v>Hair salons and barbershops</v>
       </c>
       <c r="B183" t="str">
-        <v>The [guidance for the communications infrastructure industry](https://files.covid19.ca.gov/pdf/guidance-communications--en.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the communications infrastructure industry](https://files.covid19.ca.gov/pdf/checklist-communications.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for hair salons and barbershops](https://files.covid19.ca.gov/pdf/guidance-hair-salons--en.pdf) to create a safer environment for workers and customers. Review the guidance, prepare a plan, and post the [checklist for hair salons](https://files.covid19.ca.gov/pdf/checklist-hair-salons.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C183" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5140,10 +5140,10 @@
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>Construction</v>
+        <v>Higher education</v>
       </c>
       <c r="B184" t="str">
-        <v>This [guidance for the construction industry](https://files.covid19.ca.gov/pdf/guidance-construction--en.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the construction industry](https://files.covid19.ca.gov/pdf/checklist-construction.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple):\n\n*   Closed for in-person instruction\n\nSubstantial (red):\n\n*   Open for in-person instruction once the county has been this tier for at least two weeks\n\nModerate (orange): Open with modifications\n\nMinimal (yellow): Open with modifications\n\nThis interim [guidance for institutions of higher education](https://files.covid19.ca.gov/pdf/guidance-higher-education--en.pdf) provides guidelines to help institutions and their communities plan and prepare to resume in-person instruction. Review the guidance and prepare a plan to reduce the risk and support a safer environment for students, faculty, workers, and families.\n\nCohorts of youth and adults in controlled, supervised settings\n\nA **cohort** is a stable group of no more than 14 youth and no more than two supervising adults in a supervised environment. The group stays together for all activities, including meals and recreation. And this group avoids contact with anyone not in their group.\n\nFollow the [guidance for cohorts of children](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/small-groups-child-youth.aspx) and youth in controlled, supervised and indoor environments operated by local educational agencies, nonprofits, or other authorized providers. These environments include, but are not limited to, the following:\n\n*   public and private schools\n*   organized and supervised environments, like “distance learning hubs”\n*   recreation programs\n*   before and after school programs\n*   youth groups\n\nSee the answers to [frequently asked questions](https://files.covid19.ca.gov/pdf/guidance-schools-cohort-FAQ.pdf) about cohort guidance.\n\nYouth and adults in supervised environments must be in groups as small as possible. Youth and supervising adults in one group must not physically interact with:\n\n*   youth and supervising adults in other groups\n*   other facility staff\n*   parents of youth in other groups\n\nPracticing a cohort structure:\n\n*   decreases opportunities for exposure to or transmission of the virus\n*   facilitates more efficient contact tracing in the event of a positive case\n*   allows for targeted testing, quarantine, and isolation of a single group instead of an entire population of youth and supervising adults\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C184" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5166,10 +5166,10 @@
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>Day camps</v>
+        <v>Hotels, lodging, and short term rentals</v>
       </c>
       <c r="B185" t="str">
-        <v>The updated [guidance for day camps](https://files.covid19.ca.gov/pdf/guidance-day-camps--en.pdf) provides guidelines to create a plan for safe re-opening. Implementation of these guidelines should be tailored for each setting. Implementation requires training and support for staff and adequate consideration of camper and family needs. All decisions about following these recommendations should be made in collaboration with local health officials and other authorities, and should depend on the levels of COVID-19 community transmission and the capacities of the local public health and healthcare systems, among other relevant factors.\n\nReview the guidance, prepare a plan, and post the [checklist for day camps](https://files.covid19.ca.gov/pdf/checklist-daycamps--en.pdf) in your facility to show employees, campers, and families that you’ve reduced the risk and are open for operation.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple): \n\n*   Open with modifications\n*   Fitness centers can be open outdoors only with modifications\n*   Saunas and steam rooms must close\n\nSubstantial (red): \n\n*   Open with modifications\n*   Fitness centers can open to 10% capacity\n\nModerate (orange)\n\n*   Open with modifications\n*   Fitness centers can open to 25% capacity\n*   Indoor pools can open\n\nMinimal (yellow)\n\n*   Open with modifications\n*   Fitness centers can open to 50% capacity\n*   Indoor pools can open\n*   Spa facilities can open\n\nHotels and lodging\n\n*   Follow this [guidance for hotels and lodging](https://files.covid19.ca.gov/pdf/guidance-hotels--en.pdf) to create a safer environment for workers and customers.\n\nHotels, lodging, and short term rentals\n\n*   Follow this [guidance for hotels and short term rentals](https://files.covid19.ca.gov/pdf/guidance-hotels-lodging-rentals--en.pdf) for tourism and individual travel to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for hotels, lodging, and short-term rentals](https://files.covid19.ca.gov/pdf/checklist-hotels.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C185" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5192,10 +5192,10 @@
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>Delivery services</v>
+        <v>Life sciences</v>
       </c>
       <c r="B186" t="str">
-        <v>The [guidance for the delivery services industry](https://files.covid19.ca.gov/pdf/guidance-delivery-services--en.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the delivery services industry](https://files.covid19.ca.gov/pdf/checklist-delivery-services.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for the life sciences industry](https://files.covid19.ca.gov/pdf/guidance-life-sciences--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the life sciences industry](https://files.covid19.ca.gov/pdf/checklist-life-sciences.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C186" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5218,10 +5218,10 @@
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>Energy and utilities</v>
+        <v>Limited services</v>
       </c>
       <c r="B187" t="str">
-        <v>The [guidance for the energy and utilities industry](https://files.covid19.ca.gov/pdf/guidance-energy--en.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the energy and utilities industry](https://files.covid19.ca.gov/pdf/checklist-energy.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Limited Services are defined as those which do not generally require close contact. Follow this [guidance for Limited Services](https://files.covid19.ca.gov/pdf/guidance-limited-services--en.pdf) to create a safer environment for workers and patrons.\n\nFaith-based counseling can reopen within the following parameters:\n\n1.  Counseling services are permissible in-person where the service cannot reasonably be practiced remotely;\n2.  Counseling services should adopt state guidance on Limited Services, where applicable;\n3.  This designation does not permit gatherings beyond counseling to members of a single household.\n\nReview the guidance, prepare a plan, and post the [checklist for Limited Services](https://files.covid19.ca.gov/pdf/checklist-limited-services.pdf) in your workplace to show clients and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)&lt;!-- laundromat, dry cleaner, laundry, auto repair, car wash, landscaper, door to door, sales, pet groom, dog walk, entry to private residences, community 2 facilities, residential, janitorial, cleaning services, house keep, house clean, HVAC, appliance repair, electrician, plumbers, mechanical trade, handyperson, handyman, general contractors, lessees, subcontractors --&gt;</v>
       </c>
       <c r="C187" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5244,10 +5244,10 @@
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>Family friendly practices for employers</v>
+        <v>Logistics and warehousing facilities</v>
       </c>
       <c r="B188" t="str">
-        <v>The [guidance for family friendly practices for employers](https://files.covid19.ca.gov/pdf/guidance-family-friendly-practices-employers--en.pdf) provides guidelines for family-friendly practices to keep employees safe and be responsive to their needs in order to ensure continued productivity. As workplaces reopen, employees will require both child care supports and workplace flexibility. Work-life balance policies will become even more important and continued investment in family-friendly workplace policies by employers is critical.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for businesses operating in the logistics/warehousing industry](https://files.covid19.ca.gov/pdf/guidance-logistics-warehousing--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post  the [checklist for the logistics/warehousing industry](https://files.covid19.ca.gov/pdf/checklist-logistics-warehousing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C188" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5270,10 +5270,10 @@
     </row>
     <row r="189">
       <c r="A189" t="str">
-        <v>Food packing</v>
+        <v>Manufacturing</v>
       </c>
       <c r="B189" t="str">
-        <v>The [guidance for facilities that process or pack meat, dairy, or produce](https://files.covid19.ca.gov/pdf/guidance-food-packing--en.pdf) provides guidelines to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for facilities that process or pack meat, dairy or produce](https://files.covid19.ca.gov/pdf/checklist-food-packing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for the manufacturing industry](https://files.covid19.ca.gov/pdf/guidance-manufacturing--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the manufacturing industry](https://files.covid19.ca.gov/pdf/checklist-manufacturing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C189" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5296,10 +5296,10 @@
     </row>
     <row r="190">
       <c r="A190" t="str">
-        <v>Higher education – NEW</v>
+        <v>Mining and logging</v>
       </c>
       <c r="B190" t="str">
-        <v>This interim [guidance for institutions of higher education](https://files.covid19.ca.gov/pdf/guidance-higher-education--en.pdf) provides guidelines to help institutions and their communities plan and prepare to resume in-person instruction.\n\n**For counties on the** [**Monitoring List**](https://covid19.ca.gov/roadmap-counties/#affected-counties)**:**\n\n**Indoor** operations must be closed.\n\nReview the guidance and prepare a plan to reduce the risk and support a safer environment for students, faculty, workers, and families.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for the mining and logging industries](https://files.covid19.ca.gov/pdf/guidance-mining-logging--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the mining and logging industries](https://files.covid19.ca.gov/pdf/checklist-mining-logging.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C190" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5322,10 +5322,10 @@
     </row>
     <row r="191">
       <c r="A191" t="str">
-        <v>Hotels and lodging</v>
+        <v>Movie theaters and family entertainment centers</v>
       </c>
       <c r="B191" t="str">
-        <v>Unless your county has been approved to move further in the reopening roadmap, hotels should only open for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or providing housing solutions, including measures to protect homeless populations. Follow this [guidance for hotels and lodging](https://files.covid19.ca.gov/pdf/guidance-hotels--en.pdf) to create a safer environment for workers and customers.\n\n[Counties that have approval](https://covid19.ca.gov/roadmap-counties/) to move further can reopen hotels, lodging, and short-term rentals for tourism and individual travel. Follow this [guidance for hotels and short term rentals](https://files.covid19.ca.gov/pdf/guidance-hotels-lodging-rentals--en.pdf) for tourism and individual travel to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for hotels, lodging, and short-term rentals](https://files.covid19.ca.gov/pdf/checklist-hotels.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple)\n\n*   Movie theaters: Outdoor only with modifications\n*   Family entertainment centers: Outdoor only with modifications for activities like kart racing, mini golf, batting cages\n\nSubstantial (red)\n\n*   Movie theaters: \n    *   Indoor with modifications\n    *   Capacity must be limited to 25% or 100 people, whichever is less\n*   Family entertainment centers: Outdoor only with modifications for activities like kart racing, mini golf, batting cages\n\nModerate (orange)\n\n*   Movie theaters: \n    *   Indoor with modifications\n    *   Capacity must be limited to 50% or 200 people, whichever is less\n*   Family entertainment centers: \n    *   Outdoor with modifications for activities like kart racing, mini golf, batting cages\n    *   Indoor with modifications for naturally distanced activities, like bowling alleys and climbing walls\n    *   Capacity must be limited to 25%\n\nMinimal (yellow)\n\n*   Movie theaters: \n    *   Indoor with modifications\n    *   Capacity must be limited to 50%\n*   Family entertainment centers: \n    *   Outdoor with modifications for activities like kart racing, mini golf, batting cages\n    *   Indoor with modifications for naturally distanced activities, like bowling alleys and climbing walls\n    *   Indoor with modifications for activities with increased risk of proximity and mixing, like arcade games, ice and roller skating, and indoor playgrounds\n    *   Capacity must be limited to 50%\n\nFollow this guidance for [movie theaters and family entertainment centers](https://files.covid19.ca.gov/pdf/guidance-family-entertainment--en.pdf), like bowling alleys, miniature golf, batting cages, and arcades, to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for movie theaters and family entertainment centers](https://files.covid19.ca.gov/pdf/checklist-family-entertainment.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C191" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5348,10 +5348,10 @@
     </row>
     <row r="192">
       <c r="A192" t="str">
-        <v>Life sciences</v>
+        <v>Museums, zoos, and aquariums</v>
       </c>
       <c r="B192" t="str">
-        <v>The [guidance for the life sciences industry](https://files.covid19.ca.gov/pdf/guidance-life-sciences--en.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the life sciences industry](https://files.covid19.ca.gov/pdf/checklist-life-sciences.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple): Outdoor only with modifications\n\nSubstantial (red)\n\n*   Indoor with modifications\n*   Indoor activities must be limited to 25% of capacity\n\nModerate (orange)\n\n*   Indoor with modifications\n*   Indoor activities must be limited to 50% of capacity\n\nMinimal (yellow): Indoor with modifications\n\nOutdoor museums, open air galleries, botanical gardens, and other outdoor exhibition spaces\n\n*   Follow this [guidance for outdoor museums](https://files.covid19.ca.gov/pdf/guidance-outdoor-museums--en.pdf), open air galleries, botanical gardens, and other outdoor exhibition spaces to create a safer environment for workers and patrons. This guidance is not intended for zoos, amusement parks, or indoor gallery and museum spaces.\n*   Review the guidance, prepare a plan, and post the [checklist for outdoor museums](https://files.covid19.ca.gov/pdf/checklist-outdoor-museums.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMuseums, galleries, botanical gardens, zoos, aquariums, and other similar spaces\n\n*   Follow this [guidance for zoos, museums](https://files.covid19.ca.gov/pdf/guidance-zoos-museums--en.pdf), galleries, botanical gardens, and aquariums to create a safer environment for workers and patrons.\n*   Review the guidance, prepare a plan, and post the [checklist for zoos, museums](https://files.covid19.ca.gov/pdf/checklist-zoos-museums.pdf), galleries, and aquariums in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C192" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5374,10 +5374,10 @@
     </row>
     <row r="193">
       <c r="A193" t="str">
-        <v>Limited services</v>
+        <v>Music, film, and TV production</v>
       </c>
       <c r="B193" t="str">
-        <v>Limited Services are defined as those which do not generally require close contact. Follow this [guidance for Limited Services](https://files.covid19.ca.gov/pdf/guidance-limited-services--en.pdf) to create a safer environment for workers and patrons.\n\nFaith-based counseling can reopen within the following parameters:\n\n1.  Counseling services are permissible in-person where the service cannot reasonably be practiced remotely;\n2.  Counseling services should adopt state guidance on Limited Services, where applicable;\n3.  This designation does not permit gatherings beyond counseling to members of a single household.\n\nReview the guidance, prepare a plan, and post the [checklist for Limited Services](https://files.covid19.ca.gov/pdf/checklist-limited-services.pdf) in your workplace to show clients and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)&lt;!-- laundromat, dry cleaner, laundry, auto repair, car wash, landscaper, door to door, sales, pet groom, dog walk, entry to private residences, community 2 facilities, residential, janitorial, cleaning services, house keep, house clean, HVAC, appliance repair, electrician, plumbers, mechanical trade, handyperson, handyman, general contractors, lessees, subcontractors --&gt;</v>
+        <v>Music, TV, and film production may resume, subject to approval by county public health officers.  \n  \nTo reduce the risk of COVID-19 transmission, productions, cast, crew and other industry workers should abide by safety protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should follow the [guidance for office workspaces](https://files.covid19.ca.gov/pdf/guidance-office-workspaces--en.pdf).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C193" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5400,10 +5400,10 @@
     </row>
     <row r="194">
       <c r="A194" t="str">
-        <v>Logistics and warehousing facilities</v>
+        <v>Office workspaces</v>
       </c>
       <c r="B194" t="str">
-        <v>The [guidance for businesses operating in the logistics/warehousing industry](https://files.covid19.ca.gov/pdf/guidance-logistics-warehousing--en.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post  the [checklist for the logistics/warehousing industry](https://files.covid19.ca.gov/pdf/checklist-logistics-warehousing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple): Remote work\n\nSubstantial (red): Remote work\n\nModerate (orange): Indoor with modifications, encourage telework\n\nMinimal (yellow): Indoor with modifications, encourage telework\n\nFollow this [guidance for office workspaces](https://files.covid19.ca.gov/pdf/guidance-office-workspaces--en.pdf) to create a safer environment for workers.\n\nFaith-based office workspaces can reopen within the following parameters:\n\n1.  Faith-based facilities are considered “offices” only for those employed by the organization and where the facility is their regular place of work.\n2.  The employer should implement state guidance relating to offices before reopening the facility for employees.\n3.  This designation does not permit gatherings of non-employees, such as the organization’s congregation.\n\nReview the guidance, prepare a plan, and post the [checklist for office workspaces](https://files.covid19.ca.gov/pdf/checklist-office-workspaces.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C194" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5426,10 +5426,10 @@
     </row>
     <row r="195">
       <c r="A195" t="str">
-        <v>Manufacturing</v>
+        <v>Personal care services</v>
       </c>
       <c r="B195" t="str">
-        <v>The [guidance for the manufacturing industry](https://files.covid19.ca.gov/pdf/guidance-manufacturing--en.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the manufacturing industry](https://files.covid19.ca.gov/pdf/checklist-manufacturing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple): \n\n*   Outdoor only with modifications\n*   Tattooing, piercing, and electrolysis must close\n\nSubstantial (red): Indoor with modifications\n\nModerate (orange): Indoor with modifications\n\nMinimal (yellow): Indoor with modifications\n\nPersonal care services provided indoors\n\n*   Follow this [guidance for personal care services](https://files.covid19.ca.gov/pdf/guidance-expanded-personal-care-services--en.pdf) like nail salons, tattoo parlors, and body waxing to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for personal care services](https://files.covid19.ca.gov/pdf/checklist-expanded-personal-care-services.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nPersonal care services provided outdoors\n\n*   Follow this [guidance for personal care services provided outdoors](https://files.covid19.ca.gov/pdf/guidance-outdoor-personal-care--en.pdf) to support an outdoor safe, clean environment for workers and patrons. This guidance applies to services that require touching a client’s face, like facials and waxing. This guidance also applies to esthetic services, skin care, cosmetology, nail services, and massage therapy. Review the guidance, prepare a plan, and post the [checklist for personal care services provided outdoors](https://files.covid19.ca.gov/pdf/checklist-outdoor-personal-care--en.pdf) at your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C195" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5452,10 +5452,10 @@
     </row>
     <row r="196">
       <c r="A196" t="str">
-        <v>Mining and logging</v>
+        <v>Places of worship and cultural ceremonies</v>
       </c>
       <c r="B196" t="str">
-        <v>The [guidance for the mining and logging industries](https://files.covid19.ca.gov/pdf/guidance-mining-logging--en.pdf) provides guidelines to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the mining and logging industries](https://files.covid19.ca.gov/pdf/checklist-mining-logging.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple): Outdoor only with modifications\n\nSubstantial (red)\n\n*   Indoor with modifications\n*   Indoor activities must be limited to 25% of capacity or 100 people, whichever is less\n\nModerate (orange)\n\n*   Indoor with modifications\n*   Indoor activities must be limited to 50% of capacity or 200 people, whichever is less\n\nMinimal (yellow)\n\n*   Indoor with modifications\n*   Indoor activities must be limited to 50% of capacity\n\nFollow this [guidance for places of worship](https://files.covid19.ca.gov/pdf/guidance-places-of-worship--en.pdf) and providers of religious services and cultural ceremonies, like weddings and funerals, to create a safer environment for workers and visitors.\n\nReview the guidance, prepare a plan, and post the [checklist for places of worship](https://files.covid19.ca.gov/pdf/checklist-places-of-worship.pdf) and cultural ceremonies in your workplace to show workers and visitors that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C196" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5478,10 +5478,10 @@
     </row>
     <row r="197">
       <c r="A197" t="str">
-        <v>Music, film, and TV production</v>
+        <v>Ports</v>
       </c>
       <c r="B197" t="str">
-        <v>Music, TV, and film production may resume, subject to approval by county public health officers. They will review local epidemiological data, including cases per 100,000 people, rate of test positivity, local preparedness to support a health care surge, vulnerable populations, contact tracing and testing.  \n  \nTo reduce the risk of COVID-19 transmission, productions, cast, crew and other industry workers should abide by safety protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should follow the [guidance for office workspaces](https://files.covid19.ca.gov/pdf/guidance-office-workspaces--en.pdf).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for the port industry](https://files.covid19.ca.gov/pdf/guidance-ports--en.pdf) to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for the port industry](https://files.covid19.ca.gov/pdf/checklist-ports.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C197" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5504,10 +5504,10 @@
     </row>
     <row r="198">
       <c r="A198" t="str">
-        <v>Office workspaces</v>
+        <v>Professional sports (without live audiences)</v>
       </c>
       <c r="B198" t="str">
-        <v>Follow this [guidance for office workspaces](https://files.covid19.ca.gov/pdf/guidance-office-workspaces--en.pdf) to create a safer environment for workers.\n\nFaith-based office workspaces can reopen within the following parameters:\n\n1.  Faith-based facilities are considered “offices” only for those employed by the organization and where the facility is their regular place of work.\n2.  The employer should implement state guidance relating to offices before reopening the facility for employees.\n3.  This designation does not permit gatherings of non-employees, such as the organization’s congregation.\n\n**For counties on the** [**Monitoring List**](https://covid19.ca.gov/roadmap-counties/#affected-counties)**:**\n\n**Indoor** operations of offices for non-essential non-critical infrastructure must be closed. \n\nReview the guidance, prepare a plan, and post the [checklist for office workspaces](https://files.covid19.ca.gov/pdf/checklist-office-workspaces.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Professional sports may resume training and competition without live audiences, subject to approval by county public health officers. This guidance does not apply to semi-professional, amateur, or recreational sports.  \n  \nTo reduce the risk of COVID-19 transmission, athletes, coaching staff, medical staff, broadcasting staff and others at sporting facilities or events should abide by COVID-19 protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should follow the [guidance for office workspaces](https://files.covid19.ca.gov/pdf/guidance-office-workspaces--en.pdf).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C198" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5530,10 +5530,10 @@
     </row>
     <row r="199">
       <c r="A199" t="str">
-        <v>Outdoor museums</v>
+        <v>Public transit and intercity passenger rail</v>
       </c>
       <c r="B199" t="str">
-        <v>Follow this [guidance for outdoor museums](https://files.covid19.ca.gov/pdf/guidance-outdoor-museums--en.pdf), open air galleries, botanical gardens, and other outdoor exhibition spaces to create a safer environment for workers and patrons. This guidance is not intended for zoos, amusement parks, or indoor gallery and museum spaces.\n\nReview the guidance, prepare a plan, and post the [checklist for outdoor museums](https://files.covid19.ca.gov/pdf/checklist-outdoor-museums.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for public transit agencies](https://files.covid19.ca.gov/pdf/guidance-transit-rail--en.pdf) to create a safer environment for workers and customers.\n\nReview the guidance, prepare a plan, and post the [checklist for public transit agencies](https://files.covid19.ca.gov/pdf/checklist-transit-rail.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C199" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5556,10 +5556,10 @@
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>Places of worship and cultural ceremonies</v>
+        <v>Real estate transaction</v>
       </c>
       <c r="B200" t="str">
-        <v>This [guidance for places of worship](https://files.covid19.ca.gov/pdf/guidance-places-of-worship--en.pdf) and providers of religious services and cultural ceremonies, like weddings and funerals, provides guidelines to create a safer environment for workers and visitors.\n\n**For counties on the** [**Monitoring List**](https://covid19.ca.gov/roadmap-counties/#affected-counties)**:**\n\n**Indoor** operations must be closed. \n\nReview the guidance, prepare a plan, and post the [checklist for places of worship](https://files.covid19.ca.gov/pdf/checklist-places-of-worship.pdf) and cultural ceremonies in your workplace to show workers and visitors that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for businesses operating in the real estate industry](https://files.covid19.ca.gov/pdf/guidance-real-estate--en.pdf) to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for the real estate industry](https://files.covid19.ca.gov/pdf/checklist-real-estate.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C200" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5582,10 +5582,10 @@
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>Ports</v>
+        <v>Restaurants, wineries, and bars</v>
       </c>
       <c r="B201" t="str">
-        <v>This [guidance for the port industry](https://files.covid19.ca.gov/pdf/guidance-ports--en.pdf) provides guidelines to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for the port industry](https://files.covid19.ca.gov/pdf/checklist-ports.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple)\n\n*   Restaurants and wineries: Outdoor only with modifications\n*   Bars, breweries, and distilleries: Closed\n\nSubstantial (red)\n\n*   Restaurants: \n    *   Indoor with modifications\n    *   Capacity must be limited to 25% or 100 people, whichever is less\n*   Wineries: Outdoor only with modifications\n*   Bars, breweries, and distilleries: Closed\n\nModerate (orange)\n\n*   Restaurants: \n    *   Indoor with modifications\n    *   Capacity must be limited to 50% or 200 people, whichever is less\n*   Wineries:\n    *   Indoor with modifications\n    *   Capacity must be limited to 25% or 100 people, whichever is less\n*   Bars, breweries, and distilleries: Outdoor only with modifications\n\nMinimal (yellow)\n\n*   Restaurants: \n    *   Indoor with modifications\n    *   Capacity must be limited to 50%\n*   Wineries:\n    *   Indoor with modifications\n    *   Capacity must be limited to 50% or 200 people, whichever is less\n*   Bars, breweries, and distilleries: \n    *   Indoor with modifications\n    *   Capacity must be limited to 50%\n\nTake-out restaurants\n\n*   Follow this [guidance for restaurants providing take-out, drive-through, and delivery](https://files.covid19.ca.gov/pdf/guidance-take-out-restaurants--en.pdf) to create a safer environment for workers and patrons.\n*   Review the guidance and prepare a plan for your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nOutdoor dining\n\n*   Follow this [guidance for restaurants providing outdoor dining, take-out, drive-through, and delivery](https://files.covid19.ca.gov/pdf/guidance-outdoor-restaurants--en.pdf) to create a safer environment for workers and patrons.\n*   Review the guidance and prepare a plan for your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nRestaurants, wineries, and bars\n\n*   Follow this [guidance for restaurants, wineries, and bars](https://files.covid19.ca.gov/pdf/guidance-restaurants-bars-wineries--en.pdf) to create a safer environment for workers and patrons.\n*   Review the guidance, prepare a plan, and post the [checklist for restaurants, wineries, and bars](https://files.covid19.ca.gov/pdf/checklist-restaurants-bars.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business. \n\nDine-in restaurants\n\n*   Follow this [guidance for dine-in restaurants](https://files.covid19.ca.gov/pdf/guidance-dine-in-restaurants--en.pdf) to create a safer environment for workers and customers.\n*   Review the guidance, prepare a plan, and post the [checklist for dine-in restaurants](https://files.covid19.ca.gov/pdf/checklist-dine-in-restaurants.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C201" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5608,10 +5608,10 @@
     </row>
     <row r="202">
       <c r="A202" t="str">
-        <v>Professional sports (without live audiences)</v>
+        <v>Retail</v>
       </c>
       <c r="B202" t="str">
-        <v>Professional sports may resume training and competition without live audiences, subject to approval by county public health officers. They will review local epidemiological data, including cases per 100,000 people, rate of test positivity, local preparedness to support a health care surge, vulnerable populations, contact tracing and testing.  \n  \nTo reduce the risk of COVID-19 transmission, athletes, coaching staff, medical staff, broadcasting staff and others at sporting facilities or events should abide by COVID-19 protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should follow the [guidance for office workspaces](https://files.covid19.ca.gov/pdf/guidance-office-workspaces--en.pdf).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple)\n\n*   Open with modifications\n*   Retail capacity must be limited to 25%\n*   Grocery store capacity must be limited to 50%\n\nSubstantial (red)\n\n*   Open with modifications\n*   Retail capacity must be limited to 50%\n\nModerate (orange): Indoor with modifications\n\nMinimal (yellow): Indoor with modifications\n\nFollow this [guidance for retailers](https://files.covid19.ca.gov/pdf/guidance-retail--en.pdf) to create a safer environment for workers and customers. Review the guidance, prepare a plan, and post the [checklist for retail](https://files.covid19.ca.gov/pdf/checklist-retail.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nRetailers and libraries can re-open, along with the manufacturing and logistics sectors that support retail.  \n  \nLibraries should follow the [guidance for retailers](https://files.covid19.ca.gov/pdf/guidance-retail--en.pdf). The State Library has also released guidance for the [re-opening of libraries for in-person services](https://library.ca.gov/Content/pdf/services/toLibraries/COVIDGuidanceLibraries.pdf). See the [State Library’s COVID-19 website](https://www.library.ca.gov/covid-19) for more information. Find [resources for public libraries](https://www.cla-net.org/page/7-1) by the California Library Association and the State Library.  \n  \nDrive-in and movie theaters can re-open with additional considerations.\n\nRetail doesn’t include personal services such as beauty salons, but does include the sale of goods such as:\n\n*   Bookstores\n*   Jewelry stores\n*   Toy stores\n*   Clothing and shoe stores\n*   Home and furnishing stores\n*   Sporting goods stores\n*   Florists\n\nRetail stores identified in the [essential workforce list](https://covid19.ca.gov/essential-workforce/) can open for in-store shopping. They include:\n\n*   Retail facilities specializing in medical goods and supplies\n*   Grocery stores, pharmacies, convenience stores, and other retail that sells food or beverage products, and animal/pet food\n*   Fuel centers such as gas stations and truck stops\n*   Hardware and building materials stores, consumer electronics, technology and appliances retail\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C202" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5634,10 +5634,10 @@
     </row>
     <row r="203">
       <c r="A203" t="str">
-        <v>Public transit and intercity passenger rail</v>
+        <v>Schools</v>
       </c>
       <c r="B203" t="str">
-        <v>This [guidance for public transit agencies](https://files.covid19.ca.gov/pdf/guidance-transit-rail--en.pdf) provides guidelines to create a safer environment for workers and customers.\n\nReview the guidance, prepare a plan, and post the [checklist for public transit agencies](https://files.covid19.ca.gov/pdf/checklist-transit-rail.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple):\n\n*   Closed for in-person instruction\n\nSubstantial (red):\n\n*   Closed for in-person instruction\n*   Can open in-person instruction if county remains in this tier for two weeks\n\nModerate (orange): \n\n*   Can open in-person instruction\n\nMinimal (yellow): \n\n*   Can open for in-person instruction\n\nFind information for [your school district](https://www.cde.ca.gov/schooldirectory).\n\nFollow this [guidance for schools and school-based programs](https://files.covid19.ca.gov/pdf/guidance-schools--en.pdf) to create a safer environment for your students, families, and staff. This guidance applies to in-person learning and distance learning. Review the guidance, prepare a plan, and post the [checklist for schools](https://files.covid19.ca.gov/pdf/checklist-schools--en.pdf) in your facility to show students, families, and staff that you’ve taken steps to mitigate COVID-19 spread.\n\n*   Guidelines for sports and extracurricular activities consistent with the [California Interscholastic Federation statement](https://cifstate.org/mediacenter/releases/2019-20/PR-34_7.20.20_CIF_Statement_2020-21_Sports_Calendar_Final.pdf) are included. \n*   Check the answers to [frequently asked questions](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Schools-FAQ.aspx) related to schools. \n*   Find all details in the [COVID-19 and Reopening In-Person Learning Framework for K-12 Schools (PDF)](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Schools%20Reopening%20Recommendations.pdf). \n\nCohorts of kids and adults in controlled, supervised settings\n\nA **cohort** is a stable group of no more than 14 children or youth and no more than two supervising adults in a supervised environment. The group stays together for all activities, including meals and recreation. And this group avoids contact with anyone not in their group.\n\nFollow the [guidance for cohorts of children](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/small-groups-child-youth.aspx) and youth in controlled, supervised and indoor environments. These environments include, but are not limited to, the following:\n\n*   public and private schools\n*   licensed and license-exempt child care settings \n*   organized and supervised care environments, like “distance learning hubs”\n*   recreation programs\n*   before and after school programs\n*   youth groups\n*   day camps\n\nSee the answers to [frequently asked questions](https://files.covid19.ca.gov/pdf/guidance-schools-cohort-FAQ.pdf) about cohort guidance. \n\nKids and adults in supervised care environments must be in groups as small as possible. Kids and supervising adults in one group must not physically interact with:\n\n*   kids and supervising adults in other groups\n*   other facility staff\n*   parents of kids in other groups\n\nPracticing a cohort structure:\n\n*   decreases opportunities for exposure to or transmission of the virus\n*   facilitates more efficient contact tracing in the event of a positive case\n*   allows for targeted testing, quarantine, and isolation of a single group instead of an entire population of kids and supervising adults\n\nElementary education waiver:\n\n*   See the [Waiver Process Overview](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/In-Person-Elementary-Waiver-Process.aspx) for details.\n*   Local health officers will need to submit the [Waiver Notice Form](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/CDPH-Waiver-Notice_8.3.2020.pdf) to CDPH.\n*   Schools seeking a waiver can use the template [Waiver Letter and Cover Form](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Waiver-Letter-Template-Cover-Form_8.3.2020.pdf).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C203" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5660,10 +5660,10 @@
     </row>
     <row r="204">
       <c r="A204" t="str">
-        <v>Real estate transaction</v>
+        <v>Shopping centers</v>
       </c>
       <c r="B204" t="str">
-        <v>This [guidance for businesses operating in the real estate industry](https://files.covid19.ca.gov/pdf/guidance-real-estate--en.pdf) provides guidelines to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for the real estate industry](https://files.covid19.ca.gov/pdf/checklist-real-estate.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple):\n\n*   Open with modifications\n*   Indoor capacity must be limited to 25% for shopping malls, destination shopping centers, and swap meets\n*   Closed common areas\n*   Closed food courts\n\nSubstantial (red):\n\n*   Open with modifications\n*   Indoor capacity must be limited to 50% for shopping malls, destination shopping centers, and swap meets\n*   Closed common areas\n*   Reduced capacity food courts (see [restaurants](https://covid19.ca.gov/industry-guidance/#restaurants))\n\nModerate (orange):\n\n*   Open with modifications\n*   Closed common areas\n*   Reduced capacity food courts (see [restaurants](https://covid19.ca.gov/industry-guidance/#restaurants))\n\nMinimal (yellow):\n\n*   Open with modifications\n*   Reduced capacity food courts (see [restaurants](https://covid19.ca.gov/industry-guidance/#restaurants))\n\nFollow this [guidance for shopping centers](https://files.covid19.ca.gov/pdf/guidance-shopping-centers--en.pdf), destination shopping centers, strip and outlet malls, and swap meets to create a safer environment for workers and customers. \n\nReview the guidance, prepare a plan, and post the [checklist for shopping centers](https://files.covid19.ca.gov/pdf/checklist-shopping-centers.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C204" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5686,10 +5686,10 @@
     </row>
     <row r="205">
       <c r="A205" t="str">
-        <v>Retail</v>
+        <v>Support for working families</v>
       </c>
       <c r="B205" t="str">
-        <v>Follow this [guidance for retailers](https://files.covid19.ca.gov/pdf/guidance-retail--en.pdf) to create a safer environment for workers and customers.\n\nReview the guidance, prepare a plan, and post the [checklist for retail](https://files.covid19.ca.gov/pdf/checklist-retail.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nRetailers and libraries can re-open, along with the manufacturing and logistics sectors that support retail.  \n  \nLibraries should follow the [guidance for retailers](https://files.covid19.ca.gov/pdf/guidance-retail--en.pdf). The State Library has also released guidance for the [re-opening of libraries for in-person services](https://library.ca.gov/Content/pdf/services/toLibraries/COVIDGuidanceLibraries.pdf). See the [State Library’s COVID-19 website](https://www.library.ca.gov/covid-19) for more information. Find [resources for public libraries](https://www.cla-net.org/page/7-1) by the California Library Association and the State Library.  \n  \nDrive-in and movie theaters can re-open with additional considerations.\n\nRetail doesn’t include personal services such as beauty salons, but does include the sale of goods such as:\n\n*   Bookstores\n*   Jewelry stores\n*   Toy stores\n*   Clothing and shoe stores\n*   Home and furnishing stores\n*   Sporting goods stores\n*   Florists\n\nRetail stores identified in the [essential workforce list](https://covid19.ca.gov/essential-workforce/) can open for in-store shopping. They include:\n\n*   Retail facilities specializing in medical goods and supplies\n*   Grocery stores, pharmacies, convenience stores, and other retail that sells food or beverage products, and animal/pet food\n*   Fuel centers such as gas stations and truck stops\n*   Hardware and building materials stores, consumer electronics, technology and appliances retail\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>The [support for working families](https://files.covid19.ca.gov/pdf/guidance-support-working-families--en.pdf) guidance provides information to help you locate child care, find assistance to pay for child care, and connect you to additional supports for your family. As stay-at-home orders are lifted for additional industries to promote California’s economic recovery, the need for child care and other supports for working families increases.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C205" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5712,10 +5712,10 @@
     </row>
     <row r="206">
       <c r="A206" t="str">
-        <v>Schools – updated August 3</v>
+        <v>Youth sports</v>
       </c>
       <c r="B206" t="str">
-        <v>Follow this updated [guidance for schools and school-based programs](https://files.covid19.ca.gov/pdf/guidance-schools--en.pdf) to create a safer environment for your students, families, and staff. This guidance applies to in-person learning and distance learning. Guidelines for sports and extracurricular activities consistent with the [California Interscholastic Federation statement](https://cifstate.org/mediacenter/releases/2019-20/PR-34_7.20.20_CIF_Statement_2020-21_Sports_Calendar_Final.pdf) are also included. Check the answers to [frequently asked questions](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Schools-FAQ.aspx) related to schools. Find all details in the [COVID-19 and Reopening In-Person Learning Framework for K-12 Schools (PDF)](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Schools%20Reopening%20Recommendations.pdf).\n\nReview the guidance, prepare a plan, and post the [checklist for schools](https://files.covid19.ca.gov/pdf/checklist-schools--en.pdf) in your facility to show students, families, and staff that you’ve taken steps to mitigate COVID-19 spread.\n\n**Elementary education waiver:**\n\n*   See the [Waiver Process Overview](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/In-Person-Elementary-Waiver-Process.aspx) for details.\n*   Local health officers will need to submit the [Waiver Notice Form](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/CDPH-Waiver-Notice_8.3.2020.pdf) to CDPH.\n*   Schools seeking a waiver can use the template [Waiver Letter and Cover Form](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Waiver-Letter-Template-Cover-Form_8.3.2020.pdf).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for youth sports](https://files.covid19.ca.gov/pdf/guidance-youth-sports--en.pdf) programs, including school-based, club, and recreational programs. Review the guidance and prepare a plan to support a safe environment for players, coaches and trainers, families, spectators, event/program/facility managers, workers, and volunteers. \n\n*   Check the [questions and answers](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Youth-Sports-FAQ.aspx) about youth sports. \n\nCohorts of kids and adults in controlled, supervised settings\n\nA **cohort** is a stable group of no more than 14 children or youth and no more than two supervising adults in a supervised environment. The group stays together for all activities, including meals and recreation. And this group avoids contact with anyone not in their group.\n\nFollow the [guidance for cohorts of children](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/small-groups-child-youth.aspx) and youth in controlled, supervised and indoor environments. These environments include, but are not limited to, the following:\n\n*   public and private schools\n*   licensed and license-exempt child care settings \n*   organized and supervised care environments, like “distance learning hubs”\n*   recreation programs\n*   before and after school programs\n*   youth groups\n*   day camps\n\nSee the answers to [frequently asked questions](https://files.covid19.ca.gov/pdf/guidance-schools-cohort-FAQ.pdf) about cohort guidance. \n\nKids and adults in supervised care environments must be in groups as small as possible. Kids and supervising adults in one group must not physically interact with:\n\n*   kids and supervising adults in other groups\n*   other facility staff\n*   parents of kids in other groups\n\nPracticing a cohort structure\n\n*   decreases opportunities for exposure to or transmission of the virus\n*   facilitates more efficient contact tracing in the event of a positive case\n*   allows for targeted testing, quarantine, and isolation of a single group instead of an entire population of kids and supervising adults\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C206" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5738,13 +5738,13 @@
     </row>
     <row r="207">
       <c r="A207" t="str">
-        <v>Shopping centers</v>
+        <v>Tools for families facing stress</v>
       </c>
       <c r="B207" t="str">
-        <v>Follow this [guidance for shopping centers](https://files.covid19.ca.gov/pdf/guidance-shopping-centers--en.pdf), destination shopping centers, strip and outlet malls, and swap meets to create a safer environment for workers and customers. Interior stores in shopping malls can do curbside pickup with modifications. \n\n**For counties on the** [**Monitoring List**](https://covid19.ca.gov/roadmap-counties/#affected-counties)**:**\n\n**Indoor** operations must be closed. \n\nReview the guidance, prepare a plan, and post the [checklist for shopping centers](https://files.covid19.ca.gov/pdf/checklist-shopping-centers.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>*   [**Noggin’s Navigating the New Normal: Parents Edition**](https://www.noggin.com/navigating-the-new-normal-parents-edition/) (video)  \n    Host Jamie-Lynn Sigler asks Dr. Nadine Burke Harris and other leading experts how to handle the stress of the pandemic on little kids. \n*   [**How to Support Our Kids During COVID-19**](https://podcasts.apple.com/us/podcast/how-to-support-our-kids-during-covid-19-dr-nadine-burke/id1468607534?i=1000470057466) (Apple podcast)  \n    Dr. Burke Harris shares advice on how to talk to your kids about COVID-19, what all of us can do to help, and how to mitigate stress while stuck at home.  \n*   [**FOCUS on the GO!**](https://nfrc.ucla.edu/focus-on-the-go) (app)  \n    Free mobile app designed to help your family enhance existing coping skills and develop new ones through gameplay.\n*   [**Young Children at Home During the COVID-19 Outbreak: The Importance of Self-Care**](https://www.zerotothree.org/resources/3262-young-children-at-home-during-the-covid-19-outbreak-the-importance-of-self-care) (article)  \n    Knowing how to take care of yourself as a caregiver during the COVID-19 outbreak is key to ensure you are most effective in parenting.\n\nMore info: [Manage stress for health](https://covid19.ca.gov/manage-stress-for-health/)</v>
       </c>
       <c r="C207" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/manage-stress-for-health/</v>
       </c>
       <c r="D207" t="str">
         <v xml:space="preserve"> </v>
@@ -5764,13 +5764,13 @@
     </row>
     <row r="208">
       <c r="A208" t="str">
-        <v>Support for working families</v>
+        <v>Tools for parents to help children</v>
       </c>
       <c r="B208" t="str">
-        <v>The [support for working families](https://files.covid19.ca.gov/pdf/guidance-support-working-families--en.pdf) guidance provides information to help you locate child care, find assistance to pay for child care, and connect you to additional supports for your family. As stay-at-home orders are lifted for additional industries to promote California’s economic recovery, the need for child care and other supports for working families increases.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>*   [**California Surgeon General’s Playbook: Stress Relief for Caregivers and Kids During COVID-19**](https://files.covid19.ca.gov/pdf/caregivers_and_kids_california_surgeon_general_stress_busting_playbook_draft_v2_clean_ada_04072020v2.pdf) (PDF)  \n    This guide can help you understand what signs of stress to look out for and what you can do to protect your family’s health. It is also available in [Arabic](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_arabic-2.pdf), Chinese ([Simplified](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_ch_simplified.pdf) and [Traditional](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_zh-hant.pdf)), [Korean](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_korean.pdf), [Spanish](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook-spanish.pdf), [Tagalog](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_tagalog.pdf), and [Vietnamese](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_vi.pdf).\n*   [**Trauma Informed Parent: Helping Adults and Children With Trauma During the Pandemic**](https://www.youtube.com/watch?v=57EAL_e5Nf0) (video)  \n    California’s Surgeon General provides context and tools for how to help kids who have endured past trauma through current stress. \n*   [**Emotional Wellbeing during the COVID-19 Pandemic**](https://www.childtrends.org/publications/resources-for-supporting-childrens-emotional-well-being-during-the-covid-19-pandemic) (guide)  \n    Supporting children’s emotional wellbeing during the COVID-19 pandemic is key to adjusting to a new sense of normal.\n\nMore info: [Manage stress for health](https://covid19.ca.gov/manage-stress-for-health/)</v>
       </c>
       <c r="C208" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/manage-stress-for-health/</v>
       </c>
       <c r="D208" t="str">
         <v xml:space="preserve"> </v>
@@ -5790,13 +5790,13 @@
     </row>
     <row r="209">
       <c r="A209" t="str">
-        <v>Take-out restaurants</v>
+        <v>Tools for families with school-related stress</v>
       </c>
       <c r="B209" t="str">
-        <v>Follow this [guidance for restaurants providing take-out, drive-through, and delivery](https://files.covid19.ca.gov/pdf/guidance-take-out-restaurants--en.pdf) to create a safer environment for workers and patrons.\n\nReview the guidance and prepare a plan for your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>*   [**School’s Out: A Parent’s Guide for Meeting the Challenge During the COVID-19 Pandemic**](https://nyulangone.org/news/schools-out-parents-guide-meeting-challenge-during-covid-19-pandemic) (article)  \n    Understanding a child’s need for structure, education, exercise, social contact, appropriate leisure time, and a calm, rational explanation about COVID-19 is key to ensuring healthy adaptation for youth.\n*   [**The Secret to Keeping Your Kids Happy, Busy and Learning if Their School Closes Due to Coronavirus**](https://time.com/5803373/coronavirus-kids-at-home-activities/) (article)  \n    This article identifies key elements to supporting children and youth as they transition to home-based learning.\n*   [**How LGBTQ Youth Can Cope with Anxiety and Stress During COVID-19**](https://www.thetrevorproject.org/2020/03/26/how-lgbtq-youth-can-cope-with-anxiety-and-stress-during-covid-19/) (blog post)   \n    Advice from The Trevor Project to help LGBTQ youth face the additional isolation and stress they experience during COVID-19. \n\nMore info: [Manage stress for health](https://covid19.ca.gov/manage-stress-for-health/)</v>
       </c>
       <c r="C209" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/manage-stress-for-health/</v>
       </c>
       <c r="D209" t="str">
         <v xml:space="preserve"> </v>
@@ -5816,13 +5816,13 @@
     </row>
     <row r="210">
       <c r="A210" t="str">
-        <v>Youth sports – NEW</v>
+        <v>Should I wear a mask or face covering to protect against COVID-19?</v>
       </c>
       <c r="B210" t="str">
-        <v>The [guidance for youth sports](https://files.covid19.ca.gov/pdf/guidance-youth-sports--en.pdf) provides guidelines for all youth sports programs, including school-based, club, and recreational programs. Check the [questions and answers](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Youth-Sports-FAQ.aspx) about youth sports. \n\nReview the guidance and prepare a plan to support a safe environment for players, coaches and trainers, families, spectators, event/program/facility managers, workers, and volunteers.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Yes. Californians must wear face coverings when in public spaces, especially indoors and other areas where physical distancing is not possible. Face coverings help reduce the spread of COVID-19. \n\nThe California Department of Public Health (CDPH) has released [guidance for the use of face coverings](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Guidance-for-Face-Coverings_06-18-2020.pdf). \n\nThe guidance reminds Californians that the best defense against COVID-19 continues to be: \n\n*   Maintain six feet of physical distance from others \n*   Wash hands frequently\n*   Avoid touching eyes, nose and mouth with unwashed hands\n*   Avoid being around people with COVID-19 symptoms\n\nMore info: [Masks and face coverings](https://covid19.ca.gov/masks-and-ppe/)</v>
       </c>
       <c r="C210" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/masks-and-ppe/</v>
       </c>
       <c r="D210" t="str">
         <v xml:space="preserve"> </v>
@@ -5842,13 +5842,13 @@
     </row>
     <row r="211">
       <c r="A211" t="str">
-        <v>Campgrounds and outdoor recreation</v>
+        <v>How well do face coverings prevent spread of COVID-19?</v>
       </c>
       <c r="B211" t="str">
-        <v>Follow this [guidance for campgrounds](https://files.covid19.ca.gov/pdf/guidance-campgrounds-outdoor-recreation--en.pdf), RV parks, and outdoor recreation to create a safer environment for workers and patrons.\n\nReview the guidance and prepare a plan for your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>There is scientific evidence to suggest that use of masks or face coverings reduces disease transmission. Their primary role is to reduce the release of infectious particles into the air when someone speaks, coughs, or sneezes. Face coverings are not a substitute for physical distancing, washing hands, and staying home when ill, but complements them.\n\nMore info: [Masks and face coverings](https://covid19.ca.gov/masks-and-ppe/)</v>
       </c>
       <c r="C211" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/masks-and-ppe/</v>
       </c>
       <c r="D211" t="str">
         <v xml:space="preserve"> </v>
@@ -5868,13 +5868,13 @@
     </row>
     <row r="212">
       <c r="A212" t="str">
-        <v>Cardrooms and racetracks</v>
+        <v>What is a face covering?</v>
       </c>
       <c r="B212" t="str">
-        <v>Follow this [guidance for cardrooms](https://files.covid19.ca.gov/pdf/guidance-cardrooms-racetracks--en.pdf), racetracks, and satellite wagering to create a safer environment for workers and patrons. **Indoor** operations at cardrooms must be closed in **all** counties. Racetracks may only operate without spectators.\n\nReview the guidance, prepare a plan, and post the [checklist for cardrooms](https://files.covid19.ca.gov/pdf/checklist-cardrooms-racetracks.pdf), racetracks, and satellite wagering in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>A face covering, also known as a cloth mask, is [material that covers the nose and mouth](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/diy-cloth-face-coverings.html). It can be secured to the head with ties or straps or simply wrapped around the lower face. It can be made of a variety of materials, such as cotton, silk, or linen. A face covering may be factory-made or sewn by hand, or can be improvised from household items such as scarfs, T-shirts, sweatshirts, or towels.\n\nMore info: [Masks and face coverings](https://covid19.ca.gov/masks-and-ppe/)</v>
       </c>
       <c r="C212" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/masks-and-ppe/</v>
       </c>
       <c r="D212" t="str">
         <v xml:space="preserve"> </v>
@@ -5894,13 +5894,13 @@
     </row>
     <row r="213">
       <c r="A213" t="str">
-        <v>Casinos</v>
+        <v>How should I care for a cloth mask or face covering?</v>
       </c>
       <c r="B213" t="str">
-        <v>In working with tribal governments, CDPH and DIR have released guidance on how to reopen casinos with reduced risk of transmission. Tribal governments should make determinations on when to reopen based on how they align with the current local public health conditions and the statewide stage of reopening and the Governor respectfully requests that until a surrounding or neighboring local jurisdiction has progressed into Stage 3, tribal casinos remain closed.\n\nFollow this [guidance for casinos](https://files.covid19.ca.gov/pdf/guidance-casinos--en.pdf) to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for casinos](https://files.covid19.ca.gov/pdf/checklist-casinos.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>It’s a good idea to [wash your face covering](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/diy-cloth-face-coverings.html) frequently, ideally after each use. Have a bag or bin to keep face coverings in until they can be laundered with detergent and hot water and dried on a hot cycle. If you must re-wear your face covering before washing, wash your hands immediately after putting it back on and avoid touching your face. Discard face coverings that:\n\n*   No longer cover the nose and mouth\n*   Have stretched out or damaged ties or straps\n*   Cannot stay on the face\n*   Have holes or tears in the fabric\n\nMore info: [Masks and face coverings](https://covid19.ca.gov/masks-and-ppe/)</v>
       </c>
       <c r="C213" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/masks-and-ppe/</v>
       </c>
       <c r="D213" t="str">
         <v xml:space="preserve"> </v>
@@ -5920,13 +5920,13 @@
     </row>
     <row r="214">
       <c r="A214" t="str">
-        <v>Dine-in restaurants</v>
+        <v>Is blood plasma authorized as a COVID-19 treatment?</v>
       </c>
       <c r="B214" t="str">
-        <v>This [guidance for dine-in restaurants](https://files.covid19.ca.gov/pdf/guidance-dine-in-restaurants--en.pdf) provides guidelines to create a safer environment for workers and customers. **Indoor** operations for dine-in restaurants must be closed in **all** counties. Bars, brewpubs, breweries, and pubs must close both **indoor and outdoor** operations in **all** counties unless they are offering sit-down, outdoor dine-in meals. Alcohol can only be sold in the same transaction as a meal.\n\n**For counties on the** [**Monitoring List**](https://covid19.ca.gov/roadmap-counties/#affected-counties)**:**\n\n**Indoor** operations must be closed. Follow this [guidance for restaurants providing outdoor dining, take-out, drive-through, and delivery](https://files.covid19.ca.gov/pdf/guidance-outdoor-restaurants--en.pdf) to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for dine-in restaurants](https://files.covid19.ca.gov/pdf/checklist-dine-in-restaurants.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>[The FDA issued an Emergency Use Authorization (EUA)](https://www.fda.gov/news-events/press-announcements/fda-issues-emergency-use-authorization-convalescent-plasma-potential-promising-covid-19-treatment) for convalescent plasma to treat hospitalized COVID-19 patients.\n\nThe FDA determined that it is reasonable to believe that COVID-19 convalescent plasma may be effective in making  COVID-19 illness shorter and less severe in some patients. The FDA also determined that the known and potential benefits of this plasma, when used to treat COVID-19, outweigh its known and potential risks. There are no adequate, approved, or available alternative treatments.\n\nMore info: [Survivors of COVID-19: Donate your plasma](https://covid19.ca.gov/plasma/)</v>
       </c>
       <c r="C214" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/plasma/</v>
       </c>
       <c r="D214" t="str">
         <v xml:space="preserve"> </v>
@@ -5946,13 +5946,13 @@
     </row>
     <row r="215">
       <c r="A215" t="str">
-        <v>Gyms and fitness centers</v>
+        <v>Is there a convalescent blood plasma donation center near me?</v>
       </c>
       <c r="B215" t="str">
-        <v>Follow this [guidance for gyms and fitness centers](https://files.covid19.ca.gov/pdf/guidance-fitness--en.pdf), including yoga and dance studios, to create a safer environment for workers and patrons. Recreational team sports are **not** permitted and will be subject to separate guidance.\n\n**For counties on the** [**Monitoring List**](https://covid19.ca.gov/roadmap-counties/#affected-counties)**:**\n\n**Indoor** operations must be closed. \n\nReview the guidance, prepare a plan, and post the [checklist for gyms and fitness centers](https://files.covid19.ca.gov/pdf/checklist-fitness.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Locate a donation center\n------------------------\n\nFind the blood center near you collecting COVID-19 blood plasma.\n\n[See the plasma donation center lookup](https://covid19.ca.gov/plasma/#plasma-lookup)\n\nMore info: [Survivors of COVID-19: Donate your plasma](https://covid19.ca.gov/plasma/)</v>
       </c>
       <c r="C215" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/plasma/</v>
       </c>
       <c r="D215" t="str">
         <v xml:space="preserve"> </v>
@@ -5972,13 +5972,13 @@
     </row>
     <row r="216">
       <c r="A216" t="str">
-        <v>Hair salons and barbershops</v>
+        <v>Where can I apply for unemployment?</v>
       </c>
       <c r="B216" t="str">
-        <v>This [guidance for hair salons and barbershops](https://files.covid19.ca.gov/pdf/guidance-hair-salons--en.pdf) provides guidelines to create a safer environment for workers and customers. Review the guidance, prepare a plan, and post the [checklist for hair salons](https://files.covid19.ca.gov/pdf/checklist-hair-salons.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\n**For counties on the** [**Monitoring List**](https://covid19.ca.gov/roadmap-counties/#affected-counties)**:**\n\nHair services provided **indoors** must be closed. Follow this [guidance for hair salons and barbershops providing services outdoors](https://files.covid19.ca.gov/pdf/guidance-outdoor-hair-salons--en.pdf) to support an outdoor safe, clean environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for hair salons and barbershops providing services outdoors](https://files.covid19.ca.gov/pdf/checklist-outdoor-hair-salons--en.pdf) at your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>If you lost your job or had your hours reduced, and meet eligibility requirements, you may be eligible to receive Unemployment Insurance (UI) benefits from California’s Employment Development Department (EDD). Check the [guide to applying for unemployment benefits](https://unemployment.edd.ca.gov/guide).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C216" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>Editorial</v>
       </c>
       <c r="D216" t="str">
         <v xml:space="preserve"> </v>
@@ -5998,13 +5998,13 @@
     </row>
     <row r="217">
       <c r="A217" t="str">
-        <v>Hotels (for tourism and individual travel)</v>
+        <v>Can my pet test positive for coronavirus? Can I take my pet to the vet?</v>
       </c>
       <c r="B217" t="str">
-        <v>Follow this [guidance for hotels and short term rentals](https://files.covid19.ca.gov/pdf/guidance-hotels-lodging-rentals--en.pdf) for tourism and individual travel to create a safer environment for workers and patrons.\n\nIf your county hasn’t been approved to move further in the reopening roadmap, hotels should only open for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or providing housing solutions, including measures to protect homeless populations. Follow this [guidance for hotels and lodging](https://files.covid19.ca.gov/pdf/guidance-hotels--en.pdf) to create a safer environment for workers and customers.\n\nReview the guidance, prepare a plan, and post the [checklist for hotels, lodging, and short-term rentals](https://files.covid19.ca.gov/pdf/checklist-hotels.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>While we are still learning about coronavirus, the risk of your pet testing positive for coronavirus is low. Because [there is still a risk](https://www.cdc.gov/coronavirus/2019-ncov/animals/pets-other-animals.html), keep your pets away from other pets and people outside of your household. Do not put face coverings on pets as this could harm your pet.\n\nYou can go to the vet or pet hospital if your pet is sick. Remember to wear a cloth face covering and to distance yourself at least 6 feet from other pets and owners.</v>
       </c>
       <c r="C217" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>Editorial</v>
       </c>
       <c r="D217" t="str">
         <v xml:space="preserve"> </v>
@@ -6024,13 +6024,13 @@
     </row>
     <row r="218">
       <c r="A218" t="str">
-        <v>Movie theaters and family entertainment centers</v>
+        <v>What is Larry David's advice?</v>
       </c>
       <c r="B218" t="str">
-        <v>Follow this guidance for [movie theaters and family entertainment centers](https://files.covid19.ca.gov/pdf/guidance-family-entertainment--en.pdf), like bowling alleys, miniature golf, batting cages, and arcades, to create a safer environment for workers and patrons. **Indoor** operations must be closed in **all** counties.\n\nReview the guidance, prepare a plan, and post the [checklist for movie theaters and family entertainment centers](https://files.covid19.ca.gov/pdf/checklist-family-entertainment.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>&lt;blockquote class="twitter-tweet"&gt;&lt;p lang="en" dir="ltr"&gt;“You’re hurting old people like me. Well, not me... I’ll never see you.”&lt;br&gt;&lt;br&gt;Larry David wants everyone to stay home to protect older Californians from &lt;a href="https://twitter.com/hashtag/COVID19?src=hash&amp;amp;ref_src=twsrc%5Etfw"&gt;#COVID19&lt;/a&gt;! &lt;br&gt;He does not do these things. &lt;br&gt;Listen to Larry.&lt;a href="https://twitter.com/hashtag/StayHomeSaveLives?src=hash&amp;amp;ref_src=twsrc%5Etfw"&gt;#StayHomeSaveLives&lt;/a&gt;&lt;a href="https://t.co/snYe5v55Rw"&gt;https://t.co/snYe5v55Rw&lt;/a&gt; &lt;a href="https://t.co/C5cKOaAufE"&gt;pic.twitter.com/C5cKOaAufE&lt;/a&gt;&lt;/p&gt;&amp;mdash; Office of the Governor of California (@CAgovernor) &lt;a href="https://twitter.com/CAgovernor/status/1245110728199045120?ref_src=twsrc%5Etfw"&gt;March 31, 2020&lt;/a&gt;&lt;/blockquote&gt; &lt;script async src="https://platform.twitter.com/widgets.js" charset="utf-8"&gt;&lt;/script&gt;</v>
       </c>
       <c r="C218" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>Editorial</v>
       </c>
       <c r="D218" t="str">
         <v xml:space="preserve"> </v>
@@ -6050,13 +6050,13 @@
     </row>
     <row r="219">
       <c r="A219" t="str">
-        <v>Personal care services</v>
+        <v>Where can I find the list of essential critical infrastructure sectors?</v>
       </c>
       <c r="B219" t="str">
-        <v>Follow this [guidance for personal care services](https://files.covid19.ca.gov/pdf/guidance-expanded-personal-care-services--en.pdf) like nail salons, tattoo parlors, and body waxing to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for personal care services](https://files.covid19.ca.gov/pdf/checklist-expanded-personal-care-services.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\n**For counties on the** [**Monitoring List**](https://covid19.ca.gov/roadmap-counties/#affected-counties)**:**\n\n*   **Indoor** operations of nail salons, skin care, waxing, and massage must be closed. \n*   **All indoor and outdoor** services for tattooing, piercing, and electrolysis must be closed.\n*   Some services may be provided **outdoors**, like nails and massage. Follow this [guidance for personal care services provided outdoors](https://files.covid19.ca.gov/pdf/guidance-outdoor-personal-care--en.pdf) to support an outdoor safe, clean environment for workers and patrons. This guidance applies to services that require touching a client’s face, like facials and waxing. This guidance also applies to esthetic services, skin care, cosmetology, nail services, and massage therapy. Review the guidance, prepare a plan, and post the [checklist for personal care services provided outdoors](https://files.covid19.ca.gov/pdf/checklist-outdoor-personal-care--en.pdf) at your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v xml:space="preserve">Visit [Essential workforce](https://covid19.ca.gov/essential-workforce/) to learn about what workers and sectors are included. </v>
       </c>
       <c r="C219" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>Editorial</v>
       </c>
       <c r="D219" t="str">
         <v xml:space="preserve"> </v>
@@ -6076,13 +6076,13 @@
     </row>
     <row r="220">
       <c r="A220" t="str">
-        <v>Restaurants, wineries, and bars</v>
+        <v>What is a cohort?</v>
       </c>
       <c r="B220" t="str">
-        <v>Follow this [guidance for restaurants, wineries, and bars](https://files.covid19.ca.gov/pdf/guidance-restaurants-bars-wineries--en.pdf) to create a safer environment for workers and patrons. **Indoor** operations for dine-in restaurants, wineries, and tasting rooms must be closed in **all** counties. Bars, brewpubs, breweries, and pubs must close both **indoor and outdoor** operations in **all** counties unless they are offering sit-down, outdoor dine-in meals. Alcohol can only be sold in the same transaction as a meal.\n\n**For counties on the** [**Monitoring List**](https://covid19.ca.gov/roadmap-counties/#affected-counties)**:**\n\n**Indoor** operations must be closed. Follow this [guidance for restaurants providing outdoor dining, take-out, drive-through, and delivery](https://files.covid19.ca.gov/pdf/guidance-outdoor-restaurants--en.pdf) to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for restaurants, wineries, and bars](https://files.covid19.ca.gov/pdf/checklist-restaurants-bars.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>A cohort is a stable group of no more than 14 children or youth and no more than two supervising adults in a supervised environment. The group stays together for all activities, including meals and recreation. And this group avoids contact with anyone not in their group. &lt;!-- pod, gathering, youth, kid, school, class, distance, learning, hub --&gt;</v>
       </c>
       <c r="C220" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>Editorial</v>
       </c>
       <c r="D220" t="str">
         <v xml:space="preserve"> </v>
@@ -6100,503 +6100,9 @@
         <v>219</v>
       </c>
     </row>
-    <row r="221">
-      <c r="A221" t="str">
-        <v>Zoos and museums</v>
-      </c>
-      <c r="B221" t="str">
-        <v>Follow this [guidance for zoos, museums](https://files.covid19.ca.gov/pdf/guidance-zoos-museums--en.pdf), galleries, botanical gardens, and aquariums to create a safer environment for workers and patrons. **Indoor** operations must be closed in **all** counties. Review the guidance, prepare a plan, and post the [checklist for zoos, museums](https://files.covid19.ca.gov/pdf/checklist-zoos-museums.pdf), galleries, and aquariums in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nIf your county hasn’t been approved to move further in the reopening roadmap, follow this [guidance for outdoor museums](https://files.covid19.ca.gov/pdf/guidance-outdoor-museums--en.pdf), open air galleries, botanical gardens, and other outdoor exhibition spaces to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for outdoor museums](https://files.covid19.ca.gov/pdf/checklist-outdoor-museums.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
-      </c>
-      <c r="C221" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
-      </c>
-      <c r="D221" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E221" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F221" t="str">
-        <v>false</v>
-      </c>
-      <c r="G221" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H221" t="str">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" t="str">
-        <v>Tools for families facing stress</v>
-      </c>
-      <c r="B222" t="str">
-        <v>*   [**Noggin’s Navigating the New Normal: Parents Edition**](https://www.noggin.com/navigating-the-new-normal-parents-edition/) (video)  \n    Host Jamie-Lynn Sigler asks Dr. Nadine Burke Harris and other leading experts how to handle the stress of the pandemic on little kids. \n*   [**How to Support Our Kids During COVID-19**](https://podcasts.apple.com/us/podcast/how-to-support-our-kids-during-covid-19-dr-nadine-burke/id1468607534?i=1000470057466) (Apple podcast)  \n    Dr. Burke Harris shares advice on how to talk to your kids about COVID-19, what all of us can do to help, and how to mitigate stress while stuck at home.  \n*   [**FOCUS on the GO!**](https://nfrc.ucla.edu/focus-on-the-go) (app)  \n    Free mobile app designed to help your family enhance existing coping skills and develop new ones through gameplay.\n*   [**Young Children at Home During the COVID-19 Outbreak: The Importance of Self-Care**](https://www.zerotothree.org/resources/3262-young-children-at-home-during-the-covid-19-outbreak-the-importance-of-self-care) (article)  \n    Knowing how to take care of yourself as a caregiver during the COVID-19 outbreak is key to ensure you are most effective in parenting.\n\nMore info: [Manage stress for health](https://covid19.ca.gov/manage-stress-for-health/)</v>
-      </c>
-      <c r="C222" t="str">
-        <v>https://covid19.ca.gov/manage-stress-for-health/</v>
-      </c>
-      <c r="D222" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E222" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F222" t="str">
-        <v>false</v>
-      </c>
-      <c r="G222" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H222" t="str">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" t="str">
-        <v>Tools for parents to help children</v>
-      </c>
-      <c r="B223" t="str">
-        <v>*   [**California Surgeon General’s Playbook: Stress Relief for Caregivers and Kids During COVID-19**](https://files.covid19.ca.gov/pdf/caregivers_and_kids_california_surgeon_general_stress_busting_playbook_draft_v2_clean_ada_04072020v2.pdf) (PDF)  \n    This guide can help you understand what signs of stress to look out for and what you can do to protect your family’s health. It is also available in [Arabic](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_arabic-2.pdf), Chinese ([Simplified](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_ch_simplified.pdf) and [Traditional](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_zh-hant.pdf)), [Korean](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_korean.pdf), [Spanish](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook-spanish.pdf), [Tagalog](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_tagalog.pdf), and [Vietnamese](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_vi.pdf).\n*   [**Trauma Informed Parent: Helping Adults and Children With Trauma During the Pandemic**](https://www.youtube.com/watch?v=57EAL_e5Nf0) (video)  \n    California’s Surgeon General provides context and tools for how to help kids who have endured past trauma through current stress. \n*   [**Emotional Wellbeing during the COVID-19 Pandemic**](https://www.childtrends.org/publications/resources-for-supporting-childrens-emotional-well-being-during-the-covid-19-pandemic) (guide)  \n    Supporting children’s emotional wellbeing during the COVID-19 pandemic is key to adjusting to a new sense of normal.\n\nMore info: [Manage stress for health](https://covid19.ca.gov/manage-stress-for-health/)</v>
-      </c>
-      <c r="C223" t="str">
-        <v>https://covid19.ca.gov/manage-stress-for-health/</v>
-      </c>
-      <c r="D223" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E223" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F223" t="str">
-        <v>false</v>
-      </c>
-      <c r="G223" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H223" t="str">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" t="str">
-        <v>Tools for families with school-related stress</v>
-      </c>
-      <c r="B224" t="str">
-        <v>*   [**School’s Out: A Parent’s Guide for Meeting the Challenge During the COVID-19 Pandemic**](https://nyulangone.org/news/schools-out-parents-guide-meeting-challenge-during-covid-19-pandemic) (article)  \n    Understanding a child’s need for structure, education, exercise, social contact, appropriate leisure time, and a calm, rational explanation about COVID-19 is key to ensuring healthy adaptation for youth.\n*   [**The Secret to Keeping Your Kids Happy, Busy and Learning if Their School Closes Due to Coronavirus**](https://time.com/5803373/coronavirus-kids-at-home-activities/) (article)  \n    This article identifies key elements to supporting children and youth as they transition to home-based learning.\n*   [**How LGBTQ Youth Can Cope with Anxiety and Stress During COVID-19**](https://www.thetrevorproject.org/2020/03/26/how-lgbtq-youth-can-cope-with-anxiety-and-stress-during-covid-19/) (blog post)   \n    Advice from The Trevor Project to help LGBTQ youth face the additional isolation and stress they experience during COVID-19. \n\nMore info: [Manage stress for health](https://covid19.ca.gov/manage-stress-for-health/)</v>
-      </c>
-      <c r="C224" t="str">
-        <v>https://covid19.ca.gov/manage-stress-for-health/</v>
-      </c>
-      <c r="D224" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E224" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F224" t="str">
-        <v>false</v>
-      </c>
-      <c r="G224" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H224" t="str">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" t="str">
-        <v>Should I wear a mask or face covering to protect against COVID-19?</v>
-      </c>
-      <c r="B225" t="str">
-        <v>Yes. Californians must wear face coverings when in public spaces, especially indoors and other areas where physical distancing is not possible. Face coverings help reduce the spread of COVID-19. \n\nThe California Department of Public Health (CDPH) has released [guidance for the use of face coverings](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Guidance-for-Face-Coverings_06-18-2020.pdf). \n\nThe guidance reminds Californians that the best defense against COVID-19 continues to be: \n\n*   Maintain six feet of physical distance from others \n*   Wash hands frequently\n*   Avoid touching eyes, nose and mouth with unwashed hands\n*   Avoid being around people with COVID-19 symptoms\n\nMore info: [Masks and face coverings](https://covid19.ca.gov/masks-and-ppe/)</v>
-      </c>
-      <c r="C225" t="str">
-        <v>https://covid19.ca.gov/masks-and-ppe/</v>
-      </c>
-      <c r="D225" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E225" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F225" t="str">
-        <v>false</v>
-      </c>
-      <c r="G225" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H225" t="str">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" t="str">
-        <v>How well do face coverings prevent spread of COVID-19?</v>
-      </c>
-      <c r="B226" t="str">
-        <v>There is scientific evidence to suggest that use of masks or face coverings reduces disease transmission. Their primary role is to reduce the release of infectious particles into the air when someone speaks, coughs, or sneezes. Face coverings are not a substitute for physical distancing, washing hands, and staying home when ill, but complements them.\n\nMore info: [Masks and face coverings](https://covid19.ca.gov/masks-and-ppe/)</v>
-      </c>
-      <c r="C226" t="str">
-        <v>https://covid19.ca.gov/masks-and-ppe/</v>
-      </c>
-      <c r="D226" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E226" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F226" t="str">
-        <v>false</v>
-      </c>
-      <c r="G226" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H226" t="str">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" t="str">
-        <v>What is a face covering?</v>
-      </c>
-      <c r="B227" t="str">
-        <v>A face covering, also known as a cloth mask, is [material that covers the nose and mouth](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/diy-cloth-face-coverings.html). It can be secured to the head with ties or straps or simply wrapped around the lower face. It can be made of a variety of materials, such as cotton, silk, or linen. A face covering may be factory-made or sewn by hand, or can be improvised from household items such as scarfs, T-shirts, sweatshirts, or towels.\n\nMore info: [Masks and face coverings](https://covid19.ca.gov/masks-and-ppe/)</v>
-      </c>
-      <c r="C227" t="str">
-        <v>https://covid19.ca.gov/masks-and-ppe/</v>
-      </c>
-      <c r="D227" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E227" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F227" t="str">
-        <v>false</v>
-      </c>
-      <c r="G227" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H227" t="str">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" t="str">
-        <v>How should I care for a cloth mask or face covering?</v>
-      </c>
-      <c r="B228" t="str">
-        <v>It’s a good idea to [wash your face covering](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/diy-cloth-face-coverings.html) frequently, ideally after each use. Have a bag or bin to keep face coverings in until they can be laundered with detergent and hot water and dried on a hot cycle. If you must re-wear your face covering before washing, wash your hands immediately after putting it back on and avoid touching your face. Discard face coverings that:\n\n*   No longer cover the nose and mouth\n*   Have stretched out or damaged ties or straps\n*   Cannot stay on the face\n*   Have holes or tears in the fabric\n\nMore info: [Masks and face coverings](https://covid19.ca.gov/masks-and-ppe/)</v>
-      </c>
-      <c r="C228" t="str">
-        <v>https://covid19.ca.gov/masks-and-ppe/</v>
-      </c>
-      <c r="D228" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E228" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F228" t="str">
-        <v>false</v>
-      </c>
-      <c r="G228" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H228" t="str">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" t="str">
-        <v>Is there a convalescent blood plasma donation center near me?</v>
-      </c>
-      <c r="B229" t="str">
-        <v>Locate a donation center\n------------------------\n\nFind the blood center near you collecting COVID-19 blood plasma.\n\n[See the plasma donation center lookup](https://covid19.ca.gov/plasma/#plasma-lookup)\n\nMore info: [Survivors of COVID-19: Donate your plasma](https://covid19.ca.gov/plasma/)</v>
-      </c>
-      <c r="C229" t="str">
-        <v>https://covid19.ca.gov/plasma/</v>
-      </c>
-      <c r="D229" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E229" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F229" t="str">
-        <v>false</v>
-      </c>
-      <c r="G229" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H229" t="str">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" t="str">
-        <v>Where can I apply for unemployment?</v>
-      </c>
-      <c r="B230" t="str">
-        <v>If you lost your job or had your hours reduced, and meet eligibility requirements, you may be eligible to receive Unemployment Insurance (UI) benefits from California’s Employment Development Department (EDD). Check the [guide to applying for unemployment benefits](https://unemployment.edd.ca.gov/guide).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
-      </c>
-      <c r="C230" t="str">
-        <v>Editorial</v>
-      </c>
-      <c r="D230" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E230" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F230" t="str">
-        <v>false</v>
-      </c>
-      <c r="G230" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H230" t="str">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" t="str">
-        <v>Are hotels allowed to open?</v>
-      </c>
-      <c r="B231" t="str">
-        <v>[Counties that have received approval from the State](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/County_Variance_Attestation_Form.aspx) may open hotels, lodging and short term rentals for tourism and individual travel as long as they follow [state guidance](https://covid19.ca.gov/pdf/guidance-hotels-lodging-rentals.pdf) for public health and safety. Large meeting venues, banquet halls or convention centers should remain closed. All other counties [should only open hotels and lodging](https://covid19.ca.gov/pdf/guidance-hotels.pdf) for COVID-19 mitigation and containment measures, treatment measures, providing accommodation for essential workers, or housing solutions, including measures to protect homeless populations. &lt;!-- motel, vacation, airbnb, vrbo, rental home --&gt;</v>
-      </c>
-      <c r="C231" t="str">
-        <v>Editorial</v>
-      </c>
-      <c r="D231" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E231" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F231" t="str">
-        <v>false</v>
-      </c>
-      <c r="G231" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H231" t="str">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" t="str">
-        <v>Can my pet test positive for coronavirus? Can I take my pet to the vet?</v>
-      </c>
-      <c r="B232" t="str">
-        <v>While we are still learning about coronavirus, the risk of your pet testing positive for coronavirus is low. Because [there is still a risk](https://www.cdc.gov/coronavirus/2019-ncov/animals/pets-other-animals.html), keep your pets away from other pets and people outside of your household. Do not put face coverings on pets as this could harm your pet.\n\nYou can go to the vet or pet hospital if your pet is sick. Remember to wear a cloth face covering and to distance yourself at least 6 feet from other pets and owners.</v>
-      </c>
-      <c r="C232" t="str">
-        <v>Editorial</v>
-      </c>
-      <c r="D232" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E232" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F232" t="str">
-        <v>false</v>
-      </c>
-      <c r="G232" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H232" t="str">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" t="str">
-        <v>What is Larry David's advice?</v>
-      </c>
-      <c r="B233" t="str">
-        <v>&lt;blockquote class="twitter-tweet"&gt;&lt;p lang="en" dir="ltr"&gt;“You’re hurting old people like me. Well, not me... I’ll never see you.”&lt;br&gt;&lt;br&gt;Larry David wants everyone to stay home to protect older Californians from &lt;a href="https://twitter.com/hashtag/COVID19?src=hash&amp;amp;ref_src=twsrc%5Etfw"&gt;#COVID19&lt;/a&gt;! &lt;br&gt;He does not do these things. &lt;br&gt;Listen to Larry.&lt;a href="https://twitter.com/hashtag/StayHomeSaveLives?src=hash&amp;amp;ref_src=twsrc%5Etfw"&gt;#StayHomeSaveLives&lt;/a&gt;&lt;a href="https://t.co/snYe5v55Rw"&gt;https://t.co/snYe5v55Rw&lt;/a&gt; &lt;a href="https://t.co/C5cKOaAufE"&gt;pic.twitter.com/C5cKOaAufE&lt;/a&gt;&lt;/p&gt;&amp;mdash; Office of the Governor of California (@CAgovernor) &lt;a href="https://twitter.com/CAgovernor/status/1245110728199045120?ref_src=twsrc%5Etfw"&gt;March 31, 2020&lt;/a&gt;&lt;/blockquote&gt; &lt;script async src="https://platform.twitter.com/widgets.js" charset="utf-8"&gt;&lt;/script&gt;</v>
-      </c>
-      <c r="C233" t="str">
-        <v>Editorial</v>
-      </c>
-      <c r="D233" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E233" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F233" t="str">
-        <v>false</v>
-      </c>
-      <c r="G233" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H233" t="str">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" t="str">
-        <v xml:space="preserve">Can I go to the movies? </v>
-      </c>
-      <c r="B234" t="str">
-        <v xml:space="preserve">Effective July 13, 2020, indoor movie theaters are closed in all counties. Drive-in movie theaters with modifications to support physical distancing may be open.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) </v>
-      </c>
-      <c r="C234" t="str">
-        <v>Editorial</v>
-      </c>
-      <c r="D234" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E234" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F234" t="str">
-        <v>false</v>
-      </c>
-      <c r="G234" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H234" t="str">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="A235" t="str">
-        <v>Can I go to a restaurant? Can I go to a winery or a brewery?</v>
-      </c>
-      <c r="B235" t="str">
-        <v xml:space="preserve">Indoor operations of all dine-in restaurants are closed in all counties. Restaurants across the state can be open for take out, drive through, delivery, and outdoor dining. \n\nIndoor operations for wineries and tasting rooms are closed in all counties. All bars, brewpubs, breweries, and pubs are closed statewide for both indoor and outdoor operations, unless they offer sit-down, outdoor dine-in meals. Alcohol can only be sold in the same transaction as a meal.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) </v>
-      </c>
-      <c r="C235" t="str">
-        <v>Editorial</v>
-      </c>
-      <c r="D235" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E235" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F235" t="str">
-        <v>false</v>
-      </c>
-      <c r="G235" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H235" t="str">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="A236" t="str">
-        <v>Are restaurants allowed to open?</v>
-      </c>
-      <c r="B236" t="str">
-        <v xml:space="preserve">Restaurants across the state can be open for [take out, drive through, and delivery](https://files.covid19.ca.gov/pdf/guidance-takeout-restaurants.pdf). Indoor operations for dine-in restaurants are closed in all counties. Bars, brewpubs, breweries, and pubs must close both indoor and outdoor operations unless they are offering [sit-down, outdoor dine-in meals](https://files.covid19.ca.gov/pdf/guidance-outdoor-restaurants.pdf). Alcohol can only be sold in the same transaction as a meal.\n\nMore info: [Industry guidance](https://covid19.ca.gov/industry-guidance/) and [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) </v>
-      </c>
-      <c r="C236" t="str">
-        <v>Editorial</v>
-      </c>
-      <c r="D236" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E236" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F236" t="str">
-        <v>false</v>
-      </c>
-      <c r="G236" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H236" t="str">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" t="str">
-        <v>Where can I find the list of essential critical infrastructure sectors?</v>
-      </c>
-      <c r="B237" t="str">
-        <v xml:space="preserve">Visit [Essential workforce](https://covid19.ca.gov/essential-workforce/) to learn about what workers and sectors are included. </v>
-      </c>
-      <c r="C237" t="str">
-        <v>Editorial</v>
-      </c>
-      <c r="D237" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E237" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F237" t="str">
-        <v>false</v>
-      </c>
-      <c r="G237" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H237" t="str">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="A238" t="str">
-        <v>Can I get my nails done? Can I get a massage? Can I get a facial?</v>
-      </c>
-      <c r="B238" t="str">
-        <v>It depends. Services like nails, waxing, facials, and massage therapy can be open in counties not on the Monitoring List. For counties on the Monitoring List for 3 consecutive days, some services may be provided outdoors, like nails, waxing, facials, and massage. All indoor operations of nail salons, skin care, waxing, and massage are closed in counties on the Monitoring List for 3 consecutive days. [Learn more about which counties are on the list](https://covid19.ca.gov/roadmap-counties/).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) &lt;!-- spa, esthetician, electrolysis, waxing, cosmetology services, electrology, body art --&gt;</v>
-      </c>
-      <c r="C238" t="str">
-        <v>Editorial</v>
-      </c>
-      <c r="D238" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E238" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F238" t="str">
-        <v>false</v>
-      </c>
-      <c r="G238" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H238" t="str">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" t="str">
-        <v>Can I get a tattoo or piercing? Can I get electrolysis?</v>
-      </c>
-      <c r="B239" t="str">
-        <v>It depends. Tattoo, piercing, and electrolysis services can be open in counties not on the Monitoring List. All indoor and outdoor services for tattooing, piercing, and electrolysis are closed in counties on the Monitoring List for 3 consecutive days. [Learn more about which counties are on the list](https://covid19.ca.gov/roadmap-counties/).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/) &lt;!-- spa, esthetician, electrolysis, waxing, cosmetology services, electrology, body art --&gt;</v>
-      </c>
-      <c r="C239" t="str">
-        <v>Editorial</v>
-      </c>
-      <c r="D239" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E239" t="str">
-        <v>[]</v>
-      </c>
-      <c r="F239" t="str">
-        <v>false</v>
-      </c>
-      <c r="G239" t="str">
-        <v>[]</v>
-      </c>
-      <c r="H239" t="str">
-        <v>238</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H239"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H220"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
no more manually curated qa pairs
</commit_message>
<xml_diff>
--- a/qnacrawler/merged.xlsx
+++ b/qnacrawler/merged.xlsx
@@ -408,10 +408,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>What are the symptoms of COVID-19?</v>
+        <v>Can air conditioning spread COVID-19 from one room to another?</v>
       </c>
       <c r="B2" t="str">
-        <v>### [Coronavirus symptoms](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html) include, but are not limited to:\n\n*   Fever or chills\n*   Cough\n*   Shortness of breath or difficulty breathing\n*   Fatigue\n*   Muscle or body aches\n*   Headache\n*   New loss of taste or smell\n*   Sore throat\n*   Congestion or runny nose\n*   Nausea or vomiting\n*   Diarrhea\n\nMore info: [Symptoms and risks](https://covid19.ca.gov/symptoms-and-risks/)</v>
+        <v>There is no evidence that COVID-19 spreads indoors through air conditioning. There are a wide variety of heating, ventilation and air conditioning (HVAC) systems. Well-designed HVAC systems can actually help reduce risk. Since the system filters air as it circulates, it adds cleaner air to the space. Introduction of fresh outdoor air dilutes the concentration of infectious particles. Air conditioning is also necessary in some areas to protect from excessive heat. For more information, see [ASHRAE guidelines for homeowners and HVAC professionals](https://www.ashrae.org/technical-resources/resources). \n\nMore info: [Symptoms and risks](https://covid19.ca.gov/symptoms-and-risks/)</v>
       </c>
       <c r="C2" t="str">
         <v>https://covid19.ca.gov/symptoms-and-risks/</v>
@@ -434,10 +434,10 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Is there a COVID-19 symptoms self-checker?</v>
+        <v>What are the symptoms of COVID-19?</v>
       </c>
       <c r="B3" t="str">
-        <v>You can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor through [telehealth](https://covid19.ca.gov/telehealth/).\n\nMore info: [Symptoms and risks](https://covid19.ca.gov/symptoms-and-risks/)</v>
+        <v>### [Coronavirus symptoms](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html) include, but are not limited to:\n\n*   Fever or chills\n*   Cough\n*   Shortness of breath or difficulty breathing\n*   Fatigue\n*   Muscle or body aches\n*   Headache\n*   New loss of taste or smell\n*   Sore throat\n*   Congestion or runny nose\n*   Nausea or vomiting\n*   Diarrhea\n\nMore info: [Symptoms and risks](https://covid19.ca.gov/symptoms-and-risks/)</v>
       </c>
       <c r="C3" t="str">
         <v>https://covid19.ca.gov/symptoms-and-risks/</v>
@@ -460,10 +460,10 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Who are high risk people for COVID-19?</v>
+        <v>Is there a COVID-19 symptoms self-checker?</v>
       </c>
       <c r="B4" t="str">
-        <v>#### Some people are at [higher risk](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-at-increased-risk.html) to get very sick from COVID-19, including:\n\nMore info: [Symptoms and risks](https://covid19.ca.gov/symptoms-and-risks/)</v>
+        <v>You can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor through [telehealth](https://covid19.ca.gov/telehealth/).\n\nMore info: [Symptoms and risks](https://covid19.ca.gov/symptoms-and-risks/)</v>
       </c>
       <c r="C4" t="str">
         <v>https://covid19.ca.gov/symptoms-and-risks/</v>
@@ -486,10 +486,10 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>What people at higher risk, seniors over 65 or compromised immune systems, should do?</v>
+        <v>Who are high risk people for COVID-19?</v>
       </c>
       <c r="B5" t="str">
-        <v>If you are at higher risk, you should take extra precautions to protect yourself: \n\n*   **Stay home.** It’s the most important thing you can do.\n*   **Avoid contact with people who are sick.** Isolate anyone sick in your home in a separate room, if possible.\n*   **Get food brought to your house** through family, social, or commercial networks. Wipe off containers with disinfectant wipes.\n*   **Listen to public health officials.** They may recommend community actions to reduce exposure in times of local outbreak.\n\nMore info: [Symptoms and risks](https://covid19.ca.gov/symptoms-and-risks/)</v>
+        <v>#### Some people are at [higher risk](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-at-increased-risk.html) to get very sick from COVID-19, including:\n\n*   [People over 65 years old](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/older-adults.html)\n*   [People of any age with certain underlying medical conditions:](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-with-medical-conditions.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fneed-extra-precautions%2Fgroups-at-higher-risk.html)\n    *   [Cancer](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-with-medical-conditions.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fneed-extra-precautions%2Fgroups-at-higher-risk.html#cancer)\n    *   [Chronic kidney disease](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-with-medical-conditions.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fneed-extra-precautions%2Fgroups-at-higher-risk.html#chronic-kidney-disease)\n    *   [COPD (chronic obstructive pulmonary disease)](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-with-medical-conditions.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fneed-extra-precautions%2Fgroups-at-higher-risk.html#copd)\n    *   [Immunocompromised state (weakened immune system) from solid organ transplant](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-with-medical-conditions.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fneed-extra-precautions%2Fgroups-at-higher-risk.html#immunocompromised-state)\n    *   [Obesity (body mass index \[BMI\] of 30 or higher)](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-with-medical-conditions.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fneed-extra-precautions%2Fgroups-at-higher-risk.html#obesity)\n    *   [Serious heart conditions, such as heart failure, coronary artery disease, or cardiomyopathies](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-with-medical-conditions.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fneed-extra-precautions%2Fgroups-at-higher-risk.html#serious-heart-conditions)\n    *   [Sickle cell disease](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-with-medical-conditions.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fneed-extra-precautions%2Fgroups-at-higher-risk.html#hemoglobin-disorders)\n    *   [Type 2 diabetes mellitus](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-with-medical-conditions.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fneed-extra-precautions%2Fgroups-at-higher-risk.html#diabetes)\n\nMore info: [Symptoms and risks](https://covid19.ca.gov/symptoms-and-risks/)</v>
       </c>
       <c r="C5" t="str">
         <v>https://covid19.ca.gov/symptoms-and-risks/</v>
@@ -512,13 +512,13 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Has the deadline for federal taxes changed?</v>
+        <v>What people at higher risk, seniors over 65 or compromised immune systems, should do?</v>
       </c>
       <c r="B6" t="str">
-        <v>The federal deadline for filing and paying taxes has been [extended to July 15, 2020](https://www.irs.gov/newsroom/payment-deadline-extended-to-july-15-2020). \n\nSee [information on the U.S. Internal Revenue Service](https://www.irs.gov/coronavirus) for more information.\n\nMore info: [Taxes](https://covid19.ca.gov/taxes/)</v>
+        <v>If you are at higher risk, you should take extra precautions to protect yourself: \n\n*   **Stay home.** It’s the most important thing you can do.\n*   **Avoid contact with people who are sick.** Isolate anyone sick in your home in a separate room, if possible.\n*   **Get food brought to your house** through family, social, or commercial networks. Wipe off containers with disinfectant wipes.\n*   **Listen to public health officials.** They may recommend community actions to reduce exposure in times of local outbreak.\n\nMore info: [Symptoms and risks](https://covid19.ca.gov/symptoms-and-risks/)</v>
       </c>
       <c r="C6" t="str">
-        <v>https://covid19.ca.gov/taxes/</v>
+        <v>https://covid19.ca.gov/symptoms-and-risks/</v>
       </c>
       <c r="D6" t="str">
         <v xml:space="preserve"> </v>
@@ -538,10 +538,10 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Are there any tax deductions for people affected by the COVID-19 outbreak?</v>
+        <v>Has the deadline for federal taxes changed?</v>
       </c>
       <c r="B7" t="str">
-        <v>No. Check with the [U.S. Internal Revenue Service](https://www.irs.gov/coronavirus), the [California Franchise Tax Board](https://www.ftb.ca.gov/), and your local government for updates.\n\nMore info: [Taxes](https://covid19.ca.gov/taxes/)</v>
+        <v>The federal deadline for filing and paying taxes has been [extended to July 15, 2020](https://www.irs.gov/newsroom/payment-deadline-extended-to-july-15-2020). \n\nSee [information on the U.S. Internal Revenue Service](https://www.irs.gov/coronavirus) for more information.\n\nMore info: [Taxes](https://covid19.ca.gov/taxes/)</v>
       </c>
       <c r="C7" t="str">
         <v>https://covid19.ca.gov/taxes/</v>
@@ -564,13 +564,13 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>What is the relationship between the stay home order and these questions and answers?</v>
+        <v>Are there any tax deductions for people affected by the COVID-19 outbreak?</v>
       </c>
       <c r="B8" t="str">
-        <v>The Governor has ordered Californians to obey the directives of the State Public Health Officer. Those directives take many forms; they include specific materials linked on this page, as well as these questions and answers. These questions and answers are directives from the State Public Health Officer, and have the same force and effect as other State Public Health Officer directives.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>No. Check with the [U.S. Internal Revenue Service](https://www.irs.gov/coronavirus), the [California Franchise Tax Board](https://www.ftb.ca.gov/), and your local government for updates.\n\nMore info: [Taxes](https://covid19.ca.gov/taxes/)</v>
       </c>
       <c r="C8" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/taxes/</v>
       </c>
       <c r="D8" t="str">
         <v xml:space="preserve"> </v>
@@ -590,10 +590,10 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>When does the stay home order go into effect and how long will we stay home? What areas of the state are covered?</v>
+        <v>What is the relationship between the stay home order and these questions and answers?</v>
       </c>
       <c r="B9" t="str">
-        <v>The order went into effect on Thursday, March 19, 2020. The order is in place until further notice. It covers the whole state of California.\n\nAs of May 8, the stay home order was modified. In addition to essential activity, retail is allowed, along with the infrastructure to support it. As of May 12, offices, limited services, and outdoor museums are also permitted to open.\n\n**\[Add new Executive Order language here.\]**\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>The Governor has ordered Californians to obey the directives of the State Public Health Officer. Those directives take many forms; they include specific materials linked on this page, as well as these questions and answers. These questions and answers are directives from the State Public Health Officer, and have the same force and effect as other State Public Health Officer directives.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C9" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -616,10 +616,10 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Is it safe to shop at open businesses?</v>
+        <v>When does the stay home order go into effect and how long will we stay home? What areas of the state are covered?</v>
       </c>
       <c r="B10" t="str">
-        <v>The risk of COVID-19 infection is still real for all Californians and continues to be fatal. That is why every business permitted to open should take every step humanly possible to reduce the risk of infection by following these [state guidelines](https://covid19.ca.gov/industry-guidance/#top).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>The order went into effect on Thursday, March 19, 2020. The order is in place until further notice. It covers the whole state of California.\n\nAs of May 8, the stay home order was modified. In addition to essential activity, retail is allowed, along with the infrastructure to support it. As of May 12, offices, limited services, and outdoor museums are also permitted to open.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C10" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -642,10 +642,10 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Can the stay home order be changed?</v>
+        <v>Is it safe to shop at open businesses?</v>
       </c>
       <c r="B11" t="str">
-        <v>Yes. The State Public Health Officer may issue new orders as the public health situation changes.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>The risk of COVID-19 infection is still real for all Californians and continues to be fatal. That is why every business permitted to open should take every step humanly possible to reduce the risk of infection by following these [state guidelines](https://covid19.ca.gov/industry-guidance/#top).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C11" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -668,10 +668,10 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>How does the stay home order interact with local orders to shelter in place? Does it supersede them?</v>
+        <v>Can the stay home order be changed?</v>
       </c>
       <c r="B12" t="str">
-        <v>This is a statewide order. Counties can have more restrictive criteria and different closures. See [your county’s status](https://covid19.ca.gov/safer-economy).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes. The State Public Health Officer may issue new orders as the public health situation changes.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C12" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -694,10 +694,10 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>If I am not an Essential Critical Infrastructure Worker, can I still leave the house?</v>
+        <v>How does the stay home order interact with local orders to shelter in place? Does it supersede them?</v>
       </c>
       <c r="B13" t="str">
-        <v>Yes. As described in more detail elsewhere in applicable state public health directives (including on this page), there are a wide range of circumstances in which you may leave your home or other place of residence, even if you are not an Essential Critical Infrastructure Worker. For example, you may leave your home to work at any business or other entity that is allowed to open, to engage in in-person worship and protest activities consistent with public health directives, to patronize local businesses, or to care for friends or family members who require assistance (as set forth under [Health care](https://covid19.ca.gov/healthcare/#top)). And errands like these are not the only reasons you may leave your home: you may also leave your home with or without a specific destination in mind (for example, to walk your dog, to engage in physical recreation, or simply to get some fresh air) as long as you maintain physical distancing and comply with any other applicable public health directives.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>This is a statewide order. Counties can have more restrictive criteria and different closures. See [your county’s status](https://covid19.ca.gov/safer-economy).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C13" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -720,10 +720,10 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Are gatherings permitted?</v>
+        <v>If I am not an Essential Critical Infrastructure Worker, can I still leave the house?</v>
       </c>
       <c r="B14" t="str">
-        <v>State public health directives prohibit professional, social and community gatherings. Gatherings are defined as meetings or other events that bring together persons from multiple households at the same time for a shared or group experience in a single room, space, or place such as an auditorium, stadium, arena, large conference room, meeting hall, or other indoor or outdoor space. They pose an especially high danger of transmission and spread of COVID-19.\n\nOn May 25, 2020, in an effort to balance First Amendment interests with public health, the State Public Health Officer created an exception to the prohibition against mass gatherings for faith-based services and cultural ceremonies as well as protests. Those types of gatherings are now permitted indoors so long as they do not exceed 100 attendees or 25% of the capacity of the space in which the gathering is held, whichever is lower. State public health directives now do not prohibit in-person outdoor faith-based services or protests as long as face coverings are worn and physical distancing of 6 feet between persons or groups of persons from different households is maintained at all times. All other gatherings are prohibited until further notice, except as otherwise specifically permitted in state public health directives (including in applicable industry guidance).\n\nCrowds and limited physical distancing increase the risk for COVID-19. If you attended a protest, remember that confidential, free testing is available. [Find a testing location near you](https://urldefense.proofpoint.com/v2/url?u=https-3A__covid19.ca.gov_testing-2Dand-2Dtreatment_-23top&amp;d=DwMGaQ&amp;c=Lr0a7ed3egkbwePCNW4ROg&amp;r=yRsi0eKVK6Khc58oFC32XROAJ-JqVGBGabDv9P6148k&amp;m=Iul4bdNDGFuRu3rXHrxPHNWT2PT2bXFITW3YP1tzG94&amp;s=4qpOZ7lX1S5M_STTblq_XAQNu05ccIFwIyu4bvl9U3c&amp;e=). If you test negative it does not mean that you may not develop COVID-19 later on. Therefore, it is advisable that you self-isolate for 14 days if possible.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- wedding, protest, funeral, banquet, event, outdoor, conference, symposium, rally, rallies, assembly, assemblies, convention, congregation, congregate, congregation, crowd, group, forum, worship --&gt;</v>
+        <v>Yes. As described in more detail elsewhere in applicable state public health directives (including on this page), there are a wide range of circumstances in which you may leave your home or other place of residence, even if you are not an Essential Critical Infrastructure Worker. For example, you may leave your home to work at any business or other entity that is allowed to open, to engage in in-person worship and protest activities consistent with public health directives, to patronize local businesses, or to care for friends or family members who require assistance (as set forth under [Health care](https://covid19.ca.gov/healthcare/#top)). And errands like these are not the only reasons you may leave your home: you may also leave your home with or without a specific destination in mind (for example, to walk your dog, to engage in physical recreation, or simply to get some fresh air) as long as you maintain physical distancing and comply with any other applicable public health directives.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C14" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -746,10 +746,10 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Can I get a haircut?</v>
+        <v>Are gatherings permitted?</v>
       </c>
       <c r="B15" t="str">
-        <v>Yes. Hair salons and barbershops are now open throughout the state with modifications for safety.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Gatherings are defined as meetings or other events that bring together persons from multiple households at the same time for a shared or group experience in a single room, space, or place such as an auditorium, stadium, arena, large conference room, meeting hall, or other indoor or outdoor space. They pose an especially high danger of transmission and spread of COVID-19.\n\nOn May 25, 2020, in an effort to balance First Amendment interests with public health, the State Public Health Officer created an exception to the prohibition against mass gatherings for faith-based services and cultural ceremonies as well as protests. Those types of gatherings are now permitted indoors in counties in Substantial (red), Moderate (orange), and Minimal (yellow) tiers, subject to [certain restrictions](https://covid19.ca.gov/industry-guidance/#worship) in those counties. State public health directives also permit in-person outdoor faith-based services or protests as long as face coverings are worn and physical distancing of 6 feet between persons or groups of persons from different households is maintained at all times.\n\nCrowds and limited physical distancing increase the risk for COVID-19. If you attended a gathering, remember that confidential, free testing is available. [Find a testing location near you](https://urldefense.proofpoint.com/v2/url?u=https-3A__covid19.ca.gov_testing-2Dand-2Dtreatment_-23top&amp;d=DwMGaQ&amp;c=Lr0a7ed3egkbwePCNW4ROg&amp;r=yRsi0eKVK6Khc58oFC32XROAJ-JqVGBGabDv9P6148k&amp;m=Iul4bdNDGFuRu3rXHrxPHNWT2PT2bXFITW3YP1tzG94&amp;s=4qpOZ7lX1S5M_STTblq_XAQNu05ccIFwIyu4bvl9U3c&amp;e=). If you test negative it does not mean that you may not develop COVID-19 later on. Therefore, it is advisable that you self-isolate for 14 days if possible.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C15" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -772,10 +772,10 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Are safety protocols being enforced? How do I report a business that isn’t complying?</v>
+        <v>Can I get a haircut?</v>
       </c>
       <c r="B16" t="str">
-        <v>They are being enforced, and you can report it. Report unsafe conditions or businesses that shouldn’t be open to your local Alcohol Beverage Control, Labor Commissioner’s office, or regional Cal/OSHA office, depending on the type of business. To find these local contacts, see Appendix B of the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- Adding keywords mask masks report reporting enforce enforcement compliance for quick answers purposes --&gt;</v>
+        <v>Yes. Hair salons and barbershops are now open throughout the state with modifications for safety.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C16" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -798,10 +798,10 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>I want to express my political views.  How can I make my voice heard without raising public health concerns?</v>
+        <v>Are safety protocols being enforced? How do I report a business that isn’t complying?</v>
       </c>
       <c r="B17" t="str">
-        <v>There are many ways for you to express your political views without holding a physical, in-person gathering.  For example, you may continue to call or write elected officials, write letters to the editor of news publications, display lawn or window signs, or use online and other electronic media (including Zoom rooms, Twitter feeds, Facebook pages, and other digital forums) to express your views.  \n\nAdditionally, as noted above, you may leave your home for any reason as long as you comply with any other applicable public health directives. When you are otherwise out in public, public health directives do not prevent you from engaging in political expression—such as by wearing or carrying a sign.\n\nIf collective action in physical space is important to you, consider whether you and other participants can safely protest from within your cars.  The State Public Health Officer does not consider in-car activities to be gatherings, if participants stay in their cars and otherwise remain apart from individuals who are not part of their households.  Many activists have organized car-based protests (honking horns, flying flags, displaying signs, and so on) to express their political views while complying with State public health directives.  \n\nWhenever you are considering a protest (including an in-car protest), make sure you comply with all other applicable laws, including any local public-health measures that may be more restrictive than statewide directives and any other applicable local laws.\n\nIf you do wish to engage in in-person protest outside of your car with a group of any size, you must follow the guidelines for political protest gatherings below.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>They are being enforced, and you can report it. Report unsafe conditions or businesses that shouldn’t be open to your local Alcohol Beverage Control, Labor Commissioner’s office, or regional Cal/OSHA office, depending on the type of business. To find these local contacts, see Appendix B of the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- Adding keywords mask masks report reporting enforce enforcement compliance for quick answers purposes --&gt;</v>
       </c>
       <c r="C17" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -824,10 +824,10 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Can I engage in political protest gatherings?</v>
+        <v>I want to express my political views.  How can I make my voice heard without raising public health concerns?</v>
       </c>
       <c r="B18" t="str">
-        <v>Yes, although in-person protests present special public health concerns. \n\nEven with adherence to physical distancing, bringing members of different households together to engage in in-person protest carries a higher risk of widespread transmission of COVID-19.  Such gatherings may result in increased rates of infection, hospitalization, and death, especially among more vulnerable populations. In particular, activities like chanting, shouting, singing, and group recitation negate the risk-reduction achieved through 6 feet of physical distancing. For this reason, people engaging in these activities should wear face coverings at all times.\n\nTherefore, it is strongly recommended that those exercising their right to engage in political expression (including, for example, their right to petition the government) should utilize alternative channels, such as the many online and broadcasting platforms available in the digital age, in place of in-person gatherings. \n\nHowever, state public health directives do not prohibit in-person _outdoor_ protests as long as you maintain a physical distance of 6 feet between persons or groups of persons from different households at all times. When you can’t maintain a safe physical distance of 6 feet from people not in your household, you must wear a face covering or mask. Local Health Officers are advised to consider appropriate limitations on outdoor attendance capacities, factoring their jurisdiction’s key COVID-19 health indicators. Failure to follow these requirements may result in an order to disperse or other enforcement action. Masks and face coverings are strongly recommended.\n\nIn counties in the [Widespread (purple) tier](https://covid19.ca.gov/safer-economy/) indoor protests are not currently permitted. In other counties, state public health directives do not prohibit in-person _indoor_ protests as long as (1) attendance is limited as as required by the [relevant local restrictions](https://covid19.ca.gov/safer-economy) places of worship (2) physical distancing of 6 feet between persons or groups of persons from different households is maintained at all times, and (3) singing and chanting activities are discontinued. Failure to follow these requirements may result in an order to disperse or other enforcement action. Masks and face coverings are required in compliance with CDPH directives.\n\nParticipants must maintain a physical distance of 6 feet from any uniformed peace officers and other public safety personnel present, unless otherwise directed, and follow all other requirements and directives imposed by local health officers and law enforcement, or other applicable authorities.\n\nThis limitation on attendance will be reviewed regularly. This review will assess the impacts of these imposed limits on public health and provide further direction as part of a phased-in restoration of gatherings that implicate the First Amendment.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>There are many ways for you to express your political views without holding a physical, in-person gathering.  For example, you may continue to call or write elected officials, write letters to the editor of news publications, display lawn or window signs, or use online and other electronic media (including Zoom rooms, Twitter feeds, Facebook pages, and other digital forums) to express your views.  \n\nAdditionally, as noted above, you may leave your home for any reason as long as you comply with any other applicable public health directives. When you are otherwise out in public, public health directives do not prevent you from engaging in political expression—such as by wearing or carrying a sign.\n\nIf collective action in physical space is important to you, consider whether you and other participants can safely protest from within your cars.  The State Public Health Officer does not consider in-car activities to be gatherings, if participants stay in their cars and otherwise remain apart from individuals who are not part of their households.  Many activists have organized car-based protests (honking horns, flying flags, displaying signs, and so on) to express their political views while complying with State public health directives.  \n\nWhenever you are considering a protest (including an in-car protest), make sure you comply with all other applicable laws, including any local public-health measures that may be more restrictive than statewide directives and any other applicable local laws.\n\nIf you do wish to engage in in-person protest outside of your car with a group of any size, you must follow the guidelines for political protest gatherings below.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C18" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -850,10 +850,10 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>How do I vote?</v>
+        <v>Can I engage in political protest gatherings?</v>
       </c>
       <c r="B19" t="str">
-        <v>**[Elections are an essential activity](https://files.covid19.ca.gov/pdf/CDPH-to-SOS-Letter-from-Acting-HO-Aug-18-1.pdf).** The Governor has issued [executive orders to ensure elections are safe and accessible](https://www.gov.ca.gov/2020/05/08/governor-newsom-issues-executive-order-to-protect-public-health-by-mailing-every-registered-voter-a-ballot-ahead-of-the-november-general-election/). Vote-by-mail ballots will be sent to all registered voters for the November 3, 2020 General Election. Most counties will provide [three days of early voting](https://www.gov.ca.gov/2020/06/03/governor-newsom-signs-executive-order-on-safe-secure-and-accessible-general-election-in-november/) in-person starting the Saturday before the election. Open ballot drop-box locations will be available between October 6 and November 3, 2020. Existing laws addressing the use of vote-by-mail ballots in California elections remain in effect except where suspended by Executive Order. Find [guidance for the safe administration of elections](https://elections.cdn.sos.ca.gov/ccrov/pdf/2020/july/20154jl.pdf) during COVID-19.\n\n Visit [online voter registration](https://registertovote.ca.gov/) to register to vote or check your voter registration status. \n\nPractice physical distancing and follow other applicable public health directives while engaged in election-related activities. These include collection and drop-off of ballots, and collection of signatures to qualify candidates or measures for the ballot.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes, although in-person protests present special public health concerns. \n\nEven with adherence to physical distancing, bringing members of different households together to engage in in-person protest carries a higher risk of widespread transmission of COVID-19.  Such gatherings may result in increased rates of infection, hospitalization, and death, especially among more vulnerable populations. In particular, activities like chanting, shouting, singing, and group recitation negate the risk-reduction achieved through 6 feet of physical distancing. For this reason, people engaging in these activities should wear face coverings at all times.\n\nTherefore, it is strongly recommended that those exercising their right to engage in political expression (including, for example, their right to petition the government) should utilize alternative channels, such as the many online and broadcasting platforms available in the digital age, in place of in-person gatherings. \n\nHowever, state public health directives do not prohibit in-person _outdoor_ protests as long as you maintain a physical distance of 6 feet between persons or groups of persons from different households at all times. When you can’t maintain a safe physical distance of 6 feet from people not in your household, you must wear a face covering or mask. Local Health Officers are advised to consider appropriate limitations on outdoor attendance capacities, factoring their jurisdiction’s key COVID-19 health indicators. Failure to follow these requirements may result in an order to disperse or other enforcement action. Masks and face coverings are strongly recommended.\n\nIn counties in the [Widespread (purple) tier](https://covid19.ca.gov/safer-economy/), indoor protests are not currently permitted. In other counties, state public health directives do not prohibit in-person _indoor_ protests as long as (1) attendance is limited as as required by the [relevant local restrictions](https://covid19.ca.gov/safer-economy) places of worship (2) physical distancing of 6 feet between persons or groups of persons from different households is maintained at all times, and (3) singing and chanting activities are discontinued. Failure to follow these requirements may result in an order to disperse or other enforcement action. Masks and face coverings are required in compliance with CDPH directives.\n\nParticipants must maintain a physical distance of 6 feet from any uniformed peace officers and other public safety personnel present, unless otherwise directed, and follow all other requirements and directives imposed by local health officers and law enforcement, or other applicable authorities.\n\nThis limitation on attendance will be reviewed regularly. This review will assess the impacts of these imposed limits on public health and provide further direction as part of a phased-in restoration of gatherings that implicate the First Amendment.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C19" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -876,10 +876,10 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>Can I go to church?</v>
+        <v>How do I vote?</v>
       </c>
       <c r="B20" t="str">
-        <v>Yes. Places of worship such as churches, mosques, temples, and synagogues can open throughout the state, with [modifications for safety (PDF)](https://files.covid19.ca.gov/pdf/guidance-places-of-worship--en.pdf).In counties in the [Widespread (purple)](https://covid19.ca.gov/safer-economy) indoor services in places of worship must be discontinued but outdoor and online services are permitted.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>**[Elections are an essential activity](https://files.covid19.ca.gov/pdf/CDPH-to-SOS-Letter-from-Acting-HO-Aug-18-1.pdf).** The Governor has issued [executive orders to ensure elections are safe and accessible](https://www.gov.ca.gov/2020/05/08/governor-newsom-issues-executive-order-to-protect-public-health-by-mailing-every-registered-voter-a-ballot-ahead-of-the-november-general-election/). Vote-by-mail ballots will be sent to all registered voters for the November 3, 2020 General Election. Most counties will provide [three days of early voting](https://www.gov.ca.gov/2020/06/03/governor-newsom-signs-executive-order-on-safe-secure-and-accessible-general-election-in-november/) in-person starting the Saturday before the election. Open ballot drop-box locations will be available between October 6 and November 3, 2020. Existing laws addressing the use of vote-by-mail ballots in California elections remain in effect except where suspended by Executive Order. Find [guidance for the safe administration of elections](https://elections.cdn.sos.ca.gov/ccrov/pdf/2020/july/20154jl.pdf) during COVID-19.\n\n Visit [online voter registration](https://registertovote.ca.gov/) to register to vote or check your voter registration status. \n\nPractice physical distancing and follow other applicable public health directives while engaged in election-related activities. These include collection and drop-off of ballots, and collection of signatures to qualify candidates or measures for the ballot.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C20" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -902,10 +902,10 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>Can I practice my religious faith?</v>
+        <v>Can I go to church?</v>
       </c>
       <c r="B21" t="str">
-        <v>Yes. Practicing your faith is a constitutionally-protected activity and may manifest in many different forms.\n\nAlthough in-person religious gatherings—like other in-person gatherings—have been restricted to prevent the transmission of COVID-19, on May 25, 2020, the State Public Health Officer began to ease restrictions on in-person religious gatherings. In particular, the State Public Health Officer now authorizes County Departments of Public Health to allow collective activities at places of worship, subject to conditions to support a safe, clean environment for employees, interns and trainees, volunteers, scholars, and all other types of workers as well as congregants, worshippers, and visitors.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- church, mosque, synagogue, temple, wedding, funeral, baptism --&gt;</v>
+        <v>Yes. Places of worship such as churches, mosques, temples, and synagogues can open throughout the state, with [modifications for safety (PDF)](https://files.covid19.ca.gov/pdf/guidance-places-of-worship--en.pdf). In counties in the [Widespread (purple)](https://covid19.ca.gov/safer-economy) tier, indoor services in places of worship must be discontinued but outdoor and online services are permitted.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C21" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -928,10 +928,10 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>What conditions must be met to resume religious services and cultural ceremonies at places of worship?</v>
+        <v>Can I practice my religious faith?</v>
       </c>
       <c r="B22" t="str">
-        <v>Information on conditions imposed by the state can be found at [guidance for places of worship (PDF)](https://files.covid19.ca.gov/pdf/guidance-places-of-worship--en.pdf). Additional conditions may be imposed by local public health officials. This guidance does not obligate places of worship to resume in-person activity. It is strongly recommended that places of worship continue to facilitate remote services and other alternatives to in-person religious practice for those who are vulnerable to COVID19.\n\nEven with adherence to physical distancing, convening in a congregational setting of multiple households to practice a personal faith carries a higher risk of widespread transmission of COVID-19, and may result in increased rates of infection, hospitalization, and death, especially among more vulnerable populations. In particular, activities like singing and group recitation dramatically increase the risk of COVID-19 transmission. For this reason, singing and chanting activities must be discontinued at indoor services, and congregants engaging in group recitation should wear face coverings at all times.\n\nPlaces of worship may only open indoor operations when permitted by [relevant local restrictions](https://covid19.ca.gov/safer-economy) and must comply with all applicable attendance limitations and guidance requirements.\n\nLocal Health Officers are advised to consider appropriate limitations on _outdoor_ attendance capacities, factoring their jurisdiction’s key COVID-19 health indicators. At a minimum, outdoor attendance should be limited naturally through implementation of strict physical distancing measures of a minimum of 6 feet between attendees from different households, in addition to other relevant protocols within this document.\n\nThis limitation will be regularly reviewed by the California Department of Public Health.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes. Practicing your faith is a constitutionally-protected activity and may manifest in many different forms.\n\nAlthough in-person religious gatherings—like other in-person gatherings—have been restricted to prevent the transmission of COVID-19, on May 25, 2020, the State Public Health Officer began to ease restrictions on in-person religious gatherings. In particular, the State Public Health Officer now authorizes County Departments of Public Health to allow collective activities at places of worship, subject to conditions to support a safe, clean environment for employees, interns and trainees, volunteers, scholars, and all other types of workers as well as congregants, worshippers, and visitors.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- church, mosque, synagogue, temple, wedding, funeral, baptism --&gt;</v>
       </c>
       <c r="C22" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -954,10 +954,10 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Can children attend group activities (like Sunday school or Hebrew school) at places of worship?</v>
+        <v>What conditions must be met to resume religious services and cultural ceremonies at places of worship?</v>
       </c>
       <c r="B23" t="str">
-        <v>Yes.  Outdoor activities are permitted, and indoor activities are permitted if they comply with the [cohort guidance](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/small-groups-child-youth.aspx).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Information on conditions imposed by the state can be found at [guidance for places of worship (PDF)](https://files.covid19.ca.gov/pdf/guidance-places-of-worship--en.pdf). Additional conditions may be imposed by local public health officials. This guidance does not obligate places of worship to resume in-person activity. It is strongly recommended that places of worship continue to facilitate remote services and other alternatives to in-person religious practice for those who are vulnerable to COVID19.\n\nEven with adherence to physical distancing, convening in a congregational setting of multiple households to practice a personal faith carries a higher risk of widespread transmission of COVID-19, and may result in increased rates of infection, hospitalization, and death, especially among more vulnerable populations. In particular, activities like singing and group recitation dramatically increase the risk of COVID-19 transmission. For this reason, singing and chanting activities must be discontinued at indoor services, and congregants engaging in group recitation should wear face coverings at all times.\n\nPlaces of worship may only open indoor operations when permitted by [relevant local restrictions](https://covid19.ca.gov/safer-economy) and must comply with all applicable attendance limitations and guidance requirements.\n\nLocal Health Officers are advised to consider appropriate limitations on _outdoor_ attendance capacities, factoring their jurisdiction’s key COVID-19 health indicators. At a minimum, outdoor attendance should be limited naturally through implementation of strict physical distancing measures of a minimum of 6 feet between attendees from different households, in addition to other relevant protocols within this document.\n\nThis limitation will be regularly reviewed by the California Department of Public Health.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C23" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -980,10 +980,10 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>When will current conditions change for places of worship?</v>
+        <v>Can children attend group activities (like Sunday school or Hebrew school) at places of worship?</v>
       </c>
       <c r="B24" t="str">
-        <v>The California Department of Public Health, in consultation with county Departments of Public Health, will regularly review and assess the impacts of these imposed limits on public health and provide further direction as part of a phased-in restoration of activities in places of worship.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes.  Outdoor activities are permitted, and indoor activities are permitted if they comply with the [cohort guidance](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/small-groups-child-youth.aspx).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C24" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1006,10 +1006,10 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>Can I still exercise? Take my kids to the park for fresh air? Take a walk around the block?</v>
+        <v>When will current conditions change for places of worship?</v>
       </c>
       <c r="B25" t="str">
-        <v>It’s okay to go outside to go for a walk, to exercise, and participate in healthy activities as long as you **maintain a safe physical distance of 6 feet and gather only with members of your household.** You can also participate in activities at [outdoor recreational facilities](https://files.covid19.ca.gov/pdf/guidance-campgrounds-outdoor-recreation--en.pdf) that are allowed to open. [Parks may be closed](https://covid19.ca.gov/public-recreation/) to help slow the spread of the virus. Young people can participate in sports as permitted by the [youth sports guidance (PDF)](https://files.covid19.ca.gov/pdf/guidance-youth-sports--en.pdf). Check with local officials about park closures in your area. Californians should not travel significant distances for recreation and should stay close to home.\n\nBelow is a list of some outdoor recreational activities.\n\n*   Badminton (singles)\n*   Throwing a baseball/softball\n*   BMX biking\n*   Canoeing (singles)\n*   Crabbing\n*   Cycling\n*   Exploring rock pools\n*   Gardening (not in groups)\n*   Golfing (doubles, only if cart has protective partition)\n*   Hiking (trails/ paths allowing distancing)\n*   Horse riding (singles)\n*   Jogging and running\n*   Kite boarding and kitesurfing\n*   Meditation\n*   Outdoor photography\n*   Picnics (with your household members only)\n*   Quad biking\n*   Rock climbing\n*   Roller skating and rollerblading\n*   Rowing (singles)\n*   Scootering (not in groups)\n*   Skateboarding (not in groups)\n*   Soft martial arts – tai chi, chi kung (not in groups)\n*   Surfing\n*   Tennis and table tennis (singles)\n*   Throwing a football, kicking a soccer ball (not in groups)\n*   Trail running\n*   Trampolining\n*   Tree climbing\n*   Volleyball (singles)\n*   Walk the dog\n*   Wash the car\n*   Watch the sunrise or sunset\n*   Yoga\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>The California Department of Public Health, in consultation with county Departments of Public Health, will regularly review and assess the impacts of these imposed limits on public health and provide further direction as part of a phased-in restoration of activities in places of worship.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C25" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1032,10 +1032,10 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Can I walk my dog? Take my pet to the vet?</v>
+        <v>Can I still exercise? Take my kids to the park for fresh air? Take a walk around the block?</v>
       </c>
       <c r="B26" t="str">
-        <v>You can walk your dog. You can go to the vet or pet hospital if your pet is sick. Remember to wear a face covering and distance yourself at least 6 feet from other pets and owners.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>It’s okay to go outside to go for a walk, to exercise, and participate in healthy activities as long as you **maintain a safe physical distance of 6 feet and gather only with members of your household.** You can also participate in activities at [outdoor recreational facilities](https://files.covid19.ca.gov/pdf/guidance-campgrounds-outdoor-recreation--en.pdf) that are allowed to open. [Parks may be closed](https://covid19.ca.gov/public-recreation/) to help slow the spread of the virus. Young people can participate in sports as permitted by the [youth sports guidance (PDF)](https://files.covid19.ca.gov/pdf/guidance-youth-sports--en.pdf). Check with local officials about park closures in your area. Californians should not travel significant distances for recreation and should stay close to home.\n\nBelow is a list of some outdoor recreational activities.\n\n*   Badminton (singles)\n*   Throwing a baseball/softball\n*   BMX biking\n*   Canoeing (singles)\n*   Crabbing\n*   Cycling\n*   Exploring rock pools\n*   Gardening (not in groups)\n*   Golfing (doubles, only if cart has protective partition)\n*   Hiking (trails/ paths allowing distancing)\n*   Horse riding (singles)\n*   Jogging and running\n*   Kite boarding and kitesurfing\n*   Meditation\n*   Outdoor photography\n*   Picnics (with your household members only)\n*   Quad biking\n*   Rock climbing\n*   Roller skating and rollerblading\n*   Rowing (singles)\n*   Scootering (not in groups)\n*   Skateboarding (not in groups)\n*   Soft martial arts – tai chi, chi kung (not in groups)\n*   Surfing\n*   Tennis and table tennis (singles)\n*   Throwing a football, kicking a soccer ball (not in groups)\n*   Trail running\n*   Trampolining\n*   Tree climbing\n*   Volleyball (singles)\n*   Walk the dog\n*   Wash the car\n*   Watch the sunrise or sunset\n*   Yoga\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C26" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1058,10 +1058,10 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>Can I visit State Parks? What outdoor spaces are open?</v>
+        <v>Can I walk my dog? Take my pet to the vet?</v>
       </c>
       <c r="B27" t="str">
-        <v>State Parks, campgrounds, museums, and visitor centers [may continue to be closed](https://www.parks.ca.gov/?page_id=30350) to help slow the spread of the virus. Starting June 12, some counties may open campgrounds and RV parks. Be sure to check [parks in your area before you travel](https://covid19.ca.gov/public-recreation/). Californians should not travel significant distances for pleasure or recreation and should stay close to home. If you do travel, take steps to keep everyone safe like wearing a face covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently.\n\nYou can walk, run, hike and bike in your local neighborhoods as long as they continue to practice physical distancing of 6 feet. This means avoiding crowded trails and parking lots.\n\nFor information on National Parks, please the [National Park Service website](https://www.nps.gov/aboutus/news/public-health-update.htm).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- park, visitor center, travel, museum, RV parks, recreation, outdoor recreation, sports, RV, tent camping, tent camp, fish, beach, lake, river, event, outdoor event, event planning, hike, walk, bike, exercise, nature, bird watching, public →&lt;/p&gt;--&gt;</v>
+        <v>You can walk your dog. You can go to the vet or pet hospital if your pet is sick. Remember to wear a face covering and distance yourself at least 6 feet from other pets and owners.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C27" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>Can I travel?</v>
+        <v>Can I visit State Parks? What outdoor spaces are open?</v>
       </c>
       <c r="B28" t="str">
-        <v>You can travel for urgent matters or if such travel is essential to your permitted work. Even though businesses around the state are opening up, avoid travelling long distances for vacations or pleasure as much as possible. This is to slow the spread of the coronavirus. Do not travel if you are sick, or if someone in your household has had coronavirus in the last two weeks. Do not travel with someone who is sick.\n\nYou should check with the local health department where you are starting from, along your route, and at your planned destination for information. Know that local rules are constantly changing and may change even after you start your trip. [Check for travel updates](https://www.visitcalifornia.com/latest-covid-19-coronavirus) before you leave your home.\n\nBefore travelling away from your community, consider these questions from the [Center for Disease Control (CDC) travel guidance](https://www.cdc.gov/coronavirus/2019-ncov/travelers/travel-in-the-us.html):\n\n*   Is coronavirus spreading where you are traveling?\n*   Are you or those you are traveling with more likely to get very sick from coronavirus?\n*   Will you be able to keep 6 feet of physical distance from others during or after your trip?\n\nIf you do travel, take steps to keep everyone safe like wearing a face covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently.  \n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- wedding, travel, gathering, tourism, funeral, motel, vacation, airbnb, vrbo, rental home --&gt;</v>
+        <v>State Parks, campgrounds, museums, and visitor centers [may continue to be closed](https://www.parks.ca.gov/?page_id=30350) to help slow the spread of the virus. Starting June 12, some counties may open campgrounds and RV parks. Be sure to check [parks in your area before you travel](https://covid19.ca.gov/public-recreation/). Californians should not travel significant distances for pleasure or recreation and should stay close to home. If you do travel, take steps to keep everyone safe like wearing a face covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently.\n\nYou can walk, run, hike and bike in your local neighborhoods as long as they continue to practice physical distancing of 6 feet. This means avoiding crowded trails and parking lots.\n\n\--&gt;\n\n#### Can I travel?\n\nYou can travel for urgent matters or if such travel is essential to your permitted work. Even though businesses around the state are opening up, avoid travelling long distances for vacations or pleasure as much as possible. This is to slow the spread of the coronavirus. Do not travel if you are sick, or if someone in your household has had coronavirus in the last two weeks. Do not travel with someone who is sick.\n\nYou should check with the local health department where you are starting from, along your route, and at your planned destination for information. Know that local rules are constantly changing and may change even after you start your trip. [Check for travel updates](https://www.visitcalifornia.com/latest-covid-19-coronavirus) before you leave your home.\n\nBefore travelling away from your community, consider these questions from the [Center for Disease Control (CDC) travel guidance](https://www.cdc.gov/coronavirus/2019-ncov/travelers/travel-in-the-us.html):\n\n*   Is coronavirus spreading where you are traveling?\n*   Are you or those you are traveling with more likely to get very sick from coronavirus?\n*   Will you be able to keep 6 feet of physical distance from others during or after your trip?\n\nIf you do travel, take steps to keep everyone safe like wearing a face covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently. \n\n#### Are there travel restrictions within California?\n\nTo prevent further spread of COVID-19, Californians should not travel significant distances and should stay close to home as much as possible.\n\n#### Are there travel restrictions into or out of California?\n\nThere are currently no restrictions for entering California if you are coming from another state in the U.S. The federal government has placed restrictions on certain international travelers. With specific exceptions, foreign nationals who visited certain countries during the past 14 days are prohibited from entry to the United States. All international travelers, including US citizens and permanent residents, should quarantine for 14 days after coming to California from any other country. All travelers should take safety precautions when considering traveling.·       \n\n*   Don’t travel if you have been sick in the past 14 days or if you live with someone with COVID-19·        \n*   Don’t travel with someone who is sick\n*   Wear a mask in public\n*   Wash your hands\n*   Keep 6 feet from anyone you don’t live with\n\n#### Are swimming pools open?\n\nOutdoor swimming pools are allowed to open in all counties in California. Outdoor pools must close slides, rides, or other attractions. \n\nIndoor swimming pools are closed in counties in the [Widespread (purple) or Substantial (red) tiers](https://covid19.ca.gov/safer-economy).\n\nWater parks, both indoor and outdoor, remain closed throughout the state.\n\nWhen out of the water, masks or face coverings should be worn. Physical distancing should be practiced at all times. Group gatherings are not allowed. Bring your own towel, and don’t share items that are worn on the face (like goggles, nose clips, or snorkels). Pool operators should follow heightened cleaning and safety guidance in response to COVID-19. See sector guidance for [gyms and fitness centers](https://files.covid19.ca.gov/pdf/guidance-fitness--en.pdf) and [campgrounds and outdoor recreation](https://files.covid19.ca.gov/pdf/guidance-campgrounds-outdoor-recreation--en.pdf).\n\n### Government services\n\n#### Can I go to the Department of Motor Vehicles (DMV)?\n\nYes, but first check if an in-person visit is required. Several deadlines have been extended, and many DMV services can be accessed online.\n\n##### **Extended deadlines**\n\nDMV has extended deadlines for:\n\n*   Drivers 70 years of age and older with licenses expiring between March 1 through December 31, 2020. Your license is valid for one year from the original expiration date.\n*   Drivers 69 years of age and younger with licenses expiring between March 1 through July 31, 2020. Though the extension has now expired, you can [renew your license online.](https://www.dmv.ca.gov/portal/driver-licenses-identification-cards/driver-license-id-card-online-renewal/) An in-person visit is not required.\n*   Expiring commercial licenses, endorsements, and certificates. They are valid through September 30, 2020.\n*   In-person renewals for vehicle registrations that expire between the dates of March 16, 2020, and May 31, 2020.\n*   In-person renewals for those with safe driving records whose last DMV visit was 15 years ago.\n*   Driver license permits expiring between March and November 2020. They are extended six months or to a date 24 months from the date of application, whichever is earlier.\n*   Commercial learner’s permits expiring between March and September 2020. They are now valid through September 30, 2020.\n\n##### Online services\n\nDMV offers many services that can be handled online, including simple vehicle registration, renewing a driver’s license, getting a duplicate license, and more. See:\n\n*   [DMV Online Services](https://www.dmv.ca.gov/portal/dmv-online/)\n\nSome DMV services that used to require an in-person office visit can now be accessed online, including driver’s license renewals, vehicle registrations, title transfers, temporary driver’s license extensions, commercial driver’s license renewals, and more. See:\n\n*   [DMV Virtual Field Office](https://virtual.dmv.ca.gov/)\n\n##### **In-person visits**\n\nBeginning June 11, [all DMV offices](https://www.dmv.ca.gov/portal/news-and-media/dmv-reopens-remaining-field-offices-to-public/) are open to the public for appointments that require an in-person visit. You will be required to wear a mask and must remain 6 feet apart in line.\n\nIn-person appointments are limited to:\n\n*   Paying registration for a vehicle impounded because of registration-related issues\n*   Reinstating a suspended or revoked driver license\n*   Applying for a reduced-fee or no-fee identification card\n*   Processing commercial driver license transactions\n*   Applying for a disabled person parking placards\n*   Adding an ambulance certificate or firefighter endorsement to a driver license\n*   Verifying a transit training document to drive a transit bus\n*   Processing DMV Express customers for REAL ID transactions, if time and space allows\n*   Behind-the-wheel driving tests\n    *   On June 26, the DMV began behind-the-wheel driving tests. All cancelled driving test appointments will be rescheduled. New tests will not be available until all cancelled appointments are completed. \n    *   For the health and safety of drivers and DMV staff, [you must wear a face covering and will have your temperature checked](https://www.dmv.ca.gov/portal/dmv-expands-its-health-screening-and-temperature-check-protocols-to-protect-customers-and-employees/) before the test.\n\n#### Can I get my car smog checked?\n\nIt depends. Some smog check locations may be closed. The [Bureau of Automotive Repair](https://www.bar.ca.gov/COVID-19_Impacts_on_BAR_Programs_and_Services.aspx) advises drivers to still pay DMV vehicle registration fees to avoid any late fees. However, you will not receive your new registration or year sticker until the smog information has been received by DMV. Once state and local orders or directives are no longer in effect, you can then obtain the required smog check certificate to complete the DMV vehicle registration process.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- park, visitor center, travel, museum, RV parks, recreation, outdoor recreation, sports, RV, tent camping, tent camp, fish, beach, lake, river, event, outdoor event, event planning, hike, walk, bike, exercise, nature, bird watching, public →&lt;/p&gt;&lt;p&gt;For information on National Parks, please the &lt;a href="https://www.nps.gov/aboutus/news/public-health-update.htm"&gt;National Park Service website&lt;/a&gt;.&lt;!-- park, visitor center, travel, museum, RV parks, recreation, outdoor recreation, sports, RV, tent camping, tent camp, fish, beach, lake, river, event, outdoor event, event planning, hike, walk, bike, exercise, nature, bird watching, public →&lt;/p&gt;      &lt;/div&gt;    &lt;/div&gt;  &lt;/div&gt;&lt;/cwds-accordion&gt;--&gt;</v>
       </c>
       <c r="C28" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1110,10 +1110,10 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>Are there travel restrictions within California?</v>
+        <v>Can I travel?</v>
       </c>
       <c r="B29" t="str">
-        <v>To prevent further spread of COVID-19, Californians should not travel significant distances and should stay close to home as much as possible.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>You can travel for urgent matters or if such travel is essential to your permitted work. Even though businesses around the state are opening up, avoid travelling long distances for vacations or pleasure as much as possible. This is to slow the spread of the coronavirus. Do not travel if you are sick, or if someone in your household has had coronavirus in the last two weeks. Do not travel with someone who is sick.\n\nYou should check with the local health department where you are starting from, along your route, and at your planned destination for information. Know that local rules are constantly changing and may change even after you start your trip. [Check for travel updates](https://www.visitcalifornia.com/latest-covid-19-coronavirus) before you leave your home.\n\nBefore travelling away from your community, consider these questions from the [Center for Disease Control (CDC) travel guidance](https://www.cdc.gov/coronavirus/2019-ncov/travelers/travel-in-the-us.html):\n\n*   Is coronavirus spreading where you are traveling?\n*   Are you or those you are traveling with more likely to get very sick from coronavirus?\n*   Will you be able to keep 6 feet of physical distance from others during or after your trip?\n\nIf you do travel, take steps to keep everyone safe like wearing a face covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently.  \n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- wedding, travel, gathering, tourism, funeral, motel, vacation, airbnb, vrbo, rental home --&gt;</v>
       </c>
       <c r="C29" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1136,10 +1136,10 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>Are there travel restrictions into or out of California?</v>
+        <v>Are there travel restrictions within California?</v>
       </c>
       <c r="B30" t="str">
-        <v>There are currently no restrictions for entering California if you are coming from another state in the U.S. The federal government has placed restrictions on certain international travelers. With specific exceptions, foreign nationals who visited certain countries during the past 14 days are prohibited from entry to the United States. All international travelers, including US citizens and permanent residents, should quarantine for 14 days after coming to California from any other country. All travelers should take safety precautions when considering traveling.·       \n\n*   Don’t travel if you have been sick in the past 14 days or if you live with someone with COVID-19·        \n*   Don’t travel with someone who is sick\n*   Wear a mask in public\n*   Wash your hands\n*   Keep 6 feet from anyone you don’t live with\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>To prevent further spread of COVID-19, Californians should not travel significant distances and should stay close to home as much as possible.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C30" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1162,10 +1162,10 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>Are swimming pools open?</v>
+        <v>Are there travel restrictions into or out of California?</v>
       </c>
       <c r="B31" t="str">
-        <v>Outdoor swimming pools are allowed to open in all counties in California. Outdoor pools must close slides, rides, or other attractions. \n\nIndoor swimming pools are closed in counties in the [Widespread (purple) or Substantial (red) tiers](https://covid19.ca.gov/safer-economy).\n\nWater parks, both indoor and outdoor, remain closed throughout the state.\n\nWhen out of the water, masks or face coverings should be worn. Physical distancing should be practiced at all times. Group gatherings are not allowed. Bring your own towel, and don’t share items that are worn on the face (like goggles, nose clips, or snorkels). Pool operators should follow heightened cleaning and safety guidance in response to COVID-19. See sector guidance for [gyms and fitness centers](https://files.covid19.ca.gov/pdf/guidance-fitness--en.pdf) and [campgrounds and outdoor recreation](https://files.covid19.ca.gov/pdf/guidance-campgrounds-outdoor-recreation--en.pdf).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>There are currently no restrictions for entering California if you are coming from another state in the U.S. The federal government has placed restrictions on certain international travelers. With specific exceptions, foreign nationals who visited certain countries during the past 14 days are prohibited from entry to the United States. All international travelers, including US citizens and permanent residents, should quarantine for 14 days after coming to California from any other country. All travelers should take safety precautions when considering traveling.·       \n\n*   Don’t travel if you have been sick in the past 14 days or if you live with someone with COVID-19·        \n*   Don’t travel with someone who is sick\n*   Wear a mask in public\n*   Wash your hands\n*   Keep 6 feet from anyone you don’t live with\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C31" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1188,10 +1188,10 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>Can I go to the Department of Motor Vehicles (DMV)?</v>
+        <v>Are swimming pools open?</v>
       </c>
       <c r="B32" t="str">
-        <v>Yes, but first check if an in-person visit is required. Several deadlines have been extended, and many DMV services can be accessed online.\n\n##### **Extended deadlines**\n\nDMV has extended deadlines for:\n\n*   Drivers 70 years of age and older with licenses expiring between March 1 through December 31, 2020. Your license is valid for one year from the original expiration date.\n*   Drivers 69 years of age and younger with licenses expiring between March 1 through July 31, 2020. Though the extension has now expired, you can [renew your license online.](https://www.dmv.ca.gov/portal/driver-licenses-identification-cards/driver-license-id-card-online-renewal/) An in-person visit is not required.\n*   Expiring commercial licenses, endorsements, and certificates. They are valid through September 30, 2020.\n*   In-person renewals for vehicle registrations that expire between the dates of March 16, 2020, and May 31, 2020.\n*   In-person renewals for those with safe driving records whose last DMV visit was 15 years ago.\n*   Driver license permits expiring between March and November 2020. They are extended six months or to a date 24 months from the date of application, whichever is earlier.\n*   Commercial learner’s permits expiring between March and September 2020. They are now valid through September 30, 2020.\n\n##### Online services\n\nDMV offers many services that can be handled online, including simple vehicle registration, renewing a driver’s license, getting a duplicate license, and more. See:\n\n*   [DMV Online Services](https://www.dmv.ca.gov/portal/dmv-online/)\n\nSome DMV services that used to require an in-person office visit can now be accessed online, including driver’s license renewals, vehicle registrations, title transfers, temporary driver’s license extensions, commercial driver’s license renewals, and more. See:\n\n*   [DMV Virtual Field Office](https://virtual.dmv.ca.gov/)\n\n##### **In-person visits**\n\nBeginning June 11, [all DMV offices](https://www.dmv.ca.gov/portal/news-and-media/dmv-reopens-remaining-field-offices-to-public/) are open to the public for appointments that require an in-person visit. You will be required to wear a mask and must remain 6 feet apart in line.\n\nIn-person appointments are limited to:\n\n*   Paying registration for a vehicle impounded because of registration-related issues\n*   Reinstating a suspended or revoked driver license\n*   Applying for a reduced-fee or no-fee identification card\n*   Processing commercial driver license transactions\n*   Applying for a disabled person parking placards\n*   Adding an ambulance certificate or firefighter endorsement to a driver license\n*   Verifying a transit training document to drive a transit bus\n*   Processing DMV Express customers for REAL ID transactions, if time and space allows\n*   Behind-the-wheel driving tests\n    *   On June 26, the DMV began behind-the-wheel driving tests. All cancelled driving test appointments will be rescheduled. New tests will not be available until all cancelled appointments are completed. \n    *   For the health and safety of drivers and DMV staff, [you must wear a face covering and will have your temperature checked](https://www.dmv.ca.gov/portal/dmv-expands-its-health-screening-and-temperature-check-protocols-to-protect-customers-and-employees/) before the test.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Outdoor swimming pools are allowed to open in all counties in California. Outdoor pools must close slides, rides, or other attractions. \n\nIndoor swimming pools are closed in counties in the [Widespread (purple) or Substantial (red) tiers](https://covid19.ca.gov/safer-economy).\n\nWater parks, both indoor and outdoor, remain closed throughout the state.\n\nWhen out of the water, masks or face coverings should be worn. Physical distancing should be practiced at all times. Group gatherings are not allowed. Bring your own towel, and don’t share items that are worn on the face (like goggles, nose clips, or snorkels). Pool operators should follow heightened cleaning and safety guidance in response to COVID-19. See sector guidance for [gyms and fitness centers](https://files.covid19.ca.gov/pdf/guidance-fitness--en.pdf) and [campgrounds and outdoor recreation](https://files.covid19.ca.gov/pdf/guidance-campgrounds-outdoor-recreation--en.pdf).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C32" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1214,10 +1214,10 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>Can I get my car smog checked?</v>
+        <v>Can I go to the Department of Motor Vehicles (DMV)?</v>
       </c>
       <c r="B33" t="str">
-        <v>It depends. Some smog check locations may be closed. The [Bureau of Automotive Repair](https://www.bar.ca.gov/COVID-19_Impacts_on_BAR_Programs_and_Services.aspx) advises drivers to still pay DMV vehicle registration fees to avoid any late fees. However, you will not receive your new registration or year sticker until the smog information has been received by DMV. Once state and local orders or directives are no longer in effect, you can then obtain the required smog check certificate to complete the DMV vehicle registration process.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes, but first check if an in-person visit is required. Several deadlines have been extended, and many DMV services can be accessed online.\n\n##### **Extended deadlines**\n\nDMV has extended deadlines for:\n\n*   Drivers 70 years of age and older with licenses expiring between March 1 through December 31, 2020. Your license is valid for one year from the original expiration date.\n*   Drivers 69 years of age and younger with licenses expiring between March 1 through July 31, 2020. Though the extension has now expired, you can [renew your license online.](https://www.dmv.ca.gov/portal/driver-licenses-identification-cards/driver-license-id-card-online-renewal/) An in-person visit is not required.\n*   Expiring commercial licenses, endorsements, and certificates. They are valid through September 30, 2020.\n*   In-person renewals for vehicle registrations that expire between the dates of March 16, 2020, and May 31, 2020.\n*   In-person renewals for those with safe driving records whose last DMV visit was 15 years ago.\n*   Driver license permits expiring between March and November 2020. They are extended six months or to a date 24 months from the date of application, whichever is earlier.\n*   Commercial learner’s permits expiring between March and September 2020. They are now valid through September 30, 2020.\n\n##### Online services\n\nDMV offers many services that can be handled online, including simple vehicle registration, renewing a driver’s license, getting a duplicate license, and more. See:\n\n*   [DMV Online Services](https://www.dmv.ca.gov/portal/dmv-online/)\n\nSome DMV services that used to require an in-person office visit can now be accessed online, including driver’s license renewals, vehicle registrations, title transfers, temporary driver’s license extensions, commercial driver’s license renewals, and more. See:\n\n*   [DMV Virtual Field Office](https://virtual.dmv.ca.gov/)\n\n##### **In-person visits**\n\nBeginning June 11, [all DMV offices](https://www.dmv.ca.gov/portal/news-and-media/dmv-reopens-remaining-field-offices-to-public/) are open to the public for appointments that require an in-person visit. You will be required to wear a mask and must remain 6 feet apart in line.\n\nIn-person appointments are limited to:\n\n*   Paying registration for a vehicle impounded because of registration-related issues\n*   Reinstating a suspended or revoked driver license\n*   Applying for a reduced-fee or no-fee identification card\n*   Processing commercial driver license transactions\n*   Applying for a disabled person parking placards\n*   Adding an ambulance certificate or firefighter endorsement to a driver license\n*   Verifying a transit training document to drive a transit bus\n*   Processing DMV Express customers for REAL ID transactions, if time and space allows\n*   Behind-the-wheel driving tests\n    *   On June 26, the DMV began behind-the-wheel driving tests. All cancelled driving test appointments will be rescheduled. New tests will not be available until all cancelled appointments are completed. \n    *   For the health and safety of drivers and DMV staff, [you must wear a face covering and will have your temperature checked](https://www.dmv.ca.gov/portal/dmv-expands-its-health-screening-and-temperature-check-protocols-to-protect-customers-and-employees/) before the test.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C33" t="str">
         <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
@@ -1240,13 +1240,13 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>What if I don’t have health insurance and I need COVID-19 diagnosis, testing or treatment?</v>
+        <v>Can I get my car smog checked?</v>
       </c>
       <c r="B34" t="str">
-        <v>The cost of needed COVID-19 diagnosis, testing and treatment for the uninsured is [paid for by the government](https://www.hrsa.gov/CovidUninsuredClaim). Check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by talking to your doctor. Medically necessary [testing](https://covid19.ca.gov/testing-and-treatment/) is also free through Verily’s Project Baseline or OptumServe\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>It depends. Some smog check locations may be closed. The [Bureau of Automotive Repair](https://www.bar.ca.gov/COVID-19_Impacts_on_BAR_Programs_and_Services.aspx) advises drivers to still pay DMV vehicle registration fees to avoid any late fees. However, you will not receive your new registration or year sticker until the smog information has been received by DMV. Once state and local orders or directives are no longer in effect, you can then obtain the required smog check certificate to complete the DMV vehicle registration process.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C34" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
       </c>
       <c r="D34" t="str">
         <v xml:space="preserve"> </v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>Does my health plan have to cover my COVID-19 test?</v>
+        <v>Can my pet test positive for coronavirus? Can I take my pet to the vet?</v>
       </c>
       <c r="B35" t="str">
-        <v>Yes, if you:\n\n*   Have COVID-19 symptoms,\n*   Were exposed to someone who has COVID-19, or\n*   The test is medically necessary for your situation. \n\nIf you have COVID-19 symptoms or think you’ve been exposed, under federal law, you can get a test anywhere and your health plan must pay for it.\n\nIf you are an [essential worker](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf), your health plan must cover your COVID-19 test. But you must contact your health plan before getting tested. \n\nIf none of these things above are true but you’d still like a test, contact your health plan or health care provider.\n\nAs a first step, you can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>While we are still learning about coronavirus, the risk of your pet testing positive for coronavirus is low. Because [there is still a risk](https://www.cdc.gov/coronavirus/2019-ncov/animals/pets-other-animals.html), keep your pets away from other pets and people outside of your household. Do not put face coverings on pets as this could harm your pet.\n\nYou can go to the vet or pet hospital if your pet is sick. Remember to wear a cloth face covering and to distance yourself at least 6 feet from other pets and owners.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
       </c>
       <c r="C35" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
       </c>
       <c r="D35" t="str">
         <v xml:space="preserve"> </v>
@@ -1292,10 +1292,10 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>How long will I have to wait to get a coronavirus test?</v>
+        <v>What if I don’t have health insurance and I need COVID-19 diagnosis, testing or treatment?</v>
       </c>
       <c r="B36" t="str">
-        <v>Your wait time depends on why you are seeking a test. \n\n**If you have COVID-19 symptoms or think you were exposed,** under federal law, you can go immediately to any testing site. Find a testing site on our [Testing page](https://covid19.ca.gov/testing-and-treatment/#top), or call your health plan for an available testing location.\n\n**If you are an [essential worker](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf),** your health plan must offer you a test appointment within 48 hours. The testing site must be within 15 miles or 30 minutes of your home or workplace. If your health plan can’t find you such an appointment, then you can go to any available testing site. Your health plan will pay for the test. \n\n**If neither of these cases above are true,** your provider may still decide that a COVID-19 test is medically necessary for you. In that case, your health plan must offer you a test appointment within 96 hours. The testing site must be within 15 miles or 30 minutes of your home or workplace. If your health plan can’t find you such an appointment, then you can go to any available testing site.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>The cost of needed COVID-19 diagnosis, testing and treatment for the uninsured is [paid for by the government](https://www.hrsa.gov/CovidUninsuredClaim). Check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by talking to your doctor. Medically necessary [testing](https://covid19.ca.gov/testing-and-treatment/) is also free through Verily’s Project Baseline or OptumServe\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C36" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1318,10 +1318,10 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>I get my health care coverage through my employer, who has a “self-insured” plan. Do the California Department of Managed Health Care (DMHC) regulations apply to me?</v>
+        <v>Does my health plan have to cover my COVID-19 test?</v>
       </c>
       <c r="B37" t="str">
-        <v>Self-insured plans are regulated by the federal government, not the state. If you have COVID-19 symptoms or were exposed to someone with symptoms, under federal law, your self-insured plan must cover your test. In all other instances, you should talk to your plan to find out whether they will cover COVID-19 testing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes, if you:\n\n*   Have COVID-19 symptoms,\n*   Were exposed to someone who has COVID-19, or\n*   The test is medically necessary for your situation. \n\nIf you have COVID-19 symptoms or think you’ve been exposed, under federal law, you can get a test anywhere and your health plan must pay for it.\n\nIf you are an [essential worker](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf), your health plan must cover your COVID-19 test. But you must contact your health plan before getting tested. \n\nIf none of these things above are true but you’d still like a test, contact your health plan or health care provider.\n\nAs a first step, you can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C37" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1344,10 +1344,10 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>How does my health plan know if I’m an essential worker?</v>
+        <v>How long will I have to wait to get a coronavirus test?</v>
       </c>
       <c r="B38" t="str">
-        <v>Your health plan can ask you questions about why you want a COVID-19 test and about the nature of your work. This helps them determine whether a COVID-19 test is medically necessary for you.\n\nBut they can’t ask you to provide further documentation or evidence of your work status. For example, they can’t ask you to provide written proof of where you work or the conditions of your workplace.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Your wait time depends on why you are seeking a test. \n\n**If you have COVID-19 symptoms or think you were exposed,** under federal law, you can go immediately to any testing site. Find a testing site on our [Testing page](https://covid19.ca.gov/testing-and-treatment/#top), or call your health plan for an available testing location.\n\n**If you are an [essential worker](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf),** your health plan must offer you a test appointment within 48 hours. The testing site must be within 15 miles or 30 minutes of your home or workplace. If your health plan can’t find you such an appointment, then you can go to any available testing site. Your health plan will pay for the test. \n\n**If neither of these cases above are true,** your provider may still decide that a COVID-19 test is medically necessary for you. In that case, your health plan must offer you a test appointment within 96 hours. The testing site must be within 15 miles or 30 minutes of your home or workplace. If your health plan can’t find you such an appointment, then you can go to any available testing site.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C38" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1370,10 +1370,10 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>I have a concern or complaint about getting care for COVID-19 under my health insurance. What can I do?</v>
+        <v>I get my health care coverage through my employer, who has a “self-insured” plan. Do the California Department of Managed Health Care (DMHC) regulations apply to me?</v>
       </c>
       <c r="B39" t="str">
-        <v>If you can’t access care, or were charged in error, follow up with your health plan. Call the member phone number listed on your health plan card. If they don’t fix the problem, call the [California Department of Managed Health Care (DMHC)](http://www.dmhc.ca.gov/?referral=healthhelp.ca.gov) Help Center at [1-888-466-2219](tel:888-466-2219).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Self-insured plans are regulated by the federal government, not the state. If you have COVID-19 symptoms or were exposed to someone with symptoms, under federal law, your self-insured plan must cover your test. In all other instances, you should talk to your plan to find out whether they will cover COVID-19 testing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C39" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1396,10 +1396,10 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>Do Medicare or Medicare Advantage Plans cover coronavirus tests or coronavirus antibody tests?</v>
+        <v>How does my health plan know if I’m an essential worker?</v>
       </c>
       <c r="B40" t="str">
-        <v>Yes. Both [Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) cover [diagnostic](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test), with no out-of-pocket costs.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Your health plan can ask you questions about why you want a COVID-19 test and about the nature of your work. This helps them determine whether a COVID-19 test is medically necessary for you.\n\nBut they can’t ask you to provide further documentation or evidence of your work status. For example, they can’t ask you to provide written proof of where you work or the conditions of your workplace.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C40" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1422,10 +1422,10 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>Can I use telehealth if I am on Medicare?</v>
+        <v>I have a concern or complaint about getting care for COVID-19 under my health insurance. What can I do?</v>
       </c>
       <c r="B41" t="str">
-        <v>Yes. Medicare has expanded its [telehealth services](https://www.medicare.gov/coverage/telehealth) to respond to the public health emergency. You can now use your smartphone, video chat, or online portal from home to talk with a range of providers, like doctors, nurse practitioners, clinical psychologists, licensed clinical social workers, physical therapists, occupational therapists, and speech language pathologists. If you have original Medicare, you can get many services for free through [telehealth](https://covid19.ca.gov/telehealth/). This includes common office visits, mental health counseling, and preventive health screenings.\n\nIf you have a [Medicare Advantage Plan](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans), you have access to these same benefits. Many plans offer more [telehealth](https://covid19.ca.gov/telehealth/) and other benefits, like meal delivery or medical transport. Check with your plan about coverage and costs.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>If you can’t access care, or were charged in error, follow up with your health plan. Call the member phone number listed on your health plan card. If they don’t fix the problem, call the [California Department of Managed Health Care (DMHC)](http://www.dmhc.ca.gov/?referral=healthhelp.ca.gov) Help Center at [1-888-466-2219](tel:888-466-2219).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C41" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>I am uninsured and diagnosed with COVID-19. What testing and treatment for me are paid for by the federal government?</v>
+        <v>Do Medicare or Medicare Advantage Plans cover coronavirus tests or coronavirus antibody tests?</v>
       </c>
       <c r="B42" t="str">
-        <v>The following services are covered:\n\n*   Specimen collection, diagnostic and antibody testing\n*   Testing-related visits, including in the following settings: \n    *   Office \n    *   Urgent care \n    *   Emergency room, or \n    *   Telehealth\n*   Treatment, including:\n    *   Office visit\n    *   [Telehealth](https://covid19.ca.gov/telehealth/#top)\n    *   Emergency room \n    *   Inpatient \n    *   Outpatient/observation \n    *   Skilled nursing facility \n    *   Long-term acute care (LTAC) \n    *   Acute inpatient rehab \n    *   Home health \n    *   Durable Medical Equipment (DME), like oxygen and ventilator\n    *   Emergency ambulance transportation \n    *   Non-emergent patient transfers via ambulance, and\n    *   FDA-approved drugs administered as part of an inpatient stay\n    *   FDA-approved vaccine, when available\n\nFor more details, see the [HRSA website](https://www.hrsa.gov/CovidUninsuredClaim) and their [frequently asked questions](https://www.hrsa.gov/coviduninsuredclaim/frequently-asked-questions).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. Both [Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) cover [diagnostic](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test), with no out-of-pocket costs.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C42" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1474,10 +1474,10 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>Does Medi-Cal provide free COVID-19 diagnosis, testing and treatments for the uninsured?</v>
+        <v>Can I use telehealth if I am on Medicare?</v>
       </c>
       <c r="B43" t="str">
-        <v>Yes. [Medi-Cal is available](https://www.dhcs.ca.gov/services/medi-cal/eligibility/Pages/COVID-19-Presumptive-Eligibility-Program.aspx#:~:text=Presumptive%20Eligibility%20(PE)%20for%20COVID,associated%20office%2C%20clinic%2C%20or%20emergency) to those with no insurance or whose insurance does not cover COVID-19 diagnosis, testing, and treatment. COVID-19 diagnosis, testing and treatment are considered emergency services. This allows all Medi-Cal beneficiaries, regardless of their scope of coverage under Medi-Cal or their immigration status, to receive at no cost all medically necessary testing, testing-related, and treatment services, which may include inpatient or outpatient services related to a COVID-19 diagnosis.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. Medicare has expanded its [telehealth services](https://www.medicare.gov/coverage/telehealth) to respond to the public health emergency. You can now use your smartphone, video chat, or online portal from home to talk with a range of providers, like doctors, nurse practitioners, clinical psychologists, licensed clinical social workers, physical therapists, occupational therapists, and speech language pathologists. If you have original Medicare, you can get many services for free through [telehealth](https://covid19.ca.gov/telehealth/). This includes common office visits, mental health counseling, and preventive health screenings.\n\nIf you have a [Medicare Advantage Plan](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans), you have access to these same benefits. Many plans offer more [telehealth](https://covid19.ca.gov/telehealth/) and other benefits, like meal delivery or medical transport. Check with your plan about coverage and costs.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C43" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1500,10 +1500,10 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>My Medi-Cal eligibility is expiring. Do I need to renew it now?</v>
+        <v>I am uninsured and diagnosed with COVID-19. What testing and treatment for me are paid for by the federal government?</v>
       </c>
       <c r="B44" t="str">
-        <v>**No.** [DHCS instructed counties](https://www.dhcs.ca.gov/services/medi-cal/eligibility/letters/Documents/I20-14.pdf) to freeze the Medi-Cal eligibility redeterminations for the duration of the COVID-19 public health emergency.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>The following services are covered:\n\n*   Specimen collection, diagnostic and antibody testing\n*   Testing-related visits, including in the following settings: \n    *   Office \n    *   Urgent care \n    *   Emergency room, or \n    *   Telehealth\n*   Treatment, including:\n    *   Office visit\n    *   [Telehealth](https://covid19.ca.gov/telehealth/#top)\n    *   Emergency room \n    *   Inpatient \n    *   Outpatient/observation \n    *   Skilled nursing facility \n    *   Long-term acute care (LTAC) \n    *   Acute inpatient rehab \n    *   Home health \n    *   Durable Medical Equipment (DME), like oxygen and ventilator\n    *   Emergency ambulance transportation \n    *   Non-emergent patient transfers via ambulance, and\n    *   FDA-approved drugs administered as part of an inpatient stay\n    *   FDA-approved vaccine, when available\n\nFor more details, see the [HRSA website](https://www.hrsa.gov/CovidUninsuredClaim) and their [frequently asked questions](https://www.hrsa.gov/coviduninsuredclaim/frequently-asked-questions).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C44" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1526,10 +1526,10 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>I don’t have health insurance and/or a regular doctor. How can I get quick access to medical advice?</v>
+        <v>Does Medi-Cal provide free COVID-19 diagnosis, testing and treatments for the uninsured?</v>
       </c>
       <c r="B45" t="str">
-        <v>Call Medi-Nurse. Medi-Nurse is a [free, 24/7 nurse advice line](https://www.dhcs.ca.gov/Pages/DHCS-COVID%E2%80%9119-Medi-Nurse-Line.aspx) available at [1-877-409-9052](tel:877-409-9052). You can speak directly with a healthcare professional about your symptoms, get advice on testing and treatment in your area, or ask how to apply for health insurance.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. [Medi-Cal is available](https://www.dhcs.ca.gov/services/medi-cal/eligibility/Pages/COVID-19-Presumptive-Eligibility-Program.aspx#:~:text=Presumptive%20Eligibility%20(PE)%20for%20COVID,associated%20office%2C%20clinic%2C%20or%20emergency) to those with no insurance or whose insurance does not cover COVID-19 diagnosis, testing, and treatment. COVID-19 diagnosis, testing and treatment are considered emergency services. This allows all Medi-Cal beneficiaries, regardless of their scope of coverage under Medi-Cal or their immigration status, to receive at no cost all medically necessary testing, testing-related, and treatment services, which may include inpatient or outpatient services related to a COVID-19 diagnosis.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C45" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1552,10 +1552,10 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>I am nervous or scared. What can I do?</v>
+        <v>My Medi-Cal eligibility is expiring. Do I need to renew it now?</v>
       </c>
       <c r="B46" t="str">
-        <v>You are not alone. The California Surgeon General released [two playbooks for managing stress](https://covid19.ca.gov/manage-stress-for-health/#top) and tips for care-givers and kids. If you feel like you need to talk to someone and want emotional support see this [list of resources](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/#top).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>**No.** [DHCS instructed counties](https://www.dhcs.ca.gov/services/medi-cal/eligibility/letters/Documents/I20-14.pdf) to freeze the Medi-Cal eligibility redeterminations for the duration of the COVID-19 public health emergency.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C46" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1578,10 +1578,10 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>What if I need to visit a health care provider?</v>
+        <v>I don’t have health insurance and/or a regular doctor. How can I get quick access to medical advice?</v>
       </c>
       <c r="B47" t="str">
-        <v>If you have [coronavirus symptoms](https://covid19.ca.gov/symptoms-and-risks/#top), please contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) or use the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html).\n\nIf you have other illnesses or chronic conditions, use [telehealth](https://covid19.ca.gov/telehealth/) to get care from home.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call [911](tel:911), tell the operator your symptoms so the ambulance provider can be ready to treat you safely.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Call Medi-Nurse. Medi-Nurse is a [free, 24/7 nurse advice line](https://www.dhcs.ca.gov/Pages/DHCS-COVID%E2%80%9119-Medi-Nurse-Line.aspx) available at [1-877-409-9052](tel:877-409-9052). You can speak directly with a healthcare professional about your symptoms, get advice on testing and treatment in your area, or ask how to apply for health insurance.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C47" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1604,10 +1604,10 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>What about routine, elective, or non-urgent medical or dental appointments?</v>
+        <v>I am nervous or scared. What can I do?</v>
       </c>
       <c r="B48" t="str">
-        <v>Non-emergency surgeries, like organ replacements and tumor removals, can take place. Your doctor will know if your hospital has enough capacity and protective equipment. Elective procedures should be cancelled or rescheduled. If possible, health care visits should be done remotely. [Dental services and preventive dental care](https://www.cdc.gov/coronavirus/2019-ncov/hcp/dental-settings.html) may be resumed. Contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) to see what services they are providing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>You are not alone. The California Surgeon General released [two playbooks for managing stress](https://covid19.ca.gov/manage-stress-for-health/#top) and tips for care-givers and kids. If you feel like you need to talk to someone and want emotional support see this [list of resources](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/#top).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C48" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1630,10 +1630,10 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>Can I get my prescriptions filled?</v>
+        <v>What if I need to visit a health care provider?</v>
       </c>
       <c r="B49" t="str">
-        <v>Yes. Pharmacies and medical cannabis dispensaries are open.\n\nCall your doctor to get a new prescription or adjust your existing prescriptions.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>If you have [coronavirus symptoms](https://covid19.ca.gov/symptoms-and-risks/#top), please contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) or use the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html).\n\nIf you have other illnesses or chronic conditions, use [telehealth](https://covid19.ca.gov/telehealth/) to get care from home.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call [911](tel:911), tell the operator your symptoms so the ambulance provider can be ready to treat you safely.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C49" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1656,10 +1656,10 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>I am an older Californian who is isolating at home and I need non-urgent help. What can I do?</v>
+        <v>What about routine, elective, or non-urgent medical or dental appointments?</v>
       </c>
       <c r="B50" t="str">
-        <v>Call the statewide hotline for older Californians at [1-833-544-2374](tel:833-544-2374). They can help you with non-urgent medical needs, meal delivery, tracking down prescriptions, and more. The most important thing you can do is stay home for your health and wellbeing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Non-emergency surgeries, like organ replacements and tumor removals, can take place. Your doctor will know if your hospital has enough capacity and protective equipment. Elective procedures should be cancelled or rescheduled. If possible, health care visits should be done remotely. [Dental services and preventive dental care](https://www.cdc.gov/coronavirus/2019-ncov/hcp/dental-settings.html) may be resumed. Contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) to see what services they are providing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C50" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1682,10 +1682,10 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>How can I make sure the older Californians in my life are safe and healthy during the stay home order?</v>
+        <v>Can I get my prescriptions filled?</v>
       </c>
       <c r="B51" t="str">
-        <v>Check in on your older neighbors and loved ones to make sure they are okay. Give them a call, text, or physically-distanced door knock. You can also teach them how to use FaceTime, Zoom, Google Duo, or Facebook video to communicate. It’s important to keep in touch with older loved ones for their mental health and safety.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. Pharmacies and medical cannabis dispensaries are open.\n\nCall your doctor to get a new prescription or adjust your existing prescriptions.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C51" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1708,10 +1708,10 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>Can I care for my elderly parents or friends who need help? Or a friend or family member who has disabilities?</v>
+        <v>I am an older Californian who is isolating at home and I need non-urgent help. What can I do?</v>
       </c>
       <c r="B52" t="str">
-        <v>Yes. Protect them and yourself by following physical distancing guidelines. Wear a [mask](https://covid19.ca.gov/masks-and-ppe/#top), wash your hands often, maintain at least six feet of distance between you, and cover your cough or sneeze. If you have early signs of a cold, please stay away from your older loved ones.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Call the statewide hotline for older Californians at [1-833-544-2374](tel:833-544-2374). They can help you with non-urgent medical needs, meal delivery, tracking down prescriptions, and more. The most important thing you can do is stay home for your health and wellbeing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C52" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1734,10 +1734,10 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>Can I visit loved ones in the hospital, nursing home, or residential care facility?</v>
+        <v>How can I make sure the older Californians in my life are safe and healthy during the stay home order?</v>
       </c>
       <c r="B53" t="str">
-        <v>Generally, no. There are exceptions, such as if you are taking a minor or someone who is developmentally disabled to the hospital. For most other situations, the order prohibits visitation to these kinds of facilities. This is difficult, but necessary to protect hospital staff and other patients. See more about this in [frequently asked questions for friends and family with a loved one in a skilled nursing or residential care facility](https://www.aging.ca.gov/download.ashx?lE0rcNUV0zaaXLD5JZ%2f6Uw%3d%3d).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Check in on your older neighbors and loved ones to make sure they are okay. Give them a call, text, or physically-distanced door knock. You can also teach them how to use FaceTime, Zoom, Google Duo, or Facebook video to communicate. It’s important to keep in touch with older loved ones for their mental health and safety.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C53" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1760,10 +1760,10 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>Can I get free COVID-19 testing or treatment if I am a senior over 65, disabled, uninsured, or an undocumented immigrant?</v>
+        <v>Can I care for my elderly parents or friends who need help? Or a friend or family member who has disabilities?</v>
       </c>
       <c r="B54" t="str">
-        <v>[Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) provide free COVID-19 [diagnostic](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test). Needed COVID-19 diagnosis, testing, and treatment for the uninsured is [paid for by the government](https://www.hrsa.gov/CovidUninsuredClaim). \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. Protect them and yourself by following physical distancing guidelines. Wear a [mask](https://covid19.ca.gov/masks-and-ppe/#top), wash your hands often, maintain at least six feet of distance between you, and cover your cough or sneeze. If you have early signs of a cold, please stay away from your older loved ones.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C54" t="str">
         <v>https://covid19.ca.gov/healthcare/</v>
@@ -1786,13 +1786,13 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>What do taxpayers need to do if they want to take advantage of relief from the California Department of Tax and Fee Administration?</v>
+        <v>Can I visit loved ones in the hospital, nursing home, or residential care facility?</v>
       </c>
       <c r="B55" t="str">
-        <v>Interested taxpayers should contact CDTFA by visiting the [CDTFA website](http://cdtfa.ca.gov/) or calling [800-400-7115](tel:800-400-7115).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Generally, no. There are exceptions, such as if you are taking a minor or someone who is developmentally disabled to the hospital. For most other situations, the order prohibits visitation to these kinds of facilities. This is difficult, but necessary to protect hospital staff and other patients. See more about this in [frequently asked questions for friends and family with a loved one in a skilled nursing or residential care facility](https://www.aging.ca.gov/download.ashx?lE0rcNUV0zaaXLD5JZ%2f6Uw%3d%3d).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C55" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/healthcare/</v>
       </c>
       <c r="D55" t="str">
         <v xml:space="preserve"> </v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>When will taxpayers start on these payment plans?</v>
+        <v>Can I get free COVID-19 testing or treatment if I am a senior over 65, disabled, uninsured, or an undocumented immigrant?</v>
       </c>
       <c r="B56" t="str">
-        <v>Given that the April deadline to file and pay sales and use tax returns has been extended to late July for all but the largest taxpayers, CDTFA expects that most participating taxpayers will begin their payment arrangements in late July of this year.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>[Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) provide free COVID-19 [diagnostic](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test). Needed COVID-19 diagnosis, testing, and treatment for the uninsured is [paid for by the government](https://www.hrsa.gov/CovidUninsuredClaim). \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
       </c>
       <c r="C56" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/healthcare/</v>
       </c>
       <c r="D56" t="str">
         <v xml:space="preserve"> </v>
@@ -1838,10 +1838,10 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>How will the payment plans work?</v>
+        <v>What do taxpayers need to do if they want to take advantage of relief from the California Department of Tax and Fee Administration?</v>
       </c>
       <c r="B57" t="str">
-        <v>Qualifying sales and use taxpayers with deferred liabilities up to $50,000 will pay their tax due in 12 equal monthly installments. No interest or penalties will be assessed against the liability.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Interested taxpayers should contact CDTFA by visiting the [CDTFA website](http://cdtfa.ca.gov/) or calling [800-400-7115](tel:800-400-7115).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C57" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1864,10 +1864,10 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>Is this only for tax payments due for the 1st quarter of 2020?</v>
+        <v>When will taxpayers start on these payment plans?</v>
       </c>
       <c r="B58" t="str">
-        <v>If taxpayers choose to use this program to distribute the burden of their May or June prepayments or their July return, CDTFA will work to accommodate those taxpayers.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Given that the April deadline to file and pay sales and use tax returns has been extended to late July for all but the largest taxpayers, CDTFA expects that most participating taxpayers will begin their payment arrangements in late July of this year.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C58" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1890,10 +1890,10 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>What if taxpayers owe more than the $50,000 limit on the relief?</v>
+        <v>How will the payment plans work?</v>
       </c>
       <c r="B59" t="str">
-        <v>The maximum amount that any taxpayer can defer interest-free under this relief effort is $50,000.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Qualifying sales and use taxpayers with deferred liabilities up to $50,000 will pay their tax due in 12 equal monthly installments. No interest or penalties will be assessed against the liability.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C59" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1916,10 +1916,10 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>What if taxpayers with more than $5 million in annual taxable sales need this relief?</v>
+        <v>Is this only for tax payments due for the 1st quarter of 2020?</v>
       </c>
       <c r="B60" t="str">
-        <v>We recognize that some taxpayers, particularly in low margin businesses, with annual taxable sales over $5 million may also need this relief. Those taxpayers are encouraged to reach out to CDTFA, which will work with them to provide relief where appropriate.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>If taxpayers choose to use this program to distribute the burden of their May or June prepayments or their July return, CDTFA will work to accommodate those taxpayers.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C60" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1942,10 +1942,10 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>Is the deadline for filing California tax returns extended?</v>
+        <v>What if taxpayers owe more than the $50,000 limit on the relief?</v>
       </c>
       <c r="B61" t="str">
-        <v>Yes. All California taxpayers (individuals and businesses) can file and pay by July 15, 2020. See [information from the CA Franchise Tax Board](https://www.ftb.ca.gov/about-ftb/newsroom/news-releases/2020-3-state-postpones-tax-deadlines-until-july-15-due-to-the-covid-19-pandemic.html) for more information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The maximum amount that any taxpayer can defer interest-free under this relief effort is $50,000.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C61" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1968,10 +1968,10 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>What is a loan guarantee?</v>
+        <v>What if taxpayers with more than $5 million in annual taxable sales need this relief?</v>
       </c>
       <c r="B62" t="str">
-        <v>A loan guarantee is a credit enhancement that helps mitigate the risk assumed by a lending institution when making a loan. With the Small Business Finance Center’s Disaster Relief Loan Guarantee Program, IBank agrees to guarantee up to 95% of the loan, removing the barriers to capital that often exist for small business borrowers that may not otherwise be eligible for traditional lending. This program also can assist those who may not be eligible for a U.S. Small Business Administration (SBA) loan.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>We recognize that some taxpayers, particularly in low margin businesses, with annual taxable sales over $5 million may also need this relief. Those taxpayers are encouraged to reach out to CDTFA, which will work with them to provide relief where appropriate.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C62" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -1994,10 +1994,10 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>Who is eligible to apply for a loan guarantee?</v>
+        <v>Is the deadline for filing California tax returns extended?</v>
       </c>
       <c r="B63" t="str">
-        <v>Small business entities that have been affected by loss, damage or other economic injury due to the COVID-19 pandemic and meet the program’s eligibility requirements. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Yes. All California taxpayers (individuals and businesses) can file and pay by July 15, 2020. See [information from the CA Franchise Tax Board](https://www.ftb.ca.gov/about-ftb/newsroom/news-releases/2020-3-state-postpones-tax-deadlines-until-july-15-due-to-the-covid-19-pandemic.html) for more information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C63" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2020,10 +2020,10 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>What do you consider a small business?</v>
+        <v>What is a loan guarantee?</v>
       </c>
       <c r="B64" t="str">
-        <v>The business must have between 1-750 employees and be established as an entity, including:\n\n*   Sole Proprietor – Individual using legal name as business name that files a Schedule C, Schedule F, or has a fictitious business name or DBA statement\n    *   If the loan appears to be in the name of an individual, evidence of Sole Proprietorship will be required and may include a Schedule C, Schedule F, Seller’s Permit, and/or fictitious business name or DBA statement\n*   Limited Liability Company \n*   Cooperative\n*   Corporation\n*   Partnership\n*   S-Corporation\n*   Not-for-profit\n\nThe program will not accept an _individual_ as the borrower. It is permissible for an individual to be a guarantor or co-borrower on the loan, but the primary borrower must be a small business. It does not consider citizenship or immigration status for eligibility requirements**,** as long as the entity/individual meets the above criteria. Trucking owners/operators are eligible as long as they are registered as a legal business entity.\n\n**AND**\n\n*   The business activity must be eligible under the program and in one of the industries listed in the [North American Industry Classification System (NAICS) codes list](http://www.census.gov/eos/www/naics), and\n*   It must be located in a declared disaster area. A major disaster area declaration was made for the state of California on March 22, 2020 in regards to the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>A loan guarantee is a credit enhancement that helps mitigate the risk assumed by a lending institution when making a loan. With the Small Business Finance Center’s Disaster Relief Loan Guarantee Program, IBank agrees to guarantee up to 95% of the loan, removing the barriers to capital that often exist for small business borrowers that may not otherwise be eligible for traditional lending. This program also can assist those who may not be eligible for a U.S. Small Business Administration (SBA) loan.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C64" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2046,10 +2046,10 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>What are excluded businesses?</v>
+        <v>Who is eligible to apply for a loan guarantee?</v>
       </c>
       <c r="B65" t="str">
-        <v>Businesses that are not eligible include passive real estate businesses (rental income, etc.).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Small business entities that have been affected by loss, damage or other economic injury due to the COVID-19 pandemic and meet the program’s eligibility requirements. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C65" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2072,10 +2072,10 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>Can I apply for a loan guarantee only if I am ineligible for federal disaster fund financing, such as a SBA loan?</v>
+        <v>What do you consider a small business?</v>
       </c>
       <c r="B66" t="str">
-        <v>Yes, this program is designed for those who do not qualify for federal programs. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The business must have between 1-750 employees and be established as an entity, including:\n\n*   Sole Proprietor – Individual using legal name as business name that files a Schedule C, Schedule F, or has a fictitious business name or DBA statement\n    *   If the loan appears to be in the name of an individual, evidence of Sole Proprietorship will be required and may include a Schedule C, Schedule F, Seller’s Permit, and/or fictitious business name or DBA statement\n*   Limited Liability Company \n*   Cooperative\n*   Corporation\n*   Partnership\n*   S-Corporation\n*   Not-for-profit\n\nThe program will not accept an _individual_ as the borrower. It is permissible for an individual to be a guarantor or co-borrower on the loan, but the primary borrower must be a small business. It does not consider citizenship or immigration status for eligibility requirements**,** as long as the entity/individual meets the above criteria. Trucking owners/operators are eligible as long as they are registered as a legal business entity.\n\n**AND**\n\n*   The business activity must be eligible under the program and in one of the industries listed in the [North American Industry Classification System (NAICS) codes list](http://www.census.gov/eos/www/naics), and\n*   It must be located in a declared disaster area. A major disaster area declaration was made for the state of California on March 22, 2020 in regards to the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C66" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2098,10 +2098,10 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>How much can I borrow?</v>
+        <v>What are excluded businesses?</v>
       </c>
       <c r="B67" t="str">
-        <v>The Small Business Finance Center’s Disaster Relief Loan Guarantee Program allows a maximum loan of $1.25 million and a maximum guarantee of $1 million. To serve as many California small businesses as possible, the COVID-19 disaster program is focused on serving small businesses, especially those in low-wealth and immigrant communities with needs from $500 to $50,000. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Businesses that are not eligible include passive real estate businesses (rental income, etc.).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C67" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2124,10 +2124,10 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>What are the loan terms?</v>
+        <v>Can I apply for a loan guarantee only if I am ineligible for federal disaster fund financing, such as a SBA loan?</v>
       </c>
       <c r="B68" t="str">
-        <v>The length of the loan can be negotiated with your lender, but the guarantee is good for up to seven years. The interest rate and loan criteria will be determined by the lender and could depend on the credit strength of the business. The guarantee is designed to lower the interest rate in exchange for a higher guarantee to your lender. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Yes, this program is designed for those who do not qualify for federal programs. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C68" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2150,10 +2150,10 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>How can I apply for a loan guarantee?</v>
+        <v>How much can I borrow?</v>
       </c>
       <c r="B69" t="str">
-        <v>The Small Business Finance Center partners with Community Development Financial Institutions (CDFIs), Community Lending Institutions, and Financial Development Corporations (FDCs) to provide loan guarantees for small businesses.  To apply,\n\n*   View the [list of FDCs and participating lenders](http://www.ibank.ca.gov/small-business-finance-center/) interested in this Small Business Disaster Relief Loan Guarantee Program. \n*   Contact the lender on the list nearest to your business to apply.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The Small Business Finance Center’s Disaster Relief Loan Guarantee Program allows a maximum loan of $1.25 million and a maximum guarantee of $1 million. To serve as many California small businesses as possible, the COVID-19 disaster program is focused on serving small businesses, especially those in low-wealth and immigrant communities with needs from $500 to $50,000. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C69" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2176,10 +2176,10 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>What is the timing for the funding of loans?</v>
+        <v>What are the loan terms?</v>
       </c>
       <c r="B70" t="str">
-        <v>The program is in place and businesses can apply immediately. Once you provide your lender with complete information, you could be funded in a matter of days.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The length of the loan can be negotiated with your lender, but the guarantee is good for up to seven years. The interest rate and loan criteria will be determined by the lender and could depend on the credit strength of the business. The guarantee is designed to lower the interest rate in exchange for a higher guarantee to your lender. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C70" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2202,10 +2202,10 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>What can the money be used for?</v>
+        <v>How can I apply for a loan guarantee?</v>
       </c>
       <c r="B71" t="str">
-        <v>The funds are meant to help small businesses through this challenging time. Loan proceeds can be used for business continuance or to cure “economic injury” as a result of COVID-19.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The Small Business Finance Center partners with Community Development Financial Institutions (CDFIs), Community Lending Institutions, and Financial Development Corporations (FDCs) to provide loan guarantees for small businesses.  To apply,\n\n*   View the [list of FDCs and participating lenders](http://www.ibank.ca.gov/small-business-finance-center/) interested in this Small Business Disaster Relief Loan Guarantee Program. \n*   Contact the lender on the list nearest to your business to apply.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C71" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2228,10 +2228,10 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>How will this program assist low-wealth and minority communities?</v>
+        <v>What is the timing for the funding of loans?</v>
       </c>
       <c r="B72" t="str">
-        <v>By working with the Community Development Financial Institutions (CDFIs) throughout the state of California, this disaster relief program can play an important role in generating economic growth and opportunity in some of our most distressed communities. CDFIs and mission-based lenders play a vital role across the state and have experience steering lending and investment to where it is needed and will matter the most, in particular in low-wealth and immigrant communities. CDFIs and our partner Financial Development Corporations (FDCs) that process the loan guarantees are embedded in communities across the state, speak several languages, and are invested in the community successfully managing its way through this pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The program is in place and businesses can apply immediately. Once you provide your lender with complete information, you could be funded in a matter of days.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C72" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2254,10 +2254,10 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>Are faith-based businesses eligible for this loan guarantee program?</v>
+        <v>What can the money be used for?</v>
       </c>
       <c r="B73" t="str">
-        <v>Faith-based businesses (non-profit or otherwise) that have business activity outside of worship are eligible as long as they are a legal business that has been affected by the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The funds are meant to help small businesses through this challenging time. Loan proceeds can be used for business continuance or to cure “economic injury” as a result of COVID-19.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C73" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2280,10 +2280,10 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>What SBA programs are available to small businesses right now?</v>
+        <v>How will this program assist low-wealth and minority communities?</v>
       </c>
       <c r="B74" t="str">
-        <v>The U.S. SBA offers the **Economic Injury Disaster Loan (EIDL)**.\n\nThe U.S. SBA is accepting new applications from all eligible businesses, and will continue to process **EIDL Loan applications** already submitted on a first come, first-served basis. Check the U.S. SBA’s [Disaster Loan Applications website](https://www.sba.gov/page/disaster-loan-applications#section-header-0) for more information.\n\nThe EIDL is a direct loan for up to $2 million at a rate of 3.75% for small businesses and 2.75% for nonprofits. [Apply directly with the SBA](https://covid19relief.sba.gov/#/). For questions, you can contact SBA’s Customer Service Line at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or send an email to [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nThe **Economic Injury Disaster Loan (**EIDL) **Advance** has been [discontinued](https://www.sba.gov/page/disaster-loan-applications#section-header-0). EIDL loan applications will still be processed even though the Advance is no longer available.\n\nThe [**Paycheck Protection Program (PPP)**](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program#section-header-0) closed August 8, 2020. The U.S. SBA is no longer accepting PPP applications from approved lenders.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>By working with the Community Development Financial Institutions (CDFIs) throughout the state of California, this disaster relief program can play an important role in generating economic growth and opportunity in some of our most distressed communities. CDFIs and mission-based lenders play a vital role across the state and have experience steering lending and investment to where it is needed and will matter the most, in particular in low-wealth and immigrant communities. CDFIs and our partner Financial Development Corporations (FDCs) that process the loan guarantees are embedded in communities across the state, speak several languages, and are invested in the community successfully managing its way through this pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C74" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2306,10 +2306,10 @@
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>Where do I find more information on allowable expenses for a forgivable loan under the Paycheck Protection Program?</v>
+        <v>Are faith-based businesses eligible for this loan guarantee program?</v>
       </c>
       <c r="B75" t="str">
-        <v>You can find this on the Paycheck Protection Program’s [Loan Forgiveness Application](https://www.sba.gov/sites/default/files/2020-06/PPP%20Loan%20Forgiveness%20Application%20%28Revised%206.16.2020%29-fillable_0-508.pdf). The application provides detailed [instructions](https://www.sba.gov/sites/default/files/2020-06/PPP%20Loan%20Forgiveness%20Application%20Instructions%20%28Revised%206.16.2020%29-508.pdf) on how to apply for forgiveness of PPP loans. Once your business has expended the PPP funds and is ready to pursue loan forgiveness, please review the Loan Forgiveness Application and consult with your accountant, lender, or one of California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) for assistance. See SBA’s [loan details and forgiveness](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program#section-header-5) information, and check the [frequently asked questions](https://www.sba.gov/sites/default/files/2020-08/PPP%20--%20Loan%20Forgiveness%20FAQs%20%28August%2011%2C%202020%29.pdf) on PPP loan forgiveness.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Faith-based businesses (non-profit or otherwise) that have business activity outside of worship are eligible as long as they are a legal business that has been affected by the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C75" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2332,10 +2332,10 @@
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>How does a business know if it is eligible for an SBA loan or loan guarantee program?</v>
+        <v>What SBA programs are available to small businesses right now?</v>
       </c>
       <c r="B76" t="str">
-        <v>Small businesses with 500 employees or less are eligible to apply for the Small Business Debt Relief Program. Small businesses are also eligible to apply for the Economic Injury Disaster Loan (EIDL) program. Visit SBA’s comprehensive [COVID-19 support website](https://www.sba.gov/page/coronavirus-covid-19-small-business-guidance-loan-resources#section-header-4%20.) to find out more about SBA’s eligibility requirements for each program.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The U.S. SBA offers the **Economic Injury Disaster Loan (EIDL)**.\n\nThe U.S. SBA is accepting new applications from all eligible businesses, and will continue to process **EIDL Loan applications** already submitted on a first come, first-served basis. Check the U.S. SBA’s [Disaster Loan Applications website](https://www.sba.gov/page/disaster-loan-applications#section-header-0) for more information.\n\nThe EIDL is a direct loan for up to $2 million at a rate of 3.75% for small businesses and 2.75% for nonprofits. [Apply directly with the SBA](https://covid19relief.sba.gov/#/). For questions, you can contact SBA’s Customer Service Line at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or send an email to [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nThe **Economic Injury Disaster Loan (**EIDL) **Advance** has been [discontinued](https://www.sba.gov/page/disaster-loan-applications#section-header-0). EIDL loan applications will still be processed even though the Advance is no longer available.\n\nThe [**Paycheck Protection Program (PPP)**](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program#section-header-0) closed August 8, 2020. The U.S. SBA is no longer accepting PPP applications from approved lenders.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C76" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2358,10 +2358,10 @@
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>How do I reach SBA for any questions or assistance?</v>
+        <v>Where do I find more information on allowable expenses for a forgivable loan under the Paycheck Protection Program?</v>
       </c>
       <c r="B77" t="str">
-        <v>SBA has district offices in California that are open to answer questions. You can use the [SBA’s Local Assistance Directory](https://www.sba.gov/local-assistance) to locate the office nearest you. You can also contact the SBA by phone at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or by email at [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).  \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>You can find this on the Paycheck Protection Program’s [Loan Forgiveness Application](https://www.sba.gov/sites/default/files/2020-06/PPP%20Loan%20Forgiveness%20Application%20%28Revised%206.16.2020%29-fillable_0-508.pdf). The application provides detailed [instructions](https://www.sba.gov/sites/default/files/2020-06/PPP%20Loan%20Forgiveness%20Application%20Instructions%20%28Revised%206.16.2020%29-508.pdf) on how to apply for forgiveness of PPP loans. Once your business has expended the PPP funds and is ready to pursue loan forgiveness, please review the Loan Forgiveness Application and consult with your accountant, lender, or one of California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) for assistance. See SBA’s [loan details and forgiveness](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program#section-header-5) information, and check the [frequently asked questions](https://www.sba.gov/sites/default/files/2020-08/PPP%20--%20Loan%20Forgiveness%20FAQs%20%28August%2011%2C%202020%29.pdf) on PPP loan forgiveness.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C77" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2384,10 +2384,10 @@
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>How does a small business know which SBA loan or loan guarantee program is the right one? Can a small business apply to more than one?</v>
+        <v>How does a business know if it is eligible for an SBA loan or loan guarantee program?</v>
       </c>
       <c r="B78" t="str">
-        <v>Call or email the SBA to find out which program is right for you. While businesses can apply for and receive more than one form of capital assistance through the SBA, they cannot be used for the same purpose. The SBA can advise you on your options. Call [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or email [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Small businesses with 500 employees or less are eligible to apply for the Small Business Debt Relief Program. Small businesses are also eligible to apply for the Economic Injury Disaster Loan (EIDL) program. Visit SBA’s comprehensive [COVID-19 support website](https://www.sba.gov/page/coronavirus-covid-19-small-business-guidance-loan-resources#section-header-4%20.) to find out more about SBA’s eligibility requirements for each program.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C78" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2410,10 +2410,10 @@
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>How do I get SBA to cover my loan payments on my existing 7(a), 504, or microloan if I cannot pay due to COVID-19?</v>
+        <v>How do I reach SBA for any questions or assistance?</v>
       </c>
       <c r="B79" t="str">
-        <v>SBA has a [Debt Relief program](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/sba-debt-relief) and will pay the principal and interest of existing SBA loans. Please contact your lender for information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>SBA has district offices in California that are open to answer questions. You can use the [SBA’s Local Assistance Directory](https://www.sba.gov/local-assistance) to locate the office nearest you. You can also contact the SBA by phone at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or by email at [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).  \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C79" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2436,10 +2436,10 @@
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>If I need help to figure out which program is best for me or to submit an application, where can I find support?</v>
+        <v>How does a small business know which SBA loan or loan guarantee program is the right one? Can a small business apply to more than one?</v>
       </c>
       <c r="B80" t="str">
-        <v>California’s network of small business support centers can help you figure out which loans and programs are best for your business, develop resiliency strategies, and find other resources. Go to California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) to find the closest center.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Call or email the SBA to find out which program is right for you. While businesses can apply for and receive more than one form of capital assistance through the SBA, they cannot be used for the same purpose. The SBA can advise you on your options. Call [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or email [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C80" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2462,10 +2462,10 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>How do I maintain a safe workplace?</v>
+        <v>How do I get SBA to cover my loan payments on my existing 7(a), 504, or microloan if I cannot pay due to COVID-19?</v>
       </c>
       <c r="B81" t="str">
-        <v>As California reopens, every business will need to create a safer, low-risk environment. If you own or manage a business, follow the [industry-specific guidance](https://covid19.ca.gov/industry-guidance/) that applies to protect your workers and customers.\n\nIf your business is approved to reopen, you should take steps to ensure the safety and health of your workers. It’s important that employees with COVID-19 know they should stay home. Your sick leave policies need to support that. \n\n*   Encourage sick employees to stay home if they are sick. See government programs supporting [COVID-19 sick leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) and [workers’ compensation](https://www.labor.ca.gov/coronavirus2019/#chart).\n*   Establish routine cleaning throughout the workplace.\n*   Reduce travel. If possible, encourage video conferencing and limit larger gatherings.\n*   See [Cal/OSHA interim guidelines for general industry](https://www.dir.ca.gov/dosh/coronavirus/General-Industry.html).\n*   Follow [CDC guidance on keeping the workplace safe (PDF)](https://www.cdc.gov/coronavirus/2019-ncov/downloads/workplace-school-and-home-guidance.pdf).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>SBA has a [Debt Relief program](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/sba-debt-relief) and will pay the principal and interest of existing SBA loans. Please contact your lender for information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C81" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2488,10 +2488,10 @@
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>Should a business owner notify customers if an employee has been exposed to COVID-19?</v>
+        <v>If I need help to figure out which program is best for me or to submit an application, where can I find support?</v>
       </c>
       <c r="B82" t="str">
-        <v>The business owner isn’t required to notify customers if an employee was exposed to COVID-19. The local health department will use contact tracing to notify those who were in close contact with the COVID-19 positive worker.\n\nWhen an employer discovers a worker who has tested positive or has symptoms of COVID-19, the employer should:\n\n*   make sure the worker does not remain at work, and\n*   work with the local health department to support isolation or quarantine, testing, and about when the worker may return to work. \n\nEmployers must follow the [Employer playbook](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf) which includes detailed information on:\n\n*   When and how an employer must report a COVID-19 positive employee.\n*   What is defined as an outbreak.\n*   Notifying all workers who may have been exposed to the worker with COVID-19. This is especially important for those with high-risk medical conditions (e.g., immune compromise or pregnancy).\n*   Guidance for employers who may be considering whether to suspend operations due to COVID-19 spread in the workplace.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>California’s network of small business support centers can help you figure out which loans and programs are best for your business, develop resiliency strategies, and find other resources. Go to California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) to find the closest center.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C82" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2514,10 +2514,10 @@
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>What precautions should healthcare workers and organizations take?</v>
+        <v>How do I maintain a safe workplace?</v>
       </c>
       <c r="B83" t="str">
-        <v>See [Cal/OSHA’s guidance on protecting workers from coronavirus](https://www.dir.ca.gov/dosh/coronavirus/Health-Care-General-Industry.html).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>As California reopens, every business will need to create a safer, low-risk environment. If you own or manage a business, follow the [industry-specific guidance](https://covid19.ca.gov/industry-guidance/) that applies to protect your workers and customers.\n\nIf your business is approved to reopen, you should take steps to ensure the safety and health of your workers. It’s important that employees with COVID-19 know they should stay home. Your sick leave policies need to support that. \n\n*   Encourage sick employees to stay home if they are sick. See government programs supporting [COVID-19 sick leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) and [workers’ compensation](https://www.labor.ca.gov/coronavirus2019/#chart).\n*   Establish routine cleaning throughout the workplace.\n*   Reduce travel. If possible, encourage video conferencing and limit larger gatherings.\n*   See [Cal/OSHA interim guidelines for general industry](https://www.dir.ca.gov/dosh/coronavirus/General-Industry.html).\n*   Follow [CDC guidance on keeping the workplace safe (PDF)](https://www.cdc.gov/coronavirus/2019-ncov/downloads/workplace-school-and-home-guidance.pdf).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C83" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2540,10 +2540,10 @@
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>How can I avoid laying off employees if my business is impacted by COVID-19?</v>
+        <v>Should a business owner notify customers if an employee has been exposed to COVID-19?</v>
       </c>
       <c r="B84" t="str">
-        <v>Apply for the [Unemployment Insurance (UI) Work Sharing Program](https://www.edd.ca.gov/Unemployment/Work_Sharing_Program.htm).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)&lt;!-- workshare, furlough, reduce hours --&gt;</v>
+        <v>The business owner isn’t required to notify customers if an employee was exposed to COVID-19. The local health department will use contact tracing to notify those who were in close contact with the COVID-19 positive worker.\n\nWhen an employer discovers a worker who has tested positive or has symptoms of COVID-19, the employer should:\n\n*   make sure the worker does not remain at work, and\n*   work with the local health department to support isolation or quarantine, testing, and about when the worker may return to work. \n\nEmployers must follow the [Employer playbook](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf) which includes detailed information on:\n\n*   When and how an employer must report a COVID-19 positive employee.\n*   What is defined as an outbreak.\n*   Notifying all workers who may have been exposed to the worker with COVID-19. This is especially important for those with high-risk medical conditions (e.g., immune compromise or pregnancy).\n*   Guidance for employers who may be considering whether to suspend operations due to COVID-19 spread in the workplace.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C84" t="str">
         <v>https://covid19.ca.gov/business-and-employers/</v>
@@ -2566,13 +2566,13 @@
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>What action is the state taking to ensure all schools are providing meaningful instruction during the pandemic whether they are physically open or closed?</v>
+        <v>What precautions should healthcare workers and organizations take?</v>
       </c>
       <c r="B85" t="str">
-        <v>*   California has made $5.3 billion in investments to support safe reopening and rigorous distance learning.\n*   Funds prioritize low-income students, English language learners, and special education students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>See [Cal/OSHA’s guidance on protecting workers from coronavirus](https://www.dir.ca.gov/dosh/coronavirus/Health-Care-General-Industry.html).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C85" t="str">
-        <v>https://covid19.ca.gov/education/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D85" t="str">
         <v xml:space="preserve"> </v>
@@ -2592,13 +2592,13 @@
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>What determines whether schools are conducting in-person learning or distance learning?</v>
+        <v>How can I avoid laying off employees if my business is impacted by COVID-19?</v>
       </c>
       <c r="B86" t="str">
-        <v>Using health data, schools can reopen for in-person instruction once their county has been in the Substantial (red) tier for at least two weeks. Schools must follow the **[Blueprint for a Safer Economy](https://covid19.ca.gov/safer-economy)** to reopen or if they have to close again.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>Apply for the [Unemployment Insurance (UI) Work Sharing Program](https://www.edd.ca.gov/Unemployment/Work_Sharing_Program.htm).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)&lt;!-- workshare, furlough, reduce hours --&gt;</v>
       </c>
       <c r="C86" t="str">
-        <v>https://covid19.ca.gov/education/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D86" t="str">
         <v xml:space="preserve"> </v>
@@ -2618,10 +2618,10 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>What are the health and safety requirements for schools doing in-person learning?</v>
+        <v>What action is the state taking to ensure all schools are providing meaningful instruction during the pandemic whether they are physically open or closed?</v>
       </c>
       <c r="B87" t="str">
-        <v>*   Everyone entering the school must do daily health checks.\n*   If someone experiences symptoms while at school, they will be sent home.\n*   Masks are required for all staff and students 3rd grade and above. Younger students should be encouraged to wear masks.\n*   Staff members must maintain 6ft distance from each other and students. Students should maintain 6ft distance as practicable.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>*   California has made $5.3 billion in investments to support safe reopening and rigorous distance learning.\n*   Funds prioritize low-income students, English language learners, and special education students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C87" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2644,10 +2644,10 @@
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>What happens if someone gets COVID-19 at my child’s school?</v>
+        <v>What determines whether schools are conducting in-person learning or distance learning?</v>
       </c>
       <c r="B88" t="str">
-        <v>*   A classroom goes home when there is a confirmed case\n*   A school should switch to distance learning when there are multiple positive cases in multiple classroom cohorts\n*   A district should switch to distance learning if 25% of schools in the district are closed within a 14-day period\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>Using health data, schools can reopen for in-person instruction once their county has been in the Substantial (red) tier for at least two weeks. Schools must follow the **[Blueprint for a Safer Economy](https://covid19.ca.gov/safer-economy)** to reopen or if they have to close again.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C88" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2670,10 +2670,10 @@
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>If my child’s school is engaged in distance learning, what should I expect?</v>
+        <v>What are the health and safety requirements for schools doing in-person learning?</v>
       </c>
       <c r="B89" t="str">
-        <v>*   New statewide requirements include:\n    *   Access to devices and connectivity for all students\n    *   Daily live interaction with teachers and other students\n    *   Classes and assignments that are challenging and are equivalent to in-person instruction\n    *   Special requirements for English language learners and special education students\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>*   Everyone entering the school must do daily health checks.\n*   If someone experiences symptoms while at school, they will be sent home.\n*   Masks are required for all staff and students 3rd grade and above. Younger students should be encouraged to wear masks.\n*   Staff members must maintain 6ft distance from each other and students. Students should maintain 6ft distance as practicable.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C89" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2696,10 +2696,10 @@
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>My school provides free grab-and-go meals. Are those still available?</v>
+        <v>What happens if someone gets COVID-19 at my child’s school?</v>
       </c>
       <c r="B90" t="str">
-        <v>Yes. It is essential to keep children fed. Check with your local school district for days and times meals are offered.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>*   A classroom goes home when there is a confirmed case\n*   A school should switch to distance learning when there are multiple positive cases in multiple classroom cohorts\n*   A district should switch to distance learning if 25% of schools in the district are closed within a 14-day period\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C90" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2722,10 +2722,10 @@
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>When can colleges or universities in counties resume indoor lectures?</v>
+        <v>If my child’s school is engaged in distance learning, what should I expect?</v>
       </c>
       <c r="B91" t="str">
-        <v>Certain indoor operations in institutions of higher education must remain closed in counties in the Widespread (purple) tier. In other counties, those indoor operations can reopen consistent with the [Blueprint for a Safer Economy](https://covid19.ca.gov/safer-economy/) requirements for movie theaters and places of worship.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>*   New statewide requirements include:\n    *   Access to devices and connectivity for all students\n    *   Daily live interaction with teachers and other students\n    *   Classes and assignments that are challenging and are equivalent to in-person instruction\n    *   Special requirements for English language learners and special education students\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C91" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2748,10 +2748,10 @@
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>Is there financial help for student loans?</v>
+        <v>My school provides free grab-and-go meals. Are those still available?</v>
       </c>
       <c r="B92" t="str">
-        <v>The [governor has ordered](https://www.gov.ca.gov/2020/04/23/governor-newsom-announces-additional-relief-for-californians-impacted-by-covid-19/) relief for students with federal loans. Check with your lender to see what options are available for you.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>Yes. It is essential to keep children fed. Check with your local school district for days and times meals are offered.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C92" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2774,10 +2774,10 @@
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>What if I don’t have internet access at home?</v>
+        <v>When can colleges or universities in counties resume indoor lectures?</v>
       </c>
       <c r="B93" t="str">
-        <v>Check with your local school district or college to see what resources are available for you.  List of providers offering free internet access currently:\n\n[Spectrum mobile](https://mobile.spectrum.com/support/article/360040980371/coronavirus-covid19-update)  has opened wifi hotspots and are working on assisting school districts with facilitating home internet access. \n\n[Comcast](https://corporate.comcast.com/covid-19) has opened free Xfinity WiFi hotspot access across the country. Xfinity has also paused data plans, late fees, and disconnects for the next 60 days. Families with limited income can receive internet services for free for the next 60 days (usually $9.95 per month). \n\n[AT&amp;T](https://about.att.com/pages/COVID-19.html)  has opened all public WiFi hotspots and will not charge customers for any late fees or overages. AT&amp;T also offers internet access for [$10/month for households on limited income](https://www.att.com/shop/internet/access/index.html?source=ECmj0000000000mbU&amp;wtExtndSource=access#!/#%2F).\n\n[Low-cost Internet access plans](https://www.cde.ca.gov/ls/he/hn/availableinternetplans.asp) are also available.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>Certain indoor operations in institutions of higher education must remain closed in counties in the Widespread (purple) tier. In other counties, those indoor operations can reopen consistent with the [Blueprint for a Safer Economy](https://covid19.ca.gov/safer-economy/) requirements for movie theaters and places of worship.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C93" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2800,10 +2800,10 @@
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>How will students with disabilities receive services during school closures?</v>
+        <v>Is there financial help for student loans?</v>
       </c>
       <c r="B94" t="str">
-        <v>The Department of Education has released [guidance on distance learning](https://www.cde.ca.gov/ls/he/hn/distancelearning.asp) to support schools. This guidance includes recommendations to ensure equity and access for all students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>The [governor has ordered](https://www.gov.ca.gov/2020/04/23/governor-newsom-announces-additional-relief-for-californians-impacted-by-covid-19/) relief for students with federal loans. Check with your lender to see what options are available for you.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C94" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2826,10 +2826,10 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>Will there be standardized testing for students? When?</v>
+        <v>What if I don’t have internet access at home?</v>
       </c>
       <c r="B95" t="str">
-        <v>Probably not: on March 18, 2020, Governor Newsom issued an [executive order](https://www.gov.ca.gov/2020/03/18/governor-newsom-issues-executive-order-to-suspend-standardized-testing-for-students-in-response-to-covid-19-outbreak/)  to waive this year’s statewide testing for K-12 schools.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
+        <v>Check with your local school district or college to see what resources are available for you.  List of providers offering free internet access currently:\n\n[Spectrum mobile](https://mobile.spectrum.com/support/article/360040980371/coronavirus-covid19-update)  has opened wifi hotspots and are working on assisting school districts with facilitating home internet access. \n\n[Comcast](https://corporate.comcast.com/covid-19) has opened free Xfinity WiFi hotspot access across the country. Xfinity has also paused data plans, late fees, and disconnects for the next 60 days. Families with limited income can receive internet services for free for the next 60 days (usually $9.95 per month). \n\n[AT&amp;T](https://about.att.com/pages/COVID-19.html)  has opened all public WiFi hotspots and will not charge customers for any late fees or overages. AT&amp;T also offers internet access for [$10/month for households on limited income](https://www.att.com/shop/internet/access/index.html?source=ECmj0000000000mbU&amp;wtExtndSource=access#!/#%2F).\n\n[Low-cost Internet access plans](https://www.cde.ca.gov/ls/he/hn/availableinternetplans.asp) are also available.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C95" t="str">
         <v>https://covid19.ca.gov/education/</v>
@@ -2852,13 +2852,13 @@
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>Am I allowed to work during the outbreak?</v>
+        <v>How will students with disabilities receive services during school closures?</v>
       </c>
       <c r="B96" t="str">
-        <v>It depends what your job is. Any member of the [essential workforce](https://files.covid19.ca.gov/pdf/EssentialCriticalInfrastructureWorkers.pdf) is allowed to work during the [stay home order](https://covid19.ca.gov/stay-home-except-for-essential-needs/#top). And anyone is allowed to work from their home that has arranged to do so with their employer.\n\nFor information on businesses and industry sectors that are allowed to reopen, visit [industry guidance](https://covid19.ca.gov/industry-guidance/).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>The Department of Education has released [guidance on distance learning](https://www.cde.ca.gov/ls/he/hn/distancelearning.asp) to support schools. This guidance includes recommendations to ensure equity and access for all students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C96" t="str">
-        <v>https://covid19.ca.gov/workers/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D96" t="str">
         <v xml:space="preserve"> </v>
@@ -2878,13 +2878,13 @@
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>What can I do if my work hours are reduced or I am furloughed because of COVID-19?</v>
+        <v>Will there be standardized testing for students? When?</v>
       </c>
       <c r="B97" t="str">
-        <v>You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>Probably not: on March 18, 2020, Governor Newsom issued an [executive order](https://www.gov.ca.gov/2020/03/18/governor-newsom-issues-executive-order-to-suspend-standardized-testing-for-students-in-response-to-covid-19-outbreak/)  to waive this year’s statewide testing for K-12 schools.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C97" t="str">
-        <v>https://covid19.ca.gov/workers/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D97" t="str">
         <v xml:space="preserve"> </v>
@@ -2904,10 +2904,10 @@
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>Do I need a note or certificate from a medical provider to file for unemployment?</v>
+        <v>Am I allowed to work during the outbreak?</v>
       </c>
       <c r="B98" t="str">
-        <v>No, a medical certificate is not required.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>It depends what your job is. Any member of the [essential workforce](https://files.covid19.ca.gov/pdf/EssentialCriticalInfrastructureWorkers.pdf) is allowed to work during the [stay home order](https://covid19.ca.gov/stay-home-except-for-essential-needs/#top). And anyone is allowed to work from their home that has arranged to do so with their employer.\n\nFor information on businesses and industry sectors that are allowed to reopen, visit [industry guidance](https://covid19.ca.gov/industry-guidance/).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C98" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2930,10 +2930,10 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>How long will it take to process a claim for unemployment or insurance benefits and to receive a payment?</v>
+        <v>What can I do if my work hours are reduced or I am furloughed because of COVID-19?</v>
       </c>
       <c r="B99" t="str">
-        <v>After your claim is submitted, it will take at least three weeks to be processed. It may take longer if your information doesn’t match wage records or your identity can’t be verified. \n\nThe Governor has [waived the one-week waiting period](https://www.gov.ca.gov/2020/03/12/governor-newsom-issues-new-executive-order-further-enhancing-state-and-local-governments-ability-to-respond-to-covid-19-pandemic/). This means you can collect benefits for the first week that you were out of work or had reduced hours.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C99" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2956,10 +2956,10 @@
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>Can I file a workplace safety complaint?</v>
+        <v>Do I need a note or certificate from a medical provider to file for unemployment?</v>
       </c>
       <c r="B100" t="str">
-        <v>Yes, you have the right to file a complaint. Find [information and instructions](https://www.dir.ca.gov/dosh/complaint.htm) for how to file a complaint. If you submit a complaint, your name must be kept confidential by law.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>No, a medical certificate is not required.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C100" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -2982,10 +2982,10 @@
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>What can I do if I miss work because of school closures?</v>
+        <v>How long will it take to process a claim for unemployment or insurance benefits and to receive a payment?</v>
       </c>
       <c r="B101" t="str">
-        <v>*   You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n*   You may be eligible for up to 80 hours of paid sick leave at two-thirds of your regular rate under the Families First Coronavirus Response Act ([FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-employee-paid-leave)) if your employer has less than 500 workers. You may also be eligible for up to 10 additional weeks of paid expanded family and medical leave at two-thirds of your regular rate. \n    *   Check [quick tips about FFCRA paid leave](https://www.dol.gov/sites/dolgov/files/WHD/Pandemic/Quick%20Tip%20Poster%20FFCRA.pdf) from the U.S. Department of Labor. \n    *   Use the [FFCRA tool](https://www.dol.gov/agencies/whd/ffcra/benefits-eligibility-webtool) to find out if you may be eligible. \n    *   See detailed information in the [questions and answers about FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-questions). \n*   Other options may be available. See the [chart of benefits for workers impacted by COVID-19](https://www.labor.ca.gov/coronavirus2019/#chart).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>After your claim is submitted, it will take at least three weeks to be processed. It may take longer if your information doesn’t match wage records or your identity can’t be verified. \n\nThe Governor has [waived the one-week waiting period](https://www.gov.ca.gov/2020/03/12/governor-newsom-issues-new-executive-order-further-enhancing-state-and-local-governments-ability-to-respond-to-covid-19-pandemic/). This means you can collect benefits for the first week that you were out of work or had reduced hours.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C101" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -3008,10 +3008,10 @@
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>What if I can’t work because I’m taking care of someone who’s sick or quarantined?</v>
+        <v>Can I file a workplace safety complaint?</v>
       </c>
       <c r="B102" t="str">
-        <v>*   You may be eligible for up to 80 hours of paid expanded family and medical leave at two-thirds of your regular rate under the Families First Coronavirus Response Act ([FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-employee-paid-leave)) if your employer has less than 500 workers. \n    *   Check the [quick tips about FFCRA paid leave](https://www.dol.gov/sites/dolgov/files/WHD/Pandemic/Quick%20Tip%20Poster%20FFCRA.pdf) from the U.S. Department of Labor. \n    *   Use this [tool](https://www.dol.gov/agencies/whd/ffcra/benefits-eligibility-webtool) to see if you’re eligible for FFCRA paid expanded family and medical leave. \n    *   Find detailed information in the [questions and answers about FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-questions). \n*   You may use other [paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). See the [chart of paid sick and family leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) available under state and federal law. \n*   You can [file a Paid Family Leave (PFL) claim](https://www.edd.ca.gov/Disability/How_to_File_a_PFL_Claim_in_SDI_Online.htm). \n    *   See if you may be [eligible for paid family leave](https://edd.ca.gov/Disability/Am_I_Eligible_for_PFL_Benefits.htm). \n    *   Find details about the [paid family leave process](https://www.edd.ca.gov/Disability/PFL_Claim_Process.htm). \n    *   Check the [frequently asked questions](https://www.edd.ca.gov/Disability/FAQs.htm) about paid family leave. \n    *   See the [chart of paid family and sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) available under state and federal law. \n*   Unpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf) about employment and COVID-19.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>Yes, you have the right to file a complaint. Find [information and instructions](https://www.dir.ca.gov/dosh/complaint.htm) for how to file a complaint. If you submit a complaint, your name must be kept confidential by law.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C102" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -3034,10 +3034,10 @@
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>What can I do if I can’t work because I’m sick or quarantined because of COVID-19?</v>
+        <v>What can I do if I miss work because of school closures?</v>
       </c>
       <c r="B103" t="str">
-        <v>Extra federal, state, and in some cases, local sick leave are available if you are having COVID-19 symptoms, seeking a medical diagnosis, or are in quarantine. Check the side-by-side [comparison of COVID-19 paid leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) to learn what options may be available to you.\n\n*   You may be eligible for up to 80 hours of paid sick leave under the Families First Coronavirus Response Act ([FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-employee-paid-leave)) if your employer has less than 500 workers. \n    *   Check the [quick tips about FFCRA paid leave](https://www.dol.gov/sites/dolgov/files/WHD/Pandemic/Quick%20Tip%20Poster%20FFCRA.pdf) from the U.S. Department of Labor. \n    *   Use this [tool](https://www.dol.gov/agencies/whd/ffcra/benefits-eligibility-webtool) to see if you’re eligible for FFCRA paid sick leave. \n    *   Find detailed information in the [questions and answers about FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-questions).\n*   You may be eligible for up to 80 hours of California COVID-19 supplemental paid sick leave if you work for a business in the food sector with more than 500 workers. See [frequently asked questions](https://www.dir.ca.gov/dlse/FAQ-for-PSL.html) about supplemental paid sick leave for food sector workers.\n*   Some local areas have paid sick leave ordinances, such as San Jose, San Francisco, and Los Angeles. Check with the local labor law enforcement agency in your area.\n\nCheck the chart of all [benefits for workers impacted by COVID-19](https://www.labor.ca.gov/coronavirus2019/#chart) to learn about other resources that may be available.\n\n*   You may be able to use paid sick leave. See the [frequently asked questions about paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). \n*   You can [file a Disability Insurance (DI) claim](https://www.edd.ca.gov/Disability/How_to_File_a_DI_Claim_in_SDI_Online.htm) if you’re unable to work due to having or being exposed to COVID-19. \n    *   See if you may be [eligible for disability insurance benefits](https://edd.ca.gov/Disability/Am_I_Eligible_for_DI_Benefits.htm). \n    *   Check the [frequently asked questions](https://www.edd.ca.gov/Disability/FAQs.htm) about state disability insurance. \n*   You can file a [Workers’ Compensation claim](https://www.dir.ca.gov/dwc/FileAClaim.htm) if you suffered a COVID-19 illness that arose from an exposure during the course of your work. Find more information on [COVID-19 Resources and Workers’ Compensation](https://www.dir.ca.gov/dwc/Covid-19/Index.html).\n*   You may be able to use job-protected unpaid leave. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf) about employment and COVID-19.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>*   You can file for [Unemployment Insurance (UI)](https://www.edd.ca.gov/Unemployment/Filing_a_Claim.htm).\n*   You may be eligible for up to 80 hours of paid sick leave at two-thirds of your regular rate under the Families First Coronavirus Response Act ([FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-employee-paid-leave)) if your employer has less than 500 workers. You may also be eligible for up to 10 additional weeks of paid expanded family and medical leave at two-thirds of your regular rate. \n    *   Check [quick tips about FFCRA paid leave](https://www.dol.gov/sites/dolgov/files/WHD/Pandemic/Quick%20Tip%20Poster%20FFCRA.pdf) from the U.S. Department of Labor. \n    *   Use the [FFCRA tool](https://www.dol.gov/agencies/whd/ffcra/benefits-eligibility-webtool) to find out if you may be eligible. \n    *   See detailed information in the [questions and answers about FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-questions). \n*   Other options may be available. See the [chart of benefits for workers impacted by COVID-19](https://www.labor.ca.gov/coronavirus2019/#chart).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C103" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -3060,10 +3060,10 @@
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>What if I don’t have any available sick leave to use?</v>
+        <v>What if I can’t work because I’m taking care of someone who’s sick or quarantined?</v>
       </c>
       <c r="B104" t="str">
-        <v>Check the Labor and Workforce Development Agency’s [chart detailing the available sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law.\n\nUnpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>*   You may be eligible for up to 80 hours of paid expanded family and medical leave at two-thirds of your regular rate under the Families First Coronavirus Response Act ([FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-employee-paid-leave)) if your employer has less than 500 workers. \n    *   Check the [quick tips about FFCRA paid leave](https://www.dol.gov/sites/dolgov/files/WHD/Pandemic/Quick%20Tip%20Poster%20FFCRA.pdf) from the U.S. Department of Labor. \n    *   Use this [tool](https://www.dol.gov/agencies/whd/ffcra/benefits-eligibility-webtool) to see if you’re eligible for FFCRA paid expanded family and medical leave. \n    *   Find detailed information in the [questions and answers about FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-questions). \n*   You may use other [paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). See the [chart of paid sick and family leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) available under state and federal law. \n*   You can [file a Paid Family Leave (PFL) claim](https://www.edd.ca.gov/Disability/How_to_File_a_PFL_Claim_in_SDI_Online.htm). \n    *   See if you may be [eligible for paid family leave](https://edd.ca.gov/Disability/Am_I_Eligible_for_PFL_Benefits.htm). \n    *   Find details about the [paid family leave process](https://www.edd.ca.gov/Disability/PFL_Claim_Process.htm). \n    *   Check the [frequently asked questions](https://www.edd.ca.gov/Disability/FAQs.htm) about paid family leave. \n    *   See the [chart of paid family and sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) available under state and federal law. \n*   Unpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf) about employment and COVID-19.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C104" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -3086,10 +3086,10 @@
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>When can I return to work once my isolation or quarantine is over?</v>
+        <v>What can I do if I can’t work because I’m sick or quarantined because of COVID-19?</v>
       </c>
       <c r="B105" t="str">
-        <v>When you can return to work depends on your situation. \n\nIf you have symptoms, you should stay home until:\n\n*   at least 10 days have passed since symptoms started, AND\n*    your fever has been gone for 24 hours without the aid of medication, AND \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested.\n\nIf you have tested positive but have no symptoms, you should [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) at home for at least 10 days.\n\nIf you had close contact with someone who tested positive but you have tested negative, you should still [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) at home for at least 14 days.\n\nGet tested as soon as possible if you have symptoms or have come in contact with someone who has tested positive or has symptoms.\n\nRead more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>Extra federal, state, and in some cases, local sick leave are available if you are having COVID-19 symptoms, seeking a medical diagnosis, or are in quarantine. Check the side-by-side [comparison of COVID-19 paid leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) to learn what options may be available to you.\n\n*   You may be eligible for up to 80 hours of paid sick leave under the Families First Coronavirus Response Act ([FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-employee-paid-leave)) if your employer has less than 500 workers. \n    *   Check the [quick tips about FFCRA paid leave](https://www.dol.gov/sites/dolgov/files/WHD/Pandemic/Quick%20Tip%20Poster%20FFCRA.pdf) from the U.S. Department of Labor. \n    *   Use this [tool](https://www.dol.gov/agencies/whd/ffcra/benefits-eligibility-webtool) to see if you’re eligible for FFCRA paid sick leave. \n    *   Find detailed information in the [questions and answers about FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-questions).\n*   You may be eligible for up to 80 hours of California COVID-19 supplemental paid sick leave if you work for a business in the food sector with more than 500 workers. See [frequently asked questions](https://www.dir.ca.gov/dlse/FAQ-for-PSL.html) about supplemental paid sick leave for food sector workers.\n*   Some local areas have paid sick leave ordinances, such as San Jose, San Francisco, and Los Angeles. Check with the local labor law enforcement agency in your area.\n\nCheck the chart of all [benefits for workers impacted by COVID-19](https://www.labor.ca.gov/coronavirus2019/#chart) to learn about other resources that may be available.\n\n*   You may be able to use paid sick leave. See the [frequently asked questions about paid sick leave](https://www.dir.ca.gov/dlse/2019-Novel-Coronavirus.htm). \n*   You can [file a Disability Insurance (DI) claim](https://www.edd.ca.gov/Disability/How_to_File_a_DI_Claim_in_SDI_Online.htm) if you’re unable to work due to having or being exposed to COVID-19. \n    *   See if you may be [eligible for disability insurance benefits](https://edd.ca.gov/Disability/Am_I_Eligible_for_DI_Benefits.htm). \n    *   Check the [frequently asked questions](https://www.edd.ca.gov/Disability/FAQs.htm) about state disability insurance. \n*   You can file a [Workers’ Compensation claim](https://www.dir.ca.gov/dwc/FileAClaim.htm) if you suffered a COVID-19 illness that arose from an exposure during the course of your work. Find more information on [COVID-19 Resources and Workers’ Compensation](https://www.dir.ca.gov/dwc/Covid-19/Index.html).\n*   You may be able to use job-protected unpaid leave. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf) about employment and COVID-19.\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C105" t="str">
         <v>https://covid19.ca.gov/workers/</v>
@@ -3112,13 +3112,13 @@
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>What effect will late payments have on my credit report?</v>
+        <v>What if I don’t have any available sick leave to use?</v>
       </c>
       <c r="B106" t="str">
-        <v>Financial institutions will not report derogatory information (like late payments) to credit reporting agencies but may report a forbearance. Typically this does not negatively affect a credit score on its own.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>Check the Labor and Workforce Development Agency’s [chart detailing the available sick leave](https://www.labor.ca.gov/wp-content/uploads/2020/04/Side-by-Side-CA-Paid-Leave-FFCRA-Paid-Leave-4.9.20.pdf) under state and federal law and emergency paid family and medical leave under federal law.\n\nUnpaid leave may be available to you through the California Family Rights Act. Check the California Department of Fair Employment and Housing’s [frequently asked questions](https://www.dfeh.ca.gov/wp-content/uploads/sites/32/2020/03/DFEH-Employment-Information-on-COVID-19-FAQ_ENG.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C106" t="str">
-        <v>https://covid19.ca.gov/get-financial-help/</v>
+        <v>https://covid19.ca.gov/workers/</v>
       </c>
       <c r="D106" t="str">
         <v xml:space="preserve"> </v>
@@ -3138,13 +3138,13 @@
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>How long will financial relief programs last?</v>
+        <v>When can I return to work once my isolation or quarantine is over?</v>
       </c>
       <c r="B107" t="str">
-        <v>It is still unclear how severe or how long the COVID-19 impact will be. Financial institutions have committed to necessary relief and will be assessing the ongoing conditions and need for continuing relief.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>When you can return to work depends on your situation. \n\nIf you have symptoms, you should stay home until:\n\n*   at least 10 days have passed since symptoms started, AND\n*    your fever has been gone for 24 hours without the aid of medication, AND \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested.\n\nIf you have tested positive but have no symptoms, you should [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) at home for at least 10 days.\n\nIf you had close contact with someone who tested positive but you have tested negative, you should still [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) at home for at least 14 days.\n\nGet tested as soon as possible if you have symptoms or have come in contact with someone who has tested positive or has symptoms.\n\nRead more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
       </c>
       <c r="C107" t="str">
-        <v>https://covid19.ca.gov/get-financial-help/</v>
+        <v>https://covid19.ca.gov/workers/</v>
       </c>
       <c r="D107" t="str">
         <v xml:space="preserve"> </v>
@@ -3164,13 +3164,13 @@
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>What if my financial institution isn’t offering payment relief?</v>
+        <v>Where can I apply for unemployment?</v>
       </c>
       <c r="B108" t="str">
-        <v>Call or check their website to be sure. At this time, JP Morgan Chase, US Bank, Wells Fargo and Citigroup, [and nearly 200 state-chartered banks](https://dbo.ca.gov/covid19-updates-fi/), credit unions are supporting these commitments. \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>If you lost your job or had your hours reduced, and meet eligibility requirements, you may be eligible to receive Unemployment Insurance (UI) benefits from California’s Employment Development Department (EDD). Check the [guide to applying for unemployment benefits](https://unemployment.edd.ca.gov/guide).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)&lt;!-- laid off, hours cut, lost my job, file for unemployment, file for UI --&gt;</v>
       </c>
       <c r="C108" t="str">
-        <v>https://covid19.ca.gov/get-financial-help/</v>
+        <v>https://covid19.ca.gov/workers/</v>
       </c>
       <c r="D108" t="str">
         <v xml:space="preserve"> </v>
@@ -3190,10 +3190,10 @@
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>Is mortgage relief available to businesses?</v>
+        <v>What effect will late payments have on my credit report?</v>
       </c>
       <c r="B109" t="str">
-        <v>The relief is currently only available for residential mortgages.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>Financial institutions will not report derogatory information (like late payments) to credit reporting agencies but may report a forbearance. Typically this does not negatively affect a credit score on its own.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C109" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -3216,10 +3216,10 @@
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>What if my mortgage servicer is not communicative or cooperative?</v>
+        <v>How long will financial relief programs last?</v>
       </c>
       <c r="B110" t="str">
-        <v>You can file a complaint with the Department of Business Oversight:\n\n*   File on their [website](https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fdbo.ca.gov%2Ffile-a-complaint%2F&amp;data=02%7C01%7CManuel.Alvarez%40dbo.ca.gov%7Ce2673837ec6f42fce84508d7d114ed59%7Cd6910b1745b44b7bbb66cb7936fabafe%7C1%7C0%7C637207760136603083&amp;sdata=VR6CdqCvrBGkfC%2Bm%2B6Yj9emco9ldVY5BLWSiLpe3f4c%3D&amp;reserved=0)\n*    Call their Consumer Services Office at [(866) 275-2677](tel:(866) 275-2677) or [(916) 327-7585](tel:(916) 327-7585) \n*   Or email Ask.DBO@dbo.ca.gov\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>It is still unclear how severe or how long the COVID-19 impact will be. Financial institutions have committed to necessary relief and will be assessing the ongoing conditions and need for continuing relief.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C110" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -3242,10 +3242,10 @@
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>Can I get child care during the stay home order?</v>
+        <v>What if my financial institution isn’t offering payment relief?</v>
       </c>
       <c r="B111" t="str">
-        <v>Yes, all [childcare](https://covid19.ca.gov/childcare/) facilities can open with necessary modifications.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
+        <v>Call or check their website to be sure. At this time, JP Morgan Chase, US Bank, Wells Fargo and Citigroup, [and nearly 200 state-chartered banks](https://dbo.ca.gov/covid19-updates-fi/), credit unions are supporting these commitments. \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C111" t="str">
         <v>https://covid19.ca.gov/get-financial-help/</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>I am homeless and I may have come in contact with coronavirus. How can I self-isolate with nowhere to go and services closing down?</v>
+        <v>Is mortgage relief available to businesses?</v>
       </c>
       <c r="B112" t="str">
-        <v>A motel or hotel room may be available for you and your family. Contact your local homeless [continuum of care](https://www.bcsh.ca.gov/hcfc/documents/coc_poc.pdf) to connect you to this service.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>The relief is currently only available for residential mortgages.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C112" t="str">
-        <v>https://covid19.ca.gov/housing-and-homelessness/</v>
+        <v>https://covid19.ca.gov/get-financial-help/</v>
       </c>
       <c r="D112" t="str">
         <v xml:space="preserve"> </v>
@@ -3294,13 +3294,13 @@
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>Will there be a rent freeze or waiver for renters? Are evictions allowed during the stay at home order?</v>
+        <v>What if my mortgage servicer is not communicative or cooperative?</v>
       </c>
       <c r="B113" t="str">
-        <v>There is an [order](https://www.gov.ca.gov/2020/06/30/governor-newsom-signs-executive-order-on-actions-in-response-to-covid-19-6-30-20/) in place to halt evictions and protect renters. If you are financially affected by COVID-19 and [can’t pay your full rent](https://bcsh.ca.gov/coronavirus19/graphic_rent.pdf), let your landlord know in writing within seven days of the rent due date. Save documentation as proof. The order does not relieve you from the obligation to pay rent. It also does not restrict the landlord from recovering rent that is due.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>You can file a complaint with the Department of Business Oversight:\n\n*   File on the [DBO website](https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fdbo.ca.gov%2Ffile-a-complaint%2F&amp;data=02%7C01%7CManuel.Alvarez%40dbo.ca.gov%7Ce2673837ec6f42fce84508d7d114ed59%7Cd6910b1745b44b7bbb66cb7936fabafe%7C1%7C0%7C637207760136603083&amp;sdata=VR6CdqCvrBGkfC%2Bm%2B6Yj9emco9ldVY5BLWSiLpe3f4c%3D&amp;reserved=0)\n*   Call their Consumer Services Office at [(866) 275-2677](tel:(866) 275-2677) or [(916) 327-7585](tel:(916) 327-7585) \n*   Or email [Ask.DBO@dbo.ca.gov](mailto:Ask.DBO@dbo.ca.gov)\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C113" t="str">
-        <v>https://covid19.ca.gov/housing-and-homelessness/</v>
+        <v>https://covid19.ca.gov/get-financial-help/</v>
       </c>
       <c r="D113" t="str">
         <v xml:space="preserve"> </v>
@@ -3320,13 +3320,13 @@
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>Can landlords delay their payments while their tenants cannot pay rent?</v>
+        <v>Can I get child care during the stay home order?</v>
       </c>
       <c r="B114" t="str">
-        <v>Yes, there are protections in effect through September 30, 2020 for landlords. The [order](https://www.gov.ca.gov/2020/03/16/governor-newsom-issues-executive-order-to-protect-renters-and-homeowners-during-covid-19-pandemic/) requests lenders to halt foreclosures and related evictions during this time. Property owners should contact their financial institutions.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>Yes, all [childcare](https://covid19.ca.gov/childcare/) facilities can open with necessary modifications.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C114" t="str">
-        <v>https://covid19.ca.gov/housing-and-homelessness/</v>
+        <v>https://covid19.ca.gov/get-financial-help/</v>
       </c>
       <c r="D114" t="str">
         <v xml:space="preserve"> </v>
@@ -3346,10 +3346,10 @@
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>How do I get mortgage relief and/or forbearance?</v>
+        <v>I am homeless and I may have come in contact with coronavirus. How can I self-isolate with nowhere to go and services closing down?</v>
       </c>
       <c r="B115" t="str">
-        <v>You should contact and work directly with your mortgage servicer to learn about and apply for available relief. Please note that financial institutions and their servicers are experiencing high volumes of inquiries.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>A motel or hotel room may be available for you and your family. Contact your local homeless [continuum of care](https://www.bcsh.ca.gov/hcfc/documents/coc_poc.pdf) to connect you to this service.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C115" t="str">
         <v>https://covid19.ca.gov/housing-and-homelessness/</v>
@@ -3372,10 +3372,10 @@
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>How long will the forbearance last?</v>
+        <v>Will there be a rent freeze or waiver for renters? Are evictions allowed during the stay at home order?</v>
       </c>
       <c r="B116" t="str">
-        <v>The terms of a forbearance will be agreed to between you and your mortgage service. Financial institutions will confirm approval of and terms of the forbearance program.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
+        <v>The [Tenant, Homeowner and Small Landlord Relief and Stabilization Act](https://www.gov.ca.gov/wp-content/uploads/2020/08/Factsheet-Tenant-Homeowner-and-Small-Landlord-Relief-and-Stabilization-Act-of-2020.pdf) and an executive [order](https://www.gov.ca.gov/2020/06/30/governor-newsom-signs-executive-order-on-actions-in-response-to-covid-19-6-30-20/) have halted evictions and protected renters. If you are financially affected by  coronavirus and [can’t pay your full rent](https://bcsh.ca.gov/coronavirus19/graphic_rent.pdf), let your landlord know in writing within seven days of the rent due date. Save documentation as proof. The order does not relieve you from paying rent. It also does not restrict your landlord from collecting rent later.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C116" t="str">
         <v>https://covid19.ca.gov/housing-and-homelessness/</v>
@@ -3398,13 +3398,13 @@
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>What if a provider says they have availability on MyChildCare.ca.gov but when I connect with them they have no space?</v>
+        <v>How do I get mortgage relief and/or forbearance?</v>
       </c>
       <c r="B117" t="str">
-        <v>The information on [MyChildCare.ca.gov](http://mychildcare.ca.gov/) will be updated twice each week but it is possible that vacancies are filled between updates. Contact your [local childcare resource and referral agency](http://rrnetwork.org/family-services/find-child-care) to find more vacancies. \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
+        <v>Contact and work directly with your mortgage servicer to learn about and apply for available relief. Some financial institutions and their servicers are experiencing a high volume of inquiries.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C117" t="str">
-        <v>https://covid19.ca.gov/childcare/</v>
+        <v>https://covid19.ca.gov/housing-and-homelessness/</v>
       </c>
       <c r="D117" t="str">
         <v xml:space="preserve"> </v>
@@ -3424,13 +3424,13 @@
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>How can I find out more about the provider listed in MyChildCare.ca.gov?</v>
+        <v>How long will the mortgage forbearance last?</v>
       </c>
       <c r="B118" t="str">
-        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) includes each provider’s facility/license number. This number can be searched at [CDSS Community Care Licensing Database](https://www.ccld.dss.ca.gov/carefacilitysearch/) to find more information about the provider, like information on inspections and complaints.  \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
+        <v>You’ll agree on the terms of a forbearance with your mortgage service. Financial institutions will confirm approval of and terms of the forbearance program.\n\nMore info: [Housing and homelessness](https://covid19.ca.gov/housing-and-homelessness/)</v>
       </c>
       <c r="C118" t="str">
-        <v>https://covid19.ca.gov/childcare/</v>
+        <v>https://covid19.ca.gov/housing-and-homelessness/</v>
       </c>
       <c r="D118" t="str">
         <v xml:space="preserve"> </v>
@@ -3450,10 +3450,10 @@
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>How can I find help paying for childcare?</v>
+        <v>What if a provider says they have availability on MyChildCare.ca.gov but when I connect with them they have no space?</v>
       </c>
       <c r="B119" t="str">
-        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) provides information on all licensed center-based and family childcare homes. This includes both private-pay and subsidized childcare. Children of essential workers are now eligible to enroll in subsidized emergency childcare through June 30, 2020, or 60 calendar days after the date of the child’s enrollment, whichever is longer. This is subject to capacity and eligibility requirements. Your [local childcare resource and referral agency](https://rrnetwork.org/index.php?p=family-services/find-child-care) can answer more questions about childcare subsidies.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
+        <v>The information on [MyChildCare.ca.gov](http://mychildcare.ca.gov/) will be updated twice each week but it is possible that vacancies are filled between updates. Contact your [local childcare resource and referral agency](http://rrnetwork.org/family-services/find-child-care) to find more vacancies. \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
       </c>
       <c r="C119" t="str">
         <v>https://covid19.ca.gov/childcare/</v>
@@ -3476,10 +3476,10 @@
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>Can I get childcare during the stay home order?</v>
+        <v>How can I find out more about the provider listed in MyChildCare.ca.gov?</v>
       </c>
       <c r="B120" t="str">
-        <v>Yes, all childcare facilities can open with necessary modifications.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
+        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) includes each provider’s facility/license number. This number can be searched at [CDSS Community Care Licensing Database](https://www.ccld.dss.ca.gov/carefacilitysearch/) to find more information about the provider, like information on inspections and complaints.  \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
       </c>
       <c r="C120" t="str">
         <v>https://covid19.ca.gov/childcare/</v>
@@ -3502,10 +3502,10 @@
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>Can my babysitter still come to the house?</v>
+        <v>How can I find help paying for childcare?</v>
       </c>
       <c r="B121" t="str">
-        <v>Yes, a childcare worker can come to your home if necessary and should practice basic prevention guidelines (like handwashing for at least 20 seconds, physical distancing, and staying home if feeling ill).\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
+        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) provides information on all licensed center-based and family childcare homes. This includes both private-pay and subsidized childcare. Children of essential workers are now eligible to enroll in subsidized emergency childcare through June 30, 2020, or 60 calendar days after the date of the child’s enrollment, whichever is longer. This is subject to capacity and eligibility requirements. Your [local childcare resource and referral agency](https://rrnetwork.org/index.php?p=family-services/find-child-care) can answer more questions about childcare subsidies.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
       </c>
       <c r="C121" t="str">
         <v>https://covid19.ca.gov/childcare/</v>
@@ -3528,13 +3528,13 @@
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>Fin your county websites</v>
+        <v>Can I get childcare during the stay home order?</v>
       </c>
       <c r="B122" t="str">
-        <v>*   [Alameda County](http://www.acphd.org/2019-ncov.aspx)\n*   [Alpine County](http://alpinecountyca.gov/Index.aspx?NID=516)\n*   [Amador County](https://www.amadorgov.org/services/covid-19)\n*   [Butte County](https://www.buttecounty.net/publichealth)\n*   [Calaveras County](https://covid19.calaverasgov.us/)\n*   [Colusa County](https://www.countyofcolusa.org/99/Public-Health)\n*   [Contra Costa County](https://www.coronavirus.cchealth.org/)\n*   [Del Norte County](http://www.co.del-norte.ca.us/departments/health-human-services/public-health)\n*   [El Dorado County](https://www.edcgov.us/Government/hhsa/Pages/EDCCOVID-19.aspx)\n*   [Fresno County](https://www.co.fresno.ca.us/departments/public-health/covid-19)\n*   [Glenn County](https://www.countyofglenn.net/dept/health-human-services/public-health/covid-19)\n*   [Humboldt County](https://humboldtgov.org/2018/Humboldt-Health-Alert)\n*   [Imperial County](http://www.icphd.org/health-information-and-resources/healthy-facts/covid-19/)\n*   [Inyo County](https://www.inyocounty.us/coronavirus-covid-19-response)\n*   [Kern County](https://kernpublichealth.com/2019-novel-coronavirus/)\n*   [Kings County](https://www.countyofkings.com/departments/health-welfare/public-health/coronavirus-disease-2019-covid-19/-fsiteid-1)\n*   [Lake County](http://health.co.lake.ca.us/Coronavirus.htm)\n*   [Lassen County](http://www.co.lassen.ca.us/)\n*   [Los Angeles County](http://publichealth.lacounty.gov/media/Coronavirus/)\n*   [Madera County](https://www.maderacounty.com/government/public-health/health-updates/corona-virus)\n*   [Marin County](https://coronavirus.marinhhs.org/)\n*   [Mariposa County](http://www.mariposacounty.org/1592/COVID-19-Information)\n*   [Mendocino County](https://www.mendocinocounty.org/community/novel-coronavirus)\n*   [Merced County](https://www.co.merced.ca.us/3350/Coronavirus-Disease-2019)\n*   [Modoc County](http://www.co.modoc.ca.us/)\n*   [Mono County](https://coronavirus.monocounty.ca.gov/)\n*   [Monterey County](https://www.co.monterey.ca.us/government/departments-a-h/health/diseases/2019-novel-coronavirus-covid-19)\n*   [Napa County](https://www.countyofnapa.org/2739/Coronavirus)\n*   [Nevada County](https://www.mynevadacounty.com/2924/Coronavirus)\n*   [Orange County](https://www.ochealthinfo.com/phs/about/epidasmt/epi/dip/prevention/novel_coronavirus)\n*   [Placer County](https://www.placer.ca.gov/coronavirus)\n*   [Plumas County](https://www.plumascounty.us/2669/Novel-Coronavirus-2019-COVID-19)\n*   [Riverside County](https://www.rivcoph.org/coronavirus)\n*   [Sacramento County](https://dhs.saccounty.net/PUB/Pages/PUB-Home.aspx)\n*   [San Benito County](https://hhsa.cosb.us/publichealth/communicable-disease/coronavirus/)\n*   [San Bernardino County](http://wp.sbcounty.gov/dph/coronavirus/)\n*   [San Diego County](https://www.sandiegocounty.gov/coronavirus.html)\n*   [San Francisco City and County](https://sf.gov/topics/coronavirus-covid-19)\n*   [San Joaquin County](https://www.sjgov.org/covid19/)\n*   [San Luis Obispo County](https://www.emergencyslo.org/en/covid19.aspx)\n*   [San Mateo County](https://www.smchealth.org/coronavirus)\n*   [Santa Barbara County](https://publichealthsbc.org/)\n*   [Santa Clara County](https://www.sccgov.org/sites/phd/DiseaseInformation/novel-coronavirus/Pages/home.aspx)\n*   [Santa Cruz County](https://www.santacruzhealth.org/HSAHome/HSADivisions/PublicHealth/CommunicableDiseaseControl/Coronavirus.aspx)\n*   [Shasta County](https://www.co.shasta.ca.us/index/hhsa/health-safety/current-heath-concerns/coronavirus)\n*   [Sierra County](http://sierracounty.ca.gov/582/Coronavirus-COVID-19)\n*   [Siskiyou County](https://www.co.siskiyou.ca.us/publichealth/page/covid-19-what-siskiyou-county-residents-need-know-now)\n*   [Solano County](http://www.solanocounty.com/depts/ph/ncov.asp)\n*   [Sonoma County](https://socoemergency.org/emergency/novel-coronavirus/)\n*   [Stanislaus County](http://schsa.org/publichealth/pages/corona-virus/)\n*   [Sutter County](https://www.suttercounty.org/doc/government/depts/cao/em/coronavirus)\n*   [Tehama County](https://www.tehamacohealthservices.net/services/communicable-diseases/#current-events)\n*   [Trinity County](https://www.trinitycounty.org/)\n*   [Tulare County](https://tchhsa.org/eng/index.cfm/public-health/covid-19-updates-novel-coronavirus/)\n*   [Tuolumne County](https://www.tuolumnecounty.ca.gov/250/Public-Health)\n*   [Ventura County](https://www.vcemergency.com/)\n*   [Yolo County](https://www.yolocounty.org/health-human-services/adults/communicable-disease-investigation-and-control/novel-coronavirus-2019)\n*   [Yuba County](https://www.yuba.org/coronavirus/)\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>Yes, all childcare facilities can open with necessary modifications.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
       </c>
       <c r="C122" t="str">
-        <v>https://covid19.ca.gov/state-local-resources/</v>
+        <v>https://covid19.ca.gov/childcare/</v>
       </c>
       <c r="D122" t="str">
         <v xml:space="preserve"> </v>
@@ -3554,13 +3554,13 @@
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>What are the restrictions in my area?</v>
+        <v>Can my babysitter still come to the house?</v>
       </c>
       <c r="B123" t="str">
-        <v>While each county may have different restrictions, it is important to stay home as much as possible. If you do go out, stay 6 feet away from others who are not in your household and wear a mask or face covering. Your actions save lives.\n\nSee what [industries are open or closed](https://covid19.ca.gov/safer-economy) in your county.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>Yes, a childcare worker can come to your home if necessary and should practice basic prevention guidelines (like handwashing for at least 20 seconds, physical distancing, and staying home if feeling ill).\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
       </c>
       <c r="C123" t="str">
-        <v>https://covid19.ca.gov/state-local-resources/</v>
+        <v>https://covid19.ca.gov/childcare/</v>
       </c>
       <c r="D123" t="str">
         <v xml:space="preserve"> </v>
@@ -3580,10 +3580,10 @@
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>How are we helping the homeless?</v>
+        <v>Find your county websites</v>
       </c>
       <c r="B124" t="str">
-        <v>Each county and local government in California has [increased resources](https://covid19.ca.gov/housing-and-homelessness/#top) to protect people experiencing homelessness during COVID-19. [Financial protections](https://covid19.ca.gov/housing-and-homelessness/#top) were added to prevent others from losing their homes during the outbreak.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>*   [Alameda County](http://www.acphd.org/2019-ncov.aspx)\n*   [Alpine County](http://alpinecountyca.gov/Index.aspx?NID=516)\n*   [Amador County](https://www.amadorgov.org/services/covid-19)\n*   [Butte County](https://www.buttecounty.net/publichealth)\n*   [Calaveras County](https://covid19.calaverasgov.us/)\n*   [Colusa County](https://www.countyofcolusa.org/99/Public-Health)\n*   [Contra Costa County](https://www.coronavirus.cchealth.org/)\n*   [Del Norte County](http://www.co.del-norte.ca.us/departments/health-human-services/public-health)\n*   [El Dorado County](https://www.edcgov.us/Government/hhsa/Pages/EDCCOVID-19.aspx)\n*   [Fresno County](https://www.co.fresno.ca.us/departments/public-health/covid-19)\n*   [Glenn County](https://www.countyofglenn.net/dept/health-human-services/public-health/covid-19)\n*   [Humboldt County](https://humboldtgov.org/2018/Humboldt-Health-Alert)\n*   [Imperial County](http://www.icphd.org/health-information-and-resources/healthy-facts/covid-19/)\n*   [Inyo County](https://www.inyocounty.us/coronavirus-covid-19-response)\n*   [Kern County](https://kernpublichealth.com/2019-novel-coronavirus/)\n*   [Kings County](https://www.countyofkings.com/departments/health-welfare/public-health/coronavirus-disease-2019-covid-19/-fsiteid-1)\n*   [Lake County](http://health.co.lake.ca.us/Coronavirus.htm)\n*   [Lassen County](http://www.co.lassen.ca.us/)\n*   [Los Angeles County](http://publichealth.lacounty.gov/media/Coronavirus/)\n*   [Madera County](https://www.maderacounty.com/government/public-health/health-updates/corona-virus)\n*   [Marin County](https://coronavirus.marinhhs.org/)\n*   [Mariposa County](http://www.mariposacounty.org/1592/COVID-19-Information)\n*   [Mendocino County](https://www.mendocinocounty.org/community/novel-coronavirus)\n*   [Merced County](https://www.co.merced.ca.us/3350/Coronavirus-Disease-2019)\n*   [Modoc County](http://www.co.modoc.ca.us/)\n*   [Mono County](https://coronavirus.monocounty.ca.gov/)\n*   [Monterey County](https://www.co.monterey.ca.us/government/departments-a-h/health/diseases/2019-novel-coronavirus-covid-19)\n*   [Napa County](https://www.countyofnapa.org/2739/Coronavirus)\n*   [Nevada County](https://www.mynevadacounty.com/2924/Coronavirus)\n*   [Orange County](https://www.ochealthinfo.com/phs/about/epidasmt/epi/dip/prevention/novel_coronavirus)\n*   [Placer County](https://www.placer.ca.gov/coronavirus)\n*   [Plumas County](https://www.plumascounty.us/2669/Novel-Coronavirus-2019-COVID-19)\n*   [Riverside County](https://www.rivcoph.org/coronavirus)\n*   [Sacramento County](https://dhs.saccounty.net/PUB/Pages/PUB-Home.aspx)\n*   [San Benito County](https://hhsa.cosb.us/publichealth/communicable-disease/coronavirus/)\n*   [San Bernardino County](http://wp.sbcounty.gov/dph/coronavirus/)\n*   [San Diego County](https://www.sandiegocounty.gov/coronavirus.html)\n*   [San Francisco City and County](https://sf.gov/topics/coronavirus-covid-19)\n*   [San Joaquin County](https://www.sjgov.org/covid19/)\n*   [San Luis Obispo County](https://www.emergencyslo.org/en/covid19.aspx)\n*   [San Mateo County](https://www.smchealth.org/coronavirus)\n*   [Santa Barbara County](https://publichealthsbc.org/)\n*   [Santa Clara County](https://www.sccgov.org/sites/phd/DiseaseInformation/novel-coronavirus/Pages/home.aspx)\n*   [Santa Cruz County](https://www.santacruzhealth.org/HSAHome/HSADivisions/PublicHealth/CommunicableDiseaseControl/Coronavirus.aspx)\n*   [Shasta County](https://www.co.shasta.ca.us/index/hhsa/health-safety/current-heath-concerns/coronavirus)\n*   [Sierra County](http://sierracounty.ca.gov/582/Coronavirus-COVID-19)\n*   [Siskiyou County](https://www.co.siskiyou.ca.us/publichealth/page/covid-19-what-siskiyou-county-residents-need-know-now)\n*   [Solano County](http://www.solanocounty.com/depts/ph/ncov.asp)\n*   [Sonoma County](https://socoemergency.org/emergency/novel-coronavirus/)\n*   [Stanislaus County](http://schsa.org/publichealth/pages/corona-virus/)\n*   [Sutter County](https://www.suttercounty.org/doc/government/depts/cao/em/coronavirus)\n*   [Tehama County](https://www.tehamacohealthservices.net/services/communicable-diseases/#current-events)\n*   [Trinity County](https://www.trinitycounty.org/)\n*   [Tulare County](https://tchhsa.org/eng/index.cfm/public-health/covid-19-updates-novel-coronavirus/)\n*   [Tuolumne County](https://www.tuolumnecounty.ca.gov/250/Public-Health)\n*   [Ventura County](https://www.vcemergency.com/)\n*   [Yolo County](https://www.yolocounty.org/health-human-services/adults/communicable-disease-investigation-and-control/novel-coronavirus-2019)\n*   [Yuba County](https://www.yuba.org/coronavirus/)\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C124" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3606,10 +3606,10 @@
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v>How is the state protecting incarcerated people in California?</v>
+        <v>What are the restrictions in my area?</v>
       </c>
       <c r="B125" t="str">
-        <v>[California Department of Corrections and Rehabilitation (CDCR)](https://www.cdcr.ca.gov/covid19/) is dedicated to the safety of everyone who lives in, works in, and visits state prisons. CDCR has given all staff and inmates 2 reusable cloth masks to wear while moving between cells, dorms, meetings with others, or health care appointments. CDCR also requires ongoing testing for all staff working in adult institutions, suspended non-essential transfer of inmates, and suspended volunteer services and in-person visiting.\n\nSee [CDCR’s COVID-19 Response Efforts](https://www.cdcr.ca.gov/covid19/covid-19-response-efforts/) for more detailed information.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>While each county may have different restrictions, it is important to stay home as much as possible. If you do go out, stay 6 feet away from others who are not in your household and wear a mask or face covering. Your actions save lives.\n\nSee what [industries are open or closed](https://covid19.ca.gov/safer-economy) in your county.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C125" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3632,10 +3632,10 @@
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v>Who can I contact about my child custody order and child visitation rights?</v>
+        <v>How are we helping the homeless?</v>
       </c>
       <c r="B126" t="str">
-        <v>Court operations vary from county to county. You can use the [California Courts Self-Help Center](https://www.courts.ca.gov/selfhelp.htm) or reach out to your [local government office](https://www.courts.ca.gov/find-my-court.htm?query=browse_courts) for more information. \n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
+        <v>Each county and local government in California has [increased resources](https://covid19.ca.gov/housing-and-homelessness/#top) to protect people experiencing homelessness during COVID-19. [Financial protections](https://covid19.ca.gov/housing-and-homelessness/#top) were added to prevent others from losing their homes during the outbreak.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C126" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3658,10 +3658,10 @@
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v>Do I have to report to jury duty if summoned?</v>
+        <v>How is the state protecting incarcerated people in California?</v>
       </c>
       <c r="B127" t="str">
-        <v>Court operations vary from county to county. You can use the [California Courts Self-Help Center](https://www.courts.ca.gov/selfhelp.htm) or reach out to your [local government office](https://www.courts.ca.gov/find-my-court.htm?query=browse_courts) for more information about jury duty.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)&lt;!-- jury duty, summons, courts, court, court operations--&gt;</v>
+        <v>[California Department of Corrections and Rehabilitation (CDCR)](https://www.cdcr.ca.gov/covid19/) is dedicated to the safety of everyone who lives in, works in, and visits state prisons. CDCR has given all staff and inmates 2 reusable cloth masks to wear while moving between cells, dorms, meetings with others, or health care appointments. CDCR also requires ongoing testing for all staff working in adult institutions, suspended non-essential transfer of inmates, and suspended volunteer services and in-person visiting.\n\nSee [CDCR’s COVID-19 Response Efforts](https://www.cdcr.ca.gov/covid19/covid-19-response-efforts/) for more detailed information.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C127" t="str">
         <v>https://covid19.ca.gov/state-local-resources/</v>
@@ -3684,13 +3684,13 @@
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v>I am an immigrant Californian. Are there organizations that can help me?</v>
+        <v>Who can I contact about my child custody order and child visitation rights?</v>
       </c>
       <c r="B128" t="str">
-        <v>Yes. The California Immigrant Resilience Fund is raising $50 million to provide cash assistance to undocumented Californians who are ineligible for other COVID-19 programs. Visit the [California Immigrant Resilience Fund](http://www.immigrantfundca.org) website to see if you can benefit from this program.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>Court operations vary from county to county. You can use the [California Courts Self-Help Center](https://www.courts.ca.gov/selfhelp.htm) or reach out to your [local government office](https://www.courts.ca.gov/find-my-court.htm?query=browse_courts) for more information. \n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)</v>
       </c>
       <c r="C128" t="str">
-        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
+        <v>https://covid19.ca.gov/state-local-resources/</v>
       </c>
       <c r="D128" t="str">
         <v xml:space="preserve"> </v>
@@ -3710,13 +3710,13 @@
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v>What other government programs are immigrants eligible for during the COVID-19 pandemic?</v>
+        <v>Do I have to report to jury duty if summoned?</v>
       </c>
       <c r="B129" t="str">
-        <v>Check the [Guide for Immigrant Californians (PDF)](/wp-content/uploads/2020/04/LISTOS_COVID_19_immigrant_guidance_EN_dAf.pdf). It has information about jobs, wages, benefits, and small business and housing support.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
+        <v>Court operations vary from county to county. You can use the [California Courts Self-Help Center](https://www.courts.ca.gov/selfhelp.htm) or reach out to your [local government office](https://www.courts.ca.gov/find-my-court.htm?query=browse_courts) for more information about jury duty.\n\nMore info: [Get local information](https://covid19.ca.gov/state-local-resources/)&lt;!-- jury duty, summons, courts, court, court operations--&gt;</v>
       </c>
       <c r="C129" t="str">
-        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
+        <v>https://covid19.ca.gov/state-local-resources/</v>
       </c>
       <c r="D129" t="str">
         <v xml:space="preserve"> </v>
@@ -3736,13 +3736,13 @@
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v>Youth and Teens</v>
+        <v>I am an immigrant Californian. Are there organizations that can help me?</v>
       </c>
       <c r="B130" t="str">
-        <v>*   [California Youth Crisis Line](https://calyouth.org/cycl/)**:** Youth ages 12-24 can call or text [800-843-5200](tel:800-843-5200) or [chat online](https://m2.icarol.com/ConsumerRegistration.aspx?org=53141&amp;pid=326&amp;cc=en-US) for 24/7 crisis support.\n*   [TEEN LINE](https://teenlineonline.org/talk-now/): Teens can talk to another teen by texting “TEEN” to [839863](sms:839863) from 6pm – 9pm, or call [800-852-8336](tel:800-852-8336) from 6pm – 10pm.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>Yes. The California Immigrant Resilience Fund is raising $50 million to provide cash assistance to undocumented Californians who are ineligible for other COVID-19 programs. Visit the [California Immigrant Resilience Fund](http://www.immigrantfundca.org) website to see if you can benefit from this program.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C130" t="str">
-        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
+        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
       </c>
       <c r="D130" t="str">
         <v xml:space="preserve"> </v>
@@ -3762,13 +3762,13 @@
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v>Veterans</v>
+        <v>What other government programs are immigrants eligible for during the COVID-19 pandemic?</v>
       </c>
       <c r="B131" t="str">
-        <v>[Veterans Crisis Line](https://www.veteranscrisisline.net): Call [800-273-8255](tel:800-273-8255) and Press 1 or text [838255](sms:838255) for 24/7 support.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>Check the [Guide for Immigrant Californians (PDF)](/wp-content/uploads/2020/04/LISTOS_COVID_19_immigrant_guidance_EN_dAf.pdf). It has information about jobs, wages, benefits, and small business and housing support.\n\nMore info: [Help for immigrants](https://covid19.ca.gov/guide-immigrant-californians/)</v>
       </c>
       <c r="C131" t="str">
-        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
+        <v>https://covid19.ca.gov/guide-immigrant-californians/</v>
       </c>
       <c r="D131" t="str">
         <v xml:space="preserve"> </v>
@@ -3788,10 +3788,10 @@
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v>First Responders and Law Enforcement</v>
+        <v>Youth and Teens</v>
       </c>
       <c r="B132" t="str">
-        <v>*   [Fire/EMS helpline](https://www.nvfc.org/fireems-helpline/): Call [888-731-FIRE](tel:888-731-FIRE) to get 24/7 help for a variety of behavioral health issues.\n*   [COPLINE](https://www.copline.org/): Call [800-267-5463](tel:800-267-5463) to find support 24/7 for law enforcement officers.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>*   [California Youth Crisis Line](https://calyouth.org/cycl/)**:** Youth ages 12-24 can call or text [800-843-5200](tel:800-843-5200) or [chat online](https://m2.icarol.com/ConsumerRegistration.aspx?org=53141&amp;pid=326&amp;cc=en-US) for 24/7 crisis support.\n*   [TEEN LINE](https://teenlineonline.org/talk-now/): Teens can talk to another teen by texting “TEEN” to [839863](sms:839863) from 6pm – 9pm, or call [800-852-8336](tel:800-852-8336) from 6pm – 10pm.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C132" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -3814,10 +3814,10 @@
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v>Older Californians</v>
+        <v>Veterans</v>
       </c>
       <c r="B133" t="str">
-        <v>*   [Friendship Line](https://www.ioaging.org/services/all-inclusive-health-care/friendship-line): Call [888-670-1360](tel:888-670-1360) for 24/7 support if you are 60 years or older, or an adult living with disabilities.  \n*   California Aging and Adult Information Line: Call [800-510-2020](tel:800-510-2020) for help finding local assistance. \n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>[Veterans Crisis Line](https://www.veteranscrisisline.net): Call [800-273-8255](tel:800-273-8255) and Press 1 or text [838255](sms:838255) for 24/7 support.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C133" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -3840,10 +3840,10 @@
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v>Deaf and Hard of Hearing Individuals</v>
+        <v>First Responders and Law Enforcement</v>
       </c>
       <c r="B134" t="str">
-        <v>[National Suicide Prevention Deaf and Hard of Hearing Hotline](https://suicidepreventionlifeline.org/help-yourself/for-deaf-hard-of-hearing/): Access 24/7 video relay service by dialing [800-273-8255](tel:800-273-8255) (TTY [800-799-4889](tel:800-799-4889)).\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>*   [Fire/EMS helpline](https://www.nvfc.org/fireems-helpline/): Call [888-731-FIRE](tel:888-731-FIRE) to get 24/7 help for a variety of behavioral health issues.\n*   [COPLINE](https://www.copline.org/): Call [800-267-5463](tel:800-267-5463) to find support 24/7 for law enforcement officers.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C134" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -3866,10 +3866,10 @@
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v>Services for Substance Use Disorders</v>
+        <v>Older Californians</v>
       </c>
       <c r="B135" t="str">
-        <v>*   [SAMHSA National Helpline](https://www.samhsa.gov/find-help/national-helpline): Call [800-662-HELP](tel:1-800-662-4357) for 24/7 information and referrals in English and Spanish. \n*   [SAMHSA Treatment Locator](https://findtreatment.samhsa.gov)**:**  Find drug or alcohol treatment programs. \n*   [Local county access lines](https://gcc01.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.dhcs.ca.gov%2Findividuals%2FPages%2FSUD_County_Access_Lines.aspx&amp;data=02%7C01%7CJanne.Olson-Morgan%40osg.ca.gov%7C122307be91754d12e5dc08d7d984f958%7C265c2dcd2a6e43aab2e826421a8c8526%7C0%7C0%7C637217037446186621&amp;sdata=5sx4UdIlVkRL%2BEJR7FrpK0gYAn20yE71TyBDFIw1kJM%3D&amp;reserved=0): Find your local number for help seeking substance use disorder services.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>*   [Friendship Line](https://www.ioaging.org/services/all-inclusive-health-care/friendship-line): Call [888-670-1360](tel:888-670-1360) for 24/7 support if you are 60 years or older, or an adult living with disabilities.  \n*   California Aging and Adult Information Line: Call [800-510-2020](tel:800-510-2020) for help finding local assistance. \n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C135" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -3892,10 +3892,10 @@
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v>LGBTQ Individuals</v>
+        <v>Deaf and Hard of Hearing Individuals</v>
       </c>
       <c r="B136" t="str">
-        <v>*   [Trevor Project](https://www.thetrevorproject.org): Call [866-488-7386](tel:866-488-7386) or text START to [678678](sms:678678) for 24/7 information and suicide prevention resources for LGBTQ youth.\n*   [Lesbian, Gay, Bisexual and Transgender National Hotline](https://www.glbthotline.org/hotline.html): Call [800-273-8255](tel:800-273-8255) from 1pm – 9pm for support, information or help finding resources.\n*   [Victims of Crime Resource Center](https://1800victims.org/): Call or text [800-842-8467](tel:800-842-8467) or [chat online](https://1800victims.org/) for information about LGTBQ rights, legal protections, and local resources.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
+        <v>[National Suicide Prevention Deaf and Hard of Hearing Hotline](https://suicidepreventionlifeline.org/help-yourself/for-deaf-hard-of-hearing/): Access 24/7 video relay service by dialing [800-273-8255](tel:800-273-8255) (TTY [800-799-4889](tel:800-799-4889)).\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C136" t="str">
         <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
@@ -3918,13 +3918,13 @@
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v>What is a close contact?</v>
+        <v>Services for Substance Use Disorders</v>
       </c>
       <c r="B137" t="str">
-        <v>A [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) is someone who was within 6 feet of a person with COVID-19 for at least 15 minutes starting from 2 days before symptoms appeared (or, for asymptomatic patients, 2 days prior to their test) until the time the patient is isolated. This usually includes household members, intimate contacts, and caregivers, but can include others.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>*   [SAMHSA National Helpline](https://www.samhsa.gov/find-help/national-helpline): Call [800-662-HELP](tel:1-800-662-4357) for 24/7 information and referrals in English and Spanish. \n*   [SAMHSA Treatment Locator](https://findtreatment.samhsa.gov)**:**  Find drug or alcohol treatment programs. \n*   [Local county access lines](https://gcc01.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.dhcs.ca.gov%2Findividuals%2FPages%2FSUD_County_Access_Lines.aspx&amp;data=02%7C01%7CJanne.Olson-Morgan%40osg.ca.gov%7C122307be91754d12e5dc08d7d984f958%7C265c2dcd2a6e43aab2e826421a8c8526%7C0%7C0%7C637217037446186621&amp;sdata=5sx4UdIlVkRL%2BEJR7FrpK0gYAn20yE71TyBDFIw1kJM%3D&amp;reserved=0): Find your local number for help seeking substance use disorder services.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C137" t="str">
-        <v>https://covid19.ca.gov/contact-tracing/</v>
+        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
       </c>
       <c r="D137" t="str">
         <v xml:space="preserve"> </v>
@@ -3944,13 +3944,13 @@
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v>Will contact tracers track my location?</v>
+        <v>LGBTQ Individuals</v>
       </c>
       <c r="B138" t="str">
-        <v>California’s contact tracing program does not use any cell phone tracking technology. Someone from your local public health department will simply speak privately with you. All information is confidential and protected by California’s strict privacy laws. They may stay in touch to make sure your symptoms aren’t worsening.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>*   [Trevor Project](https://www.thetrevorproject.org): Call [866-488-7386](tel:866-488-7386) or text START to [678678](sms:678678) for 24/7 information and suicide prevention resources for LGBTQ youth.\n*   [Lesbian, Gay, Bisexual and Transgender National Hotline](https://www.glbthotline.org/hotline.html): Call [800-273-8255](tel:800-273-8255) from 1pm – 9pm for support, information or help finding resources.\n*   [Victims of Crime Resource Center](https://1800victims.org/): Call or text [800-842-8467](tel:800-842-8467) or [chat online](https://1800victims.org/) for information about LGTBQ rights, legal protections, and local resources.\n\nMore info: [Resources for emotional support and well-being](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/)</v>
       </c>
       <c r="C138" t="str">
-        <v>https://covid19.ca.gov/contact-tracing/</v>
+        <v>https://covid19.ca.gov/resources-for-emotional-support-and-well-being/</v>
       </c>
       <c r="D138" t="str">
         <v xml:space="preserve"> </v>
@@ -3970,10 +3970,10 @@
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>Is contact tracing help available in my language?</v>
+        <v>What is a close contact?</v>
       </c>
       <c r="B139" t="str">
-        <v>Your [local health department](https://covid19.ca.gov/get-local-information/) can communicate with you in many different languages.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>A [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) is someone who was within 6 feet of a person with COVID-19 for at least 15 minutes starting from 2 days before symptoms appeared (or, for asymptomatic patients, 2 days prior to their test) until the time the patient is isolated. This usually includes household members, intimate contacts, and caregivers, but can include others.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C139" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -3996,10 +3996,10 @@
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>Who should get tested for coronavirus?</v>
+        <v>Will contact tracers track my location?</v>
       </c>
       <c r="B140" t="str">
-        <v>You should get tested if you:\n\n*   Had [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) with anyone who has tested positive for COVID-19\n*   Have COVID-19 symptoms\n*   Get a call from a contact tracer\n*   Are at [high risk](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Updated-COVID-19-Testing-Guidance.aspx)\n\nFind a [testing site in your area](https://covid19.ca.gov/testing-and-treatment/).\n\nIf you think you may have been exposed, call your doctor.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>California’s contact tracing program does not use any cell phone tracking technology. Someone from your local public health department will simply speak privately with you. All information is confidential and protected by California’s strict privacy laws. They may stay in touch to make sure your symptoms aren’t worsening.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C140" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4022,10 +4022,10 @@
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>How do I find a coronavirus testing location?</v>
+        <v>Is contact tracing help available in my language?</v>
       </c>
       <c r="B141" t="str">
-        <v>To learn more about testing and care, visit the [Testing and treatment page](https://covid19.ca.gov/testing-and-treatment/). You can search for testing locations there using your zip code. \n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>Your [local health department](https://covid19.ca.gov/get-local-information/) can communicate with you in many different languages.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C141" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4048,10 +4048,10 @@
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>What if I have COVID-19 symptoms and have not been contacted by the health department?</v>
+        <v>Who should get tested for coronavirus?</v>
       </c>
       <c r="B142" t="str">
-        <v>[Get tested](https://covid19.ca.gov/testing-and-treatment/) immediately. Contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing, and [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) yourself until:\n\n*   at least 10 days have passed since symptoms started, **AND**\n*   your fever has been gone for 24 hours without the aid of medication, **AND** \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested. Read more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>You should get tested if you:\n\n*   Had [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) with anyone who has tested positive for COVID-19\n*   Have COVID-19 symptoms\n*   Get a call from a contact tracer\n*   Are at [high risk](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Updated-COVID-19-Testing-Guidance.aspx)\n\nFind a [testing site in your area](https://covid19.ca.gov/testing-and-treatment/).\n\nIf you think you may have been exposed, call your doctor.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C142" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4074,10 +4074,10 @@
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>What if I came in contact with someone who has COVID-19 symptoms, but my local health department is not aware of it?</v>
+        <v>How do I find a coronavirus testing location?</v>
       </c>
       <c r="B143" t="str">
-        <v>You should [get tested](https://covid19.ca.gov/testing-and-treatment/). Contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing. [Quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) yourself while waiting for your test results.\n\n**If you tested positive but have no symptoms**, you should [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) at home for at least 10 days.\n\n**If you develop symptoms**, you should stay home until:\n\n*   at least 10 days have passed since symptoms started, **AND**\n*   your fever has been gone for 24 hours without the aid of medication, **AND** \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested.\n\n**If you had [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) with someone who tested positive but you tested negative**, you should still [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) at home for at least 14 days.\n\nRead more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>To learn more about testing and care, visit the [Testing and treatment page](https://covid19.ca.gov/testing-and-treatment/). You can search for testing locations there using your zip code. \n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C143" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4100,10 +4100,10 @@
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>How do I become a contact tracer?</v>
+        <v>What if I have COVID-19 symptoms and have not been contacted by the health department?</v>
       </c>
       <c r="B144" t="str">
-        <v>California Connected is using existing state employees for contact tracing. We appreciate offers of additional support from the private sector and qualified members of the public, but they are not needed at this time.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>[Get tested](https://covid19.ca.gov/testing-and-treatment/) immediately. Contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing, and [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) yourself until:\n\n*   at least 10 days have passed since symptoms started, **AND**\n*   your fever has been gone for 24 hours without the aid of medication, **AND** \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested. Read more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C144" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4126,10 +4126,10 @@
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>Is there extra sick leave available for workers who have COVID-19 symptoms or are waiting for test results?</v>
+        <v>What if I came in contact with someone who has COVID-19 symptoms, but my local health department is not aware of it?</v>
       </c>
       <c r="B145" t="str">
-        <v>Yes. There are extra federal, state, and in some cases, local sick leaves available for workers in this situation:\n\n*   **Federal paid sick leave:** Up to 80 hours under the Families First Coronavirus Response Act ([FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-employee-paid-leave)) for businesses with less than 500 workers. See [more information on FFCRA in its FAQs](https://www.dol.gov/agencies/whd/pandemic/ffcra-questions).\n*   **California COVID-19 supplemental paid sick leave:** Food businesses with more than 500 workers must give up to 80 hours of [paid sick leave](https://www.gov.ca.gov/wp-content/uploads/2020/04/4.16.20-EO-N-51-20.pdf).  See [more information on supplemental paid sick leave](https://www.dir.ca.gov/dlse/FAQ-for-PSL.html). \n*   **Local paid sick leave ordinances:** Certain local areas also have paid sick leave ordinances.  Consult with the local enforcement agency in your area.\n\nTo understand what may be available, see the comparison of [COVID-19 sick leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) and [benefits for workers impacted by COVID-19](https://www.labor.ca.gov/coronavirus2019/#chart).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>You should [get tested](https://covid19.ca.gov/testing-and-treatment/). Contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing. [Quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) yourself while waiting for your test results.\n\n**If you tested positive but have no symptoms**, you should [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) at home for at least 10 days.\n\n**If you develop symptoms**, you should stay home until:\n\n*   at least 10 days have passed since symptoms started, **AND**\n*   your fever has been gone for 24 hours without the aid of medication, **AND** \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested.\n\n**If you had [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) with someone who tested positive but you tested negative**, you should still [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) at home for at least 14 days.\n\nRead more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C145" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4152,10 +4152,10 @@
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>Can I return to work once my isolation or quarantine is over?</v>
+        <v>How do I become a contact tracer?</v>
       </c>
       <c r="B146" t="str">
-        <v>Yes, but when you return depends on your situation.\n\n**If you have symptoms**, you should stay home until:\n\n*   at least 10 days have passed since symptoms started, **AND**\n*    your fever has been gone for 24 hours without the aid of medication, **AND** \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested.\n\n**If you have tested positive but have no symptoms**, you should [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) at home for at least 10 days.\n\n**If you had [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) with someone who tested positive but you have tested negative**, you should still [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) at home for at least 14 days.\n\nGet tested as soon as possible if you have symptoms, or have come in contact with someone who has tested positive or has symptoms.\n\nRead more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>California Connected is using existing state employees for contact tracing. We appreciate offers of additional support from the private sector and qualified members of the public, but they are not needed at this time.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C146" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4178,10 +4178,10 @@
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>What steps are required when a business has an employee who tests positive?</v>
+        <v>Is there extra sick leave available for workers who have COVID-19 symptoms or are waiting for test results?</v>
       </c>
       <c r="B147" t="str">
-        <v>If an employer discovers a worker has tested positive for COVID-19 or has symptoms, they should send the worker home. Then [follow guidance](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf) about isolation, quarantine, testing, and when the worker should return to work. Employers should have flexible leave policies. This supports the need for workers to stay home for the protection of others. \n\nThe employer must notify the local health department about the confirmed COVID-19 workers. They must tell their:\n\n*   job titles, \n*   work areas, \n*   [close contacts](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) in the workplace, \n*   dates of symptom onset, and \n*   shifts worked while infectious.\n\nSee “What to do if there is a Case of COVID-19 in the Workplace” in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf). \n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>Yes. There are extra federal, state, and in some cases, local sick leaves available for workers in this situation:\n\n*   **Federal paid sick leave:** Up to 80 hours under the Families First Coronavirus Response Act ([FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-employee-paid-leave)) for businesses with less than 500 workers. See [more information on FFCRA in its FAQs](https://www.dol.gov/agencies/whd/pandemic/ffcra-questions).\n*   **California COVID-19 supplemental paid sick leave:** Food businesses with more than 500 workers must give up to 80 hours of [paid sick leave](https://www.gov.ca.gov/wp-content/uploads/2020/04/4.16.20-EO-N-51-20.pdf).  See [more information on supplemental paid sick leave](https://www.dir.ca.gov/dlse/FAQ-for-PSL.html). \n*   **Local paid sick leave ordinances:** Certain local areas also have paid sick leave ordinances.  Consult with the local enforcement agency in your area.\n\nTo understand what may be available, see the comparison of [COVID-19 sick leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) and [benefits for workers impacted by COVID-19](https://www.labor.ca.gov/coronavirus2019/#chart).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C147" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4204,10 +4204,10 @@
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>Can people who recover from COVID-19 be re-infected?</v>
+        <v>Can I return to work once my isolation or quarantine is over?</v>
       </c>
       <c r="B148" t="str">
-        <v>We don’t yet know. The duration of immunity to coronavirus infection is not yet understood. Patients infected with similar viruses are unlikely to be re-infected in the months after they recover. But we don’t yet know if  similar immune protection happens in patients with COVID-19.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>Yes, but when you return depends on your situation.\n\n**If you have symptoms**, you should stay home until:\n\n*   at least 10 days have passed since symptoms started, **AND**\n*    your fever has been gone for 24 hours without the aid of medication, **AND** \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested.\n\n**If you have tested positive but have no symptoms**, you should [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) at home for at least 10 days.\n\n**If you had [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) with someone who tested positive but you have tested negative**, you should still [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) at home for at least 14 days.\n\nGet tested as soon as possible if you have symptoms, or have come in contact with someone who has tested positive or has symptoms.\n\nRead more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C148" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4230,10 +4230,10 @@
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v>How do I apply for a contact tracer position?</v>
+        <v>What steps are required when a business has an employee who tests positive?</v>
       </c>
       <c r="B149" t="str">
-        <v>California Connected is using existing state employees for contact tracing. We appreciate offers of additional support from the private sector and qualified members of the public, but they are not needed at this time.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>If an employer discovers a worker has tested positive for COVID-19 or has symptoms, they should send the worker home. Then [follow guidance](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf) about isolation, quarantine, testing, and when the worker should return to work. Employers should have flexible leave policies. This supports the need for workers to stay home for the protection of others. \n\nThe employer must notify the local health department about the confirmed COVID-19 workers. They must tell their:\n\n*   job titles, \n*   work areas, \n*   [close contacts](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) in the workplace, \n*   dates of symptom onset, and \n*   shifts worked while infectious.\n\nSee “What to do if there is a Case of COVID-19 in the Workplace” in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf). \n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C149" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4256,10 +4256,10 @@
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>How do I sign-up for a contact tracer position?</v>
+        <v>Can people who recover from COVID-19 be re-infected?</v>
       </c>
       <c r="B150" t="str">
-        <v>California Connected is using existing state employees for contact tracing. We appreciate offers of additional support from the private sector and qualified members of the public, but they are not needed at this time.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
+        <v>We don’t yet know. The duration of immunity to coronavirus infection is not yet understood. Patients infected with similar viruses are unlikely to be re-infected in the months after they recover. But we don’t yet know if  similar immune protection happens in patients with COVID-19.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C150" t="str">
         <v>https://covid19.ca.gov/contact-tracing/</v>
@@ -4282,13 +4282,13 @@
     </row>
     <row r="151">
       <c r="A151" t="str">
-        <v>Drive-through testing in Northern California</v>
+        <v>How do I apply for a contact tracer position?</v>
       </c>
       <c r="B151" t="str">
-        <v>*   Alturas (Modoc County)\n*   American Canyon (Napa County)\n*   Antioch (Contra Costa County)\n*   Atascadero (San Luis Obispo County)\n*   Bear Valley (Alpine County)\n*   Bieber (Lassen County)\n*   Bishop (Inyo County)\n*   Calistoga (Napa County)\n*   Calpine (Sierra County)\n*   Cedarville (Modoc County)\n*   Ceres (Sanislaus County)\n*   Chowchilla (Madera County)\n*   Clearlake (Lake County)\n*   Coleville (Mono County)\n*   Corcoran (King County)\n*   Corona (King County)\n*   Crescent City (Del Norte County)\n*   Daly City (San Mateo County)\n*   Dinuba (Tulare County)\n*   Downieville (Sierra County)\n*   Doyle (Lassen County)\n*   East Palo Alto (San Mateo County)\n*   Elk Grove (Sacramento County)\n*   Exeter (Tulare County)\n*   Farmersville (Tulare County)\n*   French Camp (San Joaquin County)\n*   Fresno (Fresno County)\n*   Gridley (Butte County)\n*   Half Moon Bay (San Mateo County)\n*   Hanford (King County)\n*   Hayfork (Trinity County)\n*   Herlong (Lassen County)\n*   Huron (Fresno County)\n*   Jackson (Amador County)\n*   Kerman (Fresno County)\n*   Lakeport (Lake County)\n*   Lee Vining (Mono County)\n*   Lemoore (King County)\n*   Lewiston (Trinity County)\n*   Livingston (Merced County)\n*   Lone Pine (Inyo County)\n*   Los Banos (Merced County)\n*   Loyalton (Sierra County)\n*   Magalia (Butte County)\n*   Mammoth Lakes (Mono County)\n*   Markleeville (Alpine County)\n*   Mendota (Fresno County)\n*   Merced (Merced County)\n*   Middletown (Lake County)\n*   Napa (Napa County)\n*   North San Juan (Nevada County)\n*   Oakland (Alameda County)\n*   Placerville (El Dorado County)\n*   Porterville (Tulare County)\n*   Redding (Shasta County)\n*   Redwood City (San Mateo County)\n*   Reedley (Fresno County)\n*   Rio Linda (Sacramento County)\n*   Sacramento (Sacramento County)\n*   Salida (Stanislaus County)\n*   San Bruno (San Mateo County)\n*   San Francisco (San Francisco)\n*   San Jose (Santa Clara County)\n*   San Mateo (San Mateo County)\n*   Santa Rosa (Sonoma County)\n*   Selma (Fresno County)\n*   St. Helena (Napa County)\n*   Stockton (San Joaquin County)\n*   Susanville (Lassen County)\n*   Tracy (San Joaquin County)\n*   Tulare (Tulare County)\n*   Turlock (Stanislaus County)\n*   Upper Lake (Lake County)\n*   Vallejo (Solano County)\n*   Visalia (Tulare County)\n*   Wawona (Mariposa County)\n*   Weaverville (Trinity County)\n*   Westwood (Lassen County)\n\n*   Woodlake (Tulare County)\n*   Woodland (Yolo County)\n*   Yosemite Valley (Mariposa County)\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>California Connected is using existing state employees for contact tracing. We appreciate offers of additional support from the private sector and qualified members of the public, but they are not needed at this time.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C151" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D151" t="str">
         <v xml:space="preserve"> </v>
@@ -4308,13 +4308,13 @@
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>Drive-through testing in Southern California</v>
+        <v>How do I sign-up for a contact tracer position?</v>
       </c>
       <c r="B152" t="str">
-        <v>*   Alpine (San Diego County) \n*   Anaheim (Orange County)\n*   Apple Valley (San Bernardino County)\n*   Bakersfield (Kern County)\n*   Banning (Riverside County)\n*   Barstow (San Bernardino County)\n*   Beaumont (Riverside County)\n*   Bell (Los Angeles County)\n*   Blythe (Riverside County)\n*   Calexico (Imperial County)\n*   Coachella (Riverside County)\n*   Compton (Los Angeles County)\n*   Costa Mesa (Orange County)\n*   Delano (Kern County)\n*   Desert Hot Springs (Riverside County)\n*   El Centro (Imperial County)\n*   Fallbrook (San Diego)\n*   Fontana (San Bernardino County)\n*   Fullerton (Orange County)\n*   Gardena (Los Angeles County)\n*   Hemet (Riverside County)\n*   Hesperia (San Bernardino County)\n*   Indio (Riverside County)\n*   La Habra (Orange County)\n*   Lake Elsinore (Riverside County)\n*   Lamont (Kern County)\n*   Lancaster (Los Angeles County)\n*   Lemon Grove (San Diego County)\n*   Los Angeles (Los Angeles County)\n*   McFarland (Kern County)\n*   Oceanside (San Diego)\n*   Ontario (San Bernardino County)\n*   Palmdale (Los Angeles County)\n*   Paramount (Los Angeles County)\n*   Pasadena (Los Angeles County)\n*   Perris (Riverside County)\n*   Phelan (San Bernardino County)\n*   Pico Rivera (Los Angeles County)\n*   Pomona (Los Angeles County)\n*   Port Hueneme (Ventura County)\n*   Riverside (Riverside County)\n*   Rosamond (Kern County)\n*   San Jucinta (Riverside County)\n*   San Juan Capistrano (Orange County)\n*   Santa Maria (Santa Barbara County)\n*   Santa Paula (Ventura County)\n*   Shafter (Kern County)\n*   Valley Center (San Diego County)\n*   Victorville (San Bernardino County)\n*   Wasco (Kern County) \n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>California Connected is using existing state employees for contact tracing. We appreciate offers of additional support from the private sector and qualified members of the public, but they are not needed at this time.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C152" t="str">
-        <v>https://covid19.ca.gov/testing-and-treatment/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D152" t="str">
         <v xml:space="preserve"> </v>
@@ -4334,10 +4334,10 @@
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v>How do I get a drive-through test by Verily’s Project Baseline?</v>
+        <v>Drive-through testing in Northern California</v>
       </c>
       <c r="B153" t="str">
-        <v>There are two steps to this process: screening and testing. First, you will create an account and take the online screener. If you are eligible, you will get details on how and where to get tested. Once tested, you’ll get an email or phone call with your COVID-19 test results.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>*   Alturas (Modoc County)\n*   American Canyon (Napa County)\n*   Antioch (Contra Costa County)\n*   Atascadero (San Luis Obispo County)\n*   Bear Valley (Alpine County)\n*   Bieber (Lassen County)\n*   Bishop (Inyo County)\n*   Calistoga (Napa County)\n*   Calpine (Sierra County)\n*   Cedarville (Modoc County)\n*   Ceres (Sanislaus County)\n*   Chowchilla (Madera County)\n*   Clearlake (Lake County)\n*   Coleville (Mono County)\n*   Corcoran (King County)\n*   Corona (King County)\n*   Crescent City (Del Norte County)\n*   Daly City (San Mateo County)\n*   Dinuba (Tulare County)\n*   Downieville (Sierra County)\n*   Doyle (Lassen County)\n*   East Palo Alto (San Mateo County)\n*   Elk Grove (Sacramento County)\n*   Exeter (Tulare County)\n*   Farmersville (Tulare County)\n*   French Camp (San Joaquin County)\n*   Fresno (Fresno County)\n*   Gridley (Butte County)\n*   Half Moon Bay (San Mateo County)\n*   Hanford (King County)\n*   Hayfork (Trinity County)\n*   Herlong (Lassen County)\n*   Huron (Fresno County)\n*   Jackson (Amador County)\n*   Kerman (Fresno County)\n*   Lakeport (Lake County)\n*   Lee Vining (Mono County)\n*   Lemoore (King County)\n*   Lewiston (Trinity County)\n*   Livingston (Merced County)\n*   Lone Pine (Inyo County)\n*   Los Banos (Merced County)\n*   Loyalton (Sierra County)\n*   Magalia (Butte County)\n*   Mammoth Lakes (Mono County)\n*   Markleeville (Alpine County)\n*   Mendota (Fresno County)\n*   Merced (Merced County)\n*   Middletown (Lake County)\n*   Napa (Napa County)\n*   North San Juan (Nevada County)\n*   Oakland (Alameda County)\n*   Placerville (El Dorado County)\n*   Porterville (Tulare County)\n*   Redding (Shasta County)\n*   Redwood City (San Mateo County)\n*   Reedley (Fresno County)\n*   Rio Linda (Sacramento County)\n*   Sacramento (Sacramento County)\n*   Salida (Stanislaus County)\n*   San Bruno (San Mateo County)\n*   San Francisco (San Francisco)\n*   San Jose (Santa Clara County)\n*   San Mateo (San Mateo County)\n*   Santa Rosa (Sonoma County)\n*   Selma (Fresno County)\n*   St. Helena (Napa County)\n*   Stockton (San Joaquin County)\n*   Susanville (Lassen County)\n*   Tracy (San Joaquin County)\n*   Tulare (Tulare County)\n*   Turlock (Stanislaus County)\n*   Upper Lake (Lake County)\n*   Vallejo (Solano County)\n*   Visalia (Tulare County)\n*   Wawona (Mariposa County)\n*   Weaverville (Trinity County)\n*   Westwood (Lassen County)\n\n*   Woodlake (Tulare County)\n*   Woodland (Yolo County)\n*   Yosemite Valley (Mariposa County)\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C153" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4360,10 +4360,10 @@
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v>Why am I asked to create an account for Verily?</v>
+        <v>Drive-through testing in Southern California</v>
       </c>
       <c r="B154" t="str">
-        <v>Verily needs a way to authenticate and protect user information. They turned to Google for this service, because Google accounts have best-in-class authentication. Simply link to an existing Google account or create a new one (which you can do with any email address). Then Verily can contact you securely during the screening and testing process. All data r collected by Verily is kept private and is not linked to a user’s Google account.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>*   Alpine (San Diego County) \n*   Anaheim (Orange County)\n*   Apple Valley (San Bernardino County)\n*   Bakersfield (Kern County)\n*   Banning (Riverside County)\n*   Barstow (San Bernardino County)\n*   Beaumont (Riverside County)\n*   Bell (Los Angeles County)\n*   Blythe (Riverside County)\n*   Calexico (Imperial County)\n*   Coachella (Riverside County)\n*   Compton (Los Angeles County)\n*   Costa Mesa (Orange County)\n*   Delano (Kern County)\n*   Desert Hot Springs (Riverside County)\n*   El Centro (Imperial County)\n*   Fallbrook (San Diego)\n*   Fontana (San Bernardino County)\n*   Fullerton (Orange County)\n*   Gardena (Los Angeles County)\n*   Hemet (Riverside County)\n*   Hesperia (San Bernardino County)\n*   Indio (Riverside County)\n*   La Habra (Orange County)\n*   Lake Elsinore (Riverside County)\n*   Lamont (Kern County)\n*   Lancaster (Los Angeles County)\n*   Lemon Grove (San Diego County)\n*   Los Angeles (Los Angeles County)\n*   McFarland (Kern County)\n*   Oceanside (San Diego)\n*   Ontario (San Bernardino County)\n*   Palmdale (Los Angeles County)\n*   Paramount (Los Angeles County)\n*   Pasadena (Los Angeles County)\n*   Perris (Riverside County)\n*   Phelan (San Bernardino County)\n*   Pico Rivera (Los Angeles County)\n*   Pomona (Los Angeles County)\n*   Port Hueneme (Ventura County)\n*   Riverside (Riverside County)\n*   Rosamond (Kern County)\n*   San Jucinta (Riverside County)\n*   San Juan Capistrano (Orange County)\n*   Santa Maria (Santa Barbara County)\n*   Santa Paula (Ventura County)\n*   Shafter (Kern County)\n*   Valley Center (San Diego County)\n*   Victorville (San Bernardino County)\n*   Wasco (Kern County) \n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C154" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4386,10 +4386,10 @@
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>Do I need emergency treatment?</v>
+        <v>How do I get a drive-through test by Verily’s Project Baseline?</v>
       </c>
       <c r="B155" t="str">
-        <v>If you develop any of these symptoms of COVID-19, get medical attention immediately:\n\n*   Trouble breathing\n*   Persistent pain or pressure in the chest\n*   New confusion \n*   Inability to awake or stay awake\n*   Bluish lips or face\n\nThere are other, less-common symptoms. Please call your medical provider if you have any symptoms that are severe or concern you.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call [911](tel:911), tell the operator you have coronavirus symptoms. This is so ambulance workers can be ready to treat you safely.\n\nNot sure if this applies to you? Check your symptoms with the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>There are two steps to this process: screening and testing. First, you will create an account and take the online screener. If you are eligible, you will get details on how and where to get tested. Once tested, you’ll get an email or phone call with your COVID-19 test results.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C155" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4412,10 +4412,10 @@
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v>When can I be around other people after I had or likely had COVID-19?</v>
+        <v>Why am I asked to create an account for Verily?</v>
       </c>
       <c r="B156" t="str">
-        <v>You can be with others after:\n\n*   10 days since symptoms first appeared **and**\n*   At least 24 hours with no fever without fever-reducing medication **and**\n*   After symptoms have improved\n\nCDC has [detailed recommendations](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/end-home-isolation.html) for people who had tested positive but had no symptoms.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>Verily needs a way to authenticate and protect user information. They turned to Google for this service, because Google accounts have best-in-class authentication. Simply link to an existing Google account or create a new one (which you can do with any email address). Then Verily can contact you securely during the screening and testing process. All data r collected by Verily is kept private and is not linked to a user’s Google account.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C156" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4438,10 +4438,10 @@
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>When can I be around other people after I tested positive for COVID-19 but had no symptoms?</v>
+        <v>Do I need emergency treatment?</v>
       </c>
       <c r="B157" t="str">
-        <v>If you continue to have no symptoms, you can be with others after 10 days have passed since your test.\n\nCDC has [detailed recommendations](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/end-home-isolation.html) for people who had tested positive for coronavirus but had no symptoms.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>If you develop any of these symptoms of COVID-19, get medical attention immediately:\n\n*   Trouble breathing\n*   Persistent pain or pressure in the chest\n*   New confusion \n*   Inability to awake or stay awake\n*   Bluish lips or face\n\nThere are other, less-common symptoms. Please call your medical provider if you have any symptoms that are severe or concern you.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call [911](tel:911), tell the operator you have coronavirus symptoms. This is so ambulance workers can be ready to treat you safely.\n\nNot sure if this applies to you? Check your symptoms with the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C157" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4464,10 +4464,10 @@
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>Should employees be required to provide proof of a negative coronavirus test before returning to work after they had COVID-19?</v>
+        <v>When can I be around other people after I had or likely had COVID-19?</v>
       </c>
       <c r="B158" t="str">
-        <v>No. Proof of a negative test should not be required prior to returning to the workplace after documented COVID infection, since PCR tests can remain positive long after an individual is no longer infectious. CDPH [COVID-19 Testing Guidance](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Updated-COVID-19-Testing-Guidance.aspx) recommends symptom- or protocol-based criteria be used to determine when an employee is safe to return to the workplace.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>You can be with others after:\n\n*   10 days since symptoms first appeared **and**\n*   At least 24 hours with no fever without fever-reducing medication **and**\n*   After symptoms have improved\n\nCDC has [detailed recommendations](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/end-home-isolation.html) for people who had tested positive but had no symptoms.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C158" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4490,10 +4490,10 @@
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>Can two people that both tested positive hang out/stay together?</v>
+        <v>When can I be around other people after I tested positive for COVID-19 but had no symptoms?</v>
       </c>
       <c r="B159" t="str">
-        <v>No. You should take preventive measures to protect yourself and others. We do not know yet if or when a person can be reinfected with COVID-19. \n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>If you continue to have no symptoms, you can be with others after 10 days have passed since your test.\n\nCDC has [detailed recommendations](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/end-home-isolation.html) for people who had tested positive for coronavirus but had no symptoms.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C159" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4516,10 +4516,10 @@
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>If I test positive for COVID-19 in a viral test, what should I do to protect others in my household?</v>
+        <v>Should employees be required to provide proof of a negative coronavirus test before returning to work after they had COVID-19?</v>
       </c>
       <c r="B160" t="str">
-        <v>You should [self-isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) from others in your household who have not tested positive. Sleep and stay in a separate room from them, and use a separate bathroom, if possible. Multiple infected people in the same household can use the same room for isolation.\n\nMembers of your household should get tested right away. They should [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) for at least 14 days. Symptoms can develop even after testing negative within 14 days after exposure. Multiple people in the same household should not quarantine in the same room, since some may be infected.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>No. Proof of a negative test should not be required prior to returning to the workplace after documented COVID infection, since PCR tests can remain positive long after an individual is no longer infectious. CDPH [COVID-19 Testing Guidance](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Updated-COVID-19-Testing-Guidance.aspx) recommends symptom- or protocol-based criteria be used to determine when an employee is safe to return to the workplace.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C160" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4542,10 +4542,10 @@
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>How can I find a coronavirus testing location near me?</v>
+        <v>Can two people that both tested positive hang out/stay together?</v>
       </c>
       <c r="B161" t="str">
-        <v>&gt; [Find a testing location](https://arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401)\n&gt; -----------------------------------------------------------------------------------------------------------\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>No. You should take preventive measures to protect yourself and others. We do not know yet if or when a person can be reinfected with COVID-19. \n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C161" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4568,10 +4568,10 @@
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>What is an antibody test? Where can I get an antibody test?</v>
+        <v>If I test positive for COVID-19 in a viral test, what should I do to protect others in my household?</v>
       </c>
       <c r="B162" t="str">
-        <v>[**Antibody tests**](https://www.cdc.gov/coronavirus/2019-ncov/testing/serology-overview.html) detect past infections. They can determine if you are a good candidate to [donate blood plasma](https://covid19.ca.gov/plasma/). It can take 1-3 weeks after infection for your body to make antibodies.\n\nYou can find locations for both viral and antibody tests on [California’s testing map](https://www.arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
+        <v>You should [self-isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) from others in your household who have not tested positive. Sleep and stay in a separate room from them, and use a separate bathroom, if possible. Multiple infected people in the same household can use the same room for isolation.\n\nMembers of your household should get tested right away. They should [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) for at least 14 days. Symptoms can develop even after testing negative within 14 days after exposure. Multiple people in the same household should not quarantine in the same room, since some may be infected.\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C162" t="str">
         <v>https://covid19.ca.gov/testing-and-treatment/</v>
@@ -4594,13 +4594,13 @@
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>What are the pay and benefits for California Health Corps professionals?</v>
+        <v>How can I find a coronavirus testing location near me?</v>
       </c>
       <c r="B163" t="str">
-        <v>Salary rates for most of the health care professionals being hired for this emergency are listed in the [CalHR Pay Scales](https://www.calhr.ca.gov/Pay%20Scales%20Library/PS_Sec_05.pdf) (pages 5.12 and 5.13). In addition, CalHR has established pay rates for medical roles that don’t have a corresponding regular classification and pay schedule, such as paramedics and EMTs. CalHR will determine specific salary and benefits after conducting a review of each application.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>&gt; [Find a testing location](https://arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401)\n&gt; -----------------------------------------------------------------------------------------------------------\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C163" t="str">
-        <v>https://covid19.ca.gov/healthcorps/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D163" t="str">
         <v xml:space="preserve"> </v>
@@ -4620,13 +4620,13 @@
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>Some healthcare professions are not listed. Are health professionals who are not listed (e.g., Medical Technicians, Lab Technicians, etc.) eligible for the California Health Corps?</v>
+        <v>What is an antibody test? Where can I get an antibody test?</v>
       </c>
       <c r="B164" t="str">
-        <v>California Health Corps are currently only accepting applications for the healthcare professions listed on the website. However, we are constantly re-evaluating our needs during this fluid situation and will open the registration for other professionals, if the need arises.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>[**Antibody tests**](https://www.cdc.gov/coronavirus/2019-ncov/testing/serology-overview.html) detect past infections. They can determine if you are a good candidate to [donate blood plasma](https://covid19.ca.gov/plasma/). It can take 1-3 weeks after infection for your body to make antibodies.\n\nYou can find locations for both viral and antibody tests on [California’s testing map](https://www.arcgis.com/apps/Nearby/index.html?appid=43118dc0d5d348d8ab20a81967a15401).\n\nMore info: [Testing and treatment](https://covid19.ca.gov/testing-and-treatment/)</v>
       </c>
       <c r="C164" t="str">
-        <v>https://covid19.ca.gov/healthcorps/</v>
+        <v>https://covid19.ca.gov/testing-and-treatment/</v>
       </c>
       <c r="D164" t="str">
         <v xml:space="preserve"> </v>
@@ -4646,10 +4646,10 @@
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>When can I expect to hear a response after completing my California Health Corps registration?</v>
+        <v>What are the pay and benefits for California Health Corps professionals?</v>
       </c>
       <c r="B165" t="str">
-        <v>Currently we anticipate the process may take up to two weeks, since an incredible number of responses are received and need to prioritize certain parts of the state, where the needs are the greatest. We will begin to contact the volunteers after verification of credentials, and based on current and anticipated needs.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>Salary rates for most of the health care professionals being hired for this emergency are listed in the [CalHR Pay Scales](https://www.calhr.ca.gov/Pay%20Scales%20Library/PS_Sec_05.pdf) (pages 5.12 and 5.13). In addition, CalHR has established pay rates for medical roles that don’t have a corresponding regular classification and pay schedule, such as paramedics and EMTs. CalHR will determine specific salary and benefits after conducting a review of each application.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C165" t="str">
         <v>https://covid19.ca.gov/healthcorps/</v>
@@ -4672,10 +4672,10 @@
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>How do I return to the California Health Corps application after logging out?</v>
+        <v>Some healthcare professions are not listed. Are health professionals who are not listed (e.g., Medical Technicians, Lab Technicians, etc.) eligible for the California Health Corps?</v>
       </c>
       <c r="B166" t="str">
-        <v>Visit [https://healthcarevolunteers.ca.gov/](https://healthcarevolunteers.ca.gov/) and use the account you created while applying to correct or update any information you want.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>California Health Corps are currently only accepting applications for the healthcare professions listed on the website. However, we are constantly re-evaluating our needs during this fluid situation and will open the registration for other professionals, if the need arises.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C166" t="str">
         <v>https://covid19.ca.gov/healthcorps/</v>
@@ -4698,10 +4698,10 @@
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>Resources for the California Health Corps participants</v>
+        <v>When can I expect to hear a response after completing my California Health Corps registration?</v>
       </c>
       <c r="B167" t="str">
-        <v>*   Health Corps FAQ: [FAQ-Health-Corps (PDF)](https://files.covid19.ca.gov/pdf/FAQ-Health-Corps.pdf)\n*   Travel Reimbursement FAQ: [FAQ-Travel-Reimbursement (PDF)](https://files.covid19.ca.gov/pdf/FAQ-Travel-Reimbursement.pdf)\n*   SNF Orientation: [SNF-Nursing-Staff-Orientation (PDF)](https://files.covid19.ca.gov/pdf/SNF-Nursing-Staff-Orientation.pdf)\n*   How to file a complaint: [How-to-file-a-complaint (PDF)](https://files.covid19.ca.gov/pdf/How-to-file-a-complaint.pdf)\n*   Direct deposit: [std699-Direct-Deposit (PDF)](https://files.covid19.ca.gov/pdf/std699-Direct-Deposit.pdf)\n*   Travel expense claim: [Std262-Travel-Expense-Claim (PDF)](https://files.covid19.ca.gov/pdf/Std262-Travel-Expense-Claim.pdf)\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>Currently we anticipate the process may take up to two weeks, since an incredible number of responses are received and need to prioritize certain parts of the state, where the needs are the greatest. We will begin to contact the volunteers after verification of credentials, and based on current and anticipated needs.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C167" t="str">
         <v>https://covid19.ca.gov/healthcorps/</v>
@@ -4724,10 +4724,10 @@
     </row>
     <row r="168">
       <c r="A168" t="str">
-        <v>Can a doctor with out of state license or foreign medical graduate without California license work for the California Health Corps?</v>
+        <v>How do I return to the California Health Corps application after logging out?</v>
       </c>
       <c r="B168" t="str">
-        <v>To be eligible for COVID-19 emergency medical staffing roles, you must:\n\n*   Have a valid California License for clinical practice (if you are a MD, DO, etc.) \n*   **OR** are a medical resident or nursing student \n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
+        <v>Visit [https://healthcarevolunteers.ca.gov/](https://healthcarevolunteers.ca.gov/) and use the account you created while applying to correct or update any information you want.\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C168" t="str">
         <v>https://covid19.ca.gov/healthcorps/</v>
@@ -4750,13 +4750,13 @@
     </row>
     <row r="169">
       <c r="A169" t="str">
-        <v>Agriculture and livestock</v>
+        <v>Resources for the California Health Corps participants</v>
       </c>
       <c r="B169" t="str">
-        <v>Follow this [guidance for the agriculture and livestock industry](https://files.covid19.ca.gov/pdf/guidance-agriculture--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the agriculture and livestock industry](https://files.covid19.ca.gov/pdf/checklist-agriculture.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>*   Health Corps FAQ: [FAQ-Health-Corps (PDF)](https://files.covid19.ca.gov/pdf/FAQ-Health-Corps.pdf)\n*   Travel Reimbursement FAQ: [FAQ-Travel-Reimbursement (PDF)](https://files.covid19.ca.gov/pdf/FAQ-Travel-Reimbursement.pdf)\n*   SNF Orientation: [SNF-Nursing-Staff-Orientation (PDF)](https://files.covid19.ca.gov/pdf/SNF-Nursing-Staff-Orientation.pdf)\n*   How to file a complaint: [How-to-file-a-complaint (PDF)](https://files.covid19.ca.gov/pdf/How-to-file-a-complaint.pdf)\n*   Direct deposit: [std699-Direct-Deposit (PDF)](https://files.covid19.ca.gov/pdf/std699-Direct-Deposit.pdf)\n*   Travel expense claim: [Std262-Travel-Expense-Claim (PDF)](https://files.covid19.ca.gov/pdf/Std262-Travel-Expense-Claim.pdf)\n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C169" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/healthcorps/</v>
       </c>
       <c r="D169" t="str">
         <v xml:space="preserve"> </v>
@@ -4776,13 +4776,13 @@
     </row>
     <row r="170">
       <c r="A170" t="str">
-        <v>Auto dealerships</v>
+        <v>Can a doctor with out of state license or foreign medical graduate without California license work for the California Health Corps?</v>
       </c>
       <c r="B170" t="str">
-        <v>Follow this [guidance for the automobile dealerships and rental operators industry](https://files.covid19.ca.gov/pdf/guidance-auto-dealerships--en.pdf) to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for the automobile dealerships and rental operators](https://files.covid19.ca.gov/pdf/checklist-auto-dealerships.pdf) industry in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>To be eligible for COVID-19 emergency medical staffing roles, you must:\n\n*   Have a valid California License for clinical practice (if you are a MD, DO, etc.) \n*   **OR** are a medical resident or nursing student \n\nMore info: [California Health Corps](https://covid19.ca.gov/healthcorps/)</v>
       </c>
       <c r="C170" t="str">
-        <v>https://covid19.ca.gov/industry-guidance/</v>
+        <v>https://covid19.ca.gov/healthcorps/</v>
       </c>
       <c r="D170" t="str">
         <v xml:space="preserve"> </v>
@@ -4802,10 +4802,10 @@
     </row>
     <row r="171">
       <c r="A171" t="str">
-        <v>Campgrounds and outdoor recreation</v>
+        <v>Agriculture and livestock</v>
       </c>
       <c r="B171" t="str">
-        <v>Follow this [guidance for campgrounds](https://files.covid19.ca.gov/pdf/guidance-campgrounds-outdoor-recreation--en.pdf), RV parks, and outdoor recreation to create a safer environment for workers and patrons.\n\nReview the guidance and prepare a plan for your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for the agriculture and livestock industry](https://files.covid19.ca.gov/pdf/guidance-agriculture--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the agriculture and livestock industry](https://files.covid19.ca.gov/pdf/checklist-agriculture.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C171" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4828,10 +4828,10 @@
     </row>
     <row r="172">
       <c r="A172" t="str">
-        <v>Cardrooms and racetracks</v>
+        <v>Auto dealerships</v>
       </c>
       <c r="B172" t="str">
-        <v>**Tier status:**\n\nWidespread (purple): Outdoor only with modifications\n\nSubstantial (red): Outdoor only with modifications\n\nModerate (orange)\n\n*   Indoor with modifications\n*   Capacity must be limited to 25%\n\nMinimal (yellow)\n\n*   Indoor with modifications\n*   Capacity must be limited to 50%\n\nFollow this [guidance for cardrooms](https://files.covid19.ca.gov/pdf/guidance-cardrooms-racetracks--en.pdf), racetracks, and satellite wagering to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for cardrooms](https://files.covid19.ca.gov/pdf/checklist-cardrooms-racetracks.pdf), racetracks, and satellite wagering in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for the automobile dealerships and rental operators industry](https://files.covid19.ca.gov/pdf/guidance-auto-dealerships--en.pdf) to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for the automobile dealerships and rental operators](https://files.covid19.ca.gov/pdf/checklist-auto-dealerships.pdf) industry in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C172" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4854,10 +4854,10 @@
     </row>
     <row r="173">
       <c r="A173" t="str">
-        <v>Childcare</v>
+        <v>Campgrounds and outdoor recreation</v>
       </c>
       <c r="B173" t="str">
-        <v>Childcare facilities\n\n*   Follow the [guidance for the childcare industry](https://files.covid19.ca.gov/pdf/guidance-childcare--en.pdf) to minimize the spread of COVID-19. \n*   Follow the [case and contact management guidance](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/contact-management-childcare-facilities.aspx), which includes:\n    *   What to do when kids or staff develop symptoms while in the facility.\n    *   What to do for kids and adults who may have been exposed to someone with COVID-19.\n    *   When closure of a facility should be considered, and when it can reopen.\n*   See the answers to [frequently asked questions about waivers](https://www.cdss.ca.gov/Portals/9/CCLD/PINs/2020/CCP/PIN-20-22-CCP.pdf) that are available to providers.\n*   Review the guidance, prepare a plan, and post the [checklist for childcare](https://files.covid19.ca.gov/pdf/checklist-childcare--en.pdf) in your facility to show employees and families that you’ve reduced the risk and are open for operation.\n\nCohorts of kids and adults in controlled, supervised settings\n\nA **cohort** is a stable group of no more than 14 children or youth and no more than two supervising adults in a supervised environment. The group stays together for all activities, including meals and recreation. And this group avoids contact with anyone not in their group.\n\nFollow the [guidance for cohorts of children](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/small-groups-child-youth.aspx) and youth in controlled, supervised and indoor environments. See the answers to [frequently asked questions](https://files.covid19.ca.gov/pdf/guidance-schools-cohort-FAQ.pdf) about cohort guidance.\n\nKids and adults in supervised care environments must be in groups as small as possible. Kids and supervising adults in one group must not physically interact with:\n\n*   kids and supervising adults in other groups\n*   other facility staff\n*   parents of kids in other groups\n\nPracticing a cohort structure\n\n*   decreases opportunities for exposure to or transmission of the virus\n*   facilitates more efficient contact tracing in the event of a positive case\n*   allows for targeted testing, quarantine, and isolation of a single group instead of an entire population of kids and supervising adults\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for campgrounds](https://files.covid19.ca.gov/pdf/guidance-campgrounds-outdoor-recreation--en.pdf), RV parks, and outdoor recreation to create a safer environment for workers and patrons.\n\nReview the guidance and prepare a plan for your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C173" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4880,10 +4880,10 @@
     </row>
     <row r="174">
       <c r="A174" t="str">
-        <v>Cohorts for children and youth in supervised settings</v>
+        <v>Cardrooms and racetracks</v>
       </c>
       <c r="B174" t="str">
-        <v>A **cohort** is a stable group of no more than 14 children or youth and no more than two supervising adults in a supervised environment. The group stays together for all activities, including meals and recreation. And this group avoids contact with anyone not in their group.\n\nThe [guidance related to cohorts](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/small-groups-child-youth.aspx) sets minimum guidelines for providing specialized, targeted support services, necessary in-person child supervision and limited instruction, and facilitation of distance learning in small group environments in ways that maintain the focus on health and safety to minimize transmission. This guidance enables schools to provide specialized services for students with disabilities and English learners, and in-person support for at-risk and high-need students. \n\nSee the answers to [frequently asked questions](https://files.covid19.ca.gov/pdf/guidance-schools-cohort-FAQ.pdf) about cohort guidance. \n\nLocal educational agencies, nonprofits, or other authorized providers must follow the guidance for cohorts of children and youth in controlled, supervised and indoor environments. These environments include, but are not limited to, the following:\n\n*   public and private schools\n*   licensed and license-exempt child care settings \n*   organized and supervised care environments, like “distance learning hubs”\n*   recreation programs\n*   before and after school programs\n*   youth groups\n*   day camps\n\nKids and adults in supervised care environments must be in groups as small as possible. Kids and supervising adults in one group must not physically interact with:\n\n*   kids and supervising adults in other groups\n*   other facility staff\n*   parents of kids in other groups\n\nPracticing a cohort structure:\n\n*   decreases opportunities for exposure to or transmission of the virus\n*   facilitates more efficient contact tracing in the event of a positive case\n*   allows for targeted testing, quarantine, and isolation of a single group instead of an entire population of kids and supervising adults\n\nChildcare facilities\n\n*   Follow the [case and contact management guidance](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/contact-management-childcare-facilities.aspx), which includes:\n    *   What to do when kids or staff develop symptoms while in the facility.\n    *   What to do for kids and adults who may have been exposed to someone with COVID-19.\n    *   When closure of a facility should be considered, and when it can reopen.\n*   See the answers to [frequently asked questions about waivers](https://www.cdss.ca.gov/Portals/9/CCLD/PINs/2020/CCP/PIN-20-22-CCP.pdf) that are available to providers. \n\nGuidance and directives related to [schools](https://covid19.ca.gov/industry-guidance/#schools-guidance), [childcare](https://covid19.ca.gov/industry-guidance/#childcare-guidance), [day camps](https://covid19.ca.gov/industry-guidance/#daycamps-guidance), [youth sports](https://covid19.ca.gov/industry-guidance/#youthsports-guidance), and [institutions of higher education](https://covid19.ca.gov/industry-guidance/#higher-education) are not superseded by this guidance for cohorts of children and youth and still apply to those specified settings.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple): \n\n*   Outdoor only with modifications\n*   Racetracks may resume training and competition without live audiences, subject to approval by county public health officers\n\nSubstantial (red): \n\n*   Outdoor only with modifications\n*   Racetracks may resume training and competition without live audiences, subject to approval by county public health officers\n\nModerate (orange)\n\n*   Indoor with modifications\n*   Capacity must be limited to 25%\n*   Racetracks may resume training and competition without live audiences, subject to approval by county public health officers\n\nMinimal (yellow)\n\n*   Indoor with modifications\n*   Capacity must be limited to 50%\n*   Racetracks may resume training and competition without live audiences, subject to approval by county public health officers\n\nFollow this [guidance for cardrooms](https://files.covid19.ca.gov/pdf/guidance-cardrooms-racetracks--en.pdf), racetracks, and satellite wagering to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for cardrooms](https://files.covid19.ca.gov/pdf/checklist-cardrooms-racetracks.pdf), racetracks, and satellite wagering in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C174" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4906,10 +4906,10 @@
     </row>
     <row r="175">
       <c r="A175" t="str">
-        <v>Communications infrastructure</v>
+        <v>Childcare</v>
       </c>
       <c r="B175" t="str">
-        <v>Follow this [guidance for the communications infrastructure industry](https://files.covid19.ca.gov/pdf/guidance-communications--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the communications infrastructure industry](https://files.covid19.ca.gov/pdf/checklist-communications.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow the [guidance for the childcare industry](https://files.covid19.ca.gov/pdf/guidance-childcare--en.pdf) to minimize the spread of COVID-19. Review the guidance, prepare a plan, and post the [checklist for childcare](https://files.covid19.ca.gov/pdf/checklist-childcare--en.pdf) in your facility to show employees and families that you’ve reduced the risk and are open for operation.\n\n*   Follow the [guidance related to cohorts](https://covid19.ca.gov/industry-guidance/#cohort-guidance) of children and youth.\n*   See the answers to [frequently asked questions about cohorts and waivers](https://www.cdss.ca.gov/Portals/9/CCLD/PINs/2020/CCP/PIN-20-22-CCP.pdf) for childcare providers.\n*   Follow the [case and contact management guidance](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/contact-management-childcare-facilities.aspx) related to cohorts for childcare facilities.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C175" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4932,10 +4932,10 @@
     </row>
     <row r="176">
       <c r="A176" t="str">
-        <v>Construction</v>
+        <v>Cohorts for children and youth in supervised settings – updated September 4</v>
       </c>
       <c r="B176" t="str">
-        <v>Follow this [guidance for the construction industry](https://files.covid19.ca.gov/pdf/guidance-construction--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the construction industry](https://files.covid19.ca.gov/pdf/checklist-construction.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>A **cohort** is a stable group of no more than 14 children or youth and no more than two supervising adults in a supervised environment. The group stays together for all activities, including meals and recreation. And this group avoids contact with anyone not in their group.\n\nKids and adults in supervised care environments must be in groups as small as possible. Kids and supervising adults in one group must not physically interact with:\n\n*   kids and supervising adults in other groups\n*   other facility staff\n*   parents of kids in other groups\n\nPracticing a cohort structure:\n\n*   decreases opportunities for exposure to or transmission of the virus\n*   facilitates more efficient contact tracing in the event of a positive case\n*   allows for targeted testing, quarantine, and isolation of a single group instead of an entire population of kids and supervising adults\n\nThe [guidance related to cohorts](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/small-groups-child-youth.aspx) of children and youth sets minimum guidelines for providing specialized, targeted support services, necessary in-person child supervision and limited instruction, and facilitation of distance learning in small group environments in ways that maintain the focus on health and safety to minimize transmission. This guidance enables schools to provide specialized services for students with disabilities and English learners, and in-person support for at-risk and high-need students. \n\n*   See the answers to [frequently asked questions](https://files.covid19.ca.gov/pdf/guidance-schools-cohort-FAQ.pdf) about cohort guidance in K-12 school settings.\n*   See the answers to [frequently asked questions about cohorts and waivers](https://www.cdss.ca.gov/Portals/9/CCLD/PINs/2020/CCP/PIN-20-22-CCP.pdf) for childcare providers.\n*   Follow the [case and contact management guidance](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/contact-management-childcare-facilities.aspx) related to cohorts for childcare facilities. \n\nLocal educational agencies, nonprofits, or other authorized providers must follow the guidance for cohorts of children and youth in controlled, supervised and indoor environments. These environments include, but are not limited to, the following:\n\n*   public and private schools\n*   licensed and license-exempt childcare settings \n*   organized and supervised care environments, like “distance learning hubs”\n*   recreation programs\n*   before and after school programs\n*   youth groups\n*   day camps\n\nGuidance and directives related to [schools](https://covid19.ca.gov/industry-guidance/#schools-guidance), [childcare](https://covid19.ca.gov/industry-guidance/#childcare-guidance), [day camps](https://covid19.ca.gov/industry-guidance/#daycamps-guidance), and [youth sports](https://covid19.ca.gov/industry-guidance/#youthsports-guidance) are not superseded by this guidance for cohorts of children and youth and still apply to those specified settings.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C176" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4958,10 +4958,10 @@
     </row>
     <row r="177">
       <c r="A177" t="str">
-        <v>Day camps</v>
+        <v>Communications infrastructure</v>
       </c>
       <c r="B177" t="str">
-        <v>Follow this [guidance for day camps](https://files.covid19.ca.gov/pdf/guidance-day-camps--en.pdf) to create a plan for safe re-opening. Implementation of these guidelines should be tailored for each setting. Implementation requires training and support for staff and adequate consideration of camper and family needs. All decisions about following these recommendations should be made in collaboration with local health officials and other authorities, and should depend on the levels of COVID-19 community transmission and the capacities of the local public health and healthcare systems, among other relevant factors. \n\nReview the guidance, prepare a plan, and post the [checklist for day camps](https://files.covid19.ca.gov/pdf/checklist-daycamps--en.pdf) in your facility to show employees, campers, and families that you’ve reduced the risk and are open for operation.\n\nCohorts of kids and adults in controlled, supervised settings\n\nA **cohort** is a stable group of no more than 14 children or youth and no more than two supervising adults in a supervised environment. The group stays together for all activities, including meals and recreation. And this group avoids contact with anyone not in their group.\n\nDay camp operators must follow the [guidance for cohorts of children](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/small-groups-child-youth.aspx) and youth in controlled, supervised and indoor environments. See the answers to [frequently asked questions](https://files.covid19.ca.gov/pdf/guidance-schools-cohort-FAQ.pdf) about cohort guidance.\n\nKids and adults in supervised care environments must be in groups as small as possible. Kids and supervising adults in one group must not physically interact with:\n\n*   kids and supervising adults in other groups\n*   other facility staff\n*   parents of kids in other groups\n\nPracticing a cohort structure\n\n*   decreases opportunities for exposure to or transmission of the virus\n*   facilitates more efficient contact tracing in the event of a positive case\n*   allows for targeted testing, quarantine, and isolation of a single group instead of an entire population of kids and supervising adults\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for the communications infrastructure industry](https://files.covid19.ca.gov/pdf/guidance-communications--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the communications infrastructure industry](https://files.covid19.ca.gov/pdf/checklist-communications.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C177" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -4984,10 +4984,10 @@
     </row>
     <row r="178">
       <c r="A178" t="str">
-        <v>Delivery services</v>
+        <v>Construction</v>
       </c>
       <c r="B178" t="str">
-        <v>Follow this [guidance for the delivery services industry](https://files.covid19.ca.gov/pdf/guidance-delivery-services--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the delivery services industry](https://files.covid19.ca.gov/pdf/checklist-delivery-services.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for the construction industry](https://files.covid19.ca.gov/pdf/guidance-construction--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the construction industry](https://files.covid19.ca.gov/pdf/checklist-construction.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C178" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5010,10 +5010,10 @@
     </row>
     <row r="179">
       <c r="A179" t="str">
-        <v>Energy and utilities</v>
+        <v>Day camps</v>
       </c>
       <c r="B179" t="str">
-        <v>Follow this [guidance for the energy and utilities industry](https://files.covid19.ca.gov/pdf/guidance-energy--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the energy and utilities industry](https://files.covid19.ca.gov/pdf/checklist-energy.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for day camps](https://files.covid19.ca.gov/pdf/guidance-day-camps--en.pdf) to minimize the spread of COVID-19. Review the guidance, prepare a plan, and post the [checklist for day camps](https://files.covid19.ca.gov/pdf/checklist-daycamps--en.pdf) in your facility to show employees, campers, and families that you’ve reduced the risk and are open for operation. Follow the [guidance related to cohorts](https://covid19.ca.gov/industry-guidance/#cohort-guidance) of children and youth.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C179" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5036,10 +5036,10 @@
     </row>
     <row r="180">
       <c r="A180" t="str">
-        <v>Family friendly practices for employers</v>
+        <v>Delivery services</v>
       </c>
       <c r="B180" t="str">
-        <v>Follow this [guidance for family friendly practices for employers](https://files.covid19.ca.gov/pdf/guidance-family-friendly-practices-employers--en.pdf) to keep employees safe and be responsive to their needs in order to ensure continued productivity. As workplaces reopen, employees will require both child care supports and workplace flexibility. Work-life balance policies will become even more important and continued investment in family-friendly workplace policies by employers is critical.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for the delivery services industry](https://files.covid19.ca.gov/pdf/guidance-delivery-services--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the delivery services industry](https://files.covid19.ca.gov/pdf/checklist-delivery-services.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C180" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5062,10 +5062,10 @@
     </row>
     <row r="181">
       <c r="A181" t="str">
-        <v>Food packing</v>
+        <v>Energy and utilities</v>
       </c>
       <c r="B181" t="str">
-        <v>Follow this [guidance for facilities that process or pack meat, dairy, or produce](https://files.covid19.ca.gov/pdf/guidance-food-packing--en.pdf) to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for facilities that process or pack meat, dairy or produce](https://files.covid19.ca.gov/pdf/checklist-food-packing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for the energy and utilities industry](https://files.covid19.ca.gov/pdf/guidance-energy--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the energy and utilities industry](https://files.covid19.ca.gov/pdf/checklist-energy--en.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C181" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5088,10 +5088,10 @@
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>Gyms and fitness centers</v>
+        <v>Family friendly practices for employers</v>
       </c>
       <c r="B182" t="str">
-        <v>**Tier status:**\n\nWidespread (purple):\n\n*   Outdoor only with modifications\n*   Saunas and steam rooms must close\n\nSubstantial (red): \n\n*   Indoor with modifications\n*   Capacity must be limited to 10%\n\nModerate (orange)\n\n*   Indoor with modifications\n*   Capacity must be limited to 25%\n*   Indoor pools can open\n\nMinimal (yellow)\n\n*   Indoor with modifications\n*   Capacity must be limited to 50%\n*   Indoor pools can open\n*   Saunas, spas, and steam rooms can open\n\nFollow this [guidance for gyms and fitness centers](https://files.covid19.ca.gov/pdf/guidance-fitness--en.pdf), including yoga and dance studios, to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for gyms and fitness centers](https://files.covid19.ca.gov/pdf/checklist-fitness.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for family friendly practices for employers](https://files.covid19.ca.gov/pdf/guidance-family-friendly-practices-employers--en.pdf) to keep employees safe and be responsive to their needs in order to ensure continued productivity. As workplaces reopen, employees will require both child care supports and workplace flexibility. Work-life balance policies will become even more important and continued investment in family-friendly workplace policies by employers is critical.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C182" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5114,10 +5114,10 @@
     </row>
     <row r="183">
       <c r="A183" t="str">
-        <v>Hair salons and barbershops</v>
+        <v>Food packing</v>
       </c>
       <c r="B183" t="str">
-        <v>Follow this [guidance for hair salons and barbershops](https://files.covid19.ca.gov/pdf/guidance-hair-salons--en.pdf) to create a safer environment for workers and customers. Review the guidance, prepare a plan, and post the [checklist for hair salons](https://files.covid19.ca.gov/pdf/checklist-hair-salons.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for facilities that process or pack meat, dairy, or produce](https://files.covid19.ca.gov/pdf/guidance-food-packing--en.pdf) to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for facilities that process or pack meat, dairy or produce](https://files.covid19.ca.gov/pdf/checklist-food-packing--en.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C183" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5140,10 +5140,10 @@
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>Higher education</v>
+        <v>Gyms and fitness centers</v>
       </c>
       <c r="B184" t="str">
-        <v>**Tier status:**\n\nWidespread (purple):\n\n*   Closed for in-person instruction\n\nSubstantial (red):\n\n*   Open for in-person instruction once the county has been this tier for at least two weeks\n\nModerate (orange): Open with modifications\n\nMinimal (yellow): Open with modifications\n\nThis interim [guidance for institutions of higher education](https://files.covid19.ca.gov/pdf/guidance-higher-education--en.pdf) provides guidelines to help institutions and their communities plan and prepare to resume in-person instruction. Review the guidance and prepare a plan to reduce the risk and support a safer environment for students, faculty, workers, and families.\n\nCohorts of youth and adults in controlled, supervised settings\n\nA **cohort** is a stable group of no more than 14 youth and no more than two supervising adults in a supervised environment. The group stays together for all activities, including meals and recreation. And this group avoids contact with anyone not in their group.\n\nFollow the [guidance for cohorts of children](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/small-groups-child-youth.aspx) and youth in controlled, supervised and indoor environments operated by local educational agencies, nonprofits, or other authorized providers. These environments include, but are not limited to, the following:\n\n*   public and private schools\n*   organized and supervised environments, like “distance learning hubs”\n*   recreation programs\n*   before and after school programs\n*   youth groups\n\nSee the answers to [frequently asked questions](https://files.covid19.ca.gov/pdf/guidance-schools-cohort-FAQ.pdf) about cohort guidance.\n\nYouth and adults in supervised environments must be in groups as small as possible. Youth and supervising adults in one group must not physically interact with:\n\n*   youth and supervising adults in other groups\n*   other facility staff\n*   parents of youth in other groups\n\nPracticing a cohort structure:\n\n*   decreases opportunities for exposure to or transmission of the virus\n*   facilitates more efficient contact tracing in the event of a positive case\n*   allows for targeted testing, quarantine, and isolation of a single group instead of an entire population of youth and supervising adults\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple):\n\n*   Outdoor only with modifications\n*   Saunas and steam rooms must close\n\nSubstantial (red): \n\n*   Indoor with modifications\n*   Capacity must be limited to 10%\n\nModerate (orange)\n\n*   Indoor with modifications\n*   Capacity must be limited to 25%\n*   Indoor pools can open\n\nMinimal (yellow)\n\n*   Indoor with modifications\n*   Capacity must be limited to 50%\n*   Indoor pools can open\n*   Saunas, spas, and steam rooms can open\n\nFollow this [guidance for gyms and fitness centers](https://files.covid19.ca.gov/pdf/guidance-fitness--en.pdf), including yoga and dance studios, to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for gyms and fitness centers](https://files.covid19.ca.gov/pdf/checklist-fitness--en.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C184" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5166,10 +5166,10 @@
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>Hotels, lodging, and short term rentals</v>
+        <v>Hair salons and barbershops</v>
       </c>
       <c r="B185" t="str">
-        <v>**Tier status:**\n\nWidespread (purple): \n\n*   Open with modifications\n*   Fitness centers can be open outdoors only with modifications\n*   Saunas and steam rooms must close\n\nSubstantial (red): \n\n*   Open with modifications\n*   Fitness centers can open to 10% capacity\n\nModerate (orange)\n\n*   Open with modifications\n*   Fitness centers can open to 25% capacity\n*   Indoor pools can open\n\nMinimal (yellow)\n\n*   Open with modifications\n*   Fitness centers can open to 50% capacity\n*   Indoor pools can open\n*   Spa facilities can open\n\nHotels and lodging\n\n*   Follow this [guidance for hotels and lodging](https://files.covid19.ca.gov/pdf/guidance-hotels--en.pdf) to create a safer environment for workers and customers.\n\nHotels, lodging, and short term rentals\n\n*   Follow this [guidance for hotels and short term rentals](https://files.covid19.ca.gov/pdf/guidance-hotels-lodging-rentals--en.pdf) for tourism and individual travel to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for hotels, lodging, and short-term rentals](https://files.covid19.ca.gov/pdf/checklist-hotels.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for hair salons and barbershops](https://files.covid19.ca.gov/pdf/guidance-hair-salons--en.pdf) to create a safer environment for workers and customers. Review the guidance, prepare a plan, and post the [checklist for hair salons](https://files.covid19.ca.gov/pdf/checklist-hair-salons--en.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C185" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5192,10 +5192,10 @@
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>Life sciences</v>
+        <v>Higher education</v>
       </c>
       <c r="B186" t="str">
-        <v>Follow this [guidance for the life sciences industry](https://files.covid19.ca.gov/pdf/guidance-life-sciences--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the life sciences industry](https://files.covid19.ca.gov/pdf/checklist-life-sciences.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple):\n\n*   Closed for indoor lectures and student gatherings\n*   Some courses conducted in certain indoor settings, like labs and studio arts, may be open\n\nSubstantial (red):\n\n*   Capacity for indoor lectures and student gatherings must be limited to 25% or 100 people, whichever is less\n*   Some courses conducted in certain indoor settings, like labs and studio arts, may be open at regular capacity\n*   Conduct student activities virtually when possible\n\nModerate (orange):\n\n*   Capacity for indoor lectures and student gatherings must be limited to 50% or 200 people, whichever is less\n*   Some courses conducted in certain indoor settings, like labs and studio arts, may be open at regular capacity\n*   Conduct student activities virtually when possible\n\nMinimal (yellow):\n\n*   Capacity for indoor lectures and student gatherings must be limited to 50%\n*   Some courses conducted in certain indoor settings, like labs and studio arts, may be open at regular capacity\n*   Conduct student activities virtually when possible\n\nThis interim [guidance for institutions of higher education](https://files.covid19.ca.gov/pdf/guidance-higher-education--en.pdf) provides guidelines to help institutions and their communities plan and prepare to resume in-person instruction. Review the guidance and prepare a plan to reduce the risk and support a safer environment for students, faculty, workers, and families.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C186" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5218,10 +5218,10 @@
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>Limited services</v>
+        <v>Hotels, lodging, and short-term lodging rentals</v>
       </c>
       <c r="B187" t="str">
-        <v>Limited Services are defined as those which do not generally require close contact. Follow this [guidance for Limited Services](https://files.covid19.ca.gov/pdf/guidance-limited-services--en.pdf) to create a safer environment for workers and patrons.\n\nFaith-based counseling can reopen within the following parameters:\n\n1.  Counseling services are permissible in-person where the service cannot reasonably be practiced remotely;\n2.  Counseling services should adopt state guidance on Limited Services, where applicable;\n3.  This designation does not permit gatherings beyond counseling to members of a single household.\n\nReview the guidance, prepare a plan, and post the [checklist for Limited Services](https://files.covid19.ca.gov/pdf/checklist-limited-services.pdf) in your workplace to show clients and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)&lt;!-- laundromat, dry cleaner, laundry, auto repair, car wash, landscaper, door to door, sales, pet groom, dog walk, entry to private residences, community 2 facilities, residential, janitorial, cleaning services, house keep, house clean, HVAC, appliance repair, electrician, plumbers, mechanical trade, handyperson, handyman, general contractors, lessees, subcontractors --&gt;</v>
+        <v>**Tier status:**\n\nWidespread (purple): \n\n*   Open with modifications\n*   Fitness centers can be open outdoors only with modifications\n*   Saunas and steam rooms must close\n\nSubstantial (red): \n\n*   Open with modifications\n*   Fitness centers can open to 10% capacity\n\nModerate (orange)\n\n*   Open with modifications\n*   Fitness centers can open to 25% capacity\n*   Indoor pools can open\n\nMinimal (yellow)\n\n*   Open with modifications\n*   Fitness centers can open to 50% capacity\n*   Indoor pools can open\n*   Spa facilities can open\n\nHotels and lodging\n\n*   Follow this [guidance for hotels and lodging](https://files.covid19.ca.gov/pdf/guidance-hotels--en.pdf) to create a safer environment for workers and customers.\n\nHotels, lodging, and short term rentals\n\n*   Follow this [guidance for hotels and short term rentals](https://files.covid19.ca.gov/pdf/guidance-hotels-lodging-rentals--en.pdf) for tourism and individual travel to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for hotels, lodging, and short-term rentals](https://files.covid19.ca.gov/pdf/checklist-hotels.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C187" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5244,10 +5244,10 @@
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>Logistics and warehousing facilities</v>
+        <v>Life sciences</v>
       </c>
       <c r="B188" t="str">
-        <v>Follow this [guidance for businesses operating in the logistics/warehousing industry](https://files.covid19.ca.gov/pdf/guidance-logistics-warehousing--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post  the [checklist for the logistics/warehousing industry](https://files.covid19.ca.gov/pdf/checklist-logistics-warehousing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for the life sciences industry](https://files.covid19.ca.gov/pdf/guidance-life-sciences--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the life sciences industry](https://files.covid19.ca.gov/pdf/checklist-life-sciences--en.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C188" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5270,10 +5270,10 @@
     </row>
     <row r="189">
       <c r="A189" t="str">
-        <v>Manufacturing</v>
+        <v>Limited services</v>
       </c>
       <c r="B189" t="str">
-        <v>Follow this [guidance for the manufacturing industry](https://files.covid19.ca.gov/pdf/guidance-manufacturing--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the manufacturing industry](https://files.covid19.ca.gov/pdf/checklist-manufacturing.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Limited Services are defined as those which do not generally require close contact. Follow this [guidance for Limited Services](https://files.covid19.ca.gov/pdf/guidance-limited-services--en.pdf) to create a safer environment for workers and patrons.\n\nFaith-based counseling can reopen within the following parameters:\n\n1.  Counseling services are permissible in-person where the service cannot reasonably be practiced remotely;\n2.  Counseling services should adopt state guidance on Limited Services, where applicable;\n3.  This designation does not permit gatherings beyond counseling to members of a single household.\n\nReview the guidance, prepare a plan, and post the [checklist for Limited Services](https://files.covid19.ca.gov/pdf/checklist-limited-services--en.pdf) in your workplace to show clients and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)&lt;!-- laundromat, dry cleaner, laundry, auto repair, car wash, landscaper, door to door, sales, pet groom, dog walk, entry to private residences, community 2 facilities, residential, janitorial, cleaning services, house keep, house clean, HVAC, appliance repair, electrician, plumbers, mechanical trade, handyperson, handyman, general contractors, lessees, subcontractors --&gt;</v>
       </c>
       <c r="C189" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5296,10 +5296,10 @@
     </row>
     <row r="190">
       <c r="A190" t="str">
-        <v>Mining and logging</v>
+        <v>Logistics and warehousing facilities</v>
       </c>
       <c r="B190" t="str">
-        <v>Follow this [guidance for the mining and logging industries](https://files.covid19.ca.gov/pdf/guidance-mining-logging--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the mining and logging industries](https://files.covid19.ca.gov/pdf/checklist-mining-logging.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for businesses operating in the logistics/warehousing industry](https://files.covid19.ca.gov/pdf/guidance-logistics-warehousing--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post  the [checklist for the logistics/warehousing industry](https://files.covid19.ca.gov/pdf/checklist-logistics-warehousing--en.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C190" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5322,10 +5322,10 @@
     </row>
     <row r="191">
       <c r="A191" t="str">
-        <v>Movie theaters and family entertainment centers</v>
+        <v>Manufacturing</v>
       </c>
       <c r="B191" t="str">
-        <v>**Tier status:**\n\nWidespread (purple)\n\n*   Movie theaters: Outdoor only with modifications\n*   Family entertainment centers: Outdoor only with modifications for activities like kart racing, mini golf, batting cages\n\nSubstantial (red)\n\n*   Movie theaters: \n    *   Indoor with modifications\n    *   Capacity must be limited to 25% or 100 people, whichever is less\n*   Family entertainment centers: Outdoor only with modifications for activities like kart racing, mini golf, batting cages\n\nModerate (orange)\n\n*   Movie theaters: \n    *   Indoor with modifications\n    *   Capacity must be limited to 50% or 200 people, whichever is less\n*   Family entertainment centers: \n    *   Outdoor with modifications for activities like kart racing, mini golf, batting cages\n    *   Indoor with modifications for naturally distanced activities, like bowling alleys and climbing walls\n    *   Capacity must be limited to 25%\n\nMinimal (yellow)\n\n*   Movie theaters: \n    *   Indoor with modifications\n    *   Capacity must be limited to 50%\n*   Family entertainment centers: \n    *   Outdoor with modifications for activities like kart racing, mini golf, batting cages\n    *   Indoor with modifications for naturally distanced activities, like bowling alleys and climbing walls\n    *   Indoor with modifications for activities with increased risk of proximity and mixing, like arcade games, ice and roller skating, and indoor playgrounds\n    *   Capacity must be limited to 50%\n\nFollow this guidance for [movie theaters and family entertainment centers](https://files.covid19.ca.gov/pdf/guidance-family-entertainment--en.pdf), like bowling alleys, miniature golf, batting cages, and arcades, to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for movie theaters and family entertainment centers](https://files.covid19.ca.gov/pdf/checklist-family-entertainment.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for the manufacturing industry](https://files.covid19.ca.gov/pdf/guidance-manufacturing--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the manufacturing industry](https://files.covid19.ca.gov/pdf/checklist-manufacturing--en.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C191" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5348,10 +5348,10 @@
     </row>
     <row r="192">
       <c r="A192" t="str">
-        <v>Museums, zoos, and aquariums</v>
+        <v>Mining and logging</v>
       </c>
       <c r="B192" t="str">
-        <v>**Tier status:**\n\nWidespread (purple): Outdoor only with modifications\n\nSubstantial (red)\n\n*   Indoor with modifications\n*   Indoor activities must be limited to 25% of capacity\n\nModerate (orange)\n\n*   Indoor with modifications\n*   Indoor activities must be limited to 50% of capacity\n\nMinimal (yellow): Indoor with modifications\n\nOutdoor museums, open air galleries, botanical gardens, and other outdoor exhibition spaces\n\n*   Follow this [guidance for outdoor museums](https://files.covid19.ca.gov/pdf/guidance-outdoor-museums--en.pdf), open air galleries, botanical gardens, and other outdoor exhibition spaces to create a safer environment for workers and patrons. This guidance is not intended for zoos, amusement parks, or indoor gallery and museum spaces.\n*   Review the guidance, prepare a plan, and post the [checklist for outdoor museums](https://files.covid19.ca.gov/pdf/checklist-outdoor-museums.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMuseums, galleries, botanical gardens, zoos, aquariums, and other similar spaces\n\n*   Follow this [guidance for zoos, museums](https://files.covid19.ca.gov/pdf/guidance-zoos-museums--en.pdf), galleries, botanical gardens, and aquariums to create a safer environment for workers and patrons.\n*   Review the guidance, prepare a plan, and post the [checklist for zoos, museums](https://files.covid19.ca.gov/pdf/checklist-zoos-museums.pdf), galleries, and aquariums in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for the mining and logging industries](https://files.covid19.ca.gov/pdf/guidance-mining-logging--en.pdf) to create a safer environment for workers.  \n  \nReview the guidance, prepare a plan, and post the [checklist for the mining and logging industries](https://files.covid19.ca.gov/pdf/checklist-mining-logging--en.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C192" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5374,10 +5374,10 @@
     </row>
     <row r="193">
       <c r="A193" t="str">
-        <v>Music, film, and TV production</v>
+        <v>Movie theaters and family entertainment centers</v>
       </c>
       <c r="B193" t="str">
-        <v>Music, TV, and film production may resume, subject to approval by county public health officers.  \n  \nTo reduce the risk of COVID-19 transmission, productions, cast, crew and other industry workers should abide by safety protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should follow the [guidance for office workspaces](https://files.covid19.ca.gov/pdf/guidance-office-workspaces--en.pdf).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple)\n\n*   Movie theaters: Outdoor only with modifications\n*   Family entertainment centers: Outdoor only with modifications for activities like kart racing, mini golf, batting cages\n\nSubstantial (red)\n\n*   Movie theaters: \n    *   Indoor with modifications\n    *   Capacity must be limited to 25% or 100 people, whichever is less\n*   Family entertainment centers: Outdoor only with modifications for activities like kart racing, mini golf, batting cages\n\nModerate (orange)\n\n*   Movie theaters: \n    *   Indoor with modifications\n    *   Capacity must be limited to 50% or 200 people, whichever is less\n*   Family entertainment centers: \n    *   Outdoor with modifications for activities like kart racing, mini golf, batting cages\n    *   Indoor with modifications for naturally distanced activities, like bowling alleys and climbing walls\n    *   Capacity must be limited to 25%\n\nMinimal (yellow)\n\n*   Movie theaters: \n    *   Indoor with modifications\n    *   Capacity must be limited to 50%\n*   Family entertainment centers: \n    *   Outdoor with modifications for activities like kart racing, mini golf, batting cages\n    *   Indoor with modifications for naturally distanced activities, like bowling alleys and climbing walls\n    *   Indoor with modifications for activities with increased risk of proximity and mixing, like arcade games, ice and roller skating, and indoor playgrounds\n    *   Capacity must be limited to 50%\n\nFollow this guidance for [movie theaters and family entertainment centers](https://files.covid19.ca.gov/pdf/guidance-family-entertainment--en.pdf), like bowling alleys, miniature golf, batting cages, and arcades, to create a safer environment for workers and patrons.\n\nReview the guidance, prepare a plan, and post the [checklist for movie theaters and family entertainment centers](https://files.covid19.ca.gov/pdf/checklist-family-entertainment--en.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C193" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5400,10 +5400,10 @@
     </row>
     <row r="194">
       <c r="A194" t="str">
-        <v>Office workspaces</v>
+        <v>Museums, zoos, and aquariums</v>
       </c>
       <c r="B194" t="str">
-        <v>**Tier status:**\n\nWidespread (purple): Remote work\n\nSubstantial (red): Remote work\n\nModerate (orange): Indoor with modifications, encourage telework\n\nMinimal (yellow): Indoor with modifications, encourage telework\n\nFollow this [guidance for office workspaces](https://files.covid19.ca.gov/pdf/guidance-office-workspaces--en.pdf) to create a safer environment for workers.\n\nFaith-based office workspaces can reopen within the following parameters:\n\n1.  Faith-based facilities are considered “offices” only for those employed by the organization and where the facility is their regular place of work.\n2.  The employer should implement state guidance relating to offices before reopening the facility for employees.\n3.  This designation does not permit gatherings of non-employees, such as the organization’s congregation.\n\nReview the guidance, prepare a plan, and post the [checklist for office workspaces](https://files.covid19.ca.gov/pdf/checklist-office-workspaces.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple): Outdoor only with modifications\n\nSubstantial (red)\n\n*   Indoor with modifications\n*   Indoor activities must be limited to 25% of capacity\n\nModerate (orange)\n\n*   Indoor with modifications\n*   Indoor activities must be limited to 50% of capacity\n\nMinimal (yellow): Indoor with modifications\n\nOutdoor museums, open air galleries, botanical gardens, and other outdoor exhibition spaces\n\n*   Follow this [guidance for outdoor museums](https://files.covid19.ca.gov/pdf/guidance-outdoor-museums--en.pdf), open air galleries, botanical gardens, and other outdoor exhibition spaces to create a safer environment for workers and patrons. This guidance is not intended for zoos, amusement parks, or indoor gallery and museum spaces.\n*   Review the guidance, prepare a plan, and post the [checklist for outdoor museums](https://files.covid19.ca.gov/pdf/checklist-outdoor-museums--en.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMuseums, galleries, botanical gardens, zoos, aquariums, and other similar spaces\n\n*   Follow this [guidance for zoos, museums](https://files.covid19.ca.gov/pdf/guidance-zoos-museums--en.pdf), galleries, botanical gardens, and aquariums to create a safer environment for workers and patrons.\n*   Review the guidance, prepare a plan, and post the [checklist for zoos, museums](https://files.covid19.ca.gov/pdf/checklist-zoos-museums--en.pdf), galleries, and aquariums in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C194" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5426,10 +5426,10 @@
     </row>
     <row r="195">
       <c r="A195" t="str">
-        <v>Personal care services</v>
+        <v>Music, film, and TV production</v>
       </c>
       <c r="B195" t="str">
-        <v>**Tier status:**\n\nWidespread (purple): \n\n*   Outdoor only with modifications\n*   Tattooing, piercing, and electrolysis must close\n\nSubstantial (red): Indoor with modifications\n\nModerate (orange): Indoor with modifications\n\nMinimal (yellow): Indoor with modifications\n\nPersonal care services provided indoors\n\n*   Follow this [guidance for personal care services](https://files.covid19.ca.gov/pdf/guidance-expanded-personal-care-services--en.pdf) like nail salons, tattoo parlors, and body waxing to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for personal care services](https://files.covid19.ca.gov/pdf/checklist-expanded-personal-care-services.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nPersonal care services provided outdoors\n\n*   Follow this [guidance for personal care services provided outdoors](https://files.covid19.ca.gov/pdf/guidance-outdoor-personal-care--en.pdf) to support an outdoor safe, clean environment for workers and patrons. This guidance applies to services that require touching a client’s face, like facials and waxing. This guidance also applies to esthetic services, skin care, cosmetology, nail services, and massage therapy. Review the guidance, prepare a plan, and post the [checklist for personal care services provided outdoors](https://files.covid19.ca.gov/pdf/checklist-outdoor-personal-care--en.pdf) at your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Music, TV, and film production may resume, subject to approval by county public health officers.  \n  \nTo reduce the risk of COVID-19 transmission, productions, cast, crew and other industry workers should abide by safety protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should follow the [guidance for office workspaces](https://files.covid19.ca.gov/pdf/guidance-office-workspaces--en.pdf).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C195" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5452,10 +5452,10 @@
     </row>
     <row r="196">
       <c r="A196" t="str">
-        <v>Places of worship and cultural ceremonies</v>
+        <v>Office workspaces</v>
       </c>
       <c r="B196" t="str">
-        <v>**Tier status:**\n\nWidespread (purple): Outdoor only with modifications\n\nSubstantial (red)\n\n*   Indoor with modifications\n*   Indoor activities must be limited to 25% of capacity or 100 people, whichever is less\n\nModerate (orange)\n\n*   Indoor with modifications\n*   Indoor activities must be limited to 50% of capacity or 200 people, whichever is less\n\nMinimal (yellow)\n\n*   Indoor with modifications\n*   Indoor activities must be limited to 50% of capacity\n\nFollow this [guidance for places of worship](https://files.covid19.ca.gov/pdf/guidance-places-of-worship--en.pdf) and providers of religious services and cultural ceremonies, like weddings and funerals, to create a safer environment for workers and visitors.\n\nReview the guidance, prepare a plan, and post the [checklist for places of worship](https://files.covid19.ca.gov/pdf/checklist-places-of-worship.pdf) and cultural ceremonies in your workplace to show workers and visitors that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple): Remote work\n\nSubstantial (red): Remote work\n\nModerate (orange): Indoor with modifications, encourage telework\n\nMinimal (yellow): Indoor with modifications, encourage telework\n\nFollow this [guidance for office workspaces](https://files.covid19.ca.gov/pdf/guidance-office-workspaces--en.pdf) to create a safer environment for workers.\n\nFaith-based office workspaces can reopen within the following parameters:\n\n1.  Faith-based facilities are considered “offices” only for those employed by the organization and where the facility is their regular place of work.\n2.  The employer should implement state guidance relating to offices before reopening the facility for employees.\n3.  This designation does not permit gatherings of non-employees, such as the organization’s congregation.\n\nReview the guidance, prepare a plan, and post the [checklist for office workspaces](https://files.covid19.ca.gov/pdf/checklist-office-workspaces--en.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C196" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5478,10 +5478,10 @@
     </row>
     <row r="197">
       <c r="A197" t="str">
-        <v>Ports</v>
+        <v>Personal care services</v>
       </c>
       <c r="B197" t="str">
-        <v>Follow this [guidance for the port industry](https://files.covid19.ca.gov/pdf/guidance-ports--en.pdf) to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for the port industry](https://files.covid19.ca.gov/pdf/checklist-ports.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple): \n\n*   Outdoor only with modifications\n*   Tattooing, piercing, and non-medical electrolysis must close\n*   Physician-ordered electrolysis may be performed indoors\n\nSubstantial (red): Indoor with modifications\n\nModerate (orange): Indoor with modifications\n\nMinimal (yellow): Indoor with modifications\n\nPersonal care services provided indoors\n\n*   Follow this [guidance for personal care services](https://files.covid19.ca.gov/pdf/guidance-expanded-personal-care-services--en.pdf) like nail salons, tattoo parlors, and body waxing to create a safer environment for workers and patrons. Review the guidance, prepare a plan, and post the [checklist for personal care services](https://files.covid19.ca.gov/pdf/checklist-expanded-personal-care-services.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nPersonal care services provided outdoors\n\n*   Follow this [guidance for personal care services provided outdoors](https://files.covid19.ca.gov/pdf/guidance-outdoor-personal-care--en.pdf) to support an outdoor safe, clean environment for workers and patrons. This guidance applies to services that require touching a client’s face, like facials and waxing. This guidance also applies to esthetic services, skin care, nail services, and massage therapy. Review the guidance, prepare a plan, and post the [checklist for personal care services provided outdoors](https://files.covid19.ca.gov/pdf/checklist-outdoor-personal-care--en.pdf) at your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C197" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5504,10 +5504,10 @@
     </row>
     <row r="198">
       <c r="A198" t="str">
-        <v>Professional sports (without live audiences)</v>
+        <v>Places of worship and cultural ceremonies</v>
       </c>
       <c r="B198" t="str">
-        <v>Professional sports may resume training and competition without live audiences, subject to approval by county public health officers. This guidance does not apply to semi-professional, amateur, or recreational sports.  \n  \nTo reduce the risk of COVID-19 transmission, athletes, coaching staff, medical staff, broadcasting staff and others at sporting facilities or events should abide by COVID-19 protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should follow the [guidance for office workspaces](https://files.covid19.ca.gov/pdf/guidance-office-workspaces--en.pdf).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple): Outdoor only with modifications\n\nSubstantial (red)\n\n*   Indoor with modifications\n*   Indoor activities must be limited to 25% of capacity or 100 people, whichever is less\n\nModerate (orange)\n\n*   Indoor with modifications\n*   Indoor activities must be limited to 50% of capacity or 200 people, whichever is less\n\nMinimal (yellow)\n\n*   Indoor with modifications\n*   Indoor activities must be limited to 50% of capacity\n\nFollow this [guidance for places of worship](https://files.covid19.ca.gov/pdf/guidance-places-of-worship--en.pdf) and providers of religious services and cultural ceremonies, like weddings and funerals, to create a safer environment for workers and visitors.\n\nReview the guidance, prepare a plan, and post the [checklist for places of worship](https://files.covid19.ca.gov/pdf/checklist-places-of-worship--en.pdf) and cultural ceremonies in your workplace to show workers and visitors that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C198" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5530,10 +5530,10 @@
     </row>
     <row r="199">
       <c r="A199" t="str">
-        <v>Public transit and intercity passenger rail</v>
+        <v>Ports</v>
       </c>
       <c r="B199" t="str">
-        <v>Follow this [guidance for public transit agencies](https://files.covid19.ca.gov/pdf/guidance-transit-rail--en.pdf) to create a safer environment for workers and customers.\n\nReview the guidance, prepare a plan, and post the [checklist for public transit agencies](https://files.covid19.ca.gov/pdf/checklist-transit-rail.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for the port industry](https://files.covid19.ca.gov/pdf/guidance-ports--en.pdf) to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for the port industry](https://files.covid19.ca.gov/pdf/checklist-ports--en.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C199" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5556,10 +5556,10 @@
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>Real estate transaction</v>
+        <v>Professional sports (without live audiences)</v>
       </c>
       <c r="B200" t="str">
-        <v>Follow this [guidance for businesses operating in the real estate industry](https://files.covid19.ca.gov/pdf/guidance-real-estate--en.pdf) to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for the real estate industry](https://files.covid19.ca.gov/pdf/checklist-real-estate.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Professional sports may resume training and competition without live audiences, subject to approval by county public health officers. This guidance does not apply to semi-professional, amateur, or recreational sports.  \n  \nTo reduce the risk of COVID-19 transmission, athletes, coaching staff, medical staff, broadcasting staff and others at sporting facilities or events should abide by COVID-19 protocols agreed by labor and management, which may be further enhanced by county public health officers. Back office staff and management should follow the [guidance for office workspaces](https://files.covid19.ca.gov/pdf/guidance-office-workspaces--en.pdf).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C200" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5582,10 +5582,10 @@
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>Restaurants, wineries, and bars</v>
+        <v>Public transit and intercity passenger rail</v>
       </c>
       <c r="B201" t="str">
-        <v>**Tier status:**\n\nWidespread (purple)\n\n*   Restaurants and wineries: Outdoor only with modifications\n*   Bars, breweries, and distilleries: Closed\n\nSubstantial (red)\n\n*   Restaurants: \n    *   Indoor with modifications\n    *   Capacity must be limited to 25% or 100 people, whichever is less\n*   Wineries: Outdoor only with modifications\n*   Bars, breweries, and distilleries: Closed\n\nModerate (orange)\n\n*   Restaurants: \n    *   Indoor with modifications\n    *   Capacity must be limited to 50% or 200 people, whichever is less\n*   Wineries:\n    *   Indoor with modifications\n    *   Capacity must be limited to 25% or 100 people, whichever is less\n*   Bars, breweries, and distilleries: Outdoor only with modifications\n\nMinimal (yellow)\n\n*   Restaurants: \n    *   Indoor with modifications\n    *   Capacity must be limited to 50%\n*   Wineries:\n    *   Indoor with modifications\n    *   Capacity must be limited to 50% or 200 people, whichever is less\n*   Bars, breweries, and distilleries: \n    *   Indoor with modifications\n    *   Capacity must be limited to 50%\n\nTake-out restaurants\n\n*   Follow this [guidance for restaurants providing take-out, drive-through, and delivery](https://files.covid19.ca.gov/pdf/guidance-take-out-restaurants--en.pdf) to create a safer environment for workers and patrons.\n*   Review the guidance and prepare a plan for your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nOutdoor dining\n\n*   Follow this [guidance for restaurants providing outdoor dining, take-out, drive-through, and delivery](https://files.covid19.ca.gov/pdf/guidance-outdoor-restaurants--en.pdf) to create a safer environment for workers and patrons.\n*   Review the guidance and prepare a plan for your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nRestaurants, wineries, and bars\n\n*   Follow this [guidance for restaurants, wineries, and bars](https://files.covid19.ca.gov/pdf/guidance-restaurants-bars-wineries--en.pdf) to create a safer environment for workers and patrons.\n*   Review the guidance, prepare a plan, and post the [checklist for restaurants, wineries, and bars](https://files.covid19.ca.gov/pdf/checklist-restaurants-bars.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business. \n\nDine-in restaurants\n\n*   Follow this [guidance for dine-in restaurants](https://files.covid19.ca.gov/pdf/guidance-dine-in-restaurants--en.pdf) to create a safer environment for workers and customers.\n*   Review the guidance, prepare a plan, and post the [checklist for dine-in restaurants](https://files.covid19.ca.gov/pdf/checklist-dine-in-restaurants.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for public transit agencies](https://files.covid19.ca.gov/pdf/guidance-transit-rail--en.pdf) to create a safer environment for workers and customers.\n\nReview the guidance, prepare a plan, and post the [checklist for public transit agencies](https://files.covid19.ca.gov/pdf/checklist-transit-rail--en.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C201" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5608,10 +5608,10 @@
     </row>
     <row r="202">
       <c r="A202" t="str">
-        <v>Retail</v>
+        <v>Real estate transaction</v>
       </c>
       <c r="B202" t="str">
-        <v>**Tier status:**\n\nWidespread (purple)\n\n*   Open with modifications\n*   Retail capacity must be limited to 25%\n*   Grocery store capacity must be limited to 50%\n\nSubstantial (red)\n\n*   Open with modifications\n*   Retail capacity must be limited to 50%\n\nModerate (orange): Indoor with modifications\n\nMinimal (yellow): Indoor with modifications\n\nFollow this [guidance for retailers](https://files.covid19.ca.gov/pdf/guidance-retail--en.pdf) to create a safer environment for workers and customers. Review the guidance, prepare a plan, and post the [checklist for retail](https://files.covid19.ca.gov/pdf/checklist-retail.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nRetailers and libraries can re-open, along with the manufacturing and logistics sectors that support retail.  \n  \nLibraries should follow the [guidance for retailers](https://files.covid19.ca.gov/pdf/guidance-retail--en.pdf). The State Library has also released guidance for the [re-opening of libraries for in-person services](https://library.ca.gov/Content/pdf/services/toLibraries/COVIDGuidanceLibraries.pdf). See the [State Library’s COVID-19 website](https://www.library.ca.gov/covid-19) for more information. Find [resources for public libraries](https://www.cla-net.org/page/7-1) by the California Library Association and the State Library.  \n  \nDrive-in and movie theaters can re-open with additional considerations.\n\nRetail doesn’t include personal services such as beauty salons, but does include the sale of goods such as:\n\n*   Bookstores\n*   Jewelry stores\n*   Toy stores\n*   Clothing and shoe stores\n*   Home and furnishing stores\n*   Sporting goods stores\n*   Florists\n\nRetail stores identified in the [essential workforce list](https://covid19.ca.gov/essential-workforce/) can open for in-store shopping. They include:\n\n*   Retail facilities specializing in medical goods and supplies\n*   Grocery stores, pharmacies, convenience stores, and other retail that sells food or beverage products, and animal/pet food\n*   Fuel centers such as gas stations and truck stops\n*   Hardware and building materials stores, consumer electronics, technology and appliances retail\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Follow this [guidance for businesses operating in the real estate industry](https://files.covid19.ca.gov/pdf/guidance-real-estate--en.pdf) to create a safer environment for workers.\n\nReview the guidance, prepare a plan, and post the [checklist for the real estate industry](https://files.covid19.ca.gov/pdf/checklist-real-estate--en.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C202" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5634,10 +5634,10 @@
     </row>
     <row r="203">
       <c r="A203" t="str">
-        <v>Schools</v>
+        <v>Restaurants, wineries, and bars</v>
       </c>
       <c r="B203" t="str">
-        <v>**Tier status:**\n\nWidespread (purple):\n\n*   Closed for in-person instruction\n\nSubstantial (red):\n\n*   Closed for in-person instruction\n*   Can open in-person instruction if county remains in this tier for two weeks\n\nModerate (orange): \n\n*   Can open in-person instruction\n\nMinimal (yellow): \n\n*   Can open for in-person instruction\n\nFind information for [your school district](https://www.cde.ca.gov/schooldirectory).\n\nFollow this [guidance for schools and school-based programs](https://files.covid19.ca.gov/pdf/guidance-schools--en.pdf) to create a safer environment for your students, families, and staff. This guidance applies to in-person learning and distance learning. Review the guidance, prepare a plan, and post the [checklist for schools](https://files.covid19.ca.gov/pdf/checklist-schools--en.pdf) in your facility to show students, families, and staff that you’ve taken steps to mitigate COVID-19 spread.\n\n*   Guidelines for sports and extracurricular activities consistent with the [California Interscholastic Federation statement](https://cifstate.org/mediacenter/releases/2019-20/PR-34_7.20.20_CIF_Statement_2020-21_Sports_Calendar_Final.pdf) are included. \n*   Check the answers to [frequently asked questions](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Schools-FAQ.aspx) related to schools. \n*   Find all details in the [COVID-19 and Reopening In-Person Learning Framework for K-12 Schools (PDF)](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Schools%20Reopening%20Recommendations.pdf). \n\nCohorts of kids and adults in controlled, supervised settings\n\nA **cohort** is a stable group of no more than 14 children or youth and no more than two supervising adults in a supervised environment. The group stays together for all activities, including meals and recreation. And this group avoids contact with anyone not in their group.\n\nFollow the [guidance for cohorts of children](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/small-groups-child-youth.aspx) and youth in controlled, supervised and indoor environments. These environments include, but are not limited to, the following:\n\n*   public and private schools\n*   licensed and license-exempt child care settings \n*   organized and supervised care environments, like “distance learning hubs”\n*   recreation programs\n*   before and after school programs\n*   youth groups\n*   day camps\n\nSee the answers to [frequently asked questions](https://files.covid19.ca.gov/pdf/guidance-schools-cohort-FAQ.pdf) about cohort guidance. \n\nKids and adults in supervised care environments must be in groups as small as possible. Kids and supervising adults in one group must not physically interact with:\n\n*   kids and supervising adults in other groups\n*   other facility staff\n*   parents of kids in other groups\n\nPracticing a cohort structure:\n\n*   decreases opportunities for exposure to or transmission of the virus\n*   facilitates more efficient contact tracing in the event of a positive case\n*   allows for targeted testing, quarantine, and isolation of a single group instead of an entire population of kids and supervising adults\n\nElementary education waiver:\n\n*   See the [Waiver Process Overview](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/In-Person-Elementary-Waiver-Process.aspx) for details.\n*   Local health officers will need to submit the [Waiver Notice Form](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/CDPH-Waiver-Notice_8.3.2020.pdf) to CDPH.\n*   Schools seeking a waiver can use the template [Waiver Letter and Cover Form](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Waiver-Letter-Template-Cover-Form_8.3.2020.pdf).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple)\n\n*   Restaurants and wineries: Outdoor only with modifications\n*   Bars, breweries, and distilleries: Closed\n\nSubstantial (red)\n\n*   Restaurants: \n    *   Indoor with modifications\n    *   Capacity must be limited to 25% or 100 people, whichever is less\n*   Wineries: Outdoor only with modifications\n*   Bars, breweries, and distilleries: Closed\n\nModerate (orange)\n\n*   Restaurants: \n    *   Indoor with modifications\n    *   Capacity must be limited to 50% or 200 people, whichever is less\n*   Wineries:\n    *   Indoor with modifications\n    *   Capacity must be limited to 25% or 100 people, whichever is less\n*   Bars, breweries, and distilleries: Outdoor only with modifications\n\nMinimal (yellow)\n\n*   Restaurants: \n    *   Indoor with modifications\n    *   Capacity must be limited to 50%\n*   Wineries:\n    *   Indoor with modifications\n    *   Capacity must be limited to 50% or 200 people, whichever is less\n*   Bars, breweries, and distilleries: \n    *   Indoor with modifications\n    *   Capacity must be limited to 50%\n\nTake-out restaurants\n\n*   Follow this [guidance for restaurants providing take-out, drive-through, and delivery](https://files.covid19.ca.gov/pdf/guidance-take-out-restaurants--en.pdf) to create a safer environment for workers and patrons.\n*   Review the guidance and prepare a plan for your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nOutdoor dining\n\n*   Follow this [guidance for restaurants providing outdoor dining, take-out, drive-through, and delivery](https://files.covid19.ca.gov/pdf/guidance-outdoor-restaurants--en.pdf) to create a safer environment for workers and patrons.\n*   Review the guidance and prepare a plan for your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nRestaurants, wineries, and bars\n\n*   Follow this [guidance for restaurants, wineries, and bars](https://files.covid19.ca.gov/pdf/guidance-restaurants-bars-wineries--en.pdf) to create a safer environment for workers and patrons.\n*   Review the guidance, prepare a plan, and post the [checklist for restaurants, wineries, and bars](https://files.covid19.ca.gov/pdf/checklist-restaurants-bars--en.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business. \n\nDine-in restaurants\n\n*   Follow this [guidance for dine-in restaurants](https://files.covid19.ca.gov/pdf/guidance-dine-in-restaurants--en.pdf) to create a safer environment for workers and customers.\n*   Review the guidance, prepare a plan, and post the [checklist for dine-in restaurants](https://files.covid19.ca.gov/pdf/checklist-dine-in-restaurants--en.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C203" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5660,10 +5660,10 @@
     </row>
     <row r="204">
       <c r="A204" t="str">
-        <v>Shopping centers</v>
+        <v>Retail</v>
       </c>
       <c r="B204" t="str">
-        <v>**Tier status:**\n\nWidespread (purple):\n\n*   Open with modifications\n*   Indoor capacity must be limited to 25% for shopping malls, destination shopping centers, and swap meets\n*   Closed common areas\n*   Closed food courts\n\nSubstantial (red):\n\n*   Open with modifications\n*   Indoor capacity must be limited to 50% for shopping malls, destination shopping centers, and swap meets\n*   Closed common areas\n*   Reduced capacity food courts (see [restaurants](https://covid19.ca.gov/industry-guidance/#restaurants))\n\nModerate (orange):\n\n*   Open with modifications\n*   Closed common areas\n*   Reduced capacity food courts (see [restaurants](https://covid19.ca.gov/industry-guidance/#restaurants))\n\nMinimal (yellow):\n\n*   Open with modifications\n*   Reduced capacity food courts (see [restaurants](https://covid19.ca.gov/industry-guidance/#restaurants))\n\nFollow this [guidance for shopping centers](https://files.covid19.ca.gov/pdf/guidance-shopping-centers--en.pdf), destination shopping centers, strip and outlet malls, and swap meets to create a safer environment for workers and customers. \n\nReview the guidance, prepare a plan, and post the [checklist for shopping centers](https://files.covid19.ca.gov/pdf/checklist-shopping-centers.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple)\n\n*   Open with modifications\n*   Retail capacity must be limited to 25%\n*   Grocery store capacity must be limited to 50%\n\nSubstantial (red)\n\n*   Open with modifications\n*   Retail capacity must be limited to 50%\n\nModerate (orange): Indoor with modifications\n\nMinimal (yellow): Indoor with modifications\n\nFollow this [guidance for retailers](https://files.covid19.ca.gov/pdf/guidance-retail--en.pdf) to create a safer environment for workers and customers. Review the guidance, prepare a plan, and post the [checklist for retail](https://files.covid19.ca.gov/pdf/checklist-retail--en.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nRetailers and libraries can re-open, along with the manufacturing and logistics sectors that support retail.  \n  \nLibraries should follow the [guidance for retailers](https://files.covid19.ca.gov/pdf/guidance-retail--en.pdf). The State Library has also released guidance for the [re-opening of libraries for in-person services](https://library.ca.gov/Content/pdf/services/toLibraries/COVIDGuidanceLibraries.pdf). See the [State Library’s COVID-19 website](https://www.library.ca.gov/covid-19) for more information. Find [resources for public libraries](https://www.cla-net.org/page/7-1) by the California Library Association and the State Library.  \n  \nDrive-in and movie theaters can re-open with additional considerations.\n\nRetail doesn’t include personal services such as beauty salons, but does include the sale of goods such as:\n\n*   Bookstores\n*   Jewelry stores\n*   Toy stores\n*   Clothing and shoe stores\n*   Home and furnishing stores\n*   Sporting goods stores\n*   Florists\n\nRetail stores identified in the [essential workforce list](https://covid19.ca.gov/essential-workforce/) can open for in-store shopping. They include:\n\n*   Retail facilities specializing in medical goods and supplies\n*   Grocery stores, pharmacies, convenience stores, and other retail that sells food or beverage products, and animal/pet food\n*   Fuel centers such as gas stations and truck stops\n*   Hardware and building materials stores, consumer electronics, technology and appliances retail\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C204" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5686,10 +5686,10 @@
     </row>
     <row r="205">
       <c r="A205" t="str">
-        <v>Support for working families</v>
+        <v>Schools</v>
       </c>
       <c r="B205" t="str">
-        <v>The [support for working families](https://files.covid19.ca.gov/pdf/guidance-support-working-families--en.pdf) guidance provides information to help you locate child care, find assistance to pay for child care, and connect you to additional supports for your family. As stay-at-home orders are lifted for additional industries to promote California’s economic recovery, the need for child care and other supports for working families increases.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>Find information for [your school district](https://www.cde.ca.gov/schooldirectory).\n\nFollow this [guidance for schools and school-based programs](https://files.covid19.ca.gov/pdf/guidance-schools--en.pdf) to create a safer environment for your students, families, and staff. This guidance applies to in-person learning and distance learning.\n\n*   Review the guidance, prepare a plan, and post the [checklist for schools](https://files.covid19.ca.gov/pdf/checklist-schools--en.pdf) in your facility to show students, families, and staff that you’ve taken steps to mitigate COVID-19 spread.\n*   Check the answers to [frequently asked questions](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Schools-FAQ.aspx) about guidance for schools. \n*   Follow the [guidance related to cohorts](https://covid19.ca.gov/industry-guidance/#cohort-guidance) of children and youth.\n*   See the [California Interscholastic Federation statement](https://cifstate.org/mediacenter/releases/2019-20/PR-34_7.20.20_CIF_Statement_2020-21_Sports_Calendar_Final.pdf) for information about seasonal sports.\n\nSome schools may have reopened based on the [COVID-19 and Reopening In-Person Learning Framework for K-12 Schools](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Schools%20Reopening%20Recommendations.pdf). These schools should follow the guidance on school closure provided in that framework when determining whether to close due to COVID-19 spread.\n\nElementary education waiver:\n\n*   See the [Waiver Process Overview](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/In-Person-Elementary-Waiver-Process.aspx) for details.\n*   Local health officers will need to submit the [Waiver Notice Form](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/CDPH-Waiver-Notice_8.3.2020.pdf) to CDPH.\n*   Schools seeking a waiver can use the template [Waiver Letter and Cover Form](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Waiver-Letter-Template-Cover-Form_8.3.2020.pdf).\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C205" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5712,10 +5712,10 @@
     </row>
     <row r="206">
       <c r="A206" t="str">
-        <v>Youth sports</v>
+        <v>Shopping centers</v>
       </c>
       <c r="B206" t="str">
-        <v>Follow this [guidance for youth sports](https://files.covid19.ca.gov/pdf/guidance-youth-sports--en.pdf) programs, including school-based, club, and recreational programs. Review the guidance and prepare a plan to support a safe environment for players, coaches and trainers, families, spectators, event/program/facility managers, workers, and volunteers. \n\n*   Check the [questions and answers](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Youth-Sports-FAQ.aspx) about youth sports. \n\nCohorts of kids and adults in controlled, supervised settings\n\nA **cohort** is a stable group of no more than 14 children or youth and no more than two supervising adults in a supervised environment. The group stays together for all activities, including meals and recreation. And this group avoids contact with anyone not in their group.\n\nFollow the [guidance for cohorts of children](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/small-groups-child-youth.aspx) and youth in controlled, supervised and indoor environments. These environments include, but are not limited to, the following:\n\n*   public and private schools\n*   licensed and license-exempt child care settings \n*   organized and supervised care environments, like “distance learning hubs”\n*   recreation programs\n*   before and after school programs\n*   youth groups\n*   day camps\n\nSee the answers to [frequently asked questions](https://files.covid19.ca.gov/pdf/guidance-schools-cohort-FAQ.pdf) about cohort guidance. \n\nKids and adults in supervised care environments must be in groups as small as possible. Kids and supervising adults in one group must not physically interact with:\n\n*   kids and supervising adults in other groups\n*   other facility staff\n*   parents of kids in other groups\n\nPracticing a cohort structure\n\n*   decreases opportunities for exposure to or transmission of the virus\n*   facilitates more efficient contact tracing in the event of a positive case\n*   allows for targeted testing, quarantine, and isolation of a single group instead of an entire population of kids and supervising adults\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
+        <v>**Tier status:**\n\nWidespread (purple):\n\n*   Open with modifications\n*   Indoor capacity must be limited to 25% for shopping malls, destination shopping centers, and swap meets\n*   Closed common areas\n*   Closed food courts\n\nSubstantial (red):\n\n*   Open with modifications\n*   Indoor capacity must be limited to 50% for shopping malls, destination shopping centers, and swap meets\n*   Closed common areas\n*   Reduced capacity food courts (see [restaurants](https://covid19.ca.gov/industry-guidance/#restaurants))\n\nModerate (orange):\n\n*   Open with modifications\n*   Closed common areas\n*   Reduced capacity food courts (see [restaurants](https://covid19.ca.gov/industry-guidance/#restaurants))\n\nMinimal (yellow):\n\n*   Open with modifications\n*   Reduced capacity food courts (see [restaurants](https://covid19.ca.gov/industry-guidance/#restaurants))\n\nFollow this [guidance for shopping centers](https://files.covid19.ca.gov/pdf/guidance-shopping-centers--en.pdf), destination shopping centers, strip and outlet malls, and swap meets to create a safer environment for workers and customers. \n\nReview the guidance, prepare a plan, and post the [checklist for shopping centers](https://files.covid19.ca.gov/pdf/checklist-shopping-centers--en.pdf) in your workplace to show customers and employees that you’ve reduced the risk and are open for business.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C206" t="str">
         <v>https://covid19.ca.gov/industry-guidance/</v>
@@ -5738,13 +5738,13 @@
     </row>
     <row r="207">
       <c r="A207" t="str">
-        <v>Tools for families facing stress</v>
+        <v>Support for working families</v>
       </c>
       <c r="B207" t="str">
-        <v>*   [**Noggin’s Navigating the New Normal: Parents Edition**](https://www.noggin.com/navigating-the-new-normal-parents-edition/) (video)  \n    Host Jamie-Lynn Sigler asks Dr. Nadine Burke Harris and other leading experts how to handle the stress of the pandemic on little kids. \n*   [**How to Support Our Kids During COVID-19**](https://podcasts.apple.com/us/podcast/how-to-support-our-kids-during-covid-19-dr-nadine-burke/id1468607534?i=1000470057466) (Apple podcast)  \n    Dr. Burke Harris shares advice on how to talk to your kids about COVID-19, what all of us can do to help, and how to mitigate stress while stuck at home.  \n*   [**FOCUS on the GO!**](https://nfrc.ucla.edu/focus-on-the-go) (app)  \n    Free mobile app designed to help your family enhance existing coping skills and develop new ones through gameplay.\n*   [**Young Children at Home During the COVID-19 Outbreak: The Importance of Self-Care**](https://www.zerotothree.org/resources/3262-young-children-at-home-during-the-covid-19-outbreak-the-importance-of-self-care) (article)  \n    Knowing how to take care of yourself as a caregiver during the COVID-19 outbreak is key to ensure you are most effective in parenting.\n\nMore info: [Manage stress for health](https://covid19.ca.gov/manage-stress-for-health/)</v>
+        <v>The [support for working families](https://files.covid19.ca.gov/pdf/guidance-support-working-families--en.pdf) guidance provides information to help you locate child care, find assistance to pay for child care, and connect you to additional supports for your family. As stay-at-home orders are lifted for additional industries to promote California’s economic recovery, the need for child care and other supports for working families increases.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C207" t="str">
-        <v>https://covid19.ca.gov/manage-stress-for-health/</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D207" t="str">
         <v xml:space="preserve"> </v>
@@ -5764,13 +5764,13 @@
     </row>
     <row r="208">
       <c r="A208" t="str">
-        <v>Tools for parents to help children</v>
+        <v>Youth sports</v>
       </c>
       <c r="B208" t="str">
-        <v>*   [**California Surgeon General’s Playbook: Stress Relief for Caregivers and Kids During COVID-19**](https://files.covid19.ca.gov/pdf/caregivers_and_kids_california_surgeon_general_stress_busting_playbook_draft_v2_clean_ada_04072020v2.pdf) (PDF)  \n    This guide can help you understand what signs of stress to look out for and what you can do to protect your family’s health. It is also available in [Arabic](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_arabic-2.pdf), Chinese ([Simplified](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_ch_simplified.pdf) and [Traditional](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_zh-hant.pdf)), [Korean](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_korean.pdf), [Spanish](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook-spanish.pdf), [Tagalog](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_tagalog.pdf), and [Vietnamese](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_vi.pdf).\n*   [**Trauma Informed Parent: Helping Adults and Children With Trauma During the Pandemic**](https://www.youtube.com/watch?v=57EAL_e5Nf0) (video)  \n    California’s Surgeon General provides context and tools for how to help kids who have endured past trauma through current stress. \n*   [**Emotional Wellbeing during the COVID-19 Pandemic**](https://www.childtrends.org/publications/resources-for-supporting-childrens-emotional-well-being-during-the-covid-19-pandemic) (guide)  \n    Supporting children’s emotional wellbeing during the COVID-19 pandemic is key to adjusting to a new sense of normal.\n\nMore info: [Manage stress for health](https://covid19.ca.gov/manage-stress-for-health/)</v>
+        <v>Follow this [guidance for youth sports](https://files.covid19.ca.gov/pdf/guidance-youth-sports--en.pdf) programs, including school-based, club, and recreational programs. Review the guidance and prepare a plan to support a safe environment for players, coaches and trainers, families, spectators, event/program/facility managers, workers, and volunteers. \n\n*   Check the [questions and answers](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Youth-Sports-FAQ.aspx) about youth sports.\n*   Follow the [guidance related to cohorts](https://covid19.ca.gov/industry-guidance/#cohort-guidance) of children and youth.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)</v>
       </c>
       <c r="C208" t="str">
-        <v>https://covid19.ca.gov/manage-stress-for-health/</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D208" t="str">
         <v xml:space="preserve"> </v>
@@ -5790,13 +5790,13 @@
     </row>
     <row r="209">
       <c r="A209" t="str">
-        <v>Tools for families with school-related stress</v>
+        <v>What is a cohort?</v>
       </c>
       <c r="B209" t="str">
-        <v>*   [**School’s Out: A Parent’s Guide for Meeting the Challenge During the COVID-19 Pandemic**](https://nyulangone.org/news/schools-out-parents-guide-meeting-challenge-during-covid-19-pandemic) (article)  \n    Understanding a child’s need for structure, education, exercise, social contact, appropriate leisure time, and a calm, rational explanation about COVID-19 is key to ensuring healthy adaptation for youth.\n*   [**The Secret to Keeping Your Kids Happy, Busy and Learning if Their School Closes Due to Coronavirus**](https://time.com/5803373/coronavirus-kids-at-home-activities/) (article)  \n    This article identifies key elements to supporting children and youth as they transition to home-based learning.\n*   [**How LGBTQ Youth Can Cope with Anxiety and Stress During COVID-19**](https://www.thetrevorproject.org/2020/03/26/how-lgbtq-youth-can-cope-with-anxiety-and-stress-during-covid-19/) (blog post)   \n    Advice from The Trevor Project to help LGBTQ youth face the additional isolation and stress they experience during COVID-19. \n\nMore info: [Manage stress for health](https://covid19.ca.gov/manage-stress-for-health/)</v>
+        <v>A cohort is a stable group of no more than 14 children or youth and no more than two supervising adults in a supervised environment. The group stays together for all activities, including meals and recreation. And this group avoids contact with anyone not in their group. Check the guidance about [cohorts for children and youth.](https://covid19.ca.gov/industry-guidance/#cohort-guidance)\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)&lt;!-- pod, gathering, youth, kid, school, class, distance, learning, hub --&gt;</v>
       </c>
       <c r="C209" t="str">
-        <v>https://covid19.ca.gov/manage-stress-for-health/</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D209" t="str">
         <v xml:space="preserve"> </v>
@@ -5816,13 +5816,13 @@
     </row>
     <row r="210">
       <c r="A210" t="str">
-        <v>Should I wear a mask or face covering to protect against COVID-19?</v>
+        <v>What are the rules for cosmetology? What guidance applies for this industry?</v>
       </c>
       <c r="B210" t="str">
-        <v>Yes. Californians must wear face coverings when in public spaces, especially indoors and other areas where physical distancing is not possible. Face coverings help reduce the spread of COVID-19. \n\nThe California Department of Public Health (CDPH) has released [guidance for the use of face coverings](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Guidance-for-Face-Coverings_06-18-2020.pdf). \n\nThe guidance reminds Californians that the best defense against COVID-19 continues to be: \n\n*   Maintain six feet of physical distance from others \n*   Wash hands frequently\n*   Avoid touching eyes, nose and mouth with unwashed hands\n*   Avoid being around people with COVID-19 symptoms\n\nMore info: [Masks and face coverings](https://covid19.ca.gov/masks-and-ppe/)</v>
+        <v>Check the guidance for [hair salons and barbershops.](https://covid19.ca.gov/industry-guidance/#hair-salons-guidance) And check the guidance for [personal care services](https://covid19.ca.gov/industry-guidance/#personal-care-services), such as nails, waxing, and facials.\n\nMore info: [Industry guidance to reduce risk](https://covid19.ca.gov/industry-guidance/)&lt;!-- face, electrolysis, esthetic, skin, cosmetology, electrology, body art, tattoo, permanent makeup, piercing shops, massage, esthetician --&gt;</v>
       </c>
       <c r="C210" t="str">
-        <v>https://covid19.ca.gov/masks-and-ppe/</v>
+        <v>https://covid19.ca.gov/industry-guidance/</v>
       </c>
       <c r="D210" t="str">
         <v xml:space="preserve"> </v>
@@ -5842,13 +5842,13 @@
     </row>
     <row r="211">
       <c r="A211" t="str">
-        <v>How well do face coverings prevent spread of COVID-19?</v>
+        <v>Tools for families facing stress</v>
       </c>
       <c r="B211" t="str">
-        <v>There is scientific evidence to suggest that use of masks or face coverings reduces disease transmission. Their primary role is to reduce the release of infectious particles into the air when someone speaks, coughs, or sneezes. Face coverings are not a substitute for physical distancing, washing hands, and staying home when ill, but complements them.\n\nMore info: [Masks and face coverings](https://covid19.ca.gov/masks-and-ppe/)</v>
+        <v>*   [**Noggin’s Navigating the New Normal: Parents Edition**](https://www.noggin.com/navigating-the-new-normal-parents-edition/) (video)  \n    Host Jamie-Lynn Sigler asks Dr. Nadine Burke Harris and other leading experts how to handle the stress of the pandemic on little kids. \n*   [**How to Support Our Kids During COVID-19**](https://podcasts.apple.com/us/podcast/how-to-support-our-kids-during-covid-19-dr-nadine-burke/id1468607534?i=1000470057466) (Apple podcast)  \n    Dr. Burke Harris shares advice on how to talk to your kids about COVID-19, what all of us can do to help, and how to mitigate stress while stuck at home.  \n*   [**FOCUS on the GO!**](https://nfrc.ucla.edu/focus-on-the-go) (app)  \n    Free mobile app designed to help your family enhance existing coping skills and develop new ones through gameplay.\n*   [**Young Children at Home During the COVID-19 Outbreak: The Importance of Self-Care**](https://www.zerotothree.org/resources/3262-young-children-at-home-during-the-covid-19-outbreak-the-importance-of-self-care) (article)  \n    Knowing how to take care of yourself as a caregiver during the COVID-19 outbreak is key to ensure you are most effective in parenting.\n\nMore info: [Manage stress for health](https://covid19.ca.gov/manage-stress-for-health/)</v>
       </c>
       <c r="C211" t="str">
-        <v>https://covid19.ca.gov/masks-and-ppe/</v>
+        <v>https://covid19.ca.gov/manage-stress-for-health/</v>
       </c>
       <c r="D211" t="str">
         <v xml:space="preserve"> </v>
@@ -5868,13 +5868,13 @@
     </row>
     <row r="212">
       <c r="A212" t="str">
-        <v>What is a face covering?</v>
+        <v>Tools for parents to help children</v>
       </c>
       <c r="B212" t="str">
-        <v>A face covering, also known as a cloth mask, is [material that covers the nose and mouth](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/diy-cloth-face-coverings.html). It can be secured to the head with ties or straps or simply wrapped around the lower face. It can be made of a variety of materials, such as cotton, silk, or linen. A face covering may be factory-made or sewn by hand, or can be improvised from household items such as scarfs, T-shirts, sweatshirts, or towels.\n\nMore info: [Masks and face coverings](https://covid19.ca.gov/masks-and-ppe/)</v>
+        <v>*   [**California Surgeon General’s Playbook: Stress Relief for Caregivers and Kids During COVID-19**](https://files.covid19.ca.gov/pdf/caregivers_and_kids_california_surgeon_general_stress_busting_playbook_draft_v2_clean_ada_04072020v2.pdf) (PDF)  \n    This guide can help you understand what signs of stress to look out for and what you can do to protect your family’s health. It is also available in [Arabic](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_arabic-2.pdf), Chinese ([Simplified](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_ch_simplified.pdf) and [Traditional](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_zh-hant.pdf)), [Korean](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_korean.pdf), [Spanish](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook-spanish.pdf), [Tagalog](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_tagalog.pdf), and [Vietnamese](https://files.covid19.ca.gov/pdf/wp/osg-caregivers-and-kids-playbook_vi.pdf).\n*   [**Trauma Informed Parent: Helping Adults and Children With Trauma During the Pandemic**](https://www.youtube.com/watch?v=57EAL_e5Nf0) (video)  \n    California’s Surgeon General provides context and tools for how to help kids who have endured past trauma through current stress. \n*   [**Emotional Wellbeing during the COVID-19 Pandemic**](https://www.childtrends.org/publications/resources-for-supporting-childrens-emotional-well-being-during-the-covid-19-pandemic) (guide)  \n    Supporting children’s emotional wellbeing during the COVID-19 pandemic is key to adjusting to a new sense of normal.\n\nMore info: [Manage stress for health](https://covid19.ca.gov/manage-stress-for-health/)</v>
       </c>
       <c r="C212" t="str">
-        <v>https://covid19.ca.gov/masks-and-ppe/</v>
+        <v>https://covid19.ca.gov/manage-stress-for-health/</v>
       </c>
       <c r="D212" t="str">
         <v xml:space="preserve"> </v>
@@ -5894,13 +5894,13 @@
     </row>
     <row r="213">
       <c r="A213" t="str">
-        <v>How should I care for a cloth mask or face covering?</v>
+        <v>Tools for families with school-related stress</v>
       </c>
       <c r="B213" t="str">
-        <v>It’s a good idea to [wash your face covering](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/diy-cloth-face-coverings.html) frequently, ideally after each use. Have a bag or bin to keep face coverings in until they can be laundered with detergent and hot water and dried on a hot cycle. If you must re-wear your face covering before washing, wash your hands immediately after putting it back on and avoid touching your face. Discard face coverings that:\n\n*   No longer cover the nose and mouth\n*   Have stretched out or damaged ties or straps\n*   Cannot stay on the face\n*   Have holes or tears in the fabric\n\nMore info: [Masks and face coverings](https://covid19.ca.gov/masks-and-ppe/)</v>
+        <v>*   [**School’s Out: A Parent’s Guide for Meeting the Challenge During the COVID-19 Pandemic**](https://nyulangone.org/news/schools-out-parents-guide-meeting-challenge-during-covid-19-pandemic) (article)  \n    Understanding a child’s need for structure, education, exercise, social contact, appropriate leisure time, and a calm, rational explanation about COVID-19 is key to ensuring healthy adaptation for youth.\n*   [**The Secret to Keeping Your Kids Happy, Busy and Learning if Their School Closes Due to Coronavirus**](https://time.com/5803373/coronavirus-kids-at-home-activities/) (article)  \n    This article identifies key elements to supporting children and youth as they transition to home-based learning.\n*   [**How LGBTQ Youth Can Cope with Anxiety and Stress During COVID-19**](https://www.thetrevorproject.org/2020/03/26/how-lgbtq-youth-can-cope-with-anxiety-and-stress-during-covid-19/) (blog post)   \n    Advice from The Trevor Project to help LGBTQ youth face the additional isolation and stress they experience during COVID-19. \n\nMore info: [Manage stress for health](https://covid19.ca.gov/manage-stress-for-health/)</v>
       </c>
       <c r="C213" t="str">
-        <v>https://covid19.ca.gov/masks-and-ppe/</v>
+        <v>https://covid19.ca.gov/manage-stress-for-health/</v>
       </c>
       <c r="D213" t="str">
         <v xml:space="preserve"> </v>
@@ -5920,13 +5920,13 @@
     </row>
     <row r="214">
       <c r="A214" t="str">
-        <v>Is blood plasma authorized as a COVID-19 treatment?</v>
+        <v>Should I wear a mask or face covering to protect against COVID-19?</v>
       </c>
       <c r="B214" t="str">
-        <v>[The FDA issued an Emergency Use Authorization (EUA)](https://www.fda.gov/news-events/press-announcements/fda-issues-emergency-use-authorization-convalescent-plasma-potential-promising-covid-19-treatment) for convalescent plasma to treat hospitalized COVID-19 patients.\n\nThe FDA determined that it is reasonable to believe that COVID-19 convalescent plasma may be effective in making  COVID-19 illness shorter and less severe in some patients. The FDA also determined that the known and potential benefits of this plasma, when used to treat COVID-19, outweigh its known and potential risks. There are no adequate, approved, or available alternative treatments.\n\nMore info: [Survivors of COVID-19: Donate your plasma](https://covid19.ca.gov/plasma/)</v>
+        <v>Yes. Californians must wear face coverings when in public spaces, especially indoors and other areas where physical distancing is not possible. Face coverings help reduce the spread of COVID-19. \n\nThe California Department of Public Health (CDPH) has released [guidance for the use of face coverings](https://www.cdph.ca.gov/Programs/CID/DCDC/CDPH%20Document%20Library/COVID-19/Guidance-for-Face-Coverings_06-18-2020.pdf). \n\nThe guidance reminds Californians that the best defense against COVID-19 continues to be: \n\n*   Maintain six feet of physical distance from others \n*   Wash hands frequently\n*   Avoid touching eyes, nose and mouth with unwashed hands\n*   Avoid being around people with COVID-19 symptoms\n\nMore info: [Masks and face coverings](https://covid19.ca.gov/masks-and-ppe/)</v>
       </c>
       <c r="C214" t="str">
-        <v>https://covid19.ca.gov/plasma/</v>
+        <v>https://covid19.ca.gov/masks-and-ppe/</v>
       </c>
       <c r="D214" t="str">
         <v xml:space="preserve"> </v>
@@ -5946,13 +5946,13 @@
     </row>
     <row r="215">
       <c r="A215" t="str">
-        <v>Is there a convalescent blood plasma donation center near me?</v>
+        <v>What is a face covering?</v>
       </c>
       <c r="B215" t="str">
-        <v>Locate a donation center\n------------------------\n\nFind the blood center near you collecting COVID-19 blood plasma.\n\n[See the plasma donation center lookup](https://covid19.ca.gov/plasma/#plasma-lookup)\n\nMore info: [Survivors of COVID-19: Donate your plasma](https://covid19.ca.gov/plasma/)</v>
+        <v>A face covering, also known as a cloth mask, is [material that covers the nose and mouth](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/diy-cloth-face-coverings.html). It can be secured to the head with ties or straps or simply wrapped around the lower face. It can be made of a variety of materials, such as cotton, silk, or linen. A face covering may be factory-made or sewn by hand, or can be improvised from household items such as scarfs, T-shirts, sweatshirts, or towels.\n\nMore info: [Masks and face coverings](https://covid19.ca.gov/masks-and-ppe/)</v>
       </c>
       <c r="C215" t="str">
-        <v>https://covid19.ca.gov/plasma/</v>
+        <v>https://covid19.ca.gov/masks-and-ppe/</v>
       </c>
       <c r="D215" t="str">
         <v xml:space="preserve"> </v>
@@ -5972,13 +5972,13 @@
     </row>
     <row r="216">
       <c r="A216" t="str">
-        <v>Where can I apply for unemployment?</v>
+        <v>How well do face coverings prevent spread of COVID-19?</v>
       </c>
       <c r="B216" t="str">
-        <v>If you lost your job or had your hours reduced, and meet eligibility requirements, you may be eligible to receive Unemployment Insurance (UI) benefits from California’s Employment Development Department (EDD). Check the [guide to applying for unemployment benefits](https://unemployment.edd.ca.gov/guide).\n\nMore info: [Workers](https://covid19.ca.gov/workers/)</v>
+        <v>There is scientific evidence to suggest that use of masks or face coverings reduces disease transmission. Their primary role is to reduce the release of infectious particles into the air when someone speaks, coughs, or sneezes. Face coverings are not a substitute for physical distancing, washing hands, and staying home when ill, but complements them.\n\nMore info: [Masks and face coverings](https://covid19.ca.gov/masks-and-ppe/)</v>
       </c>
       <c r="C216" t="str">
-        <v>Editorial</v>
+        <v>https://covid19.ca.gov/masks-and-ppe/</v>
       </c>
       <c r="D216" t="str">
         <v xml:space="preserve"> </v>
@@ -5998,13 +5998,13 @@
     </row>
     <row r="217">
       <c r="A217" t="str">
-        <v>Can my pet test positive for coronavirus? Can I take my pet to the vet?</v>
+        <v>How should I care for a cloth mask or face covering?</v>
       </c>
       <c r="B217" t="str">
-        <v>While we are still learning about coronavirus, the risk of your pet testing positive for coronavirus is low. Because [there is still a risk](https://www.cdc.gov/coronavirus/2019-ncov/animals/pets-other-animals.html), keep your pets away from other pets and people outside of your household. Do not put face coverings on pets as this could harm your pet.\n\nYou can go to the vet or pet hospital if your pet is sick. Remember to wear a cloth face covering and to distance yourself at least 6 feet from other pets and owners.</v>
+        <v>It’s a good idea to [wash your face covering](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/diy-cloth-face-coverings.html) frequently, ideally after each use. Have a bag or bin to keep face coverings in until they can be laundered with detergent and hot water and dried on a hot cycle. If you must re-wear your face covering before washing, wash your hands immediately after putting it back on and avoid touching your face. Discard face coverings that:\n\n*   No longer cover the nose and mouth\n*   Have stretched out or damaged ties or straps\n*   Cannot stay on the face\n*   Have holes or tears in the fabric\n\nSee advice from the CDC on [how to select, wear, and clean your mask](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/about-face-coverings.html).\n\nMore info: [Masks and face coverings](https://covid19.ca.gov/masks-and-ppe/)</v>
       </c>
       <c r="C217" t="str">
-        <v>Editorial</v>
+        <v>https://covid19.ca.gov/masks-and-ppe/</v>
       </c>
       <c r="D217" t="str">
         <v xml:space="preserve"> </v>
@@ -6024,13 +6024,13 @@
     </row>
     <row r="218">
       <c r="A218" t="str">
-        <v>What is Larry David's advice?</v>
+        <v>Is blood plasma authorized as a COVID-19 treatment?</v>
       </c>
       <c r="B218" t="str">
-        <v>&lt;blockquote class="twitter-tweet"&gt;&lt;p lang="en" dir="ltr"&gt;“You’re hurting old people like me. Well, not me... I’ll never see you.”&lt;br&gt;&lt;br&gt;Larry David wants everyone to stay home to protect older Californians from &lt;a href="https://twitter.com/hashtag/COVID19?src=hash&amp;amp;ref_src=twsrc%5Etfw"&gt;#COVID19&lt;/a&gt;! &lt;br&gt;He does not do these things. &lt;br&gt;Listen to Larry.&lt;a href="https://twitter.com/hashtag/StayHomeSaveLives?src=hash&amp;amp;ref_src=twsrc%5Etfw"&gt;#StayHomeSaveLives&lt;/a&gt;&lt;a href="https://t.co/snYe5v55Rw"&gt;https://t.co/snYe5v55Rw&lt;/a&gt; &lt;a href="https://t.co/C5cKOaAufE"&gt;pic.twitter.com/C5cKOaAufE&lt;/a&gt;&lt;/p&gt;&amp;mdash; Office of the Governor of California (@CAgovernor) &lt;a href="https://twitter.com/CAgovernor/status/1245110728199045120?ref_src=twsrc%5Etfw"&gt;March 31, 2020&lt;/a&gt;&lt;/blockquote&gt; &lt;script async src="https://platform.twitter.com/widgets.js" charset="utf-8"&gt;&lt;/script&gt;</v>
+        <v>[The FDA issued an Emergency Use Authorization (EUA)](https://www.fda.gov/news-events/press-announcements/fda-issues-emergency-use-authorization-convalescent-plasma-potential-promising-covid-19-treatment) for convalescent plasma to treat hospitalized COVID-19 patients.\n\nThe FDA determined that it is reasonable to believe that COVID-19 convalescent plasma may be effective in making  COVID-19 illness shorter and less severe in some patients. The FDA also determined that the known and potential benefits of this plasma, when used to treat COVID-19, outweigh its known and potential risks. There are no adequate, approved, or available alternative treatments.\n\nMore info: [Survivors of COVID-19: Donate your plasma](https://covid19.ca.gov/plasma/)</v>
       </c>
       <c r="C218" t="str">
-        <v>Editorial</v>
+        <v>https://covid19.ca.gov/plasma/</v>
       </c>
       <c r="D218" t="str">
         <v xml:space="preserve"> </v>
@@ -6050,13 +6050,13 @@
     </row>
     <row r="219">
       <c r="A219" t="str">
-        <v>Where can I find the list of essential critical infrastructure sectors?</v>
+        <v>Is there a convalescent blood plasma donation center near me?</v>
       </c>
       <c r="B219" t="str">
-        <v xml:space="preserve">Visit [Essential workforce](https://covid19.ca.gov/essential-workforce/) to learn about what workers and sectors are included. </v>
+        <v>Locate a donation center\n------------------------\n\nFind the blood center near you collecting COVID-19 blood plasma.\n\n[See the plasma donation center lookup](https://covid19.ca.gov/plasma/#plasma-lookup)\n\nMore info: [Survivors of COVID-19: Donate your plasma](https://covid19.ca.gov/plasma/)</v>
       </c>
       <c r="C219" t="str">
-        <v>Editorial</v>
+        <v>https://covid19.ca.gov/plasma/</v>
       </c>
       <c r="D219" t="str">
         <v xml:space="preserve"> </v>
@@ -6076,10 +6076,10 @@
     </row>
     <row r="220">
       <c r="A220" t="str">
-        <v>What is a cohort?</v>
+        <v>What is Larry David's advice?</v>
       </c>
       <c r="B220" t="str">
-        <v>A cohort is a stable group of no more than 14 children or youth and no more than two supervising adults in a supervised environment. The group stays together for all activities, including meals and recreation. And this group avoids contact with anyone not in their group. &lt;!-- pod, gathering, youth, kid, school, class, distance, learning, hub --&gt;</v>
+        <v>&lt;blockquote class="twitter-tweet"&gt;&lt;p lang="en" dir="ltr"&gt;“You’re hurting old people like me. Well, not me... I’ll never see you.”&lt;br&gt;&lt;br&gt;Larry David wants everyone to stay home to protect older Californians from &lt;a href="https://twitter.com/hashtag/COVID19?src=hash&amp;amp;ref_src=twsrc%5Etfw"&gt;#COVID19&lt;/a&gt;! &lt;br&gt;He does not do these things. &lt;br&gt;Listen to Larry.&lt;a href="https://twitter.com/hashtag/StayHomeSaveLives?src=hash&amp;amp;ref_src=twsrc%5Etfw"&gt;#StayHomeSaveLives&lt;/a&gt;&lt;a href="https://t.co/snYe5v55Rw"&gt;https://t.co/snYe5v55Rw&lt;/a&gt; &lt;a href="https://t.co/C5cKOaAufE"&gt;pic.twitter.com/C5cKOaAufE&lt;/a&gt;&lt;/p&gt;&amp;mdash; Office of the Governor of California (@CAgovernor) &lt;a href="https://twitter.com/CAgovernor/status/1245110728199045120?ref_src=twsrc%5Etfw"&gt;March 31, 2020&lt;/a&gt;&lt;/blockquote&gt; &lt;script async src="https://platform.twitter.com/widgets.js" charset="utf-8"&gt;&lt;/script&gt;</v>
       </c>
       <c r="C220" t="str">
         <v>Editorial</v>

</xml_diff>

<commit_message>
reset url set to crawl
</commit_message>
<xml_diff>
--- a/qnacrawler/merged.xlsx
+++ b/qnacrawler/merged.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H220"/>
+  <dimension ref="A1:H235"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -408,13 +408,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Can air conditioning spread COVID-19 from one room to another?</v>
+        <v>What do taxpayers need to do if they want to take advantage of relief from the California Department of Tax and Fee Administration?</v>
       </c>
       <c r="B2" t="str">
-        <v>There is no evidence that COVID-19 spreads indoors through air conditioning. There are a wide variety of heating, ventilation and air conditioning (HVAC) systems. Well-designed HVAC systems can actually help reduce risk. Since the system filters air as it circulates, it adds cleaner air to the space. Introduction of fresh outdoor air dilutes the concentration of infectious particles. Air conditioning is also necessary in some areas to protect from excessive heat. For more information, see [ASHRAE guidelines for homeowners and HVAC professionals](https://www.ashrae.org/technical-resources/resources). \n\nMore info: [Symptoms and risks](https://covid19.ca.gov/symptoms-and-risks/)</v>
+        <v>Interested taxpayers should contact CDTFA by visiting the [CDTFA website](http://cdtfa.ca.gov/) or calling [800-400-7115](tel:800-400-7115).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C2" t="str">
-        <v>https://covid19.ca.gov/symptoms-and-risks/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D2" t="str">
         <v xml:space="preserve"> </v>
@@ -434,13 +434,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>What are the symptoms of COVID-19?</v>
+        <v>When will taxpayers start on these payment plans?</v>
       </c>
       <c r="B3" t="str">
-        <v>### [Coronavirus symptoms](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html) include, but are not limited to:\n\n*   Fever or chills\n*   Cough\n*   Shortness of breath or difficulty breathing\n*   Fatigue\n*   Muscle or body aches\n*   Headache\n*   New loss of taste or smell\n*   Sore throat\n*   Congestion or runny nose\n*   Nausea or vomiting\n*   Diarrhea\n\nMore info: [Symptoms and risks](https://covid19.ca.gov/symptoms-and-risks/)</v>
+        <v>Given that the April deadline to file and pay sales and use tax returns has been extended to late July for all but the largest taxpayers, CDTFA expects that most participating taxpayers will begin their payment arrangements in late July of this year.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C3" t="str">
-        <v>https://covid19.ca.gov/symptoms-and-risks/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D3" t="str">
         <v xml:space="preserve"> </v>
@@ -460,13 +460,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Is there a COVID-19 symptoms self-checker?</v>
+        <v>How will the payment plans work?</v>
       </c>
       <c r="B4" t="str">
-        <v>You can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor through [telehealth](https://covid19.ca.gov/telehealth/).\n\nMore info: [Symptoms and risks](https://covid19.ca.gov/symptoms-and-risks/)</v>
+        <v>Qualifying sales and use taxpayers with deferred liabilities up to $50,000 will pay their tax due in 12 equal monthly installments. No interest or penalties will be assessed against the liability.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C4" t="str">
-        <v>https://covid19.ca.gov/symptoms-and-risks/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D4" t="str">
         <v xml:space="preserve"> </v>
@@ -486,13 +486,13 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Who are high risk people for COVID-19?</v>
+        <v>Is this only for tax payments due for the 1st quarter of 2020?</v>
       </c>
       <c r="B5" t="str">
-        <v>#### Some people are at [higher risk](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-at-increased-risk.html) to get very sick from COVID-19, including:\n\n*   [People over 65 years old](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/older-adults.html)\n*   [People of any age with certain underlying medical conditions:](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-with-medical-conditions.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fneed-extra-precautions%2Fgroups-at-higher-risk.html)\n    *   [Cancer](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-with-medical-conditions.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fneed-extra-precautions%2Fgroups-at-higher-risk.html#cancer)\n    *   [Chronic kidney disease](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-with-medical-conditions.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fneed-extra-precautions%2Fgroups-at-higher-risk.html#chronic-kidney-disease)\n    *   [COPD (chronic obstructive pulmonary disease)](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-with-medical-conditions.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fneed-extra-precautions%2Fgroups-at-higher-risk.html#copd)\n    *   [Immunocompromised state (weakened immune system) from solid organ transplant](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-with-medical-conditions.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fneed-extra-precautions%2Fgroups-at-higher-risk.html#immunocompromised-state)\n    *   [Obesity (body mass index \[BMI\] of 30 or higher)](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-with-medical-conditions.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fneed-extra-precautions%2Fgroups-at-higher-risk.html#obesity)\n    *   [Serious heart conditions, such as heart failure, coronary artery disease, or cardiomyopathies](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-with-medical-conditions.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fneed-extra-precautions%2Fgroups-at-higher-risk.html#serious-heart-conditions)\n    *   [Sickle cell disease](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-with-medical-conditions.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fneed-extra-precautions%2Fgroups-at-higher-risk.html#hemoglobin-disorders)\n    *   [Type 2 diabetes mellitus](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/people-with-medical-conditions.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fneed-extra-precautions%2Fgroups-at-higher-risk.html#diabetes)\n\nMore info: [Symptoms and risks](https://covid19.ca.gov/symptoms-and-risks/)</v>
+        <v>If taxpayers choose to use this program to distribute the burden of their May or June prepayments or their July return, CDTFA will work to accommodate those taxpayers.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C5" t="str">
-        <v>https://covid19.ca.gov/symptoms-and-risks/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D5" t="str">
         <v xml:space="preserve"> </v>
@@ -512,13 +512,13 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>What people at higher risk, seniors over 65 or compromised immune systems, should do?</v>
+        <v>What if taxpayers owe more than the $50,000 limit on the relief?</v>
       </c>
       <c r="B6" t="str">
-        <v>If you are at higher risk, you should take extra precautions to protect yourself: \n\n*   **Stay home.** It’s the most important thing you can do.\n*   **Avoid contact with people who are sick.** Isolate anyone sick in your home in a separate room, if possible.\n*   **Get food brought to your house** through family, social, or commercial networks. Wipe off containers with disinfectant wipes.\n*   **Listen to public health officials.** They may recommend community actions to reduce exposure in times of local outbreak.\n\nMore info: [Symptoms and risks](https://covid19.ca.gov/symptoms-and-risks/)</v>
+        <v>The maximum amount that any taxpayer can defer interest-free under this relief effort is $50,000.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C6" t="str">
-        <v>https://covid19.ca.gov/symptoms-and-risks/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D6" t="str">
         <v xml:space="preserve"> </v>
@@ -538,13 +538,13 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Has the deadline for federal taxes changed?</v>
+        <v>What if taxpayers with more than $5 million in annual taxable sales need this relief?</v>
       </c>
       <c r="B7" t="str">
-        <v>The federal deadline for filing and paying taxes has been [extended to July 15, 2020](https://www.irs.gov/newsroom/payment-deadline-extended-to-july-15-2020). \n\nSee [information on the U.S. Internal Revenue Service](https://www.irs.gov/coronavirus) for more information.\n\nMore info: [Taxes](https://covid19.ca.gov/taxes/)</v>
+        <v>We recognize that some taxpayers, particularly in low margin businesses, with annual taxable sales over $5 million may also need this relief. Those taxpayers are encouraged to reach out to CDTFA, which will work with them to provide relief where appropriate.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C7" t="str">
-        <v>https://covid19.ca.gov/taxes/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D7" t="str">
         <v xml:space="preserve"> </v>
@@ -564,13 +564,13 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Are there any tax deductions for people affected by the COVID-19 outbreak?</v>
+        <v>Is the deadline for filing California tax returns extended?</v>
       </c>
       <c r="B8" t="str">
-        <v>No. Check with the [U.S. Internal Revenue Service](https://www.irs.gov/coronavirus), the [California Franchise Tax Board](https://www.ftb.ca.gov/), and your local government for updates.\n\nMore info: [Taxes](https://covid19.ca.gov/taxes/)</v>
+        <v>Yes. All California taxpayers (individuals and businesses) can file and pay by July 15, 2020. See [information from the CA Franchise Tax Board](https://www.ftb.ca.gov/about-ftb/newsroom/news-releases/2020-3-state-postpones-tax-deadlines-until-july-15-due-to-the-covid-19-pandemic.html) for more information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C8" t="str">
-        <v>https://covid19.ca.gov/taxes/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D8" t="str">
         <v xml:space="preserve"> </v>
@@ -590,13 +590,13 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>What is the relationship between the stay home order and these questions and answers?</v>
+        <v>What is a loan guarantee?</v>
       </c>
       <c r="B9" t="str">
-        <v>The Governor has ordered Californians to obey the directives of the State Public Health Officer. Those directives take many forms; they include specific materials linked on this page, as well as these questions and answers. These questions and answers are directives from the State Public Health Officer, and have the same force and effect as other State Public Health Officer directives.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>A loan guarantee is a credit enhancement that helps mitigate the risk assumed by a lending institution when making a loan. With the Small Business Finance Center’s Disaster Relief Loan Guarantee Program, IBank agrees to guarantee up to 95% of the loan, removing the barriers to capital that often exist for small business borrowers that may not otherwise be eligible for traditional lending. This program also can assist those who may not be eligible for a U.S. Small Business Administration (SBA) loan.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C9" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D9" t="str">
         <v xml:space="preserve"> </v>
@@ -616,13 +616,13 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>When does the stay home order go into effect and how long will we stay home? What areas of the state are covered?</v>
+        <v>Who is eligible to apply for a loan guarantee?</v>
       </c>
       <c r="B10" t="str">
-        <v>The order went into effect on Thursday, March 19, 2020. The order is in place until further notice. It covers the whole state of California.\n\nAs of May 8, the stay home order was modified. In addition to essential activity, retail is allowed, along with the infrastructure to support it. As of May 12, offices, limited services, and outdoor museums are also permitted to open.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Small business entities that have been affected by loss, damage or other economic injury due to the COVID-19 pandemic and meet the program’s eligibility requirements. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C10" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D10" t="str">
         <v xml:space="preserve"> </v>
@@ -642,13 +642,13 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Is it safe to shop at open businesses?</v>
+        <v>What do you consider a small business?</v>
       </c>
       <c r="B11" t="str">
-        <v>The risk of COVID-19 infection is still real for all Californians and continues to be fatal. That is why every business permitted to open should take every step humanly possible to reduce the risk of infection by following these [state guidelines](https://covid19.ca.gov/industry-guidance/#top).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>The business must have between 1-750 employees and be established as an entity, including:\n\n*   Sole Proprietor – Individual using legal name as business name that files a Schedule C, Schedule F, or has a fictitious business name or DBA statement\n    *   If the loan appears to be in the name of an individual, evidence of Sole Proprietorship will be required and may include a Schedule C, Schedule F, Seller’s Permit, and/or fictitious business name or DBA statement\n*   Limited Liability Company \n*   Cooperative\n*   Corporation\n*   Partnership\n*   S-Corporation\n*   Not-for-profit\n\nThe program will not accept an _individual_ as the borrower. It is permissible for an individual to be a guarantor or co-borrower on the loan, but the primary borrower must be a small business. It does not consider citizenship or immigration status for eligibility requirements**,** as long as the entity/individual meets the above criteria. Trucking owners/operators are eligible as long as they are registered as a legal business entity.\n\n**AND**\n\n*   The business activity must be eligible under the program and in one of the industries listed in the [North American Industry Classification System (NAICS) codes list](http://www.census.gov/eos/www/naics), and\n*   It must be located in a declared disaster area. A major disaster area declaration was made for the state of California on March 22, 2020 in regards to the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C11" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D11" t="str">
         <v xml:space="preserve"> </v>
@@ -668,13 +668,13 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Can the stay home order be changed?</v>
+        <v>What are excluded businesses?</v>
       </c>
       <c r="B12" t="str">
-        <v>Yes. The State Public Health Officer may issue new orders as the public health situation changes.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Businesses that are not eligible include passive real estate businesses (rental income, etc.).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C12" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D12" t="str">
         <v xml:space="preserve"> </v>
@@ -694,13 +694,13 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>How does the stay home order interact with local orders to shelter in place? Does it supersede them?</v>
+        <v>Can I apply for a loan guarantee only if I am ineligible for federal disaster fund financing, such as a SBA loan?</v>
       </c>
       <c r="B13" t="str">
-        <v>This is a statewide order. Counties can have more restrictive criteria and different closures. See [your county’s status](https://covid19.ca.gov/safer-economy).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes, this program is designed for those who do not qualify for federal programs. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C13" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D13" t="str">
         <v xml:space="preserve"> </v>
@@ -720,13 +720,13 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>If I am not an Essential Critical Infrastructure Worker, can I still leave the house?</v>
+        <v>How much can I borrow?</v>
       </c>
       <c r="B14" t="str">
-        <v>Yes. As described in more detail elsewhere in applicable state public health directives (including on this page), there are a wide range of circumstances in which you may leave your home or other place of residence, even if you are not an Essential Critical Infrastructure Worker. For example, you may leave your home to work at any business or other entity that is allowed to open, to engage in in-person worship and protest activities consistent with public health directives, to patronize local businesses, or to care for friends or family members who require assistance (as set forth under [Health care](https://covid19.ca.gov/healthcare/#top)). And errands like these are not the only reasons you may leave your home: you may also leave your home with or without a specific destination in mind (for example, to walk your dog, to engage in physical recreation, or simply to get some fresh air) as long as you maintain physical distancing and comply with any other applicable public health directives.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>The Small Business Finance Center’s Disaster Relief Loan Guarantee Program allows a maximum loan of $1.25 million and a maximum guarantee of $1 million. To serve as many California small businesses as possible, the COVID-19 disaster program is focused on serving small businesses, especially those in low-wealth and immigrant communities with needs from $500 to $50,000. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C14" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D14" t="str">
         <v xml:space="preserve"> </v>
@@ -746,13 +746,13 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Are gatherings permitted?</v>
+        <v>What are the loan terms?</v>
       </c>
       <c r="B15" t="str">
-        <v>Gatherings are defined as meetings or other events that bring together persons from multiple households at the same time for a shared or group experience in a single room, space, or place such as an auditorium, stadium, arena, large conference room, meeting hall, or other indoor or outdoor space. They pose an especially high danger of transmission and spread of COVID-19.\n\nOn May 25, 2020, in an effort to balance First Amendment interests with public health, the State Public Health Officer created an exception to the prohibition against mass gatherings for faith-based services and cultural ceremonies as well as protests. Those types of gatherings are now permitted indoors in counties in Substantial (red), Moderate (orange), and Minimal (yellow) tiers, subject to [certain restrictions](https://covid19.ca.gov/industry-guidance/#worship) in those counties. State public health directives also permit in-person outdoor faith-based services or protests as long as face coverings are worn and physical distancing of 6 feet between persons or groups of persons from different households is maintained at all times.\n\nCrowds and limited physical distancing increase the risk for COVID-19. If you attended a gathering, remember that confidential, free testing is available. [Find a testing location near you](https://urldefense.proofpoint.com/v2/url?u=https-3A__covid19.ca.gov_testing-2Dand-2Dtreatment_-23top&amp;d=DwMGaQ&amp;c=Lr0a7ed3egkbwePCNW4ROg&amp;r=yRsi0eKVK6Khc58oFC32XROAJ-JqVGBGabDv9P6148k&amp;m=Iul4bdNDGFuRu3rXHrxPHNWT2PT2bXFITW3YP1tzG94&amp;s=4qpOZ7lX1S5M_STTblq_XAQNu05ccIFwIyu4bvl9U3c&amp;e=). If you test negative it does not mean that you may not develop COVID-19 later on. Therefore, it is advisable that you self-isolate for 14 days if possible.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>The length of the loan can be negotiated with your lender, but the guarantee is good for up to seven years. The interest rate and loan criteria will be determined by the lender and could depend on the credit strength of the business. The guarantee is designed to lower the interest rate in exchange for a higher guarantee to your lender. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C15" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D15" t="str">
         <v xml:space="preserve"> </v>
@@ -772,13 +772,13 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Can I get a haircut?</v>
+        <v>How can I apply for a loan guarantee?</v>
       </c>
       <c r="B16" t="str">
-        <v>Yes. Hair salons and barbershops are now open throughout the state with modifications for safety.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>The Small Business Finance Center partners with Community Development Financial Institutions (CDFIs), Community Lending Institutions, and Financial Development Corporations (FDCs) to provide loan guarantees for small businesses.  To apply,\n\n*   View the [list of FDCs and participating lenders](http://www.ibank.ca.gov/small-business-finance-center/) interested in this Small Business Disaster Relief Loan Guarantee Program. \n*   Contact the lender on the list nearest to your business to apply.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C16" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D16" t="str">
         <v xml:space="preserve"> </v>
@@ -798,13 +798,13 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Are safety protocols being enforced? How do I report a business that isn’t complying?</v>
+        <v>What is the timing for the funding of loans?</v>
       </c>
       <c r="B17" t="str">
-        <v>They are being enforced, and you can report it. Report unsafe conditions or businesses that shouldn’t be open to your local Alcohol Beverage Control, Labor Commissioner’s office, or regional Cal/OSHA office, depending on the type of business. To find these local contacts, see Appendix B of the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- Adding keywords mask masks report reporting enforce enforcement compliance for quick answers purposes --&gt;</v>
+        <v>The program is in place and businesses can apply immediately. Once you provide your lender with complete information, you could be funded in a matter of days.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C17" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D17" t="str">
         <v xml:space="preserve"> </v>
@@ -824,13 +824,13 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>I want to express my political views.  How can I make my voice heard without raising public health concerns?</v>
+        <v>What can the money be used for?</v>
       </c>
       <c r="B18" t="str">
-        <v>There are many ways for you to express your political views without holding a physical, in-person gathering.  For example, you may continue to call or write elected officials, write letters to the editor of news publications, display lawn or window signs, or use online and other electronic media (including Zoom rooms, Twitter feeds, Facebook pages, and other digital forums) to express your views.  \n\nAdditionally, as noted above, you may leave your home for any reason as long as you comply with any other applicable public health directives. When you are otherwise out in public, public health directives do not prevent you from engaging in political expression—such as by wearing or carrying a sign.\n\nIf collective action in physical space is important to you, consider whether you and other participants can safely protest from within your cars.  The State Public Health Officer does not consider in-car activities to be gatherings, if participants stay in their cars and otherwise remain apart from individuals who are not part of their households.  Many activists have organized car-based protests (honking horns, flying flags, displaying signs, and so on) to express their political views while complying with State public health directives.  \n\nWhenever you are considering a protest (including an in-car protest), make sure you comply with all other applicable laws, including any local public-health measures that may be more restrictive than statewide directives and any other applicable local laws.\n\nIf you do wish to engage in in-person protest outside of your car with a group of any size, you must follow the guidelines for political protest gatherings below.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>The funds are meant to help small businesses through this challenging time. Loan proceeds can be used for business continuance or to cure “economic injury” as a result of COVID-19.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C18" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D18" t="str">
         <v xml:space="preserve"> </v>
@@ -850,13 +850,13 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Can I engage in political protest gatherings?</v>
+        <v>How will this program assist low-wealth and minority communities?</v>
       </c>
       <c r="B19" t="str">
-        <v>Yes, although in-person protests present special public health concerns. \n\nEven with adherence to physical distancing, bringing members of different households together to engage in in-person protest carries a higher risk of widespread transmission of COVID-19.  Such gatherings may result in increased rates of infection, hospitalization, and death, especially among more vulnerable populations. In particular, activities like chanting, shouting, singing, and group recitation negate the risk-reduction achieved through 6 feet of physical distancing. For this reason, people engaging in these activities should wear face coverings at all times.\n\nTherefore, it is strongly recommended that those exercising their right to engage in political expression (including, for example, their right to petition the government) should utilize alternative channels, such as the many online and broadcasting platforms available in the digital age, in place of in-person gatherings. \n\nHowever, state public health directives do not prohibit in-person _outdoor_ protests as long as you maintain a physical distance of 6 feet between persons or groups of persons from different households at all times. When you can’t maintain a safe physical distance of 6 feet from people not in your household, you must wear a face covering or mask. Local Health Officers are advised to consider appropriate limitations on outdoor attendance capacities, factoring their jurisdiction’s key COVID-19 health indicators. Failure to follow these requirements may result in an order to disperse or other enforcement action. Masks and face coverings are strongly recommended.\n\nIn counties in the [Widespread (purple) tier](https://covid19.ca.gov/safer-economy/), indoor protests are not currently permitted. In other counties, state public health directives do not prohibit in-person _indoor_ protests as long as (1) attendance is limited as as required by the [relevant local restrictions](https://covid19.ca.gov/safer-economy) places of worship (2) physical distancing of 6 feet between persons or groups of persons from different households is maintained at all times, and (3) singing and chanting activities are discontinued. Failure to follow these requirements may result in an order to disperse or other enforcement action. Masks and face coverings are required in compliance with CDPH directives.\n\nParticipants must maintain a physical distance of 6 feet from any uniformed peace officers and other public safety personnel present, unless otherwise directed, and follow all other requirements and directives imposed by local health officers and law enforcement, or other applicable authorities.\n\nThis limitation on attendance will be reviewed regularly. This review will assess the impacts of these imposed limits on public health and provide further direction as part of a phased-in restoration of gatherings that implicate the First Amendment.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>By working with the Community Development Financial Institutions (CDFIs) throughout the state of California, this disaster relief program can play an important role in generating economic growth and opportunity in some of our most distressed communities. CDFIs and mission-based lenders play a vital role across the state and have experience steering lending and investment to where it is needed and will matter the most, in particular in low-wealth and immigrant communities. CDFIs and our partner Financial Development Corporations (FDCs) that process the loan guarantees are embedded in communities across the state, speak several languages, and are invested in the community successfully managing its way through this pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C19" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D19" t="str">
         <v xml:space="preserve"> </v>
@@ -876,13 +876,13 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>How do I vote?</v>
+        <v>Are faith-based businesses eligible for this loan guarantee program?</v>
       </c>
       <c r="B20" t="str">
-        <v>**[Elections are an essential activity](https://files.covid19.ca.gov/pdf/CDPH-to-SOS-Letter-from-Acting-HO-Aug-18-1.pdf).** The Governor has issued [executive orders to ensure elections are safe and accessible](https://www.gov.ca.gov/2020/05/08/governor-newsom-issues-executive-order-to-protect-public-health-by-mailing-every-registered-voter-a-ballot-ahead-of-the-november-general-election/). Vote-by-mail ballots will be sent to all registered voters for the November 3, 2020 General Election. Most counties will provide [three days of early voting](https://www.gov.ca.gov/2020/06/03/governor-newsom-signs-executive-order-on-safe-secure-and-accessible-general-election-in-november/) in-person starting the Saturday before the election. Open ballot drop-box locations will be available between October 6 and November 3, 2020. Existing laws addressing the use of vote-by-mail ballots in California elections remain in effect except where suspended by Executive Order. Find [guidance for the safe administration of elections](https://elections.cdn.sos.ca.gov/ccrov/pdf/2020/july/20154jl.pdf) during COVID-19.\n\n Visit [online voter registration](https://registertovote.ca.gov/) to register to vote or check your voter registration status. \n\nPractice physical distancing and follow other applicable public health directives while engaged in election-related activities. These include collection and drop-off of ballots, and collection of signatures to qualify candidates or measures for the ballot.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Faith-based businesses (non-profit or otherwise) that have business activity outside of worship are eligible as long as they are a legal business that has been affected by the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C20" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D20" t="str">
         <v xml:space="preserve"> </v>
@@ -902,13 +902,13 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>Can I go to church?</v>
+        <v>What SBA programs are available to small businesses right now?</v>
       </c>
       <c r="B21" t="str">
-        <v>Yes. Places of worship such as churches, mosques, temples, and synagogues can open throughout the state, with [modifications for safety (PDF)](https://files.covid19.ca.gov/pdf/guidance-places-of-worship--en.pdf). In counties in the [Widespread (purple)](https://covid19.ca.gov/safer-economy) tier, indoor services in places of worship must be discontinued but outdoor and online services are permitted.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>The U.S. SBA offers the **Economic Injury Disaster Loan (EIDL)**.\n\nThe U.S. SBA is accepting new applications from all eligible businesses, and will continue to process **EIDL Loan applications** already submitted on a first come, first-served basis. Check the U.S. SBA’s [Disaster Loan Applications website](https://www.sba.gov/page/disaster-loan-applications#section-header-0) for more information.\n\nThe EIDL is a direct loan for up to $2 million at a rate of 3.75% for small businesses and 2.75% for nonprofits. [Apply directly with the SBA](https://covid19relief.sba.gov/#/). For questions, you can contact SBA’s Customer Service Line at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or send an email to [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nThe **Economic Injury Disaster Loan (**EIDL) **Advance** has been [discontinued](https://www.sba.gov/page/disaster-loan-applications#section-header-0). EIDL loan applications will still be processed even though the Advance is no longer available.\n\nThe [**Paycheck Protection Program (PPP)**](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program#section-header-0) closed August 8, 2020. The U.S. SBA is no longer accepting PPP applications from approved lenders.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C21" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D21" t="str">
         <v xml:space="preserve"> </v>
@@ -928,13 +928,13 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>Can I practice my religious faith?</v>
+        <v>Where do I find more information on allowable expenses for a forgivable loan under the Paycheck Protection Program?</v>
       </c>
       <c r="B22" t="str">
-        <v>Yes. Practicing your faith is a constitutionally-protected activity and may manifest in many different forms.\n\nAlthough in-person religious gatherings—like other in-person gatherings—have been restricted to prevent the transmission of COVID-19, on May 25, 2020, the State Public Health Officer began to ease restrictions on in-person religious gatherings. In particular, the State Public Health Officer now authorizes County Departments of Public Health to allow collective activities at places of worship, subject to conditions to support a safe, clean environment for employees, interns and trainees, volunteers, scholars, and all other types of workers as well as congregants, worshippers, and visitors.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- church, mosque, synagogue, temple, wedding, funeral, baptism --&gt;</v>
+        <v>You can find this on the Paycheck Protection Program’s [Loan Forgiveness Application](https://www.sba.gov/sites/default/files/2020-06/PPP%20Loan%20Forgiveness%20Application%20%28Revised%206.16.2020%29-fillable_0-508.pdf). The application provides detailed [instructions](https://www.sba.gov/sites/default/files/2020-06/PPP%20Loan%20Forgiveness%20Application%20Instructions%20%28Revised%206.16.2020%29-508.pdf) on how to apply for forgiveness of PPP loans. Once your business has expended the PPP funds and is ready to pursue loan forgiveness, please review the Loan Forgiveness Application and consult with your accountant, lender, or one of California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) for assistance. See SBA’s [loan details and forgiveness](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/paycheck-protection-program#section-header-5) information, and check the [frequently asked questions](https://www.sba.gov/sites/default/files/2020-08/PPP%20--%20Loan%20Forgiveness%20FAQs%20%28August%2011%2C%202020%29.pdf) on PPP loan forgiveness.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C22" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D22" t="str">
         <v xml:space="preserve"> </v>
@@ -954,13 +954,13 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>What conditions must be met to resume religious services and cultural ceremonies at places of worship?</v>
+        <v>How does a business know if it is eligible for an SBA loan or loan guarantee program?</v>
       </c>
       <c r="B23" t="str">
-        <v>Information on conditions imposed by the state can be found at [guidance for places of worship (PDF)](https://files.covid19.ca.gov/pdf/guidance-places-of-worship--en.pdf). Additional conditions may be imposed by local public health officials. This guidance does not obligate places of worship to resume in-person activity. It is strongly recommended that places of worship continue to facilitate remote services and other alternatives to in-person religious practice for those who are vulnerable to COVID19.\n\nEven with adherence to physical distancing, convening in a congregational setting of multiple households to practice a personal faith carries a higher risk of widespread transmission of COVID-19, and may result in increased rates of infection, hospitalization, and death, especially among more vulnerable populations. In particular, activities like singing and group recitation dramatically increase the risk of COVID-19 transmission. For this reason, singing and chanting activities must be discontinued at indoor services, and congregants engaging in group recitation should wear face coverings at all times.\n\nPlaces of worship may only open indoor operations when permitted by [relevant local restrictions](https://covid19.ca.gov/safer-economy) and must comply with all applicable attendance limitations and guidance requirements.\n\nLocal Health Officers are advised to consider appropriate limitations on _outdoor_ attendance capacities, factoring their jurisdiction’s key COVID-19 health indicators. At a minimum, outdoor attendance should be limited naturally through implementation of strict physical distancing measures of a minimum of 6 feet between attendees from different households, in addition to other relevant protocols within this document.\n\nThis limitation will be regularly reviewed by the California Department of Public Health.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Small businesses with 500 employees or less are eligible to apply for the Small Business Debt Relief Program. Small businesses are also eligible to apply for the Economic Injury Disaster Loan (EIDL) program. Visit SBA’s comprehensive [COVID-19 support website](https://www.sba.gov/page/coronavirus-covid-19-small-business-guidance-loan-resources#section-header-4%20.) to find out more about SBA’s eligibility requirements for each program.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C23" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D23" t="str">
         <v xml:space="preserve"> </v>
@@ -980,13 +980,13 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>Can children attend group activities (like Sunday school or Hebrew school) at places of worship?</v>
+        <v>How do I reach SBA for any questions or assistance?</v>
       </c>
       <c r="B24" t="str">
-        <v>Yes.  Outdoor activities are permitted, and indoor activities are permitted if they comply with the [cohort guidance](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/small-groups-child-youth.aspx).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>SBA has district offices in California that are open to answer questions. You can use the [SBA’s Local Assistance Directory](https://www.sba.gov/local-assistance) to locate the office nearest you. You can also contact the SBA by phone at [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or by email at [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).  \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C24" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D24" t="str">
         <v xml:space="preserve"> </v>
@@ -1006,13 +1006,13 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>When will current conditions change for places of worship?</v>
+        <v>How does a small business know which SBA loan or loan guarantee program is the right one? Can a small business apply to more than one?</v>
       </c>
       <c r="B25" t="str">
-        <v>The California Department of Public Health, in consultation with county Departments of Public Health, will regularly review and assess the impacts of these imposed limits on public health and provide further direction as part of a phased-in restoration of activities in places of worship.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Call or email the SBA to find out which program is right for you. While businesses can apply for and receive more than one form of capital assistance through the SBA, they cannot be used for the same purpose. The SBA can advise you on your options. Call [1-800-659-2955](tel:1-800-659-2955) / [1-800-877-8339](tel:1-800-877-8339) (TTY), or email [disastercustomerservice@sba.gov](mailto:disastercustomerservice@sba.gov).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C25" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D25" t="str">
         <v xml:space="preserve"> </v>
@@ -1032,13 +1032,13 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Can I still exercise? Take my kids to the park for fresh air? Take a walk around the block?</v>
+        <v>How do I get SBA to cover my loan payments on my existing 7(a), 504, or microloan if I cannot pay due to COVID-19?</v>
       </c>
       <c r="B26" t="str">
-        <v>It’s okay to go outside to go for a walk, to exercise, and participate in healthy activities as long as you **maintain a safe physical distance of 6 feet and gather only with members of your household.** You can also participate in activities at [outdoor recreational facilities](https://files.covid19.ca.gov/pdf/guidance-campgrounds-outdoor-recreation--en.pdf) that are allowed to open. [Parks may be closed](https://covid19.ca.gov/public-recreation/) to help slow the spread of the virus. Young people can participate in sports as permitted by the [youth sports guidance (PDF)](https://files.covid19.ca.gov/pdf/guidance-youth-sports--en.pdf). Check with local officials about park closures in your area. Californians should not travel significant distances for recreation and should stay close to home.\n\nBelow is a list of some outdoor recreational activities.\n\n*   Badminton (singles)\n*   Throwing a baseball/softball\n*   BMX biking\n*   Canoeing (singles)\n*   Crabbing\n*   Cycling\n*   Exploring rock pools\n*   Gardening (not in groups)\n*   Golfing (doubles, only if cart has protective partition)\n*   Hiking (trails/ paths allowing distancing)\n*   Horse riding (singles)\n*   Jogging and running\n*   Kite boarding and kitesurfing\n*   Meditation\n*   Outdoor photography\n*   Picnics (with your household members only)\n*   Quad biking\n*   Rock climbing\n*   Roller skating and rollerblading\n*   Rowing (singles)\n*   Scootering (not in groups)\n*   Skateboarding (not in groups)\n*   Soft martial arts – tai chi, chi kung (not in groups)\n*   Surfing\n*   Tennis and table tennis (singles)\n*   Throwing a football, kicking a soccer ball (not in groups)\n*   Trail running\n*   Trampolining\n*   Tree climbing\n*   Volleyball (singles)\n*   Walk the dog\n*   Wash the car\n*   Watch the sunrise or sunset\n*   Yoga\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>SBA has a [Debt Relief program](https://www.sba.gov/funding-programs/loans/coronavirus-relief-options/sba-debt-relief) and will pay the principal and interest of existing SBA loans. Please contact your lender for information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C26" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D26" t="str">
         <v xml:space="preserve"> </v>
@@ -1058,13 +1058,13 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>Can I walk my dog? Take my pet to the vet?</v>
+        <v>If I need help to figure out which program is best for me or to submit an application, where can I find support?</v>
       </c>
       <c r="B27" t="str">
-        <v>You can walk your dog. You can go to the vet or pet hospital if your pet is sick. Remember to wear a face covering and distance yourself at least 6 feet from other pets and owners.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>California’s network of small business support centers can help you figure out which loans and programs are best for your business, develop resiliency strategies, and find other resources. Go to California’s [small business centers](https://business.ca.gov/advantages/small-business-innovation-and-entrepreneurship/how-we-can-help/covid-19-resources-map/) to find the closest center.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C27" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D27" t="str">
         <v xml:space="preserve"> </v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>Can I visit State Parks? What outdoor spaces are open?</v>
+        <v>How do I maintain a safe workplace?</v>
       </c>
       <c r="B28" t="str">
-        <v>State Parks, campgrounds, museums, and visitor centers [may continue to be closed](https://www.parks.ca.gov/?page_id=30350) to help slow the spread of the virus. Starting June 12, some counties may open campgrounds and RV parks. Be sure to check [parks in your area before you travel](https://covid19.ca.gov/public-recreation/). Californians should not travel significant distances for pleasure or recreation and should stay close to home. If you do travel, take steps to keep everyone safe like wearing a face covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently.\n\nYou can walk, run, hike and bike in your local neighborhoods as long as they continue to practice physical distancing of 6 feet. This means avoiding crowded trails and parking lots.\n\n\--&gt;\n\n#### Can I travel?\n\nYou can travel for urgent matters or if such travel is essential to your permitted work. Even though businesses around the state are opening up, avoid travelling long distances for vacations or pleasure as much as possible. This is to slow the spread of the coronavirus. Do not travel if you are sick, or if someone in your household has had coronavirus in the last two weeks. Do not travel with someone who is sick.\n\nYou should check with the local health department where you are starting from, along your route, and at your planned destination for information. Know that local rules are constantly changing and may change even after you start your trip. [Check for travel updates](https://www.visitcalifornia.com/latest-covid-19-coronavirus) before you leave your home.\n\nBefore travelling away from your community, consider these questions from the [Center for Disease Control (CDC) travel guidance](https://www.cdc.gov/coronavirus/2019-ncov/travelers/travel-in-the-us.html):\n\n*   Is coronavirus spreading where you are traveling?\n*   Are you or those you are traveling with more likely to get very sick from coronavirus?\n*   Will you be able to keep 6 feet of physical distance from others during or after your trip?\n\nIf you do travel, take steps to keep everyone safe like wearing a face covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently. \n\n#### Are there travel restrictions within California?\n\nTo prevent further spread of COVID-19, Californians should not travel significant distances and should stay close to home as much as possible.\n\n#### Are there travel restrictions into or out of California?\n\nThere are currently no restrictions for entering California if you are coming from another state in the U.S. The federal government has placed restrictions on certain international travelers. With specific exceptions, foreign nationals who visited certain countries during the past 14 days are prohibited from entry to the United States. All international travelers, including US citizens and permanent residents, should quarantine for 14 days after coming to California from any other country. All travelers should take safety precautions when considering traveling.·       \n\n*   Don’t travel if you have been sick in the past 14 days or if you live with someone with COVID-19·        \n*   Don’t travel with someone who is sick\n*   Wear a mask in public\n*   Wash your hands\n*   Keep 6 feet from anyone you don’t live with\n\n#### Are swimming pools open?\n\nOutdoor swimming pools are allowed to open in all counties in California. Outdoor pools must close slides, rides, or other attractions. \n\nIndoor swimming pools are closed in counties in the [Widespread (purple) or Substantial (red) tiers](https://covid19.ca.gov/safer-economy).\n\nWater parks, both indoor and outdoor, remain closed throughout the state.\n\nWhen out of the water, masks or face coverings should be worn. Physical distancing should be practiced at all times. Group gatherings are not allowed. Bring your own towel, and don’t share items that are worn on the face (like goggles, nose clips, or snorkels). Pool operators should follow heightened cleaning and safety guidance in response to COVID-19. See sector guidance for [gyms and fitness centers](https://files.covid19.ca.gov/pdf/guidance-fitness--en.pdf) and [campgrounds and outdoor recreation](https://files.covid19.ca.gov/pdf/guidance-campgrounds-outdoor-recreation--en.pdf).\n\n### Government services\n\n#### Can I go to the Department of Motor Vehicles (DMV)?\n\nYes, but first check if an in-person visit is required. Several deadlines have been extended, and many DMV services can be accessed online.\n\n##### **Extended deadlines**\n\nDMV has extended deadlines for:\n\n*   Drivers 70 years of age and older with licenses expiring between March 1 through December 31, 2020. Your license is valid for one year from the original expiration date.\n*   Drivers 69 years of age and younger with licenses expiring between March 1 through July 31, 2020. Though the extension has now expired, you can [renew your license online.](https://www.dmv.ca.gov/portal/driver-licenses-identification-cards/driver-license-id-card-online-renewal/) An in-person visit is not required.\n*   Expiring commercial licenses, endorsements, and certificates. They are valid through September 30, 2020.\n*   In-person renewals for vehicle registrations that expire between the dates of March 16, 2020, and May 31, 2020.\n*   In-person renewals for those with safe driving records whose last DMV visit was 15 years ago.\n*   Driver license permits expiring between March and November 2020. They are extended six months or to a date 24 months from the date of application, whichever is earlier.\n*   Commercial learner’s permits expiring between March and September 2020. They are now valid through September 30, 2020.\n\n##### Online services\n\nDMV offers many services that can be handled online, including simple vehicle registration, renewing a driver’s license, getting a duplicate license, and more. See:\n\n*   [DMV Online Services](https://www.dmv.ca.gov/portal/dmv-online/)\n\nSome DMV services that used to require an in-person office visit can now be accessed online, including driver’s license renewals, vehicle registrations, title transfers, temporary driver’s license extensions, commercial driver’s license renewals, and more. See:\n\n*   [DMV Virtual Field Office](https://virtual.dmv.ca.gov/)\n\n##### **In-person visits**\n\nBeginning June 11, [all DMV offices](https://www.dmv.ca.gov/portal/news-and-media/dmv-reopens-remaining-field-offices-to-public/) are open to the public for appointments that require an in-person visit. You will be required to wear a mask and must remain 6 feet apart in line.\n\nIn-person appointments are limited to:\n\n*   Paying registration for a vehicle impounded because of registration-related issues\n*   Reinstating a suspended or revoked driver license\n*   Applying for a reduced-fee or no-fee identification card\n*   Processing commercial driver license transactions\n*   Applying for a disabled person parking placards\n*   Adding an ambulance certificate or firefighter endorsement to a driver license\n*   Verifying a transit training document to drive a transit bus\n*   Processing DMV Express customers for REAL ID transactions, if time and space allows\n*   Behind-the-wheel driving tests\n    *   On June 26, the DMV began behind-the-wheel driving tests. All cancelled driving test appointments will be rescheduled. New tests will not be available until all cancelled appointments are completed. \n    *   For the health and safety of drivers and DMV staff, [you must wear a face covering and will have your temperature checked](https://www.dmv.ca.gov/portal/dmv-expands-its-health-screening-and-temperature-check-protocols-to-protect-customers-and-employees/) before the test.\n\n#### Can I get my car smog checked?\n\nIt depends. Some smog check locations may be closed. The [Bureau of Automotive Repair](https://www.bar.ca.gov/COVID-19_Impacts_on_BAR_Programs_and_Services.aspx) advises drivers to still pay DMV vehicle registration fees to avoid any late fees. However, you will not receive your new registration or year sticker until the smog information has been received by DMV. Once state and local orders or directives are no longer in effect, you can then obtain the required smog check certificate to complete the DMV vehicle registration process.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- park, visitor center, travel, museum, RV parks, recreation, outdoor recreation, sports, RV, tent camping, tent camp, fish, beach, lake, river, event, outdoor event, event planning, hike, walk, bike, exercise, nature, bird watching, public →&lt;/p&gt;&lt;p&gt;For information on National Parks, please the &lt;a href="https://www.nps.gov/aboutus/news/public-health-update.htm"&gt;National Park Service website&lt;/a&gt;.&lt;!-- park, visitor center, travel, museum, RV parks, recreation, outdoor recreation, sports, RV, tent camping, tent camp, fish, beach, lake, river, event, outdoor event, event planning, hike, walk, bike, exercise, nature, bird watching, public →&lt;/p&gt;      &lt;/div&gt;    &lt;/div&gt;  &lt;/div&gt;&lt;/cwds-accordion&gt;--&gt;</v>
+        <v>As California reopens, every business will need to create a safer, low-risk environment. If you own or manage a business, follow the [industry-specific guidance](https://covid19.ca.gov/industry-guidance/) that applies to protect your workers and customers.\n\nIf your business is approved to reopen, you should take steps to ensure the safety and health of your workers. It’s important that employees with COVID-19 know they should stay home. Your sick leave policies need to support that. \n\n*   Encourage sick employees to stay home if they are sick. See government programs supporting [COVID-19 sick leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) and [workers’ compensation](https://www.labor.ca.gov/coronavirus2019/#chart).\n*   Establish routine cleaning throughout the workplace.\n*   Reduce travel. If possible, encourage video conferencing and limit larger gatherings.\n*   See [Cal/OSHA interim guidelines for general industry](https://www.dir.ca.gov/dosh/coronavirus/General-Industry.html).\n*   Follow [CDC guidance on keeping the workplace safe (PDF)](https://www.cdc.gov/coronavirus/2019-ncov/downloads/workplace-school-and-home-guidance.pdf).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C28" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D28" t="str">
         <v xml:space="preserve"> </v>
@@ -1110,13 +1110,13 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>Can I travel?</v>
+        <v>Should a business owner notify customers if an employee has been exposed to COVID-19?</v>
       </c>
       <c r="B29" t="str">
-        <v>You can travel for urgent matters or if such travel is essential to your permitted work. Even though businesses around the state are opening up, avoid travelling long distances for vacations or pleasure as much as possible. This is to slow the spread of the coronavirus. Do not travel if you are sick, or if someone in your household has had coronavirus in the last two weeks. Do not travel with someone who is sick.\n\nYou should check with the local health department where you are starting from, along your route, and at your planned destination for information. Know that local rules are constantly changing and may change even after you start your trip. [Check for travel updates](https://www.visitcalifornia.com/latest-covid-19-coronavirus) before you leave your home.\n\nBefore travelling away from your community, consider these questions from the [Center for Disease Control (CDC) travel guidance](https://www.cdc.gov/coronavirus/2019-ncov/travelers/travel-in-the-us.html):\n\n*   Is coronavirus spreading where you are traveling?\n*   Are you or those you are traveling with more likely to get very sick from coronavirus?\n*   Will you be able to keep 6 feet of physical distance from others during or after your trip?\n\nIf you do travel, take steps to keep everyone safe like wearing a face covering, keeping 6 feet of physical distance from those not in your household, and washing your hands frequently.  \n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)&lt;!-- wedding, travel, gathering, tourism, funeral, motel, vacation, airbnb, vrbo, rental home --&gt;</v>
+        <v>The business owner isn’t required to notify customers if an employee was exposed to COVID-19. The local health department will use contact tracing to notify those who were in close contact with the COVID-19 positive worker.\n\nWhen an employer discovers a worker who has tested positive or has symptoms of COVID-19, the employer should:\n\n*   make sure the worker does not remain at work, and\n*   work with the local health department to support isolation or quarantine, testing, and about when the worker may return to work. \n\nEmployers must follow the [Employer playbook](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf) which includes detailed information on:\n\n*   When and how an employer must report a COVID-19 positive employee.\n*   What is defined as an outbreak.\n*   Notifying all workers who may have been exposed to the worker with COVID-19. This is especially important for those with high-risk medical conditions (e.g., immune compromise or pregnancy).\n*   Guidance for employers who may be considering whether to suspend operations due to COVID-19 spread in the workplace.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C29" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D29" t="str">
         <v xml:space="preserve"> </v>
@@ -1136,13 +1136,13 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>Are there travel restrictions within California?</v>
+        <v>What precautions should healthcare workers and organizations take?</v>
       </c>
       <c r="B30" t="str">
-        <v>To prevent further spread of COVID-19, Californians should not travel significant distances and should stay close to home as much as possible.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>See [Cal/OSHA’s guidance on protecting workers from coronavirus](https://www.dir.ca.gov/dosh/coronavirus/Health-Care-General-Industry.html).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
       </c>
       <c r="C30" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D30" t="str">
         <v xml:space="preserve"> </v>
@@ -1162,13 +1162,13 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>Are there travel restrictions into or out of California?</v>
+        <v>How can I avoid laying off employees if my business is impacted by COVID-19?</v>
       </c>
       <c r="B31" t="str">
-        <v>There are currently no restrictions for entering California if you are coming from another state in the U.S. The federal government has placed restrictions on certain international travelers. With specific exceptions, foreign nationals who visited certain countries during the past 14 days are prohibited from entry to the United States. All international travelers, including US citizens and permanent residents, should quarantine for 14 days after coming to California from any other country. All travelers should take safety precautions when considering traveling.·       \n\n*   Don’t travel if you have been sick in the past 14 days or if you live with someone with COVID-19·        \n*   Don’t travel with someone who is sick\n*   Wear a mask in public\n*   Wash your hands\n*   Keep 6 feet from anyone you don’t live with\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Apply for the [Unemployment Insurance (UI) Work Sharing Program](https://www.edd.ca.gov/Unemployment/Work_Sharing_Program.htm).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)&lt;!-- workshare, furlough, reduce hours --&gt;</v>
       </c>
       <c r="C31" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/business-and-employers/</v>
       </c>
       <c r="D31" t="str">
         <v xml:space="preserve"> </v>
@@ -1188,13 +1188,13 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>Are swimming pools open?</v>
+        <v>What if a provider says they have availability on MyChildCare.ca.gov but when I connect with them they have no space?</v>
       </c>
       <c r="B32" t="str">
-        <v>Outdoor swimming pools are allowed to open in all counties in California. Outdoor pools must close slides, rides, or other attractions. \n\nIndoor swimming pools are closed in counties in the [Widespread (purple) or Substantial (red) tiers](https://covid19.ca.gov/safer-economy).\n\nWater parks, both indoor and outdoor, remain closed throughout the state.\n\nWhen out of the water, masks or face coverings should be worn. Physical distancing should be practiced at all times. Group gatherings are not allowed. Bring your own towel, and don’t share items that are worn on the face (like goggles, nose clips, or snorkels). Pool operators should follow heightened cleaning and safety guidance in response to COVID-19. See sector guidance for [gyms and fitness centers](https://files.covid19.ca.gov/pdf/guidance-fitness--en.pdf) and [campgrounds and outdoor recreation](https://files.covid19.ca.gov/pdf/guidance-campgrounds-outdoor-recreation--en.pdf).\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>The information on [MyChildCare.ca.gov](http://mychildcare.ca.gov/) will be updated twice each week but it is possible that vacancies are filled between updates. Contact your [local childcare resource and referral agency](http://rrnetwork.org/family-services/find-child-care) to find more vacancies. \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
       </c>
       <c r="C32" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/childcare/</v>
       </c>
       <c r="D32" t="str">
         <v xml:space="preserve"> </v>
@@ -1214,13 +1214,13 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>Can I go to the Department of Motor Vehicles (DMV)?</v>
+        <v>How can I find out more about the provider listed in MyChildCare.ca.gov?</v>
       </c>
       <c r="B33" t="str">
-        <v>Yes, but first check if an in-person visit is required. Several deadlines have been extended, and many DMV services can be accessed online.\n\n##### **Extended deadlines**\n\nDMV has extended deadlines for:\n\n*   Drivers 70 years of age and older with licenses expiring between March 1 through December 31, 2020. Your license is valid for one year from the original expiration date.\n*   Drivers 69 years of age and younger with licenses expiring between March 1 through July 31, 2020. Though the extension has now expired, you can [renew your license online.](https://www.dmv.ca.gov/portal/driver-licenses-identification-cards/driver-license-id-card-online-renewal/) An in-person visit is not required.\n*   Expiring commercial licenses, endorsements, and certificates. They are valid through September 30, 2020.\n*   In-person renewals for vehicle registrations that expire between the dates of March 16, 2020, and May 31, 2020.\n*   In-person renewals for those with safe driving records whose last DMV visit was 15 years ago.\n*   Driver license permits expiring between March and November 2020. They are extended six months or to a date 24 months from the date of application, whichever is earlier.\n*   Commercial learner’s permits expiring between March and September 2020. They are now valid through September 30, 2020.\n\n##### Online services\n\nDMV offers many services that can be handled online, including simple vehicle registration, renewing a driver’s license, getting a duplicate license, and more. See:\n\n*   [DMV Online Services](https://www.dmv.ca.gov/portal/dmv-online/)\n\nSome DMV services that used to require an in-person office visit can now be accessed online, including driver’s license renewals, vehicle registrations, title transfers, temporary driver’s license extensions, commercial driver’s license renewals, and more. See:\n\n*   [DMV Virtual Field Office](https://virtual.dmv.ca.gov/)\n\n##### **In-person visits**\n\nBeginning June 11, [all DMV offices](https://www.dmv.ca.gov/portal/news-and-media/dmv-reopens-remaining-field-offices-to-public/) are open to the public for appointments that require an in-person visit. You will be required to wear a mask and must remain 6 feet apart in line.\n\nIn-person appointments are limited to:\n\n*   Paying registration for a vehicle impounded because of registration-related issues\n*   Reinstating a suspended or revoked driver license\n*   Applying for a reduced-fee or no-fee identification card\n*   Processing commercial driver license transactions\n*   Applying for a disabled person parking placards\n*   Adding an ambulance certificate or firefighter endorsement to a driver license\n*   Verifying a transit training document to drive a transit bus\n*   Processing DMV Express customers for REAL ID transactions, if time and space allows\n*   Behind-the-wheel driving tests\n    *   On June 26, the DMV began behind-the-wheel driving tests. All cancelled driving test appointments will be rescheduled. New tests will not be available until all cancelled appointments are completed. \n    *   For the health and safety of drivers and DMV staff, [you must wear a face covering and will have your temperature checked](https://www.dmv.ca.gov/portal/dmv-expands-its-health-screening-and-temperature-check-protocols-to-protect-customers-and-employees/) before the test.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) includes each provider’s facility/license number. This number can be searched at [CDSS Community Care Licensing Database](https://www.ccld.dss.ca.gov/carefacilitysearch/) to find more information about the provider, like information on inspections and complaints.  \n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)</v>
       </c>
       <c r="C33" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/childcare/</v>
       </c>
       <c r="D33" t="str">
         <v xml:space="preserve"> </v>
@@ -1240,13 +1240,13 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>Can I get my car smog checked?</v>
+        <v>How can I find help paying for childcare?</v>
       </c>
       <c r="B34" t="str">
-        <v>It depends. Some smog check locations may be closed. The [Bureau of Automotive Repair](https://www.bar.ca.gov/COVID-19_Impacts_on_BAR_Programs_and_Services.aspx) advises drivers to still pay DMV vehicle registration fees to avoid any late fees. However, you will not receive your new registration or year sticker until the smog information has been received by DMV. Once state and local orders or directives are no longer in effect, you can then obtain the required smog check certificate to complete the DMV vehicle registration process.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>[MyChildCare.ca.gov](http://mychildcare.ca.gov/) provides information on all licensed center-based and family childcare homes. This includes both private-pay and subsidized childcare. Children of essential workers are now eligible to enroll in subsidized emergency childcare through June 30, 2020, or 60 calendar days after the date of the child’s enrollment, whichever is longer. This is subject to capacity and eligibility requirements. Your [local childcare resource and referral agency](https://rrnetwork.org/index.php?p=family-services/find-child-care) can answer more questions about childcare subsidies.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
       </c>
       <c r="C34" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/childcare/</v>
       </c>
       <c r="D34" t="str">
         <v xml:space="preserve"> </v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>Can my pet test positive for coronavirus? Can I take my pet to the vet?</v>
+        <v>Can I get childcare during the stay home order?</v>
       </c>
       <c r="B35" t="str">
-        <v>While we are still learning about coronavirus, the risk of your pet testing positive for coronavirus is low. Because [there is still a risk](https://www.cdc.gov/coronavirus/2019-ncov/animals/pets-other-animals.html), keep your pets away from other pets and people outside of your household. Do not put face coverings on pets as this could harm your pet.\n\nYou can go to the vet or pet hospital if your pet is sick. Remember to wear a cloth face covering and to distance yourself at least 6 feet from other pets and owners.\n\nMore info: [Stay home Q&amp;A](https://covid19.ca.gov/stay-home-except-for-essential-needs/)</v>
+        <v>Yes, all childcare facilities can open with necessary modifications.\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
       </c>
       <c r="C35" t="str">
-        <v>https://covid19.ca.gov/stay-home-except-for-essential-needs/</v>
+        <v>https://covid19.ca.gov/childcare/</v>
       </c>
       <c r="D35" t="str">
         <v xml:space="preserve"> </v>
@@ -1292,13 +1292,13 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>What if I don’t have health insurance and I need COVID-19 diagnosis, testing or treatment?</v>
+        <v>Can my babysitter still come to the house?</v>
       </c>
       <c r="B36" t="str">
-        <v>The cost of needed COVID-19 diagnosis, testing and treatment for the uninsured is [paid for by the government](https://www.hrsa.gov/CovidUninsuredClaim). Check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by talking to your doctor. Medically necessary [testing](https://covid19.ca.gov/testing-and-treatment/) is also free through Verily’s Project Baseline or OptumServe\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes, a childcare worker can come to your home if necessary and should practice basic prevention guidelines (like handwashing for at least 20 seconds, physical distancing, and staying home if feeling ill).\n\nMore info: [Find childcare options near you](https://covid19.ca.gov/childcare/)&lt;!-- child care, childcare, daycare, day care --&gt;</v>
       </c>
       <c r="C36" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/childcare/</v>
       </c>
       <c r="D36" t="str">
         <v xml:space="preserve"> </v>
@@ -1318,13 +1318,13 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>Does my health plan have to cover my COVID-19 test?</v>
+        <v>What is a close contact?</v>
       </c>
       <c r="B37" t="str">
-        <v>Yes, if you:\n\n*   Have COVID-19 symptoms,\n*   Were exposed to someone who has COVID-19, or\n*   The test is medically necessary for your situation. \n\nIf you have COVID-19 symptoms or think you’ve been exposed, under federal law, you can get a test anywhere and your health plan must pay for it.\n\nIf you are an [essential worker](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf), your health plan must cover your COVID-19 test. But you must contact your health plan before getting tested. \n\nIf none of these things above are true but you’d still like a test, contact your health plan or health care provider.\n\nAs a first step, you can check your symptoms using the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html) or by contacting your doctor.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>A [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) is someone who was within 6 feet of a person with COVID-19 for at least 15 minutes starting from 2 days before symptoms appeared (or, for asymptomatic patients, 2 days prior to their test) until the time the patient is isolated. This usually includes household members, intimate contacts, and caregivers, but can include others.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C37" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D37" t="str">
         <v xml:space="preserve"> </v>
@@ -1344,13 +1344,13 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>How long will I have to wait to get a coronavirus test?</v>
+        <v>Will contact tracers track my location?</v>
       </c>
       <c r="B38" t="str">
-        <v>Your wait time depends on why you are seeking a test. \n\n**If you have COVID-19 symptoms or think you were exposed,** under federal law, you can go immediately to any testing site. Find a testing site on our [Testing page](https://covid19.ca.gov/testing-and-treatment/#top), or call your health plan for an available testing location.\n\n**If you are an [essential worker](https://www.dmhc.ca.gov/Portals/0/Docs/DO/DMHC-FAQForHealthCoverageOfCOVID-19Testing.pdf),** your health plan must offer you a test appointment within 48 hours. The testing site must be within 15 miles or 30 minutes of your home or workplace. If your health plan can’t find you such an appointment, then you can go to any available testing site. Your health plan will pay for the test. \n\n**If neither of these cases above are true,** your provider may still decide that a COVID-19 test is medically necessary for you. In that case, your health plan must offer you a test appointment within 96 hours. The testing site must be within 15 miles or 30 minutes of your home or workplace. If your health plan can’t find you such an appointment, then you can go to any available testing site.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>California’s contact tracing program does not use any cell phone tracking technology. Someone from your local public health department will simply speak privately with you. All information is confidential and protected by California’s strict privacy laws. They may stay in touch to make sure your symptoms aren’t worsening.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C38" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D38" t="str">
         <v xml:space="preserve"> </v>
@@ -1370,13 +1370,13 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>I get my health care coverage through my employer, who has a “self-insured” plan. Do the California Department of Managed Health Care (DMHC) regulations apply to me?</v>
+        <v>Is contact tracing help available in my language?</v>
       </c>
       <c r="B39" t="str">
-        <v>Self-insured plans are regulated by the federal government, not the state. If you have COVID-19 symptoms or were exposed to someone with symptoms, under federal law, your self-insured plan must cover your test. In all other instances, you should talk to your plan to find out whether they will cover COVID-19 testing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Your [local health department](https://covid19.ca.gov/get-local-information/) can communicate with you in many different languages.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C39" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D39" t="str">
         <v xml:space="preserve"> </v>
@@ -1396,13 +1396,13 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>How does my health plan know if I’m an essential worker?</v>
+        <v>Who should get tested for coronavirus?</v>
       </c>
       <c r="B40" t="str">
-        <v>Your health plan can ask you questions about why you want a COVID-19 test and about the nature of your work. This helps them determine whether a COVID-19 test is medically necessary for you.\n\nBut they can’t ask you to provide further documentation or evidence of your work status. For example, they can’t ask you to provide written proof of where you work or the conditions of your workplace.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>You should get tested if you:\n\n*   Had [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) with anyone who has tested positive for COVID-19\n*   Have COVID-19 symptoms\n*   Get a call from a contact tracer\n*   Are at [high risk](https://www.cdph.ca.gov/Programs/CID/DCDC/Pages/COVID-19/Updated-COVID-19-Testing-Guidance.aspx)\n\nFind a [testing site in your area](https://covid19.ca.gov/testing-and-treatment/).\n\nIf you think you may have been exposed, call your doctor.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C40" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D40" t="str">
         <v xml:space="preserve"> </v>
@@ -1422,13 +1422,13 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>I have a concern or complaint about getting care for COVID-19 under my health insurance. What can I do?</v>
+        <v>How do I find a coronavirus testing location?</v>
       </c>
       <c r="B41" t="str">
-        <v>If you can’t access care, or were charged in error, follow up with your health plan. Call the member phone number listed on your health plan card. If they don’t fix the problem, call the [California Department of Managed Health Care (DMHC)](http://www.dmhc.ca.gov/?referral=healthhelp.ca.gov) Help Center at [1-888-466-2219](tel:888-466-2219).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>To learn more about testing and care, visit the [Testing and treatment page](https://covid19.ca.gov/testing-and-treatment/). You can search for testing locations there using your zip code. \n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C41" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D41" t="str">
         <v xml:space="preserve"> </v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>Do Medicare or Medicare Advantage Plans cover coronavirus tests or coronavirus antibody tests?</v>
+        <v>What if I have COVID-19 symptoms and have not been contacted by the health department?</v>
       </c>
       <c r="B42" t="str">
-        <v>Yes. Both [Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) cover [diagnostic](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test), with no out-of-pocket costs.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>[Get tested](https://covid19.ca.gov/testing-and-treatment/) immediately. Contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing, and [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) yourself until:\n\n*   at least 10 days have passed since symptoms started, **AND**\n*   your fever has been gone for 24 hours without the aid of medication, **AND** \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested. Read more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C42" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D42" t="str">
         <v xml:space="preserve"> </v>
@@ -1474,13 +1474,13 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>Can I use telehealth if I am on Medicare?</v>
+        <v>What if I came in contact with someone who has COVID-19 symptoms, but my local health department is not aware of it?</v>
       </c>
       <c r="B43" t="str">
-        <v>Yes. Medicare has expanded its [telehealth services](https://www.medicare.gov/coverage/telehealth) to respond to the public health emergency. You can now use your smartphone, video chat, or online portal from home to talk with a range of providers, like doctors, nurse practitioners, clinical psychologists, licensed clinical social workers, physical therapists, occupational therapists, and speech language pathologists. If you have original Medicare, you can get many services for free through [telehealth](https://covid19.ca.gov/telehealth/). This includes common office visits, mental health counseling, and preventive health screenings.\n\nIf you have a [Medicare Advantage Plan](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans), you have access to these same benefits. Many plans offer more [telehealth](https://covid19.ca.gov/telehealth/) and other benefits, like meal delivery or medical transport. Check with your plan about coverage and costs.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>You should [get tested](https://covid19.ca.gov/testing-and-treatment/). Contact your [local health department](https://covid19.ca.gov/get-local-information/) for contact tracing. [Quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) yourself while waiting for your test results.\n\n**If you tested positive but have no symptoms**, you should [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) at home for at least 10 days.\n\n**If you develop symptoms**, you should stay home until:\n\n*   at least 10 days have passed since symptoms started, **AND**\n*   your fever has been gone for 24 hours without the aid of medication, **AND** \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested.\n\n**If you had [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) with someone who tested positive but you tested negative**, you should still [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) at home for at least 14 days.\n\nRead more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C43" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D43" t="str">
         <v xml:space="preserve"> </v>
@@ -1500,13 +1500,13 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>I am uninsured and diagnosed with COVID-19. What testing and treatment for me are paid for by the federal government?</v>
+        <v>How do I become a contact tracer?</v>
       </c>
       <c r="B44" t="str">
-        <v>The following services are covered:\n\n*   Specimen collection, diagnostic and antibody testing\n*   Testing-related visits, including in the following settings: \n    *   Office \n    *   Urgent care \n    *   Emergency room, or \n    *   Telehealth\n*   Treatment, including:\n    *   Office visit\n    *   [Telehealth](https://covid19.ca.gov/telehealth/#top)\n    *   Emergency room \n    *   Inpatient \n    *   Outpatient/observation \n    *   Skilled nursing facility \n    *   Long-term acute care (LTAC) \n    *   Acute inpatient rehab \n    *   Home health \n    *   Durable Medical Equipment (DME), like oxygen and ventilator\n    *   Emergency ambulance transportation \n    *   Non-emergent patient transfers via ambulance, and\n    *   FDA-approved drugs administered as part of an inpatient stay\n    *   FDA-approved vaccine, when available\n\nFor more details, see the [HRSA website](https://www.hrsa.gov/CovidUninsuredClaim) and their [frequently asked questions](https://www.hrsa.gov/coviduninsuredclaim/frequently-asked-questions).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>California Connected is using existing state employees for contact tracing. We appreciate offers of additional support from the private sector and qualified members of the public, but they are not needed at this time.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C44" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D44" t="str">
         <v xml:space="preserve"> </v>
@@ -1526,13 +1526,13 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>Does Medi-Cal provide free COVID-19 diagnosis, testing and treatments for the uninsured?</v>
+        <v>Is there extra sick leave available for workers who have COVID-19 symptoms or are waiting for test results?</v>
       </c>
       <c r="B45" t="str">
-        <v>Yes. [Medi-Cal is available](https://www.dhcs.ca.gov/services/medi-cal/eligibility/Pages/COVID-19-Presumptive-Eligibility-Program.aspx#:~:text=Presumptive%20Eligibility%20(PE)%20for%20COVID,associated%20office%2C%20clinic%2C%20or%20emergency) to those with no insurance or whose insurance does not cover COVID-19 diagnosis, testing, and treatment. COVID-19 diagnosis, testing and treatment are considered emergency services. This allows all Medi-Cal beneficiaries, regardless of their scope of coverage under Medi-Cal or their immigration status, to receive at no cost all medically necessary testing, testing-related, and treatment services, which may include inpatient or outpatient services related to a COVID-19 diagnosis.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes. There are extra federal, state, and in some cases, local sick leaves available for workers in this situation:\n\n*   **Federal paid sick leave:** Up to 80 hours under the Families First Coronavirus Response Act ([FFCRA](https://www.dol.gov/agencies/whd/pandemic/ffcra-employee-paid-leave)) for businesses with less than 500 workers. See [more information on FFCRA in its FAQs](https://www.dol.gov/agencies/whd/pandemic/ffcra-questions).\n*   **California COVID-19 supplemental paid sick leave:** Food businesses, healthcare providers, and emergency responders with more than 500 workers must give up to 80 hours of [paid sick leave](https://leginfo.legislature.ca.gov/faces/billTextClient.xhtml?bill_id=201920200AB1867).\n*   **Local paid sick leave ordinances:** Certain local areas also have paid sick leave ordinances.  Consult with the local enforcement agency in your area.\n\nTo understand what may be available, see the comparison of [COVID-19 sick leave](https://www.dir.ca.gov/dlse/Comparison-COVID-19-Paid-Leave.html) and [benefits for workers impacted by COVID-19](https://www.labor.ca.gov/coronavirus2019/#chart).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C45" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D45" t="str">
         <v xml:space="preserve"> </v>
@@ -1552,13 +1552,13 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>My Medi-Cal eligibility is expiring. Do I need to renew it now?</v>
+        <v>Can I return to work once my isolation or quarantine is over?</v>
       </c>
       <c r="B46" t="str">
-        <v>**No.** [DHCS instructed counties](https://www.dhcs.ca.gov/services/medi-cal/eligibility/letters/Documents/I20-14.pdf) to freeze the Medi-Cal eligibility redeterminations for the duration of the COVID-19 public health emergency.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Yes, but when you return depends on your situation.\n\n**If you have symptoms**, you should stay home until:\n\n*   at least 10 days have passed since symptoms started, **AND**\n*    your fever has been gone for 24 hours without the aid of medication, **AND** \n*   your [symptoms](https://covid19.ca.gov/symptoms-and-risks/#top) (like cough and shortness of breath) have improved.\n\nThis is true whether you’ve tested positive, negative, or are untested.\n\n**If you have tested positive but have no symptoms**, you should [isolate](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/isolation.html) at home for at least 10 days.\n\n**If you had [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) with someone who tested positive but you have tested negative**, you should still [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) at home for at least 14 days.\n\nGet tested as soon as possible if you have symptoms, or have come in contact with someone who has tested positive or has symptoms.\n\nRead more in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf).\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C46" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D46" t="str">
         <v xml:space="preserve"> </v>
@@ -1578,13 +1578,13 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>I don’t have health insurance and/or a regular doctor. How can I get quick access to medical advice?</v>
+        <v>What steps are required when a business has an employee who tests positive?</v>
       </c>
       <c r="B47" t="str">
-        <v>Call Medi-Nurse. Medi-Nurse is a [free, 24/7 nurse advice line](https://www.dhcs.ca.gov/Pages/DHCS-COVID%E2%80%9119-Medi-Nurse-Line.aspx) available at [1-877-409-9052](tel:877-409-9052). You can speak directly with a healthcare professional about your symptoms, get advice on testing and treatment in your area, or ask how to apply for health insurance.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>If an employer discovers a worker has tested positive for COVID-19 or has symptoms, they should send the worker home. Then [follow guidance](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf) about isolation, quarantine, testing, and when the worker should return to work. Employers should have flexible leave policies. This supports the need for workers to stay home for the protection of others. \n\nThe employer must notify the local health department about the confirmed COVID-19 workers. They must tell their:\n\n*   job titles, \n*   work areas, \n*   [close contacts](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) in the workplace, \n*   dates of symptom onset, and \n*   shifts worked while infectious.\n\nSee “What to do if there is a Case of COVID-19 in the Workplace” in the [Employer Playbook for a Safe Reopening (PDF)](https://files.covid19.ca.gov/pdf/employer-playbook-for-safe-reopening--en.pdf). \n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C47" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D47" t="str">
         <v xml:space="preserve"> </v>
@@ -1604,13 +1604,13 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>I am nervous or scared. What can I do?</v>
+        <v>Can people who recover from COVID-19 be re-infected?</v>
       </c>
       <c r="B48" t="str">
-        <v>You are not alone. The California Surgeon General released [two playbooks for managing stress](https://covid19.ca.gov/manage-stress-for-health/#top) and tips for care-givers and kids. If you feel like you need to talk to someone and want emotional support see this [list of resources](https://covid19.ca.gov/resources-for-emotional-support-and-well-being/#top).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>We don’t yet know. The duration of immunity to coronavirus infection is not yet understood. Patients infected with similar viruses are unlikely to be re-infected in the months after they recover. But we don’t yet know if  similar immune protection happens in patients with COVID-19.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C48" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D48" t="str">
         <v xml:space="preserve"> </v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>What if I need to visit a health care provider?</v>
+        <v>Who needs to quarantine?</v>
       </c>
       <c r="B49" t="str">
-        <v>If you have [coronavirus symptoms](https://covid19.ca.gov/symptoms-and-risks/#top), please contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) or use the [Symptom Screener](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fsymptoms-testing%2Findex.html).\n\nIf you have other illnesses or chronic conditions, use [telehealth](https://covid19.ca.gov/telehealth/) to get care from home.\n\nIf you need to go to the hospital, call ahead so they can prepare for your arrival. If you call [911](tel:911), tell the operator your symptoms so the ambulance provider can be ready to treat you safely.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>You should [quarantine](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) if you have had close contact with someone who has COVID-19. If you tested positive for COVID-19 in the 3 months prior to the close contact but do not currently have symptoms, you do not need to quarantine or be tested again. If you develop symptoms, you may need to quarantine and be tested again.\n\nYou have had [close contact](https://www.cdc.gov/coronavirus/2019-ncov/php/contact-tracing/contact-tracing-plan/appendix.html#contact) if:\n\n*   You were within 6 feet of someone who has COVID-19 for 15 minutes or more\n*   You provided care at home to someone who is sick with COVID-19\n*   You had direct physical contact with the person (hugging or kissing them)\n*   You shared eating or drinking utensils\n*   They sneezed, coughed, or somehow got respiratory droplets on you\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C49" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D49" t="str">
         <v xml:space="preserve"> </v>
@@ -1656,13 +1656,13 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>What about routine, elective, or non-urgent medical or dental appointments?</v>
+        <v>How do I apply for a contact tracer position?</v>
       </c>
       <c r="B50" t="str">
-        <v>Non-emergency surgeries, like organ replacements and tumor removals, can take place. Your doctor will know if your hospital has enough capacity and protective equipment. Elective procedures should be cancelled or rescheduled. If possible, health care visits should be done remotely. [Dental services and preventive dental care](https://www.cdc.gov/coronavirus/2019-ncov/hcp/dental-settings.html) may be resumed. Contact your doctor through [telehealth](https://covid19.ca.gov/telehealth/) to see what services they are providing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>California Connected is using existing state employees for contact tracing. We appreciate offers of additional support from the private sector and qualified members of the public, but they are not needed at this time.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C50" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D50" t="str">
         <v xml:space="preserve"> </v>
@@ -1682,13 +1682,13 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>Can I get my prescriptions filled?</v>
+        <v>How do I sign-up for a contact tracer position?</v>
       </c>
       <c r="B51" t="str">
-        <v>Yes. Pharmacies and medical cannabis dispensaries are open.\n\nCall your doctor to get a new prescription or adjust your existing prescriptions.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>California Connected is using existing state employees for contact tracing. We appreciate offers of additional support from the private sector and qualified members of the public, but they are not needed at this time.\n\nMore info: [Contact tracing](https://covid19.ca.gov/contact-tracing/)</v>
       </c>
       <c r="C51" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/contact-tracing/</v>
       </c>
       <c r="D51" t="str">
         <v xml:space="preserve"> </v>
@@ -1708,13 +1708,13 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>I am an older Californian who is isolating at home and I need non-urgent help. What can I do?</v>
+        <v>What action is the state taking to ensure all schools are providing meaningful instruction during the pandemic whether they are physically open or closed?</v>
       </c>
       <c r="B52" t="str">
-        <v>Call the statewide hotline for older Californians at [1-833-544-2374](tel:833-544-2374). They can help you with non-urgent medical needs, meal delivery, tracking down prescriptions, and more. The most important thing you can do is stay home for your health and wellbeing.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>*   California has made $5.3 billion in investments to support safe reopening and rigorous distance learning.\n*   Funds prioritize low-income students, English language learners, and special education students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C52" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D52" t="str">
         <v xml:space="preserve"> </v>
@@ -1734,13 +1734,13 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>How can I make sure the older Californians in my life are safe and healthy during the stay home order?</v>
+        <v>What determines whether schools are conducting in-person learning or distance learning?</v>
       </c>
       <c r="B53" t="str">
-        <v>Check in on your older neighbors and loved ones to make sure they are okay. Give them a call, text, or physically-distanced door knock. You can also teach them how to use FaceTime, Zoom, Google Duo, or Facebook video to communicate. It’s important to keep in touch with older loved ones for their mental health and safety.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>Using health data, schools can reopen for in-person instruction once their county has been in the Substantial (red) tier for at least two weeks. Schools must follow the **[Blueprint for a Safer Economy](https://covid19.ca.gov/safer-economy)** to reopen or if they have to close again.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C53" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D53" t="str">
         <v xml:space="preserve"> </v>
@@ -1760,13 +1760,13 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>Can I care for my elderly parents or friends who need help? Or a friend or family member who has disabilities?</v>
+        <v>What are the health and safety requirements for schools doing in-person learning?</v>
       </c>
       <c r="B54" t="str">
-        <v>Yes. Protect them and yourself by following physical distancing guidelines. Wear a [mask](https://covid19.ca.gov/masks-and-ppe/#top), wash your hands often, maintain at least six feet of distance between you, and cover your cough or sneeze. If you have early signs of a cold, please stay away from your older loved ones.\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>*   Everyone entering the school must do daily health checks.\n*   If someone experiences symptoms while at school, they will be sent home.\n*   Masks are required for all staff and students 3rd grade and above. Younger students should be encouraged to wear masks.\n*   Staff members must maintain 6ft distance from each other and students. Students should maintain 6ft distance as practicable.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C54" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D54" t="str">
         <v xml:space="preserve"> </v>
@@ -1786,13 +1786,13 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>Can I visit loved ones in the hospital, nursing home, or residential care facility?</v>
+        <v>What happens if someone gets COVID-19 at my child’s school?</v>
       </c>
       <c r="B55" t="str">
-        <v>Generally, no. There are exceptions, such as if you are taking a minor or someone who is developmentally disabled to the hospital. For most other situations, the order prohibits visitation to these kinds of facilities. This is difficult, but necessary to protect hospital staff and other patients. See more about this in [frequently asked questions for friends and family with a loved one in a skilled nursing or residential care facility](https://www.aging.ca.gov/download.ashx?lE0rcNUV0zaaXLD5JZ%2f6Uw%3d%3d).\n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>*   A classroom goes home when there is a confirmed case\n*   A school should switch to distance learning when there are multiple positive cases in multiple classroom cohorts\n*   A district should switch to distance learning if 25% of schools in the district are closed within a 14-day period\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C55" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D55" t="str">
         <v xml:space="preserve"> </v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>Can I get free COVID-19 testing or treatment if I am a senior over 65, disabled, uninsured, or an undocumented immigrant?</v>
+        <v>If my child’s school is engaged in distance learning, what should I expect?</v>
       </c>
       <c r="B56" t="str">
-        <v>[Medicare](https://www.medicare.gov/medicare-coronavirus) and [Medicare Advantage Plans](https://www.medicare.gov/sign-up-change-plans/types-of-medicare-health-plans/medicare-advantage-plans) provide free COVID-19 [diagnostic](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-tests) and [antibody tests](https://www.medicare.gov/coverage/coronavirus-disease-2019-covid-19-antibody-test). Needed COVID-19 diagnosis, testing, and treatment for the uninsured is [paid for by the government](https://www.hrsa.gov/CovidUninsuredClaim). \n\nMore info: [Health care](https://covid19.ca.gov/healthcare/)</v>
+        <v>*   New statewide requirements include:\n    *   Access to devices and connectivity for all students\n    *   Daily live interaction with teachers and other students\n    *   Classes and assignments that are challenging and are equivalent to in-person instruction\n    *   Special requirements for English language learners and special education students\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C56" t="str">
-        <v>https://covid19.ca.gov/healthcare/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D56" t="str">
         <v xml:space="preserve"> </v>
@@ -1838,13 +1838,13 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>What do taxpayers need to do if they want to take advantage of relief from the California Department of Tax and Fee Administration?</v>
+        <v>My school provides free grab-and-go meals. Are those still available?</v>
       </c>
       <c r="B57" t="str">
-        <v>Interested taxpayers should contact CDTFA by visiting the [CDTFA website](http://cdtfa.ca.gov/) or calling [800-400-7115](tel:800-400-7115).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Yes. It is essential to keep children fed. Check with your local school district for days and times meals are offered.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C57" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D57" t="str">
         <v xml:space="preserve"> </v>
@@ -1864,13 +1864,13 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>When will taxpayers start on these payment plans?</v>
+        <v>When can colleges or universities in counties resume indoor lectures?</v>
       </c>
       <c r="B58" t="str">
-        <v>Given that the April deadline to file and pay sales and use tax returns has been extended to late July for all but the largest taxpayers, CDTFA expects that most participating taxpayers will begin their payment arrangements in late July of this year.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Certain indoor operations in institutions of higher education must remain closed in counties in the Widespread (purple) tier. In other counties, those indoor operations can reopen consistent with the [Blueprint for a Safer Economy](https://covid19.ca.gov/safer-economy/) requirements for movie theaters and places of worship.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C58" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D58" t="str">
         <v xml:space="preserve"> </v>
@@ -1890,13 +1890,13 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>How will the payment plans work?</v>
+        <v>Is there financial help for student loans?</v>
       </c>
       <c r="B59" t="str">
-        <v>Qualifying sales and use taxpayers with deferred liabilities up to $50,000 will pay their tax due in 12 equal monthly installments. No interest or penalties will be assessed against the liability.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The [governor has ordered](https://www.gov.ca.gov/2020/04/23/governor-newsom-announces-additional-relief-for-californians-impacted-by-covid-19/) relief for students with federal loans. Check with your lender to see what options are available for you.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C59" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D59" t="str">
         <v xml:space="preserve"> </v>
@@ -1916,13 +1916,13 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>Is this only for tax payments due for the 1st quarter of 2020?</v>
+        <v>What if I don’t have internet access at home?</v>
       </c>
       <c r="B60" t="str">
-        <v>If taxpayers choose to use this program to distribute the burden of their May or June prepayments or their July return, CDTFA will work to accommodate those taxpayers.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Check with your local school district or college to see what resources are available for you.  List of providers offering free internet access currently:\n\n[Spectrum mobile](https://mobile.spectrum.com/support/article/360040980371/coronavirus-covid19-update)  has opened wifi hotspots and are working on assisting school districts with facilitating home internet access. \n\n[Comcast](https://corporate.comcast.com/covid-19) has opened free Xfinity WiFi hotspot access across the country. Xfinity has also paused data plans, late fees, and disconnects for the next 60 days. Families with limited income can receive internet services for free for the next 60 days (usually $9.95 per month). \n\n[AT&amp;T](https://about.att.com/pages/COVID-19.html)  has opened all public WiFi hotspots and will not charge customers for any late fees or overages. AT&amp;T also offers internet access for [$10/month for households on limited income](https://www.att.com/shop/internet/access/index.html?source=ECmj0000000000mbU&amp;wtExtndSource=access#!/#%2F).\n\n[Low-cost Internet access plans](https://www.cde.ca.gov/ls/he/hn/availableinternetplans.asp) are also available.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C60" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D60" t="str">
         <v xml:space="preserve"> </v>
@@ -1942,13 +1942,13 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>What if taxpayers owe more than the $50,000 limit on the relief?</v>
+        <v>How will students with disabilities receive services during school closures?</v>
       </c>
       <c r="B61" t="str">
-        <v>The maximum amount that any taxpayer can defer interest-free under this relief effort is $50,000.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The Department of Education has released [guidance on distance learning](https://www.cde.ca.gov/ls/he/hn/distancelearning.asp) to support schools. This guidance includes recommendations to ensure equity and access for all students.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C61" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D61" t="str">
         <v xml:space="preserve"> </v>
@@ -1968,13 +1968,13 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>What if taxpayers with more than $5 million in annual taxable sales need this relief?</v>
+        <v>Will there be standardized testing for students? When?</v>
       </c>
       <c r="B62" t="str">
-        <v>We recognize that some taxpayers, particularly in low margin businesses, with annual taxable sales over $5 million may also need this relief. Those taxpayers are encouraged to reach out to CDTFA, which will work with them to provide relief where appropriate.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Probably not: on March 18, 2020, Governor Newsom issued an [executive order](https://www.gov.ca.gov/2020/03/18/governor-newsom-issues-executive-order-to-suspend-standardized-testing-for-students-in-response-to-covid-19-outbreak/)  to waive this year’s statewide testing for K-12 schools.\n\nMore info: [Education](https://covid19.ca.gov/education/)</v>
       </c>
       <c r="C62" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/education/</v>
       </c>
       <c r="D62" t="str">
         <v xml:space="preserve"> </v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>Is the deadline for filing California tax returns extended?</v>
+        <v>What effect will late payments have on my credit report?</v>
       </c>
       <c r="B63" t="str">
-        <v>Yes. All California taxpayers (individuals and businesses) can file and pay by July 15, 2020. See [information from the CA Franchise Tax Board](https://www.ftb.ca.gov/about-ftb/newsroom/news-releases/2020-3-state-postpones-tax-deadlines-until-july-15-due-to-the-covid-19-pandemic.html) for more information.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Financial institutions will not report derogatory information (like late payments) to credit reporting agencies but may report a forbearance. Typically this does not negatively affect a credit score on its own.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C63" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/get-financial-help/</v>
       </c>
       <c r="D63" t="str">
         <v xml:space="preserve"> </v>
@@ -2020,13 +2020,13 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>What is a loan guarantee?</v>
+        <v>How long will financial relief programs last?</v>
       </c>
       <c r="B64" t="str">
-        <v>A loan guarantee is a credit enhancement that helps mitigate the risk assumed by a lending institution when making a loan. With the Small Business Finance Center’s Disaster Relief Loan Guarantee Program, IBank agrees to guarantee up to 95% of the loan, removing the barriers to capital that often exist for small business borrowers that may not otherwise be eligible for traditional lending. This program also can assist those who may not be eligible for a U.S. Small Business Administration (SBA) loan.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>It is still unclear how severe or how long the COVID-19 impact will be. Financial institutions have committed to necessary relief and will be assessing the ongoing conditions and need for continuing relief.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C64" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/get-financial-help/</v>
       </c>
       <c r="D64" t="str">
         <v xml:space="preserve"> </v>
@@ -2046,13 +2046,13 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>Who is eligible to apply for a loan guarantee?</v>
+        <v>What if my financial institution isn’t offering payment relief?</v>
       </c>
       <c r="B65" t="str">
-        <v>Small business entities that have been affected by loss, damage or other economic injury due to the COVID-19 pandemic and meet the program’s eligibility requirements. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Call or check their website to be sure. At this time, JP Morgan Chase, US Bank, Wells Fargo and Citigroup, [and nearly 200 state-chartered banks](https://dbo.ca.gov/covid19-updates-fi/), credit unions are supporting these commitments. \n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C65" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/get-financial-help/</v>
       </c>
       <c r="D65" t="str">
         <v xml:space="preserve"> </v>
@@ -2072,13 +2072,13 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>What do you consider a small business?</v>
+        <v>Is mortgage relief available to businesses?</v>
       </c>
       <c r="B66" t="str">
-        <v>The business must have between 1-750 employees and be established as an entity, including:\n\n*   Sole Proprietor – Individual using legal name as business name that files a Schedule C, Schedule F, or has a fictitious business name or DBA statement\n    *   If the loan appears to be in the name of an individual, evidence of Sole Proprietorship will be required and may include a Schedule C, Schedule F, Seller’s Permit, and/or fictitious business name or DBA statement\n*   Limited Liability Company \n*   Cooperative\n*   Corporation\n*   Partnership\n*   S-Corporation\n*   Not-for-profit\n\nThe program will not accept an _individual_ as the borrower. It is permissible for an individual to be a guarantor or co-borrower on the loan, but the primary borrower must be a small business. It does not consider citizenship or immigration status for eligibility requirements**,** as long as the entity/individual meets the above criteria. Trucking owners/operators are eligible as long as they are registered as a legal business entity.\n\n**AND**\n\n*   The business activity must be eligible under the program and in one of the industries listed in the [North American Industry Classification System (NAICS) codes list](http://www.census.gov/eos/www/naics), and\n*   It must be located in a declared disaster area. A major disaster area declaration was made for the state of California on March 22, 2020 in regards to the COVID-19 pandemic.\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>The relief is currently only available for residential mortgages.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C66" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/get-financial-help/</v>
       </c>
       <c r="D66" t="str">
         <v xml:space="preserve"> </v>
@@ -2098,13 +2098,13 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>What are excluded businesses?</v>
+        <v>What if my mortgage servicer is not communicative or cooperative?</v>
       </c>
       <c r="B67" t="str">
-        <v>Businesses that are not eligible include passive real estate businesses (rental income, etc.).\n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>You can file a complaint with the Department of Business Oversight:\n\n*   File on the [DBO website](https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fdbo.ca.gov%2Ffile-a-complaint%2F&amp;data=02%7C01%7CManuel.Alvarez%40dbo.ca.gov%7Ce2673837ec6f42fce84508d7d114ed59%7Cd6910b1745b44b7bbb66cb7936fabafe%7C1%7C0%7C637207760136603083&amp;sdata=VR6CdqCvrBGkfC%2Bm%2B6Yj9emco9ldVY5BLWSiLpe3f4c%3D&amp;reserved=0)\n*   Call their Consumer Services Office at [(866) 275-2677](tel:(866) 275-2677) or [(916) 327-7585](tel:(916) 327-7585) \n*   Or email [Ask.DBO@dbo.ca.gov](mailto:Ask.DBO@dbo.ca.gov)\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C67" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/get-financial-help/</v>
       </c>
       <c r="D67" t="str">
         <v xml:space="preserve"> </v>
@@ -2124,13 +2124,13 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>Can I apply for a loan guarantee only if I am ineligible for federal disaster fund financing, such as a SBA loan?</v>
+        <v>Can I get child care during the stay home order?</v>
       </c>
       <c r="B68" t="str">
-        <v>Yes, this program is designed for those who do not qualify for federal programs. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>Yes, all [childcare](https://covid19.ca.gov/childcare/) facilities can open with necessary modifications.\n\nMore info: [Get financial help](https://covid19.ca.gov/get-financial-help/)</v>
       </c>
       <c r="C68" t="str">
-        <v>https://covid19.ca.gov/business-and-employers/</v>
+        <v>https://covid19.ca.gov/get-financial-help/</v>
       </c>
       <c r="D68" t="str">
         <v xml:space="preserve"> </v>
@@ -2150,13 +2150,13 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>How much can I borrow?</v>
+        <v>Find your county websites</v>
       </c>
       <c r="B69" t="str">
-        <v>The Small Business Finance Center’s Disaster Relief Loan Guarantee Program allows a maximum loan of $1.25 million and a maximum guarantee of $1 million. To serve as many California small businesses as possible, the COVID-19 disaster program is focused on serving small businesses, especially those in low-wealth and immigrant communities with needs from $500 to $50,000. \n\nMore info: [Businesses and employers](https://covid19.ca.gov/business-and-employers/)</v>
+        <v>*   [Alameda County](http://www.acphd.org/2019-ncov.aspx)\n*   [Alpine County](http://alpinecountyca.gov/Index.aspx?NID=516)\n*   [Amador County](https://www.amadorgov.org/services/covid-19)\n*   [Butte County](https://www.buttecounty.net/publichealth)\n*   [Calaveras County](https://covid19.calaverasgov.us/)\n*   [Colusa County](https://www.countyofcolusa.org/99/Public-Health)\n*   [Contra Costa County](https://www.coronavirus.cchealth.org/)\n*   [Del Norte County](http://www.co.del-norte.ca.us/departments/health-human-services/public-health)\n*   [El Dorado County](https://www.edcgov.us/Government/hhsa/Pages/EDCCOVID-19.aspx)\n*   [Fresno County](https://www.co.fresno.ca.us/departments/public-health/covid-19)\n*   [Glenn County](https://www.countyofglenn.net/dept/health-human-services/public-health/covid-19)\n*   [Humboldt County](https://humboldtgov.org/2018/Humboldt-Health-Alert)\n*   [Imperial County](http://www.icphd.org/health-information-and-resources/healthy-facts/covid-19/)\n*   [Inyo County](https://www.inyocounty.us/coronavirus-covid-19-response)\n*   [Kern County](https://kernpublichealth.com/2019-novel-coronavirus/)\n*   [Kings County](https://www.countyofkings.com/departments/health-welfare/public-health/coronavirus-disease-2019-covid-19/-fsiteid-1)\n*   [Lake County](http://health.co.lake.ca.us/Coronavirus.htm)\n*   [Lassen County](http://www.co.lassen.ca.us/)\n*   [Los Angeles County](http://publichealth.lacounty.gov/media/Coronavirus/)\n*   [Madera County](https://www.maderaco